<commit_message>
Update 3dunet session annotations.xlsx
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBBFD11-A238-4417-A902-91FBC94FA651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9038D98E-610D-478C-86F4-28811EAFD00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="182">
   <si>
     <t>patch z</t>
   </si>
@@ -213,9 +213,6 @@
     <t>230830-0</t>
   </si>
   <si>
-    <t>result/answer</t>
-  </si>
-  <si>
     <t>goal/question</t>
   </si>
   <si>
@@ -387,9 +384,6 @@
     <t>expect VRAM ~ patch volume, expect out of VRAM error</t>
   </si>
   <si>
-    <t>stride = foor (resolution - patch) / 2</t>
-  </si>
-  <si>
     <t>TBD copy</t>
   </si>
   <si>
@@ -492,9 +486,6 @@
     <t>reason for automatic abortion</t>
   </si>
   <si>
-    <t>out of time (srun)</t>
-  </si>
-  <si>
     <t>wanted to get a node with faster, i.e., more CPUs for faster loading, but failed</t>
   </si>
   <si>
@@ -553,6 +544,45 @@
   </si>
   <si>
     <t>Yes, the logs are still there after train3dunet abortion, and yes, train3dunet produces tensorboard logs without preceding tensorboard command.</t>
+  </si>
+  <si>
+    <t>230907-0</t>
+  </si>
+  <si>
+    <t>increase val frequency to achieve decreasing learning rate with hope for increasing val eval score (plateau above previous from 230906-1, at 0.3)</t>
+  </si>
+  <si>
+    <t>expect that plateau will be higher than previously, because the learning rate will decrease with higher validation frequency</t>
+  </si>
+  <si>
+    <t>increasing train &amp; val eval score achieved, but both peek at 0.3 after 300 train iterations, val eval score decreases afterwards, train eval score plateaus there.</t>
+  </si>
+  <si>
+    <t>higher val frequency leads to decreasing learning rate but train &amp; val eval scores both still peek at 0.3 after about the same train iterations, vale eval score still decreases afterwards, train eval score still plateaus there. Conclusion: The plateau / maximum is not due to hyper parameters but is just the best this model can do with this dataset.</t>
+  </si>
+  <si>
+    <t>result/answer/conclusion</t>
+  </si>
+  <si>
+    <t>out of time</t>
+  </si>
+  <si>
+    <t>train eval plateau, val eval decreases after peek</t>
+  </si>
+  <si>
+    <t>stride = floor (resolution - patch) / 2</t>
+  </si>
+  <si>
+    <t>higher val eval score increase &amp; better val prediction images by increasing train sample size by creating a new pooled heart stain dataset (dataset04).</t>
+  </si>
+  <si>
+    <t>Good enough performance metrics &amp; val prediction images to merit test3dunet session.</t>
+  </si>
+  <si>
+    <t>dataset04</t>
+  </si>
+  <si>
+    <t>patch = arbitrary even int_2^3 as large a possible</t>
   </si>
 </sst>
 </file>
@@ -683,9 +713,7 @@
       <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -711,10 +739,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1029,34 +1057,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:AX31"/>
+  <dimension ref="A1:AX33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB31" sqref="AB31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" customWidth="1"/>
-    <col min="5" max="5" width="55.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="10"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.140625" collapsed="1"/>
-    <col min="19" max="19" width="6.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="22" width="5.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="5.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="8.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="5.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="9.140625" style="10" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="9.5703125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="6.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="22" width="5.140625" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="5.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="8.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="5.140625" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="7" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="9.140625" style="10" customWidth="1"/>
     <col min="28" max="30" width="9.140625" customWidth="1"/>
     <col min="31" max="31" width="7.28515625" style="1" customWidth="1" outlineLevel="1"/>
     <col min="32" max="33" width="7.28515625" customWidth="1" outlineLevel="1"/>
@@ -1087,49 +1114,49 @@
         <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="I1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="P1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>3</v>
@@ -1138,49 +1165,49 @@
         <v>4</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="U1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="Z1" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AA1" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="AC1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AE1" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>124</v>
-      </c>
       <c r="AF1" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="AH1" s="2" t="s">
         <v>40</v>
@@ -1207,13 +1234,13 @@
         <v>55</v>
       </c>
       <c r="AP1" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="AS1" s="2" t="s">
         <v>56</v>
@@ -1225,10 +1252,10 @@
         <v>23</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="AX1" s="2" t="s">
         <v>27</v>
@@ -1236,19 +1263,19 @@
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
         <v>140</v>
       </c>
-      <c r="B2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>142</v>
       </c>
-      <c r="D2" t="s">
-        <v>144</v>
-      </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
@@ -1263,7 +1290,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
@@ -1281,13 +1308,13 @@
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q2">
         <v>5</v>
       </c>
       <c r="R2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="S2">
         <v>3</v>
@@ -1305,13 +1332,13 @@
         <v>16</v>
       </c>
       <c r="X2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y2">
         <v>8</v>
       </c>
       <c r="Z2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA2" s="10">
         <v>0</v>
@@ -1326,7 +1353,7 @@
         <v>8</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AF2" t="s">
         <v>8</v>
@@ -1335,7 +1362,7 @@
         <v>8</v>
       </c>
       <c r="AH2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AI2" s="10">
         <v>125</v>
@@ -1347,40 +1374,40 @@
         <v>414</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AM2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AN2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AO2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AQ2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AR2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AS2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AT2" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AU2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AV2">
         <v>1</v>
       </c>
       <c r="AW2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AX2" t="s">
         <v>8</v>
@@ -1388,20 +1415,20 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" t="s">
         <v>142</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>144</v>
       </c>
-      <c r="E3" t="s">
-        <v>146</v>
-      </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
@@ -1415,31 +1442,31 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q3">
         <v>5</v>
       </c>
       <c r="R3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="S3">
         <v>3</v>
@@ -1457,16 +1484,16 @@
         <v>16</v>
       </c>
       <c r="X3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y3">
         <v>8</v>
       </c>
       <c r="Z3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA3" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AB3" t="s">
         <v>8</v>
@@ -1478,7 +1505,7 @@
         <v>8</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AF3" t="s">
         <v>8</v>
@@ -1487,7 +1514,7 @@
         <v>8</v>
       </c>
       <c r="AH3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AI3" s="10">
         <v>125</v>
@@ -1499,34 +1526,34 @@
         <v>414</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AM3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AN3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AO3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AP3" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AQ3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AR3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AS3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AT3" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AU3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AV3">
         <v>0</v>
@@ -1543,16 +1570,16 @@
         <v>57</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F4" s="13">
         <v>0</v>
@@ -1561,7 +1588,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I4" s="12">
         <v>0</v>
@@ -1585,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q4" s="12">
         <v>5</v>
@@ -1609,13 +1636,13 @@
         <v>16</v>
       </c>
       <c r="X4" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y4" s="12">
         <v>8</v>
       </c>
       <c r="Z4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA4" s="13" t="s">
         <v>36</v>
@@ -1695,16 +1722,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
         <v>135</v>
       </c>
-      <c r="C5" t="s">
-        <v>137</v>
-      </c>
       <c r="D5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -1713,7 +1740,7 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1727,7 +1754,7 @@
       <c r="L5" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="16" t="s">
+      <c r="M5" t="s">
         <v>8</v>
       </c>
       <c r="N5" t="s">
@@ -1737,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q5">
         <v>5</v>
@@ -1761,13 +1788,13 @@
         <v>16</v>
       </c>
       <c r="X5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y5">
         <v>8</v>
       </c>
       <c r="Z5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA5" s="10" t="s">
         <v>36</v>
@@ -1832,7 +1859,7 @@
       <c r="AU5" t="s">
         <v>16</v>
       </c>
-      <c r="AV5" s="16">
+      <c r="AV5">
         <v>0</v>
       </c>
       <c r="AW5" t="s">
@@ -1847,16 +1874,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
         <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="10">
         <v>0</v>
@@ -1879,7 +1906,7 @@
       <c r="L6" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M6" t="s">
         <v>8</v>
       </c>
       <c r="N6" t="s">
@@ -1889,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q6">
         <v>5</v>
@@ -1913,13 +1940,13 @@
         <v>16</v>
       </c>
       <c r="X6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y6">
         <v>8</v>
       </c>
       <c r="Z6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA6" s="10" t="s">
         <v>8</v>
@@ -1984,7 +2011,7 @@
       <c r="AU6" t="s">
         <v>10</v>
       </c>
-      <c r="AV6" s="16">
+      <c r="AV6">
         <v>1</v>
       </c>
       <c r="AW6" t="s">
@@ -1999,16 +2026,16 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
         <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="10">
         <v>0</v>
@@ -2031,7 +2058,7 @@
       <c r="L7" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="16" t="s">
+      <c r="M7" t="s">
         <v>8</v>
       </c>
       <c r="N7" t="s">
@@ -2041,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q7">
         <v>5</v>
@@ -2065,13 +2092,13 @@
         <v>16</v>
       </c>
       <c r="X7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y7">
         <v>8</v>
       </c>
       <c r="Z7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA7" s="10" t="s">
         <v>8</v>
@@ -2136,7 +2163,7 @@
       <c r="AU7" t="s">
         <v>9</v>
       </c>
-      <c r="AV7" s="16">
+      <c r="AV7">
         <v>1</v>
       </c>
       <c r="AW7" t="s">
@@ -2151,16 +2178,16 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
         <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="10">
         <v>0</v>
@@ -2169,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -2183,7 +2210,7 @@
       <c r="L8" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="16" t="s">
+      <c r="M8" t="s">
         <v>8</v>
       </c>
       <c r="N8" t="s">
@@ -2193,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q8">
         <v>5</v>
@@ -2217,13 +2244,13 @@
         <v>16</v>
       </c>
       <c r="X8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y8">
         <v>8</v>
       </c>
       <c r="Z8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA8" s="10" t="s">
         <v>36</v>
@@ -2288,7 +2315,7 @@
       <c r="AU8" t="s">
         <v>16</v>
       </c>
-      <c r="AV8" s="16">
+      <c r="AV8">
         <v>1</v>
       </c>
       <c r="AW8" t="s">
@@ -2303,16 +2330,16 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
         <v>135</v>
       </c>
-      <c r="C9" t="s">
-        <v>137</v>
-      </c>
       <c r="D9" t="s">
         <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9" s="10">
         <v>0</v>
@@ -2335,7 +2362,7 @@
       <c r="L9" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" t="s">
         <v>8</v>
       </c>
       <c r="N9" t="s">
@@ -2345,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q9">
         <v>5</v>
@@ -2369,13 +2396,13 @@
         <v>16</v>
       </c>
       <c r="X9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y9">
         <v>8</v>
       </c>
       <c r="Z9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA9" s="10" t="s">
         <v>8</v>
@@ -2446,7 +2473,7 @@
       <c r="AU9" t="s">
         <v>16</v>
       </c>
-      <c r="AV9" s="16">
+      <c r="AV9">
         <v>1</v>
       </c>
       <c r="AW9" t="s">
@@ -2461,16 +2488,16 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
         <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F10" s="10">
         <v>0</v>
@@ -2493,7 +2520,7 @@
       <c r="L10" t="s">
         <v>8</v>
       </c>
-      <c r="M10" s="16" t="s">
+      <c r="M10" t="s">
         <v>8</v>
       </c>
       <c r="N10" t="s">
@@ -2503,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q10">
         <v>5</v>
@@ -2527,13 +2554,13 @@
         <v>16</v>
       </c>
       <c r="X10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y10">
         <v>8</v>
       </c>
       <c r="Z10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA10" s="10" t="s">
         <v>8</v>
@@ -2596,9 +2623,9 @@
         <v>30</v>
       </c>
       <c r="AU10" t="s">
-        <v>76</v>
-      </c>
-      <c r="AV10" s="16">
+        <v>75</v>
+      </c>
+      <c r="AV10">
         <v>1</v>
       </c>
       <c r="AW10" t="s">
@@ -2613,16 +2640,16 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
         <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" s="10">
         <v>0</v>
@@ -2631,7 +2658,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2645,7 +2672,7 @@
       <c r="L11" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="16" t="s">
+      <c r="M11" t="s">
         <v>8</v>
       </c>
       <c r="N11" t="s">
@@ -2655,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q11">
         <v>5</v>
@@ -2679,13 +2706,13 @@
         <v>16</v>
       </c>
       <c r="X11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y11">
         <v>8</v>
       </c>
       <c r="Z11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA11" s="10" t="s">
         <v>36</v>
@@ -2750,7 +2777,7 @@
       <c r="AU11" t="s">
         <v>31</v>
       </c>
-      <c r="AV11" s="16">
+      <c r="AV11">
         <v>1</v>
       </c>
       <c r="AW11" t="s">
@@ -2765,10 +2792,10 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
         <v>51</v>
@@ -2789,7 +2816,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -2797,7 +2824,7 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12">
         <v>0</v>
       </c>
       <c r="N12">
@@ -2807,7 +2834,7 @@
         <v>1</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q12">
         <v>5</v>
@@ -2831,13 +2858,13 @@
         <v>16</v>
       </c>
       <c r="X12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y12">
         <v>8</v>
       </c>
       <c r="Z12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA12" s="10">
         <v>10135</v>
@@ -2902,7 +2929,7 @@
       <c r="AU12" t="s">
         <v>31</v>
       </c>
-      <c r="AV12" s="16">
+      <c r="AV12">
         <v>0</v>
       </c>
       <c r="AW12" t="s">
@@ -2917,13 +2944,13 @@
         <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C13" t="s">
         <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
         <v>50</v>
@@ -2949,7 +2976,7 @@
       <c r="L13" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M13" t="s">
         <v>8</v>
       </c>
       <c r="N13" t="s">
@@ -2959,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q13">
         <v>5</v>
@@ -2983,13 +3010,13 @@
         <v>16</v>
       </c>
       <c r="X13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y13">
         <v>8</v>
       </c>
       <c r="Z13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA13" s="10" t="s">
         <v>8</v>
@@ -3054,7 +3081,7 @@
       <c r="AU13" t="s">
         <v>31</v>
       </c>
-      <c r="AV13" s="16">
+      <c r="AV13">
         <v>1</v>
       </c>
       <c r="AW13" t="s">
@@ -3069,13 +3096,13 @@
         <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C14" t="s">
         <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
         <v>50</v>
@@ -3101,7 +3128,7 @@
       <c r="L14" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="16" t="s">
+      <c r="M14" t="s">
         <v>8</v>
       </c>
       <c r="N14" t="s">
@@ -3111,7 +3138,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q14">
         <v>5</v>
@@ -3135,13 +3162,13 @@
         <v>16</v>
       </c>
       <c r="X14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y14">
         <v>8</v>
       </c>
       <c r="Z14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA14" s="10" t="s">
         <v>8</v>
@@ -3206,7 +3233,7 @@
       <c r="AU14" t="s">
         <v>49</v>
       </c>
-      <c r="AV14" s="16">
+      <c r="AV14">
         <v>1</v>
       </c>
       <c r="AW14" t="s">
@@ -3221,13 +3248,13 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C15" t="s">
         <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
         <v>51</v>
@@ -3245,7 +3272,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -3253,7 +3280,7 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
@@ -3263,7 +3290,7 @@
         <v>1</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q15">
         <v>5</v>
@@ -3287,13 +3314,13 @@
         <v>16</v>
       </c>
       <c r="X15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y15">
         <v>8</v>
       </c>
       <c r="Z15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA15" s="10">
         <v>13843</v>
@@ -3358,7 +3385,7 @@
       <c r="AU15" t="s">
         <v>31</v>
       </c>
-      <c r="AV15" s="16">
+      <c r="AV15">
         <v>0</v>
       </c>
       <c r="AW15" t="s">
@@ -3373,13 +3400,13 @@
         <v>48</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>51</v>
@@ -3397,7 +3424,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K16" s="7">
         <v>0</v>
@@ -3415,7 +3442,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q16" s="7">
         <v>5</v>
@@ -3439,13 +3466,13 @@
         <v>16</v>
       </c>
       <c r="X16" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y16" s="7">
         <v>8</v>
       </c>
       <c r="Z16" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA16" s="11">
         <v>13843</v>
@@ -3505,7 +3532,7 @@
         <v>51</v>
       </c>
       <c r="AT16" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU16" s="7" t="s">
         <v>49</v>
@@ -3525,16 +3552,16 @@
         <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -3549,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -3557,7 +3584,7 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17" s="16">
+      <c r="M17">
         <v>0</v>
       </c>
       <c r="N17">
@@ -3567,7 +3594,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q17">
         <v>5</v>
@@ -3591,13 +3618,13 @@
         <v>16</v>
       </c>
       <c r="X17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y17">
         <v>8</v>
       </c>
       <c r="Z17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA17" s="10">
         <v>10135</v>
@@ -3657,12 +3684,12 @@
         <v>51</v>
       </c>
       <c r="AT17" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU17" t="s">
-        <v>78</v>
-      </c>
-      <c r="AV17" s="16">
+        <v>77</v>
+      </c>
+      <c r="AV17">
         <v>0</v>
       </c>
       <c r="AW17" t="s">
@@ -3677,13 +3704,13 @@
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18" t="s">
         <v>51</v>
@@ -3701,7 +3728,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -3709,7 +3736,7 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18" s="16">
+      <c r="M18">
         <v>0</v>
       </c>
       <c r="N18">
@@ -3719,7 +3746,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q18">
         <v>5</v>
@@ -3743,13 +3770,13 @@
         <v>16</v>
       </c>
       <c r="X18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y18">
         <v>8</v>
       </c>
       <c r="Z18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA18" s="10">
         <v>10135</v>
@@ -3809,12 +3836,12 @@
         <v>51</v>
       </c>
       <c r="AT18" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU18" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV18" s="16">
+        <v>74</v>
+      </c>
+      <c r="AV18">
         <v>0</v>
       </c>
       <c r="AW18" t="s">
@@ -3829,13 +3856,13 @@
         <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E19" t="s">
         <v>51</v>
@@ -3853,7 +3880,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -3861,7 +3888,7 @@
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="M19" s="16">
+      <c r="M19">
         <v>0</v>
       </c>
       <c r="N19">
@@ -3871,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q19">
         <v>5</v>
@@ -3895,13 +3922,13 @@
         <v>16</v>
       </c>
       <c r="X19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y19">
         <v>8</v>
       </c>
       <c r="Z19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA19" s="10">
         <v>10999</v>
@@ -3961,12 +3988,12 @@
         <v>51</v>
       </c>
       <c r="AT19" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU19" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV19" s="16">
+        <v>74</v>
+      </c>
+      <c r="AV19">
         <v>0</v>
       </c>
       <c r="AW19" t="s">
@@ -3978,16 +4005,16 @@
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
         <v>51</v>
@@ -4005,7 +4032,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -4013,7 +4040,7 @@
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20" s="16">
+      <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
@@ -4023,7 +4050,7 @@
         <v>1</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q20">
         <v>5</v>
@@ -4047,13 +4074,13 @@
         <v>16</v>
       </c>
       <c r="X20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y20">
         <v>8</v>
       </c>
       <c r="Z20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA20" s="10">
         <v>11843</v>
@@ -4113,12 +4140,12 @@
         <v>51</v>
       </c>
       <c r="AT20" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU20" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV20" s="16">
+        <v>74</v>
+      </c>
+      <c r="AV20">
         <v>0</v>
       </c>
       <c r="AW20" t="s">
@@ -4130,16 +4157,16 @@
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E21" t="s">
         <v>51</v>
@@ -4157,7 +4184,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -4165,7 +4192,7 @@
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="M21" s="16">
+      <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
@@ -4175,7 +4202,7 @@
         <v>1</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q21">
         <v>5</v>
@@ -4199,13 +4226,13 @@
         <v>16</v>
       </c>
       <c r="X21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y21">
         <v>8</v>
       </c>
       <c r="Z21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA21" s="10">
         <v>10473</v>
@@ -4265,12 +4292,12 @@
         <v>51</v>
       </c>
       <c r="AT21" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU21" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV21" s="16">
+        <v>74</v>
+      </c>
+      <c r="AV21">
         <v>0</v>
       </c>
       <c r="AW21" t="s">
@@ -4282,16 +4309,16 @@
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E22" t="s">
         <v>51</v>
@@ -4309,7 +4336,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -4317,7 +4344,7 @@
       <c r="L22">
         <v>0</v>
       </c>
-      <c r="M22" s="16">
+      <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
@@ -4327,7 +4354,7 @@
         <v>1</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q22">
         <v>5</v>
@@ -4351,13 +4378,13 @@
         <v>16</v>
       </c>
       <c r="X22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y22">
         <v>8</v>
       </c>
       <c r="Z22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA22" s="10">
         <v>10825</v>
@@ -4417,12 +4444,12 @@
         <v>51</v>
       </c>
       <c r="AT22" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV22" s="16">
+        <v>74</v>
+      </c>
+      <c r="AV22">
         <v>0</v>
       </c>
       <c r="AW22" t="s">
@@ -4434,16 +4461,16 @@
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
         <v>51</v>
@@ -4461,7 +4488,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -4469,7 +4496,7 @@
       <c r="L23">
         <v>0</v>
       </c>
-      <c r="M23" s="16">
+      <c r="M23">
         <v>0</v>
       </c>
       <c r="N23">
@@ -4479,7 +4506,7 @@
         <v>1</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q23">
         <v>5</v>
@@ -4503,13 +4530,13 @@
         <v>16</v>
       </c>
       <c r="X23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y23">
         <v>8</v>
       </c>
       <c r="Z23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA23" s="10">
         <v>12317</v>
@@ -4569,12 +4596,12 @@
         <v>51</v>
       </c>
       <c r="AT23" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU23" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV23" s="16">
+        <v>74</v>
+      </c>
+      <c r="AV23">
         <v>0</v>
       </c>
       <c r="AW23" t="s">
@@ -4586,16 +4613,16 @@
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E24" t="s">
         <v>51</v>
@@ -4613,7 +4640,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -4621,7 +4648,7 @@
       <c r="L24">
         <v>0</v>
       </c>
-      <c r="M24" s="16">
+      <c r="M24">
         <v>0</v>
       </c>
       <c r="N24">
@@ -4631,7 +4658,7 @@
         <v>1</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q24">
         <v>5</v>
@@ -4655,13 +4682,13 @@
         <v>16</v>
       </c>
       <c r="X24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y24">
         <v>8</v>
       </c>
       <c r="Z24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA24" s="10">
         <v>14443</v>
@@ -4721,12 +4748,12 @@
         <v>51</v>
       </c>
       <c r="AT24" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU24" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV24" s="16">
+        <v>74</v>
+      </c>
+      <c r="AV24">
         <v>0</v>
       </c>
       <c r="AW24" t="s">
@@ -4738,7 +4765,7 @@
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -4747,11 +4774,11 @@
         <v>8</v>
       </c>
       <c r="D25" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" t="s">
         <v>109</v>
       </c>
-      <c r="E25" t="s">
-        <v>110</v>
-      </c>
       <c r="F25" s="10" t="s">
         <v>8</v>
       </c>
@@ -4878,7 +4905,7 @@
       <c r="AU25" t="s">
         <v>8</v>
       </c>
-      <c r="AV25" s="16">
+      <c r="AV25">
         <v>0</v>
       </c>
       <c r="AW25" t="s">
@@ -4890,7 +4917,7 @@
     </row>
     <row r="26" spans="1:50" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>8</v>
@@ -4899,10 +4926,10 @@
         <v>8</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>8</v>
@@ -5042,19 +5069,19 @@
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F27" s="10">
         <v>0</v>
@@ -5069,7 +5096,7 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -5077,7 +5104,7 @@
       <c r="L27">
         <v>0</v>
       </c>
-      <c r="M27" s="16">
+      <c r="M27">
         <v>0</v>
       </c>
       <c r="N27">
@@ -5087,7 +5114,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q27">
         <v>5</v>
@@ -5111,16 +5138,16 @@
         <v>16</v>
       </c>
       <c r="X27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y27">
         <v>8</v>
       </c>
       <c r="Z27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA27" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AB27" t="s">
         <v>8</v>
@@ -5142,7 +5169,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AH27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AI27" s="10">
         <v>125</v>
@@ -5181,12 +5208,12 @@
         <v>51</v>
       </c>
       <c r="AT27" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU27" t="s">
-        <v>116</v>
-      </c>
-      <c r="AV27" s="16">
+        <v>177</v>
+      </c>
+      <c r="AV27">
         <v>0</v>
       </c>
       <c r="AW27" t="s">
@@ -5198,19 +5225,19 @@
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F28" s="10">
         <v>0</v>
@@ -5219,7 +5246,7 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -5233,7 +5260,7 @@
       <c r="L28">
         <v>0</v>
       </c>
-      <c r="M28" s="16">
+      <c r="M28">
         <v>0</v>
       </c>
       <c r="N28">
@@ -5243,7 +5270,7 @@
         <v>0</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q28">
         <v>5</v>
@@ -5267,16 +5294,16 @@
         <v>16</v>
       </c>
       <c r="X28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Y28">
         <v>8</v>
       </c>
       <c r="Z28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AA28" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="AB28">
         <v>82032.639999999999</v>
@@ -5286,7 +5313,7 @@
         <v>80.11</v>
       </c>
       <c r="AD28">
-        <f t="shared" ref="AD28:AD31" si="3" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AL28*AM28*AN28)</f>
+        <f t="shared" ref="AD28:AD32" si="3" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AL28*AM28*AN28)</f>
         <v>81518.129922434266</v>
       </c>
       <c r="AE28" s="1">
@@ -5299,7 +5326,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AH28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AI28" s="10">
         <v>125</v>
@@ -5338,258 +5365,264 @@
         <v>51</v>
       </c>
       <c r="AT28" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AU28" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV28">
+        <v>1</v>
+      </c>
+      <c r="AW28" t="s">
         <v>116</v>
       </c>
-      <c r="AV28" s="16">
-        <v>1</v>
-      </c>
-      <c r="AW28" t="s">
-        <v>118</v>
-      </c>
       <c r="AX28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:50" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F29" s="11">
-        <v>0</v>
-      </c>
-      <c r="G29" s="7">
-        <v>1</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="I29" s="7">
-        <v>0</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K29" s="7">
-        <v>1</v>
-      </c>
-      <c r="L29" s="7">
-        <v>0</v>
-      </c>
-      <c r="M29" s="7">
-        <v>1</v>
-      </c>
-      <c r="N29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="O29" s="7">
-        <v>1</v>
-      </c>
-      <c r="P29" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q29" s="7">
+    <row r="29" spans="1:50" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+      <c r="G29" s="18">
+        <v>1</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="I29" s="18">
+        <v>0</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K29" s="18">
+        <v>1</v>
+      </c>
+      <c r="L29" s="18">
+        <v>0</v>
+      </c>
+      <c r="M29" s="18">
+        <v>1</v>
+      </c>
+      <c r="N29" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="O29" s="18">
+        <v>1</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q29" s="18">
         <v>5</v>
       </c>
-      <c r="R29" s="7">
+      <c r="R29" s="18">
         <v>5</v>
       </c>
-      <c r="S29" s="7">
+      <c r="S29" s="18">
         <v>3</v>
       </c>
-      <c r="T29" s="7">
+      <c r="T29" s="18">
         <v>2</v>
       </c>
-      <c r="U29" s="7">
+      <c r="U29" s="18">
         <v>3</v>
       </c>
-      <c r="V29" s="7">
-        <v>1</v>
-      </c>
-      <c r="W29" s="7">
+      <c r="V29" s="18">
+        <v>1</v>
+      </c>
+      <c r="W29" s="18">
         <v>16</v>
       </c>
-      <c r="X29" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y29" s="7">
-        <v>8</v>
-      </c>
-      <c r="Z29" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA29" s="11">
+      <c r="X29" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y29" s="18">
+        <v>8</v>
+      </c>
+      <c r="Z29" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA29" s="10">
         <v>77887</v>
       </c>
-      <c r="AB29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD29" s="7">
+      <c r="AB29" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC29" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD29" s="18">
         <f t="shared" si="3"/>
         <v>76989.258353221856</v>
       </c>
-      <c r="AE29" s="8">
+      <c r="AE29" s="1">
         <v>81920</v>
       </c>
-      <c r="AF29" s="7">
+      <c r="AF29" s="18">
         <v>81049.600000000006</v>
       </c>
-      <c r="AG29" s="7">
+      <c r="AG29" s="18">
         <v>79.150000000000006</v>
       </c>
-      <c r="AH29" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="AI29" s="11">
+      <c r="AH29" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI29" s="10">
         <v>125</v>
       </c>
-      <c r="AJ29" s="7">
+      <c r="AJ29" s="18">
         <v>1169</v>
       </c>
-      <c r="AK29" s="7">
+      <c r="AK29" s="18">
         <v>414</v>
       </c>
-      <c r="AL29" s="8">
+      <c r="AL29" s="1">
         <v>112</v>
       </c>
-      <c r="AM29" s="7">
+      <c r="AM29" s="18">
         <v>800</v>
       </c>
-      <c r="AN29" s="7">
+      <c r="AN29" s="18">
         <v>400</v>
       </c>
-      <c r="AO29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP29" s="8">
+      <c r="AO29" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP29" s="1">
         <f xml:space="preserve"> _xlfn.FLOOR.MATH((AI29 - AL29) / 2)</f>
         <v>6</v>
       </c>
-      <c r="AQ29" s="7">
+      <c r="AQ29" s="18">
         <f t="shared" ref="AQ29" si="6" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ29 - AM29) / 2)</f>
         <v>184</v>
       </c>
-      <c r="AR29" s="7">
+      <c r="AR29" s="18">
         <f t="shared" ref="AR29" si="7" xml:space="preserve"> _xlfn.FLOOR.MATH((AK29 - AN29) / 2)</f>
         <v>7</v>
       </c>
-      <c r="AS29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="AT29" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="AU29" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="AV29" s="7">
-        <v>0</v>
-      </c>
-      <c r="AW29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX29" s="7" t="s">
+      <c r="AS29" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT29" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="AU29" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV29" s="18">
+        <v>0</v>
+      </c>
+      <c r="AW29" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX29" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="E30" s="16" t="s">
-        <v>171</v>
+      <c r="A30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" t="s">
+        <v>163</v>
+      </c>
+      <c r="E30" t="s">
+        <v>168</v>
       </c>
       <c r="F30" s="10">
         <v>0</v>
       </c>
-      <c r="G30" s="16">
-        <v>0</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="16">
-        <v>1</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="K30" s="16">
-        <v>0</v>
-      </c>
-      <c r="L30" s="16">
-        <v>0</v>
-      </c>
-      <c r="M30" s="16">
-        <v>0</v>
-      </c>
-      <c r="N30" s="16">
-        <v>0</v>
-      </c>
-      <c r="O30" s="16">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>153</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
         <v>1</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q30" s="16">
+        <v>73</v>
+      </c>
+      <c r="Q30">
         <v>5</v>
       </c>
-      <c r="R30" s="16">
+      <c r="R30">
         <v>5</v>
       </c>
-      <c r="S30" s="16">
+      <c r="S30">
         <v>3</v>
       </c>
-      <c r="T30" s="16">
+      <c r="T30">
         <v>2</v>
       </c>
-      <c r="U30" s="16">
+      <c r="U30">
         <v>3</v>
       </c>
-      <c r="V30" s="16">
-        <v>1</v>
-      </c>
-      <c r="W30" s="16">
+      <c r="V30">
+        <v>1</v>
+      </c>
+      <c r="W30">
         <v>16</v>
       </c>
-      <c r="X30" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y30" s="16">
-        <v>8</v>
-      </c>
-      <c r="Z30" s="16" t="s">
-        <v>104</v>
+      <c r="X30" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y30">
+        <v>8</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>103</v>
       </c>
       <c r="AA30" s="10">
         <v>77885</v>
+      </c>
+      <c r="AB30" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC30" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="AD30">
         <f t="shared" si="3"/>
@@ -5604,8 +5637,8 @@
       <c r="AG30">
         <v>79.150000000000006</v>
       </c>
-      <c r="AH30" s="18" t="s">
-        <v>113</v>
+      <c r="AH30" s="17" t="s">
+        <v>112</v>
       </c>
       <c r="AI30" s="10">
         <v>125</v>
@@ -5641,95 +5674,110 @@
         <v>51</v>
       </c>
       <c r="AT30" s="10" t="s">
-        <v>70</v>
+        <v>181</v>
       </c>
       <c r="AU30" t="s">
-        <v>116</v>
+        <v>177</v>
+      </c>
+      <c r="AV30" s="15">
+        <v>0</v>
+      </c>
+      <c r="AW30" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX30" s="15" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:50" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="E31" s="16" t="s">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="I31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="J31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="K31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="L31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="M31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="N31" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="O31" s="16" t="s">
-        <v>133</v>
+      <c r="C31" t="s">
+        <v>160</v>
+      </c>
+      <c r="D31" t="s">
+        <v>161</v>
+      </c>
+      <c r="E31" t="s">
+        <v>172</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>175</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q31" s="15">
+        <v>73</v>
+      </c>
+      <c r="Q31">
         <v>5</v>
       </c>
-      <c r="R31" s="16">
+      <c r="R31">
         <v>5</v>
       </c>
-      <c r="S31" s="15">
+      <c r="S31">
         <v>3</v>
       </c>
-      <c r="T31" s="15">
+      <c r="T31">
         <v>2</v>
       </c>
-      <c r="U31" s="15">
+      <c r="U31">
         <v>3</v>
       </c>
-      <c r="V31" s="15">
-        <v>1</v>
-      </c>
-      <c r="W31" s="15">
+      <c r="V31">
+        <v>1</v>
+      </c>
+      <c r="W31">
         <v>16</v>
       </c>
-      <c r="X31" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y31" s="15">
-        <v>8</v>
-      </c>
-      <c r="Z31" s="15" t="s">
-        <v>104</v>
+      <c r="X31" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y31">
+        <v>8</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>103</v>
       </c>
       <c r="AA31" s="10">
         <v>78017</v>
       </c>
-      <c r="AD31" s="15">
+      <c r="AB31" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC31" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD31">
         <f t="shared" si="3"/>
         <v>76989.258353221856</v>
       </c>
@@ -5742,47 +5790,286 @@
       <c r="AG31">
         <v>79.150000000000006</v>
       </c>
-      <c r="AH31" s="15" t="s">
-        <v>113</v>
+      <c r="AH31" t="s">
+        <v>112</v>
       </c>
       <c r="AI31" s="10">
         <v>125</v>
       </c>
-      <c r="AJ31" s="15">
+      <c r="AJ31">
         <v>1169</v>
       </c>
-      <c r="AK31" s="15">
+      <c r="AK31">
         <v>414</v>
       </c>
       <c r="AL31" s="1">
         <v>112</v>
       </c>
-      <c r="AM31" s="15">
+      <c r="AM31">
         <v>800</v>
       </c>
-      <c r="AN31" s="15">
+      <c r="AN31">
         <v>400</v>
       </c>
-      <c r="AO31" s="15" t="s">
+      <c r="AO31" t="s">
         <v>51</v>
       </c>
       <c r="AP31" s="1">
         <v>6</v>
       </c>
-      <c r="AQ31" s="15">
+      <c r="AQ31">
         <v>184</v>
       </c>
-      <c r="AR31" s="15">
+      <c r="AR31">
         <v>7</v>
       </c>
-      <c r="AS31" s="15" t="s">
+      <c r="AS31" t="s">
         <v>51</v>
       </c>
       <c r="AT31" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="AU31" s="15" t="s">
-        <v>116</v>
+        <v>181</v>
+      </c>
+      <c r="AU31" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV31" s="15">
+        <v>0</v>
+      </c>
+      <c r="AW31" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX31" s="15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:50" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="F32" s="11">
+        <v>0</v>
+      </c>
+      <c r="G32" s="7">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="7">
+        <v>1</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+      <c r="L32" s="7">
+        <v>1</v>
+      </c>
+      <c r="M32" s="7">
+        <v>1</v>
+      </c>
+      <c r="N32" s="7">
+        <v>1</v>
+      </c>
+      <c r="O32" s="7">
+        <v>1</v>
+      </c>
+      <c r="P32" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>5</v>
+      </c>
+      <c r="R32" s="7">
+        <v>5</v>
+      </c>
+      <c r="S32" s="7">
+        <v>3</v>
+      </c>
+      <c r="T32" s="7">
+        <v>2</v>
+      </c>
+      <c r="U32" s="7">
+        <v>3</v>
+      </c>
+      <c r="V32" s="7">
+        <v>1</v>
+      </c>
+      <c r="W32" s="7">
+        <v>16</v>
+      </c>
+      <c r="X32" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y32" s="7">
+        <v>8</v>
+      </c>
+      <c r="Z32" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA32" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB32" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC32" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD32" s="7">
+        <f t="shared" si="3"/>
+        <v>76989.258353221856</v>
+      </c>
+      <c r="AE32" s="8">
+        <v>81920</v>
+      </c>
+      <c r="AF32" s="7">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="AG32" s="7">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="AH32" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI32" s="11">
+        <v>125</v>
+      </c>
+      <c r="AJ32" s="7">
+        <v>1169</v>
+      </c>
+      <c r="AK32" s="7">
+        <v>414</v>
+      </c>
+      <c r="AL32" s="8">
+        <v>112</v>
+      </c>
+      <c r="AM32" s="7">
+        <v>800</v>
+      </c>
+      <c r="AN32" s="7">
+        <v>400</v>
+      </c>
+      <c r="AO32" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP32" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ32" s="7">
+        <v>184</v>
+      </c>
+      <c r="AR32" s="7">
+        <v>7</v>
+      </c>
+      <c r="AS32" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT32" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="AU32" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AW32" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX32" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D33" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="L33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="M33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="N33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="O33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="R33" t="s">
+        <v>131</v>
+      </c>
+      <c r="S33" t="s">
+        <v>131</v>
+      </c>
+      <c r="T33" t="s">
+        <v>131</v>
+      </c>
+      <c r="U33" s="15">
+        <v>1</v>
+      </c>
+      <c r="V33" s="15">
+        <v>1</v>
+      </c>
+      <c r="W33" s="15">
+        <v>16</v>
+      </c>
+      <c r="X33" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y33">
+        <v>8</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prep train config yaml
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEDC766-3EE8-43B6-9508-0C4A61128A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F34B195-E639-4145-83DA-EB4DEB7D5223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -766,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -785,10 +785,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1105,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:AY39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE35" sqref="AE35"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AV22" sqref="AV22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -6421,10 +6417,10 @@
       <c r="AB34" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AC34" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD34" s="16" t="s">
+      <c r="AC34" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD34" t="s">
         <v>8</v>
       </c>
       <c r="AE34">
@@ -6452,37 +6448,37 @@
       <c r="AL34">
         <v>414</v>
       </c>
-      <c r="AM34" s="17">
+      <c r="AM34" s="1">
         <v>96</v>
       </c>
-      <c r="AN34" s="18">
+      <c r="AN34">
         <v>784</v>
       </c>
-      <c r="AO34" s="18">
+      <c r="AO34">
         <v>384</v>
       </c>
-      <c r="AP34" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ34" s="17">
+      <c r="AP34" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ34" s="1">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="AR34" s="18">
+      <c r="AR34">
         <f t="shared" si="11"/>
         <v>192</v>
       </c>
-      <c r="AS34" s="18">
+      <c r="AS34">
         <f t="shared" si="12"/>
         <v>15</v>
       </c>
-      <c r="AT34" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU34" s="19" t="s">
+      <c r="AT34" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU34" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="AV34" s="18" t="s">
+      <c r="AV34" t="s">
         <v>177</v>
       </c>
       <c r="AW34">
@@ -6581,10 +6577,10 @@
       <c r="AB35" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AC35" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD35" s="16" t="s">
+      <c r="AC35" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD35" t="s">
         <v>8</v>
       </c>
       <c r="AE35">
@@ -6612,37 +6608,37 @@
       <c r="AL35">
         <v>414</v>
       </c>
-      <c r="AM35" s="17">
+      <c r="AM35" s="1">
         <v>96</v>
       </c>
-      <c r="AN35" s="18">
+      <c r="AN35">
         <v>784</v>
       </c>
-      <c r="AO35" s="18">
+      <c r="AO35">
         <v>384</v>
       </c>
-      <c r="AP35" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ35" s="17">
+      <c r="AP35" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ35" s="1">
         <f t="shared" ref="AQ35" si="14" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ35 - AM35) / 2)</f>
         <v>14</v>
       </c>
-      <c r="AR35" s="18">
+      <c r="AR35">
         <f t="shared" ref="AR35" si="15" xml:space="preserve"> _xlfn.FLOOR.MATH((AK35 - AN35) / 2)</f>
         <v>192</v>
       </c>
-      <c r="AS35" s="18">
+      <c r="AS35">
         <f t="shared" ref="AS35" si="16" xml:space="preserve"> _xlfn.FLOOR.MATH((AL35 - AO35) / 2)</f>
         <v>15</v>
       </c>
-      <c r="AT35" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU35" s="19" t="s">
+      <c r="AT35" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU35" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="AV35" s="18" t="s">
+      <c r="AV35" t="s">
         <v>177</v>
       </c>
       <c r="AW35">

</xml_diff>

<commit_message>
add session to 3dunet excel table
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F34B195-E639-4145-83DA-EB4DEB7D5223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A845925F-82E0-4939-B936-1D4836FC96F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="203">
   <si>
     <t>patch z</t>
   </si>
@@ -628,6 +628,24 @@
   </si>
   <si>
     <t>higher val eval score increase &amp; better val prediction images by increasing train sample size by re-assigning the h5 files to train, val, and test sets (dataset04). Also, fix the job step creation disabled error.</t>
+  </si>
+  <si>
+    <t>failed, #SBATCH commands did not work. job step creation not a problem any more.</t>
+  </si>
+  <si>
+    <t>higher val eval score increase &amp; better val prediction images by increasing train sample size by re-assigning the h5 files to train, val, and test sets (dataset04). Also, fix the #SBATCH commands in the slurm job file (attempt).</t>
+  </si>
+  <si>
+    <t>out of time (default time is 1 minute)</t>
+  </si>
+  <si>
+    <t>230909-1</t>
+  </si>
+  <si>
+    <t>slurmstepd: error: *** JOB 5017703 ON u20-compute-m3 CANCELLED AT 2023-09-09T19:06:39 DUE TO TIME LIMIT ***</t>
+  </si>
+  <si>
+    <t>when I get to it.</t>
   </si>
 </sst>
 </file>
@@ -766,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -785,6 +803,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:AY39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AV22" sqref="AV22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -6505,37 +6524,37 @@
         <v>181</v>
       </c>
       <c r="E35" t="s">
-        <v>131</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G35" t="s">
-        <v>131</v>
+        <v>197</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>131</v>
-      </c>
-      <c r="I35" t="s">
-        <v>131</v>
+        <v>199</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="K35" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="L35" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="M35" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="N35" t="s">
-        <v>131</v>
-      </c>
-      <c r="O35" t="s">
-        <v>131</v>
+        <v>8</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
       </c>
       <c r="P35" s="1" t="s">
         <v>178</v>
@@ -6543,8 +6562,8 @@
       <c r="Q35">
         <v>6</v>
       </c>
-      <c r="R35" t="s">
-        <v>131</v>
+      <c r="R35">
+        <v>6</v>
       </c>
       <c r="S35">
         <v>5</v>
@@ -6651,7 +6670,170 @@
         <v>8</v>
       </c>
     </row>
+    <row r="36" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>200</v>
+      </c>
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="K36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="M36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="N36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="O36" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q36">
+        <v>6</v>
+      </c>
+      <c r="R36" t="s">
+        <v>131</v>
+      </c>
+      <c r="S36">
+        <v>5</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+      <c r="U36">
+        <f t="shared" ref="U36" si="17" xml:space="preserve"> S36 + T36</f>
+        <v>6</v>
+      </c>
+      <c r="V36">
+        <v>1</v>
+      </c>
+      <c r="W36">
+        <v>1</v>
+      </c>
+      <c r="X36">
+        <v>16</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z36">
+        <v>8</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB36" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE36">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AM36*AN36*AO36) / 5 * U36</f>
+        <v>74549.706201272784</v>
+      </c>
+      <c r="AF36" s="1">
+        <v>81920</v>
+      </c>
+      <c r="AG36">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="AH36">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="AI36" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ36" s="10">
+        <v>125</v>
+      </c>
+      <c r="AK36">
+        <v>1169</v>
+      </c>
+      <c r="AL36">
+        <v>414</v>
+      </c>
+      <c r="AM36" s="1">
+        <v>96</v>
+      </c>
+      <c r="AN36">
+        <v>784</v>
+      </c>
+      <c r="AO36">
+        <v>384</v>
+      </c>
+      <c r="AP36" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ36" s="1">
+        <f t="shared" ref="AQ36" si="18" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ36 - AM36) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AR36">
+        <f t="shared" ref="AR36" si="19" xml:space="preserve"> _xlfn.FLOOR.MATH((AK36 - AN36) / 2)</f>
+        <v>192</v>
+      </c>
+      <c r="AS36">
+        <f t="shared" ref="AS36" si="20" xml:space="preserve"> _xlfn.FLOOR.MATH((AL36 - AO36) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AT36" t="s">
+        <v>51</v>
+      </c>
+      <c r="AU36" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="AV36" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW36">
+        <v>1</v>
+      </c>
+      <c r="AX36" t="s">
+        <v>201</v>
+      </c>
+      <c r="AY36" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="39" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>202</v>
+      </c>
       <c r="B39" t="s">
         <v>133</v>
       </c>

</xml_diff>

<commit_message>
prepare another train3dunet job, correct patch shape typo
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A845925F-82E0-4939-B936-1D4836FC96F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CAF7E9-F1D0-4B45-8F8D-916B7E851465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="206">
   <si>
     <t>patch z</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>res. X</t>
-  </si>
-  <si>
-    <t>error</t>
   </si>
   <si>
     <t>AssertionError: datasets should not be an empty iterable</t>
@@ -645,7 +642,19 @@
     <t>slurmstepd: error: *** JOB 5017703 ON u20-compute-m3 CANCELLED AT 2023-09-09T19:06:39 DUE TO TIME LIMIT ***</t>
   </si>
   <si>
-    <t>when I get to it.</t>
+    <t>failed, typo in patch shape: typed 98 instead of 96 in z, resulting in torch error.</t>
+  </si>
+  <si>
+    <t>230910-0</t>
+  </si>
+  <si>
+    <t>higher val eval score increase &amp; better val prediction images by increasing train sample size by re-assigning the h5 files to train, val, and test sets (dataset04). Also, correct patch shape typo in train config yaml.</t>
+  </si>
+  <si>
+    <t>error, invalid patch shape</t>
+  </si>
+  <si>
+    <t>ValueError: requested an output size of torch.Size([49, 192, 392]), but valid sizes range from [47, 191, 391] to [48, 192, 392] (for an input of torch.Size([24, 96, 196]))</t>
   </si>
 </sst>
 </file>
@@ -784,7 +793,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -803,7 +812,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1121,7 +1129,7 @@
   <dimension ref="A1:AY39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1133,8 +1141,8 @@
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
     <col min="6" max="6" width="4.85546875" style="10" customWidth="1"/>
     <col min="7" max="7" width="5.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" customWidth="1"/>
     <col min="16" max="16" width="10.42578125" style="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="9.140625" customWidth="1" outlineLevel="1"/>
@@ -1172,52 +1180,52 @@
   <sheetData>
     <row r="1" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="K1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="P1" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>3</v>
@@ -1226,55 +1234,55 @@
         <v>4</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Y1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="AA1" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AB1" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF1" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="AC1" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>122</v>
-      </c>
       <c r="AG1" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AJ1" s="9" t="s">
         <v>11</v>
@@ -1295,52 +1303,52 @@
         <v>2</v>
       </c>
       <c r="AP1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AQ1" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="AU1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AV1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AW1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="AX1" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="AY1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
         <v>142</v>
       </c>
-      <c r="E2" t="s">
-        <v>143</v>
-      </c>
       <c r="F2" s="10">
         <v>0</v>
       </c>
@@ -1354,7 +1362,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K2" t="s">
         <v>8</v>
@@ -1372,13 +1380,13 @@
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q2">
         <v>5</v>
       </c>
       <c r="R2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S2">
         <v>3</v>
@@ -1400,13 +1408,13 @@
         <v>16</v>
       </c>
       <c r="Y2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z2">
         <v>8</v>
       </c>
       <c r="AA2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB2" s="10">
         <v>0</v>
@@ -1421,7 +1429,7 @@
         <v>8</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AG2" t="s">
         <v>8</v>
@@ -1430,7 +1438,7 @@
         <v>8</v>
       </c>
       <c r="AI2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AJ2" s="10">
         <v>125</v>
@@ -1442,40 +1450,40 @@
         <v>414</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AN2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AO2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AP2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AR2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AS2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AT2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AU2" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AV2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AW2">
         <v>1</v>
       </c>
       <c r="AX2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AY2" t="s">
         <v>8</v>
@@ -1483,19 +1491,19 @@
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
         <v>139</v>
       </c>
-      <c r="B3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" t="s">
-        <v>140</v>
-      </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
@@ -1510,31 +1518,31 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q3">
         <v>5</v>
       </c>
       <c r="R3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S3">
         <v>3</v>
@@ -1556,16 +1564,16 @@
         <v>16</v>
       </c>
       <c r="Y3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z3">
         <v>8</v>
       </c>
       <c r="AA3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AC3" t="s">
         <v>8</v>
@@ -1577,7 +1585,7 @@
         <v>8</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AG3" t="s">
         <v>8</v>
@@ -1586,7 +1594,7 @@
         <v>8</v>
       </c>
       <c r="AI3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AJ3" s="10">
         <v>125</v>
@@ -1598,34 +1606,34 @@
         <v>414</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AN3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AO3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AP3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AQ3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AR3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AS3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AT3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AU3" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AV3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AW3">
         <v>0</v>
@@ -1639,19 +1647,19 @@
     </row>
     <row r="4" spans="1:51" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>134</v>
-      </c>
       <c r="D4" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="13">
         <v>0</v>
@@ -1660,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I4" s="12">
         <v>0</v>
@@ -1684,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q4" s="12">
         <v>5</v>
@@ -1712,16 +1720,16 @@
         <v>16</v>
       </c>
       <c r="Y4" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z4" s="12">
         <v>8</v>
       </c>
       <c r="AA4" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB4" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC4" s="12" t="s">
         <v>8</v>
@@ -1742,7 +1750,7 @@
         <v>8</v>
       </c>
       <c r="AI4" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ4" s="13">
         <v>125</v>
@@ -1763,7 +1771,7 @@
         <v>394</v>
       </c>
       <c r="AP4" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ4" s="14">
         <v>10</v>
@@ -1775,13 +1783,13 @@
         <v>10</v>
       </c>
       <c r="AT4" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU4" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AV4" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AW4" s="12">
         <v>0</v>
@@ -1793,21 +1801,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="10">
         <v>0</v>
@@ -1816,9 +1824,9 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5">
+        <v>85</v>
+      </c>
+      <c r="I5" s="12">
         <v>0</v>
       </c>
       <c r="J5" t="s">
@@ -1840,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q5">
         <v>5</v>
@@ -1868,16 +1876,16 @@
         <v>16</v>
       </c>
       <c r="Y5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z5">
         <v>8</v>
       </c>
       <c r="AA5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB5" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC5" t="s">
         <v>8</v>
@@ -1898,7 +1906,7 @@
         <v>8</v>
       </c>
       <c r="AI5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ5" s="10">
         <v>125</v>
@@ -1919,7 +1927,7 @@
         <v>390</v>
       </c>
       <c r="AP5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ5" s="1">
         <v>10</v>
@@ -1931,13 +1939,13 @@
         <v>10</v>
       </c>
       <c r="AT5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU5" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AV5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AW5">
         <v>0</v>
@@ -1954,16 +1962,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F6" s="10">
         <v>0</v>
@@ -1972,7 +1980,7 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1996,7 +2004,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q6">
         <v>5</v>
@@ -2024,13 +2032,13 @@
         <v>16</v>
       </c>
       <c r="Y6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z6">
         <v>8</v>
       </c>
       <c r="AA6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB6" s="10" t="s">
         <v>8</v>
@@ -2054,7 +2062,7 @@
         <v>8</v>
       </c>
       <c r="AI6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ6" s="10">
         <v>125</v>
@@ -2075,7 +2083,7 @@
         <v>390</v>
       </c>
       <c r="AP6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ6" s="1">
         <v>26</v>
@@ -2087,10 +2095,10 @@
         <v>25</v>
       </c>
       <c r="AT6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AV6" t="s">
         <v>10</v>
@@ -2099,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="AX6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AY6" t="s">
         <v>8</v>
@@ -2107,20 +2115,20 @@
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s">
         <v>89</v>
       </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
-      </c>
       <c r="F7" s="10">
         <v>0</v>
       </c>
@@ -2128,7 +2136,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -2152,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q7">
         <v>5</v>
@@ -2180,13 +2188,13 @@
         <v>16</v>
       </c>
       <c r="Y7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z7">
         <v>8</v>
       </c>
       <c r="AA7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB7" s="10" t="s">
         <v>8</v>
@@ -2210,7 +2218,7 @@
         <v>8</v>
       </c>
       <c r="AI7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ7" s="10">
         <v>125</v>
@@ -2231,7 +2239,7 @@
         <v>390</v>
       </c>
       <c r="AP7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ7" s="1">
         <v>25</v>
@@ -2243,10 +2251,10 @@
         <v>24</v>
       </c>
       <c r="AT7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AV7" t="s">
         <v>9</v>
@@ -2255,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="AX7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AY7" t="s">
         <v>8</v>
@@ -2263,19 +2271,19 @@
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F8" s="10">
         <v>0</v>
@@ -2284,7 +2292,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -2308,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q8">
         <v>5</v>
@@ -2336,16 +2344,16 @@
         <v>16</v>
       </c>
       <c r="Y8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z8">
         <v>8</v>
       </c>
       <c r="AA8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC8" t="s">
         <v>8</v>
@@ -2366,7 +2374,7 @@
         <v>8</v>
       </c>
       <c r="AI8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ8" s="10">
         <v>125</v>
@@ -2387,7 +2395,7 @@
         <v>400</v>
       </c>
       <c r="AP8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ8" s="1">
         <v>12</v>
@@ -2399,19 +2407,19 @@
         <v>7</v>
       </c>
       <c r="AT8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AV8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AW8">
         <v>1</v>
       </c>
       <c r="AX8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AY8" t="s">
         <v>8</v>
@@ -2419,19 +2427,19 @@
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F9" s="10">
         <v>0</v>
@@ -2440,7 +2448,7 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -2464,7 +2472,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q9">
         <v>5</v>
@@ -2492,13 +2500,13 @@
         <v>16</v>
       </c>
       <c r="Y9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z9">
         <v>8</v>
       </c>
       <c r="AA9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB9" s="10" t="s">
         <v>8</v>
@@ -2522,7 +2530,7 @@
         <v>8</v>
       </c>
       <c r="AI9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ9" s="10">
         <v>125</v>
@@ -2546,7 +2554,7 @@
         <v>304</v>
       </c>
       <c r="AP9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ9" s="1">
         <f>(AJ9-AM9)/2</f>
@@ -2561,19 +2569,19 @@
         <v>55</v>
       </c>
       <c r="AT9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW9">
+        <v>1</v>
+      </c>
+      <c r="AX9" t="s">
         <v>25</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW9">
-        <v>1</v>
-      </c>
-      <c r="AX9" t="s">
-        <v>26</v>
       </c>
       <c r="AY9" t="s">
         <v>8</v>
@@ -2581,19 +2589,19 @@
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="10">
         <v>0</v>
@@ -2602,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -2626,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q10">
         <v>5</v>
@@ -2654,13 +2662,13 @@
         <v>16</v>
       </c>
       <c r="Y10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z10">
         <v>8</v>
       </c>
       <c r="AA10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB10" s="10" t="s">
         <v>8</v>
@@ -2684,7 +2692,7 @@
         <v>8</v>
       </c>
       <c r="AI10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ10" s="10">
         <v>125</v>
@@ -2705,7 +2713,7 @@
         <v>304</v>
       </c>
       <c r="AP10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ10" s="1">
         <v>24</v>
@@ -2717,39 +2725,39 @@
         <v>48</v>
       </c>
       <c r="AT10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU10" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AV10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AW10">
         <v>1</v>
       </c>
       <c r="AX10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AY10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F11" s="10">
         <v>0</v>
@@ -2758,7 +2766,7 @@
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -2782,7 +2790,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q11">
         <v>5</v>
@@ -2810,16 +2818,16 @@
         <v>16</v>
       </c>
       <c r="Y11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z11">
         <v>8</v>
       </c>
       <c r="AA11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB11" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC11" t="s">
         <v>8</v>
@@ -2840,7 +2848,7 @@
         <v>8</v>
       </c>
       <c r="AI11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ11" s="10">
         <v>125</v>
@@ -2861,7 +2869,7 @@
         <v>304</v>
       </c>
       <c r="AP11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ11" s="1">
         <v>24</v>
@@ -2873,39 +2881,39 @@
         <v>40</v>
       </c>
       <c r="AT11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU11" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AV11" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW11">
+        <v>1</v>
+      </c>
+      <c r="AX11" t="s">
         <v>31</v>
       </c>
-      <c r="AW11">
-        <v>1</v>
-      </c>
-      <c r="AX11" t="s">
-        <v>32</v>
-      </c>
       <c r="AY11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="10">
         <v>0</v>
@@ -2920,7 +2928,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -2938,7 +2946,7 @@
         <v>1</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q12">
         <v>5</v>
@@ -2966,13 +2974,13 @@
         <v>16</v>
       </c>
       <c r="Y12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z12">
         <v>8</v>
       </c>
       <c r="AA12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB12" s="10">
         <v>10135</v>
@@ -2996,7 +3004,7 @@
         <v>8</v>
       </c>
       <c r="AI12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ12" s="10">
         <v>125</v>
@@ -3017,7 +3025,7 @@
         <v>160</v>
       </c>
       <c r="AP12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ12" s="1">
         <v>24</v>
@@ -3029,13 +3037,13 @@
         <v>120</v>
       </c>
       <c r="AT12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU12" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AV12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AW12">
         <v>0</v>
@@ -3049,19 +3057,19 @@
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="10">
         <v>0</v>
@@ -3070,7 +3078,7 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -3094,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q13">
         <v>5</v>
@@ -3122,13 +3130,13 @@
         <v>16</v>
       </c>
       <c r="Y13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z13">
         <v>8</v>
       </c>
       <c r="AA13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB13" s="10" t="s">
         <v>8</v>
@@ -3152,7 +3160,7 @@
         <v>8</v>
       </c>
       <c r="AI13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ13" s="10">
         <v>125</v>
@@ -3173,7 +3181,7 @@
         <v>168</v>
       </c>
       <c r="AP13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ13" s="1">
         <v>24</v>
@@ -3185,39 +3193,39 @@
         <v>120</v>
       </c>
       <c r="AT13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU13" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AV13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AW13">
         <v>1</v>
       </c>
       <c r="AX13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AY13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
@@ -3226,7 +3234,7 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -3250,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q14">
         <v>5</v>
@@ -3278,13 +3286,13 @@
         <v>16</v>
       </c>
       <c r="Y14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z14">
         <v>8</v>
       </c>
       <c r="AA14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB14" s="10" t="s">
         <v>8</v>
@@ -3308,7 +3316,7 @@
         <v>8</v>
       </c>
       <c r="AI14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ14" s="10">
         <v>125</v>
@@ -3329,7 +3337,7 @@
         <v>168</v>
       </c>
       <c r="AP14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ14" s="1">
         <v>16</v>
@@ -3341,39 +3349,39 @@
         <v>112</v>
       </c>
       <c r="AT14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU14" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AV14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AW14">
         <v>1</v>
       </c>
       <c r="AX14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AY14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" s="10">
         <v>0</v>
@@ -3388,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -3406,7 +3414,7 @@
         <v>1</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q15">
         <v>5</v>
@@ -3434,13 +3442,13 @@
         <v>16</v>
       </c>
       <c r="Y15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z15">
         <v>8</v>
       </c>
       <c r="AA15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB15" s="10">
         <v>13843</v>
@@ -3464,7 +3472,7 @@
         <v>8</v>
       </c>
       <c r="AI15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ15" s="10">
         <v>125</v>
@@ -3485,7 +3493,7 @@
         <v>176</v>
       </c>
       <c r="AP15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ15" s="1">
         <v>8</v>
@@ -3497,13 +3505,13 @@
         <v>104</v>
       </c>
       <c r="AT15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU15" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AV15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AW15">
         <v>0</v>
@@ -3517,19 +3525,19 @@
     </row>
     <row r="16" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="11">
         <v>0</v>
@@ -3544,7 +3552,7 @@
         <v>1</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K16" s="7">
         <v>0</v>
@@ -3562,7 +3570,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q16" s="7">
         <v>5</v>
@@ -3590,13 +3598,13 @@
         <v>16</v>
       </c>
       <c r="Y16" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z16" s="7">
         <v>8</v>
       </c>
       <c r="AA16" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB16" s="11">
         <v>13843</v>
@@ -3620,7 +3628,7 @@
         <v>8</v>
       </c>
       <c r="AI16" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ16" s="11">
         <v>125</v>
@@ -3641,7 +3649,7 @@
         <v>176</v>
       </c>
       <c r="AP16" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ16" s="8">
         <v>16</v>
@@ -3653,13 +3661,13 @@
         <v>112</v>
       </c>
       <c r="AT16" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU16" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV16" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AW16" s="7">
         <v>0</v>
@@ -3673,19 +3681,19 @@
     </row>
     <row r="17" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -3700,7 +3708,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -3718,7 +3726,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q17">
         <v>5</v>
@@ -3746,13 +3754,13 @@
         <v>16</v>
       </c>
       <c r="Y17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z17">
         <v>8</v>
       </c>
       <c r="AA17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB17" s="10">
         <v>10135</v>
@@ -3776,7 +3784,7 @@
         <v>8</v>
       </c>
       <c r="AI17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ17" s="10">
         <v>125</v>
@@ -3797,7 +3805,7 @@
         <v>160</v>
       </c>
       <c r="AP17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ17" s="4">
         <v>8</v>
@@ -3809,13 +3817,13 @@
         <v>96</v>
       </c>
       <c r="AT17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU17" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AW17">
         <v>0</v>
@@ -3829,19 +3837,19 @@
     </row>
     <row r="18" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18" s="10">
         <v>0</v>
@@ -3856,7 +3864,7 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -3874,7 +3882,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q18">
         <v>5</v>
@@ -3902,13 +3910,13 @@
         <v>16</v>
       </c>
       <c r="Y18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z18">
         <v>8</v>
       </c>
       <c r="AA18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB18" s="10">
         <v>10135</v>
@@ -3932,7 +3940,7 @@
         <v>8</v>
       </c>
       <c r="AI18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ18" s="10">
         <v>125</v>
@@ -3953,7 +3961,7 @@
         <v>160</v>
       </c>
       <c r="AP18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ18" s="1">
         <v>24</v>
@@ -3965,13 +3973,13 @@
         <v>120</v>
       </c>
       <c r="AT18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU18" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AW18">
         <v>0</v>
@@ -3985,19 +3993,19 @@
     </row>
     <row r="19" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19" s="10">
         <v>0</v>
@@ -4012,7 +4020,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -4030,7 +4038,7 @@
         <v>1</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q19">
         <v>5</v>
@@ -4058,13 +4066,13 @@
         <v>16</v>
       </c>
       <c r="Y19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z19">
         <v>8</v>
       </c>
       <c r="AA19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB19" s="10">
         <v>10999</v>
@@ -4088,7 +4096,7 @@
         <v>8</v>
       </c>
       <c r="AI19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ19" s="10">
         <v>125</v>
@@ -4109,7 +4117,7 @@
         <v>176</v>
       </c>
       <c r="AP19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ19" s="1">
         <v>24</v>
@@ -4121,13 +4129,13 @@
         <v>112</v>
       </c>
       <c r="AT19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU19" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AW19">
         <v>0</v>
@@ -4141,19 +4149,19 @@
     </row>
     <row r="20" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F20" s="10">
         <v>0</v>
@@ -4168,7 +4176,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -4186,7 +4194,7 @@
         <v>1</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q20">
         <v>5</v>
@@ -4214,13 +4222,13 @@
         <v>16</v>
       </c>
       <c r="Y20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z20">
         <v>8</v>
       </c>
       <c r="AA20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB20" s="10">
         <v>11843</v>
@@ -4244,7 +4252,7 @@
         <v>8</v>
       </c>
       <c r="AI20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ20" s="10">
         <v>125</v>
@@ -4265,7 +4273,7 @@
         <v>192</v>
       </c>
       <c r="AP20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ20" s="1">
         <v>24</v>
@@ -4277,13 +4285,13 @@
         <v>104</v>
       </c>
       <c r="AT20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU20" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AW20">
         <v>0</v>
@@ -4297,19 +4305,19 @@
     </row>
     <row r="21" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F21" s="10">
         <v>0</v>
@@ -4324,7 +4332,7 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -4342,7 +4350,7 @@
         <v>1</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q21">
         <v>5</v>
@@ -4370,13 +4378,13 @@
         <v>16</v>
       </c>
       <c r="Y21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z21">
         <v>8</v>
       </c>
       <c r="AA21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB21" s="10">
         <v>10473</v>
@@ -4400,7 +4408,7 @@
         <v>8</v>
       </c>
       <c r="AI21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ21" s="10">
         <v>125</v>
@@ -4421,7 +4429,7 @@
         <v>160</v>
       </c>
       <c r="AP21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ21" s="1">
         <v>24</v>
@@ -4433,13 +4441,13 @@
         <v>120</v>
       </c>
       <c r="AT21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU21" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AW21">
         <v>0</v>
@@ -4453,19 +4461,19 @@
     </row>
     <row r="22" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" s="10">
         <v>0</v>
@@ -4480,7 +4488,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -4498,7 +4506,7 @@
         <v>1</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q22">
         <v>5</v>
@@ -4526,13 +4534,13 @@
         <v>16</v>
       </c>
       <c r="Y22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z22">
         <v>8</v>
       </c>
       <c r="AA22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB22" s="10">
         <v>10825</v>
@@ -4556,7 +4564,7 @@
         <v>8</v>
       </c>
       <c r="AI22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ22" s="10">
         <v>125</v>
@@ -4577,7 +4585,7 @@
         <v>160</v>
       </c>
       <c r="AP22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ22" s="1">
         <v>24</v>
@@ -4589,13 +4597,13 @@
         <v>120</v>
       </c>
       <c r="AT22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU22" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AW22">
         <v>0</v>
@@ -4609,19 +4617,19 @@
     </row>
     <row r="23" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" s="10">
         <v>0</v>
@@ -4636,7 +4644,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -4654,7 +4662,7 @@
         <v>1</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q23">
         <v>5</v>
@@ -4682,13 +4690,13 @@
         <v>16</v>
       </c>
       <c r="Y23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z23">
         <v>8</v>
       </c>
       <c r="AA23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB23" s="10">
         <v>12317</v>
@@ -4712,7 +4720,7 @@
         <v>8</v>
       </c>
       <c r="AI23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ23" s="10">
         <v>125</v>
@@ -4733,7 +4741,7 @@
         <v>160</v>
       </c>
       <c r="AP23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ23" s="1">
         <v>16</v>
@@ -4745,13 +4753,13 @@
         <v>120</v>
       </c>
       <c r="AT23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU23" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AW23">
         <v>0</v>
@@ -4765,19 +4773,19 @@
     </row>
     <row r="24" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F24" s="10">
         <v>0</v>
@@ -4792,7 +4800,7 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -4810,7 +4818,7 @@
         <v>1</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q24">
         <v>5</v>
@@ -4838,13 +4846,13 @@
         <v>16</v>
       </c>
       <c r="Y24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z24">
         <v>8</v>
       </c>
       <c r="AA24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB24" s="10">
         <v>14443</v>
@@ -4868,7 +4876,7 @@
         <v>8</v>
       </c>
       <c r="AI24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AJ24" s="10">
         <v>125</v>
@@ -4889,7 +4897,7 @@
         <v>160</v>
       </c>
       <c r="AP24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ24" s="1">
         <v>8</v>
@@ -4901,13 +4909,13 @@
         <v>120</v>
       </c>
       <c r="AT24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU24" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AW24">
         <v>0</v>
@@ -4921,7 +4929,7 @@
     </row>
     <row r="25" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -4930,10 +4938,10 @@
         <v>8</v>
       </c>
       <c r="D25" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" t="s">
         <v>108</v>
-      </c>
-      <c r="E25" t="s">
-        <v>109</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>8</v>
@@ -5076,7 +5084,7 @@
     </row>
     <row r="26" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>8</v>
@@ -5085,10 +5093,10 @@
         <v>8</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>8</v>
@@ -5231,19 +5239,19 @@
     </row>
     <row r="27" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F27" s="10">
         <v>0</v>
@@ -5258,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -5276,7 +5284,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q27">
         <v>5</v>
@@ -5304,16 +5312,16 @@
         <v>16</v>
       </c>
       <c r="Y27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z27">
         <v>8</v>
       </c>
       <c r="AA27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB27" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AC27" t="s">
         <v>8</v>
@@ -5335,7 +5343,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ27" s="10">
         <v>125</v>
@@ -5356,7 +5364,7 @@
         <v>400</v>
       </c>
       <c r="AP27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ27" s="1">
         <f t="shared" ref="AQ27:AQ34" si="3" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ27 - AM27) / 2)</f>
@@ -5371,13 +5379,13 @@
         <v>7</v>
       </c>
       <c r="AT27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU27" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW27">
         <v>0</v>
@@ -5391,19 +5399,19 @@
     </row>
     <row r="28" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F28" s="10">
         <v>0</v>
@@ -5412,7 +5420,7 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -5436,7 +5444,7 @@
         <v>0</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q28">
         <v>5</v>
@@ -5464,16 +5472,16 @@
         <v>16</v>
       </c>
       <c r="Y28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z28">
         <v>8</v>
       </c>
       <c r="AA28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB28" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AC28">
         <v>82032.639999999999</v>
@@ -5496,7 +5504,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ28" s="10">
         <v>125</v>
@@ -5517,7 +5525,7 @@
         <v>400</v>
       </c>
       <c r="AP28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ28" s="1">
         <f t="shared" si="3"/>
@@ -5532,39 +5540,39 @@
         <v>7</v>
       </c>
       <c r="AT28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU28" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AV28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW28">
         <v>1</v>
       </c>
       <c r="AX28" t="s">
+        <v>115</v>
+      </c>
+      <c r="AY28" t="s">
         <v>116</v>
-      </c>
-      <c r="AY28" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F29" s="10">
         <v>0</v>
@@ -5573,7 +5581,7 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -5597,7 +5605,7 @@
         <v>1</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q29">
         <v>5</v>
@@ -5625,13 +5633,13 @@
         <v>16</v>
       </c>
       <c r="Y29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z29">
         <v>8</v>
       </c>
       <c r="AA29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB29" s="10">
         <v>77887</v>
@@ -5656,7 +5664,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ29" s="10">
         <v>125</v>
@@ -5677,7 +5685,7 @@
         <v>400</v>
       </c>
       <c r="AP29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ29" s="1">
         <f t="shared" si="3"/>
@@ -5692,13 +5700,13 @@
         <v>7</v>
       </c>
       <c r="AT29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU29" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW29">
         <v>0</v>
@@ -5712,20 +5720,20 @@
     </row>
     <row r="30" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C30" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" t="s">
+        <v>162</v>
+      </c>
+      <c r="E30" t="s">
         <v>167</v>
       </c>
-      <c r="D30" t="s">
-        <v>163</v>
-      </c>
-      <c r="E30" t="s">
-        <v>168</v>
-      </c>
       <c r="F30" s="10">
         <v>0</v>
       </c>
@@ -5739,7 +5747,7 @@
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -5757,7 +5765,7 @@
         <v>1</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q30">
         <v>5</v>
@@ -5785,13 +5793,13 @@
         <v>16</v>
       </c>
       <c r="Y30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z30">
         <v>8</v>
       </c>
       <c r="AA30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB30" s="10">
         <v>77885</v>
@@ -5816,7 +5824,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI30" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ30" s="10">
         <v>125</v>
@@ -5837,7 +5845,7 @@
         <v>400</v>
       </c>
       <c r="AP30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ30" s="1">
         <f t="shared" si="3"/>
@@ -5852,13 +5860,13 @@
         <v>7</v>
       </c>
       <c r="AT30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU30" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW30">
         <v>0</v>
@@ -5872,19 +5880,19 @@
     </row>
     <row r="31" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
+        <v>159</v>
+      </c>
+      <c r="D31" t="s">
         <v>160</v>
       </c>
-      <c r="D31" t="s">
-        <v>161</v>
-      </c>
       <c r="E31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F31" s="10">
         <v>0</v>
@@ -5893,7 +5901,7 @@
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -5917,7 +5925,7 @@
         <v>1</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q31">
         <v>5</v>
@@ -5945,13 +5953,13 @@
         <v>16</v>
       </c>
       <c r="Y31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z31">
         <v>8</v>
       </c>
       <c r="AA31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB31" s="10">
         <v>78017</v>
@@ -5976,7 +5984,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ31" s="10">
         <v>125</v>
@@ -5997,7 +6005,7 @@
         <v>400</v>
       </c>
       <c r="AP31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ31" s="1">
         <f t="shared" si="3"/>
@@ -6012,13 +6020,13 @@
         <v>7</v>
       </c>
       <c r="AT31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU31" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW31">
         <v>0</v>
@@ -6032,19 +6040,19 @@
     </row>
     <row r="32" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" t="s">
         <v>169</v>
       </c>
-      <c r="B32" t="s">
-        <v>133</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>170</v>
       </c>
-      <c r="D32" t="s">
-        <v>171</v>
-      </c>
       <c r="E32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F32" s="10">
         <v>0</v>
@@ -6059,7 +6067,7 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -6077,7 +6085,7 @@
         <v>1</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q32">
         <v>5</v>
@@ -6105,16 +6113,16 @@
         <v>16</v>
       </c>
       <c r="Y32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z32">
         <v>8</v>
       </c>
       <c r="AA32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB32" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AC32" t="s">
         <v>8</v>
@@ -6136,7 +6144,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ32" s="10">
         <v>125</v>
@@ -6157,7 +6165,7 @@
         <v>400</v>
       </c>
       <c r="AP32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ32" s="1">
         <f t="shared" si="3"/>
@@ -6172,13 +6180,13 @@
         <v>7</v>
       </c>
       <c r="AT32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU32" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW32">
         <v>0</v>
@@ -6192,20 +6200,20 @@
     </row>
     <row r="33" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
+        <v>185</v>
+      </c>
+      <c r="D33" t="s">
         <v>186</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>187</v>
       </c>
-      <c r="E33" t="s">
-        <v>188</v>
-      </c>
       <c r="F33" s="10">
         <v>0</v>
       </c>
@@ -6213,7 +6221,7 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -6237,7 +6245,7 @@
         <v>0</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q33">
         <v>6</v>
@@ -6265,16 +6273,16 @@
         <v>16</v>
       </c>
       <c r="Y33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z33">
         <v>8</v>
       </c>
       <c r="AA33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB33" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AC33" t="s">
         <v>8</v>
@@ -6296,7 +6304,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ33" s="10">
         <v>125</v>
@@ -6317,7 +6325,7 @@
         <v>400</v>
       </c>
       <c r="AP33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ33" s="1">
         <f t="shared" si="3"/>
@@ -6332,19 +6340,19 @@
         <v>7</v>
       </c>
       <c r="AT33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU33" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW33">
         <v>1</v>
       </c>
       <c r="AX33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AY33" t="s">
         <v>8</v>
@@ -6352,19 +6360,19 @@
     </row>
     <row r="34" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s">
+        <v>179</v>
+      </c>
+      <c r="D34" t="s">
         <v>180</v>
       </c>
-      <c r="D34" t="s">
-        <v>181</v>
-      </c>
       <c r="E34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F34" s="10">
         <v>0</v>
@@ -6379,7 +6387,7 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K34" t="s">
         <v>8</v>
@@ -6397,7 +6405,7 @@
         <v>0</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q34">
         <v>6</v>
@@ -6425,13 +6433,13 @@
         <v>16</v>
       </c>
       <c r="Y34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z34">
         <v>8</v>
       </c>
       <c r="AA34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB34" s="10" t="s">
         <v>8</v>
@@ -6456,7 +6464,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ34" s="10">
         <v>125</v>
@@ -6477,7 +6485,7 @@
         <v>384</v>
       </c>
       <c r="AP34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ34" s="1">
         <f t="shared" si="3"/>
@@ -6492,19 +6500,19 @@
         <v>15</v>
       </c>
       <c r="AT34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU34" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW34">
         <v>1</v>
       </c>
       <c r="AX34" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AY34" t="s">
         <v>8</v>
@@ -6512,20 +6520,20 @@
     </row>
     <row r="35" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" t="s">
         <v>195</v>
       </c>
-      <c r="B35" t="s">
-        <v>133</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>180</v>
+      </c>
+      <c r="E35" t="s">
         <v>196</v>
       </c>
-      <c r="D35" t="s">
-        <v>181</v>
-      </c>
-      <c r="E35" t="s">
-        <v>197</v>
-      </c>
       <c r="F35" s="10">
         <v>0</v>
       </c>
@@ -6533,7 +6541,7 @@
         <v>1</v>
       </c>
       <c r="H35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -6557,7 +6565,7 @@
         <v>0</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q35">
         <v>6</v>
@@ -6585,13 +6593,13 @@
         <v>16</v>
       </c>
       <c r="Y35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z35">
         <v>8</v>
       </c>
       <c r="AA35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB35" s="10" t="s">
         <v>8</v>
@@ -6616,7 +6624,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ35" s="10">
         <v>125</v>
@@ -6637,7 +6645,7 @@
         <v>384</v>
       </c>
       <c r="AP35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ35" s="1">
         <f t="shared" ref="AQ35" si="14" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ35 - AM35) / 2)</f>
@@ -6652,19 +6660,19 @@
         <v>15</v>
       </c>
       <c r="AT35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU35" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AW35">
         <v>1</v>
       </c>
       <c r="AX35" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="AY35" t="s">
         <v>8</v>
@@ -6672,58 +6680,58 @@
     </row>
     <row r="36" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E36" t="s">
-        <v>131</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="K36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="M36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="N36" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="O36" s="16" t="s">
-        <v>131</v>
+        <v>201</v>
+      </c>
+      <c r="F36" s="10">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>204</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" t="s">
+        <v>8</v>
+      </c>
+      <c r="L36" t="s">
+        <v>8</v>
+      </c>
+      <c r="M36" t="s">
+        <v>8</v>
+      </c>
+      <c r="N36" t="s">
+        <v>8</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="Q36">
         <v>6</v>
       </c>
-      <c r="R36" t="s">
-        <v>131</v>
+      <c r="R36">
+        <v>6</v>
       </c>
       <c r="S36">
         <v>5</v>
@@ -6745,16 +6753,16 @@
         <v>16</v>
       </c>
       <c r="Y36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z36">
         <v>8</v>
       </c>
       <c r="AA36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB36" s="10" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="AC36" t="s">
         <v>8</v>
@@ -6764,7 +6772,7 @@
       </c>
       <c r="AE36">
         <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AM36*AN36*AO36) / 5 * U36</f>
-        <v>74549.706201272784</v>
+        <v>76071.407048528155</v>
       </c>
       <c r="AF36" s="1">
         <v>81920</v>
@@ -6776,7 +6784,7 @@
         <v>79.150000000000006</v>
       </c>
       <c r="AI36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AJ36" s="10">
         <v>125</v>
@@ -6788,7 +6796,7 @@
         <v>414</v>
       </c>
       <c r="AM36" s="1">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="AN36">
         <v>784</v>
@@ -6797,11 +6805,11 @@
         <v>384</v>
       </c>
       <c r="AP36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AQ36" s="1">
         <f t="shared" ref="AQ36" si="18" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ36 - AM36) / 2)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AR36">
         <f t="shared" ref="AR36" si="19" xml:space="preserve"> _xlfn.FLOOR.MATH((AK36 - AN36) / 2)</f>
@@ -6812,39 +6820,196 @@
         <v>15</v>
       </c>
       <c r="AT36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AU36" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AV36" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW36">
+        <v>1</v>
+      </c>
+      <c r="AX36" t="s">
+        <v>205</v>
+      </c>
+      <c r="AY36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>202</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" t="s">
+        <v>203</v>
+      </c>
+      <c r="D37" t="s">
+        <v>180</v>
+      </c>
+      <c r="E37" t="s">
+        <v>130</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H37" t="s">
+        <v>130</v>
+      </c>
+      <c r="I37" t="s">
+        <v>130</v>
+      </c>
+      <c r="J37" t="s">
+        <v>130</v>
+      </c>
+      <c r="K37" t="s">
+        <v>130</v>
+      </c>
+      <c r="L37" t="s">
+        <v>130</v>
+      </c>
+      <c r="M37" t="s">
+        <v>130</v>
+      </c>
+      <c r="N37" t="s">
+        <v>130</v>
+      </c>
+      <c r="O37" t="s">
+        <v>130</v>
+      </c>
+      <c r="P37" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="AW36">
-        <v>1</v>
-      </c>
-      <c r="AX36" t="s">
-        <v>201</v>
-      </c>
-      <c r="AY36" t="s">
-        <v>8</v>
+      <c r="Q37">
+        <v>6</v>
+      </c>
+      <c r="R37" t="s">
+        <v>130</v>
+      </c>
+      <c r="S37">
+        <v>5</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <f t="shared" ref="U37" si="21" xml:space="preserve"> S37 + T37</f>
+        <v>6</v>
+      </c>
+      <c r="V37">
+        <v>1</v>
+      </c>
+      <c r="W37">
+        <v>1</v>
+      </c>
+      <c r="X37">
+        <v>16</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z37">
+        <v>8</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB37" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE37">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AM37*AN37*AO37) / 5 * U37</f>
+        <v>74549.706201272784</v>
+      </c>
+      <c r="AF37" s="1">
+        <v>81920</v>
+      </c>
+      <c r="AG37">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="AH37">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="AI37" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ37" s="10">
+        <v>125</v>
+      </c>
+      <c r="AK37">
+        <v>1169</v>
+      </c>
+      <c r="AL37">
+        <v>414</v>
+      </c>
+      <c r="AM37" s="1">
+        <v>96</v>
+      </c>
+      <c r="AN37">
+        <v>784</v>
+      </c>
+      <c r="AO37">
+        <v>384</v>
+      </c>
+      <c r="AP37" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ37" s="1">
+        <f t="shared" ref="AQ37" si="22" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ37 - AM37) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AR37">
+        <f t="shared" ref="AR37" si="23" xml:space="preserve"> _xlfn.FLOOR.MATH((AK37 - AN37) / 2)</f>
+        <v>192</v>
+      </c>
+      <c r="AS37">
+        <f t="shared" ref="AS37" si="24" xml:space="preserve"> _xlfn.FLOOR.MATH((AL37 - AO37) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AT37" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU37" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV37" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW37" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX37" t="s">
+        <v>130</v>
+      </c>
+      <c r="AY37" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>202</v>
-      </c>
       <c r="B39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
+        <v>181</v>
+      </c>
+      <c r="D39" t="s">
         <v>182</v>
       </c>
-      <c r="D39" t="s">
-        <v>183</v>
-      </c>
       <c r="E39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepare another slurm train3dunet session
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81977EC6-2E5E-4802-A991-67A8932D2A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBB6B3A-368F-4553-9A7A-E389F78DC641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="211">
   <si>
     <t>patch z</t>
   </si>
@@ -655,6 +655,21 @@
   </si>
   <si>
     <t>ValueError: requested an output size of torch.Size([49, 192, 392]), but valid sizes range from [47, 191, 391] to [48, 192, 392] (for an input of torch.Size([24, 96, 196]))</t>
+  </si>
+  <si>
+    <t>error, out of memory</t>
+  </si>
+  <si>
+    <t>failed, slurmstepd: out of memory</t>
+  </si>
+  <si>
+    <t>230910-1</t>
+  </si>
+  <si>
+    <t>higher val eval score increase &amp; better val prediction images by increasing train sample size by re-assigning the h5 files to train, val, and test sets (dataset04). Also, give more main memory in sbatch flags.</t>
+  </si>
+  <si>
+    <t>slurmstepd: error: Detected 2 oom-kill event(s) in StepId=5017888.batch. Some of your processes may have been killed by the cgroup out-of-memory handler.</t>
   </si>
 </sst>
 </file>
@@ -1126,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:AY39"/>
+  <dimension ref="A1:AY44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -6221,7 +6236,7 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>85</v>
+        <v>206</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -6852,37 +6867,37 @@
         <v>180</v>
       </c>
       <c r="E37" t="s">
-        <v>130</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37" t="s">
-        <v>130</v>
+        <v>207</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>130</v>
-      </c>
-      <c r="I37" t="s">
-        <v>130</v>
+        <v>206</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
       </c>
       <c r="J37" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="K37" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="L37" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="M37" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="N37" t="s">
-        <v>130</v>
-      </c>
-      <c r="O37" t="s">
-        <v>130</v>
+        <v>8</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>177</v>
@@ -6890,8 +6905,8 @@
       <c r="Q37">
         <v>6</v>
       </c>
-      <c r="R37" t="s">
-        <v>130</v>
+      <c r="R37">
+        <v>6</v>
       </c>
       <c r="S37">
         <v>5</v>
@@ -6922,7 +6937,7 @@
         <v>102</v>
       </c>
       <c r="AB37" s="10" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="AC37" t="s">
         <v>8</v>
@@ -6988,27 +7003,187 @@
       <c r="AV37" t="s">
         <v>176</v>
       </c>
-      <c r="AW37" t="s">
+      <c r="AW37">
+        <v>1</v>
+      </c>
+      <c r="AX37" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38" t="s">
+        <v>209</v>
+      </c>
+      <c r="D38" t="s">
+        <v>180</v>
+      </c>
+      <c r="E38" t="s">
         <v>130</v>
       </c>
-      <c r="AX37" t="s">
+      <c r="F38" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="AY37" t="s">
+      <c r="G38" t="s">
         <v>130</v>
       </c>
+      <c r="H38" t="s">
+        <v>130</v>
+      </c>
+      <c r="I38" t="s">
+        <v>130</v>
+      </c>
+      <c r="J38" t="s">
+        <v>130</v>
+      </c>
+      <c r="K38" t="s">
+        <v>130</v>
+      </c>
+      <c r="L38" t="s">
+        <v>130</v>
+      </c>
+      <c r="M38" t="s">
+        <v>130</v>
+      </c>
+      <c r="N38" t="s">
+        <v>130</v>
+      </c>
+      <c r="O38" t="s">
+        <v>130</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q38">
+        <v>6</v>
+      </c>
+      <c r="R38" t="s">
+        <v>130</v>
+      </c>
+      <c r="S38">
+        <v>5</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <f t="shared" ref="U38" si="25" xml:space="preserve"> S38 + T38</f>
+        <v>6</v>
+      </c>
+      <c r="V38">
+        <v>1</v>
+      </c>
+      <c r="W38">
+        <v>1</v>
+      </c>
+      <c r="X38">
+        <v>16</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z38">
+        <v>8</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB38" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE38">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AM38*AN38*AO38) / 5 * U38</f>
+        <v>74549.706201272784</v>
+      </c>
+      <c r="AF38" s="1">
+        <v>81920</v>
+      </c>
+      <c r="AG38">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="AH38">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="AI38" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ38" s="10">
+        <v>125</v>
+      </c>
+      <c r="AK38">
+        <v>1169</v>
+      </c>
+      <c r="AL38">
+        <v>414</v>
+      </c>
+      <c r="AM38" s="1">
+        <v>96</v>
+      </c>
+      <c r="AN38">
+        <v>784</v>
+      </c>
+      <c r="AO38">
+        <v>384</v>
+      </c>
+      <c r="AP38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ38" s="1">
+        <f t="shared" ref="AQ38" si="26" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ38 - AM38) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AR38">
+        <f t="shared" ref="AR38" si="27" xml:space="preserve"> _xlfn.FLOOR.MATH((AK38 - AN38) / 2)</f>
+        <v>192</v>
+      </c>
+      <c r="AS38">
+        <f t="shared" ref="AS38" si="28" xml:space="preserve"> _xlfn.FLOOR.MATH((AL38 - AO38) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AT38" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU38" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV38" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW38" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX38" t="s">
+        <v>130</v>
+      </c>
+      <c r="AY38" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>132</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C44" t="s">
         <v>181</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D44" t="s">
         <v>182</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E44" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare another train3dunet slurm job
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBB6B3A-368F-4553-9A7A-E389F78DC641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AB4E47-ED6D-44FC-AC39-05673627174F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="215">
   <si>
     <t>patch z</t>
   </si>
@@ -670,6 +670,18 @@
   </si>
   <si>
     <t>slurmstepd: error: Detected 2 oom-kill event(s) in StepId=5017888.batch. Some of your processes may have been killed by the cgroup out-of-memory handler.</t>
+  </si>
+  <si>
+    <t>230910-2</t>
+  </si>
+  <si>
+    <t>higher val eval score increase &amp; better val prediction images by increasing train sample size by re-assigning the h5 files to train, val, and test sets (dataset04). Also, try to fix nvidia-smi logs not being written.</t>
+  </si>
+  <si>
+    <t>aborted, nvidia-smi logs are not writing.</t>
+  </si>
+  <si>
+    <t>nvidia-smi logs are not writing.</t>
   </si>
 </sst>
 </file>
@@ -1143,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:AY44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -7027,37 +7039,37 @@
         <v>180</v>
       </c>
       <c r="E38" t="s">
-        <v>130</v>
-      </c>
-      <c r="F38" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G38" t="s">
-        <v>130</v>
+        <v>213</v>
+      </c>
+      <c r="F38" s="10">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
       </c>
       <c r="H38" t="s">
-        <v>130</v>
-      </c>
-      <c r="I38" t="s">
-        <v>130</v>
+        <v>8</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="K38" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="L38" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="M38" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="N38" t="s">
-        <v>130</v>
-      </c>
-      <c r="O38" t="s">
-        <v>130</v>
+        <v>8</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>177</v>
@@ -7065,8 +7077,8 @@
       <c r="Q38">
         <v>6</v>
       </c>
-      <c r="R38" t="s">
-        <v>130</v>
+      <c r="R38">
+        <v>6</v>
       </c>
       <c r="S38">
         <v>5</v>
@@ -7097,7 +7109,7 @@
         <v>102</v>
       </c>
       <c r="AB38" s="10" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="AC38" t="s">
         <v>8</v>
@@ -7163,13 +7175,173 @@
       <c r="AV38" t="s">
         <v>176</v>
       </c>
-      <c r="AW38" t="s">
+      <c r="AW38">
+        <v>0</v>
+      </c>
+      <c r="AX38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>211</v>
+      </c>
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" t="s">
+        <v>212</v>
+      </c>
+      <c r="D39" t="s">
+        <v>180</v>
+      </c>
+      <c r="E39" t="s">
         <v>130</v>
       </c>
-      <c r="AX38" t="s">
+      <c r="F39" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="AY38" t="s">
+      <c r="G39" t="s">
+        <v>130</v>
+      </c>
+      <c r="H39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I39" t="s">
+        <v>130</v>
+      </c>
+      <c r="J39" t="s">
+        <v>130</v>
+      </c>
+      <c r="K39" t="s">
+        <v>130</v>
+      </c>
+      <c r="L39" t="s">
+        <v>130</v>
+      </c>
+      <c r="M39" t="s">
+        <v>130</v>
+      </c>
+      <c r="N39" t="s">
+        <v>130</v>
+      </c>
+      <c r="O39" t="s">
+        <v>130</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q39">
+        <v>6</v>
+      </c>
+      <c r="R39" t="s">
+        <v>130</v>
+      </c>
+      <c r="S39">
+        <v>5</v>
+      </c>
+      <c r="T39">
+        <v>1</v>
+      </c>
+      <c r="U39">
+        <f t="shared" ref="U39" si="29" xml:space="preserve"> S39 + T39</f>
+        <v>6</v>
+      </c>
+      <c r="V39">
+        <v>1</v>
+      </c>
+      <c r="W39">
+        <v>1</v>
+      </c>
+      <c r="X39">
+        <v>16</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z39">
+        <v>8</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB39" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD39" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE39">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AM39*AN39*AO39) / 5 * U39</f>
+        <v>74549.706201272784</v>
+      </c>
+      <c r="AF39" s="1">
+        <v>81920</v>
+      </c>
+      <c r="AG39">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="AH39">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ39" s="10">
+        <v>125</v>
+      </c>
+      <c r="AK39">
+        <v>1169</v>
+      </c>
+      <c r="AL39">
+        <v>414</v>
+      </c>
+      <c r="AM39" s="1">
+        <v>96</v>
+      </c>
+      <c r="AN39">
+        <v>784</v>
+      </c>
+      <c r="AO39">
+        <v>384</v>
+      </c>
+      <c r="AP39" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ39" s="1">
+        <f t="shared" ref="AQ39" si="30" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ39 - AM39) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AR39">
+        <f t="shared" ref="AR39" si="31" xml:space="preserve"> _xlfn.FLOOR.MATH((AK39 - AN39) / 2)</f>
+        <v>192</v>
+      </c>
+      <c r="AS39">
+        <f t="shared" ref="AS39" si="32" xml:space="preserve"> _xlfn.FLOOR.MATH((AL39 - AO39) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AT39" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU39" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV39" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW39" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX39" t="s">
+        <v>130</v>
+      </c>
+      <c r="AY39" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prep another train3dunet run, nvidia-smi logs keep not writing...
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AB4E47-ED6D-44FC-AC39-05673627174F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A5B4D2-9019-4A5D-988D-572404187AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="218">
   <si>
     <t>patch z</t>
   </si>
@@ -682,6 +682,15 @@
   </si>
   <si>
     <t>nvidia-smi logs are not writing.</t>
+  </si>
+  <si>
+    <t>230910-3</t>
+  </si>
+  <si>
+    <t>230910-4</t>
+  </si>
+  <si>
+    <t>aborted, nvidia-smi logs are not writing. But there is enough memory, now.</t>
   </si>
 </sst>
 </file>
@@ -1155,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:AY44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -7199,37 +7208,37 @@
         <v>180</v>
       </c>
       <c r="E39" t="s">
-        <v>130</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G39" t="s">
-        <v>130</v>
+        <v>213</v>
+      </c>
+      <c r="F39" s="10">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>130</v>
-      </c>
-      <c r="I39" t="s">
-        <v>130</v>
+        <v>8</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="K39" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="L39" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="M39" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="N39" t="s">
-        <v>130</v>
-      </c>
-      <c r="O39" t="s">
-        <v>130</v>
+        <v>8</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
       </c>
       <c r="P39" s="1" t="s">
         <v>177</v>
@@ -7237,8 +7246,8 @@
       <c r="Q39">
         <v>6</v>
       </c>
-      <c r="R39" t="s">
-        <v>130</v>
+      <c r="R39">
+        <v>6</v>
       </c>
       <c r="S39">
         <v>5</v>
@@ -7269,7 +7278,7 @@
         <v>102</v>
       </c>
       <c r="AB39" s="10" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="AC39" t="s">
         <v>8</v>
@@ -7335,13 +7344,333 @@
       <c r="AV39" t="s">
         <v>176</v>
       </c>
-      <c r="AW39" t="s">
+      <c r="AW39">
+        <v>0</v>
+      </c>
+      <c r="AX39" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>215</v>
+      </c>
+      <c r="B40" t="s">
+        <v>132</v>
+      </c>
+      <c r="C40" t="s">
+        <v>212</v>
+      </c>
+      <c r="D40" t="s">
+        <v>180</v>
+      </c>
+      <c r="E40" t="s">
+        <v>217</v>
+      </c>
+      <c r="F40" s="10">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>214</v>
+      </c>
+      <c r="K40" t="s">
+        <v>8</v>
+      </c>
+      <c r="L40" t="s">
+        <v>8</v>
+      </c>
+      <c r="M40" t="s">
+        <v>8</v>
+      </c>
+      <c r="N40" t="s">
+        <v>8</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q40">
+        <v>6</v>
+      </c>
+      <c r="R40">
+        <v>6</v>
+      </c>
+      <c r="S40">
+        <v>5</v>
+      </c>
+      <c r="T40">
+        <v>1</v>
+      </c>
+      <c r="U40">
+        <f t="shared" ref="U40" si="33" xml:space="preserve"> S40 + T40</f>
+        <v>6</v>
+      </c>
+      <c r="V40">
+        <v>1</v>
+      </c>
+      <c r="W40">
+        <v>1</v>
+      </c>
+      <c r="X40">
+        <v>16</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z40">
+        <v>8</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB40" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE40">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AM40*AN40*AO40) / 5 * U40</f>
+        <v>74549.706201272784</v>
+      </c>
+      <c r="AF40" s="1">
+        <v>81920</v>
+      </c>
+      <c r="AG40">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="AH40">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="AI40" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ40" s="10">
+        <v>125</v>
+      </c>
+      <c r="AK40">
+        <v>1169</v>
+      </c>
+      <c r="AL40">
+        <v>414</v>
+      </c>
+      <c r="AM40" s="1">
+        <v>96</v>
+      </c>
+      <c r="AN40">
+        <v>784</v>
+      </c>
+      <c r="AO40">
+        <v>384</v>
+      </c>
+      <c r="AP40" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ40" s="1">
+        <f t="shared" ref="AQ40" si="34" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ40 - AM40) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AR40">
+        <f t="shared" ref="AR40" si="35" xml:space="preserve"> _xlfn.FLOOR.MATH((AK40 - AN40) / 2)</f>
+        <v>192</v>
+      </c>
+      <c r="AS40">
+        <f t="shared" ref="AS40" si="36" xml:space="preserve"> _xlfn.FLOOR.MATH((AL40 - AO40) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AT40" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU40" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW40">
+        <v>0</v>
+      </c>
+      <c r="AX40" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" t="s">
+        <v>180</v>
+      </c>
+      <c r="E41" t="s">
         <v>130</v>
       </c>
-      <c r="AX39" t="s">
+      <c r="F41" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="AY39" t="s">
+      <c r="G41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H41" t="s">
+        <v>130</v>
+      </c>
+      <c r="I41" t="s">
+        <v>130</v>
+      </c>
+      <c r="J41" t="s">
+        <v>130</v>
+      </c>
+      <c r="K41" t="s">
+        <v>130</v>
+      </c>
+      <c r="L41" t="s">
+        <v>130</v>
+      </c>
+      <c r="M41" t="s">
+        <v>130</v>
+      </c>
+      <c r="N41" t="s">
+        <v>130</v>
+      </c>
+      <c r="O41" t="s">
+        <v>130</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q41">
+        <v>6</v>
+      </c>
+      <c r="R41" t="s">
+        <v>130</v>
+      </c>
+      <c r="S41">
+        <v>5</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <f t="shared" ref="U41" si="37" xml:space="preserve"> S41 + T41</f>
+        <v>6</v>
+      </c>
+      <c r="V41">
+        <v>1</v>
+      </c>
+      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="X41">
+        <v>16</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z41">
+        <v>8</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB41" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE41">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AM41*AN41*AO41) / 5 * U41</f>
+        <v>74549.706201272784</v>
+      </c>
+      <c r="AF41" s="1">
+        <v>81920</v>
+      </c>
+      <c r="AG41">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="AH41">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="AI41" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ41" s="10">
+        <v>125</v>
+      </c>
+      <c r="AK41">
+        <v>1169</v>
+      </c>
+      <c r="AL41">
+        <v>414</v>
+      </c>
+      <c r="AM41" s="1">
+        <v>96</v>
+      </c>
+      <c r="AN41">
+        <v>784</v>
+      </c>
+      <c r="AO41">
+        <v>384</v>
+      </c>
+      <c r="AP41" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ41" s="1">
+        <f t="shared" ref="AQ41" si="38" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ41 - AM41) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AR41">
+        <f t="shared" ref="AR41" si="39" xml:space="preserve"> _xlfn.FLOOR.MATH((AK41 - AN41) / 2)</f>
+        <v>192</v>
+      </c>
+      <c r="AS41">
+        <f t="shared" ref="AS41" si="40" xml:space="preserve"> _xlfn.FLOOR.MATH((AL41 - AO41) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AT41" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU41" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV41" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW41" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX41" t="s">
+        <v>130</v>
+      </c>
+      <c r="AY41" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prep longer train3dunet session
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE2295E-21AD-4EE7-81C1-DD3B9900F3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA977D2D-7C6A-432E-89A6-FE1EC4108B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="228">
   <si>
     <t>patch z</t>
   </si>
@@ -709,6 +709,18 @@
   </si>
   <si>
     <t>(TBD wait till finish) running, nvidia-smi logs are being written. Needs a `cd ~/data/cloud; bash pull-script.sh`.</t>
+  </si>
+  <si>
+    <t>230911-0</t>
+  </si>
+  <si>
+    <t>eval scores will plateau marginally higher. I think the problem is the sample size being just too small.</t>
+  </si>
+  <si>
+    <t>230911-1</t>
+  </si>
+  <si>
+    <t>higher patience, lower val frequency, let it run for longer (e.g. 72 instead of the usual 24 hours) dataset03/04, maybe the eval score will go up eventually</t>
   </si>
 </sst>
 </file>
@@ -1182,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:AY48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB43" sqref="AB43"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -8028,20 +8040,20 @@
       <c r="E44" t="s">
         <v>223</v>
       </c>
-      <c r="F44" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G44" t="s">
-        <v>130</v>
+      <c r="F44" s="10">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>130</v>
-      </c>
-      <c r="I44" t="s">
-        <v>130</v>
+        <v>8</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="K44" t="s">
         <v>130</v>
@@ -8169,6 +8181,326 @@
         <v>130</v>
       </c>
       <c r="AY44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>224</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" t="s">
+        <v>227</v>
+      </c>
+      <c r="D45" t="s">
+        <v>225</v>
+      </c>
+      <c r="E45" t="s">
+        <v>130</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G45" t="s">
+        <v>130</v>
+      </c>
+      <c r="H45" t="s">
+        <v>130</v>
+      </c>
+      <c r="I45" t="s">
+        <v>130</v>
+      </c>
+      <c r="J45" t="s">
+        <v>130</v>
+      </c>
+      <c r="K45" t="s">
+        <v>130</v>
+      </c>
+      <c r="L45" t="s">
+        <v>130</v>
+      </c>
+      <c r="M45" t="s">
+        <v>130</v>
+      </c>
+      <c r="N45" t="s">
+        <v>130</v>
+      </c>
+      <c r="O45" t="s">
+        <v>130</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q45">
+        <v>6</v>
+      </c>
+      <c r="R45">
+        <v>6</v>
+      </c>
+      <c r="S45">
+        <v>5</v>
+      </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
+      <c r="U45">
+        <f t="shared" ref="U45" si="55" xml:space="preserve"> S45 + T45</f>
+        <v>6</v>
+      </c>
+      <c r="V45">
+        <v>1</v>
+      </c>
+      <c r="W45">
+        <v>1</v>
+      </c>
+      <c r="X45">
+        <v>16</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z45">
+        <v>8</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB45" s="10">
+        <v>74967</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD45" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE45">
+        <f t="shared" ref="AE45" si="56" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AM45*AN45*AO45) / 5 * U45</f>
+        <v>74549.706201272784</v>
+      </c>
+      <c r="AF45" s="1">
+        <v>81920</v>
+      </c>
+      <c r="AG45">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="AH45">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="AI45" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ45" s="10">
+        <v>125</v>
+      </c>
+      <c r="AK45">
+        <v>1169</v>
+      </c>
+      <c r="AL45">
+        <v>414</v>
+      </c>
+      <c r="AM45" s="1">
+        <v>96</v>
+      </c>
+      <c r="AN45">
+        <v>784</v>
+      </c>
+      <c r="AO45">
+        <v>384</v>
+      </c>
+      <c r="AP45" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ45" s="1">
+        <f t="shared" ref="AQ45" si="57" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ45 - AM45) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AR45">
+        <f t="shared" ref="AR45" si="58" xml:space="preserve"> _xlfn.FLOOR.MATH((AK45 - AN45) / 2)</f>
+        <v>192</v>
+      </c>
+      <c r="AS45">
+        <f t="shared" ref="AS45" si="59" xml:space="preserve"> _xlfn.FLOOR.MATH((AL45 - AO45) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AT45" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU45" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV45" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW45" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX45" t="s">
+        <v>130</v>
+      </c>
+      <c r="AY45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>226</v>
+      </c>
+      <c r="B46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" t="s">
+        <v>130</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H46" t="s">
+        <v>130</v>
+      </c>
+      <c r="I46" t="s">
+        <v>130</v>
+      </c>
+      <c r="J46" t="s">
+        <v>130</v>
+      </c>
+      <c r="K46" t="s">
+        <v>130</v>
+      </c>
+      <c r="L46" t="s">
+        <v>130</v>
+      </c>
+      <c r="M46" t="s">
+        <v>130</v>
+      </c>
+      <c r="N46" t="s">
+        <v>130</v>
+      </c>
+      <c r="O46" t="s">
+        <v>130</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q46">
+        <v>6</v>
+      </c>
+      <c r="R46">
+        <v>6</v>
+      </c>
+      <c r="S46">
+        <v>5</v>
+      </c>
+      <c r="T46">
+        <v>1</v>
+      </c>
+      <c r="U46">
+        <f t="shared" ref="U46" si="60" xml:space="preserve"> S46 + T46</f>
+        <v>6</v>
+      </c>
+      <c r="V46">
+        <v>1</v>
+      </c>
+      <c r="W46">
+        <v>1</v>
+      </c>
+      <c r="X46">
+        <v>16</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z46">
+        <v>8</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB46" s="10">
+        <v>74967</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE46">
+        <f t="shared" ref="AE46" si="61" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AM46*AN46*AO46) / 5 * U46</f>
+        <v>74549.706201272784</v>
+      </c>
+      <c r="AF46" s="1">
+        <v>81920</v>
+      </c>
+      <c r="AG46">
+        <v>81049.600000000006</v>
+      </c>
+      <c r="AH46">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="AI46" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ46" s="10">
+        <v>125</v>
+      </c>
+      <c r="AK46">
+        <v>1169</v>
+      </c>
+      <c r="AL46">
+        <v>414</v>
+      </c>
+      <c r="AM46" s="1">
+        <v>96</v>
+      </c>
+      <c r="AN46">
+        <v>784</v>
+      </c>
+      <c r="AO46">
+        <v>384</v>
+      </c>
+      <c r="AP46" t="s">
+        <v>50</v>
+      </c>
+      <c r="AQ46" s="1">
+        <f t="shared" ref="AQ46" si="62" xml:space="preserve"> _xlfn.FLOOR.MATH((AJ46 - AM46) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AR46">
+        <f t="shared" ref="AR46" si="63" xml:space="preserve"> _xlfn.FLOOR.MATH((AK46 - AN46) / 2)</f>
+        <v>192</v>
+      </c>
+      <c r="AS46">
+        <f t="shared" ref="AS46" si="64" xml:space="preserve"> _xlfn.FLOOR.MATH((AL46 - AO46) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AT46" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU46" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="AV46" t="s">
+        <v>176</v>
+      </c>
+      <c r="AW46" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX46" t="s">
+        <v>130</v>
+      </c>
+      <c r="AY46" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
start cloud comp work after: finish creating dataset06 (all dataset06.x)
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F12854F-9503-4618-A348-BB74DB8BD537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4127893C-12E3-4026-B6D4-7AC4598C12FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1345" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="272">
   <si>
     <t>patch z</t>
   </si>
@@ -1006,7 +1006,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1029,6 +1029,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1345,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BA69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="X8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AL32" sqref="AL32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1378,7 +1379,7 @@
     <col min="31" max="33" width="9.140625" customWidth="1"/>
     <col min="34" max="34" width="7.28515625" style="1" customWidth="1" outlineLevel="1"/>
     <col min="35" max="36" width="7.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="23.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="37" width="26.28515625" customWidth="1" outlineLevel="1"/>
     <col min="38" max="38" width="6" style="10" bestFit="1" customWidth="1"/>
     <col min="39" max="40" width="6" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="5.28515625" style="1" customWidth="1"/>
@@ -8666,7 +8667,7 @@
         <v>1</v>
       </c>
       <c r="U45" s="7">
-        <f t="shared" ref="U45" si="54" xml:space="preserve"> S45 + T45</f>
+        <f t="shared" ref="U45:U46" si="54" xml:space="preserve"> S45 + T45</f>
         <v>6</v>
       </c>
       <c r="V45" s="7" t="s">
@@ -8782,6 +8783,67 @@
       </c>
       <c r="P46" s="1" t="s">
         <v>248</v>
+      </c>
+      <c r="Q46" s="18">
+        <v>6</v>
+      </c>
+      <c r="R46" t="s">
+        <v>130</v>
+      </c>
+      <c r="S46" s="18">
+        <v>5</v>
+      </c>
+      <c r="T46" s="18">
+        <v>1</v>
+      </c>
+      <c r="U46" s="18">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V46" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="W46" s="18">
+        <v>3</v>
+      </c>
+      <c r="X46" s="18">
+        <v>16</v>
+      </c>
+      <c r="Y46" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z46" s="18">
+        <v>1</v>
+      </c>
+      <c r="AA46" s="18">
+        <v>8</v>
+      </c>
+      <c r="AB46" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC46" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD46" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE46" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF46" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH46" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI46" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ46" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK46" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:53" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
complete vram study prep: new VRAM pred formula, all a priori knowledge filled in table; Sat 13:00:32 30.09.2023
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4127893C-12E3-4026-B6D4-7AC4598C12FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4004801-FDF5-4100-BDA7-4907FED6A80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="274">
   <si>
     <t>patch z</t>
   </si>
@@ -801,58 +801,64 @@
     <t>dataset06.5</t>
   </si>
   <si>
-    <t>230928-0</t>
-  </si>
-  <si>
-    <t>230928-1</t>
-  </si>
-  <si>
-    <t>230928-2</t>
-  </si>
-  <si>
-    <t>230928-3</t>
-  </si>
-  <si>
-    <t>230928-4</t>
-  </si>
-  <si>
-    <t>230928-5</t>
-  </si>
-  <si>
-    <t>230928-6</t>
-  </si>
-  <si>
-    <t>230928-7</t>
-  </si>
-  <si>
-    <t>230928-8</t>
-  </si>
-  <si>
-    <t>230928-9</t>
-  </si>
-  <si>
-    <t>230928-10</t>
-  </si>
-  <si>
-    <t>230928-11</t>
-  </si>
-  <si>
-    <t>230928-12</t>
-  </si>
-  <si>
-    <t>230928-13</t>
-  </si>
-  <si>
-    <t>230928-14</t>
-  </si>
-  <si>
-    <t>230928-15</t>
-  </si>
-  <si>
-    <t>230928-16</t>
-  </si>
-  <si>
-    <t>230928-17</t>
+    <t>patch = arbitrary even int_2^3 chosen previously when maxing out (one) A100</t>
+  </si>
+  <si>
+    <t>patch = arbitrary even int_2^3 smaller than most previous run</t>
+  </si>
+  <si>
+    <t>230930-0</t>
+  </si>
+  <si>
+    <t>230930-1</t>
+  </si>
+  <si>
+    <t>230930-2</t>
+  </si>
+  <si>
+    <t>230930-3</t>
+  </si>
+  <si>
+    <t>230930-4</t>
+  </si>
+  <si>
+    <t>230930-5</t>
+  </si>
+  <si>
+    <t>230930-6</t>
+  </si>
+  <si>
+    <t>230930-7</t>
+  </si>
+  <si>
+    <t>230930-8</t>
+  </si>
+  <si>
+    <t>230930-9</t>
+  </si>
+  <si>
+    <t>230930-10</t>
+  </si>
+  <si>
+    <t>230930-11</t>
+  </si>
+  <si>
+    <t>230930-12</t>
+  </si>
+  <si>
+    <t>230930-13</t>
+  </si>
+  <si>
+    <t>230930-14</t>
+  </si>
+  <si>
+    <t>230930-15</t>
+  </si>
+  <si>
+    <t>230930-16</t>
+  </si>
+  <si>
+    <t>230930-17</t>
   </si>
 </sst>
 </file>
@@ -1346,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BA69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL32" sqref="AL32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1368,7 @@
     <col min="8" max="8" width="30.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="1" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="12.85546875" style="1" bestFit="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="9.140625" customWidth="1" outlineLevel="1"/>
     <col min="19" max="19" width="6.7109375" customWidth="1" outlineLevel="1"/>
     <col min="20" max="20" width="5.140625" customWidth="1" outlineLevel="1"/>
@@ -1389,7 +1395,7 @@
     <col min="46" max="46" width="6.5703125" customWidth="1"/>
     <col min="47" max="47" width="5" customWidth="1"/>
     <col min="48" max="48" width="6" customWidth="1"/>
-    <col min="49" max="49" width="34.28515625" style="10" customWidth="1"/>
+    <col min="49" max="49" width="74.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="74.42578125" customWidth="1"/>
     <col min="51" max="51" width="5.140625" customWidth="1"/>
     <col min="52" max="52" width="73.85546875" customWidth="1"/>
@@ -8667,7 +8673,7 @@
         <v>1</v>
       </c>
       <c r="U45" s="7">
-        <f t="shared" ref="U45:U46" si="54" xml:space="preserve"> S45 + T45</f>
+        <f t="shared" ref="U45:U63" si="54" xml:space="preserve"> S45 + T45</f>
         <v>6</v>
       </c>
       <c r="V45" s="7" t="s">
@@ -8772,8 +8778,8 @@
       </c>
     </row>
     <row r="46" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>254</v>
+      <c r="A46" s="17" t="s">
+        <v>256</v>
       </c>
       <c r="B46" t="s">
         <v>132</v>
@@ -8781,74 +8787,159 @@
       <c r="C46" s="17" t="s">
         <v>230</v>
       </c>
+      <c r="F46" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G46" t="s">
+        <v>130</v>
+      </c>
+      <c r="H46" t="s">
+        <v>130</v>
+      </c>
+      <c r="I46" t="s">
+        <v>130</v>
+      </c>
+      <c r="J46" t="s">
+        <v>130</v>
+      </c>
+      <c r="K46" t="s">
+        <v>130</v>
+      </c>
+      <c r="L46" t="s">
+        <v>130</v>
+      </c>
+      <c r="M46" t="s">
+        <v>130</v>
+      </c>
+      <c r="N46" t="s">
+        <v>130</v>
+      </c>
+      <c r="O46" t="s">
+        <v>130</v>
+      </c>
       <c r="P46" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="Q46" s="18">
+      <c r="Q46">
         <v>6</v>
       </c>
       <c r="R46" t="s">
         <v>130</v>
       </c>
-      <c r="S46" s="18">
+      <c r="S46">
         <v>5</v>
       </c>
-      <c r="T46" s="18">
-        <v>1</v>
-      </c>
-      <c r="U46" s="18">
+      <c r="T46">
+        <v>1</v>
+      </c>
+      <c r="U46">
         <f t="shared" si="54"/>
         <v>6</v>
       </c>
-      <c r="V46" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="W46" s="18">
+      <c r="V46" t="s">
+        <v>8</v>
+      </c>
+      <c r="W46">
         <v>3</v>
       </c>
-      <c r="X46" s="18">
+      <c r="X46">
         <v>16</v>
       </c>
-      <c r="Y46" s="18" t="s">
+      <c r="Y46" t="s">
         <v>100</v>
       </c>
-      <c r="Z46" s="18">
-        <v>1</v>
-      </c>
-      <c r="AA46" s="18">
-        <v>8</v>
-      </c>
-      <c r="AB46" s="18" t="s">
+      <c r="Z46">
+        <v>1</v>
+      </c>
+      <c r="AA46">
+        <v>8</v>
+      </c>
+      <c r="AB46" t="s">
         <v>102</v>
       </c>
       <c r="AC46" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD46" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="AE46" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF46" s="18" t="s">
-        <v>8</v>
+        <v>130</v>
+      </c>
+      <c r="AD46" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG46">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO46*AP46*AQ46) * ((W46*X46 + Z46*AA46) / (3*16 + 1*8)) * (U46 / 5)</f>
+        <v>74549.706201272769</v>
       </c>
       <c r="AH46" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AI46" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ46" s="18" t="s">
-        <v>8</v>
+        <v>130</v>
+      </c>
+      <c r="AI46" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ46" t="s">
+        <v>130</v>
       </c>
       <c r="AK46" t="s">
         <v>111</v>
       </c>
+      <c r="AL46" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM46" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN46" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO46" s="1">
+        <v>96</v>
+      </c>
+      <c r="AP46">
+        <v>784</v>
+      </c>
+      <c r="AQ46">
+        <v>384</v>
+      </c>
+      <c r="AR46" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS46" s="1">
+        <f t="shared" ref="AS46:AS47" si="58" xml:space="preserve"> _xlfn.FLOOR.MATH((AL46 - AO46) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AT46">
+        <f t="shared" ref="AT46:AT47" si="59" xml:space="preserve"> _xlfn.FLOOR.MATH((AM46 - AP46) / 2)</f>
+        <v>192</v>
+      </c>
+      <c r="AU46">
+        <f t="shared" ref="AU46:AU47" si="60" xml:space="preserve"> _xlfn.FLOOR.MATH((AN46 - AQ46) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AV46" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW46" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="AX46" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY46" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ46" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA46" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="47" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>255</v>
+      <c r="A47" s="17" t="s">
+        <v>257</v>
       </c>
       <c r="B47" t="s">
         <v>132</v>
@@ -8856,13 +8947,159 @@
       <c r="C47" s="17" t="s">
         <v>231</v>
       </c>
+      <c r="F47" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G47" t="s">
+        <v>130</v>
+      </c>
+      <c r="H47" t="s">
+        <v>130</v>
+      </c>
+      <c r="I47" t="s">
+        <v>130</v>
+      </c>
+      <c r="J47" t="s">
+        <v>130</v>
+      </c>
+      <c r="K47" t="s">
+        <v>130</v>
+      </c>
+      <c r="L47" t="s">
+        <v>130</v>
+      </c>
+      <c r="M47" t="s">
+        <v>130</v>
+      </c>
+      <c r="N47" t="s">
+        <v>130</v>
+      </c>
+      <c r="O47" t="s">
+        <v>130</v>
+      </c>
       <c r="P47" s="1" t="s">
         <v>248</v>
       </c>
+      <c r="Q47">
+        <v>6</v>
+      </c>
+      <c r="R47" t="s">
+        <v>130</v>
+      </c>
+      <c r="S47">
+        <v>5</v>
+      </c>
+      <c r="T47">
+        <v>1</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V47" t="s">
+        <v>8</v>
+      </c>
+      <c r="W47">
+        <v>3</v>
+      </c>
+      <c r="X47">
+        <v>16</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z47">
+        <v>1</v>
+      </c>
+      <c r="AA47">
+        <v>8</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC47" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD47" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG47">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO47*AP47*AQ47) * ((W47*X47 + Z47*AA47) / (3*16 + 1*8)) * (U47 / 5)</f>
+        <v>22708.360330151121</v>
+      </c>
+      <c r="AH47" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI47" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK47" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL47" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM47" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN47" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO47" s="1">
+        <v>64</v>
+      </c>
+      <c r="AP47" s="18">
+        <v>512</v>
+      </c>
+      <c r="AQ47" s="18">
+        <v>256</v>
+      </c>
+      <c r="AR47" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS47" s="1">
+        <f t="shared" si="58"/>
+        <v>30</v>
+      </c>
+      <c r="AT47">
+        <f t="shared" si="59"/>
+        <v>328</v>
+      </c>
+      <c r="AU47">
+        <f t="shared" si="60"/>
+        <v>79</v>
+      </c>
+      <c r="AV47" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW47" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX47" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY47" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ47" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA47" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="48" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>256</v>
+      <c r="A48" s="17" t="s">
+        <v>258</v>
       </c>
       <c r="B48" t="s">
         <v>132</v>
@@ -8870,13 +9107,159 @@
       <c r="C48" s="17" t="s">
         <v>232</v>
       </c>
+      <c r="F48" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G48" t="s">
+        <v>130</v>
+      </c>
+      <c r="H48" t="s">
+        <v>130</v>
+      </c>
+      <c r="I48" t="s">
+        <v>130</v>
+      </c>
+      <c r="J48" t="s">
+        <v>130</v>
+      </c>
+      <c r="K48" t="s">
+        <v>130</v>
+      </c>
+      <c r="L48" t="s">
+        <v>130</v>
+      </c>
+      <c r="M48" t="s">
+        <v>130</v>
+      </c>
+      <c r="N48" t="s">
+        <v>130</v>
+      </c>
+      <c r="O48" t="s">
+        <v>130</v>
+      </c>
       <c r="P48" s="1" t="s">
         <v>248</v>
       </c>
+      <c r="Q48">
+        <v>6</v>
+      </c>
+      <c r="R48" t="s">
+        <v>130</v>
+      </c>
+      <c r="S48">
+        <v>5</v>
+      </c>
+      <c r="T48">
+        <v>1</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V48" t="s">
+        <v>8</v>
+      </c>
+      <c r="W48">
+        <v>3</v>
+      </c>
+      <c r="X48">
+        <v>16</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z48">
+        <v>1</v>
+      </c>
+      <c r="AA48">
+        <v>8</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC48" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD48" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG48">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO48*AP48*AQ48) * ((W48*X48 + Z48*AA48) / (3*16 + 1*8)) * (U48 / 5)</f>
+        <v>4158.1023826571118</v>
+      </c>
+      <c r="AH48" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI48" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ48" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK48" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL48" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM48" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN48" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO48" s="1">
+        <v>32</v>
+      </c>
+      <c r="AP48" s="18">
+        <v>256</v>
+      </c>
+      <c r="AQ48" s="18">
+        <v>128</v>
+      </c>
+      <c r="AR48" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS48" s="1">
+        <f t="shared" ref="AS48:AS63" si="61" xml:space="preserve"> _xlfn.FLOOR.MATH((AL48 - AO48) / 2)</f>
+        <v>46</v>
+      </c>
+      <c r="AT48">
+        <f t="shared" ref="AT48:AT63" si="62" xml:space="preserve"> _xlfn.FLOOR.MATH((AM48 - AP48) / 2)</f>
+        <v>456</v>
+      </c>
+      <c r="AU48">
+        <f t="shared" ref="AU48:AU63" si="63" xml:space="preserve"> _xlfn.FLOOR.MATH((AN48 - AQ48) / 2)</f>
+        <v>143</v>
+      </c>
+      <c r="AV48" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW48" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX48" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY48" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ48" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA48" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>257</v>
+    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>259</v>
       </c>
       <c r="B49" t="s">
         <v>132</v>
@@ -8884,13 +9267,159 @@
       <c r="C49" s="17" t="s">
         <v>233</v>
       </c>
+      <c r="F49" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G49" t="s">
+        <v>130</v>
+      </c>
+      <c r="H49" t="s">
+        <v>130</v>
+      </c>
+      <c r="I49" t="s">
+        <v>130</v>
+      </c>
+      <c r="J49" t="s">
+        <v>130</v>
+      </c>
+      <c r="K49" t="s">
+        <v>130</v>
+      </c>
+      <c r="L49" t="s">
+        <v>130</v>
+      </c>
+      <c r="M49" t="s">
+        <v>130</v>
+      </c>
+      <c r="N49" t="s">
+        <v>130</v>
+      </c>
+      <c r="O49" t="s">
+        <v>130</v>
+      </c>
       <c r="P49" s="1" t="s">
         <v>249</v>
       </c>
+      <c r="Q49">
+        <v>6</v>
+      </c>
+      <c r="R49" t="s">
+        <v>130</v>
+      </c>
+      <c r="S49">
+        <v>5</v>
+      </c>
+      <c r="T49">
+        <v>1</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V49" t="s">
+        <v>8</v>
+      </c>
+      <c r="W49">
+        <v>2</v>
+      </c>
+      <c r="X49">
+        <v>16</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z49">
+        <v>1</v>
+      </c>
+      <c r="AA49">
+        <v>8</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC49" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG49">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO49*AP49*AQ49) * ((W49*X49 + Z49*AA49) / (3*16 + 1*8)) * (U49 / 5)</f>
+        <v>53680.666010342022</v>
+      </c>
+      <c r="AH49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI49" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ49" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK49" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL49" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM49" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN49" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO49" s="1">
+        <v>96</v>
+      </c>
+      <c r="AP49">
+        <v>784</v>
+      </c>
+      <c r="AQ49">
+        <v>384</v>
+      </c>
+      <c r="AR49" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS49" s="1">
+        <f t="shared" si="61"/>
+        <v>14</v>
+      </c>
+      <c r="AT49">
+        <f t="shared" si="62"/>
+        <v>192</v>
+      </c>
+      <c r="AU49">
+        <f t="shared" si="63"/>
+        <v>15</v>
+      </c>
+      <c r="AV49" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW49" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="AX49" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY49" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ49" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA49" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>258</v>
+    <row r="50" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>260</v>
       </c>
       <c r="B50" t="s">
         <v>132</v>
@@ -8898,13 +9427,159 @@
       <c r="C50" s="17" t="s">
         <v>234</v>
       </c>
+      <c r="F50" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G50" t="s">
+        <v>130</v>
+      </c>
+      <c r="H50" t="s">
+        <v>130</v>
+      </c>
+      <c r="I50" t="s">
+        <v>130</v>
+      </c>
+      <c r="J50" t="s">
+        <v>130</v>
+      </c>
+      <c r="K50" t="s">
+        <v>130</v>
+      </c>
+      <c r="L50" t="s">
+        <v>130</v>
+      </c>
+      <c r="M50" t="s">
+        <v>130</v>
+      </c>
+      <c r="N50" t="s">
+        <v>130</v>
+      </c>
+      <c r="O50" t="s">
+        <v>130</v>
+      </c>
       <c r="P50" s="1" t="s">
         <v>249</v>
       </c>
+      <c r="Q50">
+        <v>6</v>
+      </c>
+      <c r="R50" t="s">
+        <v>130</v>
+      </c>
+      <c r="S50">
+        <v>5</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V50" t="s">
+        <v>8</v>
+      </c>
+      <c r="W50">
+        <v>2</v>
+      </c>
+      <c r="X50">
+        <v>16</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z50">
+        <v>1</v>
+      </c>
+      <c r="AA50">
+        <v>8</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC50" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG50">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO50*AP50*AQ50) * ((W50*X50 + Z50*AA50) / (3*16 + 1*8)) * (U50 / 5)</f>
+        <v>16651.133245255118</v>
+      </c>
+      <c r="AH50" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI50" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ50" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK50" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL50" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM50" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN50" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO50" s="1">
+        <v>64</v>
+      </c>
+      <c r="AP50" s="18">
+        <v>512</v>
+      </c>
+      <c r="AQ50" s="18">
+        <v>256</v>
+      </c>
+      <c r="AR50" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS50" s="1">
+        <f t="shared" si="61"/>
+        <v>30</v>
+      </c>
+      <c r="AT50">
+        <f t="shared" si="62"/>
+        <v>328</v>
+      </c>
+      <c r="AU50">
+        <f t="shared" si="63"/>
+        <v>79</v>
+      </c>
+      <c r="AV50" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW50" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX50" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY50" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ50" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA50" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>259</v>
+    <row r="51" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>261</v>
       </c>
       <c r="B51" t="s">
         <v>132</v>
@@ -8912,13 +9587,159 @@
       <c r="C51" s="17" t="s">
         <v>235</v>
       </c>
+      <c r="F51" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G51" t="s">
+        <v>130</v>
+      </c>
+      <c r="H51" t="s">
+        <v>130</v>
+      </c>
+      <c r="I51" t="s">
+        <v>130</v>
+      </c>
+      <c r="J51" t="s">
+        <v>130</v>
+      </c>
+      <c r="K51" t="s">
+        <v>130</v>
+      </c>
+      <c r="L51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M51" t="s">
+        <v>130</v>
+      </c>
+      <c r="N51" t="s">
+        <v>130</v>
+      </c>
+      <c r="O51" t="s">
+        <v>130</v>
+      </c>
       <c r="P51" s="1" t="s">
         <v>249</v>
       </c>
+      <c r="Q51">
+        <v>6</v>
+      </c>
+      <c r="R51" t="s">
+        <v>130</v>
+      </c>
+      <c r="S51">
+        <v>5</v>
+      </c>
+      <c r="T51">
+        <v>1</v>
+      </c>
+      <c r="U51">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V51" t="s">
+        <v>8</v>
+      </c>
+      <c r="W51">
+        <v>2</v>
+      </c>
+      <c r="X51">
+        <v>16</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z51">
+        <v>1</v>
+      </c>
+      <c r="AA51">
+        <v>8</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC51" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG51">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO51*AP51*AQ51) * ((W51*X51 + Z51*AA51) / (3*16 + 1*8)) * (U51 / 5)</f>
+        <v>3400.9489970451114</v>
+      </c>
+      <c r="AH51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI51" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ51" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK51" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL51" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM51" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN51" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO51" s="1">
+        <v>32</v>
+      </c>
+      <c r="AP51" s="18">
+        <v>256</v>
+      </c>
+      <c r="AQ51" s="18">
+        <v>128</v>
+      </c>
+      <c r="AR51" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS51" s="1">
+        <f t="shared" si="61"/>
+        <v>46</v>
+      </c>
+      <c r="AT51">
+        <f t="shared" si="62"/>
+        <v>456</v>
+      </c>
+      <c r="AU51">
+        <f t="shared" si="63"/>
+        <v>143</v>
+      </c>
+      <c r="AV51" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW51" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX51" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY51" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ51" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA51" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>260</v>
+    <row r="52" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>262</v>
       </c>
       <c r="B52" t="s">
         <v>132</v>
@@ -8926,13 +9747,159 @@
       <c r="C52" s="17" t="s">
         <v>236</v>
       </c>
+      <c r="F52" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G52" t="s">
+        <v>130</v>
+      </c>
+      <c r="H52" t="s">
+        <v>130</v>
+      </c>
+      <c r="I52" t="s">
+        <v>130</v>
+      </c>
+      <c r="J52" t="s">
+        <v>130</v>
+      </c>
+      <c r="K52" t="s">
+        <v>130</v>
+      </c>
+      <c r="L52" t="s">
+        <v>130</v>
+      </c>
+      <c r="M52" t="s">
+        <v>130</v>
+      </c>
+      <c r="N52" t="s">
+        <v>130</v>
+      </c>
+      <c r="O52" t="s">
+        <v>130</v>
+      </c>
       <c r="P52" s="1" t="s">
         <v>250</v>
       </c>
+      <c r="Q52">
+        <v>6</v>
+      </c>
+      <c r="R52" t="s">
+        <v>130</v>
+      </c>
+      <c r="S52">
+        <v>5</v>
+      </c>
+      <c r="T52">
+        <v>1</v>
+      </c>
+      <c r="U52">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V52" t="s">
+        <v>8</v>
+      </c>
+      <c r="W52">
+        <v>1</v>
+      </c>
+      <c r="X52">
+        <v>16</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z52">
+        <v>1</v>
+      </c>
+      <c r="AA52">
+        <v>8</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC52" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG52">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO52*AP52*AQ52) * ((W52*X52 + Z52*AA52) / (3*16 + 1*8)) * (U52 / 5)</f>
+        <v>32811.625819411252</v>
+      </c>
+      <c r="AH52" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI52" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ52" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK52" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL52" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM52" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN52" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO52" s="1">
+        <v>96</v>
+      </c>
+      <c r="AP52">
+        <v>784</v>
+      </c>
+      <c r="AQ52">
+        <v>384</v>
+      </c>
+      <c r="AR52" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS52" s="1">
+        <f t="shared" si="61"/>
+        <v>14</v>
+      </c>
+      <c r="AT52">
+        <f t="shared" si="62"/>
+        <v>192</v>
+      </c>
+      <c r="AU52">
+        <f t="shared" si="63"/>
+        <v>15</v>
+      </c>
+      <c r="AV52" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW52" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="AX52" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY52" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ52" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA52" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>261</v>
+    <row r="53" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>263</v>
       </c>
       <c r="B53" t="s">
         <v>132</v>
@@ -8940,13 +9907,159 @@
       <c r="C53" s="17" t="s">
         <v>237</v>
       </c>
+      <c r="F53" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G53" t="s">
+        <v>130</v>
+      </c>
+      <c r="H53" t="s">
+        <v>130</v>
+      </c>
+      <c r="I53" t="s">
+        <v>130</v>
+      </c>
+      <c r="J53" t="s">
+        <v>130</v>
+      </c>
+      <c r="K53" t="s">
+        <v>130</v>
+      </c>
+      <c r="L53" t="s">
+        <v>130</v>
+      </c>
+      <c r="M53" t="s">
+        <v>130</v>
+      </c>
+      <c r="N53" t="s">
+        <v>130</v>
+      </c>
+      <c r="O53" t="s">
+        <v>130</v>
+      </c>
       <c r="P53" s="1" t="s">
         <v>250</v>
       </c>
+      <c r="Q53">
+        <v>6</v>
+      </c>
+      <c r="R53" t="s">
+        <v>130</v>
+      </c>
+      <c r="S53">
+        <v>5</v>
+      </c>
+      <c r="T53">
+        <v>1</v>
+      </c>
+      <c r="U53">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V53" t="s">
+        <v>8</v>
+      </c>
+      <c r="W53">
+        <v>1</v>
+      </c>
+      <c r="X53">
+        <v>16</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z53">
+        <v>1</v>
+      </c>
+      <c r="AA53">
+        <v>8</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC53" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF53" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG53">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO53*AP53*AQ53) * ((W53*X53 + Z53*AA53) / (3*16 + 1*8)) * (U53 / 5)</f>
+        <v>10593.906160359114</v>
+      </c>
+      <c r="AH53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI53" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ53" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK53" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL53" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM53" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN53" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO53" s="1">
+        <v>64</v>
+      </c>
+      <c r="AP53" s="18">
+        <v>512</v>
+      </c>
+      <c r="AQ53" s="18">
+        <v>256</v>
+      </c>
+      <c r="AR53" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS53" s="1">
+        <f t="shared" si="61"/>
+        <v>30</v>
+      </c>
+      <c r="AT53">
+        <f t="shared" si="62"/>
+        <v>328</v>
+      </c>
+      <c r="AU53">
+        <f t="shared" si="63"/>
+        <v>79</v>
+      </c>
+      <c r="AV53" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW53" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX53" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY53" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ53" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA53" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>262</v>
+    <row r="54" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
+        <v>264</v>
       </c>
       <c r="B54" t="s">
         <v>132</v>
@@ -8954,13 +10067,159 @@
       <c r="C54" s="17" t="s">
         <v>238</v>
       </c>
+      <c r="F54" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G54" t="s">
+        <v>130</v>
+      </c>
+      <c r="H54" t="s">
+        <v>130</v>
+      </c>
+      <c r="I54" t="s">
+        <v>130</v>
+      </c>
+      <c r="J54" t="s">
+        <v>130</v>
+      </c>
+      <c r="K54" t="s">
+        <v>130</v>
+      </c>
+      <c r="L54" t="s">
+        <v>130</v>
+      </c>
+      <c r="M54" t="s">
+        <v>130</v>
+      </c>
+      <c r="N54" t="s">
+        <v>130</v>
+      </c>
+      <c r="O54" t="s">
+        <v>130</v>
+      </c>
       <c r="P54" s="1" t="s">
         <v>250</v>
       </c>
+      <c r="Q54">
+        <v>6</v>
+      </c>
+      <c r="R54" t="s">
+        <v>130</v>
+      </c>
+      <c r="S54">
+        <v>5</v>
+      </c>
+      <c r="T54">
+        <v>1</v>
+      </c>
+      <c r="U54">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V54" t="s">
+        <v>8</v>
+      </c>
+      <c r="W54">
+        <v>1</v>
+      </c>
+      <c r="X54">
+        <v>16</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z54">
+        <v>1</v>
+      </c>
+      <c r="AA54">
+        <v>8</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC54" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD54" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF54" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG54">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO54*AP54*AQ54) * ((W54*X54 + Z54*AA54) / (3*16 + 1*8)) * (U54 / 5)</f>
+        <v>2643.7956114331109</v>
+      </c>
+      <c r="AH54" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI54" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ54" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK54" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL54" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM54" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN54" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO54" s="1">
+        <v>32</v>
+      </c>
+      <c r="AP54" s="18">
+        <v>256</v>
+      </c>
+      <c r="AQ54" s="18">
+        <v>128</v>
+      </c>
+      <c r="AR54" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS54" s="1">
+        <f t="shared" si="61"/>
+        <v>46</v>
+      </c>
+      <c r="AT54">
+        <f t="shared" si="62"/>
+        <v>456</v>
+      </c>
+      <c r="AU54">
+        <f t="shared" si="63"/>
+        <v>143</v>
+      </c>
+      <c r="AV54" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW54" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX54" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY54" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ54" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA54" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>263</v>
+    <row r="55" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>265</v>
       </c>
       <c r="B55" t="s">
         <v>132</v>
@@ -8968,13 +10227,159 @@
       <c r="C55" s="17" t="s">
         <v>239</v>
       </c>
+      <c r="F55" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G55" t="s">
+        <v>130</v>
+      </c>
+      <c r="H55" t="s">
+        <v>130</v>
+      </c>
+      <c r="I55" t="s">
+        <v>130</v>
+      </c>
+      <c r="J55" t="s">
+        <v>130</v>
+      </c>
+      <c r="K55" t="s">
+        <v>130</v>
+      </c>
+      <c r="L55" t="s">
+        <v>130</v>
+      </c>
+      <c r="M55" t="s">
+        <v>130</v>
+      </c>
+      <c r="N55" t="s">
+        <v>130</v>
+      </c>
+      <c r="O55" t="s">
+        <v>130</v>
+      </c>
       <c r="P55" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="Q55">
+        <v>6</v>
+      </c>
+      <c r="R55" t="s">
+        <v>130</v>
+      </c>
+      <c r="S55">
+        <v>5</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+      <c r="U55">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V55" t="s">
+        <v>8</v>
+      </c>
+      <c r="W55">
+        <v>3</v>
+      </c>
+      <c r="X55">
+        <v>8</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z55">
+        <v>1</v>
+      </c>
+      <c r="AA55">
+        <v>8</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC55" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD55" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF55" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG55">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO55*AP55*AQ55) * ((W55*X55 + Z55*AA55) / (3*16 + 1*8)) * (U55 / 5)</f>
+        <v>43246.145914876637</v>
+      </c>
+      <c r="AH55" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI55" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ55" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK55" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL55" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM55" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN55" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO55" s="1">
+        <v>96</v>
+      </c>
+      <c r="AP55">
+        <v>784</v>
+      </c>
+      <c r="AQ55">
+        <v>384</v>
+      </c>
+      <c r="AR55" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS55" s="1">
+        <f t="shared" si="61"/>
+        <v>14</v>
+      </c>
+      <c r="AT55">
+        <f t="shared" si="62"/>
+        <v>192</v>
+      </c>
+      <c r="AU55">
+        <f t="shared" si="63"/>
+        <v>15</v>
+      </c>
+      <c r="AV55" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW55" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="AX55" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY55" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ55" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA55" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>264</v>
+    <row r="56" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
+        <v>266</v>
       </c>
       <c r="B56" t="s">
         <v>132</v>
@@ -8982,13 +10387,159 @@
       <c r="C56" s="17" t="s">
         <v>240</v>
       </c>
+      <c r="F56" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G56" t="s">
+        <v>130</v>
+      </c>
+      <c r="H56" t="s">
+        <v>130</v>
+      </c>
+      <c r="I56" t="s">
+        <v>130</v>
+      </c>
+      <c r="J56" t="s">
+        <v>130</v>
+      </c>
+      <c r="K56" t="s">
+        <v>130</v>
+      </c>
+      <c r="L56" t="s">
+        <v>130</v>
+      </c>
+      <c r="M56" t="s">
+        <v>130</v>
+      </c>
+      <c r="N56" t="s">
+        <v>130</v>
+      </c>
+      <c r="O56" t="s">
+        <v>130</v>
+      </c>
       <c r="P56" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="Q56">
+        <v>6</v>
+      </c>
+      <c r="R56" t="s">
+        <v>130</v>
+      </c>
+      <c r="S56">
+        <v>5</v>
+      </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
+      <c r="U56">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V56" t="s">
+        <v>8</v>
+      </c>
+      <c r="W56">
+        <v>3</v>
+      </c>
+      <c r="X56">
+        <v>8</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z56">
+        <v>1</v>
+      </c>
+      <c r="AA56">
+        <v>8</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC56" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD56" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF56" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG56">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO56*AP56*AQ56) * ((W56*X56 + Z56*AA56) / (3*16 + 1*8)) * (U56 / 5)</f>
+        <v>13622.519702807114</v>
+      </c>
+      <c r="AH56" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI56" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ56" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK56" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL56" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM56" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN56" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO56" s="1">
+        <v>64</v>
+      </c>
+      <c r="AP56" s="18">
+        <v>512</v>
+      </c>
+      <c r="AQ56" s="18">
+        <v>256</v>
+      </c>
+      <c r="AR56" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS56" s="1">
+        <f t="shared" si="61"/>
+        <v>30</v>
+      </c>
+      <c r="AT56">
+        <f t="shared" si="62"/>
+        <v>328</v>
+      </c>
+      <c r="AU56">
+        <f t="shared" si="63"/>
+        <v>79</v>
+      </c>
+      <c r="AV56" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW56" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX56" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY56" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ56" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA56" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>265</v>
+    <row r="57" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
+        <v>267</v>
       </c>
       <c r="B57" t="s">
         <v>132</v>
@@ -8996,13 +10547,159 @@
       <c r="C57" s="17" t="s">
         <v>241</v>
       </c>
+      <c r="F57" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G57" t="s">
+        <v>130</v>
+      </c>
+      <c r="H57" t="s">
+        <v>130</v>
+      </c>
+      <c r="I57" t="s">
+        <v>130</v>
+      </c>
+      <c r="J57" t="s">
+        <v>130</v>
+      </c>
+      <c r="K57" t="s">
+        <v>130</v>
+      </c>
+      <c r="L57" t="s">
+        <v>130</v>
+      </c>
+      <c r="M57" t="s">
+        <v>130</v>
+      </c>
+      <c r="N57" t="s">
+        <v>130</v>
+      </c>
+      <c r="O57" t="s">
+        <v>130</v>
+      </c>
       <c r="P57" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="Q57">
+        <v>6</v>
+      </c>
+      <c r="R57" t="s">
+        <v>130</v>
+      </c>
+      <c r="S57">
+        <v>5</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="U57">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V57" t="s">
+        <v>8</v>
+      </c>
+      <c r="W57">
+        <v>3</v>
+      </c>
+      <c r="X57">
+        <v>8</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z57">
+        <v>1</v>
+      </c>
+      <c r="AA57">
+        <v>8</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC57" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD57" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF57" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG57">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO57*AP57*AQ57) * ((W57*X57 + Z57*AA57) / (3*16 + 1*8)) * (U57 / 5)</f>
+        <v>3022.3723042391107</v>
+      </c>
+      <c r="AH57" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI57" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ57" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK57" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL57" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM57" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN57" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO57" s="1">
+        <v>32</v>
+      </c>
+      <c r="AP57" s="18">
+        <v>256</v>
+      </c>
+      <c r="AQ57" s="18">
+        <v>128</v>
+      </c>
+      <c r="AR57" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS57" s="1">
+        <f t="shared" si="61"/>
+        <v>46</v>
+      </c>
+      <c r="AT57">
+        <f t="shared" si="62"/>
+        <v>456</v>
+      </c>
+      <c r="AU57">
+        <f t="shared" si="63"/>
+        <v>143</v>
+      </c>
+      <c r="AV57" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW57" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX57" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY57" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ57" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA57" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>266</v>
+    <row r="58" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
+        <v>268</v>
       </c>
       <c r="B58" t="s">
         <v>132</v>
@@ -9010,13 +10707,159 @@
       <c r="C58" s="17" t="s">
         <v>242</v>
       </c>
+      <c r="F58" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G58" t="s">
+        <v>130</v>
+      </c>
+      <c r="H58" t="s">
+        <v>130</v>
+      </c>
+      <c r="I58" t="s">
+        <v>130</v>
+      </c>
+      <c r="J58" t="s">
+        <v>130</v>
+      </c>
+      <c r="K58" t="s">
+        <v>130</v>
+      </c>
+      <c r="L58" t="s">
+        <v>130</v>
+      </c>
+      <c r="M58" t="s">
+        <v>130</v>
+      </c>
+      <c r="N58" t="s">
+        <v>130</v>
+      </c>
+      <c r="O58" t="s">
+        <v>130</v>
+      </c>
       <c r="P58" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="Q58">
+        <v>6</v>
+      </c>
+      <c r="R58" t="s">
+        <v>130</v>
+      </c>
+      <c r="S58">
+        <v>5</v>
+      </c>
+      <c r="T58">
+        <v>1</v>
+      </c>
+      <c r="U58">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V58" t="s">
+        <v>8</v>
+      </c>
+      <c r="W58">
+        <v>2</v>
+      </c>
+      <c r="X58">
+        <v>8</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z58">
+        <v>1</v>
+      </c>
+      <c r="AA58">
+        <v>8</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC58" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD58" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE58" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF58" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG58">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO58*AP58*AQ58) * ((W58*X58 + Z58*AA58) / (3*16 + 1*8)) * (U58 / 5)</f>
+        <v>32811.625819411252</v>
+      </c>
+      <c r="AH58" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI58" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ58" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK58" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL58" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM58" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN58" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO58" s="1">
+        <v>96</v>
+      </c>
+      <c r="AP58">
+        <v>784</v>
+      </c>
+      <c r="AQ58">
+        <v>384</v>
+      </c>
+      <c r="AR58" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS58" s="1">
+        <f t="shared" si="61"/>
+        <v>14</v>
+      </c>
+      <c r="AT58">
+        <f t="shared" si="62"/>
+        <v>192</v>
+      </c>
+      <c r="AU58">
+        <f t="shared" si="63"/>
+        <v>15</v>
+      </c>
+      <c r="AV58" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW58" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="AX58" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY58" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ58" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA58" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>267</v>
+    <row r="59" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>269</v>
       </c>
       <c r="B59" t="s">
         <v>132</v>
@@ -9024,13 +10867,159 @@
       <c r="C59" s="17" t="s">
         <v>243</v>
       </c>
+      <c r="F59" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G59" t="s">
+        <v>130</v>
+      </c>
+      <c r="H59" t="s">
+        <v>130</v>
+      </c>
+      <c r="I59" t="s">
+        <v>130</v>
+      </c>
+      <c r="J59" t="s">
+        <v>130</v>
+      </c>
+      <c r="K59" t="s">
+        <v>130</v>
+      </c>
+      <c r="L59" t="s">
+        <v>130</v>
+      </c>
+      <c r="M59" t="s">
+        <v>130</v>
+      </c>
+      <c r="N59" t="s">
+        <v>130</v>
+      </c>
+      <c r="O59" t="s">
+        <v>130</v>
+      </c>
       <c r="P59" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="Q59">
+        <v>6</v>
+      </c>
+      <c r="R59" t="s">
+        <v>130</v>
+      </c>
+      <c r="S59">
+        <v>5</v>
+      </c>
+      <c r="T59">
+        <v>1</v>
+      </c>
+      <c r="U59">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V59" t="s">
+        <v>8</v>
+      </c>
+      <c r="W59">
+        <v>2</v>
+      </c>
+      <c r="X59">
+        <v>8</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z59">
+        <v>1</v>
+      </c>
+      <c r="AA59">
+        <v>8</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC59" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD59" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG59">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO59*AP59*AQ59) * ((W59*X59 + Z59*AA59) / (3*16 + 1*8)) * (U59 / 5)</f>
+        <v>10593.906160359114</v>
+      </c>
+      <c r="AH59" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI59" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ59" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK59" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL59" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM59" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN59" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO59" s="1">
+        <v>64</v>
+      </c>
+      <c r="AP59" s="18">
+        <v>512</v>
+      </c>
+      <c r="AQ59" s="18">
+        <v>256</v>
+      </c>
+      <c r="AR59" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS59" s="1">
+        <f t="shared" si="61"/>
+        <v>30</v>
+      </c>
+      <c r="AT59">
+        <f t="shared" si="62"/>
+        <v>328</v>
+      </c>
+      <c r="AU59">
+        <f t="shared" si="63"/>
+        <v>79</v>
+      </c>
+      <c r="AV59" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW59" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX59" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY59" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ59" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA59" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>268</v>
+    <row r="60" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
+        <v>270</v>
       </c>
       <c r="B60" t="s">
         <v>132</v>
@@ -9038,13 +11027,159 @@
       <c r="C60" s="17" t="s">
         <v>244</v>
       </c>
+      <c r="F60" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G60" t="s">
+        <v>130</v>
+      </c>
+      <c r="H60" t="s">
+        <v>130</v>
+      </c>
+      <c r="I60" t="s">
+        <v>130</v>
+      </c>
+      <c r="J60" t="s">
+        <v>130</v>
+      </c>
+      <c r="K60" t="s">
+        <v>130</v>
+      </c>
+      <c r="L60" t="s">
+        <v>130</v>
+      </c>
+      <c r="M60" t="s">
+        <v>130</v>
+      </c>
+      <c r="N60" t="s">
+        <v>130</v>
+      </c>
+      <c r="O60" t="s">
+        <v>130</v>
+      </c>
       <c r="P60" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="Q60">
+        <v>6</v>
+      </c>
+      <c r="R60" t="s">
+        <v>130</v>
+      </c>
+      <c r="S60">
+        <v>5</v>
+      </c>
+      <c r="T60">
+        <v>1</v>
+      </c>
+      <c r="U60">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V60" t="s">
+        <v>8</v>
+      </c>
+      <c r="W60">
+        <v>2</v>
+      </c>
+      <c r="X60">
+        <v>8</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z60">
+        <v>1</v>
+      </c>
+      <c r="AA60">
+        <v>8</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC60" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD60" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE60" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF60" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG60">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO60*AP60*AQ60) * ((W60*X60 + Z60*AA60) / (3*16 + 1*8)) * (U60 / 5)</f>
+        <v>2643.7956114331109</v>
+      </c>
+      <c r="AH60" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI60" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ60" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK60" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL60" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM60" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN60" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO60" s="1">
+        <v>32</v>
+      </c>
+      <c r="AP60" s="18">
+        <v>256</v>
+      </c>
+      <c r="AQ60" s="18">
+        <v>128</v>
+      </c>
+      <c r="AR60" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS60" s="1">
+        <f t="shared" si="61"/>
+        <v>46</v>
+      </c>
+      <c r="AT60">
+        <f t="shared" si="62"/>
+        <v>456</v>
+      </c>
+      <c r="AU60">
+        <f t="shared" si="63"/>
+        <v>143</v>
+      </c>
+      <c r="AV60" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW60" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX60" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY60" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ60" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA60" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>269</v>
+    <row r="61" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
+        <v>271</v>
       </c>
       <c r="B61" t="s">
         <v>132</v>
@@ -9052,13 +11187,159 @@
       <c r="C61" s="17" t="s">
         <v>245</v>
       </c>
+      <c r="F61" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G61" t="s">
+        <v>130</v>
+      </c>
+      <c r="H61" t="s">
+        <v>130</v>
+      </c>
+      <c r="I61" t="s">
+        <v>130</v>
+      </c>
+      <c r="J61" t="s">
+        <v>130</v>
+      </c>
+      <c r="K61" t="s">
+        <v>130</v>
+      </c>
+      <c r="L61" t="s">
+        <v>130</v>
+      </c>
+      <c r="M61" t="s">
+        <v>130</v>
+      </c>
+      <c r="N61" t="s">
+        <v>130</v>
+      </c>
+      <c r="O61" t="s">
+        <v>130</v>
+      </c>
       <c r="P61" s="1" t="s">
         <v>253</v>
       </c>
+      <c r="Q61">
+        <v>6</v>
+      </c>
+      <c r="R61" t="s">
+        <v>130</v>
+      </c>
+      <c r="S61">
+        <v>5</v>
+      </c>
+      <c r="T61">
+        <v>1</v>
+      </c>
+      <c r="U61">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V61" t="s">
+        <v>8</v>
+      </c>
+      <c r="W61">
+        <v>1</v>
+      </c>
+      <c r="X61">
+        <v>8</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z61">
+        <v>1</v>
+      </c>
+      <c r="AA61">
+        <v>8</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC61" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD61" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE61" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF61" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG61">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO61*AP61*AQ61) * ((W61*X61 + Z61*AA61) / (3*16 + 1*8)) * (U61 / 5)</f>
+        <v>22377.105723945871</v>
+      </c>
+      <c r="AH61" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI61" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ61" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK61" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL61" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM61" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN61" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO61" s="1">
+        <v>96</v>
+      </c>
+      <c r="AP61">
+        <v>784</v>
+      </c>
+      <c r="AQ61">
+        <v>384</v>
+      </c>
+      <c r="AR61" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS61" s="1">
+        <f t="shared" si="61"/>
+        <v>14</v>
+      </c>
+      <c r="AT61">
+        <f t="shared" si="62"/>
+        <v>192</v>
+      </c>
+      <c r="AU61">
+        <f t="shared" si="63"/>
+        <v>15</v>
+      </c>
+      <c r="AV61" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW61" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="AX61" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY61" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ61" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA61" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>270</v>
+    <row r="62" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
+        <v>272</v>
       </c>
       <c r="B62" t="s">
         <v>132</v>
@@ -9066,13 +11347,159 @@
       <c r="C62" s="17" t="s">
         <v>246</v>
       </c>
+      <c r="F62" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G62" t="s">
+        <v>130</v>
+      </c>
+      <c r="H62" t="s">
+        <v>130</v>
+      </c>
+      <c r="I62" t="s">
+        <v>130</v>
+      </c>
+      <c r="J62" t="s">
+        <v>130</v>
+      </c>
+      <c r="K62" t="s">
+        <v>130</v>
+      </c>
+      <c r="L62" t="s">
+        <v>130</v>
+      </c>
+      <c r="M62" t="s">
+        <v>130</v>
+      </c>
+      <c r="N62" t="s">
+        <v>130</v>
+      </c>
+      <c r="O62" t="s">
+        <v>130</v>
+      </c>
       <c r="P62" s="1" t="s">
         <v>253</v>
       </c>
+      <c r="Q62">
+        <v>6</v>
+      </c>
+      <c r="R62" t="s">
+        <v>130</v>
+      </c>
+      <c r="S62">
+        <v>5</v>
+      </c>
+      <c r="T62">
+        <v>1</v>
+      </c>
+      <c r="U62">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V62" t="s">
+        <v>8</v>
+      </c>
+      <c r="W62">
+        <v>1</v>
+      </c>
+      <c r="X62">
+        <v>8</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z62">
+        <v>1</v>
+      </c>
+      <c r="AA62">
+        <v>8</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC62" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD62" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE62" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF62" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG62">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO62*AP62*AQ62) * ((W62*X62 + Z62*AA62) / (3*16 + 1*8)) * (U62 / 5)</f>
+        <v>7565.2926179111128</v>
+      </c>
+      <c r="AH62" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI62" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ62" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK62" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL62" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM62" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN62" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO62" s="1">
+        <v>64</v>
+      </c>
+      <c r="AP62" s="18">
+        <v>512</v>
+      </c>
+      <c r="AQ62" s="18">
+        <v>256</v>
+      </c>
+      <c r="AR62" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS62" s="1">
+        <f t="shared" si="61"/>
+        <v>30</v>
+      </c>
+      <c r="AT62">
+        <f t="shared" si="62"/>
+        <v>328</v>
+      </c>
+      <c r="AU62">
+        <f t="shared" si="63"/>
+        <v>79</v>
+      </c>
+      <c r="AV62" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW62" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX62" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY62" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ62" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA62" s="18" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>271</v>
+    <row r="63" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>273</v>
       </c>
       <c r="B63" t="s">
         <v>132</v>
@@ -9080,9 +11507,175 @@
       <c r="C63" s="17" t="s">
         <v>247</v>
       </c>
+      <c r="F63" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G63" t="s">
+        <v>130</v>
+      </c>
+      <c r="H63" t="s">
+        <v>130</v>
+      </c>
+      <c r="I63" t="s">
+        <v>130</v>
+      </c>
+      <c r="J63" t="s">
+        <v>130</v>
+      </c>
+      <c r="K63" t="s">
+        <v>130</v>
+      </c>
+      <c r="L63" t="s">
+        <v>130</v>
+      </c>
+      <c r="M63" t="s">
+        <v>130</v>
+      </c>
+      <c r="N63" t="s">
+        <v>130</v>
+      </c>
+      <c r="O63" t="s">
+        <v>130</v>
+      </c>
       <c r="P63" s="1" t="s">
         <v>253</v>
       </c>
+      <c r="Q63">
+        <v>6</v>
+      </c>
+      <c r="R63" t="s">
+        <v>130</v>
+      </c>
+      <c r="S63">
+        <v>5</v>
+      </c>
+      <c r="T63">
+        <v>1</v>
+      </c>
+      <c r="U63">
+        <f t="shared" si="54"/>
+        <v>6</v>
+      </c>
+      <c r="V63" t="s">
+        <v>8</v>
+      </c>
+      <c r="W63">
+        <v>1</v>
+      </c>
+      <c r="X63">
+        <v>8</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z63">
+        <v>1</v>
+      </c>
+      <c r="AA63">
+        <v>8</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC63" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD63" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE63" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF63" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG63">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AO63*AP63*AQ63) * ((W63*X63 + Z63*AA63) / (3*16 + 1*8)) * (U63 / 5)</f>
+        <v>2265.2189186271103</v>
+      </c>
+      <c r="AH63" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI63" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ63" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK63" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL63" s="10">
+        <v>125</v>
+      </c>
+      <c r="AM63" s="18">
+        <v>1169</v>
+      </c>
+      <c r="AN63" s="18">
+        <v>414</v>
+      </c>
+      <c r="AO63" s="1">
+        <v>32</v>
+      </c>
+      <c r="AP63" s="18">
+        <v>256</v>
+      </c>
+      <c r="AQ63" s="18">
+        <v>128</v>
+      </c>
+      <c r="AR63" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS63" s="1">
+        <f t="shared" si="61"/>
+        <v>46</v>
+      </c>
+      <c r="AT63">
+        <f t="shared" si="62"/>
+        <v>456</v>
+      </c>
+      <c r="AU63">
+        <f t="shared" si="63"/>
+        <v>143</v>
+      </c>
+      <c r="AV63" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW63" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX63" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY63" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ63" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA63" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AZ64" s="18"/>
+      <c r="BA64" s="18"/>
+    </row>
+    <row r="65" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AZ65" s="18"/>
+      <c r="BA65" s="18"/>
+    </row>
+    <row r="66" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AZ66" s="18"/>
+      <c r="BA66" s="18"/>
+    </row>
+    <row r="67" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AZ67" s="18"/>
+      <c r="BA67" s="18"/>
+    </row>
+    <row r="68" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AZ68" s="18"/>
+      <c r="BA68" s="18"/>
     </row>
     <row r="69" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -9219,15 +11812,15 @@
         <v>130</v>
       </c>
       <c r="AS69" s="1" t="e">
-        <f t="shared" ref="AS69" si="58" xml:space="preserve"> _xlfn.FLOOR.MATH((AL69 - AO69) / 2)</f>
+        <f t="shared" ref="AS69" si="64" xml:space="preserve"> _xlfn.FLOOR.MATH((AL69 - AO69) / 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AT69" t="e">
-        <f t="shared" ref="AT69" si="59" xml:space="preserve"> _xlfn.FLOOR.MATH((AM69 - AP69) / 2)</f>
+        <f t="shared" ref="AT69" si="65" xml:space="preserve"> _xlfn.FLOOR.MATH((AM69 - AP69) / 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AU69" t="e">
-        <f t="shared" ref="AU69" si="60" xml:space="preserve"> _xlfn.FLOOR.MATH((AN69 - AQ69) / 2)</f>
+        <f t="shared" ref="AU69" si="66" xml:space="preserve"> _xlfn.FLOOR.MATH((AN69 - AQ69) / 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AV69" t="s">

</xml_diff>

<commit_message>
refine nvidia-smi calc script
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC861816-DADB-4E65-B011-F6317F2AD1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5BB880-4F2E-49E1-B18A-717F122AD225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1769" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="278">
   <si>
     <t>patch z</t>
   </si>
@@ -1036,7 +1036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1063,15 +1063,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -1390,22 +1387,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BD76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF35" sqref="AF35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="109" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="71" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="26.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="14.5703125" style="10" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="20" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="30.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="15.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="33" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="14.5703125" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="33" customWidth="1"/>
     <col min="16" max="16" width="12.85546875" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="18" max="18" width="9.140625" collapsed="1"/>
@@ -1420,7 +1417,7 @@
     <col min="27" max="27" width="7.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="28" max="28" width="9.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="29" max="29" width="16.7109375" style="10" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="16.7109375" style="22" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" customWidth="1"/>
     <col min="31" max="32" width="14.85546875" customWidth="1"/>
     <col min="33" max="35" width="9.140625" customWidth="1"/>
     <col min="36" max="36" width="7.28515625" style="1" customWidth="1" outlineLevel="1"/>
@@ -2196,10 +2193,10 @@
       <c r="AC5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="AD5" s="24">
+      <c r="AD5" s="22">
         <v>31715</v>
       </c>
-      <c r="AE5" s="27">
+      <c r="AE5" s="24">
         <v>785</v>
       </c>
       <c r="AF5" t="e">
@@ -2365,10 +2362,10 @@
       <c r="AC6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AD6" s="24">
+      <c r="AD6" s="22">
         <v>957</v>
       </c>
-      <c r="AE6" s="27">
+      <c r="AE6" s="24">
         <v>31543</v>
       </c>
       <c r="AF6" t="s">
@@ -2533,10 +2530,10 @@
       <c r="AC7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AD7" s="24">
+      <c r="AD7" s="22">
         <v>957</v>
       </c>
-      <c r="AE7" s="27">
+      <c r="AE7" s="24">
         <v>31543</v>
       </c>
       <c r="AF7" t="s">
@@ -2701,10 +2698,10 @@
       <c r="AC8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="AD8" s="24">
+      <c r="AD8" s="22">
         <v>31413</v>
       </c>
-      <c r="AE8" s="27">
+      <c r="AE8" s="24">
         <v>1087</v>
       </c>
       <c r="AF8" t="e">
@@ -2870,10 +2867,10 @@
       <c r="AC9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AD9" s="24">
+      <c r="AD9" s="22">
         <v>20319</v>
       </c>
-      <c r="AE9" s="27">
+      <c r="AE9" s="24">
         <v>12181</v>
       </c>
       <c r="AF9" t="s">
@@ -3044,10 +3041,10 @@
       <c r="AC10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AD10" s="24">
+      <c r="AD10" s="22">
         <v>19417</v>
       </c>
-      <c r="AE10" s="27">
+      <c r="AE10" s="24">
         <v>13083</v>
       </c>
       <c r="AF10" t="s">
@@ -3212,10 +3209,10 @@
       <c r="AC11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="AD11" s="24">
+      <c r="AD11" s="22">
         <v>30325</v>
       </c>
-      <c r="AE11" s="27">
+      <c r="AE11" s="24">
         <v>2175</v>
       </c>
       <c r="AF11" t="e">
@@ -3381,10 +3378,10 @@
       <c r="AC12" s="10">
         <v>10135</v>
       </c>
-      <c r="AD12" s="24">
+      <c r="AD12" s="22">
         <v>10135</v>
       </c>
-      <c r="AE12" s="27">
+      <c r="AE12" s="24">
         <v>22365</v>
       </c>
       <c r="AF12">
@@ -3550,10 +3547,10 @@
       <c r="AC13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AD13" s="24">
+      <c r="AD13" s="22">
         <v>5881</v>
       </c>
-      <c r="AE13" s="27">
+      <c r="AE13" s="24">
         <v>26619</v>
       </c>
       <c r="AF13" t="s">
@@ -3718,10 +3715,10 @@
       <c r="AC14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AD14" s="24">
+      <c r="AD14" s="22">
         <v>5881</v>
       </c>
-      <c r="AE14" s="27">
+      <c r="AE14" s="24">
         <v>26619</v>
       </c>
       <c r="AF14" t="s">
@@ -3886,14 +3883,14 @@
       <c r="AC15" s="10">
         <v>13843</v>
       </c>
-      <c r="AD15" s="24">
+      <c r="AD15" s="22">
         <v>13843</v>
       </c>
-      <c r="AE15" s="27">
+      <c r="AE15" s="24">
         <v>18657</v>
       </c>
       <c r="AF15">
-        <f>AC15+AE15</f>
+        <f t="shared" ref="AF15:AF24" si="1">AC15+AE15</f>
         <v>32500</v>
       </c>
       <c r="AG15" t="s">
@@ -4055,14 +4052,14 @@
       <c r="AC16" s="11">
         <v>13843</v>
       </c>
-      <c r="AD16" s="25">
+      <c r="AD16" s="23">
         <v>13843</v>
       </c>
-      <c r="AE16" s="28">
+      <c r="AE16" s="25">
         <v>18657</v>
       </c>
       <c r="AF16" s="7">
-        <f>AC16+AE16</f>
+        <f t="shared" si="1"/>
         <v>32500</v>
       </c>
       <c r="AG16" s="7" t="s">
@@ -4224,14 +4221,14 @@
       <c r="AC17" s="10">
         <v>10135</v>
       </c>
-      <c r="AD17" s="24">
+      <c r="AD17" s="22">
         <v>10135</v>
       </c>
-      <c r="AE17" s="27">
+      <c r="AE17" s="24">
         <v>22365</v>
       </c>
       <c r="AF17">
-        <f>AC17+AE17</f>
+        <f t="shared" si="1"/>
         <v>32500</v>
       </c>
       <c r="AG17" t="s">
@@ -4393,14 +4390,14 @@
       <c r="AC18" s="10">
         <v>10135</v>
       </c>
-      <c r="AD18" s="24">
+      <c r="AD18" s="22">
         <v>10135</v>
       </c>
-      <c r="AE18" s="27">
+      <c r="AE18" s="24">
         <v>22365</v>
       </c>
       <c r="AF18">
-        <f>AC18+AE18</f>
+        <f t="shared" si="1"/>
         <v>32500</v>
       </c>
       <c r="AG18" t="s">
@@ -4562,14 +4559,14 @@
       <c r="AC19" s="10">
         <v>10999</v>
       </c>
-      <c r="AD19" s="24">
+      <c r="AD19" s="22">
         <v>10999</v>
       </c>
-      <c r="AE19" s="27">
+      <c r="AE19" s="24">
         <v>21501</v>
       </c>
       <c r="AF19">
-        <f>AC19+AE19</f>
+        <f t="shared" si="1"/>
         <v>32500</v>
       </c>
       <c r="AG19" t="s">
@@ -4731,14 +4728,14 @@
       <c r="AC20" s="10">
         <v>11843</v>
       </c>
-      <c r="AD20" s="24">
+      <c r="AD20" s="22">
         <v>11843</v>
       </c>
-      <c r="AE20" s="27">
+      <c r="AE20" s="24">
         <v>20657</v>
       </c>
       <c r="AF20">
-        <f>AC20+AE20</f>
+        <f t="shared" si="1"/>
         <v>32500</v>
       </c>
       <c r="AG20" t="s">
@@ -4900,14 +4897,14 @@
       <c r="AC21" s="10">
         <v>10473</v>
       </c>
-      <c r="AD21" s="24">
+      <c r="AD21" s="22">
         <v>10473</v>
       </c>
-      <c r="AE21" s="27">
+      <c r="AE21" s="24">
         <v>22027</v>
       </c>
       <c r="AF21">
-        <f>AC21+AE21</f>
+        <f t="shared" si="1"/>
         <v>32500</v>
       </c>
       <c r="AG21" t="s">
@@ -5069,14 +5066,14 @@
       <c r="AC22" s="10">
         <v>10825</v>
       </c>
-      <c r="AD22" s="24">
+      <c r="AD22" s="22">
         <v>10825</v>
       </c>
-      <c r="AE22" s="27">
+      <c r="AE22" s="24">
         <v>21675</v>
       </c>
       <c r="AF22">
-        <f>AC22+AE22</f>
+        <f t="shared" si="1"/>
         <v>32500</v>
       </c>
       <c r="AG22" t="s">
@@ -5238,14 +5235,14 @@
       <c r="AC23" s="10">
         <v>12317</v>
       </c>
-      <c r="AD23" s="24">
+      <c r="AD23" s="22">
         <v>12317</v>
       </c>
-      <c r="AE23" s="27">
+      <c r="AE23" s="24">
         <v>20183</v>
       </c>
       <c r="AF23">
-        <f>AC23+AE23</f>
+        <f t="shared" si="1"/>
         <v>32500</v>
       </c>
       <c r="AG23" t="s">
@@ -5407,14 +5404,14 @@
       <c r="AC24" s="10">
         <v>14443</v>
       </c>
-      <c r="AD24" s="24">
+      <c r="AD24" s="22">
         <v>14443</v>
       </c>
-      <c r="AE24" s="27">
+      <c r="AE24" s="24">
         <v>18057</v>
       </c>
       <c r="AF24">
-        <f>AC24+AE24</f>
+        <f t="shared" si="1"/>
         <v>32500</v>
       </c>
       <c r="AG24" t="s">
@@ -5575,7 +5572,7 @@
       <c r="AC25" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AD25" s="26" t="s">
+      <c r="AD25" t="s">
         <v>8</v>
       </c>
       <c r="AE25" t="s">
@@ -5883,7 +5880,7 @@
         <v>2</v>
       </c>
       <c r="U27">
-        <f t="shared" ref="U27:U34" si="1" xml:space="preserve"> S27 + T27</f>
+        <f t="shared" ref="U27:U34" si="2" xml:space="preserve"> S27 + T27</f>
         <v>5</v>
       </c>
       <c r="V27" t="s">
@@ -5907,16 +5904,18 @@
       <c r="AB27" t="s">
         <v>102</v>
       </c>
-      <c r="AC27" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD27" s="23"/>
-      <c r="AE27" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="AF27" t="e">
-        <f>AC27+AE27</f>
-        <v>#VALUE!</v>
+      <c r="AC27" s="20">
+        <v>80545</v>
+      </c>
+      <c r="AD27" s="19">
+        <v>80545</v>
+      </c>
+      <c r="AE27" s="19">
+        <v>507</v>
+      </c>
+      <c r="AF27">
+        <f t="shared" ref="AF27:AF33" si="3">AC27+AE27</f>
+        <v>81052</v>
       </c>
       <c r="AG27" t="s">
         <v>8</v>
@@ -5925,7 +5924,7 @@
         <v>8</v>
       </c>
       <c r="AI27">
-        <f t="shared" ref="AI27" si="2" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ27*AR27*AS27)</f>
+        <f t="shared" ref="AI27" si="4" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ27*AR27*AS27)</f>
         <v>83027.753778838392</v>
       </c>
       <c r="AJ27" s="1">
@@ -5962,15 +5961,15 @@
         <v>50</v>
       </c>
       <c r="AU27" s="1">
-        <f t="shared" ref="AU27:AU34" si="3" xml:space="preserve"> _xlfn.FLOOR.MATH((AN27 - AQ27) / 2)</f>
+        <f t="shared" ref="AU27:AU34" si="5" xml:space="preserve"> _xlfn.FLOOR.MATH((AN27 - AQ27) / 2)</f>
         <v>6</v>
       </c>
       <c r="AV27">
-        <f t="shared" ref="AV27" si="4" xml:space="preserve"> _xlfn.FLOOR.MATH((AO27 - AR27) / 2)</f>
+        <f t="shared" ref="AV27" si="6" xml:space="preserve"> _xlfn.FLOOR.MATH((AO27 - AR27) / 2)</f>
         <v>152</v>
       </c>
       <c r="AW27">
-        <f t="shared" ref="AW27" si="5" xml:space="preserve"> _xlfn.FLOOR.MATH((AP27 - AS27) / 2)</f>
+        <f t="shared" ref="AW27" si="7" xml:space="preserve"> _xlfn.FLOOR.MATH((AP27 - AS27) / 2)</f>
         <v>7</v>
       </c>
       <c r="AX27" t="s">
@@ -6054,7 +6053,7 @@
         <v>2</v>
       </c>
       <c r="U28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="V28" t="s">
@@ -6081,12 +6080,12 @@
       <c r="AC28" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="AD28" s="23"/>
+      <c r="AD28" s="19"/>
       <c r="AE28" s="19" t="s">
         <v>130</v>
       </c>
       <c r="AF28" t="e">
-        <f>AC28+AE28</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="AG28">
@@ -6097,7 +6096,7 @@
         <v>80.11</v>
       </c>
       <c r="AI28">
-        <f t="shared" ref="AI28:AI33" si="6" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ28*AR28*AS28)</f>
+        <f t="shared" ref="AI28:AI33" si="8" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ28*AR28*AS28)</f>
         <v>81518.129922434266</v>
       </c>
       <c r="AJ28" s="1">
@@ -6134,15 +6133,15 @@
         <v>50</v>
       </c>
       <c r="AU28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AV28">
-        <f t="shared" ref="AV28" si="7" xml:space="preserve"> _xlfn.FLOOR.MATH((AO28 - AR28) / 2)</f>
+        <f t="shared" ref="AV28" si="9" xml:space="preserve"> _xlfn.FLOOR.MATH((AO28 - AR28) / 2)</f>
         <v>160</v>
       </c>
       <c r="AW28">
-        <f t="shared" ref="AW28" si="8" xml:space="preserve"> _xlfn.FLOOR.MATH((AP28 - AS28) / 2)</f>
+        <f t="shared" ref="AW28" si="10" xml:space="preserve"> _xlfn.FLOOR.MATH((AP28 - AS28) / 2)</f>
         <v>7</v>
       </c>
       <c r="AX28" t="s">
@@ -6226,7 +6225,7 @@
         <v>2</v>
       </c>
       <c r="U29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="V29" t="s">
@@ -6257,7 +6256,7 @@
         <v>130</v>
       </c>
       <c r="AF29" t="e">
-        <f>AC29+AE29</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="AG29" t="s">
@@ -6267,7 +6266,7 @@
         <v>8</v>
       </c>
       <c r="AI29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>76989.258353221856</v>
       </c>
       <c r="AJ29" s="1">
@@ -6304,15 +6303,15 @@
         <v>50</v>
       </c>
       <c r="AU29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AV29">
-        <f t="shared" ref="AV29" si="9" xml:space="preserve"> _xlfn.FLOOR.MATH((AO29 - AR29) / 2)</f>
+        <f t="shared" ref="AV29" si="11" xml:space="preserve"> _xlfn.FLOOR.MATH((AO29 - AR29) / 2)</f>
         <v>184</v>
       </c>
       <c r="AW29">
-        <f t="shared" ref="AW29" si="10" xml:space="preserve"> _xlfn.FLOOR.MATH((AP29 - AS29) / 2)</f>
+        <f t="shared" ref="AW29" si="12" xml:space="preserve"> _xlfn.FLOOR.MATH((AP29 - AS29) / 2)</f>
         <v>7</v>
       </c>
       <c r="AX29" t="s">
@@ -6396,7 +6395,7 @@
         <v>2</v>
       </c>
       <c r="U30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="V30" t="s">
@@ -6427,7 +6426,7 @@
         <v>130</v>
       </c>
       <c r="AF30" t="e">
-        <f>AC30+AE30</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="AG30" t="s">
@@ -6437,7 +6436,7 @@
         <v>8</v>
       </c>
       <c r="AI30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>76989.258353221856</v>
       </c>
       <c r="AJ30" s="1">
@@ -6474,15 +6473,15 @@
         <v>50</v>
       </c>
       <c r="AU30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AV30">
-        <f t="shared" ref="AV30:AV34" si="11" xml:space="preserve"> _xlfn.FLOOR.MATH((AO30 - AR30) / 2)</f>
+        <f t="shared" ref="AV30:AV34" si="13" xml:space="preserve"> _xlfn.FLOOR.MATH((AO30 - AR30) / 2)</f>
         <v>184</v>
       </c>
       <c r="AW30">
-        <f t="shared" ref="AW30:AW34" si="12" xml:space="preserve"> _xlfn.FLOOR.MATH((AP30 - AS30) / 2)</f>
+        <f t="shared" ref="AW30:AW34" si="14" xml:space="preserve"> _xlfn.FLOOR.MATH((AP30 - AS30) / 2)</f>
         <v>7</v>
       </c>
       <c r="AX30" t="s">
@@ -6566,7 +6565,7 @@
         <v>2</v>
       </c>
       <c r="U31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="V31" t="s">
@@ -6597,7 +6596,7 @@
         <v>130</v>
       </c>
       <c r="AF31" t="e">
-        <f>AC31+AE31</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="AG31" t="s">
@@ -6607,7 +6606,7 @@
         <v>8</v>
       </c>
       <c r="AI31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>76989.258353221856</v>
       </c>
       <c r="AJ31" s="1">
@@ -6644,15 +6643,15 @@
         <v>50</v>
       </c>
       <c r="AU31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AV31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>184</v>
       </c>
       <c r="AW31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="AX31" t="s">
@@ -6736,7 +6735,7 @@
         <v>2</v>
       </c>
       <c r="U32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="V32" t="s">
@@ -6763,12 +6762,12 @@
       <c r="AC32" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="AD32" s="23"/>
+      <c r="AD32" s="19"/>
       <c r="AE32" s="19" t="s">
         <v>130</v>
       </c>
       <c r="AF32" t="e">
-        <f>AC32+AE32</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="AG32" t="s">
@@ -6778,7 +6777,7 @@
         <v>8</v>
       </c>
       <c r="AI32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>76989.258353221856</v>
       </c>
       <c r="AJ32" s="1">
@@ -6815,15 +6814,15 @@
         <v>50</v>
       </c>
       <c r="AU32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AV32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>184</v>
       </c>
       <c r="AW32">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="AX32" t="s">
@@ -6907,7 +6906,7 @@
         <v>1</v>
       </c>
       <c r="U33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="V33" t="s">
@@ -6938,7 +6937,7 @@
         <v>130</v>
       </c>
       <c r="AF33" t="e">
-        <f>AC33+AE33</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="AG33" t="s">
@@ -6948,7 +6947,7 @@
         <v>8</v>
       </c>
       <c r="AI33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>76989.258353221856</v>
       </c>
       <c r="AJ33" s="1">
@@ -6985,15 +6984,15 @@
         <v>50</v>
       </c>
       <c r="AU33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AV33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>184</v>
       </c>
       <c r="AW33">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>7</v>
       </c>
       <c r="AX33" t="s">
@@ -7077,7 +7076,7 @@
         <v>1</v>
       </c>
       <c r="U34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="V34" t="s">
@@ -7117,7 +7116,7 @@
         <v>8</v>
       </c>
       <c r="AI34">
-        <f t="shared" ref="AI34:AI45" si="13" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ34*AR34*AS34) / 5 * U34</f>
+        <f t="shared" ref="AI34:AI45" si="15" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ34*AR34*AS34) / 5 * U34</f>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ34" s="1">
@@ -7154,15 +7153,15 @@
         <v>50</v>
       </c>
       <c r="AU34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="AV34">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>192</v>
       </c>
       <c r="AW34">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>15</v>
       </c>
       <c r="AX34" t="s">
@@ -7246,7 +7245,7 @@
         <v>1</v>
       </c>
       <c r="U35">
-        <f t="shared" ref="U35" si="14" xml:space="preserve"> S35 + T35</f>
+        <f t="shared" ref="U35" si="16" xml:space="preserve"> S35 + T35</f>
         <v>6</v>
       </c>
       <c r="V35" t="s">
@@ -7286,7 +7285,7 @@
         <v>8</v>
       </c>
       <c r="AI35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>76071.407048528155</v>
       </c>
       <c r="AJ35" s="1">
@@ -7323,15 +7322,15 @@
         <v>50</v>
       </c>
       <c r="AU35" s="1">
-        <f t="shared" ref="AU35" si="15" xml:space="preserve"> _xlfn.FLOOR.MATH((AN35 - AQ35) / 2)</f>
+        <f t="shared" ref="AU35" si="17" xml:space="preserve"> _xlfn.FLOOR.MATH((AN35 - AQ35) / 2)</f>
         <v>13</v>
       </c>
       <c r="AV35">
-        <f t="shared" ref="AV35" si="16" xml:space="preserve"> _xlfn.FLOOR.MATH((AO35 - AR35) / 2)</f>
+        <f t="shared" ref="AV35" si="18" xml:space="preserve"> _xlfn.FLOOR.MATH((AO35 - AR35) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW35">
-        <f t="shared" ref="AW35" si="17" xml:space="preserve"> _xlfn.FLOOR.MATH((AP35 - AS35) / 2)</f>
+        <f t="shared" ref="AW35" si="19" xml:space="preserve"> _xlfn.FLOOR.MATH((AP35 - AS35) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX35" t="s">
@@ -7415,7 +7414,7 @@
         <v>1</v>
       </c>
       <c r="U36">
-        <f t="shared" ref="U36" si="18" xml:space="preserve"> S36 + T36</f>
+        <f t="shared" ref="U36" si="20" xml:space="preserve"> S36 + T36</f>
         <v>6</v>
       </c>
       <c r="V36" t="s">
@@ -7455,7 +7454,7 @@
         <v>8</v>
       </c>
       <c r="AI36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>76071.407048528155</v>
       </c>
       <c r="AJ36" s="1">
@@ -7492,15 +7491,15 @@
         <v>50</v>
       </c>
       <c r="AU36" s="1">
-        <f t="shared" ref="AU36" si="19" xml:space="preserve"> _xlfn.FLOOR.MATH((AN36 - AQ36) / 2)</f>
+        <f t="shared" ref="AU36" si="21" xml:space="preserve"> _xlfn.FLOOR.MATH((AN36 - AQ36) / 2)</f>
         <v>13</v>
       </c>
       <c r="AV36">
-        <f t="shared" ref="AV36" si="20" xml:space="preserve"> _xlfn.FLOOR.MATH((AO36 - AR36) / 2)</f>
+        <f t="shared" ref="AV36" si="22" xml:space="preserve"> _xlfn.FLOOR.MATH((AO36 - AR36) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW36">
-        <f t="shared" ref="AW36" si="21" xml:space="preserve"> _xlfn.FLOOR.MATH((AP36 - AS36) / 2)</f>
+        <f t="shared" ref="AW36" si="23" xml:space="preserve"> _xlfn.FLOOR.MATH((AP36 - AS36) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX36" t="s">
@@ -7584,7 +7583,7 @@
         <v>1</v>
       </c>
       <c r="U37">
-        <f t="shared" ref="U37" si="22" xml:space="preserve"> S37 + T37</f>
+        <f t="shared" ref="U37" si="24" xml:space="preserve"> S37 + T37</f>
         <v>6</v>
       </c>
       <c r="V37" t="s">
@@ -7624,7 +7623,7 @@
         <v>8</v>
       </c>
       <c r="AI37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ37" s="1">
@@ -7661,15 +7660,15 @@
         <v>50</v>
       </c>
       <c r="AU37" s="1">
-        <f t="shared" ref="AU37" si="23" xml:space="preserve"> _xlfn.FLOOR.MATH((AN37 - AQ37) / 2)</f>
+        <f t="shared" ref="AU37" si="25" xml:space="preserve"> _xlfn.FLOOR.MATH((AN37 - AQ37) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV37">
-        <f t="shared" ref="AV37" si="24" xml:space="preserve"> _xlfn.FLOOR.MATH((AO37 - AR37) / 2)</f>
+        <f t="shared" ref="AV37" si="26" xml:space="preserve"> _xlfn.FLOOR.MATH((AO37 - AR37) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW37">
-        <f t="shared" ref="AW37" si="25" xml:space="preserve"> _xlfn.FLOOR.MATH((AP37 - AS37) / 2)</f>
+        <f t="shared" ref="AW37" si="27" xml:space="preserve"> _xlfn.FLOOR.MATH((AP37 - AS37) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX37" t="s">
@@ -7753,7 +7752,7 @@
         <v>1</v>
       </c>
       <c r="U38">
-        <f t="shared" ref="U38" si="26" xml:space="preserve"> S38 + T38</f>
+        <f t="shared" ref="U38" si="28" xml:space="preserve"> S38 + T38</f>
         <v>6</v>
       </c>
       <c r="V38" t="s">
@@ -7793,7 +7792,7 @@
         <v>8</v>
       </c>
       <c r="AI38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ38" s="1">
@@ -7830,15 +7829,15 @@
         <v>50</v>
       </c>
       <c r="AU38" s="1">
-        <f t="shared" ref="AU38" si="27" xml:space="preserve"> _xlfn.FLOOR.MATH((AN38 - AQ38) / 2)</f>
+        <f t="shared" ref="AU38" si="29" xml:space="preserve"> _xlfn.FLOOR.MATH((AN38 - AQ38) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV38">
-        <f t="shared" ref="AV38" si="28" xml:space="preserve"> _xlfn.FLOOR.MATH((AO38 - AR38) / 2)</f>
+        <f t="shared" ref="AV38" si="30" xml:space="preserve"> _xlfn.FLOOR.MATH((AO38 - AR38) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW38">
-        <f t="shared" ref="AW38" si="29" xml:space="preserve"> _xlfn.FLOOR.MATH((AP38 - AS38) / 2)</f>
+        <f t="shared" ref="AW38" si="31" xml:space="preserve"> _xlfn.FLOOR.MATH((AP38 - AS38) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX38" t="s">
@@ -7922,7 +7921,7 @@
         <v>1</v>
       </c>
       <c r="U39">
-        <f t="shared" ref="U39" si="30" xml:space="preserve"> S39 + T39</f>
+        <f t="shared" ref="U39" si="32" xml:space="preserve"> S39 + T39</f>
         <v>6</v>
       </c>
       <c r="V39" t="s">
@@ -7962,7 +7961,7 @@
         <v>8</v>
       </c>
       <c r="AI39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ39" s="1">
@@ -7999,15 +7998,15 @@
         <v>50</v>
       </c>
       <c r="AU39" s="1">
-        <f t="shared" ref="AU39" si="31" xml:space="preserve"> _xlfn.FLOOR.MATH((AN39 - AQ39) / 2)</f>
+        <f t="shared" ref="AU39" si="33" xml:space="preserve"> _xlfn.FLOOR.MATH((AN39 - AQ39) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV39">
-        <f t="shared" ref="AV39" si="32" xml:space="preserve"> _xlfn.FLOOR.MATH((AO39 - AR39) / 2)</f>
+        <f t="shared" ref="AV39" si="34" xml:space="preserve"> _xlfn.FLOOR.MATH((AO39 - AR39) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW39">
-        <f t="shared" ref="AW39" si="33" xml:space="preserve"> _xlfn.FLOOR.MATH((AP39 - AS39) / 2)</f>
+        <f t="shared" ref="AW39" si="35" xml:space="preserve"> _xlfn.FLOOR.MATH((AP39 - AS39) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX39" t="s">
@@ -8091,7 +8090,7 @@
         <v>1</v>
       </c>
       <c r="U40">
-        <f t="shared" ref="U40" si="34" xml:space="preserve"> S40 + T40</f>
+        <f t="shared" ref="U40" si="36" xml:space="preserve"> S40 + T40</f>
         <v>6</v>
       </c>
       <c r="V40" t="s">
@@ -8131,7 +8130,7 @@
         <v>8</v>
       </c>
       <c r="AI40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ40" s="1">
@@ -8168,15 +8167,15 @@
         <v>50</v>
       </c>
       <c r="AU40" s="1">
-        <f t="shared" ref="AU40" si="35" xml:space="preserve"> _xlfn.FLOOR.MATH((AN40 - AQ40) / 2)</f>
+        <f t="shared" ref="AU40" si="37" xml:space="preserve"> _xlfn.FLOOR.MATH((AN40 - AQ40) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV40">
-        <f t="shared" ref="AV40" si="36" xml:space="preserve"> _xlfn.FLOOR.MATH((AO40 - AR40) / 2)</f>
+        <f t="shared" ref="AV40" si="38" xml:space="preserve"> _xlfn.FLOOR.MATH((AO40 - AR40) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW40">
-        <f t="shared" ref="AW40" si="37" xml:space="preserve"> _xlfn.FLOOR.MATH((AP40 - AS40) / 2)</f>
+        <f t="shared" ref="AW40" si="39" xml:space="preserve"> _xlfn.FLOOR.MATH((AP40 - AS40) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX40" t="s">
@@ -8260,7 +8259,7 @@
         <v>1</v>
       </c>
       <c r="U41">
-        <f t="shared" ref="U41" si="38" xml:space="preserve"> S41 + T41</f>
+        <f t="shared" ref="U41" si="40" xml:space="preserve"> S41 + T41</f>
         <v>6</v>
       </c>
       <c r="V41" t="s">
@@ -8300,7 +8299,7 @@
         <v>8</v>
       </c>
       <c r="AI41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ41" s="1">
@@ -8337,15 +8336,15 @@
         <v>50</v>
       </c>
       <c r="AU41" s="1">
-        <f t="shared" ref="AU41" si="39" xml:space="preserve"> _xlfn.FLOOR.MATH((AN41 - AQ41) / 2)</f>
+        <f t="shared" ref="AU41" si="41" xml:space="preserve"> _xlfn.FLOOR.MATH((AN41 - AQ41) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV41">
-        <f t="shared" ref="AV41" si="40" xml:space="preserve"> _xlfn.FLOOR.MATH((AO41 - AR41) / 2)</f>
+        <f t="shared" ref="AV41" si="42" xml:space="preserve"> _xlfn.FLOOR.MATH((AO41 - AR41) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW41">
-        <f t="shared" ref="AW41" si="41" xml:space="preserve"> _xlfn.FLOOR.MATH((AP41 - AS41) / 2)</f>
+        <f t="shared" ref="AW41" si="43" xml:space="preserve"> _xlfn.FLOOR.MATH((AP41 - AS41) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX41" t="s">
@@ -8429,7 +8428,7 @@
         <v>1</v>
       </c>
       <c r="U42">
-        <f t="shared" ref="U42" si="42" xml:space="preserve"> S42 + T42</f>
+        <f t="shared" ref="U42" si="44" xml:space="preserve"> S42 + T42</f>
         <v>6</v>
       </c>
       <c r="V42" t="s">
@@ -8469,7 +8468,7 @@
         <v>8</v>
       </c>
       <c r="AI42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ42" s="1">
@@ -8506,15 +8505,15 @@
         <v>50</v>
       </c>
       <c r="AU42" s="1">
-        <f t="shared" ref="AU42" si="43" xml:space="preserve"> _xlfn.FLOOR.MATH((AN42 - AQ42) / 2)</f>
+        <f t="shared" ref="AU42" si="45" xml:space="preserve"> _xlfn.FLOOR.MATH((AN42 - AQ42) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV42">
-        <f t="shared" ref="AV42" si="44" xml:space="preserve"> _xlfn.FLOOR.MATH((AO42 - AR42) / 2)</f>
+        <f t="shared" ref="AV42" si="46" xml:space="preserve"> _xlfn.FLOOR.MATH((AO42 - AR42) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW42">
-        <f t="shared" ref="AW42" si="45" xml:space="preserve"> _xlfn.FLOOR.MATH((AP42 - AS42) / 2)</f>
+        <f t="shared" ref="AW42" si="47" xml:space="preserve"> _xlfn.FLOOR.MATH((AP42 - AS42) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX42" t="s">
@@ -8598,7 +8597,7 @@
         <v>1</v>
       </c>
       <c r="U43">
-        <f t="shared" ref="U43" si="46" xml:space="preserve"> S43 + T43</f>
+        <f t="shared" ref="U43" si="48" xml:space="preserve"> S43 + T43</f>
         <v>6</v>
       </c>
       <c r="V43" t="s">
@@ -8638,7 +8637,7 @@
         <v>8</v>
       </c>
       <c r="AI43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ43" s="1">
@@ -8675,15 +8674,15 @@
         <v>50</v>
       </c>
       <c r="AU43" s="1">
-        <f t="shared" ref="AU43" si="47" xml:space="preserve"> _xlfn.FLOOR.MATH((AN43 - AQ43) / 2)</f>
+        <f t="shared" ref="AU43" si="49" xml:space="preserve"> _xlfn.FLOOR.MATH((AN43 - AQ43) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV43">
-        <f t="shared" ref="AV43" si="48" xml:space="preserve"> _xlfn.FLOOR.MATH((AO43 - AR43) / 2)</f>
+        <f t="shared" ref="AV43" si="50" xml:space="preserve"> _xlfn.FLOOR.MATH((AO43 - AR43) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW43">
-        <f t="shared" ref="AW43" si="49" xml:space="preserve"> _xlfn.FLOOR.MATH((AP43 - AS43) / 2)</f>
+        <f t="shared" ref="AW43" si="51" xml:space="preserve"> _xlfn.FLOOR.MATH((AP43 - AS43) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX43" t="s">
@@ -8767,7 +8766,7 @@
         <v>1</v>
       </c>
       <c r="U44">
-        <f t="shared" ref="U44" si="50" xml:space="preserve"> S44 + T44</f>
+        <f t="shared" ref="U44" si="52" xml:space="preserve"> S44 + T44</f>
         <v>6</v>
       </c>
       <c r="V44" t="s">
@@ -8798,7 +8797,7 @@
         <v>6085</v>
       </c>
       <c r="AF44">
-        <f>AC44+AE44</f>
+        <f t="shared" ref="AF44:AF63" si="53">AC44+AE44</f>
         <v>81052</v>
       </c>
       <c r="AG44" t="s">
@@ -8808,7 +8807,7 @@
         <v>8</v>
       </c>
       <c r="AI44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ44" s="1">
@@ -8845,15 +8844,15 @@
         <v>50</v>
       </c>
       <c r="AU44" s="1">
-        <f t="shared" ref="AU44" si="51" xml:space="preserve"> _xlfn.FLOOR.MATH((AN44 - AQ44) / 2)</f>
+        <f t="shared" ref="AU44" si="54" xml:space="preserve"> _xlfn.FLOOR.MATH((AN44 - AQ44) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV44">
-        <f t="shared" ref="AV44" si="52" xml:space="preserve"> _xlfn.FLOOR.MATH((AO44 - AR44) / 2)</f>
+        <f t="shared" ref="AV44" si="55" xml:space="preserve"> _xlfn.FLOOR.MATH((AO44 - AR44) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW44">
-        <f t="shared" ref="AW44" si="53" xml:space="preserve"> _xlfn.FLOOR.MATH((AP44 - AS44) / 2)</f>
+        <f t="shared" ref="AW44" si="56" xml:space="preserve"> _xlfn.FLOOR.MATH((AP44 - AS44) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX44" t="s">
@@ -8937,7 +8936,7 @@
         <v>1</v>
       </c>
       <c r="U45" s="7">
-        <f t="shared" ref="U45:U63" si="54" xml:space="preserve"> S45 + T45</f>
+        <f t="shared" ref="U45:U63" si="57" xml:space="preserve"> S45 + T45</f>
         <v>6</v>
       </c>
       <c r="V45" s="7" t="s">
@@ -8968,7 +8967,7 @@
         <v>6087</v>
       </c>
       <c r="AF45" s="7">
-        <f>AC45+AE45</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG45" s="7" t="s">
@@ -8978,7 +8977,7 @@
         <v>8</v>
       </c>
       <c r="AI45" s="7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ45" s="8">
@@ -9015,15 +9014,15 @@
         <v>50</v>
       </c>
       <c r="AU45" s="8">
-        <f t="shared" ref="AU45" si="55" xml:space="preserve"> _xlfn.FLOOR.MATH((AN45 - AQ45) / 2)</f>
+        <f t="shared" ref="AU45" si="58" xml:space="preserve"> _xlfn.FLOOR.MATH((AN45 - AQ45) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV45" s="7">
-        <f t="shared" ref="AV45" si="56" xml:space="preserve"> _xlfn.FLOOR.MATH((AO45 - AR45) / 2)</f>
+        <f t="shared" ref="AV45" si="59" xml:space="preserve"> _xlfn.FLOOR.MATH((AO45 - AR45) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW45" s="7">
-        <f t="shared" ref="AW45" si="57" xml:space="preserve"> _xlfn.FLOOR.MATH((AP45 - AS45) / 2)</f>
+        <f t="shared" ref="AW45" si="60" xml:space="preserve"> _xlfn.FLOOR.MATH((AP45 - AS45) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX45" s="7" t="s">
@@ -9101,7 +9100,7 @@
         <v>1</v>
       </c>
       <c r="U46">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V46" t="s">
@@ -9132,7 +9131,7 @@
         <v>6085</v>
       </c>
       <c r="AF46">
-        <f>AC46+AE46</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG46" s="19" t="s">
@@ -9142,7 +9141,7 @@
         <v>130</v>
       </c>
       <c r="AI46">
-        <f t="shared" ref="AI46:AI63" si="58" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ46*AR46*AS46) * ((W46*X46 + Z46*AA46) / (3*16 + 1*8)) * (U46 / 5)</f>
+        <f t="shared" ref="AI46:AI63" si="61" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ46*AR46*AS46) * ((W46*X46 + Z46*AA46) / (3*16 + 1*8)) * (U46 / 5)</f>
         <v>74549.706201272769</v>
       </c>
       <c r="AJ46" s="18" t="s">
@@ -9179,15 +9178,15 @@
         <v>50</v>
       </c>
       <c r="AU46" s="1">
-        <f t="shared" ref="AU46:AU47" si="59" xml:space="preserve"> _xlfn.FLOOR.MATH((AN46 - AQ46) / 2)</f>
+        <f t="shared" ref="AU46:AU47" si="62" xml:space="preserve"> _xlfn.FLOOR.MATH((AN46 - AQ46) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV46">
-        <f t="shared" ref="AV46:AV47" si="60" xml:space="preserve"> _xlfn.FLOOR.MATH((AO46 - AR46) / 2)</f>
+        <f t="shared" ref="AV46:AV47" si="63" xml:space="preserve"> _xlfn.FLOOR.MATH((AO46 - AR46) / 2)</f>
         <v>192</v>
       </c>
       <c r="AW46">
-        <f t="shared" ref="AW46:AW47" si="61" xml:space="preserve"> _xlfn.FLOOR.MATH((AP46 - AS46) / 2)</f>
+        <f t="shared" ref="AW46:AW47" si="64" xml:space="preserve"> _xlfn.FLOOR.MATH((AP46 - AS46) / 2)</f>
         <v>15</v>
       </c>
       <c r="AX46" t="s">
@@ -9265,7 +9264,7 @@
         <v>1</v>
       </c>
       <c r="U47">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V47" t="s">
@@ -9296,7 +9295,7 @@
         <v>58019</v>
       </c>
       <c r="AF47">
-        <f>AC47+AE47</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG47" s="19" t="s">
@@ -9306,7 +9305,7 @@
         <v>130</v>
       </c>
       <c r="AI47">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>22708.360330151121</v>
       </c>
       <c r="AJ47" s="18" t="s">
@@ -9343,15 +9342,15 @@
         <v>50</v>
       </c>
       <c r="AU47" s="1">
-        <f t="shared" si="59"/>
+        <f t="shared" si="62"/>
         <v>30</v>
       </c>
       <c r="AV47">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>328</v>
       </c>
       <c r="AW47">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>79</v>
       </c>
       <c r="AX47" t="s">
@@ -9429,7 +9428,7 @@
         <v>1</v>
       </c>
       <c r="U48">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V48" t="s">
@@ -9460,7 +9459,7 @@
         <v>76313</v>
       </c>
       <c r="AF48">
-        <f>AC48+AE48</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG48" s="19" t="s">
@@ -9470,7 +9469,7 @@
         <v>130</v>
       </c>
       <c r="AI48">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>4158.1023826571118</v>
       </c>
       <c r="AJ48" s="18" t="s">
@@ -9507,15 +9506,15 @@
         <v>50</v>
       </c>
       <c r="AU48" s="1">
-        <f t="shared" ref="AU48:AU63" si="62" xml:space="preserve"> _xlfn.FLOOR.MATH((AN48 - AQ48) / 2)</f>
+        <f t="shared" ref="AU48:AU63" si="65" xml:space="preserve"> _xlfn.FLOOR.MATH((AN48 - AQ48) / 2)</f>
         <v>46</v>
       </c>
       <c r="AV48">
-        <f t="shared" ref="AV48:AV63" si="63" xml:space="preserve"> _xlfn.FLOOR.MATH((AO48 - AR48) / 2)</f>
+        <f t="shared" ref="AV48:AV63" si="66" xml:space="preserve"> _xlfn.FLOOR.MATH((AO48 - AR48) / 2)</f>
         <v>456</v>
       </c>
       <c r="AW48">
-        <f t="shared" ref="AW48:AW63" si="64" xml:space="preserve"> _xlfn.FLOOR.MATH((AP48 - AS48) / 2)</f>
+        <f t="shared" ref="AW48:AW63" si="67" xml:space="preserve"> _xlfn.FLOOR.MATH((AP48 - AS48) / 2)</f>
         <v>143</v>
       </c>
       <c r="AX48" t="s">
@@ -9593,7 +9592,7 @@
         <v>1</v>
       </c>
       <c r="U49">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V49" t="s">
@@ -9624,7 +9623,7 @@
         <v>6199</v>
       </c>
       <c r="AF49">
-        <f>AC49+AE49</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG49" s="19" t="s">
@@ -9634,7 +9633,7 @@
         <v>130</v>
       </c>
       <c r="AI49">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>53680.666010342022</v>
       </c>
       <c r="AJ49" s="18" t="s">
@@ -9671,15 +9670,15 @@
         <v>50</v>
       </c>
       <c r="AU49" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>14</v>
       </c>
       <c r="AV49">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>192</v>
       </c>
       <c r="AW49">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>15</v>
       </c>
       <c r="AX49" t="s">
@@ -9757,7 +9756,7 @@
         <v>1</v>
       </c>
       <c r="U50">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V50" t="s">
@@ -9788,7 +9787,7 @@
         <v>58053</v>
       </c>
       <c r="AF50">
-        <f>AC50+AE50</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG50" s="19" t="s">
@@ -9798,7 +9797,7 @@
         <v>130</v>
       </c>
       <c r="AI50">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>16651.133245255118</v>
       </c>
       <c r="AJ50" s="18" t="s">
@@ -9835,15 +9834,15 @@
         <v>50</v>
       </c>
       <c r="AU50" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>30</v>
       </c>
       <c r="AV50">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>328</v>
       </c>
       <c r="AW50">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>79</v>
       </c>
       <c r="AX50" t="s">
@@ -9921,7 +9920,7 @@
         <v>1</v>
       </c>
       <c r="U51">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V51" t="s">
@@ -9952,7 +9951,7 @@
         <v>76325</v>
       </c>
       <c r="AF51">
-        <f>AC51+AE51</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG51" s="19" t="s">
@@ -9962,7 +9961,7 @@
         <v>130</v>
       </c>
       <c r="AI51">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>3400.9489970451114</v>
       </c>
       <c r="AJ51" s="18" t="s">
@@ -9999,15 +9998,15 @@
         <v>50</v>
       </c>
       <c r="AU51" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>46</v>
       </c>
       <c r="AV51">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>456</v>
       </c>
       <c r="AW51">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>143</v>
       </c>
       <c r="AX51" t="s">
@@ -10085,7 +10084,7 @@
         <v>1</v>
       </c>
       <c r="U52">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V52" t="s">
@@ -10116,7 +10115,7 @@
         <v>6309</v>
       </c>
       <c r="AF52">
-        <f>AC52+AE52</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG52" s="19" t="s">
@@ -10126,7 +10125,7 @@
         <v>130</v>
       </c>
       <c r="AI52">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>32811.625819411252</v>
       </c>
       <c r="AJ52" s="18" t="s">
@@ -10163,15 +10162,15 @@
         <v>50</v>
       </c>
       <c r="AU52" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>14</v>
       </c>
       <c r="AV52">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>192</v>
       </c>
       <c r="AW52">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>15</v>
       </c>
       <c r="AX52" t="s">
@@ -10249,7 +10248,7 @@
         <v>1</v>
       </c>
       <c r="U53">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V53" t="s">
@@ -10280,7 +10279,7 @@
         <v>58085</v>
       </c>
       <c r="AF53">
-        <f>AC53+AE53</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG53" s="19" t="s">
@@ -10290,7 +10289,7 @@
         <v>130</v>
       </c>
       <c r="AI53">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>10593.906160359114</v>
       </c>
       <c r="AJ53" s="18" t="s">
@@ -10327,15 +10326,15 @@
         <v>50</v>
       </c>
       <c r="AU53" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>30</v>
       </c>
       <c r="AV53">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>328</v>
       </c>
       <c r="AW53">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>79</v>
       </c>
       <c r="AX53" t="s">
@@ -10413,7 +10412,7 @@
         <v>1</v>
       </c>
       <c r="U54">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V54" t="s">
@@ -10444,7 +10443,7 @@
         <v>76325</v>
       </c>
       <c r="AF54">
-        <f>AC54+AE54</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG54" s="19" t="s">
@@ -10454,7 +10453,7 @@
         <v>130</v>
       </c>
       <c r="AI54">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2643.7956114331109</v>
       </c>
       <c r="AJ54" s="18" t="s">
@@ -10491,15 +10490,15 @@
         <v>50</v>
       </c>
       <c r="AU54" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>46</v>
       </c>
       <c r="AV54">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>456</v>
       </c>
       <c r="AW54">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>143</v>
       </c>
       <c r="AX54" t="s">
@@ -10577,7 +10576,7 @@
         <v>1</v>
       </c>
       <c r="U55">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V55" t="s">
@@ -10608,7 +10607,7 @@
         <v>6087</v>
       </c>
       <c r="AF55">
-        <f>AC55+AE55</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG55" s="19" t="s">
@@ -10618,7 +10617,7 @@
         <v>130</v>
       </c>
       <c r="AI55">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>43246.145914876637</v>
       </c>
       <c r="AJ55" s="18" t="s">
@@ -10655,15 +10654,15 @@
         <v>50</v>
       </c>
       <c r="AU55" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>14</v>
       </c>
       <c r="AV55">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>192</v>
       </c>
       <c r="AW55">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>15</v>
       </c>
       <c r="AX55" t="s">
@@ -10741,7 +10740,7 @@
         <v>1</v>
       </c>
       <c r="U56">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V56" t="s">
@@ -10772,7 +10771,7 @@
         <v>58019</v>
       </c>
       <c r="AF56">
-        <f>AC56+AE56</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG56" s="19" t="s">
@@ -10782,7 +10781,7 @@
         <v>130</v>
       </c>
       <c r="AI56">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>13622.519702807114</v>
       </c>
       <c r="AJ56" s="18" t="s">
@@ -10819,15 +10818,15 @@
         <v>50</v>
       </c>
       <c r="AU56" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>30</v>
       </c>
       <c r="AV56">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>328</v>
       </c>
       <c r="AW56">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>79</v>
       </c>
       <c r="AX56" t="s">
@@ -10905,7 +10904,7 @@
         <v>1</v>
       </c>
       <c r="U57">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V57" t="s">
@@ -10936,7 +10935,7 @@
         <v>76313</v>
       </c>
       <c r="AF57">
-        <f>AC57+AE57</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG57" s="19" t="s">
@@ -10946,7 +10945,7 @@
         <v>130</v>
       </c>
       <c r="AI57">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>3022.3723042391107</v>
       </c>
       <c r="AJ57" s="18" t="s">
@@ -10983,15 +10982,15 @@
         <v>50</v>
       </c>
       <c r="AU57" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>46</v>
       </c>
       <c r="AV57">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>456</v>
       </c>
       <c r="AW57">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>143</v>
       </c>
       <c r="AX57" t="s">
@@ -11069,7 +11068,7 @@
         <v>1</v>
       </c>
       <c r="U58">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V58" t="s">
@@ -11100,7 +11099,7 @@
         <v>6199</v>
       </c>
       <c r="AF58">
-        <f>AC58+AE58</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG58" s="19" t="s">
@@ -11110,7 +11109,7 @@
         <v>130</v>
       </c>
       <c r="AI58">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>32811.625819411252</v>
       </c>
       <c r="AJ58" s="18" t="s">
@@ -11147,15 +11146,15 @@
         <v>50</v>
       </c>
       <c r="AU58" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>14</v>
       </c>
       <c r="AV58">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>192</v>
       </c>
       <c r="AW58">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>15</v>
       </c>
       <c r="AX58" t="s">
@@ -11233,7 +11232,7 @@
         <v>1</v>
       </c>
       <c r="U59">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V59" t="s">
@@ -11264,7 +11263,7 @@
         <v>58053</v>
       </c>
       <c r="AF59">
-        <f>AC59+AE59</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG59" s="19" t="s">
@@ -11274,7 +11273,7 @@
         <v>130</v>
       </c>
       <c r="AI59">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>10593.906160359114</v>
       </c>
       <c r="AJ59" s="18" t="s">
@@ -11311,15 +11310,15 @@
         <v>50</v>
       </c>
       <c r="AU59" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>30</v>
       </c>
       <c r="AV59">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>328</v>
       </c>
       <c r="AW59">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>79</v>
       </c>
       <c r="AX59" t="s">
@@ -11397,7 +11396,7 @@
         <v>1</v>
       </c>
       <c r="U60">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V60" t="s">
@@ -11428,7 +11427,7 @@
         <v>76325</v>
       </c>
       <c r="AF60">
-        <f>AC60+AE60</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG60" s="19" t="s">
@@ -11438,7 +11437,7 @@
         <v>130</v>
       </c>
       <c r="AI60">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2643.7956114331109</v>
       </c>
       <c r="AJ60" s="18" t="s">
@@ -11475,15 +11474,15 @@
         <v>50</v>
       </c>
       <c r="AU60" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>46</v>
       </c>
       <c r="AV60">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>456</v>
       </c>
       <c r="AW60">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>143</v>
       </c>
       <c r="AX60" t="s">
@@ -11561,7 +11560,7 @@
         <v>1</v>
       </c>
       <c r="U61">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V61" t="s">
@@ -11592,7 +11591,7 @@
         <v>6309</v>
       </c>
       <c r="AF61">
-        <f>AC61+AE61</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG61" s="19" t="s">
@@ -11602,7 +11601,7 @@
         <v>130</v>
       </c>
       <c r="AI61">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>22377.105723945871</v>
       </c>
       <c r="AJ61" s="18" t="s">
@@ -11639,15 +11638,15 @@
         <v>50</v>
       </c>
       <c r="AU61" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>14</v>
       </c>
       <c r="AV61">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>192</v>
       </c>
       <c r="AW61">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>15</v>
       </c>
       <c r="AX61" t="s">
@@ -11725,7 +11724,7 @@
         <v>1</v>
       </c>
       <c r="U62">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V62" t="s">
@@ -11756,7 +11755,7 @@
         <v>58085</v>
       </c>
       <c r="AF62">
-        <f>AC62+AE62</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG62" s="19" t="s">
@@ -11766,7 +11765,7 @@
         <v>130</v>
       </c>
       <c r="AI62">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>7565.2926179111128</v>
       </c>
       <c r="AJ62" s="18" t="s">
@@ -11803,15 +11802,15 @@
         <v>50</v>
       </c>
       <c r="AU62" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>30</v>
       </c>
       <c r="AV62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>328</v>
       </c>
       <c r="AW62">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>79</v>
       </c>
       <c r="AX62" t="s">
@@ -11889,7 +11888,7 @@
         <v>1</v>
       </c>
       <c r="U63">
-        <f t="shared" si="54"/>
+        <f t="shared" si="57"/>
         <v>6</v>
       </c>
       <c r="V63" t="s">
@@ -11920,7 +11919,7 @@
         <v>76325</v>
       </c>
       <c r="AF63">
-        <f>AC63+AE63</f>
+        <f t="shared" si="53"/>
         <v>81052</v>
       </c>
       <c r="AG63" s="19" t="s">
@@ -11930,7 +11929,7 @@
         <v>130</v>
       </c>
       <c r="AI63">
-        <f t="shared" si="58"/>
+        <f t="shared" si="61"/>
         <v>2265.2189186271103</v>
       </c>
       <c r="AJ63" s="18" t="s">
@@ -11967,15 +11966,15 @@
         <v>50</v>
       </c>
       <c r="AU63" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>46</v>
       </c>
       <c r="AV63">
-        <f t="shared" si="63"/>
+        <f t="shared" si="66"/>
         <v>456</v>
       </c>
       <c r="AW63">
-        <f t="shared" si="64"/>
+        <f t="shared" si="67"/>
         <v>143</v>
       </c>
       <c r="AX63" t="s">
@@ -12085,7 +12084,7 @@
       <c r="AC69" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="AD69" s="23"/>
+      <c r="AD69" s="19"/>
       <c r="AE69" s="19" t="s">
         <v>130</v>
       </c>
@@ -12133,15 +12132,15 @@
         <v>130</v>
       </c>
       <c r="AU69" s="1" t="e">
-        <f t="shared" ref="AU69" si="65" xml:space="preserve"> _xlfn.FLOOR.MATH((AN69 - AQ69) / 2)</f>
+        <f t="shared" ref="AU69" si="68" xml:space="preserve"> _xlfn.FLOOR.MATH((AN69 - AQ69) / 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AV69" t="e">
-        <f t="shared" ref="AV69" si="66" xml:space="preserve"> _xlfn.FLOOR.MATH((AO69 - AR69) / 2)</f>
+        <f t="shared" ref="AV69" si="69" xml:space="preserve"> _xlfn.FLOOR.MATH((AO69 - AR69) / 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AW69" t="e">
-        <f t="shared" ref="AW69" si="67" xml:space="preserve"> _xlfn.FLOOR.MATH((AP69 - AS69) / 2)</f>
+        <f t="shared" ref="AW69" si="70" xml:space="preserve"> _xlfn.FLOOR.MATH((AP69 - AS69) / 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AX69" t="s">

</xml_diff>

<commit_message>
prepare fluo single channel train3dunet run
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4479ECC5-EA09-429F-9FA9-8AB5B7937757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CAC8B0-04B4-4008-BE14-D4F502516981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="281">
   <si>
     <t>patch z</t>
   </si>
@@ -864,13 +864,22 @@
     <t>The val eval scores plateaud higher (by .05) but the peek was about the same. Nvidia-smi.log files were created again: Needs a `cd ~/data/cloud; bash pull-script.sh` (or just proper handling of working directory and sourced script files).</t>
   </si>
   <si>
-    <t>Get fluorescence segmentation to work - since autofluorescence segmentation models did reach usable predictive powers, I am switching to the classical fluo. Segm. Approach instead of the unconventional autofluorescence segmentation.</t>
-  </si>
-  <si>
     <t>I expect, 3dunet will have a substantially easier time predicting validation targets since the tissue of interest is fluorescently marked. It might have a hard time ignoring the eyes in the heart stains but I think it will manage.</t>
   </si>
   <si>
     <t>patch = arbitrary even int_2^3 as large a possible, confirmed (slightly) updated formula considered</t>
+  </si>
+  <si>
+    <t>231007-0</t>
+  </si>
+  <si>
+    <t>dataset07.0</t>
+  </si>
+  <si>
+    <t>Get fluorescence segmentation to work - since autofluorescence segmentation models did reach usable predictive powers, I am switching to the classical fluo. Segm. Approach instead of the unconventional autofluorescence segmentation. The train-config.yml file was adapted to session 230910-7, which is so far the best performing model, based on tensorboard metrics (val eval score is the most relevant metric / was the most relevant metric for the decision) and prediction images - this regards things like patience and validate_after_iters hyper parameters.</t>
+  </si>
+  <si>
+    <t>TBD (compare to session 230910-7)</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1068,11 +1077,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1389,61 +1396,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:AZ76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI38" zoomScale="73" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AV65" sqref="AV65"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="73" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="64.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="14.5546875" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="30.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="9.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="64.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="14.5703125" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="17" width="9.109375" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="12.88671875" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="9.109375" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="6.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="5.109375" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="11.109375" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="17" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="12.85546875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="6.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="5.140625" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="11.140625" customWidth="1" outlineLevel="1"/>
     <col min="25" max="25" width="6" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="7.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="8.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="15.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="7.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="9.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="16.6640625" style="10" customWidth="1"/>
-    <col min="33" max="34" width="14.88671875" customWidth="1"/>
+    <col min="26" max="26" width="14.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="7.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="8.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="15.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="7.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="9.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="16.7109375" style="10" customWidth="1"/>
+    <col min="33" max="34" width="14.85546875" customWidth="1"/>
     <col min="35" max="35" width="21" customWidth="1"/>
-    <col min="36" max="36" width="26.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="26.28515625" customWidth="1" outlineLevel="1"/>
     <col min="37" max="37" width="6" style="10" bestFit="1" customWidth="1"/>
     <col min="38" max="39" width="6" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.33203125" style="1" customWidth="1"/>
-    <col min="41" max="41" width="6.109375" customWidth="1"/>
+    <col min="40" max="40" width="5.28515625" style="1" customWidth="1"/>
+    <col min="41" max="41" width="6.140625" customWidth="1"/>
     <col min="42" max="43" width="5" customWidth="1"/>
-    <col min="44" max="44" width="6.109375" style="1" customWidth="1"/>
-    <col min="45" max="45" width="6.5546875" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="6.5703125" customWidth="1"/>
     <col min="46" max="46" width="5" customWidth="1"/>
     <col min="47" max="47" width="6" customWidth="1"/>
-    <col min="48" max="48" width="74.88671875" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="74.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="5.109375" customWidth="1"/>
-    <col min="51" max="51" width="73.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="74.85546875" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="74.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="5.140625" customWidth="1"/>
+    <col min="51" max="51" width="73.85546875" customWidth="1" outlineLevel="1"/>
     <col min="52" max="52" width="206" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.6640625" customWidth="1"/>
-    <col min="57" max="57" width="12.109375" customWidth="1"/>
+    <col min="53" max="53" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.7109375" customWidth="1"/>
+    <col min="57" max="57" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -1601,7 +1608,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -1760,7 +1767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -1920,7 +1927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:52" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:52" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>55</v>
       </c>
@@ -2079,7 +2086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2238,7 +2245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2397,7 +2404,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2556,7 +2563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2715,7 +2722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2880,7 +2887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -3039,7 +3046,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3198,7 +3205,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3358,7 +3365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -3517,7 +3524,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -3676,7 +3683,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -3836,7 +3843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
@@ -3996,7 +4003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -4156,7 +4163,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -4316,7 +4323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -4476,7 +4483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -4636,7 +4643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -4796,7 +4803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -4956,7 +4963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5116,7 +5123,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -5276,7 +5283,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -5434,7 +5441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>104</v>
       </c>
@@ -5592,7 +5599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -5756,7 +5763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -5919,7 +5926,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -6083,7 +6090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -6247,7 +6254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>152</v>
       </c>
@@ -6411,7 +6418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>159</v>
       </c>
@@ -6574,7 +6581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>172</v>
       </c>
@@ -6737,7 +6744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>173</v>
       </c>
@@ -6842,7 +6849,7 @@
         <v>81052</v>
       </c>
       <c r="AI34">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN34*AO34*AP34) / 5 * X34</f>
+        <f t="shared" ref="AI34:AI45" si="14" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN34*AO34*AP34) / 5 * X34</f>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ34" t="s">
@@ -6900,7 +6907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>182</v>
       </c>
@@ -6971,7 +6978,7 @@
         <v>1</v>
       </c>
       <c r="X35">
-        <f t="shared" ref="X35" si="14" xml:space="preserve"> V35 + W35</f>
+        <f t="shared" ref="X35" si="15" xml:space="preserve"> V35 + W35</f>
         <v>6</v>
       </c>
       <c r="Y35" t="s">
@@ -7005,7 +7012,7 @@
         <v>81052</v>
       </c>
       <c r="AI35">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN35*AO35*AP35) / 5 * X35</f>
+        <f t="shared" si="14"/>
         <v>76071.407048528155</v>
       </c>
       <c r="AJ35" t="s">
@@ -7033,15 +7040,15 @@
         <v>49</v>
       </c>
       <c r="AR35" s="1">
-        <f t="shared" ref="AR35" si="15" xml:space="preserve"> _xlfn.FLOOR.MATH((AK35 - AN35) / 2)</f>
+        <f t="shared" ref="AR35" si="16" xml:space="preserve"> _xlfn.FLOOR.MATH((AK35 - AN35) / 2)</f>
         <v>13</v>
       </c>
       <c r="AS35">
-        <f t="shared" ref="AS35" si="16" xml:space="preserve"> _xlfn.FLOOR.MATH((AL35 - AO35) / 2)</f>
+        <f t="shared" ref="AS35" si="17" xml:space="preserve"> _xlfn.FLOOR.MATH((AL35 - AO35) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT35">
-        <f t="shared" ref="AT35" si="17" xml:space="preserve"> _xlfn.FLOOR.MATH((AM35 - AP35) / 2)</f>
+        <f t="shared" ref="AT35" si="18" xml:space="preserve"> _xlfn.FLOOR.MATH((AM35 - AP35) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU35" t="s">
@@ -7063,7 +7070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>187</v>
       </c>
@@ -7134,7 +7141,7 @@
         <v>1</v>
       </c>
       <c r="X36">
-        <f t="shared" ref="X36" si="18" xml:space="preserve"> V36 + W36</f>
+        <f t="shared" ref="X36" si="19" xml:space="preserve"> V36 + W36</f>
         <v>6</v>
       </c>
       <c r="Y36" t="s">
@@ -7168,7 +7175,7 @@
         <v>81052</v>
       </c>
       <c r="AI36">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN36*AO36*AP36) / 5 * X36</f>
+        <f t="shared" si="14"/>
         <v>76071.407048528155</v>
       </c>
       <c r="AJ36" t="s">
@@ -7196,15 +7203,15 @@
         <v>49</v>
       </c>
       <c r="AR36" s="1">
-        <f t="shared" ref="AR36" si="19" xml:space="preserve"> _xlfn.FLOOR.MATH((AK36 - AN36) / 2)</f>
+        <f t="shared" ref="AR36" si="20" xml:space="preserve"> _xlfn.FLOOR.MATH((AK36 - AN36) / 2)</f>
         <v>13</v>
       </c>
       <c r="AS36">
-        <f t="shared" ref="AS36" si="20" xml:space="preserve"> _xlfn.FLOOR.MATH((AL36 - AO36) / 2)</f>
+        <f t="shared" ref="AS36" si="21" xml:space="preserve"> _xlfn.FLOOR.MATH((AL36 - AO36) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT36">
-        <f t="shared" ref="AT36" si="21" xml:space="preserve"> _xlfn.FLOOR.MATH((AM36 - AP36) / 2)</f>
+        <f t="shared" ref="AT36" si="22" xml:space="preserve"> _xlfn.FLOOR.MATH((AM36 - AP36) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU36" t="s">
@@ -7226,7 +7233,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>190</v>
       </c>
@@ -7297,7 +7304,7 @@
         <v>1</v>
       </c>
       <c r="X37">
-        <f t="shared" ref="X37" si="22" xml:space="preserve"> V37 + W37</f>
+        <f t="shared" ref="X37" si="23" xml:space="preserve"> V37 + W37</f>
         <v>6</v>
       </c>
       <c r="Y37" t="s">
@@ -7331,7 +7338,7 @@
         <v>81052</v>
       </c>
       <c r="AI37">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN37*AO37*AP37) / 5 * X37</f>
+        <f t="shared" si="14"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ37" t="s">
@@ -7359,15 +7366,15 @@
         <v>49</v>
       </c>
       <c r="AR37" s="1">
-        <f t="shared" ref="AR37" si="23" xml:space="preserve"> _xlfn.FLOOR.MATH((AK37 - AN37) / 2)</f>
+        <f t="shared" ref="AR37" si="24" xml:space="preserve"> _xlfn.FLOOR.MATH((AK37 - AN37) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS37">
-        <f t="shared" ref="AS37" si="24" xml:space="preserve"> _xlfn.FLOOR.MATH((AL37 - AO37) / 2)</f>
+        <f t="shared" ref="AS37" si="25" xml:space="preserve"> _xlfn.FLOOR.MATH((AL37 - AO37) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT37">
-        <f t="shared" ref="AT37" si="25" xml:space="preserve"> _xlfn.FLOOR.MATH((AM37 - AP37) / 2)</f>
+        <f t="shared" ref="AT37" si="26" xml:space="preserve"> _xlfn.FLOOR.MATH((AM37 - AP37) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU37" t="s">
@@ -7389,7 +7396,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>195</v>
       </c>
@@ -7460,7 +7467,7 @@
         <v>1</v>
       </c>
       <c r="X38">
-        <f t="shared" ref="X38" si="26" xml:space="preserve"> V38 + W38</f>
+        <f t="shared" ref="X38" si="27" xml:space="preserve"> V38 + W38</f>
         <v>6</v>
       </c>
       <c r="Y38" t="s">
@@ -7494,7 +7501,7 @@
         <v>81052</v>
       </c>
       <c r="AI38">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN38*AO38*AP38) / 5 * X38</f>
+        <f t="shared" si="14"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ38" t="s">
@@ -7522,15 +7529,15 @@
         <v>49</v>
       </c>
       <c r="AR38" s="1">
-        <f t="shared" ref="AR38" si="27" xml:space="preserve"> _xlfn.FLOOR.MATH((AK38 - AN38) / 2)</f>
+        <f t="shared" ref="AR38" si="28" xml:space="preserve"> _xlfn.FLOOR.MATH((AK38 - AN38) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS38">
-        <f t="shared" ref="AS38" si="28" xml:space="preserve"> _xlfn.FLOOR.MATH((AL38 - AO38) / 2)</f>
+        <f t="shared" ref="AS38" si="29" xml:space="preserve"> _xlfn.FLOOR.MATH((AL38 - AO38) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT38">
-        <f t="shared" ref="AT38" si="29" xml:space="preserve"> _xlfn.FLOOR.MATH((AM38 - AP38) / 2)</f>
+        <f t="shared" ref="AT38" si="30" xml:space="preserve"> _xlfn.FLOOR.MATH((AM38 - AP38) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU38" t="s">
@@ -7552,7 +7559,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>198</v>
       </c>
@@ -7623,7 +7630,7 @@
         <v>1</v>
       </c>
       <c r="X39">
-        <f t="shared" ref="X39" si="30" xml:space="preserve"> V39 + W39</f>
+        <f t="shared" ref="X39" si="31" xml:space="preserve"> V39 + W39</f>
         <v>6</v>
       </c>
       <c r="Y39" t="s">
@@ -7657,7 +7664,7 @@
         <v>81052</v>
       </c>
       <c r="AI39">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN39*AO39*AP39) / 5 * X39</f>
+        <f t="shared" si="14"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ39" t="s">
@@ -7685,15 +7692,15 @@
         <v>49</v>
       </c>
       <c r="AR39" s="1">
-        <f t="shared" ref="AR39" si="31" xml:space="preserve"> _xlfn.FLOOR.MATH((AK39 - AN39) / 2)</f>
+        <f t="shared" ref="AR39" si="32" xml:space="preserve"> _xlfn.FLOOR.MATH((AK39 - AN39) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS39">
-        <f t="shared" ref="AS39" si="32" xml:space="preserve"> _xlfn.FLOOR.MATH((AL39 - AO39) / 2)</f>
+        <f t="shared" ref="AS39" si="33" xml:space="preserve"> _xlfn.FLOOR.MATH((AL39 - AO39) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT39">
-        <f t="shared" ref="AT39" si="33" xml:space="preserve"> _xlfn.FLOOR.MATH((AM39 - AP39) / 2)</f>
+        <f t="shared" ref="AT39" si="34" xml:space="preserve"> _xlfn.FLOOR.MATH((AM39 - AP39) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU39" t="s">
@@ -7715,7 +7722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>202</v>
       </c>
@@ -7786,7 +7793,7 @@
         <v>1</v>
       </c>
       <c r="X40">
-        <f t="shared" ref="X40" si="34" xml:space="preserve"> V40 + W40</f>
+        <f t="shared" ref="X40" si="35" xml:space="preserve"> V40 + W40</f>
         <v>6</v>
       </c>
       <c r="Y40" t="s">
@@ -7820,7 +7827,7 @@
         <v>81052</v>
       </c>
       <c r="AI40">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN40*AO40*AP40) / 5 * X40</f>
+        <f t="shared" si="14"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ40" t="s">
@@ -7848,15 +7855,15 @@
         <v>49</v>
       </c>
       <c r="AR40" s="1">
-        <f t="shared" ref="AR40" si="35" xml:space="preserve"> _xlfn.FLOOR.MATH((AK40 - AN40) / 2)</f>
+        <f t="shared" ref="AR40" si="36" xml:space="preserve"> _xlfn.FLOOR.MATH((AK40 - AN40) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS40">
-        <f t="shared" ref="AS40" si="36" xml:space="preserve"> _xlfn.FLOOR.MATH((AL40 - AO40) / 2)</f>
+        <f t="shared" ref="AS40" si="37" xml:space="preserve"> _xlfn.FLOOR.MATH((AL40 - AO40) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT40">
-        <f t="shared" ref="AT40" si="37" xml:space="preserve"> _xlfn.FLOOR.MATH((AM40 - AP40) / 2)</f>
+        <f t="shared" ref="AT40" si="38" xml:space="preserve"> _xlfn.FLOOR.MATH((AM40 - AP40) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU40" t="s">
@@ -7878,7 +7885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>203</v>
       </c>
@@ -7949,7 +7956,7 @@
         <v>1</v>
       </c>
       <c r="X41">
-        <f t="shared" ref="X41" si="38" xml:space="preserve"> V41 + W41</f>
+        <f t="shared" ref="X41" si="39" xml:space="preserve"> V41 + W41</f>
         <v>6</v>
       </c>
       <c r="Y41" t="s">
@@ -7983,7 +7990,7 @@
         <v>81052</v>
       </c>
       <c r="AI41">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN41*AO41*AP41) / 5 * X41</f>
+        <f t="shared" si="14"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ41" t="s">
@@ -8011,15 +8018,15 @@
         <v>49</v>
       </c>
       <c r="AR41" s="1">
-        <f t="shared" ref="AR41" si="39" xml:space="preserve"> _xlfn.FLOOR.MATH((AK41 - AN41) / 2)</f>
+        <f t="shared" ref="AR41" si="40" xml:space="preserve"> _xlfn.FLOOR.MATH((AK41 - AN41) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS41">
-        <f t="shared" ref="AS41" si="40" xml:space="preserve"> _xlfn.FLOOR.MATH((AL41 - AO41) / 2)</f>
+        <f t="shared" ref="AS41" si="41" xml:space="preserve"> _xlfn.FLOOR.MATH((AL41 - AO41) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT41">
-        <f t="shared" ref="AT41" si="41" xml:space="preserve"> _xlfn.FLOOR.MATH((AM41 - AP41) / 2)</f>
+        <f t="shared" ref="AT41" si="42" xml:space="preserve"> _xlfn.FLOOR.MATH((AM41 - AP41) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU41" t="s">
@@ -8041,7 +8048,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>205</v>
       </c>
@@ -8112,7 +8119,7 @@
         <v>1</v>
       </c>
       <c r="X42">
-        <f t="shared" ref="X42" si="42" xml:space="preserve"> V42 + W42</f>
+        <f t="shared" ref="X42" si="43" xml:space="preserve"> V42 + W42</f>
         <v>6</v>
       </c>
       <c r="Y42" t="s">
@@ -8146,7 +8153,7 @@
         <v>81052</v>
       </c>
       <c r="AI42">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN42*AO42*AP42) / 5 * X42</f>
+        <f t="shared" si="14"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ42" t="s">
@@ -8174,15 +8181,15 @@
         <v>49</v>
       </c>
       <c r="AR42" s="1">
-        <f t="shared" ref="AR42" si="43" xml:space="preserve"> _xlfn.FLOOR.MATH((AK42 - AN42) / 2)</f>
+        <f t="shared" ref="AR42" si="44" xml:space="preserve"> _xlfn.FLOOR.MATH((AK42 - AN42) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS42">
-        <f t="shared" ref="AS42" si="44" xml:space="preserve"> _xlfn.FLOOR.MATH((AL42 - AO42) / 2)</f>
+        <f t="shared" ref="AS42" si="45" xml:space="preserve"> _xlfn.FLOOR.MATH((AL42 - AO42) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT42">
-        <f t="shared" ref="AT42" si="45" xml:space="preserve"> _xlfn.FLOOR.MATH((AM42 - AP42) / 2)</f>
+        <f t="shared" ref="AT42" si="46" xml:space="preserve"> _xlfn.FLOOR.MATH((AM42 - AP42) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU42" t="s">
@@ -8204,7 +8211,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>208</v>
       </c>
@@ -8275,7 +8282,7 @@
         <v>1</v>
       </c>
       <c r="X43">
-        <f t="shared" ref="X43" si="46" xml:space="preserve"> V43 + W43</f>
+        <f t="shared" ref="X43" si="47" xml:space="preserve"> V43 + W43</f>
         <v>6</v>
       </c>
       <c r="Y43" t="s">
@@ -8309,7 +8316,7 @@
         <v>81052</v>
       </c>
       <c r="AI43">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN43*AO43*AP43) / 5 * X43</f>
+        <f t="shared" si="14"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ43" t="s">
@@ -8337,15 +8344,15 @@
         <v>49</v>
       </c>
       <c r="AR43" s="1">
-        <f t="shared" ref="AR43" si="47" xml:space="preserve"> _xlfn.FLOOR.MATH((AK43 - AN43) / 2)</f>
+        <f t="shared" ref="AR43" si="48" xml:space="preserve"> _xlfn.FLOOR.MATH((AK43 - AN43) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS43">
-        <f t="shared" ref="AS43" si="48" xml:space="preserve"> _xlfn.FLOOR.MATH((AL43 - AO43) / 2)</f>
+        <f t="shared" ref="AS43" si="49" xml:space="preserve"> _xlfn.FLOOR.MATH((AL43 - AO43) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT43">
-        <f t="shared" ref="AT43" si="49" xml:space="preserve"> _xlfn.FLOOR.MATH((AM43 - AP43) / 2)</f>
+        <f t="shared" ref="AT43" si="50" xml:space="preserve"> _xlfn.FLOOR.MATH((AM43 - AP43) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU43" t="s">
@@ -8367,7 +8374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>209</v>
       </c>
@@ -8432,7 +8439,7 @@
         <v>1</v>
       </c>
       <c r="X44">
-        <f t="shared" ref="X44" si="50" xml:space="preserve"> V44 + W44</f>
+        <f t="shared" ref="X44" si="51" xml:space="preserve"> V44 + W44</f>
         <v>6</v>
       </c>
       <c r="Y44" t="s">
@@ -8463,11 +8470,11 @@
         <v>6085</v>
       </c>
       <c r="AH44">
-        <f t="shared" ref="AH44:AH63" si="51">AF44+AG44</f>
+        <f t="shared" ref="AH44:AH63" si="52">AF44+AG44</f>
         <v>81052</v>
       </c>
       <c r="AI44">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN44*AO44*AP44) / 5 * X44</f>
+        <f t="shared" si="14"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ44" t="s">
@@ -8495,15 +8502,15 @@
         <v>49</v>
       </c>
       <c r="AR44" s="1">
-        <f t="shared" ref="AR44" si="52" xml:space="preserve"> _xlfn.FLOOR.MATH((AK44 - AN44) / 2)</f>
+        <f t="shared" ref="AR44" si="53" xml:space="preserve"> _xlfn.FLOOR.MATH((AK44 - AN44) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS44">
-        <f t="shared" ref="AS44" si="53" xml:space="preserve"> _xlfn.FLOOR.MATH((AL44 - AO44) / 2)</f>
+        <f t="shared" ref="AS44" si="54" xml:space="preserve"> _xlfn.FLOOR.MATH((AL44 - AO44) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT44">
-        <f t="shared" ref="AT44" si="54" xml:space="preserve"> _xlfn.FLOOR.MATH((AM44 - AP44) / 2)</f>
+        <f t="shared" ref="AT44" si="55" xml:space="preserve"> _xlfn.FLOOR.MATH((AM44 - AP44) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU44" t="s">
@@ -8525,7 +8532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>210</v>
       </c>
@@ -8590,7 +8597,7 @@
         <v>1</v>
       </c>
       <c r="X45" s="7">
-        <f t="shared" ref="X45:X63" si="55" xml:space="preserve"> V45 + W45</f>
+        <f t="shared" ref="X45:X63" si="56" xml:space="preserve"> V45 + W45</f>
         <v>6</v>
       </c>
       <c r="Y45" s="7" t="s">
@@ -8621,11 +8628,11 @@
         <v>6087</v>
       </c>
       <c r="AH45" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI45" s="7">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN45*AO45*AP45) / 5 * X45</f>
+        <f t="shared" si="14"/>
         <v>74549.706201272784</v>
       </c>
       <c r="AJ45" s="7" t="s">
@@ -8653,15 +8660,15 @@
         <v>49</v>
       </c>
       <c r="AR45" s="8">
-        <f t="shared" ref="AR45" si="56" xml:space="preserve"> _xlfn.FLOOR.MATH((AK45 - AN45) / 2)</f>
+        <f t="shared" ref="AR45" si="57" xml:space="preserve"> _xlfn.FLOOR.MATH((AK45 - AN45) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS45" s="7">
-        <f t="shared" ref="AS45" si="57" xml:space="preserve"> _xlfn.FLOOR.MATH((AL45 - AO45) / 2)</f>
+        <f t="shared" ref="AS45" si="58" xml:space="preserve"> _xlfn.FLOOR.MATH((AL45 - AO45) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT45" s="7">
-        <f t="shared" ref="AT45" si="58" xml:space="preserve"> _xlfn.FLOOR.MATH((AM45 - AP45) / 2)</f>
+        <f t="shared" ref="AT45" si="59" xml:space="preserve"> _xlfn.FLOOR.MATH((AM45 - AP45) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU45" s="7" t="s">
@@ -8683,7 +8690,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>243</v>
       </c>
@@ -8748,7 +8755,7 @@
         <v>1</v>
       </c>
       <c r="X46">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y46" t="s">
@@ -8779,11 +8786,11 @@
         <v>6085</v>
       </c>
       <c r="AH46">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI46">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN46*AO46*AP46) * ((Z46*AA46 + AC46*AD46) / (3*16 + 1*8)) * (X46 / 5)</f>
+        <f t="shared" ref="AI46:AI63" si="60" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN46*AO46*AP46) * ((Z46*AA46 + AC46*AD46) / (3*16 + 1*8)) * (X46 / 5)</f>
         <v>74549.706201272769</v>
       </c>
       <c r="AJ46" t="s">
@@ -8811,15 +8818,15 @@
         <v>49</v>
       </c>
       <c r="AR46" s="1">
-        <f t="shared" ref="AR46:AR47" si="59" xml:space="preserve"> _xlfn.FLOOR.MATH((AK46 - AN46) / 2)</f>
+        <f t="shared" ref="AR46:AR47" si="61" xml:space="preserve"> _xlfn.FLOOR.MATH((AK46 - AN46) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS46">
-        <f t="shared" ref="AS46:AS47" si="60" xml:space="preserve"> _xlfn.FLOOR.MATH((AL46 - AO46) / 2)</f>
+        <f t="shared" ref="AS46:AS47" si="62" xml:space="preserve"> _xlfn.FLOOR.MATH((AL46 - AO46) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT46">
-        <f t="shared" ref="AT46:AT47" si="61" xml:space="preserve"> _xlfn.FLOOR.MATH((AM46 - AP46) / 2)</f>
+        <f t="shared" ref="AT46:AT47" si="63" xml:space="preserve"> _xlfn.FLOOR.MATH((AM46 - AP46) / 2)</f>
         <v>15</v>
       </c>
       <c r="AU46" t="s">
@@ -8841,7 +8848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>244</v>
       </c>
@@ -8906,7 +8913,7 @@
         <v>1</v>
       </c>
       <c r="X47">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y47" t="s">
@@ -8937,11 +8944,11 @@
         <v>58019</v>
       </c>
       <c r="AH47">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI47">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN47*AO47*AP47) * ((Z47*AA47 + AC47*AD47) / (3*16 + 1*8)) * (X47 / 5)</f>
+        <f t="shared" si="60"/>
         <v>22708.360330151121</v>
       </c>
       <c r="AJ47" t="s">
@@ -8969,15 +8976,15 @@
         <v>49</v>
       </c>
       <c r="AR47" s="1">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>30</v>
       </c>
       <c r="AS47">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>328</v>
       </c>
       <c r="AT47">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>79</v>
       </c>
       <c r="AU47" t="s">
@@ -8999,7 +9006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>245</v>
       </c>
@@ -9064,7 +9071,7 @@
         <v>1</v>
       </c>
       <c r="X48">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y48" t="s">
@@ -9095,11 +9102,11 @@
         <v>76313</v>
       </c>
       <c r="AH48">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI48">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN48*AO48*AP48) * ((Z48*AA48 + AC48*AD48) / (3*16 + 1*8)) * (X48 / 5)</f>
+        <f t="shared" si="60"/>
         <v>4158.1023826571118</v>
       </c>
       <c r="AJ48" t="s">
@@ -9127,15 +9134,15 @@
         <v>49</v>
       </c>
       <c r="AR48" s="1">
-        <f t="shared" ref="AR48:AR63" si="62" xml:space="preserve"> _xlfn.FLOOR.MATH((AK48 - AN48) / 2)</f>
+        <f t="shared" ref="AR48:AR63" si="64" xml:space="preserve"> _xlfn.FLOOR.MATH((AK48 - AN48) / 2)</f>
         <v>46</v>
       </c>
       <c r="AS48">
-        <f t="shared" ref="AS48:AS63" si="63" xml:space="preserve"> _xlfn.FLOOR.MATH((AL48 - AO48) / 2)</f>
+        <f t="shared" ref="AS48:AS63" si="65" xml:space="preserve"> _xlfn.FLOOR.MATH((AL48 - AO48) / 2)</f>
         <v>456</v>
       </c>
       <c r="AT48">
-        <f t="shared" ref="AT48:AT63" si="64" xml:space="preserve"> _xlfn.FLOOR.MATH((AM48 - AP48) / 2)</f>
+        <f t="shared" ref="AT48:AT63" si="66" xml:space="preserve"> _xlfn.FLOOR.MATH((AM48 - AP48) / 2)</f>
         <v>143</v>
       </c>
       <c r="AU48" t="s">
@@ -9157,7 +9164,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>246</v>
       </c>
@@ -9222,7 +9229,7 @@
         <v>1</v>
       </c>
       <c r="X49">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y49" t="s">
@@ -9253,11 +9260,11 @@
         <v>6199</v>
       </c>
       <c r="AH49">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI49">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN49*AO49*AP49) * ((Z49*AA49 + AC49*AD49) / (3*16 + 1*8)) * (X49 / 5)</f>
+        <f t="shared" si="60"/>
         <v>53680.666010342022</v>
       </c>
       <c r="AJ49" t="s">
@@ -9285,15 +9292,15 @@
         <v>49</v>
       </c>
       <c r="AR49" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>14</v>
       </c>
       <c r="AS49">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>192</v>
       </c>
       <c r="AT49">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>15</v>
       </c>
       <c r="AU49" t="s">
@@ -9315,7 +9322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>247</v>
       </c>
@@ -9380,7 +9387,7 @@
         <v>1</v>
       </c>
       <c r="X50">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y50" t="s">
@@ -9411,11 +9418,11 @@
         <v>58053</v>
       </c>
       <c r="AH50">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI50">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN50*AO50*AP50) * ((Z50*AA50 + AC50*AD50) / (3*16 + 1*8)) * (X50 / 5)</f>
+        <f t="shared" si="60"/>
         <v>16651.133245255118</v>
       </c>
       <c r="AJ50" t="s">
@@ -9443,15 +9450,15 @@
         <v>49</v>
       </c>
       <c r="AR50" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>30</v>
       </c>
       <c r="AS50">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>328</v>
       </c>
       <c r="AT50">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>79</v>
       </c>
       <c r="AU50" t="s">
@@ -9473,7 +9480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>248</v>
       </c>
@@ -9538,7 +9545,7 @@
         <v>1</v>
       </c>
       <c r="X51">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y51" t="s">
@@ -9569,11 +9576,11 @@
         <v>76325</v>
       </c>
       <c r="AH51">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI51">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN51*AO51*AP51) * ((Z51*AA51 + AC51*AD51) / (3*16 + 1*8)) * (X51 / 5)</f>
+        <f t="shared" si="60"/>
         <v>3400.9489970451114</v>
       </c>
       <c r="AJ51" t="s">
@@ -9601,15 +9608,15 @@
         <v>49</v>
       </c>
       <c r="AR51" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>46</v>
       </c>
       <c r="AS51">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>456</v>
       </c>
       <c r="AT51">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>143</v>
       </c>
       <c r="AU51" t="s">
@@ -9631,7 +9638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>249</v>
       </c>
@@ -9696,7 +9703,7 @@
         <v>1</v>
       </c>
       <c r="X52">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y52" t="s">
@@ -9727,11 +9734,11 @@
         <v>6309</v>
       </c>
       <c r="AH52">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI52">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN52*AO52*AP52) * ((Z52*AA52 + AC52*AD52) / (3*16 + 1*8)) * (X52 / 5)</f>
+        <f t="shared" si="60"/>
         <v>32811.625819411252</v>
       </c>
       <c r="AJ52" t="s">
@@ -9759,15 +9766,15 @@
         <v>49</v>
       </c>
       <c r="AR52" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>14</v>
       </c>
       <c r="AS52">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>192</v>
       </c>
       <c r="AT52">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>15</v>
       </c>
       <c r="AU52" t="s">
@@ -9789,7 +9796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>250</v>
       </c>
@@ -9854,7 +9861,7 @@
         <v>1</v>
       </c>
       <c r="X53">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y53" t="s">
@@ -9885,11 +9892,11 @@
         <v>58085</v>
       </c>
       <c r="AH53">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI53">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN53*AO53*AP53) * ((Z53*AA53 + AC53*AD53) / (3*16 + 1*8)) * (X53 / 5)</f>
+        <f t="shared" si="60"/>
         <v>10593.906160359114</v>
       </c>
       <c r="AJ53" t="s">
@@ -9917,15 +9924,15 @@
         <v>49</v>
       </c>
       <c r="AR53" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>30</v>
       </c>
       <c r="AS53">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>328</v>
       </c>
       <c r="AT53">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>79</v>
       </c>
       <c r="AU53" t="s">
@@ -9947,7 +9954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>251</v>
       </c>
@@ -10012,7 +10019,7 @@
         <v>1</v>
       </c>
       <c r="X54">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y54" t="s">
@@ -10043,11 +10050,11 @@
         <v>76325</v>
       </c>
       <c r="AH54">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI54">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN54*AO54*AP54) * ((Z54*AA54 + AC54*AD54) / (3*16 + 1*8)) * (X54 / 5)</f>
+        <f t="shared" si="60"/>
         <v>2643.7956114331109</v>
       </c>
       <c r="AJ54" t="s">
@@ -10075,15 +10082,15 @@
         <v>49</v>
       </c>
       <c r="AR54" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>46</v>
       </c>
       <c r="AS54">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>456</v>
       </c>
       <c r="AT54">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>143</v>
       </c>
       <c r="AU54" t="s">
@@ -10105,7 +10112,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>252</v>
       </c>
@@ -10170,7 +10177,7 @@
         <v>1</v>
       </c>
       <c r="X55">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y55" t="s">
@@ -10201,11 +10208,11 @@
         <v>6087</v>
       </c>
       <c r="AH55">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI55">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN55*AO55*AP55) * ((Z55*AA55 + AC55*AD55) / (3*16 + 1*8)) * (X55 / 5)</f>
+        <f t="shared" si="60"/>
         <v>43246.145914876637</v>
       </c>
       <c r="AJ55" t="s">
@@ -10233,15 +10240,15 @@
         <v>49</v>
       </c>
       <c r="AR55" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>14</v>
       </c>
       <c r="AS55">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>192</v>
       </c>
       <c r="AT55">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>15</v>
       </c>
       <c r="AU55" t="s">
@@ -10263,7 +10270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>253</v>
       </c>
@@ -10328,7 +10335,7 @@
         <v>1</v>
       </c>
       <c r="X56">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y56" t="s">
@@ -10359,11 +10366,11 @@
         <v>58019</v>
       </c>
       <c r="AH56">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI56">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN56*AO56*AP56) * ((Z56*AA56 + AC56*AD56) / (3*16 + 1*8)) * (X56 / 5)</f>
+        <f t="shared" si="60"/>
         <v>13622.519702807114</v>
       </c>
       <c r="AJ56" t="s">
@@ -10391,15 +10398,15 @@
         <v>49</v>
       </c>
       <c r="AR56" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>30</v>
       </c>
       <c r="AS56">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>328</v>
       </c>
       <c r="AT56">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>79</v>
       </c>
       <c r="AU56" t="s">
@@ -10421,7 +10428,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>254</v>
       </c>
@@ -10486,7 +10493,7 @@
         <v>1</v>
       </c>
       <c r="X57">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y57" t="s">
@@ -10517,11 +10524,11 @@
         <v>76313</v>
       </c>
       <c r="AH57">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI57">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN57*AO57*AP57) * ((Z57*AA57 + AC57*AD57) / (3*16 + 1*8)) * (X57 / 5)</f>
+        <f t="shared" si="60"/>
         <v>3022.3723042391107</v>
       </c>
       <c r="AJ57" t="s">
@@ -10549,15 +10556,15 @@
         <v>49</v>
       </c>
       <c r="AR57" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>46</v>
       </c>
       <c r="AS57">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>456</v>
       </c>
       <c r="AT57">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>143</v>
       </c>
       <c r="AU57" t="s">
@@ -10579,7 +10586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>255</v>
       </c>
@@ -10644,7 +10651,7 @@
         <v>1</v>
       </c>
       <c r="X58">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y58" t="s">
@@ -10675,11 +10682,11 @@
         <v>6199</v>
       </c>
       <c r="AH58">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI58">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN58*AO58*AP58) * ((Z58*AA58 + AC58*AD58) / (3*16 + 1*8)) * (X58 / 5)</f>
+        <f t="shared" si="60"/>
         <v>32811.625819411252</v>
       </c>
       <c r="AJ58" t="s">
@@ -10707,15 +10714,15 @@
         <v>49</v>
       </c>
       <c r="AR58" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>14</v>
       </c>
       <c r="AS58">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>192</v>
       </c>
       <c r="AT58">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>15</v>
       </c>
       <c r="AU58" t="s">
@@ -10737,7 +10744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>256</v>
       </c>
@@ -10802,7 +10809,7 @@
         <v>1</v>
       </c>
       <c r="X59">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y59" t="s">
@@ -10833,11 +10840,11 @@
         <v>58053</v>
       </c>
       <c r="AH59">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI59">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN59*AO59*AP59) * ((Z59*AA59 + AC59*AD59) / (3*16 + 1*8)) * (X59 / 5)</f>
+        <f t="shared" si="60"/>
         <v>10593.906160359114</v>
       </c>
       <c r="AJ59" t="s">
@@ -10865,15 +10872,15 @@
         <v>49</v>
       </c>
       <c r="AR59" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>30</v>
       </c>
       <c r="AS59">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>328</v>
       </c>
       <c r="AT59">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>79</v>
       </c>
       <c r="AU59" t="s">
@@ -10895,7 +10902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>257</v>
       </c>
@@ -10960,7 +10967,7 @@
         <v>1</v>
       </c>
       <c r="X60">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y60" t="s">
@@ -10991,11 +10998,11 @@
         <v>76325</v>
       </c>
       <c r="AH60">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI60">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN60*AO60*AP60) * ((Z60*AA60 + AC60*AD60) / (3*16 + 1*8)) * (X60 / 5)</f>
+        <f t="shared" si="60"/>
         <v>2643.7956114331109</v>
       </c>
       <c r="AJ60" t="s">
@@ -11023,15 +11030,15 @@
         <v>49</v>
       </c>
       <c r="AR60" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>46</v>
       </c>
       <c r="AS60">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>456</v>
       </c>
       <c r="AT60">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>143</v>
       </c>
       <c r="AU60" t="s">
@@ -11053,7 +11060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>258</v>
       </c>
@@ -11118,7 +11125,7 @@
         <v>1</v>
       </c>
       <c r="X61">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y61" t="s">
@@ -11149,11 +11156,11 @@
         <v>6309</v>
       </c>
       <c r="AH61">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI61">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN61*AO61*AP61) * ((Z61*AA61 + AC61*AD61) / (3*16 + 1*8)) * (X61 / 5)</f>
+        <f t="shared" si="60"/>
         <v>22377.105723945871</v>
       </c>
       <c r="AJ61" t="s">
@@ -11181,15 +11188,15 @@
         <v>49</v>
       </c>
       <c r="AR61" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>14</v>
       </c>
       <c r="AS61">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>192</v>
       </c>
       <c r="AT61">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>15</v>
       </c>
       <c r="AU61" t="s">
@@ -11211,7 +11218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>259</v>
       </c>
@@ -11276,7 +11283,7 @@
         <v>1</v>
       </c>
       <c r="X62">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y62" t="s">
@@ -11307,11 +11314,11 @@
         <v>58085</v>
       </c>
       <c r="AH62">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI62">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN62*AO62*AP62) * ((Z62*AA62 + AC62*AD62) / (3*16 + 1*8)) * (X62 / 5)</f>
+        <f t="shared" si="60"/>
         <v>7565.2926179111128</v>
       </c>
       <c r="AJ62" t="s">
@@ -11339,15 +11346,15 @@
         <v>49</v>
       </c>
       <c r="AR62" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>30</v>
       </c>
       <c r="AS62">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>328</v>
       </c>
       <c r="AT62">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>79</v>
       </c>
       <c r="AU62" t="s">
@@ -11369,7 +11376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
         <v>260</v>
       </c>
@@ -11434,7 +11441,7 @@
         <v>1</v>
       </c>
       <c r="X63" s="7">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>6</v>
       </c>
       <c r="Y63" s="7" t="s">
@@ -11465,11 +11472,11 @@
         <v>76325</v>
       </c>
       <c r="AH63" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>81052</v>
       </c>
       <c r="AI63" s="7">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AN63*AO63*AP63) * ((Z63*AA63 + AC63*AD63) / (3*16 + 1*8)) * (X63 / 5)</f>
+        <f t="shared" si="60"/>
         <v>2265.2189186271103</v>
       </c>
       <c r="AJ63" s="7" t="s">
@@ -11497,15 +11504,15 @@
         <v>49</v>
       </c>
       <c r="AR63" s="8">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>46</v>
       </c>
       <c r="AS63" s="7">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>456</v>
       </c>
       <c r="AT63" s="7">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>143</v>
       </c>
       <c r="AU63" s="7" t="s">
@@ -11527,35 +11534,38 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="B64" s="30" t="s">
+    <row r="64" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A64" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="B64" t="s">
         <v>124</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C64" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="D64" t="s">
         <v>275</v>
       </c>
-      <c r="D64" t="s">
-        <v>276</v>
-      </c>
       <c r="E64" t="s">
-        <v>122</v>
+        <v>280</v>
       </c>
       <c r="F64" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="G64" s="30" t="s">
+      <c r="G64" t="s">
         <v>122</v>
       </c>
-      <c r="H64" s="32" t="s">
+      <c r="H64" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="I64" s="30" t="s">
+      <c r="I64" t="s">
         <v>122</v>
       </c>
-      <c r="J64" s="32" t="s">
+      <c r="J64" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="K64" s="30" t="s">
+      <c r="K64" t="s">
         <v>122</v>
       </c>
       <c r="L64" t="s">
@@ -11580,7 +11590,7 @@
         <v>122</v>
       </c>
       <c r="S64" s="1" t="s">
-        <v>122</v>
+        <v>278</v>
       </c>
       <c r="T64">
         <v>6</v>
@@ -11597,34 +11607,34 @@
       <c r="X64">
         <v>6</v>
       </c>
-      <c r="Y64" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z64" s="30">
-        <v>1</v>
-      </c>
-      <c r="AA64" s="30">
+      <c r="Y64" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z64">
+        <v>1</v>
+      </c>
+      <c r="AA64">
         <v>16</v>
       </c>
-      <c r="AB64" s="30" t="s">
+      <c r="AB64" t="s">
         <v>99</v>
       </c>
-      <c r="AC64" s="30">
-        <v>1</v>
-      </c>
-      <c r="AD64" s="30">
-        <v>8</v>
-      </c>
-      <c r="AE64" s="30" t="s">
+      <c r="AC64">
+        <v>1</v>
+      </c>
+      <c r="AD64">
+        <v>8</v>
+      </c>
+      <c r="AE64" t="s">
         <v>101</v>
       </c>
       <c r="AF64" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="AG64" s="30" t="s">
+      <c r="AG64" t="s">
         <v>122</v>
       </c>
-      <c r="AH64" s="30" t="s">
+      <c r="AH64" t="s">
         <v>122</v>
       </c>
       <c r="AI64">
@@ -11637,10 +11647,10 @@
       <c r="AK64" s="10">
         <v>125</v>
       </c>
-      <c r="AL64" s="30">
+      <c r="AL64">
         <v>1169</v>
       </c>
-      <c r="AM64" s="30">
+      <c r="AM64">
         <v>414</v>
       </c>
       <c r="AN64" s="1">
@@ -11652,26 +11662,26 @@
       <c r="AP64">
         <v>384</v>
       </c>
-      <c r="AQ64" s="30" t="s">
+      <c r="AQ64" t="s">
         <v>49</v>
       </c>
       <c r="AR64" s="1">
-        <f t="shared" ref="AR64" si="65" xml:space="preserve"> _xlfn.FLOOR.MATH((AK64 - AN64) / 2)</f>
+        <f t="shared" ref="AR64" si="67" xml:space="preserve"> _xlfn.FLOOR.MATH((AK64 - AN64) / 2)</f>
         <v>14</v>
       </c>
       <c r="AS64">
-        <f t="shared" ref="AS64" si="66" xml:space="preserve"> _xlfn.FLOOR.MATH((AL64 - AO64) / 2)</f>
+        <f t="shared" ref="AS64" si="68" xml:space="preserve"> _xlfn.FLOOR.MATH((AL64 - AO64) / 2)</f>
         <v>192</v>
       </c>
       <c r="AT64">
-        <f t="shared" ref="AT64" si="67" xml:space="preserve"> _xlfn.FLOOR.MATH((AM64 - AP64) / 2)</f>
+        <f t="shared" ref="AT64" si="69" xml:space="preserve"> _xlfn.FLOOR.MATH((AM64 - AP64) / 2)</f>
         <v>15</v>
       </c>
-      <c r="AU64" s="30" t="s">
+      <c r="AU64" t="s">
         <v>49</v>
       </c>
       <c r="AV64" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AW64" t="s">
         <v>167</v>
@@ -11679,14 +11689,14 @@
       <c r="AX64" t="s">
         <v>122</v>
       </c>
-      <c r="AY64" s="32" t="s">
+      <c r="AY64" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="AZ64" s="32" t="s">
+      <c r="AZ64" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A69" s="19" t="s">
         <v>122</v>
       </c>
@@ -11809,15 +11819,15 @@
         <v>122</v>
       </c>
       <c r="AR69" s="1" t="e">
-        <f t="shared" ref="AR69" si="68" xml:space="preserve"> _xlfn.FLOOR.MATH((AK69 - AN69) / 2)</f>
+        <f t="shared" ref="AR69" si="70" xml:space="preserve"> _xlfn.FLOOR.MATH((AK69 - AN69) / 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AS69" t="e">
-        <f t="shared" ref="AS69" si="69" xml:space="preserve"> _xlfn.FLOOR.MATH((AL69 - AO69) / 2)</f>
+        <f t="shared" ref="AS69" si="71" xml:space="preserve"> _xlfn.FLOOR.MATH((AL69 - AO69) / 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AT69" t="e">
-        <f t="shared" ref="AT69" si="70" xml:space="preserve"> _xlfn.FLOOR.MATH((AM69 - AP69) / 2)</f>
+        <f t="shared" ref="AT69" si="72" xml:space="preserve"> _xlfn.FLOOR.MATH((AM69 - AP69) / 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AU69" t="s">
@@ -11839,12 +11849,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="75" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:52" x14ac:dyDescent="0.25">
       <c r="AO75" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="76" spans="1:52" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:52" x14ac:dyDescent="0.25">
       <c r="AO76" t="s">
         <v>262</v>
       </c>

</xml_diff>

<commit_message>
rename a folder, prepare test3udnet 231008-0 session
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CAC8B0-04B4-4008-BE14-D4F502516981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85F6D3D-DC61-41FE-8BBB-7E79C5EC7193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="285">
   <si>
     <t>patch z</t>
   </si>
@@ -876,10 +876,22 @@
     <t>dataset07.0</t>
   </si>
   <si>
-    <t>Get fluorescence segmentation to work - since autofluorescence segmentation models did reach usable predictive powers, I am switching to the classical fluo. Segm. Approach instead of the unconventional autofluorescence segmentation. The train-config.yml file was adapted to session 230910-7, which is so far the best performing model, based on tensorboard metrics (val eval score is the most relevant metric / was the most relevant metric for the decision) and prediction images - this regards things like patience and validate_after_iters hyper parameters.</t>
-  </si>
-  <si>
-    <t>TBD (compare to session 230910-7)</t>
+    <t>231008-0</t>
+  </si>
+  <si>
+    <t>test3dunet</t>
+  </si>
+  <si>
+    <t>Get fluorescence segmentation to work - since autofluorescence segmentation models did not reach usable predictive powers, I am switching to the classical fluo. Segm. Approach instead of the unconventional autofluorescence segmentation. The train-config.yml file was adapted to session 230910-7, which is so far the best performing model, based on tensorboard metrics (val eval score is the most relevant metric / was the most relevant metric for the decision) and prediction images - this regards things like patience and validate_after_iters hyper parameters.</t>
+  </si>
+  <si>
+    <t>Success, 3dunet did managed to segment the fluorescently labelled heart very accurately and precisely. Interestingly, the val eval scores peek and plateau around the same value as session 230910-7 (and 230911-0). The train loss decreases much more steeply than the mentioned two sessions. The validation prediction images were accurate and precise already after around 80 training iterations (which was just when I first checked the tensorboard analytics). Interestingly, the val eval scores keep increasing all the way until the end of training, compared to peeking followed by slightly decreasing and forming a plateau - I deduct that this is because in this (the fluorescence segmentation training), the brightest pixels are the tissue of interest and the 'train loss learning funnel' (gradient descent visualisation) makes it easier to reach the global loss minimum than when training with autofuorescence images as done in the other two sessions. Whether the eyes were segmented, too, is not known yet, because the browser based tensorboard statistics only show one z-slice as a sample of the prediction images and targets.</t>
+  </si>
+  <si>
+    <t>Run test3dunet on the 231007-0 train3dunet model trained on babb03 ct3 heart fluorescence images.</t>
+  </si>
+  <si>
+    <t>I expect 3dunet to succeed in the test set fluorescence segmentation.</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1077,9 +1089,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1396,61 +1408,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:AZ76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="73" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="AA50" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="AN65" sqref="AN65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="64.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="14.5703125" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="64.5546875" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="14.5546875" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="9.44140625" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="17" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="19" max="19" width="12.85546875" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="6.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="5.140625" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="11.140625" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="17" width="9.109375" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="12.88671875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="9.109375" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="6.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="5.109375" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="11.109375" customWidth="1" outlineLevel="1"/>
     <col min="25" max="25" width="6" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="7.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="8.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="15.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="7.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="9.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="16.7109375" style="10" customWidth="1"/>
-    <col min="33" max="34" width="14.85546875" customWidth="1"/>
+    <col min="26" max="26" width="14.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="7.88671875" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="8.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="15.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="7.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="9.6640625" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="16.6640625" style="10" customWidth="1"/>
+    <col min="33" max="34" width="14.88671875" customWidth="1"/>
     <col min="35" max="35" width="21" customWidth="1"/>
-    <col min="36" max="36" width="26.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="26.33203125" customWidth="1" outlineLevel="1"/>
     <col min="37" max="37" width="6" style="10" bestFit="1" customWidth="1"/>
     <col min="38" max="39" width="6" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.28515625" style="1" customWidth="1"/>
-    <col min="41" max="41" width="6.140625" customWidth="1"/>
+    <col min="40" max="40" width="5.33203125" style="1" customWidth="1"/>
+    <col min="41" max="41" width="6.109375" customWidth="1"/>
     <col min="42" max="43" width="5" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" style="1" customWidth="1"/>
-    <col min="45" max="45" width="6.5703125" customWidth="1"/>
+    <col min="44" max="44" width="6.109375" style="1" customWidth="1"/>
+    <col min="45" max="45" width="6.5546875" customWidth="1"/>
     <col min="46" max="46" width="5" customWidth="1"/>
     <col min="47" max="47" width="6" customWidth="1"/>
-    <col min="48" max="48" width="74.85546875" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="74.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="5.140625" customWidth="1"/>
-    <col min="51" max="51" width="73.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="48" width="74.88671875" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="74.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="50" width="5.109375" customWidth="1"/>
+    <col min="51" max="51" width="73.88671875" customWidth="1" outlineLevel="1"/>
     <col min="52" max="52" width="206" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.7109375" customWidth="1"/>
-    <col min="57" max="57" width="12.140625" customWidth="1"/>
+    <col min="53" max="53" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.6640625" customWidth="1"/>
+    <col min="57" max="57" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -1608,7 +1620,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -1767,7 +1779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -1813,11 +1825,11 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
+      <c r="P3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>8</v>
       </c>
       <c r="R3">
         <v>1</v>
@@ -1927,7 +1939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:52" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>55</v>
       </c>
@@ -2086,7 +2098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2245,7 +2257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2404,7 +2416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2563,7 +2575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2722,7 +2734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2887,7 +2899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -3046,7 +3058,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3205,7 +3217,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3251,11 +3263,11 @@
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
+      <c r="P12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>8</v>
       </c>
       <c r="R12">
         <v>1</v>
@@ -3365,7 +3377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -3524,7 +3536,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -3683,7 +3695,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -3729,11 +3741,11 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
+      <c r="P15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>8</v>
       </c>
       <c r="R15">
         <v>1</v>
@@ -3843,7 +3855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
@@ -3889,11 +3901,11 @@
       <c r="O16" s="7">
         <v>0</v>
       </c>
-      <c r="P16" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="7">
-        <v>0</v>
+      <c r="P16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="R16" s="7">
         <v>1</v>
@@ -4003,7 +4015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -4049,11 +4061,11 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
+      <c r="P17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="R17">
         <v>1</v>
@@ -4163,7 +4175,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -4209,11 +4221,11 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
+      <c r="P18" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>8</v>
       </c>
       <c r="R18">
         <v>1</v>
@@ -4323,7 +4335,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -4369,11 +4381,11 @@
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
+      <c r="P19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>8</v>
       </c>
       <c r="R19">
         <v>1</v>
@@ -4483,7 +4495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -4529,11 +4541,11 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
+      <c r="P20" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>8</v>
       </c>
       <c r="R20">
         <v>1</v>
@@ -4643,7 +4655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>58</v>
       </c>
@@ -4689,11 +4701,11 @@
       <c r="O21">
         <v>0</v>
       </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
+      <c r="P21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>8</v>
       </c>
       <c r="R21">
         <v>1</v>
@@ -4803,7 +4815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -4849,11 +4861,11 @@
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22">
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
+      <c r="P22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>8</v>
       </c>
       <c r="R22">
         <v>1</v>
@@ -4963,7 +4975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -5009,11 +5021,11 @@
       <c r="O23">
         <v>0</v>
       </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
+      <c r="P23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>8</v>
       </c>
       <c r="R23">
         <v>1</v>
@@ -5123,7 +5135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -5169,11 +5181,11 @@
       <c r="O24">
         <v>0</v>
       </c>
-      <c r="P24">
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
+      <c r="P24" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>8</v>
       </c>
       <c r="R24">
         <v>1</v>
@@ -5283,7 +5295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -5441,7 +5453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>104</v>
       </c>
@@ -5599,7 +5611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>105</v>
       </c>
@@ -5645,11 +5657,11 @@
       <c r="O27">
         <v>0</v>
       </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
+      <c r="P27" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>8</v>
       </c>
       <c r="R27">
         <v>0</v>
@@ -5763,7 +5775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -5926,7 +5938,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -6090,7 +6102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>148</v>
       </c>
@@ -6136,11 +6148,11 @@
       <c r="O30">
         <v>0</v>
       </c>
-      <c r="P30">
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <v>0</v>
+      <c r="P30" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>8</v>
       </c>
       <c r="R30">
         <v>1</v>
@@ -6254,7 +6266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>152</v>
       </c>
@@ -6300,11 +6312,11 @@
       <c r="O31">
         <v>0</v>
       </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>0</v>
+      <c r="P31" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>8</v>
       </c>
       <c r="R31">
         <v>1</v>
@@ -6418,7 +6430,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>159</v>
       </c>
@@ -6464,11 +6476,11 @@
       <c r="O32">
         <v>0</v>
       </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <v>0</v>
+      <c r="P32" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>8</v>
       </c>
       <c r="R32">
         <v>0</v>
@@ -6581,7 +6593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>172</v>
       </c>
@@ -6744,7 +6756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>173</v>
       </c>
@@ -6907,7 +6919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>182</v>
       </c>
@@ -7070,7 +7082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>187</v>
       </c>
@@ -7233,7 +7245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>190</v>
       </c>
@@ -7396,7 +7408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>195</v>
       </c>
@@ -7559,7 +7571,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>198</v>
       </c>
@@ -7722,7 +7734,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>202</v>
       </c>
@@ -7885,7 +7897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>203</v>
       </c>
@@ -8048,7 +8060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>205</v>
       </c>
@@ -8211,7 +8223,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>208</v>
       </c>
@@ -8374,7 +8386,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>209</v>
       </c>
@@ -8419,6 +8431,12 @@
       </c>
       <c r="O44">
         <v>0</v>
+      </c>
+      <c r="P44" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>8</v>
       </c>
       <c r="R44">
         <v>1</v>
@@ -8532,7 +8550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>210</v>
       </c>
@@ -8577,6 +8595,12 @@
       </c>
       <c r="O45" s="7">
         <v>0</v>
+      </c>
+      <c r="P45" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q45" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="R45" s="7">
         <v>1</v>
@@ -8690,7 +8714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
         <v>243</v>
       </c>
@@ -8848,7 +8872,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
         <v>244</v>
       </c>
@@ -8888,11 +8912,11 @@
       <c r="O47" s="21">
         <v>0</v>
       </c>
-      <c r="P47" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="21">
-        <v>0</v>
+      <c r="P47" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q47" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R47">
         <v>1</v>
@@ -9006,7 +9030,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>245</v>
       </c>
@@ -9046,11 +9070,11 @@
       <c r="O48" s="21">
         <v>0</v>
       </c>
-      <c r="P48" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="21">
-        <v>0</v>
+      <c r="P48" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q48" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R48">
         <v>1</v>
@@ -9164,7 +9188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
         <v>246</v>
       </c>
@@ -9204,11 +9228,11 @@
       <c r="O49" s="21">
         <v>0</v>
       </c>
-      <c r="P49" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="21">
-        <v>0</v>
+      <c r="P49" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q49" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R49">
         <v>1</v>
@@ -9322,7 +9346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
         <v>247</v>
       </c>
@@ -9362,11 +9386,11 @@
       <c r="O50" s="21">
         <v>0</v>
       </c>
-      <c r="P50" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="21">
-        <v>0</v>
+      <c r="P50" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q50" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R50">
         <v>1</v>
@@ -9480,7 +9504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
         <v>248</v>
       </c>
@@ -9520,11 +9544,11 @@
       <c r="O51" s="21">
         <v>0</v>
       </c>
-      <c r="P51" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="21">
-        <v>0</v>
+      <c r="P51" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q51" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R51">
         <v>1</v>
@@ -9638,7 +9662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
         <v>249</v>
       </c>
@@ -9678,11 +9702,11 @@
       <c r="O52" s="21">
         <v>0</v>
       </c>
-      <c r="P52" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="21">
-        <v>0</v>
+      <c r="P52" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q52" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R52">
         <v>1</v>
@@ -9796,7 +9820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
         <v>250</v>
       </c>
@@ -9836,11 +9860,11 @@
       <c r="O53" s="21">
         <v>0</v>
       </c>
-      <c r="P53" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="21">
-        <v>0</v>
+      <c r="P53" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q53" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R53">
         <v>1</v>
@@ -9954,7 +9978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
         <v>251</v>
       </c>
@@ -9994,11 +10018,11 @@
       <c r="O54" s="21">
         <v>0</v>
       </c>
-      <c r="P54" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="21">
-        <v>0</v>
+      <c r="P54" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q54" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R54">
         <v>1</v>
@@ -10112,7 +10136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
         <v>252</v>
       </c>
@@ -10270,7 +10294,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
         <v>253</v>
       </c>
@@ -10310,11 +10334,11 @@
       <c r="O56" s="21">
         <v>0</v>
       </c>
-      <c r="P56" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="21">
-        <v>0</v>
+      <c r="P56" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q56" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R56">
         <v>1</v>
@@ -10428,7 +10452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
         <v>254</v>
       </c>
@@ -10468,11 +10492,11 @@
       <c r="O57" s="21">
         <v>0</v>
       </c>
-      <c r="P57" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="21">
-        <v>0</v>
+      <c r="P57" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q57" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R57">
         <v>1</v>
@@ -10586,7 +10610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
         <v>255</v>
       </c>
@@ -10626,11 +10650,11 @@
       <c r="O58" s="21">
         <v>0</v>
       </c>
-      <c r="P58" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q58" s="21">
-        <v>0</v>
+      <c r="P58" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q58" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R58">
         <v>1</v>
@@ -10744,7 +10768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
         <v>256</v>
       </c>
@@ -10784,11 +10808,11 @@
       <c r="O59" s="21">
         <v>0</v>
       </c>
-      <c r="P59" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q59" s="21">
-        <v>0</v>
+      <c r="P59" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q59" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R59">
         <v>1</v>
@@ -10902,7 +10926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A60" s="17" t="s">
         <v>257</v>
       </c>
@@ -10942,11 +10966,11 @@
       <c r="O60" s="21">
         <v>0</v>
       </c>
-      <c r="P60" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="21">
-        <v>0</v>
+      <c r="P60" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q60" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R60">
         <v>1</v>
@@ -11060,7 +11084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A61" s="17" t="s">
         <v>258</v>
       </c>
@@ -11100,11 +11124,11 @@
       <c r="O61" s="21">
         <v>0</v>
       </c>
-      <c r="P61" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="21">
-        <v>0</v>
+      <c r="P61" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q61" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R61">
         <v>1</v>
@@ -11218,7 +11242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
         <v>259</v>
       </c>
@@ -11258,11 +11282,11 @@
       <c r="O62" s="21">
         <v>0</v>
       </c>
-      <c r="P62" s="21">
-        <v>0</v>
-      </c>
-      <c r="Q62" s="21">
-        <v>0</v>
+      <c r="P62" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q62" s="21" t="s">
+        <v>8</v>
       </c>
       <c r="R62">
         <v>1</v>
@@ -11376,7 +11400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:52" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="28" t="s">
         <v>260</v>
       </c>
@@ -11416,11 +11440,11 @@
       <c r="O63" s="22">
         <v>0</v>
       </c>
-      <c r="P63" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q63" s="22">
-        <v>0</v>
+      <c r="P63" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q63" s="22" t="s">
+        <v>8</v>
       </c>
       <c r="R63" s="7">
         <v>1</v>
@@ -11534,51 +11558,51 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A64" s="30" t="s">
+    <row r="64" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A64" s="17" t="s">
         <v>277</v>
       </c>
       <c r="B64" t="s">
         <v>124</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D64" t="s">
         <v>275</v>
       </c>
       <c r="E64" t="s">
-        <v>280</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="G64" t="s">
-        <v>122</v>
+        <v>282</v>
+      </c>
+      <c r="F64" s="10">
+        <v>1</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
       </c>
       <c r="H64" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="I64" t="s">
-        <v>122</v>
+        <v>8</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
       </c>
       <c r="J64" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="K64" t="s">
-        <v>122</v>
-      </c>
-      <c r="L64" t="s">
-        <v>122</v>
-      </c>
-      <c r="M64" t="s">
-        <v>122</v>
-      </c>
-      <c r="N64" t="s">
-        <v>122</v>
-      </c>
-      <c r="O64" t="s">
-        <v>122</v>
+        <v>8</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <v>1</v>
+      </c>
+      <c r="O64">
+        <v>1</v>
       </c>
       <c r="P64" t="s">
         <v>122</v>
@@ -11586,8 +11610,8 @@
       <c r="Q64" t="s">
         <v>122</v>
       </c>
-      <c r="R64" t="s">
-        <v>122</v>
+      <c r="R64">
+        <v>1</v>
       </c>
       <c r="S64" s="1" t="s">
         <v>278</v>
@@ -11696,7 +11720,75 @@
         <v>122</v>
       </c>
     </row>
-    <row r="69" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="A65" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="B65" t="s">
+        <v>280</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="D65" t="s">
+        <v>284</v>
+      </c>
+      <c r="E65" t="s">
+        <v>122</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="G65" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="H65" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="I65" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="J65" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="K65" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="L65" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="M65" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="N65" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="O65" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="P65" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q65" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="R65" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="S65" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AK65" s="10">
+        <v>125</v>
+      </c>
+      <c r="AL65">
+        <v>1169</v>
+      </c>
+      <c r="AM65">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="69" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A69" s="19" t="s">
         <v>122</v>
       </c>
@@ -11849,12 +11941,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="75" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:52" x14ac:dyDescent="0.3">
       <c r="AO75" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="76" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:52" x14ac:dyDescent="0.3">
       <c r="AO76" t="s">
         <v>262</v>
       </c>

</xml_diff>

<commit_message>
prep predict3dunet-231129-0 session with sample data & model
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D5E426-F769-4E70-84A0-FD58B1E699BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC39C02-6BB1-4CFF-824E-F309AC6972C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="348">
   <si>
     <t>patch z</t>
   </si>
@@ -1071,10 +1071,16 @@
     <t>TBD (Success if it looks good. Failure if not.)</t>
   </si>
   <si>
-    <t>Attempt using Wolny's pre-trained model to segment his sample data</t>
-  </si>
-  <si>
     <t>231129-0</t>
+  </si>
+  <si>
+    <t>Attempt using Wolny's pre-trained model to segment his sample data and sample config files from his README.md.</t>
+  </si>
+  <si>
+    <t>The segmentation will work without error. The quality does not matter.</t>
+  </si>
+  <si>
+    <t>TBD: Success if no error, failure if error.</t>
   </si>
 </sst>
 </file>
@@ -1722,66 +1728,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BC82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="64.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="14.5546875" style="6" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="8.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="30.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="9.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="64.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="14.5703125" style="6" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1" outlineLevel="1"/>
     <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="17" width="9.109375" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.109375" style="20"/>
-    <col min="19" max="19" width="12.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="9.109375" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="6.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="5.109375" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="11.109375" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="17" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.140625" style="20"/>
+    <col min="19" max="19" width="12.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="6.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="5.140625" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="11.140625" customWidth="1" outlineLevel="1"/>
     <col min="25" max="25" width="6" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="7.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="8.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="15.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="7.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="9.6640625" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="16.6640625" customWidth="1"/>
-    <col min="33" max="34" width="14.88671875" customWidth="1"/>
+    <col min="26" max="26" width="14.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="7.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="8.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="15.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="7.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="9.7109375" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="16.7109375" customWidth="1"/>
+    <col min="33" max="34" width="14.85546875" customWidth="1"/>
     <col min="35" max="35" width="21" customWidth="1"/>
-    <col min="36" max="36" width="26.33203125" style="10" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="26.28515625" style="10" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="37" max="37" width="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="38" max="38" width="6" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="6" style="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.33203125" customWidth="1"/>
-    <col min="41" max="41" width="6.109375" customWidth="1"/>
+    <col min="40" max="40" width="5.28515625" customWidth="1"/>
+    <col min="41" max="41" width="6.140625" customWidth="1"/>
     <col min="42" max="42" width="5" customWidth="1"/>
     <col min="43" max="43" width="5" style="20" customWidth="1"/>
-    <col min="44" max="44" width="6.109375" customWidth="1"/>
-    <col min="45" max="45" width="6.5546875" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" customWidth="1"/>
+    <col min="45" max="45" width="6.5703125" customWidth="1"/>
     <col min="46" max="46" width="5" customWidth="1"/>
     <col min="47" max="47" width="6" style="20" customWidth="1"/>
     <col min="48" max="49" width="6" customWidth="1"/>
     <col min="50" max="50" width="6" style="10" customWidth="1"/>
-    <col min="51" max="51" width="74.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="74.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="5.109375" customWidth="1"/>
-    <col min="54" max="54" width="135.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="51" max="51" width="74.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="52" max="52" width="74.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="5.140625" customWidth="1"/>
+    <col min="54" max="54" width="135.28515625" customWidth="1" outlineLevel="1"/>
     <col min="55" max="55" width="206" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.6640625" customWidth="1"/>
-    <col min="60" max="60" width="12.109375" customWidth="1"/>
+    <col min="56" max="56" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.7109375" customWidth="1"/>
+    <col min="60" max="60" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1948,7 +1954,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -2110,7 +2116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -2273,7 +2279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:55" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:55" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>54</v>
       </c>
@@ -2435,7 +2441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2594,7 +2600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2753,7 +2759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2912,7 +2918,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -3071,7 +3077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -3236,7 +3242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -3395,7 +3401,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -3554,7 +3560,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -3714,7 +3720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -3873,7 +3879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -4032,7 +4038,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -4192,7 +4198,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -4353,7 +4359,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -4513,7 +4519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -4673,7 +4679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -4833,7 +4839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -4993,7 +4999,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -5153,7 +5159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -5313,7 +5319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -5473,7 +5479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -5633,7 +5639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>103</v>
       </c>
@@ -5800,7 +5806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>103</v>
       </c>
@@ -5967,7 +5973,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -6131,7 +6137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -6294,7 +6300,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>115</v>
       </c>
@@ -6458,7 +6464,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -6622,7 +6628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -6786,7 +6792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>158</v>
       </c>
@@ -6949,7 +6955,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>171</v>
       </c>
@@ -7112,7 +7118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>172</v>
       </c>
@@ -7275,7 +7281,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>181</v>
       </c>
@@ -7438,7 +7444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>186</v>
       </c>
@@ -7601,7 +7607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>189</v>
       </c>
@@ -7764,7 +7770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>194</v>
       </c>
@@ -7927,7 +7933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>197</v>
       </c>
@@ -8090,7 +8096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>201</v>
       </c>
@@ -8253,7 +8259,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>202</v>
       </c>
@@ -8416,7 +8422,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>204</v>
       </c>
@@ -8579,7 +8585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>207</v>
       </c>
@@ -8742,7 +8748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>208</v>
       </c>
@@ -8906,7 +8912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>209</v>
       </c>
@@ -9071,7 +9077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>241</v>
       </c>
@@ -9229,7 +9235,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>242</v>
       </c>
@@ -9387,7 +9393,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>243</v>
       </c>
@@ -9545,7 +9551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>244</v>
       </c>
@@ -9703,7 +9709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>245</v>
       </c>
@@ -9861,7 +9867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>246</v>
       </c>
@@ -10019,7 +10025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>247</v>
       </c>
@@ -10177,7 +10183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>248</v>
       </c>
@@ -10335,7 +10341,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>249</v>
       </c>
@@ -10493,7 +10499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>250</v>
       </c>
@@ -10651,7 +10657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>251</v>
       </c>
@@ -10809,7 +10815,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>252</v>
       </c>
@@ -10967,7 +10973,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>253</v>
       </c>
@@ -11125,7 +11131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>254</v>
       </c>
@@ -11283,7 +11289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>255</v>
       </c>
@@ -11441,7 +11447,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>256</v>
       </c>
@@ -11599,7 +11605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>257</v>
       </c>
@@ -11757,7 +11763,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>258</v>
       </c>
@@ -11916,7 +11922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:55" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:55" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="32" t="s">
         <v>273</v>
       </c>
@@ -12079,7 +12085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>275</v>
       </c>
@@ -12249,7 +12255,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="66" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>280</v>
       </c>
@@ -12419,7 +12425,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="67" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>296</v>
       </c>
@@ -12589,7 +12595,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="68" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>299</v>
       </c>
@@ -12759,7 +12765,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="69" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>300</v>
       </c>
@@ -12929,7 +12935,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="70" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>305</v>
       </c>
@@ -13102,7 +13108,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="71" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>306</v>
       </c>
@@ -13272,7 +13278,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="72" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>309</v>
       </c>
@@ -13442,7 +13448,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="73" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>328</v>
       </c>
@@ -13615,7 +13621,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="74" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>330</v>
       </c>
@@ -13785,18 +13791,171 @@
         <v>292</v>
       </c>
     </row>
-    <row r="75" spans="1:55" x14ac:dyDescent="0.3">
-      <c r="A75" s="44" t="s">
-        <v>345</v>
+    <row r="75" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>344</v>
       </c>
       <c r="B75" t="s">
         <v>281</v>
       </c>
-      <c r="C75" s="44" t="s">
-        <v>344</v>
+      <c r="C75" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="D75" s="44" t="s">
+        <v>346</v>
+      </c>
+      <c r="E75" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G75" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="H75" t="s">
+        <v>121</v>
+      </c>
+      <c r="I75" t="s">
+        <v>121</v>
+      </c>
+      <c r="J75" t="s">
+        <v>121</v>
+      </c>
+      <c r="K75" t="s">
+        <v>121</v>
+      </c>
+      <c r="L75" t="s">
+        <v>121</v>
+      </c>
+      <c r="M75" t="s">
+        <v>121</v>
+      </c>
+      <c r="N75" t="s">
+        <v>121</v>
+      </c>
+      <c r="O75" t="s">
+        <v>121</v>
+      </c>
+      <c r="P75" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>121</v>
+      </c>
+      <c r="R75" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S75" t="s">
+        <v>121</v>
+      </c>
+      <c r="T75" t="s">
+        <v>121</v>
+      </c>
+      <c r="U75" t="s">
+        <v>121</v>
+      </c>
+      <c r="V75" t="s">
+        <v>121</v>
+      </c>
+      <c r="W75" t="s">
+        <v>121</v>
+      </c>
+      <c r="X75" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE75" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AK75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM75" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="AN75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AO75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ75" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="AR75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AS75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AU75" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="AV75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AX75" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AY75" t="s">
+        <v>121</v>
+      </c>
+      <c r="AZ75" t="s">
+        <v>121</v>
+      </c>
+      <c r="BA75" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB75" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC75" t="s">
+        <v>121</v>
       </c>
     </row>
-    <row r="77" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>121</v>
       </c>
@@ -13963,7 +14122,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="78" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>121</v>
       </c>
@@ -14133,7 +14292,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="81" spans="1:55" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:55" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="38" t="s">
         <v>121</v>
       </c>
@@ -14303,7 +14462,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="82" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:55" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>335</v>
       </c>

</xml_diff>

<commit_message>
generic commit message, Tue 13:19:09 12.12.2023.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB304DB5-3503-43B3-8E91-7831401F298E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA23427-BA63-4B2F-9C05-7B6D6F7C2ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="379">
   <si>
     <t>patch z</t>
   </si>
@@ -1128,9 +1128,6 @@
     <t>The training will work without error. The quality does not matter much, 1 hour run time as limit.</t>
   </si>
   <si>
-    <t>TBD: Success if no error, failure otherwise.</t>
-  </si>
-  <si>
     <t>stride = the default shape in Wolny's train_config.yml for this model type</t>
   </si>
   <si>
@@ -1174,6 +1171,9 @@
   </si>
   <si>
     <t>out of time (1 hour test session)</t>
+  </si>
+  <si>
+    <t>231211-0</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1450,8 +1450,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1768,8 +1766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BC88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -14246,13 +14244,13 @@
         <v>8</v>
       </c>
       <c r="V79" t="s">
+        <v>372</v>
+      </c>
+      <c r="W79" t="s">
+        <v>372</v>
+      </c>
+      <c r="X79" t="s">
         <v>373</v>
-      </c>
-      <c r="W79" t="s">
-        <v>373</v>
-      </c>
-      <c r="X79" t="s">
-        <v>374</v>
       </c>
       <c r="Y79">
         <v>4</v>
@@ -14333,16 +14331,16 @@
         <v>130</v>
       </c>
       <c r="AY79" t="s">
+        <v>364</v>
+      </c>
+      <c r="AZ79" t="s">
+        <v>363</v>
+      </c>
+      <c r="BA79">
+        <v>1</v>
+      </c>
+      <c r="BB79" t="s">
         <v>365</v>
-      </c>
-      <c r="AZ79" t="s">
-        <v>364</v>
-      </c>
-      <c r="BA79">
-        <v>1</v>
-      </c>
-      <c r="BB79" t="s">
-        <v>366</v>
       </c>
       <c r="BC79" t="s">
         <v>292</v>
@@ -14350,28 +14348,28 @@
     </row>
     <row r="80" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B80" t="s">
         <v>123</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D80" s="12" t="s">
         <v>362</v>
       </c>
       <c r="E80" s="12" t="s">
+        <v>376</v>
+      </c>
+      <c r="F80" s="6">
+        <v>0</v>
+      </c>
+      <c r="G80" s="12">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
         <v>377</v>
-      </c>
-      <c r="F80" s="6">
-        <v>0</v>
-      </c>
-      <c r="G80" s="12">
-        <v>1</v>
-      </c>
-      <c r="H80" t="s">
-        <v>378</v>
       </c>
       <c r="I80">
         <v>0</v>
@@ -14410,16 +14408,16 @@
         <v>348</v>
       </c>
       <c r="U80" t="s">
+        <v>372</v>
+      </c>
+      <c r="V80" t="s">
+        <v>372</v>
+      </c>
+      <c r="W80" t="s">
+        <v>372</v>
+      </c>
+      <c r="X80" t="s">
         <v>373</v>
-      </c>
-      <c r="V80" t="s">
-        <v>373</v>
-      </c>
-      <c r="W80" t="s">
-        <v>373</v>
-      </c>
-      <c r="X80" t="s">
-        <v>374</v>
       </c>
       <c r="Y80">
         <v>4</v>
@@ -14443,45 +14441,45 @@
         <v>347</v>
       </c>
       <c r="AF80" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AG80" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AH80" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AI80" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AK80" t="s">
+        <v>367</v>
+      </c>
+      <c r="AL80" t="s">
         <v>368</v>
       </c>
-      <c r="AL80" t="s">
+      <c r="AM80" s="20" t="s">
         <v>369</v>
       </c>
-      <c r="AM80" s="20" t="s">
-        <v>370</v>
-      </c>
-      <c r="AN80" s="38">
+      <c r="AN80">
         <v>80</v>
       </c>
-      <c r="AO80" s="38">
+      <c r="AO80">
         <v>240</v>
       </c>
-      <c r="AP80" s="38">
+      <c r="AP80">
         <v>240</v>
       </c>
-      <c r="AQ80" s="39" t="s">
+      <c r="AQ80" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="AR80" s="38">
+      <c r="AR80">
         <v>64</v>
       </c>
-      <c r="AS80" s="38">
+      <c r="AS80">
         <v>144</v>
       </c>
-      <c r="AT80" s="38">
+      <c r="AT80">
         <v>144</v>
       </c>
       <c r="AU80" s="20" t="s">
@@ -14503,7 +14501,7 @@
         <v>66</v>
       </c>
       <c r="AZ80" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="BA80">
         <v>0</v>
@@ -14517,58 +14515,58 @@
     </row>
     <row r="81" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B81" t="s">
         <v>123</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D81" s="12" t="s">
         <v>362</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>363</v>
-      </c>
-      <c r="F81" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G81" s="12" t="s">
-        <v>121</v>
+        <v>376</v>
+      </c>
+      <c r="F81" s="6">
+        <v>1</v>
+      </c>
+      <c r="G81" s="12">
+        <v>0</v>
       </c>
       <c r="H81" t="s">
-        <v>121</v>
-      </c>
-      <c r="I81" t="s">
-        <v>121</v>
+        <v>8</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
       </c>
       <c r="J81" t="s">
-        <v>121</v>
-      </c>
-      <c r="K81" t="s">
-        <v>121</v>
-      </c>
-      <c r="L81" t="s">
-        <v>121</v>
-      </c>
-      <c r="M81" t="s">
-        <v>121</v>
-      </c>
-      <c r="N81" t="s">
-        <v>121</v>
-      </c>
-      <c r="O81" t="s">
-        <v>121</v>
+        <v>8</v>
+      </c>
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="M81">
+        <v>1</v>
+      </c>
+      <c r="N81">
+        <v>1</v>
+      </c>
+      <c r="O81">
+        <v>0</v>
       </c>
       <c r="P81" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="Q81" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="R81" s="20" t="s">
-        <v>121</v>
+        <v>8</v>
+      </c>
+      <c r="R81" s="20">
+        <v>0</v>
       </c>
       <c r="S81" t="s">
         <v>349</v>
@@ -14580,13 +14578,13 @@
         <v>121</v>
       </c>
       <c r="V81" t="s">
+        <v>372</v>
+      </c>
+      <c r="W81" t="s">
+        <v>372</v>
+      </c>
+      <c r="X81" t="s">
         <v>373</v>
-      </c>
-      <c r="W81" t="s">
-        <v>373</v>
-      </c>
-      <c r="X81" t="s">
-        <v>374</v>
       </c>
       <c r="Y81">
         <v>4</v>
@@ -14622,33 +14620,33 @@
         <v>121</v>
       </c>
       <c r="AK81" t="s">
+        <v>367</v>
+      </c>
+      <c r="AL81" t="s">
         <v>368</v>
       </c>
-      <c r="AL81" t="s">
+      <c r="AM81" s="20" t="s">
         <v>369</v>
       </c>
-      <c r="AM81" s="20" t="s">
-        <v>370</v>
-      </c>
-      <c r="AN81" s="38">
+      <c r="AN81">
         <v>80</v>
       </c>
-      <c r="AO81" s="38">
+      <c r="AO81">
         <v>240</v>
       </c>
-      <c r="AP81" s="38">
+      <c r="AP81">
         <v>240</v>
       </c>
-      <c r="AQ81" s="39" t="s">
+      <c r="AQ81" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="AR81" s="38">
+      <c r="AR81">
         <v>64</v>
       </c>
-      <c r="AS81" s="38">
+      <c r="AS81">
         <v>144</v>
       </c>
-      <c r="AT81" s="38">
+      <c r="AT81">
         <v>144</v>
       </c>
       <c r="AU81" s="20" t="s">
@@ -14670,21 +14668,21 @@
         <v>66</v>
       </c>
       <c r="AZ81" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA81" t="s">
-        <v>121</v>
+        <v>366</v>
+      </c>
+      <c r="BA81">
+        <v>0</v>
       </c>
       <c r="BB81" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="BC81" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>121</v>
+        <v>378</v>
       </c>
       <c r="B82" t="s">
         <v>281</v>
@@ -14698,44 +14696,44 @@
       <c r="E82" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="F82" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G82" t="s">
-        <v>121</v>
-      </c>
-      <c r="H82" t="s">
-        <v>121</v>
-      </c>
-      <c r="I82" t="s">
-        <v>121</v>
+      <c r="F82" s="6">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
       </c>
       <c r="J82" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="K82" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="L82" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="M82" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="N82" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="O82" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="P82" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="Q82" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="R82" s="20" t="s">
-        <v>121</v>
+        <v>8</v>
+      </c>
+      <c r="R82" s="20">
+        <v>0</v>
       </c>
       <c r="S82" t="s">
         <v>349</v>
@@ -14800,55 +14798,225 @@
       <c r="AM82" s="20">
         <v>414</v>
       </c>
-      <c r="AN82" t="s">
+      <c r="AN82">
+        <v>80</v>
+      </c>
+      <c r="AO82">
+        <v>170</v>
+      </c>
+      <c r="AP82">
+        <v>170</v>
+      </c>
+      <c r="AQ82" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR82">
+        <v>40</v>
+      </c>
+      <c r="AS82">
+        <v>90</v>
+      </c>
+      <c r="AT82">
+        <v>90</v>
+      </c>
+      <c r="AU82" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV82">
+        <f>AN82-AR82</f>
+        <v>40</v>
+      </c>
+      <c r="AW82">
+        <f>AO82-AS82</f>
+        <v>80</v>
+      </c>
+      <c r="AX82" s="10">
+        <f>AP82-AT82</f>
+        <v>80</v>
+      </c>
+      <c r="AY82" t="s">
+        <v>346</v>
+      </c>
+      <c r="AZ82" t="s">
+        <v>345</v>
+      </c>
+      <c r="BA82">
+        <v>1</v>
+      </c>
+      <c r="BB82" t="s">
+        <v>291</v>
+      </c>
+      <c r="BC82" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="83" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A83" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="AO82" t="s">
+      <c r="B83" t="s">
         <v>121</v>
       </c>
-      <c r="AP82" t="s">
+      <c r="C83" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="AQ82" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR82" t="s">
+      <c r="D83" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="AS82" t="s">
+      <c r="E83" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="AT82" t="s">
+      <c r="F83" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="AU82" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV82" t="e">
-        <f>AN82-AR82</f>
+      <c r="G83" t="s">
+        <v>121</v>
+      </c>
+      <c r="H83" t="s">
+        <v>121</v>
+      </c>
+      <c r="I83" t="s">
+        <v>121</v>
+      </c>
+      <c r="J83" t="s">
+        <v>121</v>
+      </c>
+      <c r="K83" t="s">
+        <v>121</v>
+      </c>
+      <c r="L83" t="s">
+        <v>121</v>
+      </c>
+      <c r="M83" t="s">
+        <v>121</v>
+      </c>
+      <c r="N83" t="s">
+        <v>121</v>
+      </c>
+      <c r="O83" t="s">
+        <v>121</v>
+      </c>
+      <c r="P83" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q83" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R83" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S83" t="s">
+        <v>121</v>
+      </c>
+      <c r="T83" t="s">
+        <v>121</v>
+      </c>
+      <c r="U83" t="s">
+        <v>121</v>
+      </c>
+      <c r="V83" t="s">
+        <v>121</v>
+      </c>
+      <c r="W83" t="s">
+        <v>121</v>
+      </c>
+      <c r="X83" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE83" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG83" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI83" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ83" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM83" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="AN83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AO83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ83" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AS83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT83" t="s">
+        <v>121</v>
+      </c>
+      <c r="AU83" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV83" t="e">
+        <f>AN83-AR83</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AW82" t="e">
-        <f>AO82-AS82</f>
+      <c r="AW83" t="e">
+        <f>AO83-AS83</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AX82" s="10" t="e">
-        <f>AP82-AT82</f>
+      <c r="AX83" s="10" t="e">
+        <f>AP83-AT83</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AY82" t="s">
+      <c r="AY83" t="s">
         <v>121</v>
       </c>
-      <c r="AZ82" t="s">
+      <c r="AZ83" t="s">
         <v>121</v>
       </c>
-      <c r="BA82" t="s">
+      <c r="BA83" t="s">
         <v>121</v>
       </c>
-      <c r="BB82" t="s">
+      <c r="BB83" t="s">
         <v>121</v>
       </c>
-      <c r="BC82" t="s">
+      <c r="BC83" t="s">
         <v>121</v>
       </c>
     </row>
@@ -14858,12 +15026,7 @@
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
       <c r="G86" s="12"/>
-      <c r="AE86"/>
       <c r="AJ86"/>
-      <c r="AM86"/>
-      <c r="AQ86"/>
-      <c r="AU86"/>
-      <c r="AX86"/>
     </row>
     <row r="88" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>

</xml_diff>

<commit_message>
prep predict3dunet 231212-0, 231212-1, 231212-2
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA23427-BA63-4B2F-9C05-7B6D6F7C2ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBAAD3F-5B4C-4A69-9B11-0CC393BD023D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="386">
   <si>
     <t>patch z</t>
   </si>
@@ -1174,13 +1174,34 @@
   </si>
   <si>
     <t>231211-0</t>
+  </si>
+  <si>
+    <t>Failure: error, invalid patch shape &amp;/ invalid stride shape.</t>
+  </si>
+  <si>
+    <t>patch = same as in the github README.md under prediction tips ( https://github.com/wolny/pytorch-3dunet#prediction-tips ).</t>
+  </si>
+  <si>
+    <t>stride = such that the 'halo' is the same amount of voxels in all dimensions (32, as it is in the README.md ( https://github.com/wolny/pytorch-3dunet#prediction-tips )).</t>
+  </si>
+  <si>
+    <t>231212-0</t>
+  </si>
+  <si>
+    <t>231212-1</t>
+  </si>
+  <si>
+    <t>231212-2</t>
+  </si>
+  <si>
+    <t>stride = same as in the github README.md under prediction tips ( https://github.com/wolny/pytorch-3dunet#prediction-tips ). Also same as in previous session, chpt-231212-1.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1203,6 +1224,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1399,7 +1427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1450,6 +1478,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1764,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BC88"/>
+  <dimension ref="A1:BC94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="AK63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT83" sqref="AT83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -14694,7 +14725,7 @@
         <v>333</v>
       </c>
       <c r="E82" s="12" t="s">
-        <v>338</v>
+        <v>379</v>
       </c>
       <c r="F82" s="6">
         <v>0</v>
@@ -14823,15 +14854,15 @@
         <v>8</v>
       </c>
       <c r="AV82">
-        <f>AN82-AR82</f>
+        <f t="shared" ref="AV82:AX83" si="84">AN82-AR82</f>
         <v>40</v>
       </c>
       <c r="AW82">
-        <f>AO82-AS82</f>
+        <f t="shared" si="84"/>
         <v>80</v>
       </c>
       <c r="AX82" s="10">
-        <f>AP82-AT82</f>
+        <f t="shared" si="84"/>
         <v>80</v>
       </c>
       <c r="AY82" t="s">
@@ -14852,19 +14883,19 @@
     </row>
     <row r="83" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>121</v>
+        <v>382</v>
       </c>
       <c r="B83" t="s">
-        <v>121</v>
+        <v>281</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>121</v>
+        <v>332</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>121</v>
+        <v>333</v>
       </c>
       <c r="E83" s="12" t="s">
-        <v>121</v>
+        <v>338</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>121</v>
@@ -14906,43 +14937,43 @@
         <v>121</v>
       </c>
       <c r="S83" t="s">
-        <v>121</v>
+        <v>349</v>
       </c>
       <c r="T83" t="s">
-        <v>121</v>
+        <v>348</v>
       </c>
       <c r="U83" t="s">
         <v>121</v>
       </c>
-      <c r="V83" t="s">
-        <v>121</v>
-      </c>
-      <c r="W83" t="s">
-        <v>121</v>
-      </c>
-      <c r="X83" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y83" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA83" t="s">
-        <v>121</v>
+      <c r="V83">
+        <v>5</v>
+      </c>
+      <c r="W83">
+        <v>1</v>
+      </c>
+      <c r="X83">
+        <v>6</v>
+      </c>
+      <c r="Y83">
+        <v>1</v>
+      </c>
+      <c r="Z83">
+        <v>1</v>
+      </c>
+      <c r="AA83">
+        <v>16</v>
       </c>
       <c r="AB83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AC83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AD83" t="s">
-        <v>121</v>
+        <v>98</v>
+      </c>
+      <c r="AC83">
+        <v>1</v>
+      </c>
+      <c r="AD83">
+        <v>8</v>
       </c>
       <c r="AE83" s="10" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="AF83" t="s">
         <v>121</v>
@@ -14959,56 +14990,56 @@
       <c r="AJ83" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AM83" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AO83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AP83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AQ83" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AS83" t="s">
-        <v>121</v>
-      </c>
-      <c r="AT83" t="s">
-        <v>121</v>
+      <c r="AK83">
+        <v>125</v>
+      </c>
+      <c r="AL83">
+        <v>1169</v>
+      </c>
+      <c r="AM83" s="20">
+        <v>414</v>
+      </c>
+      <c r="AN83" s="3">
+        <v>80</v>
+      </c>
+      <c r="AO83" s="3">
+        <v>240</v>
+      </c>
+      <c r="AP83" s="3">
+        <v>240</v>
+      </c>
+      <c r="AQ83" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR83" s="3">
+        <v>64</v>
+      </c>
+      <c r="AS83" s="3">
+        <v>144</v>
+      </c>
+      <c r="AT83" s="3">
+        <v>144</v>
       </c>
       <c r="AU83" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AV83" t="e">
-        <f>AN83-AR83</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AW83" t="e">
-        <f>AO83-AS83</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AX83" s="10" t="e">
-        <f>AP83-AT83</f>
-        <v>#VALUE!</v>
+      <c r="AV83">
+        <f t="shared" si="84"/>
+        <v>16</v>
+      </c>
+      <c r="AW83">
+        <f t="shared" si="84"/>
+        <v>96</v>
+      </c>
+      <c r="AX83" s="10">
+        <f t="shared" si="84"/>
+        <v>96</v>
       </c>
       <c r="AY83" t="s">
-        <v>121</v>
+        <v>293</v>
       </c>
       <c r="AZ83" t="s">
-        <v>121</v>
+        <v>294</v>
       </c>
       <c r="BA83" t="s">
         <v>121</v>
@@ -15020,13 +15051,515 @@
         <v>121</v>
       </c>
     </row>
+    <row r="84" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="B84" t="s">
+        <v>281</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="E84" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G84" t="s">
+        <v>121</v>
+      </c>
+      <c r="H84" t="s">
+        <v>121</v>
+      </c>
+      <c r="I84" t="s">
+        <v>121</v>
+      </c>
+      <c r="J84" t="s">
+        <v>121</v>
+      </c>
+      <c r="K84" t="s">
+        <v>121</v>
+      </c>
+      <c r="L84" t="s">
+        <v>121</v>
+      </c>
+      <c r="M84" t="s">
+        <v>121</v>
+      </c>
+      <c r="N84" t="s">
+        <v>121</v>
+      </c>
+      <c r="O84" t="s">
+        <v>121</v>
+      </c>
+      <c r="P84" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q84" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R84" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S84" t="s">
+        <v>349</v>
+      </c>
+      <c r="T84" t="s">
+        <v>348</v>
+      </c>
+      <c r="U84" t="s">
+        <v>121</v>
+      </c>
+      <c r="V84">
+        <v>5</v>
+      </c>
+      <c r="W84">
+        <v>1</v>
+      </c>
+      <c r="X84">
+        <v>6</v>
+      </c>
+      <c r="Y84">
+        <v>1</v>
+      </c>
+      <c r="Z84">
+        <v>1</v>
+      </c>
+      <c r="AA84">
+        <v>16</v>
+      </c>
+      <c r="AB84" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC84">
+        <v>1</v>
+      </c>
+      <c r="AD84">
+        <v>8</v>
+      </c>
+      <c r="AE84" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF84" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG84" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH84" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI84" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ84" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK84">
+        <v>125</v>
+      </c>
+      <c r="AL84">
+        <v>1169</v>
+      </c>
+      <c r="AM84" s="20">
+        <v>414</v>
+      </c>
+      <c r="AN84" s="3">
+        <v>80</v>
+      </c>
+      <c r="AO84" s="3">
+        <v>240</v>
+      </c>
+      <c r="AP84" s="3">
+        <v>240</v>
+      </c>
+      <c r="AQ84" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR84" s="3">
+        <v>48</v>
+      </c>
+      <c r="AS84" s="3">
+        <v>208</v>
+      </c>
+      <c r="AT84" s="3">
+        <v>208</v>
+      </c>
+      <c r="AU84" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV84">
+        <f t="shared" ref="AV84" si="85">AN84-AR84</f>
+        <v>32</v>
+      </c>
+      <c r="AW84">
+        <f t="shared" ref="AW84" si="86">AO84-AS84</f>
+        <v>32</v>
+      </c>
+      <c r="AX84" s="10">
+        <f t="shared" ref="AX84" si="87">AP84-AT84</f>
+        <v>32</v>
+      </c>
+      <c r="AY84" t="s">
+        <v>293</v>
+      </c>
+      <c r="AZ84" t="s">
+        <v>381</v>
+      </c>
+      <c r="BA84" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB84" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC84" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="85" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="B85" t="s">
+        <v>281</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="E85" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G85" t="s">
+        <v>121</v>
+      </c>
+      <c r="H85" t="s">
+        <v>121</v>
+      </c>
+      <c r="I85" t="s">
+        <v>121</v>
+      </c>
+      <c r="J85" t="s">
+        <v>121</v>
+      </c>
+      <c r="K85" t="s">
+        <v>121</v>
+      </c>
+      <c r="L85" t="s">
+        <v>121</v>
+      </c>
+      <c r="M85" t="s">
+        <v>121</v>
+      </c>
+      <c r="N85" t="s">
+        <v>121</v>
+      </c>
+      <c r="O85" t="s">
+        <v>121</v>
+      </c>
+      <c r="P85" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q85" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R85" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S85" t="s">
+        <v>349</v>
+      </c>
+      <c r="T85" t="s">
+        <v>348</v>
+      </c>
+      <c r="U85" t="s">
+        <v>121</v>
+      </c>
+      <c r="V85">
+        <v>5</v>
+      </c>
+      <c r="W85">
+        <v>1</v>
+      </c>
+      <c r="X85">
+        <v>6</v>
+      </c>
+      <c r="Y85">
+        <v>1</v>
+      </c>
+      <c r="Z85">
+        <v>1</v>
+      </c>
+      <c r="AA85">
+        <v>16</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC85">
+        <v>1</v>
+      </c>
+      <c r="AD85">
+        <v>8</v>
+      </c>
+      <c r="AE85" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF85" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG85" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH85" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI85" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ85" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK85">
+        <v>125</v>
+      </c>
+      <c r="AL85">
+        <v>1169</v>
+      </c>
+      <c r="AM85" s="20">
+        <v>414</v>
+      </c>
+      <c r="AN85" s="3">
+        <v>64</v>
+      </c>
+      <c r="AO85" s="3">
+        <v>128</v>
+      </c>
+      <c r="AP85" s="3">
+        <v>128</v>
+      </c>
+      <c r="AQ85" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR85" s="3">
+        <v>32</v>
+      </c>
+      <c r="AS85" s="3">
+        <v>96</v>
+      </c>
+      <c r="AT85" s="3">
+        <v>96</v>
+      </c>
+      <c r="AU85" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV85">
+        <f t="shared" ref="AV85" si="88">AN85-AR85</f>
+        <v>32</v>
+      </c>
+      <c r="AW85">
+        <f t="shared" ref="AW85" si="89">AO85-AS85</f>
+        <v>32</v>
+      </c>
+      <c r="AX85" s="10">
+        <f t="shared" ref="AX85" si="90">AP85-AT85</f>
+        <v>32</v>
+      </c>
+      <c r="AY85" t="s">
+        <v>380</v>
+      </c>
+      <c r="AZ85" t="s">
+        <v>385</v>
+      </c>
+      <c r="BA85" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB85" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC85" t="s">
+        <v>121</v>
+      </c>
+    </row>
     <row r="86" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="G86" s="12"/>
-      <c r="AJ86"/>
+      <c r="A86" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B86" t="s">
+        <v>121</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E86" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G86" t="s">
+        <v>121</v>
+      </c>
+      <c r="H86" t="s">
+        <v>121</v>
+      </c>
+      <c r="I86" t="s">
+        <v>121</v>
+      </c>
+      <c r="J86" t="s">
+        <v>121</v>
+      </c>
+      <c r="K86" t="s">
+        <v>121</v>
+      </c>
+      <c r="L86" t="s">
+        <v>121</v>
+      </c>
+      <c r="M86" t="s">
+        <v>121</v>
+      </c>
+      <c r="N86" t="s">
+        <v>121</v>
+      </c>
+      <c r="O86" t="s">
+        <v>121</v>
+      </c>
+      <c r="P86" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q86" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R86" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S86" t="s">
+        <v>121</v>
+      </c>
+      <c r="T86" t="s">
+        <v>121</v>
+      </c>
+      <c r="U86" t="s">
+        <v>121</v>
+      </c>
+      <c r="V86" t="s">
+        <v>121</v>
+      </c>
+      <c r="W86" t="s">
+        <v>121</v>
+      </c>
+      <c r="X86" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE86" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG86" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI86" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ86" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM86" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="AN86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AO86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AQ86" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AS86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AU86" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV86" t="e">
+        <f t="shared" ref="AV86" si="91">AN86-AR86</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW86" t="e">
+        <f t="shared" ref="AW86" si="92">AO86-AS86</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AX86" s="10" t="e">
+        <f t="shared" ref="AX86" si="93">AP86-AT86</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY86" t="s">
+        <v>121</v>
+      </c>
+      <c r="AZ86" t="s">
+        <v>121</v>
+      </c>
+      <c r="BA86" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB86" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC86" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="88" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
@@ -15035,8 +15568,120 @@
       <c r="E88" s="12"/>
       <c r="Q88" s="12"/>
       <c r="AG88" s="12"/>
-      <c r="AQ88" s="25"/>
-      <c r="AU88" s="25"/>
+    </row>
+    <row r="92" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AN92">
+        <v>80</v>
+      </c>
+      <c r="AO92">
+        <v>170</v>
+      </c>
+      <c r="AP92">
+        <v>170</v>
+      </c>
+      <c r="AQ92" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR92">
+        <v>20</v>
+      </c>
+      <c r="AS92">
+        <v>40</v>
+      </c>
+      <c r="AT92">
+        <v>40</v>
+      </c>
+      <c r="AU92" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV92">
+        <f t="shared" ref="AV92" si="94">AN92-AR92</f>
+        <v>60</v>
+      </c>
+      <c r="AW92">
+        <f t="shared" ref="AW92" si="95">AO92-AS92</f>
+        <v>130</v>
+      </c>
+      <c r="AX92" s="10">
+        <f t="shared" ref="AX92" si="96">AP92-AT92</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="93" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AN93">
+        <v>80</v>
+      </c>
+      <c r="AO93">
+        <v>170</v>
+      </c>
+      <c r="AP93">
+        <v>170</v>
+      </c>
+      <c r="AQ93" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR93">
+        <v>40</v>
+      </c>
+      <c r="AS93">
+        <v>80</v>
+      </c>
+      <c r="AT93">
+        <v>80</v>
+      </c>
+      <c r="AU93" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV93">
+        <f t="shared" ref="AV93" si="97">AN93-AR93</f>
+        <v>40</v>
+      </c>
+      <c r="AW93">
+        <f t="shared" ref="AW93" si="98">AO93-AS93</f>
+        <v>90</v>
+      </c>
+      <c r="AX93" s="10">
+        <f t="shared" ref="AX93" si="99">AP93-AT93</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="AN94">
+        <v>80</v>
+      </c>
+      <c r="AO94">
+        <v>170</v>
+      </c>
+      <c r="AP94">
+        <v>170</v>
+      </c>
+      <c r="AQ94" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR94">
+        <v>60</v>
+      </c>
+      <c r="AS94">
+        <v>130</v>
+      </c>
+      <c r="AT94">
+        <v>130</v>
+      </c>
+      <c r="AU94" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV94">
+        <f t="shared" ref="AV94" si="100">AN94-AR94</f>
+        <v>20</v>
+      </c>
+      <c r="AW94">
+        <f t="shared" ref="AW94" si="101">AO94-AS94</f>
+        <v>40</v>
+      </c>
+      <c r="AX94" s="10">
+        <f t="shared" ref="AX94" si="102">AP94-AT94</f>
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
prep predict3dunet 231212-3 to 231212-10
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBAAD3F-5B4C-4A69-9B11-0CC393BD023D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1D1EE8-D67C-4145-93AF-5BED97692532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="2595" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="404">
   <si>
     <t>patch z</t>
   </si>
@@ -1035,9 +1035,6 @@
     <t>Failure: Error, invalid patch shape &amp;/ invalid stride shape (torch.size error). A predict3dunet output line says "The shape of the output prediction maps (CDHW): (1, 125, 1169, 414)", and there are 700 patches. Therefore, predict3dunet tries to segment the whole image. I will try with the same patch shape used for training this model.</t>
   </si>
   <si>
-    <t>Explore sample data regarding predict3dunet valid patch &amp; stride shapes.</t>
-  </si>
-  <si>
     <t>I expect, however illogical based on my current knowledge, that it seems to be easier to pick valid patch &amp; stride shapes than with my own datasets.</t>
   </si>
   <si>
@@ -1195,6 +1192,63 @@
   </si>
   <si>
     <t>stride = same as in the github README.md under prediction tips ( https://github.com/wolny/pytorch-3dunet#prediction-tips ). Also same as in previous session, chpt-231212-1.</t>
+  </si>
+  <si>
+    <t>231212-3</t>
+  </si>
+  <si>
+    <t>231212-4</t>
+  </si>
+  <si>
+    <t>231212-5</t>
+  </si>
+  <si>
+    <t>231212-6</t>
+  </si>
+  <si>
+    <t>231212-7</t>
+  </si>
+  <si>
+    <t>231212-8</t>
+  </si>
+  <si>
+    <t>231212-9</t>
+  </si>
+  <si>
+    <t>231212-10</t>
+  </si>
+  <si>
+    <t>Explore sample data regarding predict3dunet valid patch &amp; stride shapes. 3dunet1.6.0</t>
+  </si>
+  <si>
+    <t>Explore sample data regarding predict3dunet valid patch &amp; stride shapes. 3dunet1.8.0</t>
+  </si>
+  <si>
+    <t>Explore sample data regarding predict3dunet valid patch &amp; stride shapes. 3dunet1.6.0, cluster module cuda 12.2.1</t>
+  </si>
+  <si>
+    <t>lookup (probably variable)</t>
+  </si>
+  <si>
+    <t>5?</t>
+  </si>
+  <si>
+    <t>1?</t>
+  </si>
+  <si>
+    <t>6?</t>
+  </si>
+  <si>
+    <t>8?</t>
+  </si>
+  <si>
+    <t>16?</t>
+  </si>
+  <si>
+    <t>uint16?</t>
+  </si>
+  <si>
+    <t>uint8?</t>
   </si>
 </sst>
 </file>
@@ -1427,7 +1481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1481,6 +1535,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1797,37 +1860,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BC94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK63" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT83" sqref="AT83"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AQ68" sqref="AQ68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="64.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="14.5703125" style="6" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="33" customWidth="1"/>
-    <col min="11" max="17" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="9.140625" style="20"/>
-    <col min="19" max="19" width="12.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="6.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="5.140625" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="11.140625" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="6" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="14.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="9.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="9" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="9.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="9.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="9.7109375" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="15.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="64.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="14.5703125" style="6" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="8.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="30.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="9.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="33" customWidth="1" collapsed="1"/>
+    <col min="11" max="17" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="9.140625" style="20" collapsed="1"/>
+    <col min="19" max="19" width="12.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="20" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="9.140625" collapsed="1"/>
+    <col min="22" max="22" width="6.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="5.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="11.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="6" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="14.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="9.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="9" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="9.42578125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="9.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="9.7109375" style="10" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="16.7109375" customWidth="1" collapsed="1"/>
     <col min="33" max="34" width="14.85546875" customWidth="1"/>
     <col min="35" max="35" width="21" customWidth="1"/>
     <col min="36" max="36" width="26.28515625" style="10" hidden="1" customWidth="1" outlineLevel="1"/>
@@ -13704,7 +13768,7 @@
         <v>317</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F74" s="7">
         <v>0</v>
@@ -13845,16 +13909,16 @@
         <v>98</v>
       </c>
       <c r="AY74" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AZ74" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="AZ74" s="4" t="s">
+      <c r="BA74" s="4">
+        <v>1</v>
+      </c>
+      <c r="BB74" s="4" t="s">
         <v>335</v>
-      </c>
-      <c r="BA74" s="4">
-        <v>1</v>
-      </c>
-      <c r="BB74" s="4" t="s">
-        <v>336</v>
       </c>
       <c r="BC74" s="4" t="s">
         <v>292</v>
@@ -13862,19 +13926,19 @@
     </row>
     <row r="75" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B75" t="s">
         <v>281</v>
       </c>
       <c r="C75" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="D75" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="D75" s="12" t="s">
-        <v>341</v>
-      </c>
       <c r="E75" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F75" s="6">
         <v>0</v>
@@ -13883,7 +13947,7 @@
         <v>1</v>
       </c>
       <c r="H75" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -13916,10 +13980,10 @@
         <v>0</v>
       </c>
       <c r="S75" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="T75" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="U75" t="s">
         <v>8</v>
@@ -13937,22 +14001,22 @@
         <v>4</v>
       </c>
       <c r="Z75" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AA75" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AB75" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC75" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AD75" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AE75" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AF75" t="s">
         <v>8</v>
@@ -13967,13 +14031,13 @@
         <v>8</v>
       </c>
       <c r="AK75" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AL75" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AM75" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AN75">
         <v>80</v>
@@ -14012,36 +14076,36 @@
         <v>80</v>
       </c>
       <c r="AY75" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AZ75" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BA75">
         <v>1</v>
       </c>
       <c r="BB75" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="BC75" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="76" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B76" t="s">
         <v>281</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F76" s="6">
         <v>0</v>
@@ -14050,7 +14114,7 @@
         <v>1</v>
       </c>
       <c r="H76" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -14083,10 +14147,10 @@
         <v>0</v>
       </c>
       <c r="S76" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="T76" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="U76" t="s">
         <v>8</v>
@@ -14104,22 +14168,22 @@
         <v>4</v>
       </c>
       <c r="Z76" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AA76" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AB76" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC76" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AD76" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AE76" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AF76" t="s">
         <v>8</v>
@@ -14134,13 +14198,13 @@
         <v>8</v>
       </c>
       <c r="AK76" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AL76" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AM76" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AN76">
         <v>80</v>
@@ -14179,49 +14243,49 @@
         <v>80</v>
       </c>
       <c r="AY76" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AZ76" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="BA76">
         <v>1</v>
       </c>
       <c r="BB76" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="BC76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="77" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="BB77" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="78" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="BB78" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="79" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B79" t="s">
         <v>123</v>
       </c>
       <c r="C79" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="D79" s="12" t="s">
         <v>361</v>
-      </c>
-      <c r="D79" s="12" t="s">
-        <v>362</v>
       </c>
       <c r="E79" t="s">
         <v>323</v>
@@ -14266,43 +14330,43 @@
         <v>0</v>
       </c>
       <c r="S79" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="T79" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="U79" t="s">
         <v>8</v>
       </c>
       <c r="V79" t="s">
+        <v>371</v>
+      </c>
+      <c r="W79" t="s">
+        <v>371</v>
+      </c>
+      <c r="X79" t="s">
         <v>372</v>
-      </c>
-      <c r="W79" t="s">
-        <v>372</v>
-      </c>
-      <c r="X79" t="s">
-        <v>373</v>
       </c>
       <c r="Y79">
         <v>4</v>
       </c>
       <c r="Z79" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AA79" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AB79" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC79" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AD79" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AE79" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AF79" t="s">
         <v>8</v>
@@ -14362,16 +14426,16 @@
         <v>130</v>
       </c>
       <c r="AY79" t="s">
+        <v>363</v>
+      </c>
+      <c r="AZ79" t="s">
+        <v>362</v>
+      </c>
+      <c r="BA79">
+        <v>1</v>
+      </c>
+      <c r="BB79" t="s">
         <v>364</v>
-      </c>
-      <c r="AZ79" t="s">
-        <v>363</v>
-      </c>
-      <c r="BA79">
-        <v>1</v>
-      </c>
-      <c r="BB79" t="s">
-        <v>365</v>
       </c>
       <c r="BC79" t="s">
         <v>292</v>
@@ -14379,118 +14443,118 @@
     </row>
     <row r="80" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B80" t="s">
         <v>123</v>
       </c>
       <c r="C80" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="E80" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="F80" s="6">
+        <v>0</v>
+      </c>
+      <c r="G80" s="12">
+        <v>1</v>
+      </c>
+      <c r="H80" t="s">
+        <v>376</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80" t="s">
+        <v>8</v>
+      </c>
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="M80">
+        <v>1</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+      <c r="P80" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q80" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R80" s="20">
+        <v>1</v>
+      </c>
+      <c r="S80" t="s">
+        <v>348</v>
+      </c>
+      <c r="T80" t="s">
+        <v>347</v>
+      </c>
+      <c r="U80" t="s">
         <v>371</v>
       </c>
-      <c r="D80" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="E80" s="12" t="s">
-        <v>376</v>
-      </c>
-      <c r="F80" s="6">
-        <v>0</v>
-      </c>
-      <c r="G80" s="12">
-        <v>1</v>
-      </c>
-      <c r="H80" t="s">
-        <v>377</v>
-      </c>
-      <c r="I80">
-        <v>0</v>
-      </c>
-      <c r="J80" t="s">
-        <v>8</v>
-      </c>
-      <c r="K80">
-        <v>1</v>
-      </c>
-      <c r="L80">
-        <v>1</v>
-      </c>
-      <c r="M80">
-        <v>1</v>
-      </c>
-      <c r="N80">
-        <v>0</v>
-      </c>
-      <c r="O80">
-        <v>0</v>
-      </c>
-      <c r="P80" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q80" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="R80" s="20">
-        <v>1</v>
-      </c>
-      <c r="S80" t="s">
-        <v>349</v>
-      </c>
-      <c r="T80" t="s">
-        <v>348</v>
-      </c>
-      <c r="U80" t="s">
+      <c r="V80" t="s">
+        <v>371</v>
+      </c>
+      <c r="W80" t="s">
+        <v>371</v>
+      </c>
+      <c r="X80" t="s">
         <v>372</v>
-      </c>
-      <c r="V80" t="s">
-        <v>372</v>
-      </c>
-      <c r="W80" t="s">
-        <v>372</v>
-      </c>
-      <c r="X80" t="s">
-        <v>373</v>
       </c>
       <c r="Y80">
         <v>4</v>
       </c>
       <c r="Z80" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AA80" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AB80" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC80" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AD80" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AE80" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AF80" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AG80" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AH80" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AI80" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AK80" t="s">
+        <v>366</v>
+      </c>
+      <c r="AL80" t="s">
         <v>367</v>
       </c>
-      <c r="AL80" t="s">
+      <c r="AM80" s="20" t="s">
         <v>368</v>
-      </c>
-      <c r="AM80" s="20" t="s">
-        <v>369</v>
       </c>
       <c r="AN80">
         <v>80</v>
@@ -14532,7 +14596,7 @@
         <v>66</v>
       </c>
       <c r="AZ80" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="BA80">
         <v>0</v>
@@ -14546,20 +14610,20 @@
     </row>
     <row r="81" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B81" t="s">
         <v>123</v>
       </c>
       <c r="C81" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="E81" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="D81" s="12" t="s">
-        <v>362</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>376</v>
-      </c>
       <c r="F81" s="6">
         <v>1</v>
       </c>
@@ -14600,43 +14664,43 @@
         <v>0</v>
       </c>
       <c r="S81" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="T81" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="U81" t="s">
         <v>121</v>
       </c>
       <c r="V81" t="s">
+        <v>371</v>
+      </c>
+      <c r="W81" t="s">
+        <v>371</v>
+      </c>
+      <c r="X81" t="s">
         <v>372</v>
-      </c>
-      <c r="W81" t="s">
-        <v>372</v>
-      </c>
-      <c r="X81" t="s">
-        <v>373</v>
       </c>
       <c r="Y81">
         <v>4</v>
       </c>
       <c r="Z81" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AA81" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AB81" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AC81" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AD81" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AE81" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AF81" t="s">
         <v>121</v>
@@ -14651,13 +14715,13 @@
         <v>121</v>
       </c>
       <c r="AK81" t="s">
+        <v>366</v>
+      </c>
+      <c r="AL81" t="s">
         <v>367</v>
       </c>
-      <c r="AL81" t="s">
+      <c r="AM81" s="20" t="s">
         <v>368</v>
-      </c>
-      <c r="AM81" s="20" t="s">
-        <v>369</v>
       </c>
       <c r="AN81">
         <v>80</v>
@@ -14699,7 +14763,7 @@
         <v>66</v>
       </c>
       <c r="AZ81" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="BA81">
         <v>0</v>
@@ -14711,191 +14775,191 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
+    <row r="82" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="39" t="s">
+        <v>377</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C82" s="39" t="s">
+        <v>393</v>
+      </c>
+      <c r="D82" s="39" t="s">
+        <v>332</v>
+      </c>
+      <c r="E82" s="39" t="s">
         <v>378</v>
       </c>
-      <c r="B82" t="s">
-        <v>281</v>
-      </c>
-      <c r="C82" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="D82" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="E82" s="12" t="s">
-        <v>379</v>
-      </c>
-      <c r="F82" s="6">
-        <v>0</v>
-      </c>
-      <c r="G82">
-        <v>1</v>
-      </c>
-      <c r="H82" s="13" t="s">
+      <c r="F82" s="42">
+        <v>0</v>
+      </c>
+      <c r="G82" s="3">
+        <v>1</v>
+      </c>
+      <c r="H82" s="43" t="s">
         <v>301</v>
       </c>
-      <c r="I82">
-        <v>0</v>
-      </c>
-      <c r="J82" t="s">
-        <v>8</v>
-      </c>
-      <c r="K82" t="s">
-        <v>8</v>
-      </c>
-      <c r="L82" t="s">
-        <v>8</v>
-      </c>
-      <c r="M82" t="s">
-        <v>8</v>
-      </c>
-      <c r="N82" t="s">
-        <v>8</v>
-      </c>
-      <c r="O82" t="s">
-        <v>8</v>
-      </c>
-      <c r="P82" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q82" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="R82" s="20">
-        <v>0</v>
-      </c>
-      <c r="S82" t="s">
-        <v>349</v>
-      </c>
-      <c r="T82" t="s">
+      <c r="I82" s="3">
+        <v>0</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q82" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="R82" s="44">
+        <v>0</v>
+      </c>
+      <c r="S82" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="U82" t="s">
-        <v>121</v>
-      </c>
-      <c r="V82">
-        <v>5</v>
-      </c>
-      <c r="W82">
-        <v>1</v>
-      </c>
-      <c r="X82">
-        <v>6</v>
-      </c>
-      <c r="Y82">
-        <v>1</v>
-      </c>
-      <c r="Z82">
-        <v>1</v>
-      </c>
-      <c r="AA82">
-        <v>16</v>
-      </c>
-      <c r="AB82" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC82">
-        <v>1</v>
-      </c>
-      <c r="AD82">
-        <v>8</v>
-      </c>
-      <c r="AE82" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="AF82" t="s">
-        <v>121</v>
-      </c>
-      <c r="AG82" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="AH82" t="s">
-        <v>121</v>
-      </c>
-      <c r="AI82" t="s">
+      <c r="T82" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="U82" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="V82" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="W82" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="X82" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="Y82" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="Z82" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AA82" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="AB82" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="AC82" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="AD82" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="AE82" s="45" t="s">
+        <v>403</v>
+      </c>
+      <c r="AF82" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG82" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH82" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI82" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="AJ82" s="10" t="s">
+      <c r="AJ82" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="AK82">
-        <v>125</v>
-      </c>
-      <c r="AL82">
-        <v>1169</v>
-      </c>
-      <c r="AM82" s="20">
-        <v>414</v>
-      </c>
-      <c r="AN82">
+      <c r="AK82" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL82" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM82" s="44" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN82" s="3">
         <v>80</v>
       </c>
-      <c r="AO82">
+      <c r="AO82" s="3">
         <v>170</v>
       </c>
-      <c r="AP82">
+      <c r="AP82" s="3">
         <v>170</v>
       </c>
-      <c r="AQ82" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR82">
+      <c r="AQ82" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR82" s="3">
         <v>40</v>
       </c>
-      <c r="AS82">
+      <c r="AS82" s="3">
         <v>90</v>
       </c>
-      <c r="AT82">
+      <c r="AT82" s="3">
         <v>90</v>
       </c>
-      <c r="AU82" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV82">
+      <c r="AU82" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV82" s="3">
         <f t="shared" ref="AV82:AX83" si="84">AN82-AR82</f>
         <v>40</v>
       </c>
-      <c r="AW82">
+      <c r="AW82" s="3">
         <f t="shared" si="84"/>
         <v>80</v>
       </c>
-      <c r="AX82" s="10">
+      <c r="AX82" s="45">
         <f t="shared" si="84"/>
         <v>80</v>
       </c>
-      <c r="AY82" t="s">
-        <v>346</v>
-      </c>
-      <c r="AZ82" t="s">
+      <c r="AY82" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="BA82">
-        <v>1</v>
-      </c>
-      <c r="BB82" t="s">
+      <c r="AZ82" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="BA82" s="3">
+        <v>1</v>
+      </c>
+      <c r="BB82" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="BC82" t="s">
+      <c r="BC82" s="3" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="83" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B83" t="s">
         <v>281</v>
       </c>
       <c r="C83" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="D83" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="D83" s="12" t="s">
-        <v>333</v>
-      </c>
       <c r="E83" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>121</v>
@@ -14937,43 +15001,13 @@
         <v>121</v>
       </c>
       <c r="S83" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="T83" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="U83" t="s">
         <v>121</v>
-      </c>
-      <c r="V83">
-        <v>5</v>
-      </c>
-      <c r="W83">
-        <v>1</v>
-      </c>
-      <c r="X83">
-        <v>6</v>
-      </c>
-      <c r="Y83">
-        <v>1</v>
-      </c>
-      <c r="Z83">
-        <v>1</v>
-      </c>
-      <c r="AA83">
-        <v>16</v>
-      </c>
-      <c r="AB83" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC83">
-        <v>1</v>
-      </c>
-      <c r="AD83">
-        <v>8</v>
-      </c>
-      <c r="AE83" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="AF83" t="s">
         <v>121</v>
@@ -14990,34 +15024,34 @@
       <c r="AJ83" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK83">
-        <v>125</v>
-      </c>
-      <c r="AL83">
-        <v>1169</v>
-      </c>
-      <c r="AM83" s="20">
-        <v>414</v>
-      </c>
-      <c r="AN83" s="3">
+      <c r="AK83" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL83" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM83" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN83" s="40">
         <v>80</v>
       </c>
-      <c r="AO83" s="3">
+      <c r="AO83" s="40">
         <v>240</v>
       </c>
-      <c r="AP83" s="3">
+      <c r="AP83" s="40">
         <v>240</v>
       </c>
-      <c r="AQ83" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR83" s="3">
+      <c r="AQ83" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR83" s="40">
         <v>64</v>
       </c>
-      <c r="AS83" s="3">
+      <c r="AS83" s="40">
         <v>144</v>
       </c>
-      <c r="AT83" s="3">
+      <c r="AT83" s="40">
         <v>144</v>
       </c>
       <c r="AU83" s="25" t="s">
@@ -15053,19 +15087,19 @@
     </row>
     <row r="84" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B84" t="s">
         <v>281</v>
       </c>
       <c r="C84" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="D84" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="D84" s="12" t="s">
-        <v>333</v>
-      </c>
       <c r="E84" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>121</v>
@@ -15107,43 +15141,13 @@
         <v>121</v>
       </c>
       <c r="S84" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="T84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="U84" t="s">
         <v>121</v>
-      </c>
-      <c r="V84">
-        <v>5</v>
-      </c>
-      <c r="W84">
-        <v>1</v>
-      </c>
-      <c r="X84">
-        <v>6</v>
-      </c>
-      <c r="Y84">
-        <v>1</v>
-      </c>
-      <c r="Z84">
-        <v>1</v>
-      </c>
-      <c r="AA84">
-        <v>16</v>
-      </c>
-      <c r="AB84" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC84">
-        <v>1</v>
-      </c>
-      <c r="AD84">
-        <v>8</v>
-      </c>
-      <c r="AE84" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="AF84" t="s">
         <v>121</v>
@@ -15160,34 +15164,34 @@
       <c r="AJ84" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK84">
-        <v>125</v>
-      </c>
-      <c r="AL84">
-        <v>1169</v>
-      </c>
-      <c r="AM84" s="20">
-        <v>414</v>
-      </c>
-      <c r="AN84" s="3">
+      <c r="AK84" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL84" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM84" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN84" s="40">
         <v>80</v>
       </c>
-      <c r="AO84" s="3">
+      <c r="AO84" s="40">
         <v>240</v>
       </c>
-      <c r="AP84" s="3">
+      <c r="AP84" s="40">
         <v>240</v>
       </c>
-      <c r="AQ84" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR84" s="3">
+      <c r="AQ84" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR84" s="40">
         <v>48</v>
       </c>
-      <c r="AS84" s="3">
+      <c r="AS84" s="40">
         <v>208</v>
       </c>
-      <c r="AT84" s="3">
+      <c r="AT84" s="40">
         <v>208</v>
       </c>
       <c r="AU84" s="25" t="s">
@@ -15209,7 +15213,7 @@
         <v>293</v>
       </c>
       <c r="AZ84" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="BA84" t="s">
         <v>121</v>
@@ -15223,19 +15227,19 @@
     </row>
     <row r="85" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B85" t="s">
         <v>281</v>
       </c>
       <c r="C85" s="12" t="s">
+        <v>393</v>
+      </c>
+      <c r="D85" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="D85" s="12" t="s">
-        <v>333</v>
-      </c>
       <c r="E85" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>121</v>
@@ -15277,43 +15281,13 @@
         <v>121</v>
       </c>
       <c r="S85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="T85" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="U85" t="s">
         <v>121</v>
-      </c>
-      <c r="V85">
-        <v>5</v>
-      </c>
-      <c r="W85">
-        <v>1</v>
-      </c>
-      <c r="X85">
-        <v>6</v>
-      </c>
-      <c r="Y85">
-        <v>1</v>
-      </c>
-      <c r="Z85">
-        <v>1</v>
-      </c>
-      <c r="AA85">
-        <v>16</v>
-      </c>
-      <c r="AB85" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC85">
-        <v>1</v>
-      </c>
-      <c r="AD85">
-        <v>8</v>
-      </c>
-      <c r="AE85" s="10" t="s">
-        <v>100</v>
       </c>
       <c r="AF85" t="s">
         <v>121</v>
@@ -15330,34 +15304,34 @@
       <c r="AJ85" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK85">
-        <v>125</v>
-      </c>
-      <c r="AL85">
-        <v>1169</v>
-      </c>
-      <c r="AM85" s="20">
-        <v>414</v>
-      </c>
-      <c r="AN85" s="3">
+      <c r="AK85" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL85" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM85" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN85" s="40">
         <v>64</v>
       </c>
-      <c r="AO85" s="3">
+      <c r="AO85" s="40">
         <v>128</v>
       </c>
-      <c r="AP85" s="3">
+      <c r="AP85" s="40">
         <v>128</v>
       </c>
-      <c r="AQ85" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR85" s="3">
+      <c r="AQ85" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR85" s="40">
         <v>32</v>
       </c>
-      <c r="AS85" s="3">
+      <c r="AS85" s="40">
         <v>96</v>
       </c>
-      <c r="AT85" s="3">
+      <c r="AT85" s="40">
         <v>96</v>
       </c>
       <c r="AU85" s="25" t="s">
@@ -15376,311 +15350,1311 @@
         <v>32</v>
       </c>
       <c r="AY85" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AZ85" t="s">
+        <v>384</v>
+      </c>
+      <c r="BA85" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB85" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC85" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="86" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="39" t="s">
         <v>385</v>
       </c>
-      <c r="BA85" t="s">
-        <v>121</v>
-      </c>
-      <c r="BB85" t="s">
-        <v>121</v>
-      </c>
-      <c r="BC85" t="s">
+      <c r="B86" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C86" s="39" t="s">
+        <v>394</v>
+      </c>
+      <c r="D86" s="39" t="s">
+        <v>332</v>
+      </c>
+      <c r="E86" s="39" t="s">
+        <v>337</v>
+      </c>
+      <c r="F86" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="M86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="N86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="P86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q86" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="R86" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="S86" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="T86" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="U86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE86" s="45"/>
+      <c r="AF86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG86" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI86" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ86" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK86" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL86" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM86" s="44" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN86" s="3">
+        <v>80</v>
+      </c>
+      <c r="AO86" s="3">
+        <v>170</v>
+      </c>
+      <c r="AP86" s="3">
+        <v>170</v>
+      </c>
+      <c r="AQ86" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR86" s="3">
+        <v>40</v>
+      </c>
+      <c r="AS86" s="3">
+        <v>90</v>
+      </c>
+      <c r="AT86" s="3">
+        <v>90</v>
+      </c>
+      <c r="AU86" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV86" s="3">
+        <f t="shared" ref="AV86" si="91">AN86-AR86</f>
+        <v>40</v>
+      </c>
+      <c r="AW86" s="3">
+        <f t="shared" ref="AW86" si="92">AO86-AS86</f>
+        <v>80</v>
+      </c>
+      <c r="AX86" s="45">
+        <f t="shared" ref="AX86" si="93">AP86-AT86</f>
+        <v>80</v>
+      </c>
+      <c r="AY86" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="AZ86" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="BA86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC86" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="86" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B86" t="s">
-        <v>121</v>
-      </c>
-      <c r="C86" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E86" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="F86" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="G86" t="s">
-        <v>121</v>
-      </c>
-      <c r="H86" t="s">
-        <v>121</v>
-      </c>
-      <c r="I86" t="s">
-        <v>121</v>
-      </c>
-      <c r="J86" t="s">
-        <v>121</v>
-      </c>
-      <c r="K86" t="s">
-        <v>121</v>
-      </c>
-      <c r="L86" t="s">
-        <v>121</v>
-      </c>
-      <c r="M86" t="s">
-        <v>121</v>
-      </c>
-      <c r="N86" t="s">
-        <v>121</v>
-      </c>
-      <c r="O86" t="s">
-        <v>121</v>
-      </c>
-      <c r="P86" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q86" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="R86" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="S86" t="s">
-        <v>121</v>
-      </c>
-      <c r="T86" t="s">
-        <v>121</v>
-      </c>
-      <c r="U86" t="s">
-        <v>121</v>
-      </c>
-      <c r="V86" t="s">
-        <v>121</v>
-      </c>
-      <c r="W86" t="s">
-        <v>121</v>
-      </c>
-      <c r="X86" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y86" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AC86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AD86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AE86" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="AF86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AG86" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="AH86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AI86" t="s">
+    <row r="87" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A87" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="B87" t="s">
+        <v>281</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="E87" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F87" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G87" t="s">
+        <v>121</v>
+      </c>
+      <c r="H87" t="s">
+        <v>121</v>
+      </c>
+      <c r="I87" t="s">
+        <v>121</v>
+      </c>
+      <c r="J87" t="s">
+        <v>121</v>
+      </c>
+      <c r="K87" t="s">
+        <v>121</v>
+      </c>
+      <c r="L87" t="s">
+        <v>121</v>
+      </c>
+      <c r="M87" t="s">
+        <v>121</v>
+      </c>
+      <c r="N87" t="s">
+        <v>121</v>
+      </c>
+      <c r="O87" t="s">
+        <v>121</v>
+      </c>
+      <c r="P87" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q87" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R87" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S87" t="s">
+        <v>348</v>
+      </c>
+      <c r="T87" t="s">
+        <v>347</v>
+      </c>
+      <c r="U87" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF87" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG87" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH87" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI87" t="s">
         <v>285</v>
       </c>
-      <c r="AJ86" s="10" t="s">
+      <c r="AJ87" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AM86" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AO86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AP86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AQ86" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AR86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AS86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AT86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AU86" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AV86" t="e">
-        <f t="shared" ref="AV86" si="91">AN86-AR86</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AW86" t="e">
-        <f t="shared" ref="AW86" si="92">AO86-AS86</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AX86" s="10" t="e">
-        <f t="shared" ref="AX86" si="93">AP86-AT86</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY86" t="s">
-        <v>121</v>
-      </c>
-      <c r="AZ86" t="s">
-        <v>121</v>
-      </c>
-      <c r="BA86" t="s">
-        <v>121</v>
-      </c>
-      <c r="BB86" t="s">
-        <v>121</v>
-      </c>
-      <c r="BC86" t="s">
+      <c r="AK87" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL87" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM87" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN87" s="40">
+        <v>80</v>
+      </c>
+      <c r="AO87" s="40">
+        <v>240</v>
+      </c>
+      <c r="AP87" s="40">
+        <v>240</v>
+      </c>
+      <c r="AQ87" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR87" s="40">
+        <v>64</v>
+      </c>
+      <c r="AS87" s="40">
+        <v>144</v>
+      </c>
+      <c r="AT87" s="40">
+        <v>144</v>
+      </c>
+      <c r="AU87" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV87">
+        <f t="shared" ref="AV87" si="94">AN87-AR87</f>
+        <v>16</v>
+      </c>
+      <c r="AW87">
+        <f t="shared" ref="AW87" si="95">AO87-AS87</f>
+        <v>96</v>
+      </c>
+      <c r="AX87" s="10">
+        <f t="shared" ref="AX87" si="96">AP87-AT87</f>
+        <v>96</v>
+      </c>
+      <c r="AY87" t="s">
+        <v>293</v>
+      </c>
+      <c r="AZ87" t="s">
+        <v>294</v>
+      </c>
+      <c r="BA87" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB87" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC87" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A88" s="12"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="Q88" s="12"/>
-      <c r="AG88" s="12"/>
+      <c r="A88" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="B88" t="s">
+        <v>281</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F88" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G88" t="s">
+        <v>121</v>
+      </c>
+      <c r="H88" t="s">
+        <v>121</v>
+      </c>
+      <c r="I88" t="s">
+        <v>121</v>
+      </c>
+      <c r="J88" t="s">
+        <v>121</v>
+      </c>
+      <c r="K88" t="s">
+        <v>121</v>
+      </c>
+      <c r="L88" t="s">
+        <v>121</v>
+      </c>
+      <c r="M88" t="s">
+        <v>121</v>
+      </c>
+      <c r="N88" t="s">
+        <v>121</v>
+      </c>
+      <c r="O88" t="s">
+        <v>121</v>
+      </c>
+      <c r="P88" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q88" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R88" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S88" t="s">
+        <v>348</v>
+      </c>
+      <c r="T88" t="s">
+        <v>347</v>
+      </c>
+      <c r="U88" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF88" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG88" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH88" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI88" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ88" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK88" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL88" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM88" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN88" s="40">
+        <v>80</v>
+      </c>
+      <c r="AO88" s="40">
+        <v>240</v>
+      </c>
+      <c r="AP88" s="40">
+        <v>240</v>
+      </c>
+      <c r="AQ88" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR88" s="40">
+        <v>48</v>
+      </c>
+      <c r="AS88" s="40">
+        <v>208</v>
+      </c>
+      <c r="AT88" s="40">
+        <v>208</v>
+      </c>
+      <c r="AU88" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV88">
+        <f t="shared" ref="AV88" si="97">AN88-AR88</f>
+        <v>32</v>
+      </c>
+      <c r="AW88">
+        <f t="shared" ref="AW88" si="98">AO88-AS88</f>
+        <v>32</v>
+      </c>
+      <c r="AX88" s="10">
+        <f t="shared" ref="AX88" si="99">AP88-AT88</f>
+        <v>32</v>
+      </c>
+      <c r="AY88" t="s">
+        <v>293</v>
+      </c>
+      <c r="AZ88" t="s">
+        <v>380</v>
+      </c>
+      <c r="BA88" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB88" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC88" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="89" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="B89" t="s">
+        <v>281</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="E89" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G89" t="s">
+        <v>121</v>
+      </c>
+      <c r="H89" t="s">
+        <v>121</v>
+      </c>
+      <c r="I89" t="s">
+        <v>121</v>
+      </c>
+      <c r="J89" t="s">
+        <v>121</v>
+      </c>
+      <c r="K89" t="s">
+        <v>121</v>
+      </c>
+      <c r="L89" t="s">
+        <v>121</v>
+      </c>
+      <c r="M89" t="s">
+        <v>121</v>
+      </c>
+      <c r="N89" t="s">
+        <v>121</v>
+      </c>
+      <c r="O89" t="s">
+        <v>121</v>
+      </c>
+      <c r="P89" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q89" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R89" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S89" t="s">
+        <v>348</v>
+      </c>
+      <c r="T89" t="s">
+        <v>347</v>
+      </c>
+      <c r="U89" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF89" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG89" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH89" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI89" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ89" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK89" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL89" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM89" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN89" s="40">
+        <v>64</v>
+      </c>
+      <c r="AO89" s="40">
+        <v>128</v>
+      </c>
+      <c r="AP89" s="40">
+        <v>128</v>
+      </c>
+      <c r="AQ89" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR89" s="40">
+        <v>32</v>
+      </c>
+      <c r="AS89" s="40">
+        <v>96</v>
+      </c>
+      <c r="AT89" s="40">
+        <v>96</v>
+      </c>
+      <c r="AU89" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV89">
+        <f t="shared" ref="AV89" si="100">AN89-AR89</f>
+        <v>32</v>
+      </c>
+      <c r="AW89">
+        <f t="shared" ref="AW89" si="101">AO89-AS89</f>
+        <v>32</v>
+      </c>
+      <c r="AX89" s="10">
+        <f t="shared" ref="AX89" si="102">AP89-AT89</f>
+        <v>32</v>
+      </c>
+      <c r="AY89" t="s">
+        <v>379</v>
+      </c>
+      <c r="AZ89" t="s">
+        <v>384</v>
+      </c>
+      <c r="BA89" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB89" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC89" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="39" t="s">
+        <v>389</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C90" s="39" t="s">
+        <v>395</v>
+      </c>
+      <c r="D90" s="39" t="s">
+        <v>332</v>
+      </c>
+      <c r="E90" s="39" t="s">
+        <v>337</v>
+      </c>
+      <c r="F90" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="M90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="O90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="P90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q90" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="R90" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="T90" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE90" s="45"/>
+      <c r="AF90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG90" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI90" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ90" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK90" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL90" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM90" s="44" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN90" s="3">
+        <v>80</v>
+      </c>
+      <c r="AO90" s="3">
+        <v>170</v>
+      </c>
+      <c r="AP90" s="3">
+        <v>170</v>
+      </c>
+      <c r="AQ90" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR90" s="3">
+        <v>40</v>
+      </c>
+      <c r="AS90" s="3">
+        <v>90</v>
+      </c>
+      <c r="AT90" s="3">
+        <v>90</v>
+      </c>
+      <c r="AU90" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV90" s="3">
+        <f t="shared" ref="AV90" si="103">AN90-AR90</f>
+        <v>40</v>
+      </c>
+      <c r="AW90" s="3">
+        <f t="shared" ref="AW90" si="104">AO90-AS90</f>
+        <v>80</v>
+      </c>
+      <c r="AX90" s="45">
+        <f t="shared" ref="AX90" si="105">AP90-AT90</f>
+        <v>80</v>
+      </c>
+      <c r="AY90" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="AZ90" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="BA90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB90" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC90" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="91" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A91" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="B91" t="s">
+        <v>281</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="E91" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G91" t="s">
+        <v>121</v>
+      </c>
+      <c r="H91" t="s">
+        <v>121</v>
+      </c>
+      <c r="I91" t="s">
+        <v>121</v>
+      </c>
+      <c r="J91" t="s">
+        <v>121</v>
+      </c>
+      <c r="K91" t="s">
+        <v>121</v>
+      </c>
+      <c r="L91" t="s">
+        <v>121</v>
+      </c>
+      <c r="M91" t="s">
+        <v>121</v>
+      </c>
+      <c r="N91" t="s">
+        <v>121</v>
+      </c>
+      <c r="O91" t="s">
+        <v>121</v>
+      </c>
+      <c r="P91" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q91" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R91" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S91" t="s">
+        <v>348</v>
+      </c>
+      <c r="T91" t="s">
+        <v>347</v>
+      </c>
+      <c r="U91" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF91" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG91" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH91" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI91" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ91" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK91" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL91" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM91" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN91" s="40">
+        <v>80</v>
+      </c>
+      <c r="AO91" s="40">
+        <v>240</v>
+      </c>
+      <c r="AP91" s="40">
+        <v>240</v>
+      </c>
+      <c r="AQ91" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR91" s="40">
+        <v>64</v>
+      </c>
+      <c r="AS91" s="40">
+        <v>144</v>
+      </c>
+      <c r="AT91" s="40">
+        <v>144</v>
+      </c>
+      <c r="AU91" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV91">
+        <f t="shared" ref="AV91" si="106">AN91-AR91</f>
+        <v>16</v>
+      </c>
+      <c r="AW91">
+        <f t="shared" ref="AW91" si="107">AO91-AS91</f>
+        <v>96</v>
+      </c>
+      <c r="AX91" s="10">
+        <f t="shared" ref="AX91" si="108">AP91-AT91</f>
+        <v>96</v>
+      </c>
+      <c r="AY91" t="s">
+        <v>293</v>
+      </c>
+      <c r="AZ91" t="s">
+        <v>294</v>
+      </c>
+      <c r="BA91" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB91" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC91" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="92" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AN92">
+      <c r="A92" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="B92" t="s">
+        <v>281</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="E92" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G92" t="s">
+        <v>121</v>
+      </c>
+      <c r="H92" t="s">
+        <v>121</v>
+      </c>
+      <c r="I92" t="s">
+        <v>121</v>
+      </c>
+      <c r="J92" t="s">
+        <v>121</v>
+      </c>
+      <c r="K92" t="s">
+        <v>121</v>
+      </c>
+      <c r="L92" t="s">
+        <v>121</v>
+      </c>
+      <c r="M92" t="s">
+        <v>121</v>
+      </c>
+      <c r="N92" t="s">
+        <v>121</v>
+      </c>
+      <c r="O92" t="s">
+        <v>121</v>
+      </c>
+      <c r="P92" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q92" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R92" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S92" t="s">
+        <v>348</v>
+      </c>
+      <c r="T92" t="s">
+        <v>347</v>
+      </c>
+      <c r="U92" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF92" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG92" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH92" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI92" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ92" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK92" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL92" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM92" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN92" s="40">
         <v>80</v>
       </c>
-      <c r="AO92">
-        <v>170</v>
-      </c>
-      <c r="AP92">
-        <v>170</v>
-      </c>
-      <c r="AQ92" s="20" t="s">
+      <c r="AO92" s="40">
+        <v>240</v>
+      </c>
+      <c r="AP92" s="40">
+        <v>240</v>
+      </c>
+      <c r="AQ92" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR92" s="40">
         <v>48</v>
       </c>
-      <c r="AR92">
-        <v>20</v>
-      </c>
-      <c r="AS92">
-        <v>40</v>
-      </c>
-      <c r="AT92">
-        <v>40</v>
-      </c>
-      <c r="AU92" s="20" t="s">
-        <v>48</v>
+      <c r="AS92" s="40">
+        <v>208</v>
+      </c>
+      <c r="AT92" s="40">
+        <v>208</v>
+      </c>
+      <c r="AU92" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="AV92">
-        <f t="shared" ref="AV92" si="94">AN92-AR92</f>
-        <v>60</v>
+        <f t="shared" ref="AV92" si="109">AN92-AR92</f>
+        <v>32</v>
       </c>
       <c r="AW92">
-        <f t="shared" ref="AW92" si="95">AO92-AS92</f>
-        <v>130</v>
+        <f t="shared" ref="AW92" si="110">AO92-AS92</f>
+        <v>32</v>
       </c>
       <c r="AX92" s="10">
-        <f t="shared" ref="AX92" si="96">AP92-AT92</f>
-        <v>130</v>
+        <f t="shared" ref="AX92" si="111">AP92-AT92</f>
+        <v>32</v>
+      </c>
+      <c r="AY92" t="s">
+        <v>293</v>
+      </c>
+      <c r="AZ92" t="s">
+        <v>380</v>
+      </c>
+      <c r="BA92" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB92" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC92" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AN93">
-        <v>80</v>
-      </c>
-      <c r="AO93">
-        <v>170</v>
-      </c>
-      <c r="AP93">
-        <v>170</v>
+      <c r="A93" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="B93" t="s">
+        <v>281</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="E93" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G93" t="s">
+        <v>121</v>
+      </c>
+      <c r="H93" t="s">
+        <v>121</v>
+      </c>
+      <c r="I93" t="s">
+        <v>121</v>
+      </c>
+      <c r="J93" t="s">
+        <v>121</v>
+      </c>
+      <c r="K93" t="s">
+        <v>121</v>
+      </c>
+      <c r="L93" t="s">
+        <v>121</v>
+      </c>
+      <c r="M93" t="s">
+        <v>121</v>
+      </c>
+      <c r="N93" t="s">
+        <v>121</v>
+      </c>
+      <c r="O93" t="s">
+        <v>121</v>
+      </c>
+      <c r="P93" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q93" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R93" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S93" t="s">
+        <v>348</v>
+      </c>
+      <c r="T93" t="s">
+        <v>347</v>
+      </c>
+      <c r="U93" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF93" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG93" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH93" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI93" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ93" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK93" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AL93" s="40" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM93" s="41" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN93" s="40">
+        <v>64</v>
+      </c>
+      <c r="AO93" s="40">
+        <v>128</v>
+      </c>
+      <c r="AP93" s="40">
+        <v>128</v>
       </c>
       <c r="AQ93" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR93">
-        <v>40</v>
-      </c>
-      <c r="AS93">
-        <v>80</v>
-      </c>
-      <c r="AT93">
-        <v>80</v>
+        <v>8</v>
+      </c>
+      <c r="AR93" s="40">
+        <v>32</v>
+      </c>
+      <c r="AS93" s="40">
+        <v>96</v>
+      </c>
+      <c r="AT93" s="40">
+        <v>96</v>
       </c>
       <c r="AU93" s="25" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="AV93">
-        <f t="shared" ref="AV93" si="97">AN93-AR93</f>
-        <v>40</v>
+        <f t="shared" ref="AV93" si="112">AN93-AR93</f>
+        <v>32</v>
       </c>
       <c r="AW93">
-        <f t="shared" ref="AW93" si="98">AO93-AS93</f>
-        <v>90</v>
+        <f t="shared" ref="AW93" si="113">AO93-AS93</f>
+        <v>32</v>
       </c>
       <c r="AX93" s="10">
-        <f t="shared" ref="AX93" si="99">AP93-AT93</f>
-        <v>90</v>
+        <f t="shared" ref="AX93" si="114">AP93-AT93</f>
+        <v>32</v>
+      </c>
+      <c r="AY93" t="s">
+        <v>379</v>
+      </c>
+      <c r="AZ93" t="s">
+        <v>384</v>
+      </c>
+      <c r="BA93" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB93" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC93" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="94" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AN94">
-        <v>80</v>
-      </c>
-      <c r="AO94">
-        <v>170</v>
-      </c>
-      <c r="AP94">
-        <v>170</v>
+      <c r="A94" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B94" t="s">
+        <v>121</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E94" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G94" t="s">
+        <v>121</v>
+      </c>
+      <c r="H94" t="s">
+        <v>121</v>
+      </c>
+      <c r="I94" t="s">
+        <v>121</v>
+      </c>
+      <c r="J94" t="s">
+        <v>121</v>
+      </c>
+      <c r="K94" t="s">
+        <v>121</v>
+      </c>
+      <c r="L94" t="s">
+        <v>121</v>
+      </c>
+      <c r="M94" t="s">
+        <v>121</v>
+      </c>
+      <c r="N94" t="s">
+        <v>121</v>
+      </c>
+      <c r="O94" t="s">
+        <v>121</v>
+      </c>
+      <c r="P94" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q94" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="R94" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="S94" t="s">
+        <v>121</v>
+      </c>
+      <c r="T94" t="s">
+        <v>121</v>
+      </c>
+      <c r="U94" t="s">
+        <v>121</v>
+      </c>
+      <c r="V94" t="s">
+        <v>121</v>
+      </c>
+      <c r="W94" t="s">
+        <v>121</v>
+      </c>
+      <c r="X94" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y94" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE94" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG94" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AH94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI94" t="s">
+        <v>285</v>
+      </c>
+      <c r="AJ94" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM94" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="AN94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AO94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP94" t="s">
+        <v>121</v>
       </c>
       <c r="AQ94" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR94">
-        <v>60</v>
-      </c>
-      <c r="AS94">
-        <v>130</v>
-      </c>
-      <c r="AT94">
-        <v>130</v>
+        <v>8</v>
+      </c>
+      <c r="AR94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AS94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AT94" t="s">
+        <v>121</v>
       </c>
       <c r="AU94" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="AV94">
-        <f t="shared" ref="AV94" si="100">AN94-AR94</f>
-        <v>20</v>
-      </c>
-      <c r="AW94">
-        <f t="shared" ref="AW94" si="101">AO94-AS94</f>
-        <v>40</v>
-      </c>
-      <c r="AX94" s="10">
-        <f t="shared" ref="AX94" si="102">AP94-AT94</f>
-        <v>40</v>
+        <v>8</v>
+      </c>
+      <c r="AV94" t="e">
+        <f t="shared" ref="AV87:AV94" si="115">AN94-AR94</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW94" t="e">
+        <f t="shared" ref="AW87:AW94" si="116">AO94-AS94</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AX94" s="10" t="e">
+        <f t="shared" ref="AX87:AX94" si="117">AP94-AT94</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY94" t="s">
+        <v>121</v>
+      </c>
+      <c r="AZ94" t="s">
+        <v>121</v>
+      </c>
+      <c r="BA94" t="s">
+        <v>121</v>
+      </c>
+      <c r="BB94" t="s">
+        <v>121</v>
+      </c>
+      <c r="BC94" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generic commit message, Mon 22:08:16 18.12.2023.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1D1EE8-D67C-4145-93AF-5BED97692532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57118E0C-5EEB-4655-B269-6C17127E9581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="408">
   <si>
     <t>patch z</t>
   </si>
@@ -1249,6 +1249,18 @@
   </si>
   <si>
     <t>uint8?</t>
+  </si>
+  <si>
+    <t>ValueError: requested an output size of torch.Size([11, 31, 31]), but valid sizes range from [9, 29, 29] to [10, 30, 30] (for an input of torch.Size([5, 15, 15]))</t>
+  </si>
+  <si>
+    <t>ValueError: requested an output size of torch.Size([9, 17, 17]), but valid sizes range from [7, 15, 15] to [8, 16, 16] (for an input of torch.Size([4, 8, 8]))</t>
+  </si>
+  <si>
+    <t>File "/home/dwalth/data/conda/envs/3dunet1.8.0/lib/python3.11/site-packages/torch/nn/modules/module.py", line 2152, in load_state_dict: raise RuntimeError('Error(s) in loading state_dict for {}:\n\t{}'.format(</t>
+  </si>
+  <si>
+    <t>RuntimeError: Error(s) in loading state_dict for ResidualUNet3D: Unexpected key(s) in state_dict: "decoders.0.upsampling.upsample.bias", "decoders.1.upsampling.upsample.bias", "decoders.2.upsampling.upsample.bias", "decoders.3.upsampling.upsample.bias".</t>
   </si>
 </sst>
 </file>
@@ -1481,7 +1493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1538,8 +1550,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1860,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BC94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ68" sqref="AQ68"/>
+    <sheetView tabSelected="1" topLeftCell="BB58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BC93" sqref="BC93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -14791,13 +14801,13 @@
       <c r="E82" s="39" t="s">
         <v>378</v>
       </c>
-      <c r="F82" s="42">
+      <c r="F82" s="40">
         <v>0</v>
       </c>
       <c r="G82" s="3">
         <v>1</v>
       </c>
-      <c r="H82" s="43" t="s">
+      <c r="H82" s="41" t="s">
         <v>301</v>
       </c>
       <c r="I82" s="3">
@@ -14827,7 +14837,7 @@
       <c r="Q82" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="R82" s="44">
+      <c r="R82" s="42">
         <v>0</v>
       </c>
       <c r="S82" s="3" t="s">
@@ -14866,7 +14876,7 @@
       <c r="AD82" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="AE82" s="45" t="s">
+      <c r="AE82" s="43" t="s">
         <v>403</v>
       </c>
       <c r="AF82" s="3" t="s">
@@ -14881,7 +14891,7 @@
       <c r="AI82" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="AJ82" s="45" t="s">
+      <c r="AJ82" s="43" t="s">
         <v>109</v>
       </c>
       <c r="AK82" s="3" t="s">
@@ -14890,7 +14900,7 @@
       <c r="AL82" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="AM82" s="44" t="s">
+      <c r="AM82" s="42" t="s">
         <v>396</v>
       </c>
       <c r="AN82" s="3">
@@ -14925,7 +14935,7 @@
         <f t="shared" si="84"/>
         <v>80</v>
       </c>
-      <c r="AX82" s="45">
+      <c r="AX82" s="43">
         <f t="shared" si="84"/>
         <v>80</v>
       </c>
@@ -15024,34 +15034,34 @@
       <c r="AJ83" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK83" s="40" t="s">
+      <c r="AK83" t="s">
         <v>396</v>
       </c>
-      <c r="AL83" s="40" t="s">
+      <c r="AL83" t="s">
         <v>396</v>
       </c>
-      <c r="AM83" s="41" t="s">
+      <c r="AM83" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="AN83" s="40">
+      <c r="AN83">
         <v>80</v>
       </c>
-      <c r="AO83" s="40">
+      <c r="AO83">
         <v>240</v>
       </c>
-      <c r="AP83" s="40">
+      <c r="AP83">
         <v>240</v>
       </c>
       <c r="AQ83" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AR83" s="40">
+      <c r="AR83">
         <v>64</v>
       </c>
-      <c r="AS83" s="40">
+      <c r="AS83">
         <v>144</v>
       </c>
-      <c r="AT83" s="40">
+      <c r="AT83">
         <v>144</v>
       </c>
       <c r="AU83" s="25" t="s">
@@ -15075,14 +15085,14 @@
       <c r="AZ83" t="s">
         <v>294</v>
       </c>
-      <c r="BA83" t="s">
-        <v>121</v>
+      <c r="BA83">
+        <v>1</v>
       </c>
       <c r="BB83" t="s">
-        <v>121</v>
+        <v>404</v>
       </c>
       <c r="BC83" t="s">
-        <v>121</v>
+        <v>292</v>
       </c>
     </row>
     <row r="84" spans="1:55" x14ac:dyDescent="0.25">
@@ -15164,34 +15174,34 @@
       <c r="AJ84" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK84" s="40" t="s">
+      <c r="AK84" t="s">
         <v>396</v>
       </c>
-      <c r="AL84" s="40" t="s">
+      <c r="AL84" t="s">
         <v>396</v>
       </c>
-      <c r="AM84" s="41" t="s">
+      <c r="AM84" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="AN84" s="40">
+      <c r="AN84">
         <v>80</v>
       </c>
-      <c r="AO84" s="40">
+      <c r="AO84">
         <v>240</v>
       </c>
-      <c r="AP84" s="40">
+      <c r="AP84">
         <v>240</v>
       </c>
       <c r="AQ84" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AR84" s="40">
+      <c r="AR84">
         <v>48</v>
       </c>
-      <c r="AS84" s="40">
+      <c r="AS84">
         <v>208</v>
       </c>
-      <c r="AT84" s="40">
+      <c r="AT84">
         <v>208</v>
       </c>
       <c r="AU84" s="25" t="s">
@@ -15215,14 +15225,14 @@
       <c r="AZ84" t="s">
         <v>380</v>
       </c>
-      <c r="BA84" t="s">
-        <v>121</v>
+      <c r="BA84">
+        <v>1</v>
       </c>
       <c r="BB84" t="s">
-        <v>121</v>
+        <v>404</v>
       </c>
       <c r="BC84" t="s">
-        <v>121</v>
+        <v>292</v>
       </c>
     </row>
     <row r="85" spans="1:55" x14ac:dyDescent="0.25">
@@ -15304,34 +15314,34 @@
       <c r="AJ85" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK85" s="40" t="s">
+      <c r="AK85" t="s">
         <v>396</v>
       </c>
-      <c r="AL85" s="40" t="s">
+      <c r="AL85" t="s">
         <v>396</v>
       </c>
-      <c r="AM85" s="41" t="s">
+      <c r="AM85" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="AN85" s="40">
+      <c r="AN85">
         <v>64</v>
       </c>
-      <c r="AO85" s="40">
+      <c r="AO85">
         <v>128</v>
       </c>
-      <c r="AP85" s="40">
+      <c r="AP85">
         <v>128</v>
       </c>
       <c r="AQ85" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AR85" s="40">
+      <c r="AR85">
         <v>32</v>
       </c>
-      <c r="AS85" s="40">
+      <c r="AS85">
         <v>96</v>
       </c>
-      <c r="AT85" s="40">
+      <c r="AT85">
         <v>96</v>
       </c>
       <c r="AU85" s="25" t="s">
@@ -15355,14 +15365,14 @@
       <c r="AZ85" t="s">
         <v>384</v>
       </c>
-      <c r="BA85" t="s">
-        <v>121</v>
+      <c r="BA85">
+        <v>1</v>
       </c>
       <c r="BB85" t="s">
-        <v>121</v>
+        <v>405</v>
       </c>
       <c r="BC85" t="s">
-        <v>121</v>
+        <v>292</v>
       </c>
     </row>
     <row r="86" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -15381,7 +15391,7 @@
       <c r="E86" s="39" t="s">
         <v>337</v>
       </c>
-      <c r="F86" s="42" t="s">
+      <c r="F86" s="40" t="s">
         <v>121</v>
       </c>
       <c r="G86" s="3" t="s">
@@ -15417,7 +15427,7 @@
       <c r="Q86" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="R86" s="44" t="s">
+      <c r="R86" s="42" t="s">
         <v>121</v>
       </c>
       <c r="S86" s="3" t="s">
@@ -15429,7 +15439,7 @@
       <c r="U86" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AE86" s="45"/>
+      <c r="AE86" s="43"/>
       <c r="AF86" s="3" t="s">
         <v>121</v>
       </c>
@@ -15442,7 +15452,7 @@
       <c r="AI86" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="AJ86" s="45" t="s">
+      <c r="AJ86" s="43" t="s">
         <v>109</v>
       </c>
       <c r="AK86" s="3" t="s">
@@ -15451,7 +15461,7 @@
       <c r="AL86" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="AM86" s="44" t="s">
+      <c r="AM86" s="42" t="s">
         <v>396</v>
       </c>
       <c r="AN86" s="3">
@@ -15486,7 +15496,7 @@
         <f t="shared" ref="AW86" si="92">AO86-AS86</f>
         <v>80</v>
       </c>
-      <c r="AX86" s="45">
+      <c r="AX86" s="43">
         <f t="shared" ref="AX86" si="93">AP86-AT86</f>
         <v>80</v>
       </c>
@@ -15496,14 +15506,14 @@
       <c r="AZ86" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="BA86" s="3" t="s">
-        <v>121</v>
+      <c r="BA86" s="3">
+        <v>1</v>
       </c>
       <c r="BB86" s="3" t="s">
-        <v>121</v>
+        <v>407</v>
       </c>
       <c r="BC86" s="3" t="s">
-        <v>121</v>
+        <v>406</v>
       </c>
     </row>
     <row r="87" spans="1:55" x14ac:dyDescent="0.25">
@@ -15585,34 +15595,34 @@
       <c r="AJ87" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK87" s="40" t="s">
+      <c r="AK87" t="s">
         <v>396</v>
       </c>
-      <c r="AL87" s="40" t="s">
+      <c r="AL87" t="s">
         <v>396</v>
       </c>
-      <c r="AM87" s="41" t="s">
+      <c r="AM87" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="AN87" s="40">
+      <c r="AN87">
         <v>80</v>
       </c>
-      <c r="AO87" s="40">
+      <c r="AO87">
         <v>240</v>
       </c>
-      <c r="AP87" s="40">
+      <c r="AP87">
         <v>240</v>
       </c>
       <c r="AQ87" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AR87" s="40">
+      <c r="AR87">
         <v>64</v>
       </c>
-      <c r="AS87" s="40">
+      <c r="AS87">
         <v>144</v>
       </c>
-      <c r="AT87" s="40">
+      <c r="AT87">
         <v>144</v>
       </c>
       <c r="AU87" s="25" t="s">
@@ -15636,14 +15646,14 @@
       <c r="AZ87" t="s">
         <v>294</v>
       </c>
-      <c r="BA87" t="s">
-        <v>121</v>
+      <c r="BA87">
+        <v>1</v>
       </c>
       <c r="BB87" t="s">
-        <v>121</v>
+        <v>407</v>
       </c>
       <c r="BC87" t="s">
-        <v>121</v>
+        <v>406</v>
       </c>
     </row>
     <row r="88" spans="1:55" x14ac:dyDescent="0.25">
@@ -15725,34 +15735,34 @@
       <c r="AJ88" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK88" s="40" t="s">
+      <c r="AK88" t="s">
         <v>396</v>
       </c>
-      <c r="AL88" s="40" t="s">
+      <c r="AL88" t="s">
         <v>396</v>
       </c>
-      <c r="AM88" s="41" t="s">
+      <c r="AM88" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="AN88" s="40">
+      <c r="AN88">
         <v>80</v>
       </c>
-      <c r="AO88" s="40">
+      <c r="AO88">
         <v>240</v>
       </c>
-      <c r="AP88" s="40">
+      <c r="AP88">
         <v>240</v>
       </c>
       <c r="AQ88" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AR88" s="40">
+      <c r="AR88">
         <v>48</v>
       </c>
-      <c r="AS88" s="40">
+      <c r="AS88">
         <v>208</v>
       </c>
-      <c r="AT88" s="40">
+      <c r="AT88">
         <v>208</v>
       </c>
       <c r="AU88" s="25" t="s">
@@ -15776,14 +15786,14 @@
       <c r="AZ88" t="s">
         <v>380</v>
       </c>
-      <c r="BA88" t="s">
-        <v>121</v>
+      <c r="BA88">
+        <v>1</v>
       </c>
       <c r="BB88" t="s">
-        <v>121</v>
+        <v>407</v>
       </c>
       <c r="BC88" t="s">
-        <v>121</v>
+        <v>406</v>
       </c>
     </row>
     <row r="89" spans="1:55" x14ac:dyDescent="0.25">
@@ -15865,34 +15875,34 @@
       <c r="AJ89" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK89" s="40" t="s">
+      <c r="AK89" t="s">
         <v>396</v>
       </c>
-      <c r="AL89" s="40" t="s">
+      <c r="AL89" t="s">
         <v>396</v>
       </c>
-      <c r="AM89" s="41" t="s">
+      <c r="AM89" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="AN89" s="40">
+      <c r="AN89">
         <v>64</v>
       </c>
-      <c r="AO89" s="40">
+      <c r="AO89">
         <v>128</v>
       </c>
-      <c r="AP89" s="40">
+      <c r="AP89">
         <v>128</v>
       </c>
       <c r="AQ89" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AR89" s="40">
+      <c r="AR89">
         <v>32</v>
       </c>
-      <c r="AS89" s="40">
+      <c r="AS89">
         <v>96</v>
       </c>
-      <c r="AT89" s="40">
+      <c r="AT89">
         <v>96</v>
       </c>
       <c r="AU89" s="25" t="s">
@@ -15916,14 +15926,14 @@
       <c r="AZ89" t="s">
         <v>384</v>
       </c>
-      <c r="BA89" t="s">
-        <v>121</v>
+      <c r="BA89">
+        <v>1</v>
       </c>
       <c r="BB89" t="s">
-        <v>121</v>
+        <v>407</v>
       </c>
       <c r="BC89" t="s">
-        <v>121</v>
+        <v>406</v>
       </c>
     </row>
     <row r="90" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -15942,7 +15952,7 @@
       <c r="E90" s="39" t="s">
         <v>337</v>
       </c>
-      <c r="F90" s="42" t="s">
+      <c r="F90" s="40" t="s">
         <v>121</v>
       </c>
       <c r="G90" s="3" t="s">
@@ -15978,7 +15988,7 @@
       <c r="Q90" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="R90" s="44" t="s">
+      <c r="R90" s="42" t="s">
         <v>121</v>
       </c>
       <c r="S90" s="3" t="s">
@@ -15990,7 +16000,7 @@
       <c r="U90" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AE90" s="45"/>
+      <c r="AE90" s="43"/>
       <c r="AF90" s="3" t="s">
         <v>121</v>
       </c>
@@ -16003,7 +16013,7 @@
       <c r="AI90" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="AJ90" s="45" t="s">
+      <c r="AJ90" s="43" t="s">
         <v>109</v>
       </c>
       <c r="AK90" s="3" t="s">
@@ -16012,7 +16022,7 @@
       <c r="AL90" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="AM90" s="44" t="s">
+      <c r="AM90" s="42" t="s">
         <v>396</v>
       </c>
       <c r="AN90" s="3">
@@ -16047,7 +16057,7 @@
         <f t="shared" ref="AW90" si="104">AO90-AS90</f>
         <v>80</v>
       </c>
-      <c r="AX90" s="45">
+      <c r="AX90" s="43">
         <f t="shared" ref="AX90" si="105">AP90-AT90</f>
         <v>80</v>
       </c>
@@ -16057,14 +16067,14 @@
       <c r="AZ90" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="BA90" s="3" t="s">
-        <v>121</v>
+      <c r="BA90" s="3">
+        <v>1</v>
       </c>
       <c r="BB90" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="BC90" s="3" t="s">
-        <v>121</v>
+        <v>291</v>
+      </c>
+      <c r="BC90" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="91" spans="1:55" x14ac:dyDescent="0.25">
@@ -16146,34 +16156,34 @@
       <c r="AJ91" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK91" s="40" t="s">
+      <c r="AK91" t="s">
         <v>396</v>
       </c>
-      <c r="AL91" s="40" t="s">
+      <c r="AL91" t="s">
         <v>396</v>
       </c>
-      <c r="AM91" s="41" t="s">
+      <c r="AM91" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="AN91" s="40">
+      <c r="AN91">
         <v>80</v>
       </c>
-      <c r="AO91" s="40">
+      <c r="AO91">
         <v>240</v>
       </c>
-      <c r="AP91" s="40">
+      <c r="AP91">
         <v>240</v>
       </c>
       <c r="AQ91" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AR91" s="40">
+      <c r="AR91">
         <v>64</v>
       </c>
-      <c r="AS91" s="40">
+      <c r="AS91">
         <v>144</v>
       </c>
-      <c r="AT91" s="40">
+      <c r="AT91">
         <v>144</v>
       </c>
       <c r="AU91" s="25" t="s">
@@ -16197,14 +16207,14 @@
       <c r="AZ91" t="s">
         <v>294</v>
       </c>
-      <c r="BA91" t="s">
-        <v>121</v>
+      <c r="BA91">
+        <v>1</v>
       </c>
       <c r="BB91" t="s">
-        <v>121</v>
+        <v>404</v>
       </c>
       <c r="BC91" t="s">
-        <v>121</v>
+        <v>292</v>
       </c>
     </row>
     <row r="92" spans="1:55" x14ac:dyDescent="0.25">
@@ -16286,34 +16296,34 @@
       <c r="AJ92" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK92" s="40" t="s">
+      <c r="AK92" t="s">
         <v>396</v>
       </c>
-      <c r="AL92" s="40" t="s">
+      <c r="AL92" t="s">
         <v>396</v>
       </c>
-      <c r="AM92" s="41" t="s">
+      <c r="AM92" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="AN92" s="40">
+      <c r="AN92">
         <v>80</v>
       </c>
-      <c r="AO92" s="40">
+      <c r="AO92">
         <v>240</v>
       </c>
-      <c r="AP92" s="40">
+      <c r="AP92">
         <v>240</v>
       </c>
       <c r="AQ92" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AR92" s="40">
+      <c r="AR92">
         <v>48</v>
       </c>
-      <c r="AS92" s="40">
+      <c r="AS92">
         <v>208</v>
       </c>
-      <c r="AT92" s="40">
+      <c r="AT92">
         <v>208</v>
       </c>
       <c r="AU92" s="25" t="s">
@@ -16337,14 +16347,14 @@
       <c r="AZ92" t="s">
         <v>380</v>
       </c>
-      <c r="BA92" t="s">
-        <v>121</v>
+      <c r="BA92">
+        <v>1</v>
       </c>
       <c r="BB92" t="s">
-        <v>121</v>
+        <v>404</v>
       </c>
       <c r="BC92" t="s">
-        <v>121</v>
+        <v>292</v>
       </c>
     </row>
     <row r="93" spans="1:55" x14ac:dyDescent="0.25">
@@ -16426,34 +16436,34 @@
       <c r="AJ93" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AK93" s="40" t="s">
+      <c r="AK93" t="s">
         <v>396</v>
       </c>
-      <c r="AL93" s="40" t="s">
+      <c r="AL93" t="s">
         <v>396</v>
       </c>
-      <c r="AM93" s="41" t="s">
+      <c r="AM93" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="AN93" s="40">
+      <c r="AN93">
         <v>64</v>
       </c>
-      <c r="AO93" s="40">
+      <c r="AO93">
         <v>128</v>
       </c>
-      <c r="AP93" s="40">
+      <c r="AP93">
         <v>128</v>
       </c>
       <c r="AQ93" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AR93" s="40">
+      <c r="AR93">
         <v>32</v>
       </c>
-      <c r="AS93" s="40">
+      <c r="AS93">
         <v>96</v>
       </c>
-      <c r="AT93" s="40">
+      <c r="AT93">
         <v>96</v>
       </c>
       <c r="AU93" s="25" t="s">
@@ -16477,14 +16487,14 @@
       <c r="AZ93" t="s">
         <v>384</v>
       </c>
-      <c r="BA93" t="s">
-        <v>121</v>
+      <c r="BA93">
+        <v>1</v>
       </c>
       <c r="BB93" t="s">
-        <v>121</v>
+        <v>405</v>
       </c>
       <c r="BC93" t="s">
-        <v>121</v>
+        <v>292</v>
       </c>
     </row>
     <row r="94" spans="1:55" x14ac:dyDescent="0.25">
@@ -16630,15 +16640,15 @@
         <v>8</v>
       </c>
       <c r="AV94" t="e">
-        <f t="shared" ref="AV87:AV94" si="115">AN94-AR94</f>
+        <f t="shared" ref="AV94" si="115">AN94-AR94</f>
         <v>#VALUE!</v>
       </c>
       <c r="AW94" t="e">
-        <f t="shared" ref="AW87:AW94" si="116">AO94-AS94</f>
+        <f t="shared" ref="AW94" si="116">AO94-AS94</f>
         <v>#VALUE!</v>
       </c>
       <c r="AX94" s="10" t="e">
-        <f t="shared" ref="AX87:AX94" si="117">AP94-AT94</f>
+        <f t="shared" ref="AX94" si="117">AP94-AT94</f>
         <v>#VALUE!</v>
       </c>
       <c r="AY94" t="s">

</xml_diff>

<commit_message>
add some stuff regarding github 3dunet issue (email to wolny)
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57118E0C-5EEB-4655-B269-6C17127E9581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5547CEC-E38A-478D-B56F-B99C3E1D65CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BC94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BC93" sqref="BC93"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AZ38" sqref="AZ38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
prepare predict3dunet 231220-0 to 231220-5
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08378E0C-336C-44A3-8B8F-06F1F5045260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAC2484-5F4B-4174-ADD1-C7A46997B13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2888" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2960" uniqueCount="424">
   <si>
     <t>patch z</t>
   </si>
@@ -1260,9 +1260,6 @@
     <t>231220-1</t>
   </si>
   <si>
-    <t>231220-2</t>
-  </si>
-  <si>
     <t>231220-3</t>
   </si>
   <si>
@@ -1288,6 +1285,30 @@
   </si>
   <si>
     <t>type of session / command executed &amp; its pytorch-3dunet version tag</t>
+  </si>
+  <si>
+    <t>231220-4</t>
+  </si>
+  <si>
+    <t>231220-5</t>
+  </si>
+  <si>
+    <t>patch = arbitrary prime numbers</t>
+  </si>
+  <si>
+    <t>stride = arbitrary prime numbers</t>
+  </si>
+  <si>
+    <t>patch = some number = sum(2^i), with i&gt;=4</t>
+  </si>
+  <si>
+    <t>stride = some number = sum(2^i), with i&gt;=4</t>
+  </si>
+  <si>
+    <t>patch = some number = sum(2^i), with i&gt;=4, the same is in above ResidualUNet3D attempt.</t>
+  </si>
+  <si>
+    <t>stride = some number = sum(2^i), with i&gt;=4, the same is in above ResidualUNet3D attempt.</t>
   </si>
 </sst>
 </file>
@@ -1894,10 +1915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BE98"/>
+  <dimension ref="A1:BE100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="AJ73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AS95" sqref="AS95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1960,13 +1981,13 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>55</v>
@@ -2136,10 +2157,10 @@
         <v>404</v>
       </c>
       <c r="C2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E2" t="s">
         <v>127</v>
@@ -2304,10 +2325,10 @@
         <v>404</v>
       </c>
       <c r="C3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E3" t="s">
         <v>127</v>
@@ -2473,10 +2494,10 @@
         <v>404</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>121</v>
@@ -2641,10 +2662,10 @@
         <v>404</v>
       </c>
       <c r="C5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E5" t="s">
         <v>122</v>
@@ -2806,10 +2827,10 @@
         <v>404</v>
       </c>
       <c r="C6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E6" t="s">
         <v>84</v>
@@ -2971,10 +2992,10 @@
         <v>404</v>
       </c>
       <c r="C7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E7" t="s">
         <v>85</v>
@@ -3136,10 +3157,10 @@
         <v>404</v>
       </c>
       <c r="C8" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E8" t="s">
         <v>88</v>
@@ -3301,10 +3322,10 @@
         <v>404</v>
       </c>
       <c r="C9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E9" t="s">
         <v>122</v>
@@ -3472,10 +3493,10 @@
         <v>404</v>
       </c>
       <c r="C10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E10" t="s">
         <v>90</v>
@@ -3637,10 +3658,10 @@
         <v>404</v>
       </c>
       <c r="C11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D11" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E11" t="s">
         <v>95</v>
@@ -3802,10 +3823,10 @@
         <v>404</v>
       </c>
       <c r="C12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E12" t="s">
         <v>96</v>
@@ -3968,10 +3989,10 @@
         <v>404</v>
       </c>
       <c r="C13" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>
@@ -4133,10 +4154,10 @@
         <v>404</v>
       </c>
       <c r="C14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E14" t="s">
         <v>40</v>
@@ -4298,10 +4319,10 @@
         <v>404</v>
       </c>
       <c r="C15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E15" t="s">
         <v>41</v>
@@ -4464,10 +4485,10 @@
         <v>404</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>42</v>
@@ -4631,10 +4652,10 @@
         <v>404</v>
       </c>
       <c r="C17" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E17" t="s">
         <v>60</v>
@@ -4797,10 +4818,10 @@
         <v>404</v>
       </c>
       <c r="C18" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E18" t="s">
         <v>60</v>
@@ -4963,10 +4984,10 @@
         <v>404</v>
       </c>
       <c r="C19" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E19" t="s">
         <v>61</v>
@@ -5129,10 +5150,10 @@
         <v>404</v>
       </c>
       <c r="C20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E20" t="s">
         <v>61</v>
@@ -5295,10 +5316,10 @@
         <v>404</v>
       </c>
       <c r="C21" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E21" t="s">
         <v>62</v>
@@ -5461,10 +5482,10 @@
         <v>404</v>
       </c>
       <c r="C22" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D22" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E22" t="s">
         <v>62</v>
@@ -5627,10 +5648,10 @@
         <v>404</v>
       </c>
       <c r="C23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E23" t="s">
         <v>63</v>
@@ -5793,10 +5814,10 @@
         <v>404</v>
       </c>
       <c r="C24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D24" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E24" t="s">
         <v>63</v>
@@ -6293,10 +6314,10 @@
         <v>404</v>
       </c>
       <c r="C27" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D27" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E27" t="s">
         <v>123</v>
@@ -6463,10 +6484,10 @@
         <v>404</v>
       </c>
       <c r="C28" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E28" t="s">
         <v>145</v>
@@ -6632,10 +6653,10 @@
         <v>404</v>
       </c>
       <c r="C29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E29" t="s">
         <v>124</v>
@@ -6802,10 +6823,10 @@
         <v>404</v>
       </c>
       <c r="C30" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D30" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E30" t="s">
         <v>153</v>
@@ -6972,10 +6993,10 @@
         <v>404</v>
       </c>
       <c r="C31" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D31" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E31" t="s">
         <v>146</v>
@@ -7142,10 +7163,10 @@
         <v>404</v>
       </c>
       <c r="C32" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D32" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E32" t="s">
         <v>156</v>
@@ -7311,10 +7332,10 @@
         <v>404</v>
       </c>
       <c r="C33" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D33" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E33" t="s">
         <v>170</v>
@@ -7480,10 +7501,10 @@
         <v>404</v>
       </c>
       <c r="C34" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D34" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E34" t="s">
         <v>166</v>
@@ -7649,10 +7670,10 @@
         <v>404</v>
       </c>
       <c r="C35" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D35" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E35" t="s">
         <v>179</v>
@@ -7818,10 +7839,10 @@
         <v>404</v>
       </c>
       <c r="C36" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D36" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E36" t="s">
         <v>181</v>
@@ -7987,10 +8008,10 @@
         <v>404</v>
       </c>
       <c r="C37" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D37" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E37" t="s">
         <v>187</v>
@@ -8156,10 +8177,10 @@
         <v>404</v>
       </c>
       <c r="C38" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D38" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E38" t="s">
         <v>192</v>
@@ -8325,10 +8346,10 @@
         <v>404</v>
       </c>
       <c r="C39" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D39" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E39" t="s">
         <v>195</v>
@@ -8494,10 +8515,10 @@
         <v>404</v>
       </c>
       <c r="C40" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D40" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E40" t="s">
         <v>195</v>
@@ -8663,10 +8684,10 @@
         <v>404</v>
       </c>
       <c r="C41" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D41" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E41" t="s">
         <v>195</v>
@@ -8832,10 +8853,10 @@
         <v>404</v>
       </c>
       <c r="C42" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D42" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E42" t="s">
         <v>195</v>
@@ -9001,10 +9022,10 @@
         <v>404</v>
       </c>
       <c r="C43" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D43" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E43" t="s">
         <v>195</v>
@@ -9170,10 +9191,10 @@
         <v>404</v>
       </c>
       <c r="C44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E44" t="s">
         <v>195</v>
@@ -9340,10 +9361,10 @@
         <v>404</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>207</v>
@@ -9511,10 +9532,10 @@
         <v>404</v>
       </c>
       <c r="C46" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D46" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E46" s="12" t="s">
         <v>212</v>
@@ -9675,10 +9696,10 @@
         <v>404</v>
       </c>
       <c r="C47" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D47" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E47" s="12" t="s">
         <v>213</v>
@@ -9839,10 +9860,10 @@
         <v>404</v>
       </c>
       <c r="C48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D48" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>214</v>
@@ -10003,10 +10024,10 @@
         <v>404</v>
       </c>
       <c r="C49" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D49" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>215</v>
@@ -10167,10 +10188,10 @@
         <v>404</v>
       </c>
       <c r="C50" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D50" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>216</v>
@@ -10331,10 +10352,10 @@
         <v>404</v>
       </c>
       <c r="C51" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D51" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E51" s="12" t="s">
         <v>217</v>
@@ -10495,10 +10516,10 @@
         <v>404</v>
       </c>
       <c r="C52" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D52" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E52" s="12" t="s">
         <v>218</v>
@@ -10659,10 +10680,10 @@
         <v>404</v>
       </c>
       <c r="C53" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D53" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E53" s="12" t="s">
         <v>219</v>
@@ -10823,10 +10844,10 @@
         <v>404</v>
       </c>
       <c r="C54" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D54" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>220</v>
@@ -10987,10 +11008,10 @@
         <v>404</v>
       </c>
       <c r="C55" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D55" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E55" s="12" t="s">
         <v>221</v>
@@ -11151,10 +11172,10 @@
         <v>404</v>
       </c>
       <c r="C56" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D56" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>222</v>
@@ -11315,10 +11336,10 @@
         <v>404</v>
       </c>
       <c r="C57" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D57" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E57" s="12" t="s">
         <v>223</v>
@@ -11479,10 +11500,10 @@
         <v>404</v>
       </c>
       <c r="C58" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D58" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>224</v>
@@ -11643,10 +11664,10 @@
         <v>404</v>
       </c>
       <c r="C59" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D59" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E59" s="12" t="s">
         <v>225</v>
@@ -11807,10 +11828,10 @@
         <v>404</v>
       </c>
       <c r="C60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D60" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E60" s="12" t="s">
         <v>226</v>
@@ -11971,10 +11992,10 @@
         <v>404</v>
       </c>
       <c r="C61" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D61" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E61" s="12" t="s">
         <v>227</v>
@@ -12135,10 +12156,10 @@
         <v>404</v>
       </c>
       <c r="C62" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D62" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E62" s="12" t="s">
         <v>228</v>
@@ -12299,10 +12320,10 @@
         <v>404</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E63" s="17" t="s">
         <v>229</v>
@@ -12464,10 +12485,10 @@
         <v>404</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E64" s="31" t="s">
         <v>273</v>
@@ -12633,10 +12654,10 @@
         <v>405</v>
       </c>
       <c r="C65" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D65" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E65" s="12" t="s">
         <v>275</v>
@@ -12809,10 +12830,10 @@
         <v>405</v>
       </c>
       <c r="C66" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D66" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E66" s="12" t="s">
         <v>278</v>
@@ -12985,10 +13006,10 @@
         <v>405</v>
       </c>
       <c r="C67" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D67" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E67" s="12" t="s">
         <v>312</v>
@@ -13161,10 +13182,10 @@
         <v>405</v>
       </c>
       <c r="C68" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D68" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E68" s="12" t="s">
         <v>313</v>
@@ -13337,10 +13358,10 @@
         <v>405</v>
       </c>
       <c r="C69" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D69" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E69" s="12" t="s">
         <v>315</v>
@@ -13513,10 +13534,10 @@
         <v>405</v>
       </c>
       <c r="C70" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D70" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E70" s="12" t="s">
         <v>315</v>
@@ -13692,10 +13713,10 @@
         <v>405</v>
       </c>
       <c r="C71" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D71" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E71" s="12" t="s">
         <v>316</v>
@@ -13868,10 +13889,10 @@
         <v>405</v>
       </c>
       <c r="C72" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D72" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E72" s="12" t="s">
         <v>315</v>
@@ -14044,10 +14065,10 @@
         <v>405</v>
       </c>
       <c r="C73" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D73" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E73" s="12" t="s">
         <v>313</v>
@@ -14223,10 +14244,10 @@
         <v>405</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>313</v>
@@ -14399,10 +14420,10 @@
         <v>405</v>
       </c>
       <c r="C75" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D75" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E75" s="12" t="s">
         <v>335</v>
@@ -14572,10 +14593,10 @@
         <v>405</v>
       </c>
       <c r="C76" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D76" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E76" s="12" t="s">
         <v>346</v>
@@ -14761,10 +14782,10 @@
         <v>404</v>
       </c>
       <c r="C79" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D79" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E79" s="12" t="s">
         <v>355</v>
@@ -14934,10 +14955,10 @@
         <v>404</v>
       </c>
       <c r="C80" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D80" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E80" s="12" t="s">
         <v>365</v>
@@ -15110,10 +15131,10 @@
         <v>404</v>
       </c>
       <c r="C81" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D81" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E81" s="12" t="s">
         <v>369</v>
@@ -15286,10 +15307,10 @@
         <v>405</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E82" s="38" t="s">
         <v>388</v>
@@ -15399,7 +15420,7 @@
       <c r="AN82" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="AO82" s="3" t="s">
+      <c r="AO82" s="41" t="s">
         <v>402</v>
       </c>
       <c r="AP82" s="3">
@@ -15462,10 +15483,10 @@
         <v>405</v>
       </c>
       <c r="C83" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D83" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E83" s="12" t="s">
         <v>388</v>
@@ -15575,7 +15596,7 @@
       <c r="AN83" t="s">
         <v>402</v>
       </c>
-      <c r="AO83" t="s">
+      <c r="AO83" s="20" t="s">
         <v>402</v>
       </c>
       <c r="AP83">
@@ -15638,10 +15659,10 @@
         <v>405</v>
       </c>
       <c r="C84" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D84" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E84" s="12" t="s">
         <v>388</v>
@@ -15751,7 +15772,7 @@
       <c r="AN84" t="s">
         <v>402</v>
       </c>
-      <c r="AO84" t="s">
+      <c r="AO84" s="20" t="s">
         <v>402</v>
       </c>
       <c r="AP84">
@@ -15814,10 +15835,10 @@
         <v>405</v>
       </c>
       <c r="C85" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D85" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E85" s="12" t="s">
         <v>388</v>
@@ -15927,7 +15948,7 @@
       <c r="AN85" t="s">
         <v>402</v>
       </c>
-      <c r="AO85" t="s">
+      <c r="AO85" s="20" t="s">
         <v>402</v>
       </c>
       <c r="AP85">
@@ -15990,10 +16011,10 @@
         <v>398</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E86" s="38" t="s">
         <v>389</v>
@@ -16103,7 +16124,7 @@
       <c r="AN86" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="AO86" s="3" t="s">
+      <c r="AO86" s="41" t="s">
         <v>402</v>
       </c>
       <c r="AP86" s="3">
@@ -16166,10 +16187,10 @@
         <v>398</v>
       </c>
       <c r="C87" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D87" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E87" s="12" t="s">
         <v>389</v>
@@ -16279,7 +16300,7 @@
       <c r="AN87" t="s">
         <v>402</v>
       </c>
-      <c r="AO87" t="s">
+      <c r="AO87" s="20" t="s">
         <v>402</v>
       </c>
       <c r="AP87">
@@ -16342,10 +16363,10 @@
         <v>398</v>
       </c>
       <c r="C88" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D88" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E88" s="12" t="s">
         <v>389</v>
@@ -16455,7 +16476,7 @@
       <c r="AN88" t="s">
         <v>402</v>
       </c>
-      <c r="AO88" t="s">
+      <c r="AO88" s="20" t="s">
         <v>402</v>
       </c>
       <c r="AP88">
@@ -16518,10 +16539,10 @@
         <v>398</v>
       </c>
       <c r="C89" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D89" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E89" s="12" t="s">
         <v>389</v>
@@ -16631,7 +16652,7 @@
       <c r="AN89" t="s">
         <v>402</v>
       </c>
-      <c r="AO89" t="s">
+      <c r="AO89" s="20" t="s">
         <v>402</v>
       </c>
       <c r="AP89">
@@ -16694,10 +16715,10 @@
         <v>405</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E90" s="38" t="s">
         <v>390</v>
@@ -16807,7 +16828,7 @@
       <c r="AN90" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="AO90" s="3" t="s">
+      <c r="AO90" s="41" t="s">
         <v>402</v>
       </c>
       <c r="AP90" s="3">
@@ -16870,10 +16891,10 @@
         <v>405</v>
       </c>
       <c r="C91" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D91" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E91" s="12" t="s">
         <v>390</v>
@@ -16983,7 +17004,7 @@
       <c r="AN91" t="s">
         <v>402</v>
       </c>
-      <c r="AO91" t="s">
+      <c r="AO91" s="20" t="s">
         <v>402</v>
       </c>
       <c r="AP91">
@@ -17046,10 +17067,10 @@
         <v>405</v>
       </c>
       <c r="C92" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D92" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E92" s="12" t="s">
         <v>390</v>
@@ -17159,7 +17180,7 @@
       <c r="AN92" t="s">
         <v>402</v>
       </c>
-      <c r="AO92" t="s">
+      <c r="AO92" s="20" t="s">
         <v>402</v>
       </c>
       <c r="AP92">
@@ -17222,10 +17243,10 @@
         <v>405</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E93" s="17" t="s">
         <v>390</v>
@@ -17335,7 +17356,7 @@
       <c r="AN93" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="AO93" s="4" t="s">
+      <c r="AO93" s="22" t="s">
         <v>402</v>
       </c>
       <c r="AP93" s="4">
@@ -17398,13 +17419,13 @@
         <v>405</v>
       </c>
       <c r="C94" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D94" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E94" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F94" s="12" t="s">
         <v>396</v>
@@ -17455,106 +17476,106 @@
         <v>344</v>
       </c>
       <c r="V94" t="s">
-        <v>120</v>
+        <v>343</v>
       </c>
       <c r="W94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="X94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="Y94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="Z94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AA94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AB94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AC94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AD94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AE94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AF94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AG94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AH94" s="6" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AI94" s="12" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AJ94" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AK94" t="s">
-        <v>281</v>
+        <v>401</v>
       </c>
       <c r="AL94" s="10" t="s">
         <v>108</v>
       </c>
       <c r="AM94" t="s">
-        <v>120</v>
+        <v>402</v>
       </c>
       <c r="AN94" t="s">
-        <v>120</v>
+        <v>402</v>
       </c>
       <c r="AO94" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP94" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ94" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR94" t="s">
-        <v>120</v>
+        <v>402</v>
+      </c>
+      <c r="AP94">
+        <v>96</v>
+      </c>
+      <c r="AQ94">
+        <v>112</v>
+      </c>
+      <c r="AR94">
+        <v>112</v>
       </c>
       <c r="AS94" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT94" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU94" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV94" t="s">
-        <v>120</v>
+      <c r="AT94">
+        <v>64</v>
+      </c>
+      <c r="AU94">
+        <v>96</v>
+      </c>
+      <c r="AV94">
+        <v>96</v>
       </c>
       <c r="AW94" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX94" t="e">
+      <c r="AX94">
         <f t="shared" ref="AX94" si="115">AP94-AT94</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY94" t="e">
+        <v>32</v>
+      </c>
+      <c r="AY94">
         <f t="shared" ref="AY94" si="116">AQ94-AU94</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ94" s="10" t="e">
+        <v>16</v>
+      </c>
+      <c r="AZ94" s="10">
         <f t="shared" ref="AZ94" si="117">AR94-AV94</f>
-        <v>#VALUE!</v>
+        <v>16</v>
       </c>
       <c r="BA94" t="s">
-        <v>120</v>
+        <v>420</v>
       </c>
       <c r="BB94" t="s">
-        <v>120</v>
+        <v>421</v>
       </c>
       <c r="BC94" t="s">
         <v>120</v>
@@ -17574,13 +17595,13 @@
         <v>405</v>
       </c>
       <c r="C95" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D95" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E95" s="12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>396</v>
@@ -17631,106 +17652,106 @@
         <v>344</v>
       </c>
       <c r="V95" t="s">
-        <v>120</v>
+        <v>343</v>
       </c>
       <c r="W95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="X95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="Y95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="Z95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AA95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AB95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AC95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AD95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AE95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AF95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AG95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AH95" s="6" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AI95" s="12" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AJ95" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AK95" t="s">
-        <v>281</v>
+        <v>401</v>
       </c>
       <c r="AL95" s="10" t="s">
         <v>108</v>
       </c>
       <c r="AM95" t="s">
-        <v>120</v>
+        <v>402</v>
       </c>
       <c r="AN95" t="s">
-        <v>120</v>
+        <v>402</v>
       </c>
       <c r="AO95" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP95" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ95" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR95" t="s">
-        <v>120</v>
+        <v>402</v>
+      </c>
+      <c r="AP95">
+        <v>96</v>
+      </c>
+      <c r="AQ95">
+        <v>112</v>
+      </c>
+      <c r="AR95">
+        <v>112</v>
       </c>
       <c r="AS95" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT95" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU95" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV95" t="s">
-        <v>120</v>
+      <c r="AT95">
+        <v>64</v>
+      </c>
+      <c r="AU95">
+        <v>96</v>
+      </c>
+      <c r="AV95">
+        <v>96</v>
       </c>
       <c r="AW95" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX95" t="e">
+      <c r="AX95">
         <f t="shared" ref="AX95" si="118">AP95-AT95</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY95" t="e">
+        <v>32</v>
+      </c>
+      <c r="AY95">
         <f t="shared" ref="AY95" si="119">AQ95-AU95</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ95" s="10" t="e">
+        <v>16</v>
+      </c>
+      <c r="AZ95" s="10">
         <f t="shared" ref="AZ95" si="120">AR95-AV95</f>
-        <v>#VALUE!</v>
+        <v>16</v>
       </c>
       <c r="BA95" t="s">
-        <v>120</v>
+        <v>422</v>
       </c>
       <c r="BB95" t="s">
-        <v>120</v>
+        <v>423</v>
       </c>
       <c r="BC95" t="s">
         <v>120</v>
@@ -17744,7 +17765,7 @@
     </row>
     <row r="96" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B96" t="s">
         <v>405</v>
@@ -17753,7 +17774,7 @@
         <v>411</v>
       </c>
       <c r="D96" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E96" s="12" t="s">
         <v>409</v>
@@ -17804,109 +17825,109 @@
         <v>120</v>
       </c>
       <c r="U96" t="s">
-        <v>403</v>
+        <v>344</v>
       </c>
       <c r="V96" t="s">
-        <v>120</v>
+        <v>343</v>
       </c>
       <c r="W96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="X96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="Y96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="Z96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AA96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AB96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AC96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AD96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AE96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AF96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AG96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AH96" s="6" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AI96" s="12" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AJ96" t="s">
-        <v>120</v>
+        <v>401</v>
       </c>
       <c r="AK96" t="s">
-        <v>281</v>
+        <v>401</v>
       </c>
       <c r="AL96" s="10" t="s">
         <v>108</v>
       </c>
       <c r="AM96" t="s">
-        <v>120</v>
+        <v>402</v>
       </c>
       <c r="AN96" t="s">
-        <v>120</v>
+        <v>402</v>
       </c>
       <c r="AO96" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP96" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ96" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR96" t="s">
-        <v>120</v>
+        <v>402</v>
+      </c>
+      <c r="AP96">
+        <v>71</v>
+      </c>
+      <c r="AQ96">
+        <v>131</v>
+      </c>
+      <c r="AR96">
+        <v>131</v>
       </c>
       <c r="AS96" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT96" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU96" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV96" t="s">
-        <v>120</v>
+      <c r="AT96">
+        <v>47</v>
+      </c>
+      <c r="AU96">
+        <v>83</v>
+      </c>
+      <c r="AV96">
+        <v>83</v>
       </c>
       <c r="AW96" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX96" t="e">
+      <c r="AX96">
         <f t="shared" ref="AX96" si="121">AP96-AT96</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY96" t="e">
+        <v>24</v>
+      </c>
+      <c r="AY96">
         <f t="shared" ref="AY96" si="122">AQ96-AU96</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ96" s="10" t="e">
+        <v>48</v>
+      </c>
+      <c r="AZ96" s="10">
         <f t="shared" ref="AZ96" si="123">AR96-AV96</f>
-        <v>#VALUE!</v>
+        <v>48</v>
       </c>
       <c r="BA96" t="s">
-        <v>120</v>
+        <v>418</v>
       </c>
       <c r="BB96" t="s">
-        <v>120</v>
+        <v>419</v>
       </c>
       <c r="BC96" t="s">
         <v>120</v>
@@ -17920,19 +17941,19 @@
     </row>
     <row r="97" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B97" t="s">
         <v>405</v>
       </c>
       <c r="C97" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D97" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>396</v>
@@ -18042,47 +18063,47 @@
       <c r="AO97" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="AP97" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ97" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR97" t="s">
-        <v>120</v>
+      <c r="AP97">
+        <v>96</v>
+      </c>
+      <c r="AQ97">
+        <v>112</v>
+      </c>
+      <c r="AR97">
+        <v>112</v>
       </c>
       <c r="AS97" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT97" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU97" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV97" t="s">
-        <v>120</v>
+      <c r="AT97">
+        <v>64</v>
+      </c>
+      <c r="AU97">
+        <v>96</v>
+      </c>
+      <c r="AV97">
+        <v>96</v>
       </c>
       <c r="AW97" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX97" t="e">
+      <c r="AX97">
         <f t="shared" ref="AX97" si="124">AP97-AT97</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY97" t="e">
+        <v>32</v>
+      </c>
+      <c r="AY97">
         <f t="shared" ref="AY97" si="125">AQ97-AU97</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ97" s="10" t="e">
+        <v>16</v>
+      </c>
+      <c r="AZ97" s="10">
         <f t="shared" ref="AZ97" si="126">AR97-AV97</f>
-        <v>#VALUE!</v>
+        <v>16</v>
       </c>
       <c r="BA97" t="s">
-        <v>120</v>
+        <v>420</v>
       </c>
       <c r="BB97" t="s">
-        <v>120</v>
+        <v>421</v>
       </c>
       <c r="BC97" t="s">
         <v>120</v>
@@ -18096,25 +18117,25 @@
     </row>
     <row r="98" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
-        <v>120</v>
+        <v>416</v>
       </c>
       <c r="B98" t="s">
-        <v>120</v>
+        <v>405</v>
       </c>
       <c r="C98" t="s">
-        <v>120</v>
+        <v>411</v>
       </c>
       <c r="D98" t="s">
-        <v>120</v>
+        <v>413</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>120</v>
+        <v>409</v>
       </c>
       <c r="F98" s="12" t="s">
-        <v>120</v>
+        <v>396</v>
       </c>
       <c r="G98" s="12" t="s">
-        <v>120</v>
+        <v>397</v>
       </c>
       <c r="H98" s="6" t="s">
         <v>120</v>
@@ -18156,7 +18177,7 @@
         <v>120</v>
       </c>
       <c r="U98" t="s">
-        <v>120</v>
+        <v>403</v>
       </c>
       <c r="V98" t="s">
         <v>120</v>
@@ -18218,55 +18239,407 @@
       <c r="AO98" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="AP98" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ98" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR98" t="s">
-        <v>120</v>
+      <c r="AP98">
+        <v>96</v>
+      </c>
+      <c r="AQ98">
+        <v>112</v>
+      </c>
+      <c r="AR98">
+        <v>112</v>
       </c>
       <c r="AS98" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT98" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU98" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV98" t="s">
-        <v>120</v>
+      <c r="AT98">
+        <v>64</v>
+      </c>
+      <c r="AU98">
+        <v>96</v>
+      </c>
+      <c r="AV98">
+        <v>96</v>
       </c>
       <c r="AW98" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX98" t="e">
+      <c r="AX98">
         <f t="shared" ref="AX98" si="127">AP98-AT98</f>
+        <v>32</v>
+      </c>
+      <c r="AY98">
+        <f t="shared" ref="AY98" si="128">AQ98-AU98</f>
+        <v>16</v>
+      </c>
+      <c r="AZ98" s="10">
+        <f t="shared" ref="AZ98" si="129">AR98-AV98</f>
+        <v>16</v>
+      </c>
+      <c r="BA98" t="s">
+        <v>422</v>
+      </c>
+      <c r="BB98" t="s">
+        <v>423</v>
+      </c>
+      <c r="BC98" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD98" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE98" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A99" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="B99" t="s">
+        <v>405</v>
+      </c>
+      <c r="C99" t="s">
+        <v>411</v>
+      </c>
+      <c r="D99" t="s">
+        <v>413</v>
+      </c>
+      <c r="E99" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="H99" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I99" t="s">
+        <v>120</v>
+      </c>
+      <c r="J99" t="s">
+        <v>120</v>
+      </c>
+      <c r="K99" t="s">
+        <v>120</v>
+      </c>
+      <c r="L99" t="s">
+        <v>120</v>
+      </c>
+      <c r="M99" t="s">
+        <v>120</v>
+      </c>
+      <c r="N99" t="s">
+        <v>120</v>
+      </c>
+      <c r="O99" t="s">
+        <v>120</v>
+      </c>
+      <c r="P99" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>120</v>
+      </c>
+      <c r="R99" t="s">
+        <v>120</v>
+      </c>
+      <c r="S99" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T99" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U99" t="s">
+        <v>403</v>
+      </c>
+      <c r="V99" t="s">
+        <v>120</v>
+      </c>
+      <c r="W99" t="s">
+        <v>120</v>
+      </c>
+      <c r="X99" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y99" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH99" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI99" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK99" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL99" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN99" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO99" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP99">
+        <v>71</v>
+      </c>
+      <c r="AQ99">
+        <v>131</v>
+      </c>
+      <c r="AR99">
+        <v>131</v>
+      </c>
+      <c r="AS99" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT99">
+        <v>47</v>
+      </c>
+      <c r="AU99">
+        <v>83</v>
+      </c>
+      <c r="AV99">
+        <v>83</v>
+      </c>
+      <c r="AW99" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX99">
+        <f t="shared" ref="AX99" si="130">AP99-AT99</f>
+        <v>24</v>
+      </c>
+      <c r="AY99">
+        <f t="shared" ref="AY99" si="131">AQ99-AU99</f>
+        <v>48</v>
+      </c>
+      <c r="AZ99" s="10">
+        <f t="shared" ref="AZ99" si="132">AR99-AV99</f>
+        <v>48</v>
+      </c>
+      <c r="BA99" t="s">
+        <v>418</v>
+      </c>
+      <c r="BB99" t="s">
+        <v>419</v>
+      </c>
+      <c r="BC99" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD99" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE99" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="100" spans="1:57" x14ac:dyDescent="0.25">
+      <c r="A100" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B100" t="s">
+        <v>120</v>
+      </c>
+      <c r="C100" t="s">
+        <v>120</v>
+      </c>
+      <c r="D100" t="s">
+        <v>120</v>
+      </c>
+      <c r="E100" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H100" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I100" t="s">
+        <v>120</v>
+      </c>
+      <c r="J100" t="s">
+        <v>120</v>
+      </c>
+      <c r="K100" t="s">
+        <v>120</v>
+      </c>
+      <c r="L100" t="s">
+        <v>120</v>
+      </c>
+      <c r="M100" t="s">
+        <v>120</v>
+      </c>
+      <c r="N100" t="s">
+        <v>120</v>
+      </c>
+      <c r="O100" t="s">
+        <v>120</v>
+      </c>
+      <c r="P100" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>120</v>
+      </c>
+      <c r="R100" t="s">
+        <v>120</v>
+      </c>
+      <c r="S100" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T100" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U100" t="s">
+        <v>120</v>
+      </c>
+      <c r="V100" t="s">
+        <v>120</v>
+      </c>
+      <c r="W100" t="s">
+        <v>120</v>
+      </c>
+      <c r="X100" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y100" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH100" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI100" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK100" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL100" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO100" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS100" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV100" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW100" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX100" t="e">
+        <f t="shared" ref="AX100" si="133">AP100-AT100</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AY98" t="e">
-        <f t="shared" ref="AY98" si="128">AQ98-AU98</f>
+      <c r="AY100" t="e">
+        <f t="shared" ref="AY100" si="134">AQ100-AU100</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ98" s="10" t="e">
-        <f t="shared" ref="AZ98" si="129">AR98-AV98</f>
+      <c r="AZ100" s="10" t="e">
+        <f t="shared" ref="AZ100" si="135">AR100-AV100</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA98" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB98" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC98" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD98" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE98" t="s">
+      <c r="BA100" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB100" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC100" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD100" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE100" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare train3dunet 1.6.0 231223-0 to 231223-5
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBC8E92-182B-4D4E-A686-2D39221049B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3568A18-E5ED-4CA9-BA66-0FF59C07AB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3274" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3482" uniqueCount="452">
   <si>
     <t>patch z</t>
   </si>
@@ -1308,24 +1308,6 @@
     <t>stride = some number = sum(2^i), with i&gt;=4, the same is in above ResidualUNet3D attempt.</t>
   </si>
   <si>
-    <t>231220-6</t>
-  </si>
-  <si>
-    <t>231220-7</t>
-  </si>
-  <si>
-    <t>231220-8</t>
-  </si>
-  <si>
-    <t>231220-9</t>
-  </si>
-  <si>
-    <t>231220-10</t>
-  </si>
-  <si>
-    <t>231220-11</t>
-  </si>
-  <si>
     <t>Try out patch shape fix for "ResidualUNet3D" type pytorch-3dunet model, suggested by Adrian Wolny. See MSc/README-protocol.md for details. Use my own data set.</t>
   </si>
   <si>
@@ -1353,7 +1335,64 @@
     <t>Failure, invalid patch shape error. I assume, the patch shape used during training was invalid, negating the now valid patch shape used for prediction.</t>
   </si>
   <si>
-    <t>Wolny's patch shape fix: Train a model on sample data.</t>
+    <t>231223-0</t>
+  </si>
+  <si>
+    <t>3DUnet_confocal_boundary</t>
+  </si>
+  <si>
+    <t>231224-0</t>
+  </si>
+  <si>
+    <t>231224-1</t>
+  </si>
+  <si>
+    <t>231224-2</t>
+  </si>
+  <si>
+    <t>231224-3</t>
+  </si>
+  <si>
+    <t>231224-4</t>
+  </si>
+  <si>
+    <t>231224-5</t>
+  </si>
+  <si>
+    <t>231223-1</t>
+  </si>
+  <si>
+    <t>231223-2</t>
+  </si>
+  <si>
+    <t>231223-3</t>
+  </si>
+  <si>
+    <t>231223-4</t>
+  </si>
+  <si>
+    <t>231223-5</t>
+  </si>
+  <si>
+    <t>Wolny's patch shape fix: Train a ResidualUNet3D model on sample data. Use new info on valid patch shapes.</t>
+  </si>
+  <si>
+    <t>Wolny's patch shape fix: Train a UNet3D model on sample data.</t>
+  </si>
+  <si>
+    <t>Wolny's patch shape fix: Train a ResidualUNet3D model on my own data. Use new info on valid patch shapes.</t>
+  </si>
+  <si>
+    <t>Wolny's patch shape fix: Train a UNet3D model on sample data, using a config.yml intended for ResidualUNet3D. Does it still work?</t>
+  </si>
+  <si>
+    <t>Wolny's patch shape fix: Train a UNet3D model on my own data, using a config.yml intended for ResidualUNet3D. Does it still work?</t>
+  </si>
+  <si>
+    <t>Wolny's patch shape fix: Train a UNet3D model on my own data.</t>
+  </si>
+  <si>
+    <t>See corr. predict3dunet session for results.</t>
   </si>
 </sst>
 </file>
@@ -1404,7 +1443,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1591,11 +1630,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1656,7 +1704,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1971,10 +2034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BE106"/>
+  <dimension ref="A1:BE112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="AK84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT103" sqref="AT103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -15568,22 +15631,22 @@
       <c r="L83" t="s">
         <v>8</v>
       </c>
-      <c r="M83" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="N83" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="O83" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="P83" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q83" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="R83" s="44" t="s">
+      <c r="M83" t="s">
+        <v>8</v>
+      </c>
+      <c r="N83" t="s">
+        <v>8</v>
+      </c>
+      <c r="O83" t="s">
+        <v>8</v>
+      </c>
+      <c r="P83" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>8</v>
+      </c>
+      <c r="R83" t="s">
         <v>8</v>
       </c>
       <c r="S83" s="12" t="s">
@@ -15744,22 +15807,22 @@
       <c r="L84" t="s">
         <v>8</v>
       </c>
-      <c r="M84" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="N84" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="O84" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="P84" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q84" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="R84" s="44" t="s">
+      <c r="M84" t="s">
+        <v>8</v>
+      </c>
+      <c r="N84" t="s">
+        <v>8</v>
+      </c>
+      <c r="O84" t="s">
+        <v>8</v>
+      </c>
+      <c r="P84" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>8</v>
+      </c>
+      <c r="R84" t="s">
         <v>8</v>
       </c>
       <c r="S84" s="12" t="s">
@@ -15920,22 +15983,22 @@
       <c r="L85" t="s">
         <v>8</v>
       </c>
-      <c r="M85" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="N85" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="O85" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="P85" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q85" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="R85" s="44" t="s">
+      <c r="M85" t="s">
+        <v>8</v>
+      </c>
+      <c r="N85" t="s">
+        <v>8</v>
+      </c>
+      <c r="O85" t="s">
+        <v>8</v>
+      </c>
+      <c r="P85" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>8</v>
+      </c>
+      <c r="R85" t="s">
         <v>8</v>
       </c>
       <c r="S85" s="12" t="s">
@@ -16272,22 +16335,22 @@
       <c r="L87" t="s">
         <v>8</v>
       </c>
-      <c r="M87" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="N87" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="O87" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="P87" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q87" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="R87" s="44" t="s">
+      <c r="M87" t="s">
+        <v>8</v>
+      </c>
+      <c r="N87" t="s">
+        <v>8</v>
+      </c>
+      <c r="O87" t="s">
+        <v>8</v>
+      </c>
+      <c r="P87" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>8</v>
+      </c>
+      <c r="R87" t="s">
         <v>8</v>
       </c>
       <c r="S87" s="12" t="s">
@@ -16448,22 +16511,22 @@
       <c r="L88" t="s">
         <v>8</v>
       </c>
-      <c r="M88" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="N88" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="O88" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="P88" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q88" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="R88" s="44" t="s">
+      <c r="M88" t="s">
+        <v>8</v>
+      </c>
+      <c r="N88" t="s">
+        <v>8</v>
+      </c>
+      <c r="O88" t="s">
+        <v>8</v>
+      </c>
+      <c r="P88" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>8</v>
+      </c>
+      <c r="R88" t="s">
         <v>8</v>
       </c>
       <c r="S88" s="12" t="s">
@@ -16624,22 +16687,22 @@
       <c r="L89" t="s">
         <v>8</v>
       </c>
-      <c r="M89" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="N89" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="O89" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="P89" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q89" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="R89" s="44" t="s">
+      <c r="M89" t="s">
+        <v>8</v>
+      </c>
+      <c r="N89" t="s">
+        <v>8</v>
+      </c>
+      <c r="O89" t="s">
+        <v>8</v>
+      </c>
+      <c r="P89" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>8</v>
+      </c>
+      <c r="R89" t="s">
         <v>8</v>
       </c>
       <c r="S89" s="12" t="s">
@@ -16976,22 +17039,22 @@
       <c r="L91" t="s">
         <v>8</v>
       </c>
-      <c r="M91" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="N91" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="O91" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="P91" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q91" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="R91" s="44" t="s">
+      <c r="M91" t="s">
+        <v>8</v>
+      </c>
+      <c r="N91" t="s">
+        <v>8</v>
+      </c>
+      <c r="O91" t="s">
+        <v>8</v>
+      </c>
+      <c r="P91" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>8</v>
+      </c>
+      <c r="R91" t="s">
         <v>8</v>
       </c>
       <c r="S91" s="12" t="s">
@@ -17152,22 +17215,22 @@
       <c r="L92" t="s">
         <v>8</v>
       </c>
-      <c r="M92" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="N92" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="O92" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="P92" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q92" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="R92" s="44" t="s">
+      <c r="M92" t="s">
+        <v>8</v>
+      </c>
+      <c r="N92" t="s">
+        <v>8</v>
+      </c>
+      <c r="O92" t="s">
+        <v>8</v>
+      </c>
+      <c r="P92" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>8</v>
+      </c>
+      <c r="R92" t="s">
         <v>8</v>
       </c>
       <c r="S92" s="12" t="s">
@@ -17487,7 +17550,7 @@
         <v>396</v>
       </c>
       <c r="G94" s="12" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="H94" s="6">
         <v>0</v>
@@ -17637,7 +17700,7 @@
         <v>1</v>
       </c>
       <c r="BD94" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="BE94" s="43" t="s">
         <v>288</v>
@@ -17663,7 +17726,7 @@
         <v>396</v>
       </c>
       <c r="G95" s="12" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="H95" s="6" t="s">
         <v>120</v>
@@ -17813,7 +17876,7 @@
         <v>1</v>
       </c>
       <c r="BD95" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="BE95" t="s">
         <v>349</v>
@@ -17833,13 +17896,13 @@
         <v>412</v>
       </c>
       <c r="E96" s="12" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>396</v>
       </c>
       <c r="G96" s="12" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="H96" s="6" t="s">
         <v>120</v>
@@ -17989,10 +18052,10 @@
         <v>1</v>
       </c>
       <c r="BD96" t="s">
-        <v>434</v>
-      </c>
-      <c r="BE96" t="s">
-        <v>435</v>
+        <v>428</v>
+      </c>
+      <c r="BE96" s="44" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="97" spans="1:57" x14ac:dyDescent="0.3">
@@ -18009,13 +18072,13 @@
         <v>412</v>
       </c>
       <c r="E97" s="12" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>396</v>
       </c>
       <c r="G97" s="12" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>120</v>
@@ -18110,14 +18173,14 @@
       <c r="AL97" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM97" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN97" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO97" s="20" t="s">
-        <v>120</v>
+      <c r="AM97">
+        <v>125</v>
+      </c>
+      <c r="AN97">
+        <v>1169</v>
+      </c>
+      <c r="AO97" s="20">
+        <v>414</v>
       </c>
       <c r="AP97">
         <v>96</v>
@@ -18165,9 +18228,9 @@
         <v>1</v>
       </c>
       <c r="BD97" t="s">
-        <v>433</v>
-      </c>
-      <c r="BE97" s="43" t="s">
+        <v>427</v>
+      </c>
+      <c r="BE97" s="44" t="s">
         <v>288</v>
       </c>
     </row>
@@ -18185,13 +18248,13 @@
         <v>412</v>
       </c>
       <c r="E98" s="12" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>396</v>
       </c>
       <c r="G98" s="12" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="H98" s="6" t="s">
         <v>120</v>
@@ -18286,14 +18349,14 @@
       <c r="AL98" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM98" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN98" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO98" s="20" t="s">
-        <v>120</v>
+      <c r="AM98">
+        <v>125</v>
+      </c>
+      <c r="AN98">
+        <v>1169</v>
+      </c>
+      <c r="AO98" s="20">
+        <v>414</v>
       </c>
       <c r="AP98">
         <v>96</v>
@@ -18340,8 +18403,11 @@
       <c r="BC98">
         <v>1</v>
       </c>
+      <c r="BD98" t="s">
+        <v>428</v>
+      </c>
       <c r="BE98" t="s">
-        <v>120</v>
+        <v>429</v>
       </c>
     </row>
     <row r="99" spans="1:57" x14ac:dyDescent="0.3">
@@ -18358,13 +18424,13 @@
         <v>412</v>
       </c>
       <c r="E99" s="12" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="F99" s="12" t="s">
         <v>396</v>
       </c>
       <c r="G99" s="12" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="H99" s="6" t="s">
         <v>120</v>
@@ -18459,14 +18525,14 @@
       <c r="AL99" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM99" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN99" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO99" s="20" t="s">
-        <v>120</v>
+      <c r="AM99">
+        <v>125</v>
+      </c>
+      <c r="AN99">
+        <v>1169</v>
+      </c>
+      <c r="AO99" s="20">
+        <v>414</v>
       </c>
       <c r="AP99">
         <v>71</v>
@@ -18477,16 +18543,16 @@
       <c r="AR99">
         <v>131</v>
       </c>
-      <c r="AS99" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT99">
+      <c r="AS99" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT99" s="49">
         <v>47</v>
       </c>
-      <c r="AU99">
+      <c r="AU99" s="44">
         <v>83</v>
       </c>
-      <c r="AV99">
+      <c r="AV99" s="44">
         <v>83</v>
       </c>
       <c r="AW99" s="25" t="s">
@@ -18514,15 +18580,15 @@
         <v>1</v>
       </c>
       <c r="BD99" t="s">
-        <v>120</v>
+        <v>428</v>
       </c>
       <c r="BE99" t="s">
-        <v>120</v>
+        <v>429</v>
       </c>
     </row>
     <row r="100" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="38" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>403</v>
@@ -18533,11 +18599,11 @@
       <c r="D100" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E100" s="12" t="s">
-        <v>438</v>
+      <c r="E100" s="38" t="s">
+        <v>445</v>
       </c>
       <c r="F100" s="38" t="s">
-        <v>120</v>
+        <v>451</v>
       </c>
       <c r="G100" s="38" t="s">
         <v>397</v>
@@ -18635,56 +18701,59 @@
       <c r="AL100" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO100" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS100" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV100" s="3" t="s">
-        <v>120</v>
+      <c r="AM100" s="3">
+        <v>190</v>
+      </c>
+      <c r="AN100" s="3">
+        <v>960</v>
+      </c>
+      <c r="AO100" s="41">
+        <v>1370</v>
+      </c>
+      <c r="AP100" s="3">
+        <v>128</v>
+      </c>
+      <c r="AQ100" s="3">
+        <v>512</v>
+      </c>
+      <c r="AR100" s="3">
+        <v>512</v>
+      </c>
+      <c r="AS100" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT100" s="50">
+        <f t="shared" ref="AT100:AT105" si="133" xml:space="preserve"> _xlfn.FLOOR.MATH((AM100 - AP100) / 2)</f>
+        <v>31</v>
+      </c>
+      <c r="AU100" s="48">
+        <f t="shared" ref="AU100:AU105" si="134" xml:space="preserve"> _xlfn.FLOOR.MATH((AN100 - AQ100) / 2)</f>
+        <v>224</v>
+      </c>
+      <c r="AV100" s="48">
+        <f t="shared" ref="AV100:AV105" si="135" xml:space="preserve"> _xlfn.FLOOR.MATH((AO100 - AR100) / 2)</f>
+        <v>429</v>
       </c>
       <c r="AW100" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AX100" s="3" t="e">
-        <f t="shared" ref="AX100:AX101" si="133">AP100-AT100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY100" s="3" t="e">
-        <f t="shared" ref="AY100:AY101" si="134">AQ100-AU100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ100" s="42" t="e">
-        <f t="shared" ref="AZ100:AZ101" si="135">AR100-AV100</f>
-        <v>#VALUE!</v>
+      <c r="AX100" s="3">
+        <f t="shared" ref="AX100:AX101" si="136">AP100-AT100</f>
+        <v>97</v>
+      </c>
+      <c r="AY100" s="3">
+        <f t="shared" ref="AY100:AY101" si="137">AQ100-AU100</f>
+        <v>288</v>
+      </c>
+      <c r="AZ100" s="42">
+        <f t="shared" ref="AZ100:AZ101" si="138">AR100-AV100</f>
+        <v>83</v>
       </c>
       <c r="BA100" s="3" t="s">
-        <v>120</v>
+        <v>419</v>
       </c>
       <c r="BB100" s="3" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="BC100" s="3" t="s">
         <v>120</v>
@@ -18698,7 +18767,7 @@
     </row>
     <row r="101" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
-        <v>424</v>
+        <v>440</v>
       </c>
       <c r="B101" t="s">
         <v>403</v>
@@ -18710,10 +18779,10 @@
         <v>412</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="F101" s="12" t="s">
-        <v>120</v>
+        <v>451</v>
       </c>
       <c r="G101" s="12" t="s">
         <v>397</v>
@@ -18811,56 +18880,59 @@
       <c r="AL101" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO101" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS101" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV101" t="s">
-        <v>120</v>
+      <c r="AM101" s="45">
+        <v>190</v>
+      </c>
+      <c r="AN101" s="45">
+        <v>960</v>
+      </c>
+      <c r="AO101" s="51">
+        <v>1370</v>
+      </c>
+      <c r="AP101" s="45">
+        <v>128</v>
+      </c>
+      <c r="AQ101" s="45">
+        <v>512</v>
+      </c>
+      <c r="AR101" s="45">
+        <v>512</v>
+      </c>
+      <c r="AS101" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT101" s="49">
+        <f t="shared" si="133"/>
+        <v>31</v>
+      </c>
+      <c r="AU101" s="44">
+        <f t="shared" si="134"/>
+        <v>224</v>
+      </c>
+      <c r="AV101" s="44">
+        <f t="shared" si="135"/>
+        <v>429</v>
       </c>
       <c r="AW101" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX101" t="e">
-        <f t="shared" si="133"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY101" t="e">
-        <f t="shared" si="134"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ101" s="10" t="e">
-        <f t="shared" si="135"/>
-        <v>#VALUE!</v>
+      <c r="AX101">
+        <f t="shared" si="136"/>
+        <v>97</v>
+      </c>
+      <c r="AY101">
+        <f t="shared" si="137"/>
+        <v>288</v>
+      </c>
+      <c r="AZ101" s="10">
+        <f t="shared" si="138"/>
+        <v>83</v>
       </c>
       <c r="BA101" t="s">
-        <v>120</v>
+        <v>419</v>
       </c>
       <c r="BB101" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="BC101" t="s">
         <v>120</v>
@@ -18874,7 +18946,7 @@
     </row>
     <row r="102" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
-        <v>425</v>
+        <v>441</v>
       </c>
       <c r="B102" t="s">
         <v>403</v>
@@ -18883,13 +18955,13 @@
         <v>410</v>
       </c>
       <c r="D102" t="s">
-        <v>120</v>
+        <v>433</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>120</v>
+        <v>446</v>
       </c>
       <c r="F102" s="12" t="s">
-        <v>120</v>
+        <v>451</v>
       </c>
       <c r="G102" s="12" t="s">
         <v>397</v>
@@ -18987,56 +19059,59 @@
       <c r="AL102" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO102" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS102" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV102" t="s">
-        <v>120</v>
+      <c r="AM102" s="45">
+        <v>190</v>
+      </c>
+      <c r="AN102" s="45">
+        <v>960</v>
+      </c>
+      <c r="AO102" s="51">
+        <v>1370</v>
+      </c>
+      <c r="AP102" s="45">
+        <v>128</v>
+      </c>
+      <c r="AQ102" s="45">
+        <v>512</v>
+      </c>
+      <c r="AR102" s="45">
+        <v>512</v>
+      </c>
+      <c r="AS102" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT102" s="49">
+        <f t="shared" si="133"/>
+        <v>31</v>
+      </c>
+      <c r="AU102" s="44">
+        <f t="shared" si="134"/>
+        <v>224</v>
+      </c>
+      <c r="AV102" s="44">
+        <f t="shared" si="135"/>
+        <v>429</v>
       </c>
       <c r="AW102" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX102" t="e">
-        <f t="shared" ref="AX102" si="136">AP102-AT102</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY102" t="e">
-        <f t="shared" ref="AY102" si="137">AQ102-AU102</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ102" s="10" t="e">
-        <f t="shared" ref="AZ102" si="138">AR102-AV102</f>
-        <v>#VALUE!</v>
+      <c r="AX102">
+        <f t="shared" ref="AX102" si="139">AP102-AT102</f>
+        <v>97</v>
+      </c>
+      <c r="AY102">
+        <f t="shared" ref="AY102" si="140">AQ102-AU102</f>
+        <v>288</v>
+      </c>
+      <c r="AZ102" s="10">
+        <f t="shared" ref="AZ102" si="141">AR102-AV102</f>
+        <v>83</v>
       </c>
       <c r="BA102" t="s">
-        <v>120</v>
+        <v>419</v>
       </c>
       <c r="BB102" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="BC102" t="s">
         <v>120</v>
@@ -19050,7 +19125,7 @@
     </row>
     <row r="103" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="38" t="s">
-        <v>426</v>
+        <v>442</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>403</v>
@@ -19062,10 +19137,10 @@
         <v>412</v>
       </c>
       <c r="E103" s="38" t="s">
-        <v>120</v>
+        <v>447</v>
       </c>
       <c r="F103" s="38" t="s">
-        <v>120</v>
+        <v>451</v>
       </c>
       <c r="G103" s="38" t="s">
         <v>397</v>
@@ -19163,56 +19238,59 @@
       <c r="AL103" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO103" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS103" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV103" s="3" t="s">
-        <v>120</v>
+      <c r="AM103" s="3">
+        <v>125</v>
+      </c>
+      <c r="AN103" s="3">
+        <v>1169</v>
+      </c>
+      <c r="AO103" s="41">
+        <v>414</v>
+      </c>
+      <c r="AP103" s="3">
+        <v>96</v>
+      </c>
+      <c r="AQ103" s="3">
+        <v>960</v>
+      </c>
+      <c r="AR103" s="3">
+        <v>256</v>
+      </c>
+      <c r="AS103" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT103" s="50">
+        <f t="shared" si="133"/>
+        <v>14</v>
+      </c>
+      <c r="AU103" s="48">
+        <f t="shared" si="134"/>
+        <v>104</v>
+      </c>
+      <c r="AV103" s="48">
+        <f t="shared" si="135"/>
+        <v>79</v>
       </c>
       <c r="AW103" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="AX103" s="3" t="e">
-        <f t="shared" ref="AX103" si="139">AP103-AT103</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY103" s="3" t="e">
-        <f t="shared" ref="AY103" si="140">AQ103-AU103</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ103" s="42" t="e">
-        <f t="shared" ref="AZ103" si="141">AR103-AV103</f>
-        <v>#VALUE!</v>
+      <c r="AX103" s="3">
+        <f t="shared" ref="AX103" si="142">AP103-AT103</f>
+        <v>82</v>
+      </c>
+      <c r="AY103" s="3">
+        <f t="shared" ref="AY103" si="143">AQ103-AU103</f>
+        <v>856</v>
+      </c>
+      <c r="AZ103" s="42">
+        <f t="shared" ref="AZ103" si="144">AR103-AV103</f>
+        <v>177</v>
       </c>
       <c r="BA103" s="3" t="s">
-        <v>120</v>
+        <v>419</v>
       </c>
       <c r="BB103" s="3" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="BC103" s="3" t="s">
         <v>120</v>
@@ -19226,7 +19304,7 @@
     </row>
     <row r="104" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
-        <v>427</v>
+        <v>443</v>
       </c>
       <c r="B104" t="s">
         <v>403</v>
@@ -19238,10 +19316,10 @@
         <v>412</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>120</v>
+        <v>449</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>120</v>
+        <v>451</v>
       </c>
       <c r="G104" s="12" t="s">
         <v>397</v>
@@ -19339,56 +19417,59 @@
       <c r="AL104" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM104" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN104" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO104" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP104" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ104" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR104" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS104" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT104" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU104" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV104" t="s">
-        <v>120</v>
+      <c r="AM104">
+        <v>125</v>
+      </c>
+      <c r="AN104">
+        <v>1169</v>
+      </c>
+      <c r="AO104" s="20">
+        <v>414</v>
+      </c>
+      <c r="AP104" s="45">
+        <v>96</v>
+      </c>
+      <c r="AQ104" s="45">
+        <v>960</v>
+      </c>
+      <c r="AR104" s="45">
+        <v>256</v>
+      </c>
+      <c r="AS104" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT104" s="49">
+        <f t="shared" si="133"/>
+        <v>14</v>
+      </c>
+      <c r="AU104" s="44">
+        <f t="shared" si="134"/>
+        <v>104</v>
+      </c>
+      <c r="AV104" s="44">
+        <f t="shared" si="135"/>
+        <v>79</v>
       </c>
       <c r="AW104" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX104" t="e">
-        <f t="shared" ref="AX104" si="142">AP104-AT104</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY104" t="e">
-        <f t="shared" ref="AY104" si="143">AQ104-AU104</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ104" s="10" t="e">
-        <f t="shared" ref="AZ104" si="144">AR104-AV104</f>
-        <v>#VALUE!</v>
+      <c r="AX104">
+        <f t="shared" ref="AX104" si="145">AP104-AT104</f>
+        <v>82</v>
+      </c>
+      <c r="AY104">
+        <f t="shared" ref="AY104" si="146">AQ104-AU104</f>
+        <v>856</v>
+      </c>
+      <c r="AZ104" s="10">
+        <f t="shared" ref="AZ104" si="147">AR104-AV104</f>
+        <v>177</v>
       </c>
       <c r="BA104" t="s">
-        <v>120</v>
+        <v>419</v>
       </c>
       <c r="BB104" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="BC104" t="s">
         <v>120</v>
@@ -19402,7 +19483,7 @@
     </row>
     <row r="105" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
-        <v>428</v>
+        <v>444</v>
       </c>
       <c r="B105" t="s">
         <v>403</v>
@@ -19411,13 +19492,13 @@
         <v>410</v>
       </c>
       <c r="D105" t="s">
-        <v>120</v>
+        <v>433</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>120</v>
+        <v>450</v>
       </c>
       <c r="F105" s="12" t="s">
-        <v>120</v>
+        <v>451</v>
       </c>
       <c r="G105" s="12" t="s">
         <v>397</v>
@@ -19515,240 +19596,1299 @@
       <c r="AL105" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM105" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN105" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO105" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP105" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ105" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR105" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS105" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT105" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU105" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV105" t="s">
-        <v>120</v>
+      <c r="AM105">
+        <v>125</v>
+      </c>
+      <c r="AN105">
+        <v>1169</v>
+      </c>
+      <c r="AO105" s="20">
+        <v>414</v>
+      </c>
+      <c r="AP105" s="45">
+        <v>96</v>
+      </c>
+      <c r="AQ105" s="45">
+        <v>960</v>
+      </c>
+      <c r="AR105" s="45">
+        <v>256</v>
+      </c>
+      <c r="AS105" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT105" s="49">
+        <f t="shared" si="133"/>
+        <v>14</v>
+      </c>
+      <c r="AU105" s="44">
+        <f t="shared" si="134"/>
+        <v>104</v>
+      </c>
+      <c r="AV105" s="44">
+        <f t="shared" si="135"/>
+        <v>79</v>
       </c>
       <c r="AW105" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX105" t="e">
-        <f t="shared" ref="AX105" si="145">AP105-AT105</f>
+      <c r="AX105">
+        <f t="shared" ref="AX105" si="148">AP105-AT105</f>
+        <v>82</v>
+      </c>
+      <c r="AY105">
+        <f t="shared" ref="AY105" si="149">AQ105-AU105</f>
+        <v>856</v>
+      </c>
+      <c r="AZ105" s="10">
+        <f t="shared" ref="AZ105" si="150">AR105-AV105</f>
+        <v>177</v>
+      </c>
+      <c r="BA105" t="s">
+        <v>419</v>
+      </c>
+      <c r="BB105" t="s">
+        <v>163</v>
+      </c>
+      <c r="BC105" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD105" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE105" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="106" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="B106" s="45" t="s">
+        <v>404</v>
+      </c>
+      <c r="C106" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="D106" s="45" t="s">
+        <v>412</v>
+      </c>
+      <c r="E106" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F106" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G106" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="H106" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="I106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="J106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="K106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="L106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="M106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="N106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="O106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="P106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="R106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="S106" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T106" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="U106" s="45" t="s">
+        <v>344</v>
+      </c>
+      <c r="V106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="W106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="X106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH106" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI106" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK106" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL106" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM106" s="45">
+        <v>190</v>
+      </c>
+      <c r="AN106" s="45">
+        <v>960</v>
+      </c>
+      <c r="AO106" s="51">
+        <v>1370</v>
+      </c>
+      <c r="AP106" s="45">
+        <v>128</v>
+      </c>
+      <c r="AQ106" s="45">
+        <v>512</v>
+      </c>
+      <c r="AR106" s="45">
+        <v>512</v>
+      </c>
+      <c r="AS106" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT106" s="54">
+        <v>64</v>
+      </c>
+      <c r="AU106" s="55">
+        <v>96</v>
+      </c>
+      <c r="AV106" s="55">
+        <v>96</v>
+      </c>
+      <c r="AW106" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX106" s="45">
+        <f t="shared" ref="AX106" si="151">AP106-AT106</f>
+        <v>64</v>
+      </c>
+      <c r="AY106" s="45">
+        <f t="shared" ref="AY106" si="152">AQ106-AU106</f>
+        <v>416</v>
+      </c>
+      <c r="AZ106" s="53">
+        <f t="shared" ref="AZ106" si="153">AR106-AV106</f>
+        <v>416</v>
+      </c>
+      <c r="BA106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD106" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE106" s="45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="107" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="12" t="s">
+        <v>435</v>
+      </c>
+      <c r="B107" s="45" t="s">
+        <v>404</v>
+      </c>
+      <c r="C107" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="D107" s="45" t="s">
+        <v>412</v>
+      </c>
+      <c r="E107" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G107" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="H107" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="I107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="J107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="K107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="L107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="M107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="N107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="O107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="P107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="R107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="S107" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T107" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="U107" s="45" t="s">
+        <v>344</v>
+      </c>
+      <c r="V107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="W107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="X107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH107" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI107" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK107" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL107" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM107" s="45">
+        <v>190</v>
+      </c>
+      <c r="AN107" s="45">
+        <v>960</v>
+      </c>
+      <c r="AO107" s="51">
+        <v>1370</v>
+      </c>
+      <c r="AP107" s="45">
+        <v>128</v>
+      </c>
+      <c r="AQ107" s="45">
+        <v>512</v>
+      </c>
+      <c r="AR107" s="45">
+        <v>512</v>
+      </c>
+      <c r="AS107" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT107" s="45">
+        <v>64</v>
+      </c>
+      <c r="AU107" s="45">
+        <v>96</v>
+      </c>
+      <c r="AV107" s="45">
+        <v>96</v>
+      </c>
+      <c r="AW107" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX107" s="45">
+        <f t="shared" ref="AX107" si="154">AP107-AT107</f>
+        <v>64</v>
+      </c>
+      <c r="AY107" s="45">
+        <f t="shared" ref="AY107" si="155">AQ107-AU107</f>
+        <v>416</v>
+      </c>
+      <c r="AZ107" s="53">
+        <f t="shared" ref="AZ107" si="156">AR107-AV107</f>
+        <v>416</v>
+      </c>
+      <c r="BA107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE107" s="45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="108" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="B108" s="45" t="s">
+        <v>404</v>
+      </c>
+      <c r="C108" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="D108" s="45" t="s">
+        <v>433</v>
+      </c>
+      <c r="E108" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="H108" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="I108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="J108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="K108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="L108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="M108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="N108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="O108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="P108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="R108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="S108" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T108" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="U108" s="45" t="s">
+        <v>344</v>
+      </c>
+      <c r="V108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="W108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="X108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH108" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI108" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK108" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL108" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM108" s="45">
+        <v>190</v>
+      </c>
+      <c r="AN108" s="45">
+        <v>960</v>
+      </c>
+      <c r="AO108" s="51">
+        <v>1370</v>
+      </c>
+      <c r="AP108" s="45">
+        <v>128</v>
+      </c>
+      <c r="AQ108" s="45">
+        <v>512</v>
+      </c>
+      <c r="AR108" s="45">
+        <v>512</v>
+      </c>
+      <c r="AS108" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT108" s="45">
+        <v>64</v>
+      </c>
+      <c r="AU108" s="45">
+        <v>96</v>
+      </c>
+      <c r="AV108" s="45">
+        <v>96</v>
+      </c>
+      <c r="AW108" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX108" s="45">
+        <f t="shared" ref="AX108" si="157">AP108-AT108</f>
+        <v>64</v>
+      </c>
+      <c r="AY108" s="45">
+        <f t="shared" ref="AY108" si="158">AQ108-AU108</f>
+        <v>416</v>
+      </c>
+      <c r="AZ108" s="53">
+        <f t="shared" ref="AZ108" si="159">AR108-AV108</f>
+        <v>416</v>
+      </c>
+      <c r="BA108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD108" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE108" s="45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="109" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="B109" s="45" t="s">
+        <v>404</v>
+      </c>
+      <c r="C109" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="D109" s="45" t="s">
+        <v>412</v>
+      </c>
+      <c r="E109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G109" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="H109" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="I109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="J109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="K109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="L109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="M109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="N109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="O109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="P109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="R109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="S109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T109" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="U109" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="V109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="W109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="X109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH109" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK109" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL109" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM109" s="45">
+        <v>125</v>
+      </c>
+      <c r="AN109" s="45">
+        <v>1169</v>
+      </c>
+      <c r="AO109" s="51">
+        <v>414</v>
+      </c>
+      <c r="AP109" s="45">
+        <v>96</v>
+      </c>
+      <c r="AQ109" s="45">
+        <v>128</v>
+      </c>
+      <c r="AR109" s="45">
+        <v>128</v>
+      </c>
+      <c r="AS109" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT109" s="45">
+        <v>64</v>
+      </c>
+      <c r="AU109" s="45">
+        <v>96</v>
+      </c>
+      <c r="AV109" s="45">
+        <v>96</v>
+      </c>
+      <c r="AW109" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX109" s="45">
+        <f t="shared" ref="AX109" si="160">AP109-AT109</f>
+        <v>32</v>
+      </c>
+      <c r="AY109" s="45">
+        <f t="shared" ref="AY109" si="161">AQ109-AU109</f>
+        <v>32</v>
+      </c>
+      <c r="AZ109" s="53">
+        <f t="shared" ref="AZ109" si="162">AR109-AV109</f>
+        <v>32</v>
+      </c>
+      <c r="BA109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD109" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE109" s="45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="110" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="B110" s="45" t="s">
+        <v>404</v>
+      </c>
+      <c r="C110" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="D110" s="45" t="s">
+        <v>412</v>
+      </c>
+      <c r="E110" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F110" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G110" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="H110" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="I110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="J110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="K110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="L110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="M110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="N110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="O110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="P110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="R110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="S110" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T110" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="U110" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="V110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="W110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="X110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH110" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI110" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK110" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL110" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM110" s="45">
+        <v>125</v>
+      </c>
+      <c r="AN110" s="45">
+        <v>1169</v>
+      </c>
+      <c r="AO110" s="51">
+        <v>414</v>
+      </c>
+      <c r="AP110" s="45">
+        <v>96</v>
+      </c>
+      <c r="AQ110" s="45">
+        <v>128</v>
+      </c>
+      <c r="AR110" s="45">
+        <v>128</v>
+      </c>
+      <c r="AS110" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT110" s="45">
+        <v>64</v>
+      </c>
+      <c r="AU110" s="45">
+        <v>96</v>
+      </c>
+      <c r="AV110" s="45">
+        <v>96</v>
+      </c>
+      <c r="AW110" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX110" s="45">
+        <f t="shared" ref="AX110" si="163">AP110-AT110</f>
+        <v>32</v>
+      </c>
+      <c r="AY110" s="45">
+        <f t="shared" ref="AY110" si="164">AQ110-AU110</f>
+        <v>32</v>
+      </c>
+      <c r="AZ110" s="53">
+        <f t="shared" ref="AZ110" si="165">AR110-AV110</f>
+        <v>32</v>
+      </c>
+      <c r="BA110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD110" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE110" s="45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="111" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="B111" s="45" t="s">
+        <v>404</v>
+      </c>
+      <c r="C111" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="D111" s="45" t="s">
+        <v>433</v>
+      </c>
+      <c r="E111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G111" s="12" t="s">
+        <v>397</v>
+      </c>
+      <c r="H111" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="I111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="J111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="K111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="L111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="M111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="N111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="O111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="P111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="R111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="S111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T111" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="U111" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="V111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="W111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="X111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH111" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK111" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL111" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM111" s="45">
+        <v>125</v>
+      </c>
+      <c r="AN111" s="45">
+        <v>1169</v>
+      </c>
+      <c r="AO111" s="51">
+        <v>414</v>
+      </c>
+      <c r="AP111" s="45">
+        <v>96</v>
+      </c>
+      <c r="AQ111" s="45">
+        <v>128</v>
+      </c>
+      <c r="AR111" s="45">
+        <v>128</v>
+      </c>
+      <c r="AS111" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT111" s="45">
+        <v>64</v>
+      </c>
+      <c r="AU111" s="45">
+        <v>96</v>
+      </c>
+      <c r="AV111" s="45">
+        <v>96</v>
+      </c>
+      <c r="AW111" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX111" s="45">
+        <f t="shared" ref="AX111" si="166">AP111-AT111</f>
+        <v>32</v>
+      </c>
+      <c r="AY111" s="45">
+        <f t="shared" ref="AY111" si="167">AQ111-AU111</f>
+        <v>32</v>
+      </c>
+      <c r="AZ111" s="53">
+        <f t="shared" ref="AZ111" si="168">AR111-AV111</f>
+        <v>32</v>
+      </c>
+      <c r="BA111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD111" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE111" s="45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="112" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="E112" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F112" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G112" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H112" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="I112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="J112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="K112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="L112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="M112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="N112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="O112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="P112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="R112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="S112" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T112" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="U112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="V112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="W112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="X112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH112" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI112" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK112" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL112" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO112" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS112" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW112" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX112" s="45" t="e">
+        <f t="shared" ref="AX112" si="169">AP112-AT112</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AY105" t="e">
-        <f t="shared" ref="AY105" si="146">AQ105-AU105</f>
+      <c r="AY112" s="45" t="e">
+        <f t="shared" ref="AY112" si="170">AQ112-AU112</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ105" s="10" t="e">
-        <f t="shared" ref="AZ105" si="147">AR105-AV105</f>
+      <c r="AZ112" s="53" t="e">
+        <f t="shared" ref="AZ112" si="171">AR112-AV112</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA105" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB105" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC105" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD105" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE105" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="106" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A106" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B106" t="s">
-        <v>120</v>
-      </c>
-      <c r="C106" t="s">
-        <v>120</v>
-      </c>
-      <c r="D106" t="s">
-        <v>120</v>
-      </c>
-      <c r="E106" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F106" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G106" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="H106" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I106" t="s">
-        <v>120</v>
-      </c>
-      <c r="J106" t="s">
-        <v>120</v>
-      </c>
-      <c r="K106" t="s">
-        <v>120</v>
-      </c>
-      <c r="L106" t="s">
-        <v>120</v>
-      </c>
-      <c r="M106" t="s">
-        <v>120</v>
-      </c>
-      <c r="N106" t="s">
-        <v>120</v>
-      </c>
-      <c r="O106" t="s">
-        <v>120</v>
-      </c>
-      <c r="P106" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q106" t="s">
-        <v>120</v>
-      </c>
-      <c r="R106" t="s">
-        <v>120</v>
-      </c>
-      <c r="S106" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="T106" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="U106" t="s">
-        <v>120</v>
-      </c>
-      <c r="V106" t="s">
-        <v>120</v>
-      </c>
-      <c r="W106" t="s">
-        <v>120</v>
-      </c>
-      <c r="X106" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y106" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH106" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI106" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK106" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL106" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO106" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS106" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV106" t="s">
-        <v>120</v>
-      </c>
-      <c r="AW106" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX106" t="e">
-        <f t="shared" ref="AX106" si="148">AP106-AT106</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY106" t="e">
-        <f t="shared" ref="AY106" si="149">AQ106-AU106</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ106" s="10" t="e">
-        <f t="shared" ref="AZ106" si="150">AR106-AV106</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA106" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB106" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC106" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD106" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE106" t="s">
+      <c r="BA112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD112" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE112" s="45" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare predict3dunet 1.6.0 231224-0
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3568A18-E5ED-4CA9-BA66-0FF59C07AB97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FA1FCD-3B6D-4B35-AFD0-061A5EFA051C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3482" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3233" uniqueCount="457">
   <si>
     <t>patch z</t>
   </si>
@@ -1344,21 +1344,6 @@
     <t>231224-0</t>
   </si>
   <si>
-    <t>231224-1</t>
-  </si>
-  <si>
-    <t>231224-2</t>
-  </si>
-  <si>
-    <t>231224-3</t>
-  </si>
-  <si>
-    <t>231224-4</t>
-  </si>
-  <si>
-    <t>231224-5</t>
-  </si>
-  <si>
     <t>231223-1</t>
   </si>
   <si>
@@ -1393,13 +1378,45 @@
   </si>
   <si>
     <t>See corr. predict3dunet session for results.</t>
+  </si>
+  <si>
+    <t>slurmstepd: error: Detected 1 oom-kill event(s) in StepId=7581907.batch. Some of your processes may have been killed by the cgroup out-of-memory handler.</t>
+  </si>
+  <si>
+    <t>RuntimeError: Expected output.numel() &lt;= std::numeric_limits&lt;int32_t&gt;::max() to be true, but got false.  (Could this error message be improved?  If so, please report an enhancement request to PyTorch.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> File "/home/dwalth/data/conda/envs/3dunet/lib/python3.11/site-packages/torch/nn/functional.py", line 3933, in interpolate    return torch._C._nn.upsample_nearest3d(input, output_size, scale_factors)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  File "/home/dwalth/data/conda/envs/3dunet/lib/python3.11/site-packages/torch/nn/functional.py", line 3933, in interpolate
+    return torch._C._nn.upsample_nearest3d(input, output_size, scale_factors)</t>
+  </si>
+  <si>
+    <t>torch.cuda.OutOfMemoryError: CUDA out of memory. Tried to allocate 227.81 GiB (GPU 0; 79.15 GiB total capacity; 37.28 GiB already allocated; 35.79 GiB free; 41.78 GiB reserved in total by PyTorch) If reserved memory is &gt;&gt; allocated memory try setting max_split_size_mb to avoid fragmentation.  See documentation for Memory Management and PYTORCH_CUDA_ALLOC_CONF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  File "/home/dwalth/data/conda/envs/3dunet/lib/python3.11/site-packages/torch/nn/modules/conv.py", line 608, in _conv_forward
+    return F.conv3d(</t>
+  </si>
+  <si>
+    <t>out of memory</t>
+  </si>
+  <si>
+    <t>new error TBD</t>
+  </si>
+  <si>
+    <t>patch = same as used for training this model.</t>
+  </si>
+  <si>
+    <t>stride = same as used for training this model.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1422,13 +1439,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1643,7 +1653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1693,33 +1703,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2034,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BE112"/>
+  <dimension ref="A1:BE111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT103" sqref="AT103"/>
+    <sheetView tabSelected="1" topLeftCell="AK92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AK106" sqref="AK106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -15418,159 +15412,159 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="38" t="s">
+    <row r="82" spans="1:57" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="39" t="s">
         <v>404</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" s="39" t="s">
         <v>409</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D82" s="39" t="s">
         <v>412</v>
       </c>
-      <c r="E82" s="38" t="s">
+      <c r="E82" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="F82" s="38" t="s">
+      <c r="F82" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="G82" s="38" t="s">
+      <c r="G82" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="H82" s="39">
-        <v>0</v>
-      </c>
-      <c r="I82" s="3">
-        <v>1</v>
-      </c>
-      <c r="J82" s="40" t="s">
+      <c r="H82" s="40">
+        <v>0</v>
+      </c>
+      <c r="I82" s="39">
+        <v>1</v>
+      </c>
+      <c r="J82" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="K82" s="3">
-        <v>0</v>
-      </c>
-      <c r="L82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R82" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="S82" s="38" t="s">
+      <c r="K82" s="39">
+        <v>0</v>
+      </c>
+      <c r="L82" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M82" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="N82" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="O82" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="P82" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q82" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="R82" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="S82" s="12" t="s">
         <v>8</v>
       </c>
       <c r="T82" s="41">
         <v>0</v>
       </c>
-      <c r="U82" s="3" t="s">
+      <c r="U82" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="V82" s="3" t="s">
+      <c r="V82" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="W82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="X82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="Y82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="Z82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AA82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AB82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AC82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AD82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AE82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AF82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AG82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AH82" s="39" t="s">
-        <v>401</v>
-      </c>
-      <c r="AI82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AJ82" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AK82" s="3" t="s">
+      <c r="W82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="X82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AB82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AD82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AF82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AH82" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AJ82" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AK82" s="39" t="s">
         <v>401</v>
       </c>
       <c r="AL82" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM82" s="3" t="s">
+      <c r="AM82" s="39" t="s">
         <v>402</v>
       </c>
-      <c r="AN82" s="3" t="s">
+      <c r="AN82" s="39" t="s">
         <v>402</v>
       </c>
       <c r="AO82" s="41" t="s">
         <v>402</v>
       </c>
-      <c r="AP82" s="3">
+      <c r="AP82" s="39">
         <v>80</v>
       </c>
-      <c r="AQ82" s="3">
+      <c r="AQ82" s="39">
         <v>170</v>
       </c>
-      <c r="AR82" s="3">
+      <c r="AR82" s="39">
         <v>170</v>
       </c>
-      <c r="AS82" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT82" s="3">
+      <c r="AS82" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT82" s="39">
         <v>40</v>
       </c>
-      <c r="AU82" s="3">
+      <c r="AU82" s="39">
         <v>90</v>
       </c>
-      <c r="AV82" s="3">
+      <c r="AV82" s="39">
         <v>90</v>
       </c>
-      <c r="AW82" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX82" s="3">
+      <c r="AW82" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX82" s="39">
         <f t="shared" ref="AX82:AZ83" si="84">AP82-AT82</f>
         <v>40</v>
       </c>
-      <c r="AY82" s="3">
+      <c r="AY82" s="39">
         <f t="shared" si="84"/>
         <v>80</v>
       </c>
@@ -15578,19 +15572,19 @@
         <f t="shared" si="84"/>
         <v>80</v>
       </c>
-      <c r="BA82" s="3" t="s">
+      <c r="BA82" s="39" t="s">
         <v>341</v>
       </c>
-      <c r="BB82" s="3" t="s">
+      <c r="BB82" s="39" t="s">
         <v>340</v>
       </c>
-      <c r="BC82" s="3">
-        <v>1</v>
-      </c>
-      <c r="BD82" s="3" t="s">
+      <c r="BC82" s="39">
+        <v>1</v>
+      </c>
+      <c r="BD82" s="39" t="s">
         <v>287</v>
       </c>
-      <c r="BE82" s="3" t="s">
+      <c r="BE82" s="39" t="s">
         <v>288</v>
       </c>
     </row>
@@ -16122,159 +16116,159 @@
         <v>288</v>
       </c>
     </row>
-    <row r="86" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="38" t="s">
+    <row r="86" spans="1:57" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="12" t="s">
         <v>380</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B86" s="39" t="s">
         <v>398</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C86" s="39" t="s">
         <v>409</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" s="39" t="s">
         <v>412</v>
       </c>
-      <c r="E86" s="38" t="s">
+      <c r="E86" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="F86" s="38" t="s">
+      <c r="F86" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="G86" s="38" t="s">
+      <c r="G86" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="H86" s="39">
-        <v>0</v>
-      </c>
-      <c r="I86" s="3">
-        <v>1</v>
-      </c>
-      <c r="J86" s="3" t="s">
+      <c r="H86" s="40">
+        <v>0</v>
+      </c>
+      <c r="I86" s="39">
+        <v>1</v>
+      </c>
+      <c r="J86" s="39" t="s">
         <v>400</v>
       </c>
-      <c r="K86" s="3">
-        <v>0</v>
-      </c>
-      <c r="L86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="S86" s="38" t="s">
+      <c r="K86" s="39">
+        <v>0</v>
+      </c>
+      <c r="L86" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M86" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="N86" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="O86" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="P86" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q86" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="R86" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="S86" s="12" t="s">
         <v>8</v>
       </c>
       <c r="T86" s="41">
         <v>0</v>
       </c>
-      <c r="U86" s="3" t="s">
+      <c r="U86" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="V86" s="3" t="s">
+      <c r="V86" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="W86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="X86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="Y86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="Z86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AA86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AB86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AC86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AD86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AE86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AF86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AG86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AH86" s="39" t="s">
-        <v>401</v>
-      </c>
-      <c r="AI86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AJ86" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AK86" s="3" t="s">
+      <c r="W86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="X86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AB86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AD86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AF86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AH86" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AJ86" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AK86" s="39" t="s">
         <v>401</v>
       </c>
       <c r="AL86" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM86" s="3" t="s">
+      <c r="AM86" s="39" t="s">
         <v>402</v>
       </c>
-      <c r="AN86" s="3" t="s">
+      <c r="AN86" s="39" t="s">
         <v>402</v>
       </c>
       <c r="AO86" s="41" t="s">
         <v>402</v>
       </c>
-      <c r="AP86" s="3">
+      <c r="AP86" s="39">
         <v>80</v>
       </c>
-      <c r="AQ86" s="3">
+      <c r="AQ86" s="39">
         <v>170</v>
       </c>
-      <c r="AR86" s="3">
+      <c r="AR86" s="39">
         <v>170</v>
       </c>
-      <c r="AS86" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT86" s="3">
+      <c r="AS86" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT86" s="39">
         <v>40</v>
       </c>
-      <c r="AU86" s="3">
+      <c r="AU86" s="39">
         <v>90</v>
       </c>
-      <c r="AV86" s="3">
+      <c r="AV86" s="39">
         <v>90</v>
       </c>
-      <c r="AW86" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX86" s="3">
+      <c r="AW86" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX86" s="39">
         <f t="shared" ref="AX86" si="91">AP86-AT86</f>
         <v>40</v>
       </c>
-      <c r="AY86" s="3">
+      <c r="AY86" s="39">
         <f t="shared" ref="AY86" si="92">AQ86-AU86</f>
         <v>80</v>
       </c>
@@ -16282,33 +16276,33 @@
         <f t="shared" ref="AZ86" si="93">AR86-AV86</f>
         <v>80</v>
       </c>
-      <c r="BA86" s="3" t="s">
+      <c r="BA86" s="39" t="s">
         <v>341</v>
       </c>
-      <c r="BB86" s="3" t="s">
+      <c r="BB86" s="39" t="s">
         <v>340</v>
       </c>
-      <c r="BC86" s="3">
-        <v>1</v>
-      </c>
-      <c r="BD86" s="3" t="s">
+      <c r="BC86" s="39">
+        <v>1</v>
+      </c>
+      <c r="BD86" s="39" t="s">
         <v>394</v>
       </c>
-      <c r="BE86" s="3" t="s">
+      <c r="BE86" s="39" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="87" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:57" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="39" t="s">
         <v>398</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="39" t="s">
         <v>409</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="39" t="s">
         <v>412</v>
       </c>
       <c r="E87" s="12" t="s">
@@ -16320,171 +16314,171 @@
       <c r="G87" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="H87" s="6">
-        <v>0</v>
-      </c>
-      <c r="I87">
-        <v>1</v>
-      </c>
-      <c r="J87" t="s">
+      <c r="H87" s="40">
+        <v>0</v>
+      </c>
+      <c r="I87" s="39">
+        <v>1</v>
+      </c>
+      <c r="J87" s="39" t="s">
         <v>400</v>
       </c>
-      <c r="K87">
-        <v>0</v>
-      </c>
-      <c r="L87" t="s">
-        <v>8</v>
-      </c>
-      <c r="M87" t="s">
-        <v>8</v>
-      </c>
-      <c r="N87" t="s">
-        <v>8</v>
-      </c>
-      <c r="O87" t="s">
-        <v>8</v>
-      </c>
-      <c r="P87" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q87" t="s">
-        <v>8</v>
-      </c>
-      <c r="R87" t="s">
+      <c r="K87" s="39">
+        <v>0</v>
+      </c>
+      <c r="L87" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M87" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="N87" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="O87" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="P87" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q87" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="R87" s="39" t="s">
         <v>8</v>
       </c>
       <c r="S87" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="T87" s="20">
-        <v>0</v>
-      </c>
-      <c r="U87" t="s">
+      <c r="T87" s="41">
+        <v>0</v>
+      </c>
+      <c r="U87" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="V87" t="s">
+      <c r="V87" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="W87" t="s">
-        <v>401</v>
-      </c>
-      <c r="X87" t="s">
-        <v>401</v>
-      </c>
-      <c r="Y87" t="s">
-        <v>401</v>
-      </c>
-      <c r="Z87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AA87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AB87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AC87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AD87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AE87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AF87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AG87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AH87" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="AI87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AJ87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AK87" t="s">
-        <v>401</v>
-      </c>
-      <c r="AL87" s="10" t="s">
+      <c r="W87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="X87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AB87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AD87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AF87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AH87" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AJ87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AK87" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AL87" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM87" t="s">
+      <c r="AM87" s="39" t="s">
         <v>402</v>
       </c>
-      <c r="AN87" t="s">
+      <c r="AN87" s="39" t="s">
         <v>402</v>
       </c>
-      <c r="AO87" s="20" t="s">
+      <c r="AO87" s="41" t="s">
         <v>402</v>
       </c>
-      <c r="AP87">
+      <c r="AP87" s="39">
         <v>80</v>
       </c>
-      <c r="AQ87">
+      <c r="AQ87" s="39">
         <v>240</v>
       </c>
-      <c r="AR87">
+      <c r="AR87" s="39">
         <v>240</v>
       </c>
       <c r="AS87" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT87">
+      <c r="AT87" s="39">
         <v>64</v>
       </c>
-      <c r="AU87">
+      <c r="AU87" s="39">
         <v>144</v>
       </c>
-      <c r="AV87">
+      <c r="AV87" s="39">
         <v>144</v>
       </c>
       <c r="AW87" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX87">
+      <c r="AX87" s="39">
         <f t="shared" ref="AX87" si="94">AP87-AT87</f>
         <v>16</v>
       </c>
-      <c r="AY87">
+      <c r="AY87" s="39">
         <f t="shared" ref="AY87" si="95">AQ87-AU87</f>
         <v>96</v>
       </c>
-      <c r="AZ87" s="10">
+      <c r="AZ87" s="42">
         <f t="shared" ref="AZ87" si="96">AR87-AV87</f>
         <v>96</v>
       </c>
-      <c r="BA87" t="s">
+      <c r="BA87" s="39" t="s">
         <v>289</v>
       </c>
-      <c r="BB87" t="s">
+      <c r="BB87" s="39" t="s">
         <v>290</v>
       </c>
-      <c r="BC87">
-        <v>1</v>
-      </c>
-      <c r="BD87" t="s">
+      <c r="BC87" s="39">
+        <v>1</v>
+      </c>
+      <c r="BD87" s="39" t="s">
         <v>394</v>
       </c>
-      <c r="BE87" t="s">
+      <c r="BE87" s="39" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="88" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:57" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="39" t="s">
         <v>398</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="39" t="s">
         <v>409</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="39" t="s">
         <v>412</v>
       </c>
       <c r="E88" s="12" t="s">
@@ -16496,171 +16490,171 @@
       <c r="G88" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="H88" s="6">
-        <v>0</v>
-      </c>
-      <c r="I88">
-        <v>1</v>
-      </c>
-      <c r="J88" t="s">
+      <c r="H88" s="40">
+        <v>0</v>
+      </c>
+      <c r="I88" s="39">
+        <v>1</v>
+      </c>
+      <c r="J88" s="39" t="s">
         <v>400</v>
       </c>
-      <c r="K88">
-        <v>0</v>
-      </c>
-      <c r="L88" t="s">
-        <v>8</v>
-      </c>
-      <c r="M88" t="s">
-        <v>8</v>
-      </c>
-      <c r="N88" t="s">
-        <v>8</v>
-      </c>
-      <c r="O88" t="s">
-        <v>8</v>
-      </c>
-      <c r="P88" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q88" t="s">
-        <v>8</v>
-      </c>
-      <c r="R88" t="s">
+      <c r="K88" s="39">
+        <v>0</v>
+      </c>
+      <c r="L88" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M88" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="N88" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="O88" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="P88" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q88" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="R88" s="39" t="s">
         <v>8</v>
       </c>
       <c r="S88" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="T88" s="20">
-        <v>0</v>
-      </c>
-      <c r="U88" t="s">
+      <c r="T88" s="41">
+        <v>0</v>
+      </c>
+      <c r="U88" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="V88" t="s">
+      <c r="V88" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="W88" t="s">
-        <v>401</v>
-      </c>
-      <c r="X88" t="s">
-        <v>401</v>
-      </c>
-      <c r="Y88" t="s">
-        <v>401</v>
-      </c>
-      <c r="Z88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AA88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AB88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AC88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AD88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AE88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AF88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AG88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AH88" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="AI88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AJ88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AK88" t="s">
-        <v>401</v>
-      </c>
-      <c r="AL88" s="10" t="s">
+      <c r="W88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="X88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AB88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AD88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AF88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AH88" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AJ88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AK88" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AL88" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM88" t="s">
+      <c r="AM88" s="39" t="s">
         <v>402</v>
       </c>
-      <c r="AN88" t="s">
+      <c r="AN88" s="39" t="s">
         <v>402</v>
       </c>
-      <c r="AO88" s="20" t="s">
+      <c r="AO88" s="41" t="s">
         <v>402</v>
       </c>
-      <c r="AP88">
+      <c r="AP88" s="39">
         <v>80</v>
       </c>
-      <c r="AQ88">
+      <c r="AQ88" s="39">
         <v>240</v>
       </c>
-      <c r="AR88">
+      <c r="AR88" s="39">
         <v>240</v>
       </c>
       <c r="AS88" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT88">
+      <c r="AT88" s="39">
         <v>48</v>
       </c>
-      <c r="AU88">
+      <c r="AU88" s="39">
         <v>208</v>
       </c>
-      <c r="AV88">
+      <c r="AV88" s="39">
         <v>208</v>
       </c>
       <c r="AW88" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX88">
+      <c r="AX88" s="39">
         <f t="shared" ref="AX88" si="97">AP88-AT88</f>
         <v>32</v>
       </c>
-      <c r="AY88">
+      <c r="AY88" s="39">
         <f t="shared" ref="AY88" si="98">AQ88-AU88</f>
         <v>32</v>
       </c>
-      <c r="AZ88" s="10">
+      <c r="AZ88" s="42">
         <f t="shared" ref="AZ88" si="99">AR88-AV88</f>
         <v>32</v>
       </c>
-      <c r="BA88" t="s">
+      <c r="BA88" s="39" t="s">
         <v>289</v>
       </c>
-      <c r="BB88" t="s">
+      <c r="BB88" s="39" t="s">
         <v>375</v>
       </c>
-      <c r="BC88">
-        <v>1</v>
-      </c>
-      <c r="BD88" t="s">
+      <c r="BC88" s="39">
+        <v>1</v>
+      </c>
+      <c r="BD88" s="39" t="s">
         <v>394</v>
       </c>
-      <c r="BE88" t="s">
+      <c r="BE88" s="39" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="89" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:57" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="39" t="s">
         <v>398</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="39" t="s">
         <v>409</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="39" t="s">
         <v>412</v>
       </c>
       <c r="E89" s="12" t="s">
@@ -16672,313 +16666,313 @@
       <c r="G89" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="H89" s="6">
-        <v>0</v>
-      </c>
-      <c r="I89">
-        <v>1</v>
-      </c>
-      <c r="J89" t="s">
+      <c r="H89" s="40">
+        <v>0</v>
+      </c>
+      <c r="I89" s="39">
+        <v>1</v>
+      </c>
+      <c r="J89" s="39" t="s">
         <v>400</v>
       </c>
-      <c r="K89">
-        <v>0</v>
-      </c>
-      <c r="L89" t="s">
-        <v>8</v>
-      </c>
-      <c r="M89" t="s">
-        <v>8</v>
-      </c>
-      <c r="N89" t="s">
-        <v>8</v>
-      </c>
-      <c r="O89" t="s">
-        <v>8</v>
-      </c>
-      <c r="P89" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q89" t="s">
-        <v>8</v>
-      </c>
-      <c r="R89" t="s">
+      <c r="K89" s="39">
+        <v>0</v>
+      </c>
+      <c r="L89" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M89" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="N89" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="O89" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="P89" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q89" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="R89" s="39" t="s">
         <v>8</v>
       </c>
       <c r="S89" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="T89" s="20">
-        <v>0</v>
-      </c>
-      <c r="U89" t="s">
+      <c r="T89" s="41">
+        <v>0</v>
+      </c>
+      <c r="U89" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="V89" t="s">
+      <c r="V89" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="W89" t="s">
-        <v>401</v>
-      </c>
-      <c r="X89" t="s">
-        <v>401</v>
-      </c>
-      <c r="Y89" t="s">
-        <v>401</v>
-      </c>
-      <c r="Z89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AA89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AB89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AC89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AD89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AE89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AF89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AG89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AH89" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="AI89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AJ89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AK89" t="s">
-        <v>401</v>
-      </c>
-      <c r="AL89" s="10" t="s">
+      <c r="W89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="X89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AB89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AD89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AF89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AH89" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AJ89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AK89" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AL89" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM89" t="s">
+      <c r="AM89" s="39" t="s">
         <v>402</v>
       </c>
-      <c r="AN89" t="s">
+      <c r="AN89" s="39" t="s">
         <v>402</v>
       </c>
-      <c r="AO89" s="20" t="s">
+      <c r="AO89" s="41" t="s">
         <v>402</v>
       </c>
-      <c r="AP89">
+      <c r="AP89" s="39">
         <v>64</v>
       </c>
-      <c r="AQ89">
+      <c r="AQ89" s="39">
         <v>128</v>
       </c>
-      <c r="AR89">
+      <c r="AR89" s="39">
         <v>128</v>
       </c>
       <c r="AS89" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT89">
+      <c r="AT89" s="39">
         <v>32</v>
       </c>
-      <c r="AU89">
+      <c r="AU89" s="39">
         <v>96</v>
       </c>
-      <c r="AV89">
+      <c r="AV89" s="39">
         <v>96</v>
       </c>
       <c r="AW89" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX89">
+      <c r="AX89" s="39">
         <f t="shared" ref="AX89" si="100">AP89-AT89</f>
         <v>32</v>
       </c>
-      <c r="AY89">
+      <c r="AY89" s="39">
         <f t="shared" ref="AY89" si="101">AQ89-AU89</f>
         <v>32</v>
       </c>
-      <c r="AZ89" s="10">
+      <c r="AZ89" s="42">
         <f t="shared" ref="AZ89" si="102">AR89-AV89</f>
         <v>32</v>
       </c>
-      <c r="BA89" t="s">
+      <c r="BA89" s="39" t="s">
         <v>374</v>
       </c>
-      <c r="BB89" t="s">
+      <c r="BB89" s="39" t="s">
         <v>379</v>
       </c>
-      <c r="BC89">
-        <v>1</v>
-      </c>
-      <c r="BD89" t="s">
+      <c r="BC89" s="39">
+        <v>1</v>
+      </c>
+      <c r="BD89" s="39" t="s">
         <v>394</v>
       </c>
-      <c r="BE89" t="s">
+      <c r="BE89" s="39" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="90" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="38" t="s">
+    <row r="90" spans="1:57" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="39" t="s">
         <v>404</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C90" s="39" t="s">
         <v>409</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" s="39" t="s">
         <v>412</v>
       </c>
-      <c r="E90" s="38" t="s">
+      <c r="E90" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="F90" s="38" t="s">
+      <c r="F90" s="12" t="s">
         <v>328</v>
       </c>
-      <c r="G90" s="38" t="s">
+      <c r="G90" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="H90" s="39">
-        <v>0</v>
-      </c>
-      <c r="I90" s="3">
-        <v>1</v>
-      </c>
-      <c r="J90" s="40" t="s">
+      <c r="H90" s="40">
+        <v>0</v>
+      </c>
+      <c r="I90" s="39">
+        <v>1</v>
+      </c>
+      <c r="J90" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="K90" s="3">
-        <v>0</v>
-      </c>
-      <c r="L90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R90" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="S90" s="38" t="s">
+      <c r="K90" s="39">
+        <v>0</v>
+      </c>
+      <c r="L90" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M90" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="N90" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="O90" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="P90" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q90" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="R90" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="S90" s="12" t="s">
         <v>8</v>
       </c>
       <c r="T90" s="41">
         <v>0</v>
       </c>
-      <c r="U90" s="3" t="s">
+      <c r="U90" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="V90" s="3" t="s">
+      <c r="V90" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="W90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="X90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="Y90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="Z90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AA90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AB90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AC90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AD90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AE90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AF90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AG90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AH90" s="39" t="s">
-        <v>401</v>
-      </c>
-      <c r="AI90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AJ90" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="AK90" s="3" t="s">
+      <c r="W90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="X90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AA90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AB90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AD90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AE90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AF90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AG90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AH90" s="40" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AJ90" s="39" t="s">
+        <v>401</v>
+      </c>
+      <c r="AK90" s="39" t="s">
         <v>401</v>
       </c>
       <c r="AL90" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM90" s="3" t="s">
+      <c r="AM90" s="39" t="s">
         <v>402</v>
       </c>
-      <c r="AN90" s="3" t="s">
+      <c r="AN90" s="39" t="s">
         <v>402</v>
       </c>
       <c r="AO90" s="41" t="s">
         <v>402</v>
       </c>
-      <c r="AP90" s="3">
+      <c r="AP90" s="39">
         <v>80</v>
       </c>
-      <c r="AQ90" s="3">
+      <c r="AQ90" s="39">
         <v>170</v>
       </c>
-      <c r="AR90" s="3">
+      <c r="AR90" s="39">
         <v>170</v>
       </c>
-      <c r="AS90" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT90" s="3">
+      <c r="AS90" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT90" s="39">
         <v>40</v>
       </c>
-      <c r="AU90" s="3">
+      <c r="AU90" s="39">
         <v>90</v>
       </c>
-      <c r="AV90" s="3">
+      <c r="AV90" s="39">
         <v>90</v>
       </c>
-      <c r="AW90" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX90" s="3">
+      <c r="AW90" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX90" s="39">
         <f t="shared" ref="AX90" si="103">AP90-AT90</f>
         <v>40</v>
       </c>
-      <c r="AY90" s="3">
+      <c r="AY90" s="39">
         <f t="shared" ref="AY90" si="104">AQ90-AU90</f>
         <v>80</v>
       </c>
@@ -16986,19 +16980,19 @@
         <f t="shared" ref="AZ90" si="105">AR90-AV90</f>
         <v>80</v>
       </c>
-      <c r="BA90" s="3" t="s">
+      <c r="BA90" s="39" t="s">
         <v>341</v>
       </c>
-      <c r="BB90" s="3" t="s">
+      <c r="BB90" s="39" t="s">
         <v>340</v>
       </c>
-      <c r="BC90" s="3">
-        <v>1</v>
-      </c>
-      <c r="BD90" s="3" t="s">
+      <c r="BC90" s="39">
+        <v>1</v>
+      </c>
+      <c r="BD90" s="39" t="s">
         <v>287</v>
       </c>
-      <c r="BE90" t="s">
+      <c r="BE90" s="39" t="s">
         <v>288</v>
       </c>
     </row>
@@ -17702,7 +17696,7 @@
       <c r="BD94" t="s">
         <v>427</v>
       </c>
-      <c r="BE94" s="43" t="s">
+      <c r="BE94" s="37" t="s">
         <v>288</v>
       </c>
     </row>
@@ -18054,7 +18048,7 @@
       <c r="BD96" t="s">
         <v>428</v>
       </c>
-      <c r="BE96" s="44" t="s">
+      <c r="BE96" t="s">
         <v>429</v>
       </c>
     </row>
@@ -18230,7 +18224,7 @@
       <c r="BD97" t="s">
         <v>427</v>
       </c>
-      <c r="BE97" s="44" t="s">
+      <c r="BE97" t="s">
         <v>288</v>
       </c>
     </row>
@@ -18543,16 +18537,16 @@
       <c r="AR99">
         <v>131</v>
       </c>
-      <c r="AS99" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT99" s="49">
+      <c r="AS99" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT99" s="38">
         <v>47</v>
       </c>
-      <c r="AU99" s="44">
+      <c r="AU99">
         <v>83</v>
       </c>
-      <c r="AV99" s="44">
+      <c r="AV99">
         <v>83</v>
       </c>
       <c r="AW99" s="25" t="s">
@@ -18586,162 +18580,162 @@
         <v>429</v>
       </c>
     </row>
-    <row r="100" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="38" t="s">
+    <row r="100" spans="1:57" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="39" t="s">
         <v>403</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="C100" s="39" t="s">
         <v>409</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="D100" s="39" t="s">
         <v>412</v>
       </c>
-      <c r="E100" s="38" t="s">
-        <v>445</v>
-      </c>
-      <c r="F100" s="38" t="s">
-        <v>451</v>
-      </c>
-      <c r="G100" s="38" t="s">
+      <c r="E100" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="G100" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="H100" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="I100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="K100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="L100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="M100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="O100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="P100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="R100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="S100" s="38" t="s">
+      <c r="H100" s="45">
+        <v>0</v>
+      </c>
+      <c r="I100" s="39">
+        <v>1</v>
+      </c>
+      <c r="J100" s="39" t="s">
+        <v>453</v>
+      </c>
+      <c r="K100" s="39">
+        <v>0</v>
+      </c>
+      <c r="L100" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="N100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="O100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="P100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="R100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="S100" s="12" t="s">
         <v>120</v>
       </c>
       <c r="T100" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="U100" s="3" t="s">
+      <c r="U100" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="V100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="W100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="X100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH100" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI100" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK100" s="3" t="s">
+      <c r="V100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="W100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="X100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH100" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI100" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ100" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK100" s="39" t="s">
         <v>281</v>
       </c>
       <c r="AL100" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM100" s="3">
+      <c r="AM100" s="39">
         <v>190</v>
       </c>
-      <c r="AN100" s="3">
+      <c r="AN100" s="39">
         <v>960</v>
       </c>
       <c r="AO100" s="41">
         <v>1370</v>
       </c>
-      <c r="AP100" s="3">
+      <c r="AP100" s="39">
         <v>128</v>
       </c>
-      <c r="AQ100" s="3">
+      <c r="AQ100" s="39">
         <v>512</v>
       </c>
-      <c r="AR100" s="3">
+      <c r="AR100" s="39">
         <v>512</v>
       </c>
-      <c r="AS100" s="47" t="s">
+      <c r="AS100" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AT100" s="50">
-        <f t="shared" ref="AT100:AT105" si="133" xml:space="preserve"> _xlfn.FLOOR.MATH((AM100 - AP100) / 2)</f>
+      <c r="AT100" s="43">
+        <f t="shared" ref="AT100:AT106" si="133" xml:space="preserve"> _xlfn.FLOOR.MATH((AM100 - AP100) / 2)</f>
         <v>31</v>
       </c>
-      <c r="AU100" s="48">
-        <f t="shared" ref="AU100:AU105" si="134" xml:space="preserve"> _xlfn.FLOOR.MATH((AN100 - AQ100) / 2)</f>
+      <c r="AU100" s="39">
+        <f t="shared" ref="AU100:AU106" si="134" xml:space="preserve"> _xlfn.FLOOR.MATH((AN100 - AQ100) / 2)</f>
         <v>224</v>
       </c>
-      <c r="AV100" s="48">
-        <f t="shared" ref="AV100:AV105" si="135" xml:space="preserve"> _xlfn.FLOOR.MATH((AO100 - AR100) / 2)</f>
+      <c r="AV100" s="39">
+        <f t="shared" ref="AV100:AV106" si="135" xml:space="preserve"> _xlfn.FLOOR.MATH((AO100 - AR100) / 2)</f>
         <v>429</v>
       </c>
-      <c r="AW100" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX100" s="3">
+      <c r="AW100" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX100" s="39">
         <f t="shared" ref="AX100:AX101" si="136">AP100-AT100</f>
         <v>97</v>
       </c>
-      <c r="AY100" s="3">
+      <c r="AY100" s="39">
         <f t="shared" ref="AY100:AY101" si="137">AQ100-AU100</f>
         <v>288</v>
       </c>
@@ -18749,536 +18743,536 @@
         <f t="shared" ref="AZ100:AZ101" si="138">AR100-AV100</f>
         <v>83</v>
       </c>
-      <c r="BA100" s="3" t="s">
+      <c r="BA100" s="39" t="s">
         <v>419</v>
       </c>
-      <c r="BB100" s="3" t="s">
+      <c r="BB100" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="BC100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD100" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE100" s="3" t="s">
-        <v>120</v>
+      <c r="BC100" s="39">
+        <v>1</v>
+      </c>
+      <c r="BD100" s="39" t="s">
+        <v>447</v>
+      </c>
+      <c r="BE100" s="39" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:57" s="39" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="B101" t="s">
+        <v>435</v>
+      </c>
+      <c r="B101" s="39" t="s">
         <v>403</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="39" t="s">
         <v>410</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="39" t="s">
         <v>412</v>
       </c>
       <c r="E101" s="12" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="F101" s="12" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="G101" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="H101" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I101" t="s">
-        <v>120</v>
-      </c>
-      <c r="J101" t="s">
-        <v>120</v>
-      </c>
-      <c r="K101" t="s">
-        <v>120</v>
-      </c>
-      <c r="L101" t="s">
-        <v>120</v>
-      </c>
-      <c r="M101" t="s">
-        <v>120</v>
-      </c>
-      <c r="N101" t="s">
-        <v>120</v>
-      </c>
-      <c r="O101" t="s">
-        <v>120</v>
-      </c>
-      <c r="P101" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>120</v>
-      </c>
-      <c r="R101" t="s">
+      <c r="H101" s="40">
+        <v>0</v>
+      </c>
+      <c r="I101" s="39">
+        <v>1</v>
+      </c>
+      <c r="J101" s="39" t="s">
+        <v>454</v>
+      </c>
+      <c r="K101" s="39">
+        <v>0</v>
+      </c>
+      <c r="L101" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="N101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="O101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="P101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="R101" s="39" t="s">
         <v>120</v>
       </c>
       <c r="S101" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="T101" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="U101" t="s">
+      <c r="T101" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="U101" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="V101" t="s">
-        <v>120</v>
-      </c>
-      <c r="W101" t="s">
-        <v>120</v>
-      </c>
-      <c r="X101" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y101" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH101" s="6" t="s">
+      <c r="V101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="W101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="X101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH101" s="40" t="s">
         <v>120</v>
       </c>
       <c r="AI101" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="AJ101" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK101" t="s">
+      <c r="AJ101" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK101" s="39" t="s">
         <v>281</v>
       </c>
-      <c r="AL101" s="10" t="s">
+      <c r="AL101" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM101" s="45">
+      <c r="AM101" s="39">
         <v>190</v>
       </c>
-      <c r="AN101" s="45">
+      <c r="AN101" s="39">
         <v>960</v>
       </c>
-      <c r="AO101" s="51">
+      <c r="AO101" s="41">
         <v>1370</v>
       </c>
-      <c r="AP101" s="45">
+      <c r="AP101" s="39">
         <v>128</v>
       </c>
-      <c r="AQ101" s="45">
+      <c r="AQ101" s="39">
         <v>512</v>
       </c>
-      <c r="AR101" s="45">
+      <c r="AR101" s="39">
         <v>512</v>
       </c>
-      <c r="AS101" s="46" t="s">
+      <c r="AS101" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AT101" s="49">
+      <c r="AT101" s="43">
         <f t="shared" si="133"/>
         <v>31</v>
       </c>
-      <c r="AU101" s="44">
+      <c r="AU101" s="39">
         <f t="shared" si="134"/>
         <v>224</v>
       </c>
-      <c r="AV101" s="44">
+      <c r="AV101" s="39">
         <f t="shared" si="135"/>
         <v>429</v>
       </c>
       <c r="AW101" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX101">
+        <v>48</v>
+      </c>
+      <c r="AX101" s="39">
         <f t="shared" si="136"/>
         <v>97</v>
       </c>
-      <c r="AY101">
+      <c r="AY101" s="39">
         <f t="shared" si="137"/>
         <v>288</v>
       </c>
-      <c r="AZ101" s="10">
+      <c r="AZ101" s="42">
         <f t="shared" si="138"/>
         <v>83</v>
       </c>
-      <c r="BA101" t="s">
+      <c r="BA101" s="39" t="s">
         <v>419</v>
       </c>
-      <c r="BB101" t="s">
+      <c r="BB101" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="BC101" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD101" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE101" t="s">
-        <v>120</v>
+      <c r="BC101" s="39">
+        <v>1</v>
+      </c>
+      <c r="BD101" s="39" t="s">
+        <v>448</v>
+      </c>
+      <c r="BE101" s="39" t="s">
+        <v>449</v>
       </c>
     </row>
-    <row r="102" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:57" s="39" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="B102" s="39" t="s">
+        <v>403</v>
+      </c>
+      <c r="C102" s="39" t="s">
+        <v>410</v>
+      </c>
+      <c r="D102" s="39" t="s">
+        <v>433</v>
+      </c>
+      <c r="E102" s="12" t="s">
         <v>441</v>
       </c>
-      <c r="B102" t="s">
-        <v>403</v>
-      </c>
-      <c r="C102" t="s">
-        <v>410</v>
-      </c>
-      <c r="D102" t="s">
-        <v>433</v>
-      </c>
-      <c r="E102" s="12" t="s">
+      <c r="F102" s="12" t="s">
         <v>446</v>
-      </c>
-      <c r="F102" s="12" t="s">
-        <v>451</v>
       </c>
       <c r="G102" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="H102" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I102" t="s">
-        <v>120</v>
-      </c>
-      <c r="J102" t="s">
-        <v>120</v>
-      </c>
-      <c r="K102" t="s">
-        <v>120</v>
-      </c>
-      <c r="L102" t="s">
-        <v>120</v>
-      </c>
-      <c r="M102" t="s">
-        <v>120</v>
-      </c>
-      <c r="N102" t="s">
-        <v>120</v>
-      </c>
-      <c r="O102" t="s">
-        <v>120</v>
-      </c>
-      <c r="P102" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q102" t="s">
-        <v>120</v>
-      </c>
-      <c r="R102" t="s">
+      <c r="H102" s="40">
+        <v>0</v>
+      </c>
+      <c r="I102" s="39">
+        <v>1</v>
+      </c>
+      <c r="J102" s="39" t="s">
+        <v>454</v>
+      </c>
+      <c r="K102" s="39">
+        <v>0</v>
+      </c>
+      <c r="L102" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="N102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="O102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="P102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="R102" s="39" t="s">
         <v>120</v>
       </c>
       <c r="S102" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="T102" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="U102" t="s">
+      <c r="T102" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="U102" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="V102" t="s">
-        <v>120</v>
-      </c>
-      <c r="W102" t="s">
-        <v>120</v>
-      </c>
-      <c r="X102" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y102" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH102" s="6" t="s">
+      <c r="V102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="W102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="X102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH102" s="40" t="s">
         <v>120</v>
       </c>
       <c r="AI102" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="AJ102" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK102" t="s">
+      <c r="AJ102" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK102" s="39" t="s">
         <v>281</v>
       </c>
-      <c r="AL102" s="10" t="s">
+      <c r="AL102" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM102" s="45">
+      <c r="AM102" s="39">
         <v>190</v>
       </c>
-      <c r="AN102" s="45">
+      <c r="AN102" s="39">
         <v>960</v>
       </c>
-      <c r="AO102" s="51">
+      <c r="AO102" s="41">
         <v>1370</v>
       </c>
-      <c r="AP102" s="45">
+      <c r="AP102" s="39">
         <v>128</v>
       </c>
-      <c r="AQ102" s="45">
+      <c r="AQ102" s="39">
         <v>512</v>
       </c>
-      <c r="AR102" s="45">
+      <c r="AR102" s="39">
         <v>512</v>
       </c>
-      <c r="AS102" s="46" t="s">
+      <c r="AS102" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AT102" s="49">
+      <c r="AT102" s="43">
         <f t="shared" si="133"/>
         <v>31</v>
       </c>
-      <c r="AU102" s="44">
+      <c r="AU102" s="39">
         <f t="shared" si="134"/>
         <v>224</v>
       </c>
-      <c r="AV102" s="44">
+      <c r="AV102" s="39">
         <f t="shared" si="135"/>
         <v>429</v>
       </c>
       <c r="AW102" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX102">
+        <v>48</v>
+      </c>
+      <c r="AX102" s="39">
         <f t="shared" ref="AX102" si="139">AP102-AT102</f>
         <v>97</v>
       </c>
-      <c r="AY102">
+      <c r="AY102" s="39">
         <f t="shared" ref="AY102" si="140">AQ102-AU102</f>
         <v>288</v>
       </c>
-      <c r="AZ102" s="10">
+      <c r="AZ102" s="42">
         <f t="shared" ref="AZ102" si="141">AR102-AV102</f>
         <v>83</v>
       </c>
-      <c r="BA102" t="s">
+      <c r="BA102" s="39" t="s">
         <v>419</v>
       </c>
-      <c r="BB102" t="s">
+      <c r="BB102" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="BC102" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD102" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE102" t="s">
-        <v>120</v>
+      <c r="BC102" s="39">
+        <v>1</v>
+      </c>
+      <c r="BD102" s="39" t="s">
+        <v>448</v>
+      </c>
+      <c r="BE102" s="44" t="s">
+        <v>450</v>
       </c>
     </row>
-    <row r="103" spans="1:57" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="38" t="s">
+    <row r="103" spans="1:57" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="B103" s="39" t="s">
+        <v>403</v>
+      </c>
+      <c r="C103" s="39" t="s">
+        <v>409</v>
+      </c>
+      <c r="D103" s="39" t="s">
+        <v>412</v>
+      </c>
+      <c r="E103" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="B103" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="D103" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="E103" s="38" t="s">
-        <v>447</v>
-      </c>
-      <c r="F103" s="38" t="s">
-        <v>451</v>
-      </c>
-      <c r="G103" s="38" t="s">
+      <c r="F103" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="G103" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="H103" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="I103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="K103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="L103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="M103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="N103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="O103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="P103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="R103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="S103" s="38" t="s">
+      <c r="H103" s="40">
+        <v>1</v>
+      </c>
+      <c r="I103" s="39">
+        <v>0</v>
+      </c>
+      <c r="J103" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="K103" s="39">
+        <v>0</v>
+      </c>
+      <c r="L103" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="M103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="N103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="O103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="P103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="R103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="S103" s="12" t="s">
         <v>120</v>
       </c>
       <c r="T103" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="U103" s="3" t="s">
+      <c r="U103" s="39" t="s">
         <v>271</v>
       </c>
-      <c r="V103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="W103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="X103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH103" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI103" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK103" s="3" t="s">
+      <c r="V103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="W103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="X103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH103" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI103" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ103" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK103" s="39" t="s">
         <v>281</v>
       </c>
       <c r="AL103" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="AM103" s="3">
+      <c r="AM103" s="39">
         <v>125</v>
       </c>
-      <c r="AN103" s="3">
+      <c r="AN103" s="39">
         <v>1169</v>
       </c>
       <c r="AO103" s="41">
         <v>414</v>
       </c>
-      <c r="AP103" s="3">
+      <c r="AP103" s="39">
         <v>96</v>
       </c>
-      <c r="AQ103" s="3">
+      <c r="AQ103" s="39">
         <v>960</v>
       </c>
-      <c r="AR103" s="3">
+      <c r="AR103" s="39">
         <v>256</v>
       </c>
-      <c r="AS103" s="47" t="s">
+      <c r="AS103" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AT103" s="50">
+      <c r="AT103" s="43">
         <f t="shared" si="133"/>
         <v>14</v>
       </c>
-      <c r="AU103" s="48">
+      <c r="AU103" s="39">
         <f t="shared" si="134"/>
         <v>104</v>
       </c>
-      <c r="AV103" s="48">
+      <c r="AV103" s="39">
         <f t="shared" si="135"/>
         <v>79</v>
       </c>
-      <c r="AW103" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX103" s="3">
+      <c r="AW103" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX103" s="39">
         <f t="shared" ref="AX103" si="142">AP103-AT103</f>
         <v>82</v>
       </c>
-      <c r="AY103" s="3">
+      <c r="AY103" s="39">
         <f t="shared" ref="AY103" si="143">AQ103-AU103</f>
         <v>856</v>
       </c>
@@ -19286,25 +19280,25 @@
         <f t="shared" ref="AZ103" si="144">AR103-AV103</f>
         <v>177</v>
       </c>
-      <c r="BA103" s="3" t="s">
+      <c r="BA103" s="39" t="s">
         <v>419</v>
       </c>
-      <c r="BB103" s="3" t="s">
+      <c r="BB103" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="BC103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD103" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE103" s="3" t="s">
-        <v>120</v>
+      <c r="BC103" s="39">
+        <v>0</v>
+      </c>
+      <c r="BD103" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="BE103" s="39" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:57" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B104" t="s">
         <v>403</v>
@@ -19316,28 +19310,28 @@
         <v>412</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="F104" s="12" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="G104" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="H104" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I104" t="s">
-        <v>120</v>
+      <c r="H104" s="6">
+        <v>0</v>
+      </c>
+      <c r="I104">
+        <v>1</v>
       </c>
       <c r="J104" t="s">
-        <v>120</v>
-      </c>
-      <c r="K104" t="s">
-        <v>120</v>
-      </c>
-      <c r="L104" t="s">
-        <v>120</v>
+        <v>453</v>
+      </c>
+      <c r="K104" s="39">
+        <v>0</v>
+      </c>
+      <c r="L104" s="39" t="s">
+        <v>8</v>
       </c>
       <c r="M104" t="s">
         <v>120</v>
@@ -19426,32 +19420,32 @@
       <c r="AO104" s="20">
         <v>414</v>
       </c>
-      <c r="AP104" s="45">
+      <c r="AP104">
         <v>96</v>
       </c>
-      <c r="AQ104" s="45">
+      <c r="AQ104">
         <v>960</v>
       </c>
-      <c r="AR104" s="45">
+      <c r="AR104">
         <v>256</v>
       </c>
-      <c r="AS104" s="46" t="s">
+      <c r="AS104" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AT104" s="49">
+      <c r="AT104" s="38">
         <f t="shared" si="133"/>
         <v>14</v>
       </c>
-      <c r="AU104" s="44">
+      <c r="AU104">
         <f t="shared" si="134"/>
         <v>104</v>
       </c>
-      <c r="AV104" s="44">
+      <c r="AV104">
         <f t="shared" si="135"/>
         <v>79</v>
       </c>
       <c r="AW104" s="25" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="AX104">
         <f t="shared" ref="AX104" si="145">AP104-AT104</f>
@@ -19471,19 +19465,19 @@
       <c r="BB104" t="s">
         <v>163</v>
       </c>
-      <c r="BC104" t="s">
-        <v>120</v>
+      <c r="BC104">
+        <v>1</v>
       </c>
       <c r="BD104" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE104" t="s">
-        <v>120</v>
+        <v>451</v>
+      </c>
+      <c r="BE104" s="2" t="s">
+        <v>452</v>
       </c>
     </row>
-    <row r="105" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:57" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B105" t="s">
         <v>403</v>
@@ -19495,28 +19489,28 @@
         <v>433</v>
       </c>
       <c r="E105" s="12" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="F105" s="12" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="G105" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="H105" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I105" t="s">
-        <v>120</v>
+      <c r="H105" s="6">
+        <v>0</v>
+      </c>
+      <c r="I105">
+        <v>1</v>
       </c>
       <c r="J105" t="s">
-        <v>120</v>
-      </c>
-      <c r="K105" t="s">
-        <v>120</v>
-      </c>
-      <c r="L105" t="s">
-        <v>120</v>
+        <v>453</v>
+      </c>
+      <c r="K105" s="39">
+        <v>0</v>
+      </c>
+      <c r="L105" s="39" t="s">
+        <v>8</v>
       </c>
       <c r="M105" t="s">
         <v>120</v>
@@ -19605,32 +19599,32 @@
       <c r="AO105" s="20">
         <v>414</v>
       </c>
-      <c r="AP105" s="45">
+      <c r="AP105">
         <v>96</v>
       </c>
-      <c r="AQ105" s="45">
+      <c r="AQ105">
         <v>960</v>
       </c>
-      <c r="AR105" s="45">
+      <c r="AR105">
         <v>256</v>
       </c>
-      <c r="AS105" s="46" t="s">
+      <c r="AS105" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AT105" s="49">
+      <c r="AT105" s="38">
         <f t="shared" si="133"/>
         <v>14</v>
       </c>
-      <c r="AU105" s="44">
+      <c r="AU105">
         <f t="shared" si="134"/>
         <v>104</v>
       </c>
-      <c r="AV105" s="44">
+      <c r="AV105">
         <f t="shared" si="135"/>
         <v>79</v>
       </c>
       <c r="AW105" s="25" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="AX105">
         <f t="shared" ref="AX105" si="148">AP105-AT105</f>
@@ -19650,27 +19644,27 @@
       <c r="BB105" t="s">
         <v>163</v>
       </c>
-      <c r="BC105" t="s">
-        <v>120</v>
+      <c r="BC105">
+        <v>1</v>
       </c>
       <c r="BD105" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE105" t="s">
-        <v>120</v>
+        <v>451</v>
+      </c>
+      <c r="BE105" s="2" t="s">
+        <v>452</v>
       </c>
     </row>
-    <row r="106" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A106" s="12" t="s">
         <v>434</v>
       </c>
-      <c r="B106" s="45" t="s">
+      <c r="B106" t="s">
         <v>404</v>
       </c>
-      <c r="C106" s="45" t="s">
+      <c r="C106" t="s">
         <v>409</v>
       </c>
-      <c r="D106" s="45" t="s">
+      <c r="D106" t="s">
         <v>412</v>
       </c>
       <c r="E106" s="12" t="s">
@@ -19682,172 +19676,175 @@
       <c r="G106" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="H106" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="I106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="J106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="K106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="L106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="M106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="N106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="O106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="P106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="R106" s="45" t="s">
+      <c r="H106" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I106" t="s">
+        <v>120</v>
+      </c>
+      <c r="J106" t="s">
+        <v>120</v>
+      </c>
+      <c r="K106" t="s">
+        <v>120</v>
+      </c>
+      <c r="L106" t="s">
+        <v>120</v>
+      </c>
+      <c r="M106" t="s">
+        <v>120</v>
+      </c>
+      <c r="N106" t="s">
+        <v>120</v>
+      </c>
+      <c r="O106" t="s">
+        <v>120</v>
+      </c>
+      <c r="P106" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>120</v>
+      </c>
+      <c r="R106" t="s">
         <v>120</v>
       </c>
       <c r="S106" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="T106" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="U106" s="45" t="s">
+      <c r="T106" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U106" t="s">
         <v>344</v>
       </c>
-      <c r="V106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="W106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="X106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH106" s="52" t="s">
+      <c r="V106" t="s">
+        <v>120</v>
+      </c>
+      <c r="W106" t="s">
+        <v>120</v>
+      </c>
+      <c r="X106" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y106" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z106" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA106" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB106" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC106" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD106" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE106" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF106" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG106" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH106" s="6" t="s">
         <v>120</v>
       </c>
       <c r="AI106" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="AJ106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK106" s="45" t="s">
+      <c r="AJ106" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK106" t="s">
         <v>281</v>
       </c>
-      <c r="AL106" s="53" t="s">
+      <c r="AL106" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM106" s="45">
-        <v>190</v>
-      </c>
-      <c r="AN106" s="45">
+      <c r="AM106">
+        <v>125</v>
+      </c>
+      <c r="AN106">
+        <v>1169</v>
+      </c>
+      <c r="AO106" s="20">
+        <v>414</v>
+      </c>
+      <c r="AP106">
+        <v>96</v>
+      </c>
+      <c r="AQ106">
         <v>960</v>
       </c>
-      <c r="AO106" s="51">
-        <v>1370</v>
-      </c>
-      <c r="AP106" s="45">
-        <v>128</v>
-      </c>
-      <c r="AQ106" s="45">
-        <v>512</v>
-      </c>
-      <c r="AR106" s="45">
-        <v>512</v>
-      </c>
-      <c r="AS106" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT106" s="54">
-        <v>64</v>
-      </c>
-      <c r="AU106" s="55">
-        <v>96</v>
-      </c>
-      <c r="AV106" s="55">
-        <v>96</v>
+      <c r="AR106">
+        <v>256</v>
+      </c>
+      <c r="AS106" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT106" s="38">
+        <f t="shared" si="133"/>
+        <v>14</v>
+      </c>
+      <c r="AU106">
+        <f t="shared" si="134"/>
+        <v>104</v>
+      </c>
+      <c r="AV106">
+        <f t="shared" si="135"/>
+        <v>79</v>
       </c>
       <c r="AW106" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX106" s="45">
+      <c r="AX106">
         <f t="shared" ref="AX106" si="151">AP106-AT106</f>
-        <v>64</v>
-      </c>
-      <c r="AY106" s="45">
+        <v>82</v>
+      </c>
+      <c r="AY106">
         <f t="shared" ref="AY106" si="152">AQ106-AU106</f>
-        <v>416</v>
-      </c>
-      <c r="AZ106" s="53">
+        <v>856</v>
+      </c>
+      <c r="AZ106" s="10">
         <f t="shared" ref="AZ106" si="153">AR106-AV106</f>
-        <v>416</v>
-      </c>
-      <c r="BA106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD106" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE106" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="BA106" t="s">
+        <v>455</v>
+      </c>
+      <c r="BB106" t="s">
+        <v>456</v>
+      </c>
+      <c r="BC106" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD106" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE106" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
-        <v>435</v>
-      </c>
-      <c r="B107" s="45" t="s">
-        <v>404</v>
-      </c>
-      <c r="C107" s="45" t="s">
-        <v>410</v>
-      </c>
-      <c r="D107" s="45" t="s">
-        <v>412</v>
+        <v>120</v>
+      </c>
+      <c r="B107" t="s">
+        <v>120</v>
+      </c>
+      <c r="C107" t="s">
+        <v>120</v>
+      </c>
+      <c r="D107" t="s">
+        <v>120</v>
       </c>
       <c r="E107" s="12" t="s">
         <v>120</v>
@@ -19856,1041 +19853,201 @@
         <v>120</v>
       </c>
       <c r="G107" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="H107" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="I107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="J107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="K107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="L107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="M107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="N107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="O107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="P107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="R107" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="H107" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I107" t="s">
+        <v>120</v>
+      </c>
+      <c r="J107" t="s">
+        <v>120</v>
+      </c>
+      <c r="K107" t="s">
+        <v>120</v>
+      </c>
+      <c r="L107" t="s">
+        <v>120</v>
+      </c>
+      <c r="M107" t="s">
+        <v>120</v>
+      </c>
+      <c r="N107" t="s">
+        <v>120</v>
+      </c>
+      <c r="O107" t="s">
+        <v>120</v>
+      </c>
+      <c r="P107" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>120</v>
+      </c>
+      <c r="R107" t="s">
         <v>120</v>
       </c>
       <c r="S107" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="T107" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="U107" s="45" t="s">
-        <v>344</v>
-      </c>
-      <c r="V107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="W107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="X107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH107" s="52" t="s">
+      <c r="T107" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U107" t="s">
+        <v>120</v>
+      </c>
+      <c r="V107" t="s">
+        <v>120</v>
+      </c>
+      <c r="W107" t="s">
+        <v>120</v>
+      </c>
+      <c r="X107" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y107" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH107" s="6" t="s">
         <v>120</v>
       </c>
       <c r="AI107" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="AJ107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK107" s="45" t="s">
+      <c r="AJ107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK107" t="s">
         <v>281</v>
       </c>
-      <c r="AL107" s="53" t="s">
+      <c r="AL107" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM107" s="45">
-        <v>190</v>
-      </c>
-      <c r="AN107" s="45">
-        <v>960</v>
-      </c>
-      <c r="AO107" s="51">
-        <v>1370</v>
-      </c>
-      <c r="AP107" s="45">
-        <v>128</v>
-      </c>
-      <c r="AQ107" s="45">
-        <v>512</v>
-      </c>
-      <c r="AR107" s="45">
-        <v>512</v>
+      <c r="AM107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO107" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR107" t="s">
+        <v>120</v>
       </c>
       <c r="AS107" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT107" s="45">
-        <v>64</v>
-      </c>
-      <c r="AU107" s="45">
-        <v>96</v>
-      </c>
-      <c r="AV107" s="45">
-        <v>96</v>
+      <c r="AT107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU107" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV107" t="s">
+        <v>120</v>
       </c>
       <c r="AW107" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX107" s="45">
+      <c r="AX107" t="e">
         <f t="shared" ref="AX107" si="154">AP107-AT107</f>
-        <v>64</v>
-      </c>
-      <c r="AY107" s="45">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY107" t="e">
         <f t="shared" ref="AY107" si="155">AQ107-AU107</f>
-        <v>416</v>
-      </c>
-      <c r="AZ107" s="53">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ107" s="10" t="e">
         <f t="shared" ref="AZ107" si="156">AR107-AV107</f>
-        <v>416</v>
-      </c>
-      <c r="BA107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD107" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE107" s="45" t="s">
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA107" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB107" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC107" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD107" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE107" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="108" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="12" t="s">
-        <v>436</v>
-      </c>
-      <c r="B108" s="45" t="s">
-        <v>404</v>
-      </c>
-      <c r="C108" s="45" t="s">
-        <v>410</v>
-      </c>
-      <c r="D108" s="45" t="s">
-        <v>433</v>
-      </c>
-      <c r="E108" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F108" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G108" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="H108" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="I108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="J108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="K108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="L108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="M108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="N108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="O108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="P108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="R108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="S108" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="T108" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="U108" s="45" t="s">
-        <v>344</v>
-      </c>
-      <c r="V108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="W108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="X108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH108" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI108" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK108" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL108" s="53" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM108" s="45">
-        <v>190</v>
-      </c>
-      <c r="AN108" s="45">
-        <v>960</v>
-      </c>
-      <c r="AO108" s="51">
-        <v>1370</v>
-      </c>
-      <c r="AP108" s="45">
-        <v>128</v>
-      </c>
-      <c r="AQ108" s="45">
-        <v>512</v>
-      </c>
-      <c r="AR108" s="45">
-        <v>512</v>
-      </c>
-      <c r="AS108" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT108" s="45">
-        <v>64</v>
-      </c>
-      <c r="AU108" s="45">
-        <v>96</v>
-      </c>
-      <c r="AV108" s="45">
-        <v>96</v>
-      </c>
-      <c r="AW108" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX108" s="45">
-        <f t="shared" ref="AX108" si="157">AP108-AT108</f>
-        <v>64</v>
-      </c>
-      <c r="AY108" s="45">
-        <f t="shared" ref="AY108" si="158">AQ108-AU108</f>
-        <v>416</v>
-      </c>
-      <c r="AZ108" s="53">
-        <f t="shared" ref="AZ108" si="159">AR108-AV108</f>
-        <v>416</v>
-      </c>
-      <c r="BA108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD108" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE108" s="45" t="s">
-        <v>120</v>
-      </c>
+    <row r="108" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A108" s="12"/>
+      <c r="E108" s="12"/>
+      <c r="F108" s="12"/>
+      <c r="G108" s="12"/>
+      <c r="S108" s="12"/>
+      <c r="AI108" s="12"/>
+      <c r="AS108" s="25"/>
+      <c r="AW108" s="25"/>
     </row>
-    <row r="109" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="12" t="s">
-        <v>437</v>
-      </c>
-      <c r="B109" s="45" t="s">
-        <v>404</v>
-      </c>
-      <c r="C109" s="45" t="s">
-        <v>409</v>
-      </c>
-      <c r="D109" s="45" t="s">
-        <v>412</v>
-      </c>
-      <c r="E109" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F109" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G109" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="H109" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="I109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="J109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="K109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="L109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="M109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="N109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="O109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="P109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="R109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="S109" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="T109" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="U109" s="45" t="s">
-        <v>271</v>
-      </c>
-      <c r="V109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="W109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="X109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH109" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI109" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK109" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL109" s="53" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM109" s="45">
-        <v>125</v>
-      </c>
-      <c r="AN109" s="45">
-        <v>1169</v>
-      </c>
-      <c r="AO109" s="51">
-        <v>414</v>
-      </c>
-      <c r="AP109" s="45">
-        <v>96</v>
-      </c>
-      <c r="AQ109" s="45">
-        <v>128</v>
-      </c>
-      <c r="AR109" s="45">
-        <v>128</v>
-      </c>
-      <c r="AS109" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT109" s="45">
-        <v>64</v>
-      </c>
-      <c r="AU109" s="45">
-        <v>96</v>
-      </c>
-      <c r="AV109" s="45">
-        <v>96</v>
-      </c>
-      <c r="AW109" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX109" s="45">
-        <f t="shared" ref="AX109" si="160">AP109-AT109</f>
-        <v>32</v>
-      </c>
-      <c r="AY109" s="45">
-        <f t="shared" ref="AY109" si="161">AQ109-AU109</f>
-        <v>32</v>
-      </c>
-      <c r="AZ109" s="53">
-        <f t="shared" ref="AZ109" si="162">AR109-AV109</f>
-        <v>32</v>
-      </c>
-      <c r="BA109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD109" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE109" s="45" t="s">
-        <v>120</v>
-      </c>
+    <row r="109" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A109" s="12"/>
+      <c r="E109" s="12"/>
+      <c r="F109" s="12"/>
+      <c r="G109" s="12"/>
+      <c r="S109" s="12"/>
+      <c r="AI109" s="12"/>
+      <c r="AS109" s="25"/>
+      <c r="AW109" s="25"/>
     </row>
-    <row r="110" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="12" t="s">
-        <v>438</v>
-      </c>
-      <c r="B110" s="45" t="s">
-        <v>404</v>
-      </c>
-      <c r="C110" s="45" t="s">
-        <v>410</v>
-      </c>
-      <c r="D110" s="45" t="s">
-        <v>412</v>
-      </c>
-      <c r="E110" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F110" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G110" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="H110" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="I110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="J110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="K110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="L110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="M110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="N110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="O110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="P110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="R110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="S110" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="T110" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="U110" s="45" t="s">
-        <v>271</v>
-      </c>
-      <c r="V110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="W110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="X110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH110" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI110" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK110" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL110" s="53" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM110" s="45">
-        <v>125</v>
-      </c>
-      <c r="AN110" s="45">
-        <v>1169</v>
-      </c>
-      <c r="AO110" s="51">
-        <v>414</v>
-      </c>
-      <c r="AP110" s="45">
-        <v>96</v>
-      </c>
-      <c r="AQ110" s="45">
-        <v>128</v>
-      </c>
-      <c r="AR110" s="45">
-        <v>128</v>
-      </c>
-      <c r="AS110" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT110" s="45">
-        <v>64</v>
-      </c>
-      <c r="AU110" s="45">
-        <v>96</v>
-      </c>
-      <c r="AV110" s="45">
-        <v>96</v>
-      </c>
-      <c r="AW110" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX110" s="45">
-        <f t="shared" ref="AX110" si="163">AP110-AT110</f>
-        <v>32</v>
-      </c>
-      <c r="AY110" s="45">
-        <f t="shared" ref="AY110" si="164">AQ110-AU110</f>
-        <v>32</v>
-      </c>
-      <c r="AZ110" s="53">
-        <f t="shared" ref="AZ110" si="165">AR110-AV110</f>
-        <v>32</v>
-      </c>
-      <c r="BA110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD110" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE110" s="45" t="s">
-        <v>120</v>
-      </c>
+    <row r="110" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A110" s="12"/>
+      <c r="E110" s="12"/>
+      <c r="F110" s="12"/>
+      <c r="G110" s="12"/>
+      <c r="S110" s="12"/>
+      <c r="AI110" s="12"/>
+      <c r="AS110" s="25"/>
+      <c r="AW110" s="25"/>
     </row>
-    <row r="111" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="B111" s="45" t="s">
-        <v>404</v>
-      </c>
-      <c r="C111" s="45" t="s">
-        <v>410</v>
-      </c>
-      <c r="D111" s="45" t="s">
-        <v>433</v>
-      </c>
-      <c r="E111" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F111" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G111" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="H111" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="I111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="J111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="K111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="L111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="M111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="N111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="O111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="P111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="R111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="S111" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="T111" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="U111" s="45" t="s">
-        <v>271</v>
-      </c>
-      <c r="V111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="W111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="X111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH111" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI111" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK111" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL111" s="53" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM111" s="45">
-        <v>125</v>
-      </c>
-      <c r="AN111" s="45">
-        <v>1169</v>
-      </c>
-      <c r="AO111" s="51">
-        <v>414</v>
-      </c>
-      <c r="AP111" s="45">
-        <v>96</v>
-      </c>
-      <c r="AQ111" s="45">
-        <v>128</v>
-      </c>
-      <c r="AR111" s="45">
-        <v>128</v>
-      </c>
-      <c r="AS111" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT111" s="45">
-        <v>64</v>
-      </c>
-      <c r="AU111" s="45">
-        <v>96</v>
-      </c>
-      <c r="AV111" s="45">
-        <v>96</v>
-      </c>
-      <c r="AW111" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX111" s="45">
-        <f t="shared" ref="AX111" si="166">AP111-AT111</f>
-        <v>32</v>
-      </c>
-      <c r="AY111" s="45">
-        <f t="shared" ref="AY111" si="167">AQ111-AU111</f>
-        <v>32</v>
-      </c>
-      <c r="AZ111" s="53">
-        <f t="shared" ref="AZ111" si="168">AR111-AV111</f>
-        <v>32</v>
-      </c>
-      <c r="BA111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD111" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE111" s="45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="112" spans="1:57" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="C112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="D112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="E112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="F112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="H112" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="I112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="J112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="K112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="L112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="M112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="N112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="O112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="P112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="R112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="S112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="T112" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="U112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="V112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="W112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="X112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH112" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK112" s="45" t="s">
-        <v>281</v>
-      </c>
-      <c r="AL112" s="53" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO112" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS112" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="AW112" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX112" s="45" t="e">
-        <f t="shared" ref="AX112" si="169">AP112-AT112</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY112" s="45" t="e">
-        <f t="shared" ref="AY112" si="170">AQ112-AU112</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ112" s="53" t="e">
-        <f t="shared" ref="AZ112" si="171">AR112-AV112</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD112" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE112" s="45" t="s">
-        <v>120</v>
-      </c>
+    <row r="111" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="12"/>
+      <c r="S111" s="12"/>
+      <c r="AI111" s="12"/>
+      <c r="AS111" s="25"/>
+      <c r="AW111" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
prepare predict3dunet1.6.0 chpt-231215-0, train3dunet1.8.2 chpt-231225-1
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AC00C1-F764-4328-8361-FF4C1686F3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3046C14F-20D0-4EED-B8EC-0709FB934865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3232" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3319" uniqueCount="469">
   <si>
     <t>patch z</t>
   </si>
@@ -1417,6 +1417,36 @@
   <si>
     <t xml:space="preserve">  File "/home/dwalth/data/conda/envs/3dunet/lib/python3.11/site-packages/torch/nn/modules/conv.py", line 662, in _output_padding
     raise ValueError((</t>
+  </si>
+  <si>
+    <t>231225-0</t>
+  </si>
+  <si>
+    <t>train3dunet 1.8.2</t>
+  </si>
+  <si>
+    <t>Try out the new pytorch-3dunet 1.8.2 which has the ability of taking an arbitrary patch shape for ResidualUNet3D models. Maybe now predict3dunet works. Same patch as in most recent attempt.</t>
+  </si>
+  <si>
+    <t>stride = floor (resolution - patch) / 2; for validation: stride = patch (like in Wolny's config.yml)</t>
+  </si>
+  <si>
+    <t>231225-1</t>
+  </si>
+  <si>
+    <t>Attempt predict3dunet with same patch &amp; stride as during training.</t>
+  </si>
+  <si>
+    <t>Fail. Patch shape invalid error.</t>
+  </si>
+  <si>
+    <t>Success (no error)</t>
+  </si>
+  <si>
+    <t>Attempt predict3dunet with same patch as during training, but stride shape such that there is a halo of 32 voxels in all dimensions.</t>
+  </si>
+  <si>
+    <t>stride = such that the halo is 32 in all dimensions.</t>
   </si>
 </sst>
 </file>
@@ -2029,8 +2059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BE111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BC106" sqref="BC106"/>
+    <sheetView tabSelected="1" topLeftCell="AK83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AT108" sqref="AT108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -2077,7 +2107,7 @@
     <col min="50" max="51" width="6" customWidth="1"/>
     <col min="52" max="52" width="6" style="10" customWidth="1"/>
     <col min="53" max="53" width="74.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="74.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="76.33203125" customWidth="1" outlineLevel="1"/>
     <col min="55" max="55" width="5.109375" customWidth="1"/>
     <col min="56" max="56" width="135.33203125" customWidth="1" outlineLevel="1"/>
     <col min="57" max="57" width="206" customWidth="1" outlineLevel="1"/>
@@ -19667,28 +19697,28 @@
         <v>412</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>120</v>
+        <v>464</v>
       </c>
       <c r="F106" s="12" t="s">
-        <v>120</v>
+        <v>466</v>
       </c>
       <c r="G106" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="H106" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I106" t="s">
-        <v>120</v>
+        <v>465</v>
+      </c>
+      <c r="H106" s="6">
+        <v>0</v>
+      </c>
+      <c r="I106">
+        <v>1</v>
       </c>
       <c r="J106" t="s">
-        <v>120</v>
-      </c>
-      <c r="K106" t="s">
-        <v>120</v>
+        <v>297</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
       </c>
       <c r="L106" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="M106" t="s">
         <v>120</v>
@@ -19805,15 +19835,15 @@
         <v>8</v>
       </c>
       <c r="AX106">
-        <f t="shared" ref="AX106" si="151">AP106-AT106</f>
+        <f t="shared" ref="AX106:AX107" si="151">AP106-AT106</f>
         <v>82</v>
       </c>
       <c r="AY106">
-        <f t="shared" ref="AY106" si="152">AQ106-AU106</f>
+        <f t="shared" ref="AY106:AY107" si="152">AQ106-AU106</f>
         <v>856</v>
       </c>
       <c r="AZ106" s="10">
-        <f t="shared" ref="AZ106" si="153">AR106-AV106</f>
+        <f t="shared" ref="AZ106:AZ107" si="153">AR106-AV106</f>
         <v>177</v>
       </c>
       <c r="BA106" t="s">
@@ -19834,22 +19864,22 @@
     </row>
     <row r="107" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
-        <v>120</v>
+        <v>459</v>
       </c>
       <c r="B107" t="s">
-        <v>120</v>
+        <v>404</v>
       </c>
       <c r="C107" t="s">
-        <v>120</v>
+        <v>409</v>
       </c>
       <c r="D107" t="s">
-        <v>120</v>
+        <v>412</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>120</v>
+        <v>467</v>
       </c>
       <c r="F107" s="12" t="s">
-        <v>120</v>
+        <v>466</v>
       </c>
       <c r="G107" s="12" t="s">
         <v>120</v>
@@ -19947,56 +19977,56 @@
       <c r="AL107" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM107" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN107" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO107" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP107" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ107" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR107" t="s">
-        <v>120</v>
+      <c r="AM107">
+        <v>125</v>
+      </c>
+      <c r="AN107">
+        <v>1169</v>
+      </c>
+      <c r="AO107" s="20">
+        <v>414</v>
+      </c>
+      <c r="AP107">
+        <v>96</v>
+      </c>
+      <c r="AQ107">
+        <v>960</v>
+      </c>
+      <c r="AR107">
+        <v>256</v>
       </c>
       <c r="AS107" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT107" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU107" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV107" t="s">
-        <v>120</v>
+      <c r="AT107">
+        <v>64</v>
+      </c>
+      <c r="AU107">
+        <v>928</v>
+      </c>
+      <c r="AV107">
+        <v>224</v>
       </c>
       <c r="AW107" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX107" t="e">
-        <f t="shared" ref="AX107" si="154">AP107-AT107</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AY107" t="e">
-        <f t="shared" ref="AY107" si="155">AQ107-AU107</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ107" s="10" t="e">
-        <f t="shared" ref="AZ107" si="156">AR107-AV107</f>
-        <v>#VALUE!</v>
+      <c r="AX107">
+        <f t="shared" si="151"/>
+        <v>32</v>
+      </c>
+      <c r="AY107">
+        <f t="shared" si="152"/>
+        <v>32</v>
+      </c>
+      <c r="AZ107" s="10">
+        <f t="shared" si="153"/>
+        <v>32</v>
       </c>
       <c r="BA107" t="s">
-        <v>120</v>
+        <v>455</v>
       </c>
       <c r="BB107" t="s">
-        <v>120</v>
+        <v>468</v>
       </c>
       <c r="BC107" t="s">
         <v>120</v>
@@ -20009,24 +20039,359 @@
       </c>
     </row>
     <row r="108" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A108" s="12"/>
-      <c r="E108" s="12"/>
-      <c r="F108" s="12"/>
-      <c r="G108" s="12"/>
-      <c r="S108" s="12"/>
-      <c r="AI108" s="12"/>
-      <c r="AS108" s="25"/>
-      <c r="AW108" s="25"/>
+      <c r="A108" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="B108" t="s">
+        <v>460</v>
+      </c>
+      <c r="C108" t="s">
+        <v>409</v>
+      </c>
+      <c r="D108" t="s">
+        <v>412</v>
+      </c>
+      <c r="E108" s="12" t="s">
+        <v>461</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H108" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I108" t="s">
+        <v>120</v>
+      </c>
+      <c r="J108" t="s">
+        <v>120</v>
+      </c>
+      <c r="K108" t="s">
+        <v>120</v>
+      </c>
+      <c r="L108" t="s">
+        <v>120</v>
+      </c>
+      <c r="M108" t="s">
+        <v>120</v>
+      </c>
+      <c r="N108" t="s">
+        <v>120</v>
+      </c>
+      <c r="O108" t="s">
+        <v>120</v>
+      </c>
+      <c r="P108" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q108" t="s">
+        <v>120</v>
+      </c>
+      <c r="R108" t="s">
+        <v>120</v>
+      </c>
+      <c r="S108" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T108" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U108" t="s">
+        <v>271</v>
+      </c>
+      <c r="V108" t="s">
+        <v>120</v>
+      </c>
+      <c r="W108" t="s">
+        <v>120</v>
+      </c>
+      <c r="X108" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y108" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z108" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA108" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB108" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC108" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD108" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE108" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF108" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG108" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH108" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI108" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ108" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK108" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL108" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM108">
+        <v>125</v>
+      </c>
+      <c r="AN108">
+        <v>1169</v>
+      </c>
+      <c r="AO108" s="20">
+        <v>414</v>
+      </c>
+      <c r="AP108">
+        <v>96</v>
+      </c>
+      <c r="AQ108">
+        <v>960</v>
+      </c>
+      <c r="AR108">
+        <v>256</v>
+      </c>
+      <c r="AS108" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT108" s="38">
+        <f t="shared" ref="AT108" si="154" xml:space="preserve"> _xlfn.FLOOR.MATH((AM108 - AP108) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AU108">
+        <f t="shared" ref="AU108" si="155" xml:space="preserve"> _xlfn.FLOOR.MATH((AN108 - AQ108) / 2)</f>
+        <v>104</v>
+      </c>
+      <c r="AV108">
+        <f t="shared" ref="AV108" si="156" xml:space="preserve"> _xlfn.FLOOR.MATH((AO108 - AR108) / 2)</f>
+        <v>79</v>
+      </c>
+      <c r="AW108" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX108">
+        <f t="shared" ref="AX108" si="157">AP108-AT108</f>
+        <v>82</v>
+      </c>
+      <c r="AY108">
+        <f t="shared" ref="AY108" si="158">AQ108-AU108</f>
+        <v>856</v>
+      </c>
+      <c r="AZ108" s="10">
+        <f t="shared" ref="AZ108" si="159">AR108-AV108</f>
+        <v>177</v>
+      </c>
+      <c r="BA108" t="s">
+        <v>419</v>
+      </c>
+      <c r="BB108" t="s">
+        <v>462</v>
+      </c>
+      <c r="BC108" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD108" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE108" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="109" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A109" s="12"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="12"/>
-      <c r="G109" s="12"/>
-      <c r="S109" s="12"/>
-      <c r="AI109" s="12"/>
-      <c r="AS109" s="25"/>
-      <c r="AW109" s="25"/>
+      <c r="A109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B109" t="s">
+        <v>120</v>
+      </c>
+      <c r="C109" t="s">
+        <v>120</v>
+      </c>
+      <c r="D109" t="s">
+        <v>120</v>
+      </c>
+      <c r="E109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H109" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I109" t="s">
+        <v>120</v>
+      </c>
+      <c r="J109" t="s">
+        <v>120</v>
+      </c>
+      <c r="K109" t="s">
+        <v>120</v>
+      </c>
+      <c r="L109" t="s">
+        <v>120</v>
+      </c>
+      <c r="M109" t="s">
+        <v>120</v>
+      </c>
+      <c r="N109" t="s">
+        <v>120</v>
+      </c>
+      <c r="O109" t="s">
+        <v>120</v>
+      </c>
+      <c r="P109" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q109" t="s">
+        <v>120</v>
+      </c>
+      <c r="R109" t="s">
+        <v>120</v>
+      </c>
+      <c r="S109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T109" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U109" t="s">
+        <v>120</v>
+      </c>
+      <c r="V109" t="s">
+        <v>120</v>
+      </c>
+      <c r="W109" t="s">
+        <v>120</v>
+      </c>
+      <c r="X109" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y109" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH109" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI109" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK109" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL109" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO109" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS109" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV109" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW109" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX109" t="e">
+        <f t="shared" ref="AX109" si="160">AP109-AT109</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY109" t="e">
+        <f t="shared" ref="AY109" si="161">AQ109-AU109</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ109" s="10" t="e">
+        <f t="shared" ref="AZ109" si="162">AR109-AV109</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA109" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB109" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC109" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD109" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE109" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="110" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A110" s="12"/>

</xml_diff>

<commit_message>
prepare train3dunet 1.8.2 chpt-231225-3
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3046C14F-20D0-4EED-B8EC-0709FB934865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153675FC-27C2-4442-82F8-701169B05527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3319" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3421" uniqueCount="475">
   <si>
     <t>patch z</t>
   </si>
@@ -1447,6 +1447,24 @@
   </si>
   <si>
     <t>stride = such that the halo is 32 in all dimensions.</t>
+  </si>
+  <si>
+    <t>231225-2</t>
+  </si>
+  <si>
+    <t>gcc related</t>
+  </si>
+  <si>
+    <t>Copy test_config-231225-0.yml and rerun predict3dunet on it from an interactive A100 session.</t>
+  </si>
+  <si>
+    <t>Fail. Gcc related error.</t>
+  </si>
+  <si>
+    <t>231225-3</t>
+  </si>
+  <si>
+    <t>Copy train_config-231225-1.yml and rerun predict3dunet on it from an interactive A100 session.</t>
   </si>
 </sst>
 </file>
@@ -2059,8 +2077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BE111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AT108" sqref="AT108"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -19882,10 +19900,10 @@
         <v>466</v>
       </c>
       <c r="G107" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="H107" s="6" t="s">
-        <v>120</v>
+        <v>472</v>
+      </c>
+      <c r="H107" s="6">
+        <v>0</v>
       </c>
       <c r="I107" t="s">
         <v>120</v>
@@ -20028,11 +20046,11 @@
       <c r="BB107" t="s">
         <v>468</v>
       </c>
-      <c r="BC107" t="s">
-        <v>120</v>
+      <c r="BC107">
+        <v>1</v>
       </c>
       <c r="BD107" t="s">
-        <v>120</v>
+        <v>470</v>
       </c>
       <c r="BE107" t="s">
         <v>120</v>
@@ -20055,13 +20073,13 @@
         <v>461</v>
       </c>
       <c r="F108" s="12" t="s">
-        <v>120</v>
+        <v>466</v>
       </c>
       <c r="G108" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="H108" s="6" t="s">
-        <v>120</v>
+        <v>472</v>
+      </c>
+      <c r="H108" s="6">
+        <v>0</v>
       </c>
       <c r="I108" t="s">
         <v>120</v>
@@ -20207,40 +20225,40 @@
       <c r="BB108" t="s">
         <v>462</v>
       </c>
-      <c r="BC108" t="s">
-        <v>120</v>
+      <c r="BC108">
+        <v>1</v>
       </c>
       <c r="BD108" t="s">
-        <v>120</v>
+        <v>470</v>
       </c>
       <c r="BE108" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:57" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="12" t="s">
-        <v>120</v>
+        <v>469</v>
       </c>
       <c r="B109" t="s">
-        <v>120</v>
+        <v>404</v>
       </c>
       <c r="C109" t="s">
-        <v>120</v>
+        <v>409</v>
       </c>
       <c r="D109" t="s">
-        <v>120</v>
+        <v>412</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>120</v>
+        <v>471</v>
       </c>
       <c r="F109" s="12" t="s">
-        <v>120</v>
+        <v>466</v>
       </c>
       <c r="G109" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="H109" s="6" t="s">
-        <v>120</v>
+        <v>465</v>
+      </c>
+      <c r="H109" s="6">
+        <v>0</v>
       </c>
       <c r="I109" t="s">
         <v>120</v>
@@ -20383,35 +20401,367 @@
       <c r="BB109" t="s">
         <v>120</v>
       </c>
-      <c r="BC109" t="s">
-        <v>120</v>
+      <c r="BC109">
+        <v>1</v>
       </c>
       <c r="BD109" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE109" t="s">
-        <v>120</v>
+        <v>457</v>
+      </c>
+      <c r="BE109" s="2" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="110" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A110" s="12"/>
-      <c r="E110" s="12"/>
-      <c r="F110" s="12"/>
-      <c r="G110" s="12"/>
-      <c r="S110" s="12"/>
-      <c r="AI110" s="12"/>
-      <c r="AS110" s="25"/>
-      <c r="AW110" s="25"/>
+      <c r="A110" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="B110" t="s">
+        <v>460</v>
+      </c>
+      <c r="C110" t="s">
+        <v>409</v>
+      </c>
+      <c r="D110" t="s">
+        <v>412</v>
+      </c>
+      <c r="E110" s="12" t="s">
+        <v>474</v>
+      </c>
+      <c r="F110" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="G110" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H110" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I110" t="s">
+        <v>120</v>
+      </c>
+      <c r="J110" t="s">
+        <v>120</v>
+      </c>
+      <c r="K110" t="s">
+        <v>120</v>
+      </c>
+      <c r="L110" t="s">
+        <v>120</v>
+      </c>
+      <c r="M110" t="s">
+        <v>120</v>
+      </c>
+      <c r="N110" t="s">
+        <v>120</v>
+      </c>
+      <c r="O110" t="s">
+        <v>120</v>
+      </c>
+      <c r="P110" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>120</v>
+      </c>
+      <c r="R110" t="s">
+        <v>120</v>
+      </c>
+      <c r="S110" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T110" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U110" t="s">
+        <v>120</v>
+      </c>
+      <c r="V110" t="s">
+        <v>120</v>
+      </c>
+      <c r="W110" t="s">
+        <v>120</v>
+      </c>
+      <c r="X110" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y110" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH110" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI110" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK110" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL110" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO110" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS110" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV110" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW110" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX110" t="e">
+        <f t="shared" ref="AX110" si="163">AP110-AT110</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY110" t="e">
+        <f t="shared" ref="AY110" si="164">AQ110-AU110</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ110" s="10" t="e">
+        <f t="shared" ref="AZ110" si="165">AR110-AV110</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA110" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB110" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC110" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD110" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE110" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="111" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A111" s="12"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
-      <c r="G111" s="12"/>
-      <c r="S111" s="12"/>
-      <c r="AI111" s="12"/>
-      <c r="AS111" s="25"/>
-      <c r="AW111" s="25"/>
+      <c r="A111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B111" t="s">
+        <v>120</v>
+      </c>
+      <c r="C111" t="s">
+        <v>120</v>
+      </c>
+      <c r="D111" t="s">
+        <v>120</v>
+      </c>
+      <c r="E111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H111" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I111" t="s">
+        <v>120</v>
+      </c>
+      <c r="J111" t="s">
+        <v>120</v>
+      </c>
+      <c r="K111" t="s">
+        <v>120</v>
+      </c>
+      <c r="L111" t="s">
+        <v>120</v>
+      </c>
+      <c r="M111" t="s">
+        <v>120</v>
+      </c>
+      <c r="N111" t="s">
+        <v>120</v>
+      </c>
+      <c r="O111" t="s">
+        <v>120</v>
+      </c>
+      <c r="P111" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>120</v>
+      </c>
+      <c r="R111" t="s">
+        <v>120</v>
+      </c>
+      <c r="S111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T111" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U111" t="s">
+        <v>120</v>
+      </c>
+      <c r="V111" t="s">
+        <v>120</v>
+      </c>
+      <c r="W111" t="s">
+        <v>120</v>
+      </c>
+      <c r="X111" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y111" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH111" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI111" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK111" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL111" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO111" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS111" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV111" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW111" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX111" t="e">
+        <f t="shared" ref="AX111" si="166">AP111-AT111</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY111" t="e">
+        <f t="shared" ref="AY111" si="167">AQ111-AU111</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ111" s="10" t="e">
+        <f t="shared" ref="AZ111" si="168">AR111-AV111</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA111" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB111" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC111" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD111" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE111" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
prepare predict3dunet 1.8.2 chpt-231225-5
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D30B565-6A66-43C2-B079-E4442E3F16D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6827DF1-A229-4ED4-86C8-1159408CC55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3446" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3488" uniqueCount="486">
   <si>
     <t>patch z</t>
   </si>
@@ -1470,13 +1470,34 @@
     <t>231225-4</t>
   </si>
   <si>
-    <t>Copy train_config-231225-2.yml, reduce patch shape and rerun predict3dunet on it from an interactive A100 session.</t>
-  </si>
-  <si>
     <t xml:space="preserve">  File "/home/dwalth/data/conda/envs/3dunet1.8.2/lib/python3.11/site-packages/torch/utils/data/dataset.py", line 284, in __init__                               assert len(self.datasets) &gt; 0, 'datasets should not be an empty iterable'  # type: ignore[arg-type]</t>
   </si>
   <si>
     <t>Fail. Assert error, 'datasets' should not be an empty iterable.</t>
+  </si>
+  <si>
+    <t>Copy train_config-231225-2.yml, set validation stride to the same as train stride and rerun predict3dunet on it from an interactive A100 session.</t>
+  </si>
+  <si>
+    <t>231225-5</t>
+  </si>
+  <si>
+    <t>predict3dunet 1.8.2</t>
+  </si>
+  <si>
+    <t>Run predict3dunet with same patch as in training and stride for a halo of 32 voxels in all dimensions.</t>
+  </si>
+  <si>
+    <t>Success. Did not let the training finish, this is a test run for predict3dunet 1.8.2.</t>
+  </si>
+  <si>
+    <t>test run for predict3dunet 1.8.2, model performance satisfactory and irrelevant anyhow.</t>
+  </si>
+  <si>
+    <t>patch = same as in model training.</t>
+  </si>
+  <si>
+    <t>stride = halo of 32 voxels in all dimensions.</t>
   </si>
 </sst>
 </file>
@@ -2087,10 +2108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BE112"/>
+  <dimension ref="A1:BE113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView tabSelected="1" topLeftCell="AW92" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AZ112" sqref="AZ112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -20309,7 +20330,7 @@
         <v>120</v>
       </c>
       <c r="U109" t="s">
-        <v>120</v>
+        <v>271</v>
       </c>
       <c r="V109" t="s">
         <v>120</v>
@@ -20443,7 +20464,7 @@
         <v>466</v>
       </c>
       <c r="G110" s="12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H110" s="6">
         <v>0</v>
@@ -20485,7 +20506,7 @@
         <v>120</v>
       </c>
       <c r="U110" t="s">
-        <v>120</v>
+        <v>271</v>
       </c>
       <c r="V110" t="s">
         <v>120</v>
@@ -20560,7 +20581,7 @@
         <v>48</v>
       </c>
       <c r="AT110" s="38">
-        <f t="shared" ref="AT110:AT111" si="163" xml:space="preserve"> _xlfn.FLOOR.MATH((AM110 - AP110) / 2)</f>
+        <f t="shared" ref="AT110:AT112" si="163" xml:space="preserve"> _xlfn.FLOOR.MATH((AM110 - AP110) / 2)</f>
         <v>14</v>
       </c>
       <c r="AU110">
@@ -20599,7 +20620,7 @@
         <v>14</v>
       </c>
       <c r="BE110" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="111" spans="1:57" x14ac:dyDescent="0.3">
@@ -20616,16 +20637,16 @@
         <v>412</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="F111" s="12" t="s">
         <v>466</v>
       </c>
       <c r="G111" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="H111" s="6" t="s">
-        <v>120</v>
+        <v>482</v>
+      </c>
+      <c r="H111" s="6">
+        <v>0</v>
       </c>
       <c r="I111" t="s">
         <v>120</v>
@@ -20633,11 +20654,11 @@
       <c r="J111" t="s">
         <v>120</v>
       </c>
-      <c r="K111" t="s">
-        <v>120</v>
+      <c r="K111">
+        <v>1</v>
       </c>
       <c r="L111" t="s">
-        <v>120</v>
+        <v>483</v>
       </c>
       <c r="M111" t="s">
         <v>120</v>
@@ -20664,7 +20685,7 @@
         <v>120</v>
       </c>
       <c r="U111" t="s">
-        <v>120</v>
+        <v>271</v>
       </c>
       <c r="V111" t="s">
         <v>120</v>
@@ -20771,34 +20792,34 @@
       <c r="BB111" t="s">
         <v>163</v>
       </c>
-      <c r="BC111" t="s">
-        <v>120</v>
+      <c r="BC111">
+        <v>0</v>
       </c>
       <c r="BD111" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="BE111" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A112" s="12" t="s">
-        <v>120</v>
+        <v>479</v>
       </c>
       <c r="B112" t="s">
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="C112" t="s">
-        <v>120</v>
+        <v>409</v>
       </c>
       <c r="D112" t="s">
-        <v>120</v>
+        <v>412</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>120</v>
+        <v>481</v>
       </c>
       <c r="F112" s="12" t="s">
-        <v>120</v>
+        <v>466</v>
       </c>
       <c r="G112" s="12" t="s">
         <v>120</v>
@@ -20843,7 +20864,7 @@
         <v>120</v>
       </c>
       <c r="U112" t="s">
-        <v>120</v>
+        <v>271</v>
       </c>
       <c r="V112" t="s">
         <v>120</v>
@@ -20896,64 +20917,240 @@
       <c r="AL112" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AM112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO112" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR112" t="s">
-        <v>120</v>
+      <c r="AM112">
+        <v>125</v>
+      </c>
+      <c r="AN112">
+        <v>1169</v>
+      </c>
+      <c r="AO112" s="20">
+        <v>414</v>
+      </c>
+      <c r="AP112">
+        <v>96</v>
+      </c>
+      <c r="AQ112">
+        <v>960</v>
+      </c>
+      <c r="AR112">
+        <v>256</v>
       </c>
       <c r="AS112" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AT112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV112" t="s">
-        <v>120</v>
+      <c r="AT112">
+        <v>64</v>
+      </c>
+      <c r="AU112">
+        <v>928</v>
+      </c>
+      <c r="AV112">
+        <v>224</v>
       </c>
       <c r="AW112" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AX112" t="e">
+      <c r="AX112">
         <f t="shared" ref="AX112" si="172">AP112-AT112</f>
+        <v>32</v>
+      </c>
+      <c r="AY112">
+        <f t="shared" ref="AY112" si="173">AQ112-AU112</f>
+        <v>32</v>
+      </c>
+      <c r="AZ112" s="10">
+        <f t="shared" ref="AZ112" si="174">AR112-AV112</f>
+        <v>32</v>
+      </c>
+      <c r="BA112" t="s">
+        <v>484</v>
+      </c>
+      <c r="BB112" t="s">
+        <v>485</v>
+      </c>
+      <c r="BC112" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD112" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE112" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="113" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A113" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B113" t="s">
+        <v>120</v>
+      </c>
+      <c r="C113" t="s">
+        <v>120</v>
+      </c>
+      <c r="D113" t="s">
+        <v>120</v>
+      </c>
+      <c r="E113" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F113" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G113" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H113" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I113" t="s">
+        <v>120</v>
+      </c>
+      <c r="J113" t="s">
+        <v>120</v>
+      </c>
+      <c r="K113" t="s">
+        <v>120</v>
+      </c>
+      <c r="L113" t="s">
+        <v>120</v>
+      </c>
+      <c r="M113" t="s">
+        <v>120</v>
+      </c>
+      <c r="N113" t="s">
+        <v>120</v>
+      </c>
+      <c r="O113" t="s">
+        <v>120</v>
+      </c>
+      <c r="P113" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q113" t="s">
+        <v>120</v>
+      </c>
+      <c r="R113" t="s">
+        <v>120</v>
+      </c>
+      <c r="S113" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T113" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U113" t="s">
+        <v>120</v>
+      </c>
+      <c r="V113" t="s">
+        <v>120</v>
+      </c>
+      <c r="W113" t="s">
+        <v>120</v>
+      </c>
+      <c r="X113" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y113" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH113" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI113" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK113" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL113" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO113" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS113" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV113" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW113" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX113" t="e">
+        <f t="shared" ref="AX113" si="175">AP113-AT113</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AY112" t="e">
-        <f t="shared" ref="AY112" si="173">AQ112-AU112</f>
+      <c r="AY113" t="e">
+        <f t="shared" ref="AY113" si="176">AQ113-AU113</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ112" s="10" t="e">
-        <f t="shared" ref="AZ112" si="174">AR112-AV112</f>
+      <c r="AZ113" s="10" t="e">
+        <f t="shared" ref="AZ113" si="177">AR113-AV113</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA112" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB112" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC112" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD112" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE112" t="s">
+      <c r="BA113" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB113" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC113" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD113" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE113" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare train3dunet 1.8.2 chpt-231225-6 - autofluo multichannel model, lets go!
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6827DF1-A229-4ED4-86C8-1159408CC55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E53277-503D-4883-B84E-505436E179B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3488" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3571" uniqueCount="492">
   <si>
     <t>patch z</t>
   </si>
@@ -1498,13 +1498,31 @@
   </si>
   <si>
     <t>stride = halo of 32 voxels in all dimensions.</t>
+  </si>
+  <si>
+    <t>Success. "INFO UNetPredictor - Finished inference in 11.53 seconds"</t>
+  </si>
+  <si>
+    <t>231225-6</t>
+  </si>
+  <si>
+    <t>231226-0</t>
+  </si>
+  <si>
+    <t>Train a multi channel autofluorescence heart model.</t>
+  </si>
+  <si>
+    <t>Success (no error &amp; sensible results)</t>
+  </si>
+  <si>
+    <t>Segment the model and look at 3D results.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1528,6 +1546,23 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1741,7 +1776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1794,6 +1829,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2108,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BE113"/>
+  <dimension ref="A1:BE115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AZ112" sqref="AZ112"/>
+    <sheetView tabSelected="1" topLeftCell="AK101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AV115" sqref="AV115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -20581,7 +20642,7 @@
         <v>48</v>
       </c>
       <c r="AT110" s="38">
-        <f t="shared" ref="AT110:AT112" si="163" xml:space="preserve"> _xlfn.FLOOR.MATH((AM110 - AP110) / 2)</f>
+        <f t="shared" ref="AT110:AT111" si="163" xml:space="preserve"> _xlfn.FLOOR.MATH((AM110 - AP110) / 2)</f>
         <v>14</v>
       </c>
       <c r="AU110">
@@ -20623,534 +20684,894 @@
         <v>476</v>
       </c>
     </row>
-    <row r="111" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A111" s="12" t="s">
+    <row r="111" spans="1:57" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="40" t="s">
         <v>475</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="41" t="s">
         <v>460</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="41" t="s">
         <v>412</v>
       </c>
-      <c r="E111" s="12" t="s">
+      <c r="E111" s="40" t="s">
         <v>478</v>
       </c>
-      <c r="F111" s="12" t="s">
+      <c r="F111" s="40" t="s">
         <v>466</v>
       </c>
-      <c r="G111" s="12" t="s">
+      <c r="G111" s="40" t="s">
         <v>482</v>
       </c>
-      <c r="H111" s="6">
-        <v>0</v>
-      </c>
-      <c r="I111" t="s">
-        <v>120</v>
-      </c>
-      <c r="J111" t="s">
-        <v>120</v>
-      </c>
-      <c r="K111">
-        <v>1</v>
-      </c>
-      <c r="L111" t="s">
+      <c r="H111" s="42">
+        <v>0</v>
+      </c>
+      <c r="I111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="J111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="K111" s="41">
+        <v>1</v>
+      </c>
+      <c r="L111" s="41" t="s">
         <v>483</v>
       </c>
-      <c r="M111" t="s">
-        <v>120</v>
-      </c>
-      <c r="N111" t="s">
-        <v>120</v>
-      </c>
-      <c r="O111" t="s">
-        <v>120</v>
-      </c>
-      <c r="P111" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q111" t="s">
-        <v>120</v>
-      </c>
-      <c r="R111" t="s">
-        <v>120</v>
-      </c>
-      <c r="S111" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="T111" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="U111" t="s">
+      <c r="M111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="N111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="O111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="P111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="R111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="S111" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="T111" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="U111" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="V111" t="s">
-        <v>120</v>
-      </c>
-      <c r="W111" t="s">
-        <v>120</v>
-      </c>
-      <c r="X111" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y111" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z111" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA111" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB111" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC111" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD111" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE111" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF111" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG111" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH111" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI111" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ111" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK111" t="s">
+      <c r="V111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="W111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="X111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH111" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI111" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ111" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK111" s="41" t="s">
         <v>281</v>
       </c>
-      <c r="AL111" s="10" t="s">
+      <c r="AL111" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="AM111">
+      <c r="AM111" s="41">
         <v>125</v>
       </c>
-      <c r="AN111">
+      <c r="AN111" s="41">
         <v>1169</v>
       </c>
-      <c r="AO111" s="20">
+      <c r="AO111" s="43">
         <v>414</v>
       </c>
-      <c r="AP111">
+      <c r="AP111" s="41">
         <v>96</v>
       </c>
-      <c r="AQ111">
+      <c r="AQ111" s="41">
         <v>960</v>
       </c>
-      <c r="AR111">
+      <c r="AR111" s="41">
         <v>256</v>
       </c>
-      <c r="AS111" s="12" t="s">
+      <c r="AS111" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="AT111" s="38">
+      <c r="AT111" s="45">
         <f t="shared" si="163"/>
         <v>14</v>
       </c>
-      <c r="AU111">
+      <c r="AU111" s="41">
         <f t="shared" si="164"/>
         <v>104</v>
       </c>
-      <c r="AV111">
+      <c r="AV111" s="41">
         <f t="shared" si="165"/>
         <v>79</v>
       </c>
-      <c r="AW111" s="25" t="s">
+      <c r="AW111" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="AX111">
+      <c r="AX111" s="41">
         <f t="shared" ref="AX111" si="169">AP111-AT111</f>
         <v>82</v>
       </c>
-      <c r="AY111">
+      <c r="AY111" s="41">
         <f t="shared" ref="AY111" si="170">AQ111-AU111</f>
         <v>856</v>
       </c>
-      <c r="AZ111" s="10">
+      <c r="AZ111" s="44">
         <f t="shared" ref="AZ111" si="171">AR111-AV111</f>
         <v>177</v>
       </c>
-      <c r="BA111" t="s">
+      <c r="BA111" s="41" t="s">
         <v>419</v>
       </c>
-      <c r="BB111" t="s">
+      <c r="BB111" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="BC111">
-        <v>0</v>
-      </c>
-      <c r="BD111" t="s">
-        <v>8</v>
-      </c>
-      <c r="BE111" t="s">
+      <c r="BC111" s="41">
+        <v>0</v>
+      </c>
+      <c r="BD111" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="BE111" s="41" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:57" x14ac:dyDescent="0.3">
-      <c r="A112" s="12" t="s">
+    <row r="112" spans="1:57" s="49" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="48" t="s">
         <v>479</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="49" t="s">
         <v>480</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="49" t="s">
         <v>409</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="49" t="s">
         <v>412</v>
       </c>
-      <c r="E112" s="12" t="s">
+      <c r="E112" s="48" t="s">
         <v>481</v>
       </c>
-      <c r="F112" s="12" t="s">
+      <c r="F112" s="48" t="s">
         <v>466</v>
       </c>
-      <c r="G112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="H112" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I112" t="s">
-        <v>120</v>
-      </c>
-      <c r="J112" t="s">
-        <v>120</v>
-      </c>
-      <c r="K112" t="s">
-        <v>120</v>
-      </c>
-      <c r="L112" t="s">
-        <v>120</v>
-      </c>
-      <c r="M112" t="s">
-        <v>120</v>
-      </c>
-      <c r="N112" t="s">
-        <v>120</v>
-      </c>
-      <c r="O112" t="s">
-        <v>120</v>
-      </c>
-      <c r="P112" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q112" t="s">
-        <v>120</v>
-      </c>
-      <c r="R112" t="s">
-        <v>120</v>
-      </c>
-      <c r="S112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="T112" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="U112" t="s">
+      <c r="G112" s="48" t="s">
+        <v>486</v>
+      </c>
+      <c r="H112" s="50">
+        <v>1</v>
+      </c>
+      <c r="I112" s="49">
+        <v>0</v>
+      </c>
+      <c r="J112" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="K112" s="49">
+        <v>0</v>
+      </c>
+      <c r="L112" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="M112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="N112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="O112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="P112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="R112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="S112" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="T112" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="U112" s="49" t="s">
         <v>271</v>
       </c>
-      <c r="V112" t="s">
-        <v>120</v>
-      </c>
-      <c r="W112" t="s">
-        <v>120</v>
-      </c>
-      <c r="X112" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y112" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH112" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI112" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ112" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK112" t="s">
+      <c r="V112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="W112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="X112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH112" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI112" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK112" s="49" t="s">
         <v>281</v>
       </c>
-      <c r="AL112" s="10" t="s">
+      <c r="AL112" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="AM112">
+      <c r="AM112" s="49">
         <v>125</v>
       </c>
-      <c r="AN112">
+      <c r="AN112" s="49">
         <v>1169</v>
       </c>
-      <c r="AO112" s="20">
+      <c r="AO112" s="51">
         <v>414</v>
       </c>
-      <c r="AP112">
+      <c r="AP112" s="49">
         <v>96</v>
       </c>
-      <c r="AQ112">
+      <c r="AQ112" s="49">
         <v>960</v>
       </c>
-      <c r="AR112">
+      <c r="AR112" s="49">
         <v>256</v>
       </c>
-      <c r="AS112" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT112">
+      <c r="AS112" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT112" s="49">
         <v>64</v>
       </c>
-      <c r="AU112">
+      <c r="AU112" s="49">
         <v>928</v>
       </c>
-      <c r="AV112">
+      <c r="AV112" s="49">
         <v>224</v>
       </c>
-      <c r="AW112" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX112">
+      <c r="AW112" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX112" s="49">
         <f t="shared" ref="AX112" si="172">AP112-AT112</f>
         <v>32</v>
       </c>
-      <c r="AY112">
+      <c r="AY112" s="49">
         <f t="shared" ref="AY112" si="173">AQ112-AU112</f>
         <v>32</v>
       </c>
-      <c r="AZ112" s="10">
+      <c r="AZ112" s="52">
         <f t="shared" ref="AZ112" si="174">AR112-AV112</f>
         <v>32</v>
       </c>
-      <c r="BA112" t="s">
+      <c r="BA112" s="49" t="s">
         <v>484</v>
       </c>
-      <c r="BB112" t="s">
+      <c r="BB112" s="49" t="s">
         <v>485</v>
       </c>
-      <c r="BC112" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD112" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE112" t="s">
+      <c r="BC112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD112" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE112" s="49" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:57" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B113" t="s">
-        <v>120</v>
-      </c>
-      <c r="C113" t="s">
-        <v>120</v>
-      </c>
-      <c r="D113" t="s">
-        <v>120</v>
+        <v>487</v>
+      </c>
+      <c r="B113" s="47" t="s">
+        <v>460</v>
+      </c>
+      <c r="C113" s="47" t="s">
+        <v>409</v>
+      </c>
+      <c r="D113" s="47" t="s">
+        <v>412</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>120</v>
+        <v>489</v>
       </c>
       <c r="F113" s="12" t="s">
-        <v>120</v>
+        <v>466</v>
       </c>
       <c r="G113" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="H113" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="I113" t="s">
-        <v>120</v>
-      </c>
-      <c r="J113" t="s">
-        <v>120</v>
-      </c>
-      <c r="K113" t="s">
-        <v>120</v>
-      </c>
-      <c r="L113" t="s">
-        <v>120</v>
-      </c>
-      <c r="M113" t="s">
-        <v>120</v>
-      </c>
-      <c r="N113" t="s">
-        <v>120</v>
-      </c>
-      <c r="O113" t="s">
-        <v>120</v>
-      </c>
-      <c r="P113" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q113" t="s">
-        <v>120</v>
-      </c>
-      <c r="R113" t="s">
+      <c r="H113" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="I113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="J113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="K113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="L113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="M113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="N113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="O113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="P113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="R113" s="47" t="s">
         <v>120</v>
       </c>
       <c r="S113" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="T113" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="U113" t="s">
-        <v>120</v>
-      </c>
-      <c r="V113" t="s">
-        <v>120</v>
-      </c>
-      <c r="W113" t="s">
-        <v>120</v>
-      </c>
-      <c r="X113" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y113" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH113" s="6" t="s">
+      <c r="T113" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="U113" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="V113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="W113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="X113" s="47">
+        <v>5</v>
+      </c>
+      <c r="Y113" s="47">
+        <v>1</v>
+      </c>
+      <c r="Z113" s="47">
+        <f>X113+Y113</f>
+        <v>6</v>
+      </c>
+      <c r="AA113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH113" s="56" t="s">
         <v>120</v>
       </c>
       <c r="AI113" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="AJ113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK113" t="s">
+      <c r="AJ113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK113" s="47">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AP113*AQ113*AR113) * (Z113 / 5) + 441</f>
+        <v>73500.060473349149</v>
+      </c>
+      <c r="AL113" s="57" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM113" s="47">
+        <v>125</v>
+      </c>
+      <c r="AN113" s="47">
+        <v>1169</v>
+      </c>
+      <c r="AO113" s="54">
+        <v>414</v>
+      </c>
+      <c r="AP113" s="47">
+        <v>96</v>
+      </c>
+      <c r="AQ113" s="47">
+        <v>768</v>
+      </c>
+      <c r="AR113" s="47">
+        <v>384</v>
+      </c>
+      <c r="AS113" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT113" s="55">
+        <f t="shared" ref="AT113" si="175" xml:space="preserve"> _xlfn.FLOOR.MATH((AM113 - AP113) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AU113" s="47">
+        <f t="shared" ref="AU113" si="176" xml:space="preserve"> _xlfn.FLOOR.MATH((AN113 - AQ113) / 2)</f>
+        <v>200</v>
+      </c>
+      <c r="AV113" s="47">
+        <f t="shared" ref="AV113" si="177" xml:space="preserve"> _xlfn.FLOOR.MATH((AO113 - AR113) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AW113" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX113" s="47">
+        <f t="shared" ref="AX113" si="178">AP113-AT113</f>
+        <v>82</v>
+      </c>
+      <c r="AY113" s="47">
+        <f t="shared" ref="AY113" si="179">AQ113-AU113</f>
+        <v>568</v>
+      </c>
+      <c r="AZ113" s="57">
+        <f t="shared" ref="AZ113" si="180">AR113-AV113</f>
+        <v>369</v>
+      </c>
+      <c r="BA113" s="47" t="s">
+        <v>419</v>
+      </c>
+      <c r="BB113" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="BC113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD113" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE113" s="47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="114" spans="1:57" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="12" t="s">
+        <v>488</v>
+      </c>
+      <c r="B114" s="47" t="s">
+        <v>480</v>
+      </c>
+      <c r="C114" s="47" t="s">
+        <v>409</v>
+      </c>
+      <c r="D114" s="47" t="s">
+        <v>412</v>
+      </c>
+      <c r="E114" s="12" t="s">
+        <v>491</v>
+      </c>
+      <c r="F114" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="G114" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H114" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="I114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="J114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="K114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="L114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="M114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="N114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="O114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="P114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="R114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="S114" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T114" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="U114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="V114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="W114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="X114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH114" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI114" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK114" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="AL113" s="10" t="s">
+      <c r="AL114" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="AM113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AN113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO113" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS113" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AU113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV113" t="s">
-        <v>120</v>
-      </c>
-      <c r="AW113" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX113" t="e">
-        <f t="shared" ref="AX113" si="175">AP113-AT113</f>
+      <c r="AM114" s="47">
+        <v>125</v>
+      </c>
+      <c r="AN114" s="47">
+        <v>1169</v>
+      </c>
+      <c r="AO114" s="54">
+        <v>414</v>
+      </c>
+      <c r="AP114" s="47">
+        <v>96</v>
+      </c>
+      <c r="AQ114" s="47">
+        <v>768</v>
+      </c>
+      <c r="AR114" s="47">
+        <v>384</v>
+      </c>
+      <c r="AS114" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT114" s="55">
+        <f t="shared" ref="AT114" si="181" xml:space="preserve"> _xlfn.FLOOR.MATH((AM114 - AP114) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AU114" s="47">
+        <f t="shared" ref="AU114" si="182" xml:space="preserve"> _xlfn.FLOOR.MATH((AN114 - AQ114) / 2)</f>
+        <v>200</v>
+      </c>
+      <c r="AV114" s="47">
+        <f t="shared" ref="AV114" si="183" xml:space="preserve"> _xlfn.FLOOR.MATH((AO114 - AR114) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AW114" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX114" s="47">
+        <f t="shared" ref="AX114" si="184">AP114-AT114</f>
+        <v>82</v>
+      </c>
+      <c r="AY114" s="47">
+        <f t="shared" ref="AY114" si="185">AQ114-AU114</f>
+        <v>568</v>
+      </c>
+      <c r="AZ114" s="57">
+        <f t="shared" ref="AZ114" si="186">AR114-AV114</f>
+        <v>369</v>
+      </c>
+      <c r="BA114" s="47" t="s">
+        <v>484</v>
+      </c>
+      <c r="BB114" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="BC114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD114" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE114" s="47" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="115" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A115" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B115" t="s">
+        <v>120</v>
+      </c>
+      <c r="C115" t="s">
+        <v>120</v>
+      </c>
+      <c r="D115" t="s">
+        <v>120</v>
+      </c>
+      <c r="E115" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F115" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G115" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H115" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="I115" t="s">
+        <v>120</v>
+      </c>
+      <c r="J115" t="s">
+        <v>120</v>
+      </c>
+      <c r="K115" t="s">
+        <v>120</v>
+      </c>
+      <c r="L115" t="s">
+        <v>120</v>
+      </c>
+      <c r="M115" t="s">
+        <v>120</v>
+      </c>
+      <c r="N115" t="s">
+        <v>120</v>
+      </c>
+      <c r="O115" t="s">
+        <v>120</v>
+      </c>
+      <c r="P115" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>120</v>
+      </c>
+      <c r="R115" t="s">
+        <v>120</v>
+      </c>
+      <c r="S115" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="T115" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="U115" t="s">
+        <v>120</v>
+      </c>
+      <c r="V115" t="s">
+        <v>120</v>
+      </c>
+      <c r="W115" t="s">
+        <v>120</v>
+      </c>
+      <c r="X115" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y115" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH115" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI115" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK115" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL115" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AN115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO115" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS115" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AU115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV115" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW115" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX115" t="e">
+        <f t="shared" ref="AX115" si="187">AP115-AT115</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AY113" t="e">
-        <f t="shared" ref="AY113" si="176">AQ113-AU113</f>
+      <c r="AY115" t="e">
+        <f t="shared" ref="AY115" si="188">AQ115-AU115</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ113" s="10" t="e">
-        <f t="shared" ref="AZ113" si="177">AR113-AV113</f>
+      <c r="AZ115" s="10" t="e">
+        <f t="shared" ref="AZ115" si="189">AR115-AV115</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA113" t="s">
-        <v>120</v>
-      </c>
-      <c r="BB113" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC113" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD113" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE113" t="s">
+      <c r="BA115" t="s">
+        <v>120</v>
+      </c>
+      <c r="BB115" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC115" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD115" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE115" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare predict3dunet 1.8.2 chpt-240102-1
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1651321-1C47-4BAE-9101-157EAAB8DA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFF2650-EA7D-4970-829D-E56DFFCE52BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3643" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3678" uniqueCount="508">
   <si>
     <t>patch z</t>
   </si>
@@ -1555,6 +1555,15 @@
   </si>
   <si>
     <t>Segment the model 231225-6 and look at 3D results. Use the specimen used for validation during model training.</t>
+  </si>
+  <si>
+    <t>240101-1</t>
+  </si>
+  <si>
+    <t>Segment the model 231225-6 and look at 3D results. Use the specimen used for validation during model training. Use the last instead of best pytorch checkpoint, this should result in the same images as in the tensorboard statistics.</t>
+  </si>
+  <si>
+    <t>Partial success. No error but bad segmentation, equally bad as id07 (231226-2).</t>
   </si>
 </sst>
 </file>
@@ -1815,7 +1824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1887,9 +1896,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2206,10 +2212,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BF118"/>
+  <dimension ref="A1:BF119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -21365,7 +21371,7 @@
       <c r="J114">
         <v>1</v>
       </c>
-      <c r="K114" s="53" t="s">
+      <c r="K114" s="12" t="s">
         <v>500</v>
       </c>
       <c r="L114">
@@ -21784,22 +21790,22 @@
         <v>490</v>
       </c>
       <c r="H117" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="I117" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J117" t="s">
-        <v>120</v>
+        <v>507</v>
+      </c>
+      <c r="I117" s="6">
+        <v>1</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
       </c>
       <c r="K117" t="s">
-        <v>120</v>
-      </c>
-      <c r="L117" t="s">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="L117">
+        <v>0</v>
       </c>
       <c r="M117" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="N117" t="s">
         <v>120</v>
@@ -21834,14 +21840,15 @@
       <c r="X117" t="s">
         <v>120</v>
       </c>
-      <c r="Y117" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z117" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA117" t="s">
-        <v>120</v>
+      <c r="Y117">
+        <v>5</v>
+      </c>
+      <c r="Z117">
+        <v>1</v>
+      </c>
+      <c r="AA117">
+        <f>Y117+Z117</f>
+        <v>6</v>
       </c>
       <c r="AB117" t="s">
         <v>120</v>
@@ -21933,37 +21940,37 @@
       <c r="BC117" t="s">
         <v>163</v>
       </c>
-      <c r="BD117" t="s">
-        <v>120</v>
+      <c r="BD117">
+        <v>0</v>
       </c>
       <c r="BE117" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="BF117" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>120</v>
+        <v>505</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>120</v>
+        <v>502</v>
       </c>
       <c r="C118" t="s">
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="D118" t="s">
-        <v>120</v>
+        <v>409</v>
       </c>
       <c r="E118" t="s">
-        <v>120</v>
+        <v>412</v>
       </c>
       <c r="F118" s="12" t="s">
-        <v>120</v>
+        <v>506</v>
       </c>
       <c r="G118" s="12" t="s">
-        <v>120</v>
+        <v>490</v>
       </c>
       <c r="H118" s="12" t="s">
         <v>120</v>
@@ -22008,7 +22015,7 @@
         <v>120</v>
       </c>
       <c r="V118" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="W118" t="s">
         <v>120</v>
@@ -22016,20 +22023,21 @@
       <c r="X118" t="s">
         <v>120</v>
       </c>
-      <c r="Y118" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA118" t="s">
-        <v>120</v>
+      <c r="Y118">
+        <v>5</v>
+      </c>
+      <c r="Z118">
+        <v>1</v>
+      </c>
+      <c r="AA118">
+        <f>Y118+Z118</f>
+        <v>6</v>
       </c>
       <c r="AB118" t="s">
         <v>120</v>
       </c>
-      <c r="AC118" t="s">
-        <v>120</v>
+      <c r="AC118">
+        <v>3</v>
       </c>
       <c r="AD118" t="s">
         <v>120</v>
@@ -22061,64 +22069,246 @@
       <c r="AM118" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AN118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP118" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS118" t="s">
-        <v>120</v>
+      <c r="AN118">
+        <v>125</v>
+      </c>
+      <c r="AO118">
+        <v>1169</v>
+      </c>
+      <c r="AP118" s="20">
+        <v>414</v>
+      </c>
+      <c r="AQ118">
+        <v>96</v>
+      </c>
+      <c r="AR118">
+        <v>768</v>
+      </c>
+      <c r="AS118">
+        <v>384</v>
       </c>
       <c r="AT118" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AU118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AW118" t="s">
-        <v>120</v>
+      <c r="AU118" s="38">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN118 - AQ118) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AV118">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO118 - AR118) / 2)</f>
+        <v>200</v>
+      </c>
+      <c r="AW118">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP118 - AS118) / 2)</f>
+        <v>15</v>
       </c>
       <c r="AX118" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY118" t="e">
+        <v>48</v>
+      </c>
+      <c r="AY118">
         <f t="shared" ref="AY118" si="190">AQ118-AU118</f>
+        <v>82</v>
+      </c>
+      <c r="AZ118">
+        <f t="shared" ref="AZ118" si="191">AR118-AV118</f>
+        <v>568</v>
+      </c>
+      <c r="BA118" s="10">
+        <f t="shared" ref="BA118" si="192">AS118-AW118</f>
+        <v>369</v>
+      </c>
+      <c r="BB118" t="s">
+        <v>484</v>
+      </c>
+      <c r="BC118" t="s">
+        <v>163</v>
+      </c>
+      <c r="BD118" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE118" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF118" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="119" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A119" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C119" t="s">
+        <v>120</v>
+      </c>
+      <c r="D119" t="s">
+        <v>120</v>
+      </c>
+      <c r="E119" t="s">
+        <v>120</v>
+      </c>
+      <c r="F119" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G119" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H119" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I119" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J119" t="s">
+        <v>120</v>
+      </c>
+      <c r="K119" t="s">
+        <v>120</v>
+      </c>
+      <c r="L119" t="s">
+        <v>120</v>
+      </c>
+      <c r="M119" t="s">
+        <v>120</v>
+      </c>
+      <c r="N119" t="s">
+        <v>120</v>
+      </c>
+      <c r="O119" t="s">
+        <v>120</v>
+      </c>
+      <c r="P119" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>120</v>
+      </c>
+      <c r="R119" t="s">
+        <v>120</v>
+      </c>
+      <c r="S119" t="s">
+        <v>120</v>
+      </c>
+      <c r="T119" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U119" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="V119" t="s">
+        <v>120</v>
+      </c>
+      <c r="W119" t="s">
+        <v>120</v>
+      </c>
+      <c r="X119" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y119" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI119" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ119" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL119" t="s">
+        <v>281</v>
+      </c>
+      <c r="AM119" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP119" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AT119" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW119" t="s">
+        <v>120</v>
+      </c>
+      <c r="AX119" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY119" t="e">
+        <f t="shared" ref="AY119" si="193">AQ119-AU119</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ118" t="e">
-        <f t="shared" ref="AZ118" si="191">AR118-AV118</f>
+      <c r="AZ119" t="e">
+        <f t="shared" ref="AZ119" si="194">AR119-AV119</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA118" s="10" t="e">
-        <f t="shared" ref="BA118" si="192">AS118-AW118</f>
+      <c r="BA119" s="10" t="e">
+        <f t="shared" ref="BA119" si="195">AS119-AW119</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB118" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC118" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD118" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE118" t="s">
-        <v>120</v>
-      </c>
-      <c r="BF118" t="s">
+      <c r="BB119" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC119" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD119" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE119" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF119" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare predict3dunet 1.8.2 chpt-240110-0, id07 model dataset04 heart autofluo
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93609CC5-E16B-4AE0-9FC4-D3B86667678C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252CE0CF-963A-4602-B351-792F7129A136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3678" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3716" uniqueCount="511">
   <si>
     <t>patch z</t>
   </si>
@@ -1515,9 +1515,6 @@
     <t>Success (no error &amp; sensible results)</t>
   </si>
   <si>
-    <t>240101-0</t>
-  </si>
-  <si>
     <t>Success. Open file in Fiji via plugin HDF5, then custom channel order "czyx". Using my script "h5ToTif.py" (misleading name) extracts the segmentation~ (float to int)</t>
   </si>
   <si>
@@ -1557,13 +1554,25 @@
     <t>Segment the model 231225-6 and look at 3D results. Use the specimen used for validation during model training.</t>
   </si>
   <si>
-    <t>240101-1</t>
-  </si>
-  <si>
     <t>Segment the model 231225-6 and look at 3D results. Use the specimen used for validation during model training. Use the last instead of best pytorch checkpoint, this should result in the same images as in the tensorboard statistics.</t>
   </si>
   <si>
     <t>Partial success. No error but bad segmentation, equally bad as id07 (231226-2).</t>
+  </si>
+  <si>
+    <t>240110-0</t>
+  </si>
+  <si>
+    <t>Success.</t>
+  </si>
+  <si>
+    <t>240102-1</t>
+  </si>
+  <si>
+    <t>240102-0</t>
+  </si>
+  <si>
+    <t>Segment the model 231225-6 and look at 3D results. Use the specimen used for validation during model training. Use the last pytorch checkpoint, but use it on the test specimen, not the val specimen as in the previous segmentation (240102-1).</t>
   </si>
 </sst>
 </file>
@@ -2212,10 +2221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BF119"/>
+  <dimension ref="A1:BF120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AP64" sqref="AP64"/>
+    <sheetView tabSelected="1" topLeftCell="AO94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AQ119" sqref="AQ119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2278,7 +2287,7 @@
         <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>414</v>
@@ -19366,7 +19375,7 @@
         <v>437</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C103" t="s">
         <v>403</v>
@@ -20802,7 +20811,7 @@
         <v>475</v>
       </c>
       <c r="B111" s="40" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C111" s="41" t="s">
         <v>460</v>
@@ -20984,7 +20993,7 @@
         <v>479</v>
       </c>
       <c r="B112" s="47" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C112" s="48" t="s">
         <v>480</v>
@@ -21163,7 +21172,7 @@
         <v>487</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C113" t="s">
         <v>460</v>
@@ -21181,7 +21190,7 @@
         <v>466</v>
       </c>
       <c r="H113" s="12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I113" s="6">
         <v>1</v>
@@ -21238,7 +21247,7 @@
         <v>1</v>
       </c>
       <c r="AA113">
-        <f t="shared" ref="AA113:AA118" si="175">Y113+Z113</f>
+        <f t="shared" ref="AA113:AA119" si="175">Y113+Z113</f>
         <v>6</v>
       </c>
       <c r="AB113" t="s">
@@ -21357,22 +21366,22 @@
         <v>412</v>
       </c>
       <c r="F114" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G114" s="12" t="s">
         <v>466</v>
       </c>
       <c r="H114" s="12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I114" s="6">
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <v>1</v>
+      </c>
+      <c r="K114" s="12" t="s">
         <v>499</v>
-      </c>
-      <c r="I114" s="6">
-        <v>0</v>
-      </c>
-      <c r="J114">
-        <v>1</v>
-      </c>
-      <c r="K114" s="12" t="s">
-        <v>500</v>
       </c>
       <c r="L114">
         <v>0</v>
@@ -21465,7 +21474,7 @@
     </row>
     <row r="115" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B115" s="12"/>
       <c r="C115" t="s">
@@ -21478,13 +21487,13 @@
         <v>412</v>
       </c>
       <c r="F115" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G115" s="12" t="s">
         <v>466</v>
       </c>
       <c r="H115" s="12" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I115" s="6">
         <v>0</v>
@@ -21586,10 +21595,10 @@
     </row>
     <row r="116" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C116" t="s">
         <v>480</v>
@@ -21601,13 +21610,13 @@
         <v>412</v>
       </c>
       <c r="F116" s="12" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="G116" s="12" t="s">
         <v>490</v>
       </c>
       <c r="H116" s="12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I116" s="6">
         <v>1</v>
@@ -21769,10 +21778,10 @@
     </row>
     <row r="117" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
-        <v>491</v>
+        <v>509</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C117" t="s">
         <v>480</v>
@@ -21784,13 +21793,13 @@
         <v>412</v>
       </c>
       <c r="F117" s="12" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G117" s="12" t="s">
         <v>490</v>
       </c>
       <c r="H117" s="12" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I117" s="6">
         <v>1</v>
@@ -21908,7 +21917,7 @@
         <v>8</v>
       </c>
       <c r="AU117" s="38">
-        <f t="shared" ref="AU117:AW118" si="188" xml:space="preserve"> _xlfn.FLOOR.MATH((AN117 - AQ117) / 2)</f>
+        <f t="shared" ref="AU117:AW119" si="188" xml:space="preserve"> _xlfn.FLOOR.MATH((AN117 - AQ117) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV117">
@@ -21952,10 +21961,10 @@
     </row>
     <row r="118" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C118" t="s">
         <v>480</v>
@@ -21967,28 +21976,28 @@
         <v>412</v>
       </c>
       <c r="F118" s="12" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G118" s="12" t="s">
         <v>490</v>
       </c>
       <c r="H118" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="I118" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J118" t="s">
-        <v>120</v>
+        <v>507</v>
+      </c>
+      <c r="I118" s="6">
+        <v>1</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
       </c>
       <c r="K118" t="s">
-        <v>120</v>
-      </c>
-      <c r="L118" t="s">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
       </c>
       <c r="M118" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="N118" t="s">
         <v>120</v>
@@ -22123,37 +22132,37 @@
       <c r="BC118" t="s">
         <v>163</v>
       </c>
-      <c r="BD118" t="s">
-        <v>120</v>
+      <c r="BD118">
+        <v>0</v>
       </c>
       <c r="BE118" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="BF118" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
-        <v>120</v>
+        <v>506</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>120</v>
+        <v>501</v>
       </c>
       <c r="C119" t="s">
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="D119" t="s">
-        <v>120</v>
+        <v>409</v>
       </c>
       <c r="E119" t="s">
-        <v>120</v>
+        <v>412</v>
       </c>
       <c r="F119" s="12" t="s">
-        <v>120</v>
+        <v>510</v>
       </c>
       <c r="G119" s="12" t="s">
-        <v>120</v>
+        <v>490</v>
       </c>
       <c r="H119" s="12" t="s">
         <v>120</v>
@@ -22198,7 +22207,7 @@
         <v>120</v>
       </c>
       <c r="V119" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="W119" t="s">
         <v>120</v>
@@ -22206,20 +22215,21 @@
       <c r="X119" t="s">
         <v>120</v>
       </c>
-      <c r="Y119" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA119" t="s">
-        <v>120</v>
+      <c r="Y119">
+        <v>5</v>
+      </c>
+      <c r="Z119">
+        <v>1</v>
+      </c>
+      <c r="AA119">
+        <f t="shared" si="175"/>
+        <v>6</v>
       </c>
       <c r="AB119" t="s">
         <v>120</v>
       </c>
-      <c r="AC119" t="s">
-        <v>120</v>
+      <c r="AC119">
+        <v>3</v>
       </c>
       <c r="AD119" t="s">
         <v>120</v>
@@ -22251,64 +22261,246 @@
       <c r="AM119" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AN119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP119" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS119" t="s">
-        <v>120</v>
+      <c r="AN119">
+        <v>125</v>
+      </c>
+      <c r="AO119">
+        <v>1169</v>
+      </c>
+      <c r="AP119" s="20">
+        <v>414</v>
+      </c>
+      <c r="AQ119">
+        <v>96</v>
+      </c>
+      <c r="AR119">
+        <v>768</v>
+      </c>
+      <c r="AS119">
+        <v>384</v>
       </c>
       <c r="AT119" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AU119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AW119" t="s">
-        <v>120</v>
+      <c r="AU119" s="38">
+        <f t="shared" si="188"/>
+        <v>14</v>
+      </c>
+      <c r="AV119">
+        <f t="shared" si="188"/>
+        <v>200</v>
+      </c>
+      <c r="AW119">
+        <f t="shared" si="188"/>
+        <v>15</v>
       </c>
       <c r="AX119" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY119" t="e">
+        <v>48</v>
+      </c>
+      <c r="AY119">
         <f t="shared" ref="AY119" si="194">AQ119-AU119</f>
+        <v>82</v>
+      </c>
+      <c r="AZ119">
+        <f t="shared" ref="AZ119" si="195">AR119-AV119</f>
+        <v>568</v>
+      </c>
+      <c r="BA119" s="10">
+        <f t="shared" ref="BA119" si="196">AS119-AW119</f>
+        <v>369</v>
+      </c>
+      <c r="BB119" t="s">
+        <v>484</v>
+      </c>
+      <c r="BC119" t="s">
+        <v>163</v>
+      </c>
+      <c r="BD119" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE119" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF119" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A120" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C120" t="s">
+        <v>120</v>
+      </c>
+      <c r="D120" t="s">
+        <v>120</v>
+      </c>
+      <c r="E120" t="s">
+        <v>120</v>
+      </c>
+      <c r="F120" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G120" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H120" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I120" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J120" t="s">
+        <v>120</v>
+      </c>
+      <c r="K120" t="s">
+        <v>120</v>
+      </c>
+      <c r="L120" t="s">
+        <v>120</v>
+      </c>
+      <c r="M120" t="s">
+        <v>120</v>
+      </c>
+      <c r="N120" t="s">
+        <v>120</v>
+      </c>
+      <c r="O120" t="s">
+        <v>120</v>
+      </c>
+      <c r="P120" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>120</v>
+      </c>
+      <c r="R120" t="s">
+        <v>120</v>
+      </c>
+      <c r="S120" t="s">
+        <v>120</v>
+      </c>
+      <c r="T120" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U120" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="V120" t="s">
+        <v>120</v>
+      </c>
+      <c r="W120" t="s">
+        <v>120</v>
+      </c>
+      <c r="X120" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y120" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI120" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ120" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL120" t="s">
+        <v>281</v>
+      </c>
+      <c r="AM120" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP120" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AT120" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW120" t="s">
+        <v>120</v>
+      </c>
+      <c r="AX120" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY120" t="e">
+        <f t="shared" ref="AY120" si="197">AQ120-AU120</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ119" t="e">
-        <f t="shared" ref="AZ119" si="195">AR119-AV119</f>
+      <c r="AZ120" t="e">
+        <f t="shared" ref="AZ120" si="198">AR120-AV120</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA119" s="10" t="e">
-        <f t="shared" ref="BA119" si="196">AS119-AW119</f>
+      <c r="BA120" s="10" t="e">
+        <f t="shared" ref="BA120" si="199">AS120-AW120</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB119" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC119" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD119" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE119" t="s">
-        <v>120</v>
-      </c>
-      <c r="BF119" t="s">
+      <c r="BB120" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC120" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD120" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE120" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF120" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare train3dunet 1,8,2 chpt-240111-0 and 240111-1 (3D model 10.b and 10.c) ; Thu 14:58:19 11.01.2024
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252CE0CF-963A-4602-B351-792F7129A136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F31898-4CA0-4948-B57F-F1E81A53B8D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3716" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3789" uniqueCount="521">
   <si>
     <t>patch z</t>
   </si>
@@ -1545,9 +1534,6 @@
     <t>Error. TBD</t>
   </si>
   <si>
-    <t>dataset04-3D_model10.0-chpt-231225-6-dense-heart-autofluo-multichannel</t>
-  </si>
-  <si>
     <t>dataset07.0-3D_model09.0-chpt-231225-4-dense-heart-fluo (test model)</t>
   </si>
   <si>
@@ -1573,13 +1559,46 @@
   </si>
   <si>
     <t>Segment the model 231225-6 and look at 3D results. Use the specimen used for validation during model training. Use the last pytorch checkpoint, but use it on the test specimen, not the val specimen as in the previous segmentation (240102-1).</t>
+  </si>
+  <si>
+    <t>240111-0</t>
+  </si>
+  <si>
+    <t>240111-1</t>
+  </si>
+  <si>
+    <t>dataset04.b-3D_model10.b-chpt-240111-0-dense-heart-autofluo-multichannel</t>
+  </si>
+  <si>
+    <t>dataset04.c-3D_model10.c-chpt-240111-1-dense-heart-autofluo-multichannel</t>
+  </si>
+  <si>
+    <t>dataset04.a-3D_model10.a-chpt-231225-6-dense-heart-autofluo-multichannel</t>
+  </si>
+  <si>
+    <t>Segment equivalent models like 3D model 10.a (231225-6) but with different val and test samples.</t>
+  </si>
+  <si>
+    <t>Segment equivalent models like 3D model 10.a (231225-6) but with different val and test samples than in both models, 3D model 10.a and 10.b.</t>
+  </si>
+  <si>
+    <t>dataset04.b</t>
+  </si>
+  <si>
+    <t>dataset04.c</t>
+  </si>
+  <si>
+    <t>dataset04.a</t>
+  </si>
+  <si>
+    <t>patch = same as in training of model to be compared to.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1620,6 +1639,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1833,7 +1859,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1907,6 +1933,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2221,10 +2251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BF120"/>
+  <dimension ref="A1:BF122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ119" sqref="AQ119"/>
+    <sheetView tabSelected="1" topLeftCell="AJ70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AN120" sqref="AN120:BA121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -20811,7 +20841,7 @@
         <v>475</v>
       </c>
       <c r="B111" s="40" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C111" s="41" t="s">
         <v>460</v>
@@ -20993,7 +21023,7 @@
         <v>479</v>
       </c>
       <c r="B112" s="47" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C112" s="48" t="s">
         <v>480</v>
@@ -21172,7 +21202,7 @@
         <v>487</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>501</v>
+        <v>514</v>
       </c>
       <c r="C113" t="s">
         <v>460</v>
@@ -21232,7 +21262,7 @@
         <v>120</v>
       </c>
       <c r="V113" t="s">
-        <v>164</v>
+        <v>519</v>
       </c>
       <c r="W113" t="s">
         <v>120</v>
@@ -21247,11 +21277,11 @@
         <v>1</v>
       </c>
       <c r="AA113">
-        <f t="shared" ref="AA113:AA119" si="175">Y113+Z113</f>
+        <f t="shared" ref="AA113:AA121" si="175">Y113+Z113</f>
         <v>6</v>
       </c>
-      <c r="AB113" t="s">
-        <v>120</v>
+      <c r="AB113">
+        <v>1</v>
       </c>
       <c r="AC113">
         <v>3</v>
@@ -21321,7 +21351,7 @@
         <v>15</v>
       </c>
       <c r="AX113" s="25" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="AY113">
         <f t="shared" ref="AY113:AY115" si="179">AQ113-AU113</f>
@@ -21390,7 +21420,7 @@
         <v>8</v>
       </c>
       <c r="V114" t="s">
-        <v>164</v>
+        <v>519</v>
       </c>
       <c r="Y114">
         <v>5</v>
@@ -21401,6 +21431,9 @@
       <c r="AA114">
         <f t="shared" si="175"/>
         <v>6</v>
+      </c>
+      <c r="AB114">
+        <v>1</v>
       </c>
       <c r="AC114">
         <v>3</v>
@@ -21511,7 +21544,7 @@
         <v>8</v>
       </c>
       <c r="V115" t="s">
-        <v>164</v>
+        <v>519</v>
       </c>
       <c r="Y115">
         <v>5</v>
@@ -21522,6 +21555,9 @@
       <c r="AA115">
         <f t="shared" si="175"/>
         <v>6</v>
+      </c>
+      <c r="AB115">
+        <v>1</v>
       </c>
       <c r="AC115">
         <v>3</v>
@@ -21598,7 +21634,7 @@
         <v>497</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>501</v>
+        <v>514</v>
       </c>
       <c r="C116" t="s">
         <v>480</v>
@@ -21658,7 +21694,7 @@
         <v>120</v>
       </c>
       <c r="V116" t="s">
-        <v>164</v>
+        <v>519</v>
       </c>
       <c r="W116" t="s">
         <v>120</v>
@@ -21676,8 +21712,8 @@
         <f t="shared" si="175"/>
         <v>6</v>
       </c>
-      <c r="AB116" t="s">
-        <v>120</v>
+      <c r="AB116">
+        <v>1</v>
       </c>
       <c r="AC116">
         <v>3</v>
@@ -21778,10 +21814,10 @@
     </row>
     <row r="117" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>501</v>
+        <v>514</v>
       </c>
       <c r="C117" t="s">
         <v>480</v>
@@ -21793,13 +21829,13 @@
         <v>412</v>
       </c>
       <c r="F117" s="12" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G117" s="12" t="s">
         <v>490</v>
       </c>
       <c r="H117" s="12" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I117" s="6">
         <v>1</v>
@@ -21841,7 +21877,7 @@
         <v>120</v>
       </c>
       <c r="V117" t="s">
-        <v>164</v>
+        <v>519</v>
       </c>
       <c r="W117" t="s">
         <v>120</v>
@@ -21859,8 +21895,8 @@
         <f t="shared" si="175"/>
         <v>6</v>
       </c>
-      <c r="AB117" t="s">
-        <v>120</v>
+      <c r="AB117">
+        <v>1</v>
       </c>
       <c r="AC117">
         <v>3</v>
@@ -21917,7 +21953,7 @@
         <v>8</v>
       </c>
       <c r="AU117" s="38">
-        <f t="shared" ref="AU117:AW119" si="188" xml:space="preserve"> _xlfn.FLOOR.MATH((AN117 - AQ117) / 2)</f>
+        <f t="shared" ref="AU117:AW121" si="188" xml:space="preserve"> _xlfn.FLOOR.MATH((AN117 - AQ117) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV117">
@@ -21961,10 +21997,10 @@
     </row>
     <row r="118" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>501</v>
+        <v>514</v>
       </c>
       <c r="C118" t="s">
         <v>480</v>
@@ -21976,13 +22012,13 @@
         <v>412</v>
       </c>
       <c r="F118" s="12" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G118" s="12" t="s">
         <v>490</v>
       </c>
       <c r="H118" s="12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I118" s="6">
         <v>1</v>
@@ -22024,7 +22060,7 @@
         <v>120</v>
       </c>
       <c r="V118" t="s">
-        <v>164</v>
+        <v>519</v>
       </c>
       <c r="W118" t="s">
         <v>120</v>
@@ -22042,8 +22078,8 @@
         <f t="shared" si="175"/>
         <v>6</v>
       </c>
-      <c r="AB118" t="s">
-        <v>120</v>
+      <c r="AB118">
+        <v>1</v>
       </c>
       <c r="AC118">
         <v>3</v>
@@ -22144,10 +22180,10 @@
     </row>
     <row r="119" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>501</v>
+        <v>514</v>
       </c>
       <c r="C119" t="s">
         <v>480</v>
@@ -22159,28 +22195,28 @@
         <v>412</v>
       </c>
       <c r="F119" s="12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G119" s="12" t="s">
         <v>490</v>
       </c>
       <c r="H119" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="I119" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J119" t="s">
-        <v>120</v>
+        <v>506</v>
+      </c>
+      <c r="I119" s="6">
+        <v>1</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
       </c>
       <c r="K119" t="s">
-        <v>120</v>
-      </c>
-      <c r="L119" t="s">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
       </c>
       <c r="M119" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="N119" t="s">
         <v>120</v>
@@ -22207,7 +22243,7 @@
         <v>120</v>
       </c>
       <c r="V119" t="s">
-        <v>164</v>
+        <v>519</v>
       </c>
       <c r="W119" t="s">
         <v>120</v>
@@ -22225,8 +22261,8 @@
         <f t="shared" si="175"/>
         <v>6</v>
       </c>
-      <c r="AB119" t="s">
-        <v>120</v>
+      <c r="AB119">
+        <v>1</v>
       </c>
       <c r="AC119">
         <v>3</v>
@@ -22315,34 +22351,34 @@
       <c r="BC119" t="s">
         <v>163</v>
       </c>
-      <c r="BD119" t="s">
-        <v>120</v>
+      <c r="BD119">
+        <v>0</v>
       </c>
       <c r="BE119" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="BF119" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
-        <v>120</v>
+        <v>510</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>120</v>
+        <v>512</v>
       </c>
       <c r="C120" t="s">
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="D120" t="s">
-        <v>120</v>
+        <v>409</v>
       </c>
       <c r="E120" t="s">
-        <v>120</v>
+        <v>412</v>
       </c>
       <c r="F120" s="12" t="s">
-        <v>120</v>
+        <v>515</v>
       </c>
       <c r="G120" s="12" t="s">
         <v>120</v>
@@ -22390,7 +22426,7 @@
         <v>120</v>
       </c>
       <c r="V120" t="s">
-        <v>120</v>
+        <v>517</v>
       </c>
       <c r="W120" t="s">
         <v>120</v>
@@ -22398,20 +22434,21 @@
       <c r="X120" t="s">
         <v>120</v>
       </c>
-      <c r="Y120" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC120" t="s">
-        <v>120</v>
+      <c r="Y120">
+        <v>5</v>
+      </c>
+      <c r="Z120">
+        <v>1</v>
+      </c>
+      <c r="AA120">
+        <f t="shared" si="175"/>
+        <v>6</v>
+      </c>
+      <c r="AB120">
+        <v>1</v>
+      </c>
+      <c r="AC120">
+        <v>3</v>
       </c>
       <c r="AD120" t="s">
         <v>120</v>
@@ -22443,64 +22480,429 @@
       <c r="AM120" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AN120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP120" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AT120" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AW120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AX120" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY120" t="e">
+      <c r="AN120">
+        <v>125</v>
+      </c>
+      <c r="AO120">
+        <v>1169</v>
+      </c>
+      <c r="AP120" s="20">
+        <v>414</v>
+      </c>
+      <c r="AQ120" s="3">
+        <v>96</v>
+      </c>
+      <c r="AR120" s="3">
+        <v>768</v>
+      </c>
+      <c r="AS120" s="3">
+        <v>384</v>
+      </c>
+      <c r="AT120" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU120" s="54">
+        <f t="shared" si="188"/>
+        <v>14</v>
+      </c>
+      <c r="AV120" s="3">
+        <f t="shared" si="188"/>
+        <v>200</v>
+      </c>
+      <c r="AW120" s="3">
+        <f t="shared" si="188"/>
+        <v>15</v>
+      </c>
+      <c r="AX120" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY120">
         <f t="shared" ref="AY120" si="197">AQ120-AU120</f>
+        <v>82</v>
+      </c>
+      <c r="AZ120">
+        <f t="shared" ref="AZ120" si="198">AR120-AV120</f>
+        <v>568</v>
+      </c>
+      <c r="BA120" s="10">
+        <f t="shared" ref="BA120" si="199">AS120-AW120</f>
+        <v>369</v>
+      </c>
+      <c r="BB120" t="s">
+        <v>520</v>
+      </c>
+      <c r="BC120" t="s">
+        <v>163</v>
+      </c>
+      <c r="BD120" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE120" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF120" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A121" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="B121" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="C121" t="s">
+        <v>480</v>
+      </c>
+      <c r="D121" t="s">
+        <v>409</v>
+      </c>
+      <c r="E121" t="s">
+        <v>412</v>
+      </c>
+      <c r="F121" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="G121" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H121" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I121" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J121" t="s">
+        <v>120</v>
+      </c>
+      <c r="K121" t="s">
+        <v>120</v>
+      </c>
+      <c r="L121" t="s">
+        <v>120</v>
+      </c>
+      <c r="M121" t="s">
+        <v>120</v>
+      </c>
+      <c r="N121" t="s">
+        <v>120</v>
+      </c>
+      <c r="O121" t="s">
+        <v>120</v>
+      </c>
+      <c r="P121" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q121" t="s">
+        <v>120</v>
+      </c>
+      <c r="R121" t="s">
+        <v>120</v>
+      </c>
+      <c r="S121" t="s">
+        <v>120</v>
+      </c>
+      <c r="T121" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U121" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="V121" t="s">
+        <v>518</v>
+      </c>
+      <c r="W121" t="s">
+        <v>120</v>
+      </c>
+      <c r="X121" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y121">
+        <v>5</v>
+      </c>
+      <c r="Z121">
+        <v>1</v>
+      </c>
+      <c r="AA121">
+        <f t="shared" si="175"/>
+        <v>6</v>
+      </c>
+      <c r="AB121">
+        <v>1</v>
+      </c>
+      <c r="AC121">
+        <v>3</v>
+      </c>
+      <c r="AD121" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE121" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF121" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG121" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH121" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI121" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ121" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK121" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL121" t="s">
+        <v>281</v>
+      </c>
+      <c r="AM121" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN121">
+        <v>125</v>
+      </c>
+      <c r="AO121">
+        <v>1169</v>
+      </c>
+      <c r="AP121" s="20">
+        <v>414</v>
+      </c>
+      <c r="AQ121" s="3">
+        <v>96</v>
+      </c>
+      <c r="AR121" s="3">
+        <v>768</v>
+      </c>
+      <c r="AS121" s="3">
+        <v>384</v>
+      </c>
+      <c r="AT121" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU121" s="54">
+        <f t="shared" si="188"/>
+        <v>14</v>
+      </c>
+      <c r="AV121" s="3">
+        <f t="shared" si="188"/>
+        <v>200</v>
+      </c>
+      <c r="AW121" s="3">
+        <f t="shared" si="188"/>
+        <v>15</v>
+      </c>
+      <c r="AX121" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY121">
+        <f t="shared" ref="AY121" si="200">AQ121-AU121</f>
+        <v>82</v>
+      </c>
+      <c r="AZ121">
+        <f t="shared" ref="AZ121" si="201">AR121-AV121</f>
+        <v>568</v>
+      </c>
+      <c r="BA121" s="10">
+        <f t="shared" ref="BA121" si="202">AS121-AW121</f>
+        <v>369</v>
+      </c>
+      <c r="BB121" t="s">
+        <v>520</v>
+      </c>
+      <c r="BC121" t="s">
+        <v>163</v>
+      </c>
+      <c r="BD121" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE121" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF121" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A122" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B122" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C122" t="s">
+        <v>120</v>
+      </c>
+      <c r="D122" t="s">
+        <v>120</v>
+      </c>
+      <c r="E122" t="s">
+        <v>120</v>
+      </c>
+      <c r="F122" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G122" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H122" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I122" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J122" t="s">
+        <v>120</v>
+      </c>
+      <c r="K122" t="s">
+        <v>120</v>
+      </c>
+      <c r="L122" t="s">
+        <v>120</v>
+      </c>
+      <c r="M122" t="s">
+        <v>120</v>
+      </c>
+      <c r="N122" t="s">
+        <v>120</v>
+      </c>
+      <c r="O122" t="s">
+        <v>120</v>
+      </c>
+      <c r="P122" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q122" t="s">
+        <v>120</v>
+      </c>
+      <c r="R122" t="s">
+        <v>120</v>
+      </c>
+      <c r="S122" t="s">
+        <v>120</v>
+      </c>
+      <c r="T122" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U122" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="V122" t="s">
+        <v>120</v>
+      </c>
+      <c r="W122" t="s">
+        <v>120</v>
+      </c>
+      <c r="X122" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y122" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI122" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ122" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL122" t="s">
+        <v>281</v>
+      </c>
+      <c r="AM122" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP122" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AT122" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW122" t="s">
+        <v>120</v>
+      </c>
+      <c r="AX122" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY122" t="e">
+        <f t="shared" ref="AY122" si="203">AQ122-AU122</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ120" t="e">
-        <f t="shared" ref="AZ120" si="198">AR120-AV120</f>
+      <c r="AZ122" t="e">
+        <f t="shared" ref="AZ122" si="204">AR122-AV122</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA120" s="10" t="e">
-        <f t="shared" ref="BA120" si="199">AS120-AW120</f>
+      <c r="BA122" s="10" t="e">
+        <f t="shared" ref="BA122" si="205">AS122-AW122</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB120" t="s">
-        <v>120</v>
-      </c>
-      <c r="BC120" t="s">
-        <v>120</v>
-      </c>
-      <c r="BD120" t="s">
-        <v>120</v>
-      </c>
-      <c r="BE120" t="s">
-        <v>120</v>
-      </c>
-      <c r="BF120" t="s">
+      <c r="BB122" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC122" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD122" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE122" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF122" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix an error related to mamba loading
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F31898-4CA0-4948-B57F-F1E81A53B8D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083091B9-6377-4C56-8176-9A3BCA1623B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2253,8 +2264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BF122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN120" sqref="AN120:BA121"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
prepare predict3dunet 1,8,2 chpt-240115-0 to 240115-3 ; Mon 11:42:34 15.01.2024
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526E54D7-4F4F-4072-B8CC-8E62BECD588D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA98489A-C005-4448-9A0A-23AED7455B87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3798" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3757" uniqueCount="531">
   <si>
     <t>patch z</t>
   </si>
@@ -1609,6 +1598,114 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>240115-0</t>
+  </si>
+  <si>
+    <t>240115-1</t>
+  </si>
+  <si>
+    <t>240115-2</t>
+  </si>
+  <si>
+    <t>240115-3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segment 3D model 10.b </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">last </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkpoint on val &amp; test images</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segment 3D model 10.b </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">best </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkpoint on val &amp; test images</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segment 3D model 10.c </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">best </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkpoint on val &amp; test images</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segment 3D model 10.c </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">last </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkpoint on val &amp; test images</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1676,7 +1773,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1872,11 +1969,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1954,6 +2136,36 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2268,19 +2480,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BF123"/>
+  <dimension ref="A1:BF126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121:B122"/>
+    <sheetView tabSelected="1" topLeftCell="J77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V125" sqref="V125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1"/>
     <col min="3" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" customWidth="1"/>
-    <col min="6" max="6" width="28" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="57" style="63" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="24.85546875" customWidth="1" outlineLevel="1"/>
     <col min="8" max="8" width="64.5703125" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="14.5703125" style="6" customWidth="1" outlineLevel="1"/>
@@ -2346,7 +2558,7 @@
       <c r="E1" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="62" t="s">
         <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -2519,7 +2731,7 @@
       <c r="E2" t="s">
         <v>412</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="63" t="s">
         <v>127</v>
       </c>
       <c r="G2" t="s">
@@ -2687,7 +2899,7 @@
       <c r="E3" t="s">
         <v>412</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="63" t="s">
         <v>127</v>
       </c>
       <c r="G3" t="s">
@@ -2856,7 +3068,7 @@
       <c r="E4" s="8" t="s">
         <v>412</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="64" t="s">
         <v>121</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -3024,7 +3236,7 @@
       <c r="E5" t="s">
         <v>412</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="63" t="s">
         <v>122</v>
       </c>
       <c r="G5" t="s">
@@ -3189,7 +3401,7 @@
       <c r="E6" t="s">
         <v>412</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="63" t="s">
         <v>84</v>
       </c>
       <c r="G6" t="s">
@@ -3354,7 +3566,7 @@
       <c r="E7" t="s">
         <v>412</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="63" t="s">
         <v>85</v>
       </c>
       <c r="G7" t="s">
@@ -3519,7 +3731,7 @@
       <c r="E8" t="s">
         <v>412</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="63" t="s">
         <v>88</v>
       </c>
       <c r="G8" t="s">
@@ -3684,7 +3896,7 @@
       <c r="E9" t="s">
         <v>412</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="63" t="s">
         <v>122</v>
       </c>
       <c r="G9" t="s">
@@ -3855,7 +4067,7 @@
       <c r="E10" t="s">
         <v>412</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="63" t="s">
         <v>90</v>
       </c>
       <c r="G10" t="s">
@@ -4020,7 +4232,7 @@
       <c r="E11" t="s">
         <v>412</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="63" t="s">
         <v>95</v>
       </c>
       <c r="G11" t="s">
@@ -4185,7 +4397,7 @@
       <c r="E12" t="s">
         <v>412</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="63" t="s">
         <v>96</v>
       </c>
       <c r="G12" t="s">
@@ -4351,7 +4563,7 @@
       <c r="E13" t="s">
         <v>412</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="63" t="s">
         <v>39</v>
       </c>
       <c r="G13" t="s">
@@ -4516,7 +4728,7 @@
       <c r="E14" t="s">
         <v>412</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="63" t="s">
         <v>40</v>
       </c>
       <c r="G14" t="s">
@@ -4681,7 +4893,7 @@
       <c r="E15" t="s">
         <v>412</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="63" t="s">
         <v>41</v>
       </c>
       <c r="G15" t="s">
@@ -4847,7 +5059,7 @@
       <c r="E16" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="65" t="s">
         <v>42</v>
       </c>
       <c r="G16" s="4" t="s">
@@ -5014,7 +5226,7 @@
       <c r="E17" t="s">
         <v>412</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="63" t="s">
         <v>60</v>
       </c>
       <c r="G17" t="s">
@@ -5180,7 +5392,7 @@
       <c r="E18" t="s">
         <v>412</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="63" t="s">
         <v>60</v>
       </c>
       <c r="G18" t="s">
@@ -5346,7 +5558,7 @@
       <c r="E19" t="s">
         <v>412</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="63" t="s">
         <v>61</v>
       </c>
       <c r="G19" t="s">
@@ -5512,7 +5724,7 @@
       <c r="E20" t="s">
         <v>412</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="63" t="s">
         <v>61</v>
       </c>
       <c r="G20" t="s">
@@ -5678,7 +5890,7 @@
       <c r="E21" t="s">
         <v>412</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="63" t="s">
         <v>62</v>
       </c>
       <c r="G21" t="s">
@@ -5844,7 +6056,7 @@
       <c r="E22" t="s">
         <v>412</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="63" t="s">
         <v>62</v>
       </c>
       <c r="G22" t="s">
@@ -6010,7 +6222,7 @@
       <c r="E23" t="s">
         <v>412</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="63" t="s">
         <v>63</v>
       </c>
       <c r="G23" t="s">
@@ -6176,7 +6388,7 @@
       <c r="E24" t="s">
         <v>412</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="63" t="s">
         <v>63</v>
       </c>
       <c r="G24" t="s">
@@ -6336,7 +6548,7 @@
       <c r="C25" t="s">
         <v>8</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="63" t="s">
         <v>8</v>
       </c>
       <c r="G25" t="s">
@@ -6503,7 +6715,7 @@
       <c r="C26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="65" t="s">
         <v>8</v>
       </c>
       <c r="G26" s="4" t="s">
@@ -6676,7 +6888,7 @@
       <c r="E27" t="s">
         <v>412</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="63" t="s">
         <v>123</v>
       </c>
       <c r="G27" t="s">
@@ -6846,7 +7058,7 @@
       <c r="E28" t="s">
         <v>412</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="63" t="s">
         <v>145</v>
       </c>
       <c r="G28" t="s">
@@ -7015,7 +7227,7 @@
       <c r="E29" t="s">
         <v>412</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="63" t="s">
         <v>124</v>
       </c>
       <c r="G29" t="s">
@@ -7185,7 +7397,7 @@
       <c r="E30" t="s">
         <v>412</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="63" t="s">
         <v>153</v>
       </c>
       <c r="G30" t="s">
@@ -7355,7 +7567,7 @@
       <c r="E31" t="s">
         <v>412</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="63" t="s">
         <v>146</v>
       </c>
       <c r="G31" t="s">
@@ -7525,7 +7737,7 @@
       <c r="E32" t="s">
         <v>412</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="63" t="s">
         <v>156</v>
       </c>
       <c r="G32" t="s">
@@ -7694,7 +7906,7 @@
       <c r="E33" t="s">
         <v>412</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="63" t="s">
         <v>170</v>
       </c>
       <c r="G33" t="s">
@@ -7863,7 +8075,7 @@
       <c r="E34" t="s">
         <v>412</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="63" t="s">
         <v>166</v>
       </c>
       <c r="G34" t="s">
@@ -8032,7 +8244,7 @@
       <c r="E35" t="s">
         <v>412</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="63" t="s">
         <v>179</v>
       </c>
       <c r="G35" t="s">
@@ -8201,7 +8413,7 @@
       <c r="E36" t="s">
         <v>412</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="63" t="s">
         <v>181</v>
       </c>
       <c r="G36" t="s">
@@ -8370,7 +8582,7 @@
       <c r="E37" t="s">
         <v>412</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="63" t="s">
         <v>187</v>
       </c>
       <c r="G37" t="s">
@@ -8539,7 +8751,7 @@
       <c r="E38" t="s">
         <v>412</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="63" t="s">
         <v>192</v>
       </c>
       <c r="G38" t="s">
@@ -8708,7 +8920,7 @@
       <c r="E39" t="s">
         <v>412</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="63" t="s">
         <v>195</v>
       </c>
       <c r="G39" t="s">
@@ -8877,7 +9089,7 @@
       <c r="E40" t="s">
         <v>412</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="63" t="s">
         <v>195</v>
       </c>
       <c r="G40" t="s">
@@ -9046,7 +9258,7 @@
       <c r="E41" t="s">
         <v>412</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="63" t="s">
         <v>195</v>
       </c>
       <c r="G41" t="s">
@@ -9215,7 +9427,7 @@
       <c r="E42" t="s">
         <v>412</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="63" t="s">
         <v>195</v>
       </c>
       <c r="G42" t="s">
@@ -9384,7 +9596,7 @@
       <c r="E43" t="s">
         <v>412</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="63" t="s">
         <v>195</v>
       </c>
       <c r="G43" t="s">
@@ -9553,7 +9765,7 @@
       <c r="E44" t="s">
         <v>412</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="63" t="s">
         <v>195</v>
       </c>
       <c r="G44" t="s">
@@ -9723,7 +9935,7 @@
       <c r="E45" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="65" t="s">
         <v>207</v>
       </c>
       <c r="G45" s="4" t="s">
@@ -9895,7 +10107,7 @@
       <c r="E46" t="s">
         <v>412</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F46" s="66" t="s">
         <v>212</v>
       </c>
       <c r="I46" s="15">
@@ -10060,7 +10272,7 @@
       <c r="E47" t="s">
         <v>412</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="F47" s="66" t="s">
         <v>213</v>
       </c>
       <c r="I47" s="15">
@@ -10225,7 +10437,7 @@
       <c r="E48" t="s">
         <v>412</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F48" s="66" t="s">
         <v>214</v>
       </c>
       <c r="I48" s="15">
@@ -10390,7 +10602,7 @@
       <c r="E49" t="s">
         <v>412</v>
       </c>
-      <c r="F49" s="12" t="s">
+      <c r="F49" s="66" t="s">
         <v>215</v>
       </c>
       <c r="I49" s="15">
@@ -10555,7 +10767,7 @@
       <c r="E50" t="s">
         <v>412</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="66" t="s">
         <v>216</v>
       </c>
       <c r="I50" s="15">
@@ -10720,7 +10932,7 @@
       <c r="E51" t="s">
         <v>412</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F51" s="66" t="s">
         <v>217</v>
       </c>
       <c r="I51" s="15">
@@ -10885,7 +11097,7 @@
       <c r="E52" t="s">
         <v>412</v>
       </c>
-      <c r="F52" s="12" t="s">
+      <c r="F52" s="66" t="s">
         <v>218</v>
       </c>
       <c r="I52" s="15">
@@ -11050,7 +11262,7 @@
       <c r="E53" t="s">
         <v>412</v>
       </c>
-      <c r="F53" s="12" t="s">
+      <c r="F53" s="66" t="s">
         <v>219</v>
       </c>
       <c r="I53" s="15">
@@ -11215,7 +11427,7 @@
       <c r="E54" t="s">
         <v>412</v>
       </c>
-      <c r="F54" s="12" t="s">
+      <c r="F54" s="66" t="s">
         <v>220</v>
       </c>
       <c r="I54" s="15">
@@ -11380,7 +11592,7 @@
       <c r="E55" t="s">
         <v>412</v>
       </c>
-      <c r="F55" s="12" t="s">
+      <c r="F55" s="66" t="s">
         <v>221</v>
       </c>
       <c r="I55" s="15">
@@ -11545,7 +11757,7 @@
       <c r="E56" t="s">
         <v>412</v>
       </c>
-      <c r="F56" s="12" t="s">
+      <c r="F56" s="66" t="s">
         <v>222</v>
       </c>
       <c r="I56" s="15">
@@ -11710,7 +11922,7 @@
       <c r="E57" t="s">
         <v>412</v>
       </c>
-      <c r="F57" s="12" t="s">
+      <c r="F57" s="66" t="s">
         <v>223</v>
       </c>
       <c r="I57" s="15">
@@ -11875,7 +12087,7 @@
       <c r="E58" t="s">
         <v>412</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F58" s="66" t="s">
         <v>224</v>
       </c>
       <c r="I58" s="15">
@@ -12040,7 +12252,7 @@
       <c r="E59" t="s">
         <v>412</v>
       </c>
-      <c r="F59" s="12" t="s">
+      <c r="F59" s="66" t="s">
         <v>225</v>
       </c>
       <c r="I59" s="15">
@@ -12205,7 +12417,7 @@
       <c r="E60" t="s">
         <v>412</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F60" s="66" t="s">
         <v>226</v>
       </c>
       <c r="I60" s="15">
@@ -12370,7 +12582,7 @@
       <c r="E61" t="s">
         <v>412</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F61" s="66" t="s">
         <v>227</v>
       </c>
       <c r="I61" s="15">
@@ -12535,7 +12747,7 @@
       <c r="E62" t="s">
         <v>412</v>
       </c>
-      <c r="F62" s="12" t="s">
+      <c r="F62" s="66" t="s">
         <v>228</v>
       </c>
       <c r="I62" s="15">
@@ -12700,7 +12912,7 @@
       <c r="E63" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="F63" s="17" t="s">
+      <c r="F63" s="67" t="s">
         <v>229</v>
       </c>
       <c r="I63" s="18">
@@ -12866,7 +13078,7 @@
       <c r="E64" s="32" t="s">
         <v>412</v>
       </c>
-      <c r="F64" s="31" t="s">
+      <c r="F64" s="68" t="s">
         <v>273</v>
       </c>
       <c r="G64" s="32" t="s">
@@ -13036,7 +13248,7 @@
       <c r="E65" t="s">
         <v>412</v>
       </c>
-      <c r="F65" s="12" t="s">
+      <c r="F65" s="66" t="s">
         <v>275</v>
       </c>
       <c r="G65" t="s">
@@ -13213,7 +13425,7 @@
       <c r="E66" t="s">
         <v>412</v>
       </c>
-      <c r="F66" s="12" t="s">
+      <c r="F66" s="66" t="s">
         <v>278</v>
       </c>
       <c r="G66" s="12" t="s">
@@ -13390,7 +13602,7 @@
       <c r="E67" t="s">
         <v>412</v>
       </c>
-      <c r="F67" s="12" t="s">
+      <c r="F67" s="66" t="s">
         <v>312</v>
       </c>
       <c r="G67" s="12" t="s">
@@ -13567,7 +13779,7 @@
       <c r="E68" t="s">
         <v>412</v>
       </c>
-      <c r="F68" s="12" t="s">
+      <c r="F68" s="66" t="s">
         <v>313</v>
       </c>
       <c r="G68" s="12" t="s">
@@ -13744,7 +13956,7 @@
       <c r="E69" t="s">
         <v>412</v>
       </c>
-      <c r="F69" s="12" t="s">
+      <c r="F69" s="66" t="s">
         <v>315</v>
       </c>
       <c r="G69" s="12" t="s">
@@ -13921,7 +14133,7 @@
       <c r="E70" t="s">
         <v>412</v>
       </c>
-      <c r="F70" s="12" t="s">
+      <c r="F70" s="66" t="s">
         <v>315</v>
       </c>
       <c r="G70" s="12" t="s">
@@ -14101,7 +14313,7 @@
       <c r="E71" t="s">
         <v>412</v>
       </c>
-      <c r="F71" s="12" t="s">
+      <c r="F71" s="66" t="s">
         <v>316</v>
       </c>
       <c r="G71" s="12" t="s">
@@ -14278,7 +14490,7 @@
       <c r="E72" t="s">
         <v>412</v>
       </c>
-      <c r="F72" s="12" t="s">
+      <c r="F72" s="66" t="s">
         <v>315</v>
       </c>
       <c r="G72" s="12" t="s">
@@ -14455,7 +14667,7 @@
       <c r="E73" t="s">
         <v>412</v>
       </c>
-      <c r="F73" s="12" t="s">
+      <c r="F73" s="66" t="s">
         <v>313</v>
       </c>
       <c r="G73" s="12" t="s">
@@ -14635,7 +14847,7 @@
       <c r="E74" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="F74" s="17" t="s">
+      <c r="F74" s="67" t="s">
         <v>313</v>
       </c>
       <c r="G74" s="17" t="s">
@@ -14812,7 +15024,7 @@
       <c r="E75" t="s">
         <v>412</v>
       </c>
-      <c r="F75" s="12" t="s">
+      <c r="F75" s="66" t="s">
         <v>335</v>
       </c>
       <c r="G75" s="12" t="s">
@@ -14986,7 +15198,7 @@
       <c r="E76" t="s">
         <v>412</v>
       </c>
-      <c r="F76" s="12" t="s">
+      <c r="F76" s="66" t="s">
         <v>346</v>
       </c>
       <c r="G76" s="12" t="s">
@@ -15178,7 +15390,7 @@
       <c r="E79" t="s">
         <v>412</v>
       </c>
-      <c r="F79" s="12" t="s">
+      <c r="F79" s="66" t="s">
         <v>355</v>
       </c>
       <c r="G79" s="12" t="s">
@@ -15352,7 +15564,7 @@
       <c r="E80" t="s">
         <v>412</v>
       </c>
-      <c r="F80" s="12" t="s">
+      <c r="F80" s="66" t="s">
         <v>365</v>
       </c>
       <c r="G80" s="12" t="s">
@@ -15529,7 +15741,7 @@
       <c r="E81" t="s">
         <v>412</v>
       </c>
-      <c r="F81" s="12" t="s">
+      <c r="F81" s="66" t="s">
         <v>369</v>
       </c>
       <c r="G81" s="12" t="s">
@@ -15706,7 +15918,7 @@
       <c r="E82" t="s">
         <v>412</v>
       </c>
-      <c r="F82" s="12" t="s">
+      <c r="F82" s="66" t="s">
         <v>388</v>
       </c>
       <c r="G82" s="12" t="s">
@@ -15883,7 +16095,7 @@
       <c r="E83" t="s">
         <v>412</v>
       </c>
-      <c r="F83" s="12" t="s">
+      <c r="F83" s="66" t="s">
         <v>388</v>
       </c>
       <c r="G83" s="12" t="s">
@@ -16060,7 +16272,7 @@
       <c r="E84" t="s">
         <v>412</v>
       </c>
-      <c r="F84" s="12" t="s">
+      <c r="F84" s="66" t="s">
         <v>388</v>
       </c>
       <c r="G84" s="12" t="s">
@@ -16237,7 +16449,7 @@
       <c r="E85" t="s">
         <v>412</v>
       </c>
-      <c r="F85" s="12" t="s">
+      <c r="F85" s="66" t="s">
         <v>388</v>
       </c>
       <c r="G85" s="12" t="s">
@@ -16414,7 +16626,7 @@
       <c r="E86" t="s">
         <v>412</v>
       </c>
-      <c r="F86" s="12" t="s">
+      <c r="F86" s="66" t="s">
         <v>389</v>
       </c>
       <c r="G86" s="12" t="s">
@@ -16591,7 +16803,7 @@
       <c r="E87" t="s">
         <v>412</v>
       </c>
-      <c r="F87" s="12" t="s">
+      <c r="F87" s="66" t="s">
         <v>389</v>
       </c>
       <c r="G87" s="12" t="s">
@@ -16768,7 +16980,7 @@
       <c r="E88" t="s">
         <v>412</v>
       </c>
-      <c r="F88" s="12" t="s">
+      <c r="F88" s="66" t="s">
         <v>389</v>
       </c>
       <c r="G88" s="12" t="s">
@@ -16945,7 +17157,7 @@
       <c r="E89" t="s">
         <v>412</v>
       </c>
-      <c r="F89" s="12" t="s">
+      <c r="F89" s="66" t="s">
         <v>389</v>
       </c>
       <c r="G89" s="12" t="s">
@@ -17122,7 +17334,7 @@
       <c r="E90" t="s">
         <v>412</v>
       </c>
-      <c r="F90" s="12" t="s">
+      <c r="F90" s="66" t="s">
         <v>390</v>
       </c>
       <c r="G90" s="12" t="s">
@@ -17299,7 +17511,7 @@
       <c r="E91" t="s">
         <v>412</v>
       </c>
-      <c r="F91" s="12" t="s">
+      <c r="F91" s="66" t="s">
         <v>390</v>
       </c>
       <c r="G91" s="12" t="s">
@@ -17476,7 +17688,7 @@
       <c r="E92" t="s">
         <v>412</v>
       </c>
-      <c r="F92" s="12" t="s">
+      <c r="F92" s="66" t="s">
         <v>390</v>
       </c>
       <c r="G92" s="12" t="s">
@@ -17653,7 +17865,7 @@
       <c r="E93" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="F93" s="17" t="s">
+      <c r="F93" s="67" t="s">
         <v>390</v>
       </c>
       <c r="G93" s="17" t="s">
@@ -17830,7 +18042,7 @@
       <c r="E94" t="s">
         <v>412</v>
       </c>
-      <c r="F94" s="12" t="s">
+      <c r="F94" s="66" t="s">
         <v>407</v>
       </c>
       <c r="G94" s="12" t="s">
@@ -18007,7 +18219,7 @@
       <c r="E95" t="s">
         <v>412</v>
       </c>
-      <c r="F95" s="12" t="s">
+      <c r="F95" s="66" t="s">
         <v>408</v>
       </c>
       <c r="G95" s="12" t="s">
@@ -18184,7 +18396,7 @@
       <c r="E96" t="s">
         <v>412</v>
       </c>
-      <c r="F96" s="12" t="s">
+      <c r="F96" s="66" t="s">
         <v>425</v>
       </c>
       <c r="G96" s="12" t="s">
@@ -18361,7 +18573,7 @@
       <c r="E97" t="s">
         <v>412</v>
       </c>
-      <c r="F97" s="12" t="s">
+      <c r="F97" s="66" t="s">
         <v>423</v>
       </c>
       <c r="G97" s="12" t="s">
@@ -18538,7 +18750,7 @@
       <c r="E98" t="s">
         <v>412</v>
       </c>
-      <c r="F98" s="12" t="s">
+      <c r="F98" s="66" t="s">
         <v>424</v>
       </c>
       <c r="G98" s="12" t="s">
@@ -18715,7 +18927,7 @@
       <c r="E99" t="s">
         <v>412</v>
       </c>
-      <c r="F99" s="12" t="s">
+      <c r="F99" s="66" t="s">
         <v>426</v>
       </c>
       <c r="G99" s="12" t="s">
@@ -18892,7 +19104,7 @@
       <c r="E100" t="s">
         <v>412</v>
       </c>
-      <c r="F100" s="12" t="s">
+      <c r="F100" s="66" t="s">
         <v>440</v>
       </c>
       <c r="G100" s="12" t="s">
@@ -19072,7 +19284,7 @@
       <c r="E101" t="s">
         <v>412</v>
       </c>
-      <c r="F101" s="12" t="s">
+      <c r="F101" s="66" t="s">
         <v>443</v>
       </c>
       <c r="G101" s="12" t="s">
@@ -19252,7 +19464,7 @@
       <c r="E102" t="s">
         <v>433</v>
       </c>
-      <c r="F102" s="12" t="s">
+      <c r="F102" s="66" t="s">
         <v>441</v>
       </c>
       <c r="G102" s="12" t="s">
@@ -19434,7 +19646,7 @@
       <c r="E103" t="s">
         <v>412</v>
       </c>
-      <c r="F103" s="12" t="s">
+      <c r="F103" s="66" t="s">
         <v>442</v>
       </c>
       <c r="G103" s="12" t="s">
@@ -19616,7 +19828,7 @@
       <c r="E104" t="s">
         <v>412</v>
       </c>
-      <c r="F104" s="12" t="s">
+      <c r="F104" s="66" t="s">
         <v>444</v>
       </c>
       <c r="G104" s="12" t="s">
@@ -19798,7 +20010,7 @@
       <c r="E105" t="s">
         <v>433</v>
       </c>
-      <c r="F105" s="12" t="s">
+      <c r="F105" s="66" t="s">
         <v>445</v>
       </c>
       <c r="G105" s="12" t="s">
@@ -19980,7 +20192,7 @@
       <c r="E106" t="s">
         <v>412</v>
       </c>
-      <c r="F106" s="12" t="s">
+      <c r="F106" s="66" t="s">
         <v>464</v>
       </c>
       <c r="G106" s="12" t="s">
@@ -20162,7 +20374,7 @@
       <c r="E107" t="s">
         <v>412</v>
       </c>
-      <c r="F107" s="12" t="s">
+      <c r="F107" s="66" t="s">
         <v>467</v>
       </c>
       <c r="G107" s="12" t="s">
@@ -20341,7 +20553,7 @@
       <c r="E108" t="s">
         <v>412</v>
       </c>
-      <c r="F108" s="12" t="s">
+      <c r="F108" s="66" t="s">
         <v>461</v>
       </c>
       <c r="G108" s="12" t="s">
@@ -20523,7 +20735,7 @@
       <c r="E109" t="s">
         <v>412</v>
       </c>
-      <c r="F109" s="12" t="s">
+      <c r="F109" s="66" t="s">
         <v>471</v>
       </c>
       <c r="G109" s="12" t="s">
@@ -20702,7 +20914,7 @@
       <c r="E110" t="s">
         <v>412</v>
       </c>
-      <c r="F110" s="12" t="s">
+      <c r="F110" s="66" t="s">
         <v>474</v>
       </c>
       <c r="G110" s="12" t="s">
@@ -20884,7 +21096,7 @@
       <c r="E111" s="41" t="s">
         <v>412</v>
       </c>
-      <c r="F111" s="40" t="s">
+      <c r="F111" s="69" t="s">
         <v>478</v>
       </c>
       <c r="G111" s="40" t="s">
@@ -21066,7 +21278,7 @@
       <c r="E112" s="48" t="s">
         <v>412</v>
       </c>
-      <c r="F112" s="47" t="s">
+      <c r="F112" s="70" t="s">
         <v>481</v>
       </c>
       <c r="G112" s="47" t="s">
@@ -21245,7 +21457,7 @@
       <c r="E113" t="s">
         <v>412</v>
       </c>
-      <c r="F113" s="12" t="s">
+      <c r="F113" s="66" t="s">
         <v>489</v>
       </c>
       <c r="G113" s="12" t="s">
@@ -21290,8 +21502,8 @@
       <c r="T113" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="U113" s="20" t="s">
-        <v>120</v>
+      <c r="U113" s="20">
+        <v>1</v>
       </c>
       <c r="V113" t="s">
         <v>517</v>
@@ -21383,7 +21595,7 @@
         <v>15</v>
       </c>
       <c r="AX113" s="25" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="AY113">
         <f t="shared" ref="AY113:AY115" si="179">AQ113-AU113</f>
@@ -21429,7 +21641,7 @@
       <c r="E114" t="s">
         <v>412</v>
       </c>
-      <c r="F114" s="12" t="s">
+      <c r="F114" s="66" t="s">
         <v>493</v>
       </c>
       <c r="G114" s="12" t="s">
@@ -21509,7 +21721,7 @@
         <v>15</v>
       </c>
       <c r="AX114" s="20" t="s">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="AY114">
         <f t="shared" si="179"/>
@@ -21555,7 +21767,7 @@
       <c r="E115" t="s">
         <v>412</v>
       </c>
-      <c r="F115" s="12" t="s">
+      <c r="F115" s="66" t="s">
         <v>493</v>
       </c>
       <c r="G115" s="12" t="s">
@@ -21635,7 +21847,7 @@
         <v>15</v>
       </c>
       <c r="AX115" s="20" t="s">
-        <v>120</v>
+        <v>48</v>
       </c>
       <c r="AY115">
         <f t="shared" si="179"/>
@@ -21681,7 +21893,7 @@
       <c r="E116" t="s">
         <v>412</v>
       </c>
-      <c r="F116" s="12" t="s">
+      <c r="F116" s="66" t="s">
         <v>493</v>
       </c>
       <c r="G116" s="12" t="s">
@@ -21705,38 +21917,9 @@
       <c r="M116" t="s">
         <v>8</v>
       </c>
-      <c r="N116" t="s">
-        <v>120</v>
-      </c>
-      <c r="O116" t="s">
-        <v>120</v>
-      </c>
-      <c r="P116" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q116" t="s">
-        <v>120</v>
-      </c>
-      <c r="R116" t="s">
-        <v>120</v>
-      </c>
-      <c r="S116" t="s">
-        <v>120</v>
-      </c>
-      <c r="T116" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="U116" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="T116" s="12"/>
       <c r="V116" t="s">
         <v>517</v>
-      </c>
-      <c r="W116" t="s">
-        <v>120</v>
-      </c>
-      <c r="X116" t="s">
-        <v>120</v>
       </c>
       <c r="Y116">
         <v>5</v>
@@ -21754,33 +21937,7 @@
       <c r="AC116">
         <v>3</v>
       </c>
-      <c r="AD116" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE116" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF116" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG116" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH116" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI116" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ116" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK116" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL116" t="s">
-        <v>281</v>
-      </c>
+      <c r="AJ116" s="12"/>
       <c r="AM116" s="10" t="s">
         <v>108</v>
       </c>
@@ -21864,7 +22021,7 @@
       <c r="E117" t="s">
         <v>412</v>
       </c>
-      <c r="F117" s="12" t="s">
+      <c r="F117" s="66" t="s">
         <v>502</v>
       </c>
       <c r="G117" s="12" t="s">
@@ -21888,38 +22045,9 @@
       <c r="M117" t="s">
         <v>8</v>
       </c>
-      <c r="N117" t="s">
-        <v>120</v>
-      </c>
-      <c r="O117" t="s">
-        <v>120</v>
-      </c>
-      <c r="P117" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q117" t="s">
-        <v>120</v>
-      </c>
-      <c r="R117" t="s">
-        <v>120</v>
-      </c>
-      <c r="S117" t="s">
-        <v>120</v>
-      </c>
-      <c r="T117" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="U117" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="T117" s="12"/>
       <c r="V117" t="s">
         <v>517</v>
-      </c>
-      <c r="W117" t="s">
-        <v>120</v>
-      </c>
-      <c r="X117" t="s">
-        <v>120</v>
       </c>
       <c r="Y117">
         <v>5</v>
@@ -21937,33 +22065,7 @@
       <c r="AC117">
         <v>3</v>
       </c>
-      <c r="AD117" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE117" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF117" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG117" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH117" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI117" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ117" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK117" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL117" t="s">
-        <v>281</v>
-      </c>
+      <c r="AJ117" s="12"/>
       <c r="AM117" s="10" t="s">
         <v>108</v>
       </c>
@@ -22047,7 +22149,7 @@
       <c r="E118" t="s">
         <v>412</v>
       </c>
-      <c r="F118" s="12" t="s">
+      <c r="F118" s="66" t="s">
         <v>503</v>
       </c>
       <c r="G118" s="12" t="s">
@@ -22071,38 +22173,9 @@
       <c r="M118" t="s">
         <v>8</v>
       </c>
-      <c r="N118" t="s">
-        <v>120</v>
-      </c>
-      <c r="O118" t="s">
-        <v>120</v>
-      </c>
-      <c r="P118" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q118" t="s">
-        <v>120</v>
-      </c>
-      <c r="R118" t="s">
-        <v>120</v>
-      </c>
-      <c r="S118" t="s">
-        <v>120</v>
-      </c>
-      <c r="T118" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="U118" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="T118" s="12"/>
       <c r="V118" t="s">
         <v>517</v>
-      </c>
-      <c r="W118" t="s">
-        <v>120</v>
-      </c>
-      <c r="X118" t="s">
-        <v>120</v>
       </c>
       <c r="Y118">
         <v>5</v>
@@ -22120,33 +22193,7 @@
       <c r="AC118">
         <v>3</v>
       </c>
-      <c r="AD118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI118" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ118" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK118" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL118" t="s">
-        <v>281</v>
-      </c>
+      <c r="AJ118" s="12"/>
       <c r="AM118" s="10" t="s">
         <v>108</v>
       </c>
@@ -22230,7 +22277,7 @@
       <c r="E119" t="s">
         <v>412</v>
       </c>
-      <c r="F119" s="12" t="s">
+      <c r="F119" s="66" t="s">
         <v>509</v>
       </c>
       <c r="G119" s="12" t="s">
@@ -22254,38 +22301,9 @@
       <c r="M119" t="s">
         <v>8</v>
       </c>
-      <c r="N119" t="s">
-        <v>120</v>
-      </c>
-      <c r="O119" t="s">
-        <v>120</v>
-      </c>
-      <c r="P119" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q119" t="s">
-        <v>120</v>
-      </c>
-      <c r="R119" t="s">
-        <v>120</v>
-      </c>
-      <c r="S119" t="s">
-        <v>120</v>
-      </c>
-      <c r="T119" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="U119" s="20" t="s">
-        <v>120</v>
-      </c>
+      <c r="T119" s="12"/>
       <c r="V119" t="s">
         <v>517</v>
-      </c>
-      <c r="W119" t="s">
-        <v>120</v>
-      </c>
-      <c r="X119" t="s">
-        <v>120</v>
       </c>
       <c r="Y119">
         <v>5</v>
@@ -22303,33 +22321,7 @@
       <c r="AC119">
         <v>3</v>
       </c>
-      <c r="AD119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI119" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ119" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK119" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL119" t="s">
-        <v>281</v>
-      </c>
+      <c r="AJ119" s="12"/>
       <c r="AM119" s="10" t="s">
         <v>108</v>
       </c>
@@ -22405,7 +22397,7 @@
         <v>512</v>
       </c>
       <c r="C120" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="D120" t="s">
         <v>409</v>
@@ -22413,62 +22405,42 @@
       <c r="E120" t="s">
         <v>412</v>
       </c>
-      <c r="F120" s="12" t="s">
+      <c r="F120" s="66" t="s">
         <v>520</v>
       </c>
       <c r="G120" s="12" t="s">
         <v>519</v>
       </c>
       <c r="H120" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="I120" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J120" t="s">
-        <v>120</v>
+        <v>506</v>
+      </c>
+      <c r="I120" s="6">
+        <v>1</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
       </c>
       <c r="K120" t="s">
-        <v>120</v>
-      </c>
-      <c r="L120" t="s">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
       </c>
       <c r="M120" t="s">
-        <v>120</v>
-      </c>
-      <c r="N120" t="s">
-        <v>120</v>
-      </c>
-      <c r="O120" t="s">
-        <v>120</v>
-      </c>
-      <c r="P120" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q120" t="s">
-        <v>120</v>
-      </c>
-      <c r="R120" t="s">
-        <v>120</v>
-      </c>
-      <c r="S120" t="s">
-        <v>120</v>
-      </c>
-      <c r="T120" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="U120" s="20" t="s">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="T120" s="12"/>
+      <c r="U120" s="20">
+        <v>1</v>
       </c>
       <c r="V120" t="s">
         <v>515</v>
       </c>
-      <c r="W120" t="s">
-        <v>120</v>
-      </c>
-      <c r="X120" t="s">
-        <v>120</v>
+      <c r="W120">
+        <v>6</v>
+      </c>
+      <c r="X120">
+        <v>6</v>
       </c>
       <c r="Y120">
         <v>5</v>
@@ -22486,29 +22458,15 @@
       <c r="AC120">
         <v>3</v>
       </c>
-      <c r="AD120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH120" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI120" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ120" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK120" t="s">
-        <v>120</v>
+      <c r="AI120" s="6">
+        <v>77597</v>
+      </c>
+      <c r="AJ120" s="12">
+        <v>3455</v>
+      </c>
+      <c r="AK120">
+        <f>AI120+AJ120</f>
+        <v>81052</v>
       </c>
       <c r="AL120" t="s">
         <v>281</v>
@@ -22525,32 +22483,32 @@
       <c r="AP120" s="20">
         <v>414</v>
       </c>
-      <c r="AQ120" s="3">
+      <c r="AQ120" s="55">
         <v>96</v>
       </c>
-      <c r="AR120" s="3">
+      <c r="AR120" s="55">
         <v>768</v>
       </c>
-      <c r="AS120" s="3">
+      <c r="AS120" s="55">
         <v>384</v>
       </c>
-      <c r="AT120" s="53" t="s">
+      <c r="AT120" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="AU120" s="54">
+      <c r="AU120" s="56">
         <f t="shared" si="188"/>
         <v>14</v>
       </c>
-      <c r="AV120" s="3">
+      <c r="AV120" s="55">
         <f t="shared" si="188"/>
         <v>200</v>
       </c>
-      <c r="AW120" s="3">
+      <c r="AW120" s="55">
         <f t="shared" si="188"/>
         <v>15</v>
       </c>
-      <c r="AX120" s="53" t="s">
-        <v>48</v>
+      <c r="AX120" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="AY120">
         <f t="shared" ref="AY120" si="197">AQ120-AU120</f>
@@ -22570,14 +22528,14 @@
       <c r="BC120" t="s">
         <v>163</v>
       </c>
-      <c r="BD120" t="s">
-        <v>120</v>
+      <c r="BD120">
+        <v>0</v>
       </c>
       <c r="BE120" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="BF120" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="1:58" x14ac:dyDescent="0.25">
@@ -22588,7 +22546,7 @@
         <v>513</v>
       </c>
       <c r="C121" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="D121" t="s">
         <v>409</v>
@@ -22596,62 +22554,42 @@
       <c r="E121" t="s">
         <v>412</v>
       </c>
-      <c r="F121" s="12" t="s">
+      <c r="F121" s="66" t="s">
         <v>521</v>
       </c>
       <c r="G121" s="12" t="s">
         <v>519</v>
       </c>
       <c r="H121" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="I121" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J121" t="s">
-        <v>120</v>
+        <v>506</v>
+      </c>
+      <c r="I121" s="6">
+        <v>1</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
       </c>
       <c r="K121" t="s">
-        <v>120</v>
-      </c>
-      <c r="L121" t="s">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
       </c>
       <c r="M121" t="s">
-        <v>120</v>
-      </c>
-      <c r="N121" t="s">
-        <v>120</v>
-      </c>
-      <c r="O121" t="s">
-        <v>120</v>
-      </c>
-      <c r="P121" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q121" t="s">
-        <v>120</v>
-      </c>
-      <c r="R121" t="s">
-        <v>120</v>
-      </c>
-      <c r="S121" t="s">
-        <v>120</v>
-      </c>
-      <c r="T121" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="U121" s="20" t="s">
-        <v>120</v>
+        <v>8</v>
+      </c>
+      <c r="T121" s="12"/>
+      <c r="U121" s="20">
+        <v>1</v>
       </c>
       <c r="V121" t="s">
         <v>516</v>
       </c>
-      <c r="W121" t="s">
-        <v>120</v>
-      </c>
-      <c r="X121" t="s">
-        <v>120</v>
+      <c r="W121">
+        <v>6</v>
+      </c>
+      <c r="X121">
+        <v>6</v>
       </c>
       <c r="Y121">
         <v>5</v>
@@ -22669,29 +22607,15 @@
       <c r="AC121">
         <v>3</v>
       </c>
-      <c r="AD121" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE121" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF121" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG121" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH121" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI121" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ121" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK121" t="s">
-        <v>120</v>
+      <c r="AI121" s="6">
+        <v>77597</v>
+      </c>
+      <c r="AJ121" s="12">
+        <v>3455</v>
+      </c>
+      <c r="AK121">
+        <f>AI121+AJ121</f>
+        <v>81052</v>
       </c>
       <c r="AL121" t="s">
         <v>281</v>
@@ -22708,32 +22632,32 @@
       <c r="AP121" s="20">
         <v>414</v>
       </c>
-      <c r="AQ121" s="3">
+      <c r="AQ121" s="55">
         <v>96</v>
       </c>
-      <c r="AR121" s="3">
+      <c r="AR121" s="55">
         <v>768</v>
       </c>
-      <c r="AS121" s="3">
+      <c r="AS121" s="55">
         <v>384</v>
       </c>
-      <c r="AT121" s="53" t="s">
+      <c r="AT121" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="AU121" s="54">
+      <c r="AU121" s="56">
         <f t="shared" si="188"/>
         <v>14</v>
       </c>
-      <c r="AV121" s="3">
+      <c r="AV121" s="55">
         <f t="shared" si="188"/>
         <v>200</v>
       </c>
-      <c r="AW121" s="3">
+      <c r="AW121" s="55">
         <f t="shared" si="188"/>
         <v>15</v>
       </c>
-      <c r="AX121" s="53" t="s">
-        <v>48</v>
+      <c r="AX121" s="25" t="s">
+        <v>8</v>
       </c>
       <c r="AY121">
         <f t="shared" ref="AY121" si="200">AQ121-AU121</f>
@@ -22753,37 +22677,37 @@
       <c r="BC121" t="s">
         <v>163</v>
       </c>
-      <c r="BD121" t="s">
-        <v>120</v>
+      <c r="BD121">
+        <v>0</v>
       </c>
       <c r="BE121" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="BF121" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
-        <v>120</v>
+        <v>523</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>120</v>
+        <v>512</v>
       </c>
       <c r="C122" t="s">
-        <v>120</v>
+        <v>480</v>
       </c>
       <c r="D122" t="s">
-        <v>120</v>
+        <v>409</v>
       </c>
       <c r="E122" t="s">
-        <v>120</v>
-      </c>
-      <c r="F122" s="12" t="s">
-        <v>120</v>
+        <v>412</v>
+      </c>
+      <c r="F122" s="66" t="s">
+        <v>528</v>
       </c>
       <c r="G122" s="12" t="s">
-        <v>120</v>
+        <v>466</v>
       </c>
       <c r="H122" s="12" t="s">
         <v>120</v>
@@ -22803,134 +22727,86 @@
       <c r="M122" t="s">
         <v>120</v>
       </c>
-      <c r="N122" t="s">
-        <v>120</v>
-      </c>
-      <c r="O122" t="s">
-        <v>120</v>
-      </c>
-      <c r="P122" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q122" t="s">
-        <v>120</v>
-      </c>
-      <c r="R122" t="s">
-        <v>120</v>
-      </c>
-      <c r="S122" t="s">
-        <v>120</v>
-      </c>
-      <c r="T122" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="U122" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="V122" t="s">
-        <v>120</v>
-      </c>
-      <c r="W122" t="s">
-        <v>120</v>
-      </c>
-      <c r="X122" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y122" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AH122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AI122" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="AJ122" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL122" t="s">
-        <v>281</v>
-      </c>
+      <c r="T122" s="12"/>
+      <c r="V122" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="W122">
+        <v>1</v>
+      </c>
+      <c r="Y122">
+        <v>5</v>
+      </c>
+      <c r="Z122">
+        <v>1</v>
+      </c>
+      <c r="AA122">
+        <f t="shared" ref="AA122" si="203">Y122+Z122</f>
+        <v>6</v>
+      </c>
+      <c r="AB122">
+        <v>1</v>
+      </c>
+      <c r="AC122">
+        <v>3</v>
+      </c>
+      <c r="AJ122" s="12"/>
       <c r="AM122" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AN122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AO122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AP122" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AQ122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AR122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AT122" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AV122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AW122" t="s">
-        <v>120</v>
-      </c>
-      <c r="AX122" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY122" t="e">
-        <f t="shared" ref="AY122" si="203">AQ122-AU122</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ122" t="e">
-        <f t="shared" ref="AZ122" si="204">AR122-AV122</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA122" s="10" t="e">
-        <f t="shared" ref="BA122" si="205">AS122-AW122</f>
-        <v>#VALUE!</v>
+      <c r="AN122">
+        <v>125</v>
+      </c>
+      <c r="AO122">
+        <v>1169</v>
+      </c>
+      <c r="AP122" s="20">
+        <v>414</v>
+      </c>
+      <c r="AQ122" s="59">
+        <v>96</v>
+      </c>
+      <c r="AR122" s="60">
+        <v>768</v>
+      </c>
+      <c r="AS122" s="60">
+        <v>384</v>
+      </c>
+      <c r="AT122" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU122" s="59">
+        <f t="shared" ref="AU122" si="204" xml:space="preserve"> _xlfn.FLOOR.MATH((AN122 - AQ122) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AV122" s="60">
+        <f t="shared" ref="AV122" si="205" xml:space="preserve"> _xlfn.FLOOR.MATH((AO122 - AR122) / 2)</f>
+        <v>200</v>
+      </c>
+      <c r="AW122" s="60">
+        <f t="shared" ref="AW122" si="206" xml:space="preserve"> _xlfn.FLOOR.MATH((AP122 - AS122) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AX122" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY122">
+        <f t="shared" ref="AY122" si="207">AQ122-AU122</f>
+        <v>82</v>
+      </c>
+      <c r="AZ122">
+        <f t="shared" ref="AZ122" si="208">AR122-AV122</f>
+        <v>568</v>
+      </c>
+      <c r="BA122" s="10">
+        <f t="shared" ref="BA122" si="209">AS122-AW122</f>
+        <v>369</v>
       </c>
       <c r="BB122" t="s">
-        <v>120</v>
+        <v>484</v>
       </c>
       <c r="BC122" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
       <c r="BD122" t="s">
         <v>120</v>
@@ -22943,7 +22819,553 @@
       </c>
     </row>
     <row r="123" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="F123" s="12"/>
+      <c r="A123" s="12" t="s">
+        <v>524</v>
+      </c>
+      <c r="B123" s="12" t="s">
+        <v>512</v>
+      </c>
+      <c r="C123" t="s">
+        <v>480</v>
+      </c>
+      <c r="D123" t="s">
+        <v>409</v>
+      </c>
+      <c r="E123" t="s">
+        <v>412</v>
+      </c>
+      <c r="F123" s="66" t="s">
+        <v>527</v>
+      </c>
+      <c r="G123" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="H123" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I123" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J123" t="s">
+        <v>120</v>
+      </c>
+      <c r="K123" t="s">
+        <v>120</v>
+      </c>
+      <c r="L123" t="s">
+        <v>120</v>
+      </c>
+      <c r="M123" t="s">
+        <v>120</v>
+      </c>
+      <c r="T123" s="12"/>
+      <c r="V123" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="W123">
+        <v>1</v>
+      </c>
+      <c r="Y123">
+        <v>5</v>
+      </c>
+      <c r="Z123">
+        <v>1</v>
+      </c>
+      <c r="AA123">
+        <f t="shared" ref="AA123" si="210">Y123+Z123</f>
+        <v>6</v>
+      </c>
+      <c r="AB123">
+        <v>1</v>
+      </c>
+      <c r="AC123">
+        <v>3</v>
+      </c>
+      <c r="AJ123" s="12"/>
+      <c r="AM123" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN123">
+        <v>125</v>
+      </c>
+      <c r="AO123">
+        <v>1169</v>
+      </c>
+      <c r="AP123" s="20">
+        <v>414</v>
+      </c>
+      <c r="AQ123" s="57">
+        <v>96</v>
+      </c>
+      <c r="AR123" s="1">
+        <v>768</v>
+      </c>
+      <c r="AS123" s="1">
+        <v>384</v>
+      </c>
+      <c r="AT123" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU123" s="57">
+        <f t="shared" ref="AU122:AU125" si="211" xml:space="preserve"> _xlfn.FLOOR.MATH((AN123 - AQ123) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AV123" s="1">
+        <f t="shared" ref="AV122:AV125" si="212" xml:space="preserve"> _xlfn.FLOOR.MATH((AO123 - AR123) / 2)</f>
+        <v>200</v>
+      </c>
+      <c r="AW123" s="1">
+        <f t="shared" ref="AW122:AW125" si="213" xml:space="preserve"> _xlfn.FLOOR.MATH((AP123 - AS123) / 2)</f>
+        <v>15</v>
+      </c>
+      <c r="AX123" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY123">
+        <f t="shared" ref="AY123" si="214">AQ123-AU123</f>
+        <v>82</v>
+      </c>
+      <c r="AZ123">
+        <f t="shared" ref="AZ123" si="215">AR123-AV123</f>
+        <v>568</v>
+      </c>
+      <c r="BA123" s="10">
+        <f t="shared" ref="BA123" si="216">AS123-AW123</f>
+        <v>369</v>
+      </c>
+      <c r="BB123" t="s">
+        <v>484</v>
+      </c>
+      <c r="BC123" t="s">
+        <v>163</v>
+      </c>
+      <c r="BD123" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE123" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF123" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A124" s="12" t="s">
+        <v>525</v>
+      </c>
+      <c r="B124" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="C124" t="s">
+        <v>480</v>
+      </c>
+      <c r="D124" t="s">
+        <v>409</v>
+      </c>
+      <c r="E124" t="s">
+        <v>412</v>
+      </c>
+      <c r="F124" s="66" t="s">
+        <v>529</v>
+      </c>
+      <c r="G124" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="H124" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I124" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J124" t="s">
+        <v>120</v>
+      </c>
+      <c r="K124" t="s">
+        <v>120</v>
+      </c>
+      <c r="L124" t="s">
+        <v>120</v>
+      </c>
+      <c r="M124" t="s">
+        <v>120</v>
+      </c>
+      <c r="T124" s="12"/>
+      <c r="V124" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="W124">
+        <v>1</v>
+      </c>
+      <c r="Y124">
+        <v>5</v>
+      </c>
+      <c r="Z124">
+        <v>1</v>
+      </c>
+      <c r="AA124">
+        <f t="shared" ref="AA124:AA125" si="217">Y124+Z124</f>
+        <v>6</v>
+      </c>
+      <c r="AB124">
+        <v>1</v>
+      </c>
+      <c r="AC124">
+        <v>3</v>
+      </c>
+      <c r="AJ124" s="12"/>
+      <c r="AM124" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN124">
+        <v>125</v>
+      </c>
+      <c r="AO124">
+        <v>1169</v>
+      </c>
+      <c r="AP124" s="20">
+        <v>414</v>
+      </c>
+      <c r="AQ124" s="3">
+        <v>96</v>
+      </c>
+      <c r="AR124" s="3">
+        <v>768</v>
+      </c>
+      <c r="AS124" s="3">
+        <v>384</v>
+      </c>
+      <c r="AT124" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU124" s="54">
+        <f t="shared" si="211"/>
+        <v>14</v>
+      </c>
+      <c r="AV124" s="3">
+        <f t="shared" si="212"/>
+        <v>200</v>
+      </c>
+      <c r="AW124" s="3">
+        <f t="shared" si="213"/>
+        <v>15</v>
+      </c>
+      <c r="AX124" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY124">
+        <f t="shared" ref="AY124" si="218">AQ124-AU124</f>
+        <v>82</v>
+      </c>
+      <c r="AZ124">
+        <f t="shared" ref="AZ124" si="219">AR124-AV124</f>
+        <v>568</v>
+      </c>
+      <c r="BA124" s="10">
+        <f t="shared" ref="BA124" si="220">AS124-AW124</f>
+        <v>369</v>
+      </c>
+      <c r="BB124" t="s">
+        <v>484</v>
+      </c>
+      <c r="BC124" t="s">
+        <v>163</v>
+      </c>
+      <c r="BD124" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE124" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF124" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="125" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A125" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="B125" s="12" t="s">
+        <v>513</v>
+      </c>
+      <c r="C125" t="s">
+        <v>480</v>
+      </c>
+      <c r="D125" t="s">
+        <v>409</v>
+      </c>
+      <c r="E125" t="s">
+        <v>412</v>
+      </c>
+      <c r="F125" s="66" t="s">
+        <v>530</v>
+      </c>
+      <c r="G125" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="H125" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J125" t="s">
+        <v>120</v>
+      </c>
+      <c r="K125" t="s">
+        <v>120</v>
+      </c>
+      <c r="L125" t="s">
+        <v>120</v>
+      </c>
+      <c r="M125" t="s">
+        <v>120</v>
+      </c>
+      <c r="T125" s="12"/>
+      <c r="V125" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="W125">
+        <v>1</v>
+      </c>
+      <c r="Y125">
+        <v>5</v>
+      </c>
+      <c r="Z125">
+        <v>1</v>
+      </c>
+      <c r="AA125">
+        <f t="shared" si="217"/>
+        <v>6</v>
+      </c>
+      <c r="AB125">
+        <v>1</v>
+      </c>
+      <c r="AC125">
+        <v>3</v>
+      </c>
+      <c r="AJ125" s="12"/>
+      <c r="AM125" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN125">
+        <v>125</v>
+      </c>
+      <c r="AO125">
+        <v>1169</v>
+      </c>
+      <c r="AP125" s="20">
+        <v>414</v>
+      </c>
+      <c r="AQ125" s="57">
+        <v>96</v>
+      </c>
+      <c r="AR125" s="1">
+        <v>768</v>
+      </c>
+      <c r="AS125" s="1">
+        <v>384</v>
+      </c>
+      <c r="AT125" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU125" s="57">
+        <f t="shared" si="211"/>
+        <v>14</v>
+      </c>
+      <c r="AV125" s="1">
+        <f t="shared" si="212"/>
+        <v>200</v>
+      </c>
+      <c r="AW125" s="1">
+        <f t="shared" si="213"/>
+        <v>15</v>
+      </c>
+      <c r="AX125" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY125">
+        <f t="shared" ref="AY125" si="221">AQ125-AU125</f>
+        <v>82</v>
+      </c>
+      <c r="AZ125">
+        <f t="shared" ref="AZ125" si="222">AR125-AV125</f>
+        <v>568</v>
+      </c>
+      <c r="BA125" s="10">
+        <f t="shared" ref="BA125" si="223">AS125-AW125</f>
+        <v>369</v>
+      </c>
+      <c r="BB125" t="s">
+        <v>484</v>
+      </c>
+      <c r="BC125" t="s">
+        <v>163</v>
+      </c>
+      <c r="BD125" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE125" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF125" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A126" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C126" t="s">
+        <v>120</v>
+      </c>
+      <c r="D126" t="s">
+        <v>120</v>
+      </c>
+      <c r="E126" t="s">
+        <v>120</v>
+      </c>
+      <c r="F126" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="G126" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H126" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="I126" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="J126" t="s">
+        <v>120</v>
+      </c>
+      <c r="K126" t="s">
+        <v>120</v>
+      </c>
+      <c r="L126" t="s">
+        <v>120</v>
+      </c>
+      <c r="M126" t="s">
+        <v>120</v>
+      </c>
+      <c r="T126" s="12"/>
+      <c r="V126" t="s">
+        <v>120</v>
+      </c>
+      <c r="W126" t="s">
+        <v>120</v>
+      </c>
+      <c r="X126" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y126" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI126" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ126" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL126" t="s">
+        <v>281</v>
+      </c>
+      <c r="AM126" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AP126" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AS126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AT126" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AV126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AW126" t="s">
+        <v>120</v>
+      </c>
+      <c r="AX126" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY126" t="e">
+        <f t="shared" ref="AY126" si="224">AQ126-AU126</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ126" t="e">
+        <f t="shared" ref="AZ126" si="225">AR126-AV126</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA126" s="10" t="e">
+        <f t="shared" ref="BA126" si="226">AS126-AW126</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB126" t="s">
+        <v>120</v>
+      </c>
+      <c r="BC126" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD126" t="s">
+        <v>120</v>
+      </c>
+      <c r="BE126" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF126" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
prepare train3dunet 1.8.2 chpt-240123-0 to -3, varying LR factor
varying LR factor from 0.5 to 0.8 in steps of 0.1
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B3AF9C-FCA1-4716-A162-FFF36B77C95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B3C7E7-CB07-4794-9347-B1D9F0CFE4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="28680" yWindow="2565" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1737,7 +1737,7 @@
     <t>res. X (min)</t>
   </si>
   <si>
-    <t>patch: … max dz-ROI = 136 (id06)</t>
+    <t>patch = 2^3 &gt; max dz-ROI = 136 (id06)</t>
   </si>
 </sst>
 </file>
@@ -2512,68 +2512,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BF127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BC127" sqref="BC127"/>
+    <sheetView tabSelected="1" topLeftCell="AH106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AV127" sqref="AV127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
-    <col min="3" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" customWidth="1"/>
+    <col min="3" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
     <col min="6" max="6" width="57" style="61" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="24.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="64.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.5546875" style="6" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="8.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="9.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="64.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.5703125" style="6" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1" outlineLevel="1"/>
     <col min="13" max="13" width="33" customWidth="1"/>
-    <col min="14" max="20" width="9.109375" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="9.109375" style="20"/>
-    <col min="22" max="22" width="12.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="9.109375" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="6.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="5.109375" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="11.109375" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="20" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="9.140625" style="20"/>
+    <col min="22" max="22" width="12.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="6.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="5.140625" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="11.140625" customWidth="1" outlineLevel="1"/>
     <col min="28" max="28" width="6" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="14.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="9.5546875" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="14.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="9.5703125" customWidth="1" outlineLevel="1"/>
     <col min="31" max="31" width="9" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="9.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="9.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="9.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="16.6640625" style="6" customWidth="1"/>
-    <col min="36" max="37" width="14.88671875" customWidth="1"/>
+    <col min="32" max="32" width="9.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="9.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="9.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="16.7109375" style="6" customWidth="1"/>
+    <col min="36" max="37" width="14.85546875" customWidth="1"/>
     <col min="38" max="38" width="21" customWidth="1"/>
-    <col min="39" max="39" width="26.33203125" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="10.77734375" customWidth="1"/>
-    <col min="41" max="41" width="10.5546875" customWidth="1"/>
-    <col min="42" max="42" width="10.88671875" style="20" customWidth="1"/>
-    <col min="43" max="43" width="5.33203125" customWidth="1"/>
-    <col min="44" max="44" width="6.109375" customWidth="1"/>
+    <col min="39" max="39" width="26.28515625" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="10.7109375" customWidth="1"/>
+    <col min="41" max="41" width="10.5703125" customWidth="1"/>
+    <col min="42" max="42" width="10.85546875" style="20" customWidth="1"/>
+    <col min="43" max="43" width="5.28515625" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" customWidth="1"/>
     <col min="45" max="45" width="5" customWidth="1"/>
     <col min="46" max="46" width="5" style="20" customWidth="1"/>
-    <col min="47" max="47" width="6.109375" customWidth="1"/>
-    <col min="48" max="48" width="6.5546875" customWidth="1"/>
+    <col min="47" max="47" width="6.140625" customWidth="1"/>
+    <col min="48" max="48" width="6.5703125" customWidth="1"/>
     <col min="49" max="49" width="5" customWidth="1"/>
     <col min="50" max="50" width="6" style="20" customWidth="1"/>
     <col min="51" max="52" width="6" customWidth="1"/>
     <col min="53" max="53" width="6" style="10" customWidth="1"/>
-    <col min="54" max="54" width="74.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="76.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="5.109375" customWidth="1"/>
-    <col min="57" max="57" width="135.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="74.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="76.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="5.140625" customWidth="1"/>
+    <col min="57" max="57" width="135.28515625" customWidth="1" outlineLevel="1"/>
     <col min="58" max="58" width="206" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.6640625" customWidth="1"/>
-    <col min="63" max="63" width="12.109375" customWidth="1"/>
+    <col min="59" max="59" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.7109375" customWidth="1"/>
+    <col min="63" max="63" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:58" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>51</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -4250,7 +4250,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>99</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -7076,7 +7076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -7585,7 +7585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -7924,7 +7924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -8093,7 +8093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -8262,7 +8262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -8431,7 +8431,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>180</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -8769,7 +8769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>191</v>
       </c>
@@ -9107,7 +9107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>195</v>
       </c>
@@ -9276,7 +9276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>196</v>
       </c>
@@ -9445,7 +9445,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>198</v>
       </c>
@@ -9614,7 +9614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>201</v>
       </c>
@@ -9783,7 +9783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>202</v>
       </c>
@@ -9953,7 +9953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>203</v>
       </c>
@@ -10124,7 +10124,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>235</v>
       </c>
@@ -10289,7 +10289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>236</v>
       </c>
@@ -10454,7 +10454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>237</v>
       </c>
@@ -10619,7 +10619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>238</v>
       </c>
@@ -10784,7 +10784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>239</v>
       </c>
@@ -10949,7 +10949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>240</v>
       </c>
@@ -11114,7 +11114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>241</v>
       </c>
@@ -11279,7 +11279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>242</v>
       </c>
@@ -11444,7 +11444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>243</v>
       </c>
@@ -11609,7 +11609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>244</v>
       </c>
@@ -11774,7 +11774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>245</v>
       </c>
@@ -11939,7 +11939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>246</v>
       </c>
@@ -12104,7 +12104,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>247</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>248</v>
       </c>
@@ -12434,7 +12434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>249</v>
       </c>
@@ -12599,7 +12599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>250</v>
       </c>
@@ -12764,7 +12764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>251</v>
       </c>
@@ -12929,7 +12929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>252</v>
       </c>
@@ -13095,7 +13095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:58" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:58" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
         <v>267</v>
       </c>
@@ -13265,7 +13265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>269</v>
       </c>
@@ -13442,7 +13442,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="66" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>274</v>
       </c>
@@ -13619,7 +13619,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="67" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>289</v>
       </c>
@@ -13796,7 +13796,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="68" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>292</v>
       </c>
@@ -13973,7 +13973,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>293</v>
       </c>
@@ -14150,7 +14150,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>298</v>
       </c>
@@ -14330,7 +14330,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>299</v>
       </c>
@@ -14507,7 +14507,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="72" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>302</v>
       </c>
@@ -14684,7 +14684,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="73" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>321</v>
       </c>
@@ -14864,7 +14864,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>323</v>
       </c>
@@ -15041,7 +15041,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="75" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>331</v>
       </c>
@@ -15215,7 +15215,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="76" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>334</v>
       </c>
@@ -15389,7 +15389,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="77" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>350</v>
       </c>
@@ -15398,7 +15398,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="78" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>350</v>
       </c>
@@ -15407,7 +15407,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>351</v>
       </c>
@@ -15581,7 +15581,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="80" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>361</v>
       </c>
@@ -15758,7 +15758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>365</v>
       </c>
@@ -15935,7 +15935,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>369</v>
       </c>
@@ -16112,7 +16112,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>373</v>
       </c>
@@ -16289,7 +16289,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="84" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>374</v>
       </c>
@@ -16466,7 +16466,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="85" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>375</v>
       </c>
@@ -16643,7 +16643,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>377</v>
       </c>
@@ -16820,7 +16820,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="87" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>378</v>
       </c>
@@ -16997,7 +16997,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>379</v>
       </c>
@@ -17174,7 +17174,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="89" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>380</v>
       </c>
@@ -17351,7 +17351,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="90" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>381</v>
       </c>
@@ -17528,7 +17528,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="91" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>382</v>
       </c>
@@ -17705,7 +17705,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="92" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
         <v>383</v>
       </c>
@@ -17882,7 +17882,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="93" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>384</v>
       </c>
@@ -18059,7 +18059,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
         <v>392</v>
       </c>
@@ -18236,7 +18236,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="95" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>402</v>
       </c>
@@ -18413,7 +18413,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="96" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
         <v>402</v>
       </c>
@@ -18590,7 +18590,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="97" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>403</v>
       </c>
@@ -18767,7 +18767,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="98" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>412</v>
       </c>
@@ -18944,7 +18944,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="99" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>413</v>
       </c>
@@ -19121,7 +19121,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="100" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
         <v>429</v>
       </c>
@@ -19301,7 +19301,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>432</v>
       </c>
@@ -19481,7 +19481,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
         <v>433</v>
       </c>
@@ -19661,7 +19661,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="103" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>434</v>
       </c>
@@ -19843,7 +19843,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
         <v>435</v>
       </c>
@@ -20025,7 +20025,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="105" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
         <v>436</v>
       </c>
@@ -20207,7 +20207,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="106" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
         <v>431</v>
       </c>
@@ -20389,7 +20389,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="107" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>456</v>
       </c>
@@ -20568,7 +20568,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
         <v>460</v>
       </c>
@@ -20750,7 +20750,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>466</v>
       </c>
@@ -20929,7 +20929,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="110" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
         <v>470</v>
       </c>
@@ -21111,7 +21111,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="111" spans="1:58" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:58" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="40" t="s">
         <v>472</v>
       </c>
@@ -21293,7 +21293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:58" s="48" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:58" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="47" t="s">
         <v>476</v>
       </c>
@@ -21472,7 +21472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
         <v>484</v>
       </c>
@@ -21656,7 +21656,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
         <v>485</v>
       </c>
@@ -21782,7 +21782,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
         <v>493</v>
       </c>
@@ -21908,7 +21908,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
         <v>494</v>
       </c>
@@ -22036,7 +22036,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>505</v>
       </c>
@@ -22164,7 +22164,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
         <v>504</v>
       </c>
@@ -22292,7 +22292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>502</v>
       </c>
@@ -22420,7 +22420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
         <v>507</v>
       </c>
@@ -22569,7 +22569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>508</v>
       </c>
@@ -22718,7 +22718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
         <v>520</v>
       </c>
@@ -22849,7 +22849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
         <v>521</v>
       </c>
@@ -22980,7 +22980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
         <v>522</v>
       </c>
@@ -23111,7 +23111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>523</v>
       </c>
@@ -23242,7 +23242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
         <v>528</v>
       </c>
@@ -23342,7 +23342,7 @@
         <v>435</v>
       </c>
       <c r="AQ126">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="AR126">
         <v>512</v>
@@ -23355,7 +23355,7 @@
       </c>
       <c r="AU126">
         <f t="shared" ref="AU126" si="224" xml:space="preserve"> _xlfn.FLOOR.MATH((AN126 - AQ126) / 2)</f>
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="AV126">
         <f t="shared" ref="AV126" si="225" xml:space="preserve"> _xlfn.FLOOR.MATH((AO126 - AR126) / 2)</f>
@@ -23370,7 +23370,7 @@
       </c>
       <c r="AY126">
         <f t="shared" ref="AY126" si="227">AQ126-AU126</f>
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="AZ126">
         <f t="shared" ref="AZ126" si="228">AR126-AV126</f>
@@ -23396,7 +23396,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="127" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
update 3dunet session annotations.xlsx; Wed 09:57:52 24.01.2024
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86B812B-4961-4914-9A9C-CBAA057A7801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83945EFA-0296-41A9-8620-052AD7A5BBE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2565" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3851" uniqueCount="543">
   <si>
     <t>patch z</t>
   </si>
@@ -1710,9 +1699,6 @@
     </r>
   </si>
   <si>
-    <t>240123-0</t>
-  </si>
-  <si>
     <t>stride = floor (resolution(=min.resolution) - patch) / 2</t>
   </si>
   <si>
@@ -1722,9 +1708,6 @@
     <t>dataset10.b</t>
   </si>
   <si>
-    <t>6 (verify)</t>
-  </si>
-  <si>
     <t>res. Z (min)</t>
   </si>
   <si>
@@ -1734,24 +1717,6 @@
     <t>res. X (min)</t>
   </si>
   <si>
-    <t>patch = 2^3 &gt; max dz-ROI = 136 (id06)</t>
-  </si>
-  <si>
-    <t>240123-1</t>
-  </si>
-  <si>
-    <t>240123-2</t>
-  </si>
-  <si>
-    <t>240123-3</t>
-  </si>
-  <si>
-    <t>File "/home/dwalth/data/conda/envs/3dunet1.8.2/lib/python3.11/site-packages/torch/utils/data/dataset.py", line 284, in __init__
-    assert len(self.datasets) &gt; 0, 'datasets should not be an empty iterable'  # type: ignore[arg-type]
-    ^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^^
-AssertionError: datasets should not be an empty iterable</t>
-  </si>
-  <si>
     <t>Train an eye segmentation model using manual dense annotations, LR factor 0.6</t>
   </si>
   <si>
@@ -1761,10 +1726,22 @@
     <t>Train an eye segmentation model using manual dense annotations, LR factor 0.7</t>
   </si>
   <si>
-    <t>Train an eye segmentation model using manual dense annotations, LR factor 0.8</t>
-  </si>
-  <si>
-    <t>Failure: AssertionError: datasets should not be an empty iterable</t>
+    <t>240124-0</t>
+  </si>
+  <si>
+    <t>240124-1</t>
+  </si>
+  <si>
+    <t>240124-2</t>
+  </si>
+  <si>
+    <t>240124-3</t>
+  </si>
+  <si>
+    <t>Train an eye segmentation model using manual dense annotations, LR factor 0.4</t>
+  </si>
+  <si>
+    <t>patch = 2^3 &gt; max dz-ROI = 136 (id06), so that only 1 patch is created</t>
   </si>
 </sst>
 </file>
@@ -2117,7 +2094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2223,6 +2200,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2539,8 +2517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BF130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T129" sqref="T129"/>
+    <sheetView tabSelected="1" topLeftCell="P83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB128" sqref="BB128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2719,13 +2697,13 @@
         <v>34</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="AP1" s="19" t="s">
         <v>533</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="AP1" s="19" t="s">
-        <v>535</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>0</v>
@@ -22526,8 +22504,9 @@
         <f>AI120+AJ120</f>
         <v>81052</v>
       </c>
-      <c r="AL120" t="s">
-        <v>278</v>
+      <c r="AL120">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ120*AR120*AS120) * (AA120 / 5) + 441</f>
+        <v>73500.060473349149</v>
       </c>
       <c r="AM120" s="10" t="s">
         <v>105</v>
@@ -22675,8 +22654,9 @@
         <f>AI121+AJ121</f>
         <v>81052</v>
       </c>
-      <c r="AL121" t="s">
-        <v>278</v>
+      <c r="AL121">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ121*AR121*AS121) * (AA121 / 5) + 441</f>
+        <v>73500.060473349149</v>
       </c>
       <c r="AM121" s="10" t="s">
         <v>105</v>
@@ -23269,9 +23249,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:58" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="B126" s="12" t="s">
         <v>117</v>
@@ -23286,16 +23266,16 @@
         <v>409</v>
       </c>
       <c r="F126" s="64" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G126" s="12" t="s">
         <v>516</v>
       </c>
       <c r="H126" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="I126" s="6">
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="I126" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="J126" t="s">
         <v>117</v>
@@ -23311,16 +23291,16 @@
       </c>
       <c r="T126" s="12"/>
       <c r="U126" s="20" t="s">
+        <v>529</v>
+      </c>
+      <c r="V126" t="s">
         <v>530</v>
-      </c>
-      <c r="V126" t="s">
-        <v>531</v>
       </c>
       <c r="W126">
         <v>6</v>
       </c>
-      <c r="X126" t="s">
-        <v>532</v>
+      <c r="X126" s="69">
+        <v>6</v>
       </c>
       <c r="Y126">
         <v>5</v>
@@ -23353,8 +23333,9 @@
       <c r="AK126" t="s">
         <v>117</v>
       </c>
-      <c r="AL126" t="s">
-        <v>278</v>
+      <c r="AL126">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ126*AR126*AS126) * (AA126 / 5) + 441</f>
+        <v>73500.060473349149</v>
       </c>
       <c r="AM126" s="10" t="s">
         <v>105</v>
@@ -23408,24 +23389,19 @@
         <v>359</v>
       </c>
       <c r="BB126" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="BC126" t="s">
-        <v>529</v>
-      </c>
-      <c r="BD126">
-        <v>1</v>
-      </c>
-      <c r="BE126" t="s">
-        <v>11</v>
-      </c>
-      <c r="BF126" s="2" t="s">
-        <v>540</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="BD126" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF126" s="2"/>
     </row>
-    <row r="127" spans="1:58" ht="60" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B127" s="12" t="s">
         <v>117</v>
@@ -23440,16 +23416,16 @@
         <v>409</v>
       </c>
       <c r="F127" s="64" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="G127" s="12" t="s">
         <v>516</v>
       </c>
       <c r="H127" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="I127" s="6">
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="I127" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="J127" t="s">
         <v>117</v>
@@ -23465,16 +23441,16 @@
       </c>
       <c r="T127" s="12"/>
       <c r="U127" s="20" t="s">
+        <v>529</v>
+      </c>
+      <c r="V127" t="s">
         <v>530</v>
-      </c>
-      <c r="V127" t="s">
-        <v>531</v>
       </c>
       <c r="W127">
         <v>6</v>
       </c>
-      <c r="X127" t="s">
-        <v>532</v>
+      <c r="X127" s="69">
+        <v>6</v>
       </c>
       <c r="Y127">
         <v>5</v>
@@ -23507,76 +23483,75 @@
       <c r="AK127" t="s">
         <v>117</v>
       </c>
-      <c r="AL127" t="s">
-        <v>278</v>
+      <c r="AL127">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ127*AR127*AS127) * (AA127 / 5) + 441</f>
+        <v>73500.060473349149</v>
       </c>
       <c r="AM127" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AN127" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO127" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP127" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ127" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR127" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS127" t="s">
-        <v>117</v>
+      <c r="AN127">
+        <v>173</v>
+      </c>
+      <c r="AO127">
+        <v>743</v>
+      </c>
+      <c r="AP127" s="20">
+        <v>435</v>
+      </c>
+      <c r="AQ127">
+        <v>144</v>
+      </c>
+      <c r="AR127">
+        <v>512</v>
+      </c>
+      <c r="AS127">
+        <v>384</v>
       </c>
       <c r="AT127" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU127" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV127" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW127" t="s">
-        <v>117</v>
+        <v>45</v>
+      </c>
+      <c r="AU127">
+        <f t="shared" ref="AU127" si="230" xml:space="preserve"> _xlfn.FLOOR.MATH((AN127 - AQ127) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AV127">
+        <f t="shared" ref="AV127" si="231" xml:space="preserve"> _xlfn.FLOOR.MATH((AO127 - AR127) / 2)</f>
+        <v>115</v>
+      </c>
+      <c r="AW127">
+        <f t="shared" ref="AW127" si="232" xml:space="preserve"> _xlfn.FLOOR.MATH((AP127 - AS127) / 2)</f>
+        <v>25</v>
       </c>
       <c r="AX127" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY127" t="e">
-        <f t="shared" ref="AY127" si="230">AQ127-AU127</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ127" t="e">
-        <f t="shared" ref="AZ127" si="231">AR127-AV127</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA127" s="10" t="e">
-        <f t="shared" ref="BA127" si="232">AS127-AW127</f>
-        <v>#VALUE!</v>
+        <v>45</v>
+      </c>
+      <c r="AY127">
+        <f t="shared" ref="AY127" si="233">AQ127-AU127</f>
+        <v>130</v>
+      </c>
+      <c r="AZ127">
+        <f t="shared" ref="AZ127" si="234">AR127-AV127</f>
+        <v>397</v>
+      </c>
+      <c r="BA127" s="10">
+        <f t="shared" ref="BA127" si="235">AS127-AW127</f>
+        <v>359</v>
       </c>
       <c r="BB127" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="BC127" t="s">
-        <v>529</v>
-      </c>
-      <c r="BD127">
-        <v>1</v>
-      </c>
-      <c r="BE127" t="s">
-        <v>11</v>
-      </c>
-      <c r="BF127" s="2" t="s">
-        <v>540</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="BD127" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF127" s="2"/>
     </row>
-    <row r="128" spans="1:58" ht="60" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B128" s="12" t="s">
         <v>117</v>
@@ -23591,16 +23566,16 @@
         <v>409</v>
       </c>
       <c r="F128" s="64" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="G128" s="12" t="s">
         <v>516</v>
       </c>
       <c r="H128" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="I128" s="6">
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="I128" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="J128" t="s">
         <v>117</v>
@@ -23616,16 +23591,16 @@
       </c>
       <c r="T128" s="12"/>
       <c r="U128" s="20" t="s">
+        <v>529</v>
+      </c>
+      <c r="V128" t="s">
         <v>530</v>
-      </c>
-      <c r="V128" t="s">
-        <v>531</v>
       </c>
       <c r="W128">
         <v>6</v>
       </c>
-      <c r="X128" t="s">
-        <v>532</v>
+      <c r="X128" s="69">
+        <v>6</v>
       </c>
       <c r="Y128">
         <v>5</v>
@@ -23658,76 +23633,75 @@
       <c r="AK128" t="s">
         <v>117</v>
       </c>
-      <c r="AL128" t="s">
-        <v>278</v>
+      <c r="AL128">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ128*AR128*AS128) * (AA128 / 5) + 441</f>
+        <v>73500.060473349149</v>
       </c>
       <c r="AM128" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AN128" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO128" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP128" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ128" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR128" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS128" t="s">
-        <v>117</v>
+      <c r="AN128">
+        <v>173</v>
+      </c>
+      <c r="AO128">
+        <v>743</v>
+      </c>
+      <c r="AP128" s="20">
+        <v>435</v>
+      </c>
+      <c r="AQ128">
+        <v>144</v>
+      </c>
+      <c r="AR128">
+        <v>512</v>
+      </c>
+      <c r="AS128">
+        <v>384</v>
       </c>
       <c r="AT128" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU128" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV128" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW128" t="s">
-        <v>117</v>
+        <v>45</v>
+      </c>
+      <c r="AU128">
+        <f t="shared" ref="AU128" si="236" xml:space="preserve"> _xlfn.FLOOR.MATH((AN128 - AQ128) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AV128">
+        <f t="shared" ref="AV128" si="237" xml:space="preserve"> _xlfn.FLOOR.MATH((AO128 - AR128) / 2)</f>
+        <v>115</v>
+      </c>
+      <c r="AW128">
+        <f t="shared" ref="AW128" si="238" xml:space="preserve"> _xlfn.FLOOR.MATH((AP128 - AS128) / 2)</f>
+        <v>25</v>
       </c>
       <c r="AX128" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY128" t="e">
-        <f t="shared" ref="AY128" si="233">AQ128-AU128</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ128" t="e">
-        <f t="shared" ref="AZ128" si="234">AR128-AV128</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA128" s="10" t="e">
-        <f t="shared" ref="BA128" si="235">AS128-AW128</f>
-        <v>#VALUE!</v>
+        <v>45</v>
+      </c>
+      <c r="AY128">
+        <f t="shared" ref="AY128" si="239">AQ128-AU128</f>
+        <v>130</v>
+      </c>
+      <c r="AZ128">
+        <f t="shared" ref="AZ128" si="240">AR128-AV128</f>
+        <v>397</v>
+      </c>
+      <c r="BA128" s="10">
+        <f t="shared" ref="BA128" si="241">AS128-AW128</f>
+        <v>359</v>
       </c>
       <c r="BB128" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="BC128" t="s">
-        <v>529</v>
-      </c>
-      <c r="BD128">
-        <v>1</v>
-      </c>
-      <c r="BE128" t="s">
-        <v>11</v>
-      </c>
-      <c r="BF128" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="BD128" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF128" s="2"/>
+    </row>
+    <row r="129" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A129" s="12" t="s">
         <v>540</v>
-      </c>
-    </row>
-    <row r="129" spans="1:58" ht="60" x14ac:dyDescent="0.25">
-      <c r="A129" s="12" t="s">
-        <v>539</v>
       </c>
       <c r="B129" s="12" t="s">
         <v>117</v>
@@ -23742,16 +23716,16 @@
         <v>409</v>
       </c>
       <c r="F129" s="64" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="G129" s="12" t="s">
         <v>516</v>
       </c>
       <c r="H129" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="I129" s="6">
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="I129" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="J129" t="s">
         <v>117</v>
@@ -23767,16 +23741,16 @@
       </c>
       <c r="T129" s="12"/>
       <c r="U129" s="20" t="s">
+        <v>529</v>
+      </c>
+      <c r="V129" t="s">
         <v>530</v>
-      </c>
-      <c r="V129" t="s">
-        <v>531</v>
       </c>
       <c r="W129">
         <v>6</v>
       </c>
-      <c r="X129" t="s">
-        <v>532</v>
+      <c r="X129" s="69">
+        <v>6</v>
       </c>
       <c r="Y129">
         <v>5</v>
@@ -23809,72 +23783,71 @@
       <c r="AK129" t="s">
         <v>117</v>
       </c>
-      <c r="AL129" t="s">
-        <v>278</v>
+      <c r="AL129">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ129*AR129*AS129) * (AA129 / 5) + 441</f>
+        <v>73500.060473349149</v>
       </c>
       <c r="AM129" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AN129" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO129" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP129" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ129" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR129" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS129" t="s">
-        <v>117</v>
+      <c r="AN129">
+        <v>173</v>
+      </c>
+      <c r="AO129">
+        <v>743</v>
+      </c>
+      <c r="AP129" s="20">
+        <v>435</v>
+      </c>
+      <c r="AQ129">
+        <v>144</v>
+      </c>
+      <c r="AR129">
+        <v>512</v>
+      </c>
+      <c r="AS129">
+        <v>384</v>
       </c>
       <c r="AT129" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU129" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV129" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW129" t="s">
-        <v>117</v>
+        <v>45</v>
+      </c>
+      <c r="AU129">
+        <f t="shared" ref="AU129" si="242" xml:space="preserve"> _xlfn.FLOOR.MATH((AN129 - AQ129) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AV129">
+        <f t="shared" ref="AV129" si="243" xml:space="preserve"> _xlfn.FLOOR.MATH((AO129 - AR129) / 2)</f>
+        <v>115</v>
+      </c>
+      <c r="AW129">
+        <f t="shared" ref="AW129" si="244" xml:space="preserve"> _xlfn.FLOOR.MATH((AP129 - AS129) / 2)</f>
+        <v>25</v>
       </c>
       <c r="AX129" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY129" t="e">
-        <f t="shared" ref="AY129" si="236">AQ129-AU129</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ129" t="e">
-        <f t="shared" ref="AZ129" si="237">AR129-AV129</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA129" s="10" t="e">
-        <f t="shared" ref="BA129" si="238">AS129-AW129</f>
-        <v>#VALUE!</v>
+        <v>45</v>
+      </c>
+      <c r="AY129">
+        <f t="shared" ref="AY129" si="245">AQ129-AU129</f>
+        <v>130</v>
+      </c>
+      <c r="AZ129">
+        <f t="shared" ref="AZ129" si="246">AR129-AV129</f>
+        <v>397</v>
+      </c>
+      <c r="BA129" s="10">
+        <f t="shared" ref="BA129" si="247">AS129-AW129</f>
+        <v>359</v>
       </c>
       <c r="BB129" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="BC129" t="s">
-        <v>529</v>
-      </c>
-      <c r="BD129">
-        <v>1</v>
-      </c>
-      <c r="BE129" t="s">
-        <v>11</v>
-      </c>
-      <c r="BF129" s="2" t="s">
-        <v>540</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="BD129" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF129" s="2"/>
     </row>
     <row r="130" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
@@ -23999,15 +23972,15 @@
         <v>8</v>
       </c>
       <c r="AY130" t="e">
-        <f t="shared" ref="AY130" si="239">AQ130-AU130</f>
+        <f t="shared" ref="AY130" si="248">AQ130-AU130</f>
         <v>#VALUE!</v>
       </c>
       <c r="AZ130" t="e">
-        <f t="shared" ref="AZ130" si="240">AR130-AV130</f>
+        <f t="shared" ref="AZ130" si="249">AR130-AV130</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA130" s="10" t="e">
-        <f t="shared" ref="BA130" si="241">AS130-AW130</f>
+        <f t="shared" ref="BA130" si="250">AS130-AW130</f>
         <v>#VALUE!</v>
       </c>
       <c r="BB130" t="s">
@@ -24017,12 +23990,6 @@
         <v>117</v>
       </c>
       <c r="BD130" t="s">
-        <v>117</v>
-      </c>
-      <c r="BE130" t="s">
-        <v>117</v>
-      </c>
-      <c r="BF130" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepapre train3dunet 1.8.2 chpt-240124-4, fluo eye 3dunet
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83945EFA-0296-41A9-8620-052AD7A5BBE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B7E079-B84E-4A96-920A-3F07E54FAA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2565" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3851" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3877" uniqueCount="546">
   <si>
     <t>patch z</t>
   </si>
@@ -1717,15 +1728,6 @@
     <t>res. X (min)</t>
   </si>
   <si>
-    <t>Train an eye segmentation model using manual dense annotations, LR factor 0.6</t>
-  </si>
-  <si>
-    <t>Train an eye segmentation model using manual dense annotations, LR factor 0.5</t>
-  </si>
-  <si>
-    <t>Train an eye segmentation model using manual dense annotations, LR factor 0.7</t>
-  </si>
-  <si>
     <t>240124-0</t>
   </si>
   <si>
@@ -1738,10 +1740,28 @@
     <t>240124-3</t>
   </si>
   <si>
-    <t>Train an eye segmentation model using manual dense annotations, LR factor 0.4</t>
-  </si>
-  <si>
     <t>patch = 2^3 &gt; max dz-ROI = 136 (id06), so that only 1 patch is created</t>
+  </si>
+  <si>
+    <t>240124-4</t>
+  </si>
+  <si>
+    <t>Train an autofluo eye segmentation model using manual dense annotations, LR factor 0.4</t>
+  </si>
+  <si>
+    <t>Train an autofluo eye segmentation model using manual dense annotations, LR factor 0.5</t>
+  </si>
+  <si>
+    <t>Train an autofluo eye segmentation model using manual dense annotations, LR factor 0.6</t>
+  </si>
+  <si>
+    <t>Train an autofluo eye segmentation model using manual dense annotations, LR factor 0.7</t>
+  </si>
+  <si>
+    <t>Train a fluo eye segmentation model using manual dense annotations, LR factor 0.5</t>
+  </si>
+  <si>
+    <t>dataset10.c</t>
   </si>
 </sst>
 </file>
@@ -2094,7 +2114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2200,7 +2220,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2515,10 +2534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BF130"/>
+  <dimension ref="A1:BF131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BB128" sqref="BB128"/>
+    <sheetView tabSelected="1" topLeftCell="BC121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BD130" sqref="BD130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -23041,7 +23060,7 @@
         <v>1</v>
       </c>
       <c r="AA124">
-        <f t="shared" ref="AA124:AA129" si="217">Y124+Z124</f>
+        <f t="shared" ref="AA124:AA130" si="217">Y124+Z124</f>
         <v>6</v>
       </c>
       <c r="AB124">
@@ -23251,7 +23270,7 @@
     </row>
     <row r="126" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B126" s="12" t="s">
         <v>117</v>
@@ -23266,7 +23285,7 @@
         <v>409</v>
       </c>
       <c r="F126" s="64" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="G126" s="12" t="s">
         <v>516</v>
@@ -23299,7 +23318,7 @@
       <c r="W126">
         <v>6</v>
       </c>
-      <c r="X126" s="69">
+      <c r="X126">
         <v>6</v>
       </c>
       <c r="Y126">
@@ -23389,7 +23408,7 @@
         <v>359</v>
       </c>
       <c r="BB126" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="BC126" t="s">
         <v>528</v>
@@ -23401,7 +23420,7 @@
     </row>
     <row r="127" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B127" s="12" t="s">
         <v>117</v>
@@ -23416,7 +23435,7 @@
         <v>409</v>
       </c>
       <c r="F127" s="64" t="s">
-        <v>535</v>
+        <v>541</v>
       </c>
       <c r="G127" s="12" t="s">
         <v>516</v>
@@ -23449,7 +23468,7 @@
       <c r="W127">
         <v>6</v>
       </c>
-      <c r="X127" s="69">
+      <c r="X127">
         <v>6</v>
       </c>
       <c r="Y127">
@@ -23539,7 +23558,7 @@
         <v>359</v>
       </c>
       <c r="BB127" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="BC127" t="s">
         <v>528</v>
@@ -23551,7 +23570,7 @@
     </row>
     <row r="128" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B128" s="12" t="s">
         <v>117</v>
@@ -23566,7 +23585,7 @@
         <v>409</v>
       </c>
       <c r="F128" s="64" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="G128" s="12" t="s">
         <v>516</v>
@@ -23599,7 +23618,7 @@
       <c r="W128">
         <v>6</v>
       </c>
-      <c r="X128" s="69">
+      <c r="X128">
         <v>6</v>
       </c>
       <c r="Y128">
@@ -23689,7 +23708,7 @@
         <v>359</v>
       </c>
       <c r="BB128" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="BC128" t="s">
         <v>528</v>
@@ -23701,7 +23720,7 @@
     </row>
     <row r="129" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="B129" s="12" t="s">
         <v>117</v>
@@ -23716,7 +23735,7 @@
         <v>409</v>
       </c>
       <c r="F129" s="64" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="G129" s="12" t="s">
         <v>516</v>
@@ -23749,7 +23768,7 @@
       <c r="W129">
         <v>6</v>
       </c>
-      <c r="X129" s="69">
+      <c r="X129">
         <v>6</v>
       </c>
       <c r="Y129">
@@ -23812,15 +23831,15 @@
         <v>45</v>
       </c>
       <c r="AU129">
-        <f t="shared" ref="AU129" si="242" xml:space="preserve"> _xlfn.FLOOR.MATH((AN129 - AQ129) / 2)</f>
+        <f t="shared" ref="AU129:AU130" si="242" xml:space="preserve"> _xlfn.FLOOR.MATH((AN129 - AQ129) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV129">
-        <f t="shared" ref="AV129" si="243" xml:space="preserve"> _xlfn.FLOOR.MATH((AO129 - AR129) / 2)</f>
+        <f t="shared" ref="AV129:AV130" si="243" xml:space="preserve"> _xlfn.FLOOR.MATH((AO129 - AR129) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW129">
-        <f t="shared" ref="AW129" si="244" xml:space="preserve"> _xlfn.FLOOR.MATH((AP129 - AS129) / 2)</f>
+        <f t="shared" ref="AW129:AW130" si="244" xml:space="preserve"> _xlfn.FLOOR.MATH((AP129 - AS129) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX129" s="25" t="s">
@@ -23839,7 +23858,7 @@
         <v>359</v>
       </c>
       <c r="BB129" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="BC129" t="s">
         <v>528</v>
@@ -23851,25 +23870,25 @@
     </row>
     <row r="130" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
-        <v>117</v>
+        <v>539</v>
       </c>
       <c r="B130" s="12" t="s">
         <v>117</v>
       </c>
       <c r="C130" t="s">
-        <v>117</v>
+        <v>457</v>
       </c>
       <c r="D130" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E130" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F130" s="64" t="s">
-        <v>117</v>
+        <v>544</v>
       </c>
       <c r="G130" s="12" t="s">
-        <v>117</v>
+        <v>516</v>
       </c>
       <c r="H130" s="12" t="s">
         <v>117</v>
@@ -23891,37 +23910,38 @@
       </c>
       <c r="T130" s="12"/>
       <c r="U130" s="20" t="s">
-        <v>117</v>
+        <v>529</v>
       </c>
       <c r="V130" t="s">
-        <v>117</v>
-      </c>
-      <c r="W130" t="s">
-        <v>117</v>
-      </c>
-      <c r="X130" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y130" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z130" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA130" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB130" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC130" t="s">
-        <v>117</v>
+        <v>545</v>
+      </c>
+      <c r="W130">
+        <v>6</v>
+      </c>
+      <c r="X130">
+        <v>6</v>
+      </c>
+      <c r="Y130">
+        <v>5</v>
+      </c>
+      <c r="Z130">
+        <v>1</v>
+      </c>
+      <c r="AA130">
+        <f t="shared" si="217"/>
+        <v>6</v>
+      </c>
+      <c r="AB130">
+        <v>1</v>
+      </c>
+      <c r="AC130">
+        <v>3</v>
       </c>
       <c r="AE130" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AH130" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="AI130" s="6" t="s">
         <v>117</v>
@@ -23932,64 +23952,212 @@
       <c r="AK130" t="s">
         <v>117</v>
       </c>
-      <c r="AL130" t="s">
-        <v>278</v>
+      <c r="AL130">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ130*AR130*AS130) * (AA130 / 5) + 441</f>
+        <v>73500.060473349149</v>
       </c>
       <c r="AM130" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AN130" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO130" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP130" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ130" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR130" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS130" t="s">
-        <v>117</v>
+      <c r="AN130">
+        <v>173</v>
+      </c>
+      <c r="AO130">
+        <v>743</v>
+      </c>
+      <c r="AP130" s="20">
+        <v>435</v>
+      </c>
+      <c r="AQ130">
+        <v>144</v>
+      </c>
+      <c r="AR130">
+        <v>512</v>
+      </c>
+      <c r="AS130">
+        <v>384</v>
       </c>
       <c r="AT130" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU130" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV130" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW130" t="s">
-        <v>117</v>
+        <v>45</v>
+      </c>
+      <c r="AU130">
+        <f t="shared" si="242"/>
+        <v>14</v>
+      </c>
+      <c r="AV130">
+        <f t="shared" si="243"/>
+        <v>115</v>
+      </c>
+      <c r="AW130">
+        <f t="shared" si="244"/>
+        <v>25</v>
       </c>
       <c r="AX130" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY130" t="e">
+        <v>45</v>
+      </c>
+      <c r="AY130">
         <f t="shared" ref="AY130" si="248">AQ130-AU130</f>
+        <v>130</v>
+      </c>
+      <c r="AZ130">
+        <f t="shared" ref="AZ130" si="249">AR130-AV130</f>
+        <v>397</v>
+      </c>
+      <c r="BA130" s="10">
+        <f t="shared" ref="BA130" si="250">AS130-AW130</f>
+        <v>359</v>
+      </c>
+      <c r="BB130" t="s">
+        <v>538</v>
+      </c>
+      <c r="BC130" t="s">
+        <v>528</v>
+      </c>
+      <c r="BD130" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="131" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A131" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B131" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C131" t="s">
+        <v>117</v>
+      </c>
+      <c r="D131" t="s">
+        <v>117</v>
+      </c>
+      <c r="E131" t="s">
+        <v>117</v>
+      </c>
+      <c r="F131" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G131" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H131" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I131" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J131" t="s">
+        <v>117</v>
+      </c>
+      <c r="K131" t="s">
+        <v>117</v>
+      </c>
+      <c r="L131" t="s">
+        <v>117</v>
+      </c>
+      <c r="M131" t="s">
+        <v>117</v>
+      </c>
+      <c r="T131" s="12"/>
+      <c r="U131" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V131" t="s">
+        <v>117</v>
+      </c>
+      <c r="W131" t="s">
+        <v>117</v>
+      </c>
+      <c r="X131" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y131" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI131" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ131" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL131" t="s">
+        <v>278</v>
+      </c>
+      <c r="AM131" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP131" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT131" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW131" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX131" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY131" t="e">
+        <f t="shared" ref="AY131" si="251">AQ131-AU131</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ130" t="e">
-        <f t="shared" ref="AZ130" si="249">AR130-AV130</f>
+      <c r="AZ131" t="e">
+        <f t="shared" ref="AZ131" si="252">AR131-AV131</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA130" s="10" t="e">
-        <f t="shared" ref="BA130" si="250">AS130-AW130</f>
+      <c r="BA131" s="10" t="e">
+        <f t="shared" ref="BA131" si="253">AS131-AW131</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB130" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC130" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD130" t="s">
+      <c r="BB131" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC131" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD131" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare train3dunet 1.8.2 chpt-240125-9, val loss curve experiment
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47408899-5622-4536-91A6-6ECD17DC2CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B4A39A-C20F-4B68-9CB7-9A15DF44A8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4050" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4031" uniqueCount="581">
   <si>
     <t>patch z</t>
   </si>
@@ -1846,6 +1846,27 @@
   </si>
   <si>
     <t>error</t>
+  </si>
+  <si>
+    <t>240125-9</t>
+  </si>
+  <si>
+    <t>3channel autofluo eye dataset10.c.1 vall loss curve exp</t>
+  </si>
+  <si>
+    <t>Train an autofluo eye segmentation model using manual dense annotations, How do predictions look with just 1 LR step (LR 2e-4)?</t>
+  </si>
+  <si>
+    <t>Does the val loss curve in tensorboard decrease with higher n_val?</t>
+  </si>
+  <si>
+    <t>Success (finish training &amp; answer question)</t>
+  </si>
+  <si>
+    <t>1 (verify)</t>
+  </si>
+  <si>
+    <t>dataset10.c.1</t>
   </si>
 </sst>
 </file>
@@ -2198,7 +2219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2305,9 +2326,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2624,16 +2642,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BF140"/>
+  <dimension ref="A1:BF141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM140" sqref="AM140"/>
+    <sheetView tabSelected="1" topLeftCell="AK104" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL140" sqref="AL140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" customWidth="1"/>
     <col min="6" max="6" width="57" style="61" customWidth="1" outlineLevel="1"/>
@@ -2646,7 +2664,7 @@
     <col min="13" max="13" width="33" customWidth="1"/>
     <col min="14" max="20" width="9.140625" customWidth="1" outlineLevel="1"/>
     <col min="21" max="21" width="9.140625" style="20"/>
-    <col min="22" max="22" width="12.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="15.140625" customWidth="1" outlineLevel="1"/>
     <col min="23" max="23" width="9.140625" customWidth="1" outlineLevel="1"/>
     <col min="25" max="25" width="6.7109375" customWidth="1" outlineLevel="1"/>
     <col min="26" max="26" width="5.140625" customWidth="1" outlineLevel="1"/>
@@ -23150,7 +23168,7 @@
         <v>1</v>
       </c>
       <c r="AA124">
-        <f t="shared" ref="AA124:AA139" si="217">Y124+Z124</f>
+        <f t="shared" ref="AA124:AA140" si="217">Y124+Z124</f>
         <v>6</v>
       </c>
       <c r="AB124">
@@ -23427,17 +23445,18 @@
       <c r="AH126" t="s">
         <v>96</v>
       </c>
-      <c r="AI126" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ126" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK126" t="s">
-        <v>117</v>
+      <c r="AI126" s="6">
+        <v>77627</v>
+      </c>
+      <c r="AJ126" s="12">
+        <v>3425</v>
+      </c>
+      <c r="AK126">
+        <f>AI126+AJ126</f>
+        <v>81052</v>
       </c>
       <c r="AL126">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ126*AR126*AS126) * (AA126 / 5) + 441</f>
+        <f t="shared" ref="AL126:AL131" si="224" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ126*AR126*AS126) * (AA126 / 5) + 441</f>
         <v>73500.060473349149</v>
       </c>
       <c r="AM126" s="10" t="s">
@@ -23465,30 +23484,30 @@
         <v>45</v>
       </c>
       <c r="AU126">
-        <f t="shared" ref="AU126" si="224" xml:space="preserve"> _xlfn.FLOOR.MATH((AN126 - AQ126) / 2)</f>
+        <f t="shared" ref="AU126" si="225" xml:space="preserve"> _xlfn.FLOOR.MATH((AN126 - AQ126) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV126">
-        <f t="shared" ref="AV126" si="225" xml:space="preserve"> _xlfn.FLOOR.MATH((AO126 - AR126) / 2)</f>
+        <f t="shared" ref="AV126" si="226" xml:space="preserve"> _xlfn.FLOOR.MATH((AO126 - AR126) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW126">
-        <f t="shared" ref="AW126" si="226" xml:space="preserve"> _xlfn.FLOOR.MATH((AP126 - AS126) / 2)</f>
+        <f t="shared" ref="AW126" si="227" xml:space="preserve"> _xlfn.FLOOR.MATH((AP126 - AS126) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX126" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY126">
-        <f t="shared" ref="AY126" si="227">AQ126-AU126</f>
+        <f t="shared" ref="AY126" si="228">AQ126-AU126</f>
         <v>130</v>
       </c>
       <c r="AZ126">
-        <f t="shared" ref="AZ126" si="228">AR126-AV126</f>
+        <f t="shared" ref="AZ126" si="229">AR126-AV126</f>
         <v>397</v>
       </c>
       <c r="BA126" s="10">
-        <f t="shared" ref="BA126" si="229">AS126-AW126</f>
+        <f t="shared" ref="BA126" si="230">AS126-AW126</f>
         <v>359</v>
       </c>
       <c r="BB126" t="s">
@@ -23574,17 +23593,18 @@
       <c r="AH127" t="s">
         <v>96</v>
       </c>
-      <c r="AI127" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ127" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK127" t="s">
-        <v>117</v>
+      <c r="AI127" s="6">
+        <v>77627</v>
+      </c>
+      <c r="AJ127" s="12">
+        <v>3425</v>
+      </c>
+      <c r="AK127">
+        <f>AI127+AJ127</f>
+        <v>81052</v>
       </c>
       <c r="AL127">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ127*AR127*AS127) * (AA127 / 5) + 441</f>
+        <f t="shared" si="224"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM127" s="10" t="s">
@@ -23612,30 +23632,30 @@
         <v>45</v>
       </c>
       <c r="AU127">
-        <f t="shared" ref="AU127" si="230" xml:space="preserve"> _xlfn.FLOOR.MATH((AN127 - AQ127) / 2)</f>
+        <f t="shared" ref="AU127" si="231" xml:space="preserve"> _xlfn.FLOOR.MATH((AN127 - AQ127) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV127">
-        <f t="shared" ref="AV127" si="231" xml:space="preserve"> _xlfn.FLOOR.MATH((AO127 - AR127) / 2)</f>
+        <f t="shared" ref="AV127" si="232" xml:space="preserve"> _xlfn.FLOOR.MATH((AO127 - AR127) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW127">
-        <f t="shared" ref="AW127" si="232" xml:space="preserve"> _xlfn.FLOOR.MATH((AP127 - AS127) / 2)</f>
+        <f t="shared" ref="AW127" si="233" xml:space="preserve"> _xlfn.FLOOR.MATH((AP127 - AS127) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX127" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY127">
-        <f t="shared" ref="AY127" si="233">AQ127-AU127</f>
+        <f t="shared" ref="AY127" si="234">AQ127-AU127</f>
         <v>130</v>
       </c>
       <c r="AZ127">
-        <f t="shared" ref="AZ127" si="234">AR127-AV127</f>
+        <f t="shared" ref="AZ127" si="235">AR127-AV127</f>
         <v>397</v>
       </c>
       <c r="BA127" s="10">
-        <f t="shared" ref="BA127" si="235">AS127-AW127</f>
+        <f t="shared" ref="BA127" si="236">AS127-AW127</f>
         <v>359</v>
       </c>
       <c r="BB127" t="s">
@@ -23721,17 +23741,18 @@
       <c r="AH128" t="s">
         <v>96</v>
       </c>
-      <c r="AI128" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ128" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK128" t="s">
-        <v>117</v>
+      <c r="AI128" s="6">
+        <v>77627</v>
+      </c>
+      <c r="AJ128" s="12">
+        <v>3425</v>
+      </c>
+      <c r="AK128">
+        <f>AI128+AJ128</f>
+        <v>81052</v>
       </c>
       <c r="AL128">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ128*AR128*AS128) * (AA128 / 5) + 441</f>
+        <f t="shared" si="224"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM128" s="10" t="s">
@@ -23759,30 +23780,30 @@
         <v>45</v>
       </c>
       <c r="AU128">
-        <f t="shared" ref="AU128" si="236" xml:space="preserve"> _xlfn.FLOOR.MATH((AN128 - AQ128) / 2)</f>
+        <f t="shared" ref="AU128" si="237" xml:space="preserve"> _xlfn.FLOOR.MATH((AN128 - AQ128) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV128">
-        <f t="shared" ref="AV128" si="237" xml:space="preserve"> _xlfn.FLOOR.MATH((AO128 - AR128) / 2)</f>
+        <f t="shared" ref="AV128" si="238" xml:space="preserve"> _xlfn.FLOOR.MATH((AO128 - AR128) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW128">
-        <f t="shared" ref="AW128" si="238" xml:space="preserve"> _xlfn.FLOOR.MATH((AP128 - AS128) / 2)</f>
+        <f t="shared" ref="AW128" si="239" xml:space="preserve"> _xlfn.FLOOR.MATH((AP128 - AS128) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX128" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY128">
-        <f t="shared" ref="AY128" si="239">AQ128-AU128</f>
+        <f t="shared" ref="AY128" si="240">AQ128-AU128</f>
         <v>130</v>
       </c>
       <c r="AZ128">
-        <f t="shared" ref="AZ128" si="240">AR128-AV128</f>
+        <f t="shared" ref="AZ128" si="241">AR128-AV128</f>
         <v>397</v>
       </c>
       <c r="BA128" s="10">
-        <f t="shared" ref="BA128" si="241">AS128-AW128</f>
+        <f t="shared" ref="BA128" si="242">AS128-AW128</f>
         <v>359</v>
       </c>
       <c r="BB128" t="s">
@@ -23868,17 +23889,18 @@
       <c r="AH129" t="s">
         <v>96</v>
       </c>
-      <c r="AI129" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ129" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK129" t="s">
-        <v>117</v>
+      <c r="AI129" s="6">
+        <v>77627</v>
+      </c>
+      <c r="AJ129" s="12">
+        <v>3425</v>
+      </c>
+      <c r="AK129">
+        <f>AI129+AJ129</f>
+        <v>81052</v>
       </c>
       <c r="AL129">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ129*AR129*AS129) * (AA129 / 5) + 441</f>
+        <f t="shared" si="224"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM129" s="10" t="s">
@@ -23906,30 +23928,30 @@
         <v>45</v>
       </c>
       <c r="AU129">
-        <f t="shared" ref="AU129:AU139" si="242" xml:space="preserve"> _xlfn.FLOOR.MATH((AN129 - AQ129) / 2)</f>
+        <f t="shared" ref="AU129:AU139" si="243" xml:space="preserve"> _xlfn.FLOOR.MATH((AN129 - AQ129) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV129">
-        <f t="shared" ref="AV129:AV139" si="243" xml:space="preserve"> _xlfn.FLOOR.MATH((AO129 - AR129) / 2)</f>
+        <f t="shared" ref="AV129:AV139" si="244" xml:space="preserve"> _xlfn.FLOOR.MATH((AO129 - AR129) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW129">
-        <f t="shared" ref="AW129:AW139" si="244" xml:space="preserve"> _xlfn.FLOOR.MATH((AP129 - AS129) / 2)</f>
+        <f t="shared" ref="AW129:AW139" si="245" xml:space="preserve"> _xlfn.FLOOR.MATH((AP129 - AS129) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX129" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY129">
-        <f t="shared" ref="AY129" si="245">AQ129-AU129</f>
+        <f t="shared" ref="AY129" si="246">AQ129-AU129</f>
         <v>130</v>
       </c>
       <c r="AZ129">
-        <f t="shared" ref="AZ129" si="246">AR129-AV129</f>
+        <f t="shared" ref="AZ129" si="247">AR129-AV129</f>
         <v>397</v>
       </c>
       <c r="BA129" s="10">
-        <f t="shared" ref="BA129" si="247">AS129-AW129</f>
+        <f t="shared" ref="BA129" si="248">AS129-AW129</f>
         <v>359</v>
       </c>
       <c r="BB129" t="s">
@@ -24015,17 +24037,18 @@
       <c r="AH130" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AI130" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ130" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK130" s="4" t="s">
-        <v>117</v>
+      <c r="AI130" s="7">
+        <v>77407</v>
+      </c>
+      <c r="AJ130" s="17">
+        <v>3645</v>
+      </c>
+      <c r="AK130" s="4">
+        <f>AI130+AJ130</f>
+        <v>81052</v>
       </c>
       <c r="AL130" s="4">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ130*AR130*AS130) * (AA130 / 5) + 441</f>
+        <f t="shared" si="224"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM130" s="29" t="s">
@@ -24053,30 +24076,30 @@
         <v>45</v>
       </c>
       <c r="AU130" s="4">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV130" s="4">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW130" s="4">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX130" s="30" t="s">
         <v>45</v>
       </c>
       <c r="AY130" s="4">
-        <f t="shared" ref="AY130:AY139" si="248">AQ130-AU130</f>
+        <f t="shared" ref="AY130:AY139" si="249">AQ130-AU130</f>
         <v>130</v>
       </c>
       <c r="AZ130" s="4">
-        <f t="shared" ref="AZ130:AZ139" si="249">AR130-AV130</f>
+        <f t="shared" ref="AZ130:AZ139" si="250">AR130-AV130</f>
         <v>397</v>
       </c>
       <c r="BA130" s="29">
-        <f t="shared" ref="BA130:BA139" si="250">AS130-AW130</f>
+        <f t="shared" ref="BA130:BA139" si="251">AS130-AW130</f>
         <v>359</v>
       </c>
       <c r="BB130" s="4" t="s">
@@ -24158,17 +24181,18 @@
       <c r="AH131" t="s">
         <v>96</v>
       </c>
-      <c r="AI131" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ131" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK131" t="s">
-        <v>117</v>
+      <c r="AI131" s="6">
+        <v>77627</v>
+      </c>
+      <c r="AJ131" s="12">
+        <v>3425</v>
+      </c>
+      <c r="AK131">
+        <f>AI131+AJ131</f>
+        <v>81052</v>
       </c>
       <c r="AL131">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ131*AR131*AS131) * (AA131 / 5) + 441</f>
+        <f t="shared" si="224"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM131" s="10" t="s">
@@ -24196,30 +24220,30 @@
         <v>45</v>
       </c>
       <c r="AU131">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV131">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW131">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX131" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY131">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>130</v>
       </c>
       <c r="AZ131">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>397</v>
       </c>
       <c r="BA131" s="10">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>359</v>
       </c>
       <c r="BB131" t="s">
@@ -24301,17 +24325,18 @@
       <c r="AH132" t="s">
         <v>96</v>
       </c>
-      <c r="AI132" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ132" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK132" t="s">
-        <v>117</v>
+      <c r="AI132" s="6">
+        <v>77627</v>
+      </c>
+      <c r="AJ132" s="12">
+        <v>3425</v>
+      </c>
+      <c r="AK132">
+        <f>AI132+AJ132</f>
+        <v>81052</v>
       </c>
       <c r="AL132">
-        <f t="shared" ref="AL132:AL140" si="251" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ132*AR132*AS132) * (AA132 / 5) + 441</f>
+        <f t="shared" ref="AL132:AL140" si="252" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ132*AR132*AS132) * (AA132 / 5) + 441</f>
         <v>73500.060473349149</v>
       </c>
       <c r="AM132" s="10" t="s">
@@ -24339,30 +24364,30 @@
         <v>45</v>
       </c>
       <c r="AU132">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV132">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW132">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX132" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY132">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>130</v>
       </c>
       <c r="AZ132">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>397</v>
       </c>
       <c r="BA132" s="10">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>359</v>
       </c>
       <c r="BB132" t="s">
@@ -24444,17 +24469,18 @@
       <c r="AH133" t="s">
         <v>96</v>
       </c>
-      <c r="AI133" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ133" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK133" t="s">
-        <v>117</v>
+      <c r="AI133" s="6">
+        <v>77627</v>
+      </c>
+      <c r="AJ133" s="12">
+        <v>3425</v>
+      </c>
+      <c r="AK133">
+        <f>AI133+AJ133</f>
+        <v>81052</v>
       </c>
       <c r="AL133">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM133" s="10" t="s">
@@ -24482,30 +24508,30 @@
         <v>45</v>
       </c>
       <c r="AU133">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV133">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW133">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX133" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY133">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>130</v>
       </c>
       <c r="AZ133">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>397</v>
       </c>
       <c r="BA133" s="10">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>359</v>
       </c>
       <c r="BB133" t="s">
@@ -24587,17 +24613,18 @@
       <c r="AH134" t="s">
         <v>96</v>
       </c>
-      <c r="AI134" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ134" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK134" t="s">
-        <v>117</v>
+      <c r="AI134" s="6">
+        <v>77627</v>
+      </c>
+      <c r="AJ134" s="12">
+        <v>3425</v>
+      </c>
+      <c r="AK134">
+        <f>AI134+AJ134</f>
+        <v>81052</v>
       </c>
       <c r="AL134">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM134" s="10" t="s">
@@ -24625,30 +24652,30 @@
         <v>45</v>
       </c>
       <c r="AU134">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV134">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW134">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX134" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY134">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>130</v>
       </c>
       <c r="AZ134">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>397</v>
       </c>
       <c r="BA134" s="10">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>359</v>
       </c>
       <c r="BB134" t="s">
@@ -24730,17 +24757,18 @@
       <c r="AH135" t="s">
         <v>96</v>
       </c>
-      <c r="AI135" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ135" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK135" t="s">
-        <v>117</v>
+      <c r="AI135" s="6">
+        <v>77627</v>
+      </c>
+      <c r="AJ135" s="12">
+        <v>3425</v>
+      </c>
+      <c r="AK135">
+        <f>AI135+AJ135</f>
+        <v>81052</v>
       </c>
       <c r="AL135">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM135" s="10" t="s">
@@ -24768,30 +24796,30 @@
         <v>45</v>
       </c>
       <c r="AU135">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV135">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW135">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX135" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY135">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>130</v>
       </c>
       <c r="AZ135">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>397</v>
       </c>
       <c r="BA135" s="10">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>359</v>
       </c>
       <c r="BB135" t="s">
@@ -24873,17 +24901,18 @@
       <c r="AH136" t="s">
         <v>96</v>
       </c>
-      <c r="AI136" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ136" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK136" t="s">
-        <v>117</v>
+      <c r="AI136" s="6">
+        <v>77407</v>
+      </c>
+      <c r="AJ136" s="12">
+        <v>3645</v>
+      </c>
+      <c r="AK136">
+        <f>AI136+AJ136</f>
+        <v>81052</v>
       </c>
       <c r="AL136">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM136" s="10" t="s">
@@ -24911,30 +24940,30 @@
         <v>45</v>
       </c>
       <c r="AU136">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV136">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW136">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX136" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY136">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>130</v>
       </c>
       <c r="AZ136">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>397</v>
       </c>
       <c r="BA136" s="10">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>359</v>
       </c>
       <c r="BB136" t="s">
@@ -24964,7 +24993,7 @@
         <v>409</v>
       </c>
       <c r="F137" s="64" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="G137" s="12" t="s">
         <v>516</v>
@@ -24978,7 +25007,7 @@
       <c r="J137">
         <v>1</v>
       </c>
-      <c r="K137" s="70" t="s">
+      <c r="K137" s="12" t="s">
         <v>573</v>
       </c>
       <c r="L137">
@@ -25019,17 +25048,9 @@
       <c r="AH137" t="s">
         <v>96</v>
       </c>
-      <c r="AI137" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ137" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK137" t="s">
-        <v>117</v>
-      </c>
+      <c r="AJ137" s="12"/>
       <c r="AL137">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM137" s="10" t="s">
@@ -25057,30 +25078,30 @@
         <v>45</v>
       </c>
       <c r="AU137">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV137">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW137">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX137" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY137">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>130</v>
       </c>
       <c r="AZ137">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>397</v>
       </c>
       <c r="BA137" s="10">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>359</v>
       </c>
       <c r="BB137" t="s">
@@ -25168,17 +25189,18 @@
       <c r="AH138" t="s">
         <v>96</v>
       </c>
-      <c r="AI138" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ138" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK138" t="s">
-        <v>117</v>
+      <c r="AI138" s="6">
+        <v>77407</v>
+      </c>
+      <c r="AJ138" s="12">
+        <v>3645</v>
+      </c>
+      <c r="AK138">
+        <f>AI138+AJ138</f>
+        <v>81052</v>
       </c>
       <c r="AL138">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM138" s="10" t="s">
@@ -25206,30 +25228,30 @@
         <v>45</v>
       </c>
       <c r="AU138">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV138">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW138">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX138" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY138">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>130</v>
       </c>
       <c r="AZ138">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>397</v>
       </c>
       <c r="BA138" s="10">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>359</v>
       </c>
       <c r="BB138" t="s">
@@ -25259,7 +25281,7 @@
         <v>409</v>
       </c>
       <c r="F139" s="64" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="G139" s="12" t="s">
         <v>516</v>
@@ -25273,7 +25295,7 @@
       <c r="J139">
         <v>1</v>
       </c>
-      <c r="K139" s="70" t="s">
+      <c r="K139" s="12" t="s">
         <v>573</v>
       </c>
       <c r="L139">
@@ -25314,17 +25336,8 @@
       <c r="AH139" t="s">
         <v>96</v>
       </c>
-      <c r="AI139" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ139" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK139" t="s">
-        <v>117</v>
-      </c>
       <c r="AL139">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM139" s="10" t="s">
@@ -25352,30 +25365,30 @@
         <v>45</v>
       </c>
       <c r="AU139">
-        <f t="shared" si="242"/>
+        <f t="shared" si="243"/>
         <v>14</v>
       </c>
       <c r="AV139">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>115</v>
       </c>
       <c r="AW139">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>25</v>
       </c>
       <c r="AX139" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY139">
-        <f t="shared" si="248"/>
+        <f t="shared" si="249"/>
         <v>130</v>
       </c>
       <c r="AZ139">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>397</v>
       </c>
       <c r="BA139" s="10">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>359</v>
       </c>
       <c r="BB139" t="s">
@@ -25396,25 +25409,25 @@
     </row>
     <row r="140" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A140" s="12" t="s">
-        <v>117</v>
+        <v>574</v>
       </c>
       <c r="B140" s="12" t="s">
-        <v>117</v>
+        <v>575</v>
       </c>
       <c r="C140" t="s">
-        <v>117</v>
+        <v>457</v>
       </c>
       <c r="D140" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E140" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F140" s="64" t="s">
-        <v>117</v>
+        <v>577</v>
       </c>
       <c r="G140" s="12" t="s">
-        <v>117</v>
+        <v>578</v>
       </c>
       <c r="H140" s="12" t="s">
         <v>117</v>
@@ -25430,37 +25443,38 @@
       </c>
       <c r="T140" s="12"/>
       <c r="U140" s="20" t="s">
-        <v>117</v>
+        <v>579</v>
       </c>
       <c r="V140" t="s">
-        <v>117</v>
-      </c>
-      <c r="W140" t="s">
-        <v>117</v>
+        <v>580</v>
+      </c>
+      <c r="W140">
+        <v>6</v>
       </c>
       <c r="X140" t="s">
         <v>117</v>
       </c>
-      <c r="Y140" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC140" t="s">
-        <v>117</v>
+      <c r="Y140">
+        <v>3</v>
+      </c>
+      <c r="Z140">
+        <v>2</v>
+      </c>
+      <c r="AA140">
+        <f t="shared" si="217"/>
+        <v>5</v>
+      </c>
+      <c r="AB140">
+        <v>2</v>
+      </c>
+      <c r="AC140">
+        <v>1</v>
       </c>
       <c r="AE140" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AH140" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="AI140" s="6" t="s">
         <v>117</v>
@@ -25468,68 +25482,212 @@
       <c r="AJ140" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="AK140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AL140" t="e">
-        <f t="shared" si="251"/>
+      <c r="AK140" t="e">
+        <f>AI140+AJ140</f>
         <v>#VALUE!</v>
+      </c>
+      <c r="AL140">
+        <f t="shared" si="252"/>
+        <v>61574.894649960152</v>
       </c>
       <c r="AM140" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AN140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP140" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS140" t="s">
-        <v>117</v>
+      <c r="AN140">
+        <v>173</v>
+      </c>
+      <c r="AO140">
+        <v>743</v>
+      </c>
+      <c r="AP140" s="20">
+        <v>435</v>
+      </c>
+      <c r="AQ140">
+        <v>144</v>
+      </c>
+      <c r="AR140">
+        <v>512</v>
+      </c>
+      <c r="AS140">
+        <v>384</v>
       </c>
       <c r="AT140" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV140" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW140" t="s">
-        <v>117</v>
+        <v>45</v>
+      </c>
+      <c r="AU140">
+        <f t="shared" ref="AU140" si="253" xml:space="preserve"> _xlfn.FLOOR.MATH((AN140 - AQ140) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AV140">
+        <f t="shared" ref="AV140" si="254" xml:space="preserve"> _xlfn.FLOOR.MATH((AO140 - AR140) / 2)</f>
+        <v>115</v>
+      </c>
+      <c r="AW140">
+        <f t="shared" ref="AW140" si="255" xml:space="preserve"> _xlfn.FLOOR.MATH((AP140 - AS140) / 2)</f>
+        <v>25</v>
       </c>
       <c r="AX140" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY140" t="e">
-        <f t="shared" ref="AY140" si="252">AQ140-AU140</f>
+        <v>45</v>
+      </c>
+      <c r="AY140">
+        <f t="shared" ref="AY140" si="256">AQ140-AU140</f>
+        <v>130</v>
+      </c>
+      <c r="AZ140">
+        <f t="shared" ref="AZ140" si="257">AR140-AV140</f>
+        <v>397</v>
+      </c>
+      <c r="BA140" s="10">
+        <f t="shared" ref="BA140" si="258">AS140-AW140</f>
+        <v>359</v>
+      </c>
+      <c r="BB140" t="s">
+        <v>537</v>
+      </c>
+      <c r="BC140" t="s">
+        <v>528</v>
+      </c>
+      <c r="BD140" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="141" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A141" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B141" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C141" t="s">
+        <v>117</v>
+      </c>
+      <c r="D141" t="s">
+        <v>117</v>
+      </c>
+      <c r="E141" t="s">
+        <v>117</v>
+      </c>
+      <c r="F141" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G141" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H141" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I141" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J141" t="s">
+        <v>117</v>
+      </c>
+      <c r="L141" t="s">
+        <v>117</v>
+      </c>
+      <c r="T141" s="12"/>
+      <c r="U141" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V141" t="s">
+        <v>117</v>
+      </c>
+      <c r="W141" t="s">
+        <v>117</v>
+      </c>
+      <c r="X141" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y141" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI141" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ141" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK141" t="e">
+        <f>AI141+AJ141</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ140" t="e">
-        <f t="shared" ref="AZ140" si="253">AR140-AV140</f>
+      <c r="AL141" t="e">
+        <f t="shared" ref="AL141" si="259" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ141*AR141*AS141) * (AA141 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA140" s="10" t="e">
-        <f t="shared" ref="BA140" si="254">AS140-AW140</f>
+      <c r="AM141" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP141" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT141" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW141" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX141" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY141" t="e">
+        <f t="shared" ref="AY141" si="260">AQ141-AU141</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB140" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC140" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD140" t="s">
+      <c r="AZ141" t="e">
+        <f t="shared" ref="AZ141" si="261">AR141-AV141</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA141" s="10" t="e">
+        <f t="shared" ref="BA141" si="262">AS141-AW141</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB141" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC141" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD141" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
move some slurm scripting files
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B4A39A-C20F-4B68-9CB7-9A15DF44A8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0637A5C-B2EC-4C7A-B182-A4B088939C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-21720" yWindow="2550" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4031" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4499" uniqueCount="595">
   <si>
     <t>patch z</t>
   </si>
@@ -1867,6 +1867,48 @@
   </si>
   <si>
     <t>dataset10.c.1</t>
+  </si>
+  <si>
+    <t>240126-0</t>
+  </si>
+  <si>
+    <t>240126-1</t>
+  </si>
+  <si>
+    <t>240126-2</t>
+  </si>
+  <si>
+    <t>240126-3</t>
+  </si>
+  <si>
+    <t>240126-4</t>
+  </si>
+  <si>
+    <t>240126-5</t>
+  </si>
+  <si>
+    <t>240126-6</t>
+  </si>
+  <si>
+    <t>240126-7</t>
+  </si>
+  <si>
+    <t>240126-8</t>
+  </si>
+  <si>
+    <t>240126-9</t>
+  </si>
+  <si>
+    <t>240126-10</t>
+  </si>
+  <si>
+    <t>240126-11</t>
+  </si>
+  <si>
+    <t>240124-0 best</t>
+  </si>
+  <si>
+    <t>240124-0 last</t>
   </si>
 </sst>
 </file>
@@ -2219,7 +2261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2326,6 +2368,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2642,10 +2687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BF141"/>
+  <dimension ref="A1:BF153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL140" sqref="AL140"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -23452,11 +23497,11 @@
         <v>3425</v>
       </c>
       <c r="AK126">
-        <f>AI126+AJ126</f>
+        <f t="shared" ref="AK126:AK136" si="224">AI126+AJ126</f>
         <v>81052</v>
       </c>
       <c r="AL126">
-        <f t="shared" ref="AL126:AL131" si="224" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ126*AR126*AS126) * (AA126 / 5) + 441</f>
+        <f t="shared" ref="AL126:AL131" si="225" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ126*AR126*AS126) * (AA126 / 5) + 441</f>
         <v>73500.060473349149</v>
       </c>
       <c r="AM126" s="10" t="s">
@@ -23484,30 +23529,30 @@
         <v>45</v>
       </c>
       <c r="AU126">
-        <f t="shared" ref="AU126" si="225" xml:space="preserve"> _xlfn.FLOOR.MATH((AN126 - AQ126) / 2)</f>
+        <f t="shared" ref="AU126" si="226" xml:space="preserve"> _xlfn.FLOOR.MATH((AN126 - AQ126) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV126">
-        <f t="shared" ref="AV126" si="226" xml:space="preserve"> _xlfn.FLOOR.MATH((AO126 - AR126) / 2)</f>
+        <f t="shared" ref="AV126" si="227" xml:space="preserve"> _xlfn.FLOOR.MATH((AO126 - AR126) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW126">
-        <f t="shared" ref="AW126" si="227" xml:space="preserve"> _xlfn.FLOOR.MATH((AP126 - AS126) / 2)</f>
+        <f t="shared" ref="AW126" si="228" xml:space="preserve"> _xlfn.FLOOR.MATH((AP126 - AS126) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX126" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY126">
-        <f t="shared" ref="AY126" si="228">AQ126-AU126</f>
+        <f t="shared" ref="AY126" si="229">AQ126-AU126</f>
         <v>130</v>
       </c>
       <c r="AZ126">
-        <f t="shared" ref="AZ126" si="229">AR126-AV126</f>
+        <f t="shared" ref="AZ126" si="230">AR126-AV126</f>
         <v>397</v>
       </c>
       <c r="BA126" s="10">
-        <f t="shared" ref="BA126" si="230">AS126-AW126</f>
+        <f t="shared" ref="BA126" si="231">AS126-AW126</f>
         <v>359</v>
       </c>
       <c r="BB126" t="s">
@@ -23600,11 +23645,11 @@
         <v>3425</v>
       </c>
       <c r="AK127">
-        <f>AI127+AJ127</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL127">
-        <f t="shared" si="224"/>
+        <f t="shared" si="225"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM127" s="10" t="s">
@@ -23632,30 +23677,30 @@
         <v>45</v>
       </c>
       <c r="AU127">
-        <f t="shared" ref="AU127" si="231" xml:space="preserve"> _xlfn.FLOOR.MATH((AN127 - AQ127) / 2)</f>
+        <f t="shared" ref="AU127" si="232" xml:space="preserve"> _xlfn.FLOOR.MATH((AN127 - AQ127) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV127">
-        <f t="shared" ref="AV127" si="232" xml:space="preserve"> _xlfn.FLOOR.MATH((AO127 - AR127) / 2)</f>
+        <f t="shared" ref="AV127" si="233" xml:space="preserve"> _xlfn.FLOOR.MATH((AO127 - AR127) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW127">
-        <f t="shared" ref="AW127" si="233" xml:space="preserve"> _xlfn.FLOOR.MATH((AP127 - AS127) / 2)</f>
+        <f t="shared" ref="AW127" si="234" xml:space="preserve"> _xlfn.FLOOR.MATH((AP127 - AS127) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX127" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY127">
-        <f t="shared" ref="AY127" si="234">AQ127-AU127</f>
+        <f t="shared" ref="AY127" si="235">AQ127-AU127</f>
         <v>130</v>
       </c>
       <c r="AZ127">
-        <f t="shared" ref="AZ127" si="235">AR127-AV127</f>
+        <f t="shared" ref="AZ127" si="236">AR127-AV127</f>
         <v>397</v>
       </c>
       <c r="BA127" s="10">
-        <f t="shared" ref="BA127" si="236">AS127-AW127</f>
+        <f t="shared" ref="BA127" si="237">AS127-AW127</f>
         <v>359</v>
       </c>
       <c r="BB127" t="s">
@@ -23748,11 +23793,11 @@
         <v>3425</v>
       </c>
       <c r="AK128">
-        <f>AI128+AJ128</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL128">
-        <f t="shared" si="224"/>
+        <f t="shared" si="225"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM128" s="10" t="s">
@@ -23780,30 +23825,30 @@
         <v>45</v>
       </c>
       <c r="AU128">
-        <f t="shared" ref="AU128" si="237" xml:space="preserve"> _xlfn.FLOOR.MATH((AN128 - AQ128) / 2)</f>
+        <f t="shared" ref="AU128" si="238" xml:space="preserve"> _xlfn.FLOOR.MATH((AN128 - AQ128) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV128">
-        <f t="shared" ref="AV128" si="238" xml:space="preserve"> _xlfn.FLOOR.MATH((AO128 - AR128) / 2)</f>
+        <f t="shared" ref="AV128" si="239" xml:space="preserve"> _xlfn.FLOOR.MATH((AO128 - AR128) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW128">
-        <f t="shared" ref="AW128" si="239" xml:space="preserve"> _xlfn.FLOOR.MATH((AP128 - AS128) / 2)</f>
+        <f t="shared" ref="AW128" si="240" xml:space="preserve"> _xlfn.FLOOR.MATH((AP128 - AS128) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX128" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY128">
-        <f t="shared" ref="AY128" si="240">AQ128-AU128</f>
+        <f t="shared" ref="AY128" si="241">AQ128-AU128</f>
         <v>130</v>
       </c>
       <c r="AZ128">
-        <f t="shared" ref="AZ128" si="241">AR128-AV128</f>
+        <f t="shared" ref="AZ128" si="242">AR128-AV128</f>
         <v>397</v>
       </c>
       <c r="BA128" s="10">
-        <f t="shared" ref="BA128" si="242">AS128-AW128</f>
+        <f t="shared" ref="BA128" si="243">AS128-AW128</f>
         <v>359</v>
       </c>
       <c r="BB128" t="s">
@@ -23896,11 +23941,11 @@
         <v>3425</v>
       </c>
       <c r="AK129">
-        <f>AI129+AJ129</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL129">
-        <f t="shared" si="224"/>
+        <f t="shared" si="225"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM129" s="10" t="s">
@@ -23928,30 +23973,30 @@
         <v>45</v>
       </c>
       <c r="AU129">
-        <f t="shared" ref="AU129:AU139" si="243" xml:space="preserve"> _xlfn.FLOOR.MATH((AN129 - AQ129) / 2)</f>
+        <f t="shared" ref="AU129:AU139" si="244" xml:space="preserve"> _xlfn.FLOOR.MATH((AN129 - AQ129) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV129">
-        <f t="shared" ref="AV129:AV139" si="244" xml:space="preserve"> _xlfn.FLOOR.MATH((AO129 - AR129) / 2)</f>
+        <f t="shared" ref="AV129:AV139" si="245" xml:space="preserve"> _xlfn.FLOOR.MATH((AO129 - AR129) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW129">
-        <f t="shared" ref="AW129:AW139" si="245" xml:space="preserve"> _xlfn.FLOOR.MATH((AP129 - AS129) / 2)</f>
+        <f t="shared" ref="AW129:AW139" si="246" xml:space="preserve"> _xlfn.FLOOR.MATH((AP129 - AS129) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX129" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY129">
-        <f t="shared" ref="AY129" si="246">AQ129-AU129</f>
+        <f t="shared" ref="AY129" si="247">AQ129-AU129</f>
         <v>130</v>
       </c>
       <c r="AZ129">
-        <f t="shared" ref="AZ129" si="247">AR129-AV129</f>
+        <f t="shared" ref="AZ129" si="248">AR129-AV129</f>
         <v>397</v>
       </c>
       <c r="BA129" s="10">
-        <f t="shared" ref="BA129" si="248">AS129-AW129</f>
+        <f t="shared" ref="BA129" si="249">AS129-AW129</f>
         <v>359</v>
       </c>
       <c r="BB129" t="s">
@@ -24044,11 +24089,11 @@
         <v>3645</v>
       </c>
       <c r="AK130" s="4">
-        <f>AI130+AJ130</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL130" s="4">
-        <f t="shared" si="224"/>
+        <f t="shared" si="225"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM130" s="29" t="s">
@@ -24076,30 +24121,30 @@
         <v>45</v>
       </c>
       <c r="AU130" s="4">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV130" s="4">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW130" s="4">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX130" s="30" t="s">
         <v>45</v>
       </c>
       <c r="AY130" s="4">
-        <f t="shared" ref="AY130:AY139" si="249">AQ130-AU130</f>
+        <f t="shared" ref="AY130:AY139" si="250">AQ130-AU130</f>
         <v>130</v>
       </c>
       <c r="AZ130" s="4">
-        <f t="shared" ref="AZ130:AZ139" si="250">AR130-AV130</f>
+        <f t="shared" ref="AZ130:AZ139" si="251">AR130-AV130</f>
         <v>397</v>
       </c>
       <c r="BA130" s="29">
-        <f t="shared" ref="BA130:BA139" si="251">AS130-AW130</f>
+        <f t="shared" ref="BA130:BA139" si="252">AS130-AW130</f>
         <v>359</v>
       </c>
       <c r="BB130" s="4" t="s">
@@ -24188,11 +24233,11 @@
         <v>3425</v>
       </c>
       <c r="AK131">
-        <f>AI131+AJ131</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL131">
-        <f t="shared" si="224"/>
+        <f t="shared" si="225"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM131" s="10" t="s">
@@ -24220,30 +24265,30 @@
         <v>45</v>
       </c>
       <c r="AU131">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV131">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW131">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX131" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY131">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>130</v>
       </c>
       <c r="AZ131">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>397</v>
       </c>
       <c r="BA131" s="10">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>359</v>
       </c>
       <c r="BB131" t="s">
@@ -24332,11 +24377,11 @@
         <v>3425</v>
       </c>
       <c r="AK132">
-        <f>AI132+AJ132</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL132">
-        <f t="shared" ref="AL132:AL140" si="252" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ132*AR132*AS132) * (AA132 / 5) + 441</f>
+        <f t="shared" ref="AL132:AL140" si="253" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ132*AR132*AS132) * (AA132 / 5) + 441</f>
         <v>73500.060473349149</v>
       </c>
       <c r="AM132" s="10" t="s">
@@ -24364,30 +24409,30 @@
         <v>45</v>
       </c>
       <c r="AU132">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV132">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW132">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX132" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY132">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>130</v>
       </c>
       <c r="AZ132">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>397</v>
       </c>
       <c r="BA132" s="10">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>359</v>
       </c>
       <c r="BB132" t="s">
@@ -24476,11 +24521,11 @@
         <v>3425</v>
       </c>
       <c r="AK133">
-        <f>AI133+AJ133</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL133">
-        <f t="shared" si="252"/>
+        <f t="shared" si="253"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM133" s="10" t="s">
@@ -24508,30 +24553,30 @@
         <v>45</v>
       </c>
       <c r="AU133">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV133">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW133">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX133" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY133">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>130</v>
       </c>
       <c r="AZ133">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>397</v>
       </c>
       <c r="BA133" s="10">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>359</v>
       </c>
       <c r="BB133" t="s">
@@ -24620,11 +24665,11 @@
         <v>3425</v>
       </c>
       <c r="AK134">
-        <f>AI134+AJ134</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL134">
-        <f t="shared" si="252"/>
+        <f t="shared" si="253"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM134" s="10" t="s">
@@ -24652,30 +24697,30 @@
         <v>45</v>
       </c>
       <c r="AU134">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV134">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW134">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX134" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY134">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>130</v>
       </c>
       <c r="AZ134">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>397</v>
       </c>
       <c r="BA134" s="10">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>359</v>
       </c>
       <c r="BB134" t="s">
@@ -24764,11 +24809,11 @@
         <v>3425</v>
       </c>
       <c r="AK135">
-        <f>AI135+AJ135</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL135">
-        <f t="shared" si="252"/>
+        <f t="shared" si="253"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM135" s="10" t="s">
@@ -24796,30 +24841,30 @@
         <v>45</v>
       </c>
       <c r="AU135">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV135">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW135">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX135" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY135">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>130</v>
       </c>
       <c r="AZ135">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>397</v>
       </c>
       <c r="BA135" s="10">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>359</v>
       </c>
       <c r="BB135" t="s">
@@ -24908,11 +24953,11 @@
         <v>3645</v>
       </c>
       <c r="AK136">
-        <f>AI136+AJ136</f>
+        <f t="shared" si="224"/>
         <v>81052</v>
       </c>
       <c r="AL136">
-        <f t="shared" si="252"/>
+        <f t="shared" si="253"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM136" s="10" t="s">
@@ -24940,30 +24985,30 @@
         <v>45</v>
       </c>
       <c r="AU136">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV136">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW136">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX136" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY136">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>130</v>
       </c>
       <c r="AZ136">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>397</v>
       </c>
       <c r="BA136" s="10">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>359</v>
       </c>
       <c r="BB136" t="s">
@@ -25050,7 +25095,7 @@
       </c>
       <c r="AJ137" s="12"/>
       <c r="AL137">
-        <f t="shared" si="252"/>
+        <f t="shared" si="253"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM137" s="10" t="s">
@@ -25078,30 +25123,30 @@
         <v>45</v>
       </c>
       <c r="AU137">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV137">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW137">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX137" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY137">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>130</v>
       </c>
       <c r="AZ137">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>397</v>
       </c>
       <c r="BA137" s="10">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>359</v>
       </c>
       <c r="BB137" t="s">
@@ -25200,7 +25245,7 @@
         <v>81052</v>
       </c>
       <c r="AL138">
-        <f t="shared" si="252"/>
+        <f t="shared" si="253"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM138" s="10" t="s">
@@ -25228,30 +25273,30 @@
         <v>45</v>
       </c>
       <c r="AU138">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV138">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW138">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX138" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY138">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>130</v>
       </c>
       <c r="AZ138">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>397</v>
       </c>
       <c r="BA138" s="10">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>359</v>
       </c>
       <c r="BB138" t="s">
@@ -25337,7 +25382,7 @@
         <v>96</v>
       </c>
       <c r="AL139">
-        <f t="shared" si="252"/>
+        <f t="shared" si="253"/>
         <v>73500.060473349149</v>
       </c>
       <c r="AM139" s="10" t="s">
@@ -25365,30 +25410,30 @@
         <v>45</v>
       </c>
       <c r="AU139">
-        <f t="shared" si="243"/>
+        <f t="shared" si="244"/>
         <v>14</v>
       </c>
       <c r="AV139">
-        <f t="shared" si="244"/>
+        <f t="shared" si="245"/>
         <v>115</v>
       </c>
       <c r="AW139">
-        <f t="shared" si="245"/>
+        <f t="shared" si="246"/>
         <v>25</v>
       </c>
       <c r="AX139" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY139">
-        <f t="shared" si="249"/>
+        <f t="shared" si="250"/>
         <v>130</v>
       </c>
       <c r="AZ139">
-        <f t="shared" si="250"/>
+        <f t="shared" si="251"/>
         <v>397</v>
       </c>
       <c r="BA139" s="10">
-        <f t="shared" si="251"/>
+        <f t="shared" si="252"/>
         <v>359</v>
       </c>
       <c r="BB139" t="s">
@@ -25487,7 +25532,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AL140">
-        <f t="shared" si="252"/>
+        <f t="shared" si="253"/>
         <v>61574.894649960152</v>
       </c>
       <c r="AM140" s="10" t="s">
@@ -25515,30 +25560,30 @@
         <v>45</v>
       </c>
       <c r="AU140">
-        <f t="shared" ref="AU140" si="253" xml:space="preserve"> _xlfn.FLOOR.MATH((AN140 - AQ140) / 2)</f>
+        <f t="shared" ref="AU140" si="254" xml:space="preserve"> _xlfn.FLOOR.MATH((AN140 - AQ140) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV140">
-        <f t="shared" ref="AV140" si="254" xml:space="preserve"> _xlfn.FLOOR.MATH((AO140 - AR140) / 2)</f>
+        <f t="shared" ref="AV140" si="255" xml:space="preserve"> _xlfn.FLOOR.MATH((AO140 - AR140) / 2)</f>
         <v>115</v>
       </c>
       <c r="AW140">
-        <f t="shared" ref="AW140" si="255" xml:space="preserve"> _xlfn.FLOOR.MATH((AP140 - AS140) / 2)</f>
+        <f t="shared" ref="AW140" si="256" xml:space="preserve"> _xlfn.FLOOR.MATH((AP140 - AS140) / 2)</f>
         <v>25</v>
       </c>
       <c r="AX140" s="25" t="s">
         <v>45</v>
       </c>
       <c r="AY140">
-        <f t="shared" ref="AY140" si="256">AQ140-AU140</f>
+        <f t="shared" ref="AY140" si="257">AQ140-AU140</f>
         <v>130</v>
       </c>
       <c r="AZ140">
-        <f t="shared" ref="AZ140" si="257">AR140-AV140</f>
+        <f t="shared" ref="AZ140" si="258">AR140-AV140</f>
         <v>397</v>
       </c>
       <c r="BA140" s="10">
-        <f t="shared" ref="BA140" si="258">AS140-AW140</f>
+        <f t="shared" ref="BA140" si="259">AS140-AW140</f>
         <v>359</v>
       </c>
       <c r="BB140" t="s">
@@ -25552,14 +25597,14 @@
       </c>
     </row>
     <row r="141" spans="1:58" x14ac:dyDescent="0.25">
-      <c r="A141" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="B141" s="12" t="s">
-        <v>117</v>
+      <c r="A141" s="70" t="s">
+        <v>581</v>
+      </c>
+      <c r="B141" s="70" t="s">
+        <v>593</v>
       </c>
       <c r="C141" t="s">
-        <v>117</v>
+        <v>477</v>
       </c>
       <c r="D141" t="s">
         <v>117</v>
@@ -25630,7 +25675,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AL141" t="e">
-        <f t="shared" ref="AL141" si="259" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ141*AR141*AS141) * (AA141 / 5) + 441</f>
+        <f t="shared" ref="AL141" si="260" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ141*AR141*AS141) * (AA141 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
       <c r="AM141" s="10" t="s">
@@ -25670,15 +25715,15 @@
         <v>8</v>
       </c>
       <c r="AY141" t="e">
-        <f t="shared" ref="AY141" si="260">AQ141-AU141</f>
+        <f t="shared" ref="AY141" si="261">AQ141-AU141</f>
         <v>#VALUE!</v>
       </c>
       <c r="AZ141" t="e">
-        <f t="shared" ref="AZ141" si="261">AR141-AV141</f>
+        <f t="shared" ref="AZ141" si="262">AR141-AV141</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA141" s="10" t="e">
-        <f t="shared" ref="BA141" si="262">AS141-AW141</f>
+        <f t="shared" ref="BA141" si="263">AS141-AW141</f>
         <v>#VALUE!</v>
       </c>
       <c r="BB141" t="s">
@@ -25688,6 +25733,1686 @@
         <v>117</v>
       </c>
       <c r="BD141" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="142" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A142" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="B142" s="12" t="s">
+        <v>594</v>
+      </c>
+      <c r="C142" t="s">
+        <v>477</v>
+      </c>
+      <c r="D142" t="s">
+        <v>117</v>
+      </c>
+      <c r="E142" t="s">
+        <v>117</v>
+      </c>
+      <c r="F142" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G142" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H142" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I142" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J142" t="s">
+        <v>117</v>
+      </c>
+      <c r="L142" t="s">
+        <v>117</v>
+      </c>
+      <c r="T142" s="12"/>
+      <c r="U142" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V142" t="s">
+        <v>117</v>
+      </c>
+      <c r="W142" t="s">
+        <v>117</v>
+      </c>
+      <c r="X142" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y142" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI142" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ142" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK142" t="e">
+        <f t="shared" ref="AK142:AK152" si="264">AI142+AJ142</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL142" t="e">
+        <f t="shared" ref="AL142:AL152" si="265" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ142*AR142*AS142) * (AA142 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM142" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP142" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT142" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW142" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX142" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY142" t="e">
+        <f t="shared" ref="AY142:AY152" si="266">AQ142-AU142</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ142" t="e">
+        <f t="shared" ref="AZ142:AZ152" si="267">AR142-AV142</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA142" s="10" t="e">
+        <f t="shared" ref="BA142:BA152" si="268">AS142-AW142</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB142" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC142" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD142" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="143" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A143" s="12" t="s">
+        <v>583</v>
+      </c>
+      <c r="B143" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C143" t="s">
+        <v>477</v>
+      </c>
+      <c r="D143" t="s">
+        <v>117</v>
+      </c>
+      <c r="E143" t="s">
+        <v>117</v>
+      </c>
+      <c r="F143" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G143" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H143" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I143" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J143" t="s">
+        <v>117</v>
+      </c>
+      <c r="L143" t="s">
+        <v>117</v>
+      </c>
+      <c r="T143" s="12"/>
+      <c r="U143" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V143" t="s">
+        <v>117</v>
+      </c>
+      <c r="W143" t="s">
+        <v>117</v>
+      </c>
+      <c r="X143" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y143" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI143" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ143" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK143" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL143" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM143" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP143" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT143" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW143" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX143" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY143" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ143" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA143" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB143" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC143" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD143" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="144" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A144" s="12" t="s">
+        <v>584</v>
+      </c>
+      <c r="B144" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C144" t="s">
+        <v>477</v>
+      </c>
+      <c r="D144" t="s">
+        <v>117</v>
+      </c>
+      <c r="E144" t="s">
+        <v>117</v>
+      </c>
+      <c r="F144" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G144" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H144" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I144" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J144" t="s">
+        <v>117</v>
+      </c>
+      <c r="L144" t="s">
+        <v>117</v>
+      </c>
+      <c r="T144" s="12"/>
+      <c r="U144" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V144" t="s">
+        <v>117</v>
+      </c>
+      <c r="W144" t="s">
+        <v>117</v>
+      </c>
+      <c r="X144" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y144" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI144" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ144" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK144" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL144" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM144" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP144" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT144" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW144" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX144" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY144" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ144" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA144" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB144" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC144" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD144" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="145" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A145" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="B145" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C145" t="s">
+        <v>477</v>
+      </c>
+      <c r="D145" t="s">
+        <v>117</v>
+      </c>
+      <c r="E145" t="s">
+        <v>117</v>
+      </c>
+      <c r="F145" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G145" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H145" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I145" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J145" t="s">
+        <v>117</v>
+      </c>
+      <c r="L145" t="s">
+        <v>117</v>
+      </c>
+      <c r="T145" s="12"/>
+      <c r="U145" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V145" t="s">
+        <v>117</v>
+      </c>
+      <c r="W145" t="s">
+        <v>117</v>
+      </c>
+      <c r="X145" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y145" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI145" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ145" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK145" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL145" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM145" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP145" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT145" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW145" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX145" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY145" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ145" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA145" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB145" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC145" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD145" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="146" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A146" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="B146" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C146" t="s">
+        <v>477</v>
+      </c>
+      <c r="D146" t="s">
+        <v>117</v>
+      </c>
+      <c r="E146" t="s">
+        <v>117</v>
+      </c>
+      <c r="F146" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G146" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H146" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I146" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J146" t="s">
+        <v>117</v>
+      </c>
+      <c r="L146" t="s">
+        <v>117</v>
+      </c>
+      <c r="T146" s="12"/>
+      <c r="U146" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V146" t="s">
+        <v>117</v>
+      </c>
+      <c r="W146" t="s">
+        <v>117</v>
+      </c>
+      <c r="X146" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y146" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI146" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ146" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK146" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL146" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM146" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP146" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT146" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW146" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX146" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY146" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ146" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA146" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB146" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC146" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD146" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="147" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A147" s="12" t="s">
+        <v>587</v>
+      </c>
+      <c r="B147" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C147" t="s">
+        <v>477</v>
+      </c>
+      <c r="D147" t="s">
+        <v>117</v>
+      </c>
+      <c r="E147" t="s">
+        <v>117</v>
+      </c>
+      <c r="F147" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G147" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H147" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I147" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J147" t="s">
+        <v>117</v>
+      </c>
+      <c r="L147" t="s">
+        <v>117</v>
+      </c>
+      <c r="T147" s="12"/>
+      <c r="U147" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V147" t="s">
+        <v>117</v>
+      </c>
+      <c r="W147" t="s">
+        <v>117</v>
+      </c>
+      <c r="X147" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y147" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI147" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ147" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK147" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL147" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM147" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP147" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT147" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW147" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX147" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY147" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ147" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA147" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB147" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC147" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD147" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="148" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A148" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="B148" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C148" t="s">
+        <v>477</v>
+      </c>
+      <c r="D148" t="s">
+        <v>117</v>
+      </c>
+      <c r="E148" t="s">
+        <v>117</v>
+      </c>
+      <c r="F148" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G148" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H148" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I148" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J148" t="s">
+        <v>117</v>
+      </c>
+      <c r="L148" t="s">
+        <v>117</v>
+      </c>
+      <c r="T148" s="12"/>
+      <c r="U148" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V148" t="s">
+        <v>117</v>
+      </c>
+      <c r="W148" t="s">
+        <v>117</v>
+      </c>
+      <c r="X148" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y148" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI148" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ148" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK148" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL148" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM148" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP148" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT148" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW148" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX148" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY148" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ148" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA148" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB148" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC148" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD148" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="149" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A149" s="12" t="s">
+        <v>589</v>
+      </c>
+      <c r="B149" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C149" t="s">
+        <v>477</v>
+      </c>
+      <c r="D149" t="s">
+        <v>117</v>
+      </c>
+      <c r="E149" t="s">
+        <v>117</v>
+      </c>
+      <c r="F149" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G149" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H149" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I149" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J149" t="s">
+        <v>117</v>
+      </c>
+      <c r="L149" t="s">
+        <v>117</v>
+      </c>
+      <c r="T149" s="12"/>
+      <c r="U149" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V149" t="s">
+        <v>117</v>
+      </c>
+      <c r="W149" t="s">
+        <v>117</v>
+      </c>
+      <c r="X149" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y149" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI149" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ149" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK149" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL149" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM149" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP149" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT149" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW149" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX149" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY149" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ149" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA149" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB149" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC149" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD149" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="150" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A150" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="B150" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C150" t="s">
+        <v>477</v>
+      </c>
+      <c r="D150" t="s">
+        <v>117</v>
+      </c>
+      <c r="E150" t="s">
+        <v>117</v>
+      </c>
+      <c r="F150" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G150" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H150" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I150" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J150" t="s">
+        <v>117</v>
+      </c>
+      <c r="L150" t="s">
+        <v>117</v>
+      </c>
+      <c r="T150" s="12"/>
+      <c r="U150" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V150" t="s">
+        <v>117</v>
+      </c>
+      <c r="W150" t="s">
+        <v>117</v>
+      </c>
+      <c r="X150" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y150" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI150" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ150" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK150" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL150" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM150" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP150" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT150" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW150" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX150" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY150" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ150" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA150" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB150" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC150" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD150" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="151" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A151" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="B151" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C151" t="s">
+        <v>477</v>
+      </c>
+      <c r="D151" t="s">
+        <v>117</v>
+      </c>
+      <c r="E151" t="s">
+        <v>117</v>
+      </c>
+      <c r="F151" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G151" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H151" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I151" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J151" t="s">
+        <v>117</v>
+      </c>
+      <c r="L151" t="s">
+        <v>117</v>
+      </c>
+      <c r="T151" s="12"/>
+      <c r="U151" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V151" t="s">
+        <v>117</v>
+      </c>
+      <c r="W151" t="s">
+        <v>117</v>
+      </c>
+      <c r="X151" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y151" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI151" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ151" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK151" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL151" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM151" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP151" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT151" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW151" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX151" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY151" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ151" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA151" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB151" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC151" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD151" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="152" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A152" s="12" t="s">
+        <v>592</v>
+      </c>
+      <c r="B152" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C152" t="s">
+        <v>117</v>
+      </c>
+      <c r="D152" t="s">
+        <v>117</v>
+      </c>
+      <c r="E152" t="s">
+        <v>117</v>
+      </c>
+      <c r="F152" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G152" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H152" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I152" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J152" t="s">
+        <v>117</v>
+      </c>
+      <c r="L152" t="s">
+        <v>117</v>
+      </c>
+      <c r="T152" s="12"/>
+      <c r="U152" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V152" t="s">
+        <v>117</v>
+      </c>
+      <c r="W152" t="s">
+        <v>117</v>
+      </c>
+      <c r="X152" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y152" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI152" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ152" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK152" t="e">
+        <f t="shared" si="264"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL152" t="e">
+        <f t="shared" si="265"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM152" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP152" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT152" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW152" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX152" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY152" t="e">
+        <f t="shared" si="266"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ152" t="e">
+        <f t="shared" si="267"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA152" s="10" t="e">
+        <f t="shared" si="268"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB152" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC152" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD152" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="153" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A153" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B153" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C153" t="s">
+        <v>117</v>
+      </c>
+      <c r="D153" t="s">
+        <v>117</v>
+      </c>
+      <c r="E153" t="s">
+        <v>117</v>
+      </c>
+      <c r="F153" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G153" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H153" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I153" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J153" t="s">
+        <v>117</v>
+      </c>
+      <c r="L153" t="s">
+        <v>117</v>
+      </c>
+      <c r="T153" s="12"/>
+      <c r="U153" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V153" t="s">
+        <v>117</v>
+      </c>
+      <c r="W153" t="s">
+        <v>117</v>
+      </c>
+      <c r="X153" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y153" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI153" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ153" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK153" t="e">
+        <f t="shared" ref="AK153" si="269">AI153+AJ153</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL153" t="e">
+        <f t="shared" ref="AL153" si="270" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ153*AR153*AS153) * (AA153 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM153" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP153" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT153" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW153" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX153" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY153" t="e">
+        <f t="shared" ref="AY153" si="271">AQ153-AU153</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ153" t="e">
+        <f t="shared" ref="AZ153" si="272">AR153-AV153</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA153" s="10" t="e">
+        <f t="shared" ref="BA153" si="273">AS153-AW153</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB153" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC153" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD153" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generic commit message, Wed 17:35:48 31.01.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD654A0-7C21-4525-9C71-94C31A0CDD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D83568C-7F8E-4E59-AAEC-989FAE6D7785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4499" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4964" uniqueCount="628">
   <si>
     <t>patch z</t>
   </si>
@@ -1863,9 +1863,6 @@
     <t>Success (finish training &amp; answer question)</t>
   </si>
   <si>
-    <t>1 (verify)</t>
-  </si>
-  <si>
     <t>dataset10.c.1</t>
   </si>
   <si>
@@ -1909,6 +1906,108 @@
   </si>
   <si>
     <t>240131-11</t>
+  </si>
+  <si>
+    <t>240131-12</t>
+  </si>
+  <si>
+    <t>240131-13</t>
+  </si>
+  <si>
+    <t>240131-14</t>
+  </si>
+  <si>
+    <t>240131-15</t>
+  </si>
+  <si>
+    <t>240131-16</t>
+  </si>
+  <si>
+    <t>240131-17</t>
+  </si>
+  <si>
+    <t>240131-18</t>
+  </si>
+  <si>
+    <t>240131-19</t>
+  </si>
+  <si>
+    <t>240131-20</t>
+  </si>
+  <si>
+    <t>240131-21</t>
+  </si>
+  <si>
+    <t>240131-22</t>
+  </si>
+  <si>
+    <t>240131-23</t>
+  </si>
+  <si>
+    <t>240124-1 best</t>
+  </si>
+  <si>
+    <t>240124-1 last</t>
+  </si>
+  <si>
+    <t>240124-2 best</t>
+  </si>
+  <si>
+    <t>240124-2 last</t>
+  </si>
+  <si>
+    <t>240124-3 best</t>
+  </si>
+  <si>
+    <t>240124-3 last</t>
+  </si>
+  <si>
+    <t>240124-4 best</t>
+  </si>
+  <si>
+    <t>240124-4 last</t>
+  </si>
+  <si>
+    <t>240125-0 best</t>
+  </si>
+  <si>
+    <t>240125-0 last</t>
+  </si>
+  <si>
+    <t>240125-1 best</t>
+  </si>
+  <si>
+    <t>240125-1 last</t>
+  </si>
+  <si>
+    <t>240125-2 best</t>
+  </si>
+  <si>
+    <t>240125-2 last</t>
+  </si>
+  <si>
+    <t>240125-3 best</t>
+  </si>
+  <si>
+    <t>240125-3 last</t>
+  </si>
+  <si>
+    <t>240125-4 best</t>
+  </si>
+  <si>
+    <t>240125-4 last</t>
+  </si>
+  <si>
+    <t>240125-5 best</t>
+  </si>
+  <si>
+    <t>240125-5 last</t>
+  </si>
+  <si>
+    <t>240125-7 best</t>
+  </si>
+  <si>
+    <t>240125-7 last</t>
   </si>
 </sst>
 </file>
@@ -2261,7 +2360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2368,9 +2467,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2690,70 +2786,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BF153"/>
+  <dimension ref="A1:BF165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="50.109375" customWidth="1"/>
-    <col min="3" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="3" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
     <col min="6" max="6" width="57" style="61" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="24.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="64.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="14.5546875" style="6" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="8.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="30.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="9.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="64.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="14.5703125" style="6" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1" outlineLevel="1"/>
     <col min="13" max="13" width="33" customWidth="1"/>
-    <col min="14" max="20" width="9.109375" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="9.109375" style="20"/>
-    <col min="22" max="22" width="15.109375" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="9.109375" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="6.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="5.109375" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="11.109375" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="20" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="9.140625" style="20"/>
+    <col min="22" max="22" width="15.140625" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="25" max="25" width="6.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="5.140625" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="11.140625" customWidth="1" outlineLevel="1"/>
     <col min="28" max="28" width="6" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="14.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="9.5546875" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="14.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="9.5703125" customWidth="1" outlineLevel="1"/>
     <col min="31" max="31" width="9" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="9.44140625" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="9.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="9.6640625" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="16.6640625" style="6" customWidth="1"/>
-    <col min="36" max="37" width="14.88671875" customWidth="1"/>
+    <col min="32" max="32" width="9.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="9.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="9.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="16.7109375" style="6" customWidth="1"/>
+    <col min="36" max="37" width="14.85546875" customWidth="1"/>
     <col min="38" max="38" width="21" customWidth="1"/>
-    <col min="39" max="39" width="26.33203125" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="10.6640625" customWidth="1"/>
-    <col min="41" max="41" width="10.5546875" customWidth="1"/>
-    <col min="42" max="42" width="10.88671875" style="20" customWidth="1"/>
-    <col min="43" max="43" width="5.33203125" customWidth="1"/>
-    <col min="44" max="44" width="6.109375" customWidth="1"/>
+    <col min="39" max="39" width="26.28515625" style="10" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="10.7109375" customWidth="1"/>
+    <col min="41" max="41" width="10.5703125" customWidth="1"/>
+    <col min="42" max="42" width="10.85546875" style="20" customWidth="1"/>
+    <col min="43" max="43" width="5.28515625" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" customWidth="1"/>
     <col min="45" max="45" width="5" customWidth="1"/>
     <col min="46" max="46" width="5" style="20" customWidth="1"/>
-    <col min="47" max="47" width="6.109375" customWidth="1"/>
-    <col min="48" max="48" width="6.5546875" customWidth="1"/>
+    <col min="47" max="47" width="6.140625" customWidth="1"/>
+    <col min="48" max="48" width="6.5703125" customWidth="1"/>
     <col min="49" max="49" width="5" customWidth="1"/>
     <col min="50" max="50" width="6" style="20" customWidth="1"/>
     <col min="51" max="52" width="6" customWidth="1"/>
     <col min="53" max="53" width="6" style="10" customWidth="1"/>
-    <col min="54" max="54" width="74.88671875" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="76.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="5.109375" customWidth="1"/>
-    <col min="57" max="57" width="135.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="74.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="76.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="5.140625" customWidth="1"/>
+    <col min="57" max="57" width="135.28515625" customWidth="1" outlineLevel="1"/>
     <col min="58" max="58" width="206" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.6640625" customWidth="1"/>
-    <col min="63" max="63" width="12.109375" customWidth="1"/>
+    <col min="59" max="59" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.7109375" customWidth="1"/>
+    <col min="63" max="63" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -2929,7 +3025,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -3097,7 +3193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3266,7 +3362,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:58" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>51</v>
       </c>
@@ -3434,7 +3530,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3599,7 +3695,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -3764,7 +3860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3929,7 +4025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4094,7 +4190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4265,7 +4361,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -4430,7 +4526,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4595,7 +4691,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -4761,7 +4857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -4926,7 +5022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -5091,7 +5187,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -5257,7 +5353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
@@ -5424,7 +5520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -5590,7 +5686,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -5756,7 +5852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -5922,7 +6018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -6088,7 +6184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -6254,7 +6350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -6420,7 +6516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -6586,7 +6682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -6752,7 +6848,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -6919,7 +7015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>99</v>
       </c>
@@ -7086,7 +7182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -7256,7 +7352,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -7425,7 +7521,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -7595,7 +7691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -7765,7 +7861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -7935,7 +8031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -8104,7 +8200,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -8273,7 +8369,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -8442,7 +8538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -8611,7 +8707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>180</v>
       </c>
@@ -8780,7 +8876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -8949,7 +9045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -9118,7 +9214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>191</v>
       </c>
@@ -9287,7 +9383,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>195</v>
       </c>
@@ -9456,7 +9552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>196</v>
       </c>
@@ -9625,7 +9721,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>198</v>
       </c>
@@ -9794,7 +9890,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>201</v>
       </c>
@@ -9963,7 +10059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>202</v>
       </c>
@@ -10133,7 +10229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>203</v>
       </c>
@@ -10304,7 +10400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>235</v>
       </c>
@@ -10469,7 +10565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>236</v>
       </c>
@@ -10634,7 +10730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>237</v>
       </c>
@@ -10799,7 +10895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>238</v>
       </c>
@@ -10964,7 +11060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
         <v>239</v>
       </c>
@@ -11129,7 +11225,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>240</v>
       </c>
@@ -11294,7 +11390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>241</v>
       </c>
@@ -11459,7 +11555,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>242</v>
       </c>
@@ -11624,7 +11720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>243</v>
       </c>
@@ -11789,7 +11885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>244</v>
       </c>
@@ -11954,7 +12050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>245</v>
       </c>
@@ -12119,7 +12215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>246</v>
       </c>
@@ -12284,7 +12380,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>247</v>
       </c>
@@ -12449,7 +12545,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>248</v>
       </c>
@@ -12614,7 +12710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>249</v>
       </c>
@@ -12779,7 +12875,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>250</v>
       </c>
@@ -12944,7 +13040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>251</v>
       </c>
@@ -13109,7 +13205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>252</v>
       </c>
@@ -13275,7 +13371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:58" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:58" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
         <v>267</v>
       </c>
@@ -13445,7 +13541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>269</v>
       </c>
@@ -13622,7 +13718,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="66" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>274</v>
       </c>
@@ -13799,7 +13895,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="67" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>289</v>
       </c>
@@ -13976,7 +14072,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="68" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>292</v>
       </c>
@@ -14153,7 +14249,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>293</v>
       </c>
@@ -14330,7 +14426,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>298</v>
       </c>
@@ -14510,7 +14606,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>299</v>
       </c>
@@ -14687,7 +14783,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="72" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>302</v>
       </c>
@@ -14864,7 +14960,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="73" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>321</v>
       </c>
@@ -15044,7 +15140,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>323</v>
       </c>
@@ -15221,7 +15317,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="75" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>331</v>
       </c>
@@ -15395,7 +15491,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="76" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>334</v>
       </c>
@@ -15569,7 +15665,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="77" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>350</v>
       </c>
@@ -15578,7 +15674,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="78" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>350</v>
       </c>
@@ -15587,7 +15683,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>351</v>
       </c>
@@ -15761,7 +15857,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="80" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>361</v>
       </c>
@@ -15938,7 +16034,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>365</v>
       </c>
@@ -16115,7 +16211,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>369</v>
       </c>
@@ -16292,7 +16388,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>373</v>
       </c>
@@ -16469,7 +16565,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="84" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>374</v>
       </c>
@@ -16646,7 +16742,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="85" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>375</v>
       </c>
@@ -16823,7 +16919,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>377</v>
       </c>
@@ -17000,7 +17096,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="87" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>378</v>
       </c>
@@ -17177,7 +17273,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>379</v>
       </c>
@@ -17354,7 +17450,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="89" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>380</v>
       </c>
@@ -17531,7 +17627,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="90" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>381</v>
       </c>
@@ -17708,7 +17804,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="91" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>382</v>
       </c>
@@ -17885,7 +17981,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="92" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
         <v>383</v>
       </c>
@@ -18062,7 +18158,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="93" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>384</v>
       </c>
@@ -18239,7 +18335,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
         <v>392</v>
       </c>
@@ -18416,7 +18512,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="95" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>402</v>
       </c>
@@ -18593,7 +18689,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="96" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
         <v>402</v>
       </c>
@@ -18770,7 +18866,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="97" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>403</v>
       </c>
@@ -18947,7 +19043,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="98" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>412</v>
       </c>
@@ -19124,7 +19220,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="99" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>413</v>
       </c>
@@ -19301,7 +19397,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="100" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
         <v>429</v>
       </c>
@@ -19481,7 +19577,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>432</v>
       </c>
@@ -19661,7 +19757,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
         <v>433</v>
       </c>
@@ -19841,7 +19937,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="103" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>434</v>
       </c>
@@ -20023,7 +20119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
         <v>435</v>
       </c>
@@ -20205,7 +20301,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="105" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
         <v>436</v>
       </c>
@@ -20387,7 +20483,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="106" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
         <v>431</v>
       </c>
@@ -20569,7 +20665,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="107" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>456</v>
       </c>
@@ -20748,7 +20844,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
         <v>460</v>
       </c>
@@ -20930,7 +21026,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:58" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:58" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>466</v>
       </c>
@@ -21109,7 +21205,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="110" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
         <v>470</v>
       </c>
@@ -21291,7 +21387,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="111" spans="1:58" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:58" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="40" t="s">
         <v>472</v>
       </c>
@@ -21473,7 +21569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:58" s="48" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:58" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="47" t="s">
         <v>476</v>
       </c>
@@ -21652,7 +21748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
         <v>484</v>
       </c>
@@ -21836,7 +21932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
         <v>485</v>
       </c>
@@ -21962,7 +22058,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
         <v>493</v>
       </c>
@@ -22088,7 +22184,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
         <v>494</v>
       </c>
@@ -22216,7 +22312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>505</v>
       </c>
@@ -22344,7 +22440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
         <v>504</v>
       </c>
@@ -22472,7 +22568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>502</v>
       </c>
@@ -22600,7 +22696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
         <v>507</v>
       </c>
@@ -22750,7 +22846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>508</v>
       </c>
@@ -22900,7 +22996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
         <v>520</v>
       </c>
@@ -23031,7 +23127,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
         <v>521</v>
       </c>
@@ -23162,7 +23258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
         <v>522</v>
       </c>
@@ -23293,7 +23389,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>523</v>
       </c>
@@ -23424,7 +23520,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
         <v>533</v>
       </c>
@@ -23569,7 +23665,7 @@
       </c>
       <c r="BF126" s="2"/>
     </row>
-    <row r="127" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
         <v>534</v>
       </c>
@@ -23717,7 +23813,7 @@
       </c>
       <c r="BF127" s="2"/>
     </row>
-    <row r="128" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
         <v>535</v>
       </c>
@@ -23865,7 +23961,7 @@
       </c>
       <c r="BF128" s="2"/>
     </row>
-    <row r="129" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
         <v>536</v>
       </c>
@@ -24013,7 +24109,7 @@
       </c>
       <c r="BF129" s="2"/>
     </row>
-    <row r="130" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="17" t="s">
         <v>538</v>
       </c>
@@ -24160,7 +24256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
         <v>545</v>
       </c>
@@ -24304,7 +24400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
         <v>546</v>
       </c>
@@ -24448,7 +24544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
         <v>547</v>
       </c>
@@ -24592,7 +24688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
         <v>548</v>
       </c>
@@ -24736,7 +24832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
         <v>549</v>
       </c>
@@ -24880,7 +24976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
         <v>550</v>
       </c>
@@ -25024,7 +25120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
         <v>551</v>
       </c>
@@ -25168,7 +25264,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="138" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
         <v>552</v>
       </c>
@@ -25312,7 +25408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
         <v>553</v>
       </c>
@@ -25455,165 +25551,168 @@
         <v>117</v>
       </c>
     </row>
-    <row r="140" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>574</v>
       </c>
-      <c r="B140" s="12" t="s">
+      <c r="B140" s="17" t="s">
         <v>575</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="F140" s="64" t="s">
+      <c r="F140" s="65" t="s">
         <v>577</v>
       </c>
-      <c r="G140" s="12" t="s">
+      <c r="G140" s="17" t="s">
         <v>578</v>
       </c>
-      <c r="H140" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I140" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="J140" t="s">
-        <v>117</v>
-      </c>
-      <c r="L140" t="s">
-        <v>117</v>
-      </c>
-      <c r="T140" s="12"/>
-      <c r="U140" s="20" t="s">
+      <c r="H140" s="17" t="s">
+        <v>572</v>
+      </c>
+      <c r="I140" s="7">
+        <v>0</v>
+      </c>
+      <c r="J140" s="4">
+        <v>1</v>
+      </c>
+      <c r="K140" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="L140" s="4">
+        <v>0</v>
+      </c>
+      <c r="T140" s="17"/>
+      <c r="U140" s="22">
+        <v>0</v>
+      </c>
+      <c r="V140" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="V140" t="s">
-        <v>580</v>
-      </c>
-      <c r="W140">
+      <c r="W140" s="4">
         <v>6</v>
       </c>
-      <c r="X140" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y140">
+      <c r="X140" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y140" s="4">
         <v>3</v>
       </c>
-      <c r="Z140">
+      <c r="Z140" s="4">
         <v>2</v>
       </c>
-      <c r="AA140">
+      <c r="AA140" s="4">
         <f t="shared" si="217"/>
         <v>5</v>
       </c>
-      <c r="AB140">
+      <c r="AB140" s="4">
         <v>2</v>
       </c>
-      <c r="AC140">
-        <v>1</v>
-      </c>
-      <c r="AE140" t="s">
+      <c r="AC140" s="4">
+        <v>1</v>
+      </c>
+      <c r="AE140" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="AH140" t="s">
+      <c r="AH140" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AI140" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ140" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK140" t="e">
+      <c r="AI140" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ140" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK140" s="4" t="e">
         <f>AI140+AJ140</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AL140">
+      <c r="AL140" s="4">
         <f t="shared" si="253"/>
         <v>61574.894649960152</v>
       </c>
-      <c r="AM140" s="10" t="s">
+      <c r="AM140" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="AN140">
+      <c r="AN140" s="4">
         <v>173</v>
       </c>
-      <c r="AO140">
+      <c r="AO140" s="4">
         <v>743</v>
       </c>
-      <c r="AP140" s="20">
+      <c r="AP140" s="22">
         <v>435</v>
       </c>
-      <c r="AQ140">
+      <c r="AQ140" s="4">
         <v>144</v>
       </c>
-      <c r="AR140">
+      <c r="AR140" s="4">
         <v>512</v>
       </c>
-      <c r="AS140">
+      <c r="AS140" s="4">
         <v>384</v>
       </c>
-      <c r="AT140" s="25" t="s">
+      <c r="AT140" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="AU140">
+      <c r="AU140" s="4">
         <f t="shared" ref="AU140" si="254" xml:space="preserve"> _xlfn.FLOOR.MATH((AN140 - AQ140) / 2)</f>
         <v>14</v>
       </c>
-      <c r="AV140">
+      <c r="AV140" s="4">
         <f t="shared" ref="AV140" si="255" xml:space="preserve"> _xlfn.FLOOR.MATH((AO140 - AR140) / 2)</f>
         <v>115</v>
       </c>
-      <c r="AW140">
+      <c r="AW140" s="4">
         <f t="shared" ref="AW140" si="256" xml:space="preserve"> _xlfn.FLOOR.MATH((AP140 - AS140) / 2)</f>
         <v>25</v>
       </c>
-      <c r="AX140" s="25" t="s">
+      <c r="AX140" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="AY140">
+      <c r="AY140" s="4">
         <f t="shared" ref="AY140" si="257">AQ140-AU140</f>
         <v>130</v>
       </c>
-      <c r="AZ140">
+      <c r="AZ140" s="4">
         <f t="shared" ref="AZ140" si="258">AR140-AV140</f>
         <v>397</v>
       </c>
-      <c r="BA140" s="10">
+      <c r="BA140" s="29">
         <f t="shared" ref="BA140" si="259">AS140-AW140</f>
         <v>359</v>
       </c>
-      <c r="BB140" t="s">
+      <c r="BB140" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="BC140" t="s">
+      <c r="BC140" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="BD140" t="s">
+      <c r="BD140" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="141" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A141" s="71" t="s">
-        <v>583</v>
+    <row r="141" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A141" s="12" t="s">
+        <v>582</v>
       </c>
       <c r="B141" s="70" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C141" t="s">
         <v>477</v>
       </c>
       <c r="D141" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E141" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F141" s="64" t="s">
         <v>117</v>
@@ -25739,21 +25838,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="142" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A142" s="71" t="s">
-        <v>584</v>
+    <row r="142" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A142" s="12" t="s">
+        <v>583</v>
       </c>
       <c r="B142" s="12" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C142" t="s">
         <v>477</v>
       </c>
       <c r="D142" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E142" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F142" s="64" t="s">
         <v>117</v>
@@ -25879,21 +25978,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="143" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A143" s="71" t="s">
-        <v>585</v>
+    <row r="143" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A143" s="12" t="s">
+        <v>584</v>
       </c>
       <c r="B143" s="12" t="s">
-        <v>117</v>
+        <v>606</v>
       </c>
       <c r="C143" t="s">
         <v>477</v>
       </c>
       <c r="D143" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E143" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F143" s="64" t="s">
         <v>117</v>
@@ -26019,21 +26118,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="144" spans="1:58" x14ac:dyDescent="0.3">
-      <c r="A144" s="71" t="s">
-        <v>586</v>
+    <row r="144" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A144" s="12" t="s">
+        <v>585</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>117</v>
+        <v>607</v>
       </c>
       <c r="C144" t="s">
         <v>477</v>
       </c>
       <c r="D144" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E144" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F144" s="64" t="s">
         <v>117</v>
@@ -26159,21 +26258,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A145" s="71" t="s">
-        <v>587</v>
+    <row r="145" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A145" s="12" t="s">
+        <v>586</v>
       </c>
       <c r="B145" s="12" t="s">
-        <v>117</v>
+        <v>608</v>
       </c>
       <c r="C145" t="s">
         <v>477</v>
       </c>
       <c r="D145" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E145" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F145" s="64" t="s">
         <v>117</v>
@@ -26299,21 +26398,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="146" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A146" s="71" t="s">
-        <v>588</v>
+    <row r="146" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A146" s="12" t="s">
+        <v>587</v>
       </c>
       <c r="B146" s="12" t="s">
-        <v>117</v>
+        <v>609</v>
       </c>
       <c r="C146" t="s">
         <v>477</v>
       </c>
       <c r="D146" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E146" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F146" s="64" t="s">
         <v>117</v>
@@ -26439,21 +26538,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="147" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A147" s="71" t="s">
-        <v>589</v>
+    <row r="147" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A147" s="12" t="s">
+        <v>588</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>117</v>
+        <v>610</v>
       </c>
       <c r="C147" t="s">
         <v>477</v>
       </c>
       <c r="D147" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E147" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F147" s="64" t="s">
         <v>117</v>
@@ -26579,21 +26678,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="148" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A148" s="71" t="s">
-        <v>590</v>
+    <row r="148" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A148" s="12" t="s">
+        <v>589</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>117</v>
+        <v>611</v>
       </c>
       <c r="C148" t="s">
         <v>477</v>
       </c>
       <c r="D148" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E148" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F148" s="64" t="s">
         <v>117</v>
@@ -26719,21 +26818,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="149" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A149" s="71" t="s">
-        <v>591</v>
+    <row r="149" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A149" s="12" t="s">
+        <v>590</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>117</v>
+        <v>612</v>
       </c>
       <c r="C149" t="s">
         <v>477</v>
       </c>
       <c r="D149" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E149" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F149" s="64" t="s">
         <v>117</v>
@@ -26859,21 +26958,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="150" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A150" s="71" t="s">
-        <v>592</v>
+    <row r="150" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A150" s="12" t="s">
+        <v>591</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>117</v>
+        <v>613</v>
       </c>
       <c r="C150" t="s">
         <v>477</v>
       </c>
       <c r="D150" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E150" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F150" s="64" t="s">
         <v>117</v>
@@ -26999,21 +27098,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="151" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A151" s="71" t="s">
-        <v>593</v>
-      </c>
-      <c r="B151" s="12" t="s">
-        <v>117</v>
+    <row r="151" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A151" s="12" t="s">
+        <v>592</v>
+      </c>
+      <c r="B151" s="70" t="s">
+        <v>614</v>
       </c>
       <c r="C151" t="s">
         <v>477</v>
       </c>
       <c r="D151" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E151" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F151" s="64" t="s">
         <v>117</v>
@@ -27139,21 +27238,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="152" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A152" s="71" t="s">
-        <v>594</v>
+    <row r="152" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A152" s="12" t="s">
+        <v>593</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>117</v>
+        <v>615</v>
       </c>
       <c r="C152" t="s">
-        <v>117</v>
+        <v>477</v>
       </c>
       <c r="D152" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E152" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F152" s="64" t="s">
         <v>117</v>
@@ -27214,11 +27313,11 @@
         <v>117</v>
       </c>
       <c r="AK152" t="e">
-        <f t="shared" si="264"/>
+        <f t="shared" ref="AK152:AK164" si="269">AI152+AJ152</f>
         <v>#VALUE!</v>
       </c>
       <c r="AL152" t="e">
-        <f t="shared" si="265"/>
+        <f t="shared" ref="AL152:AL164" si="270" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ152*AR152*AS152) * (AA152 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
       <c r="AM152" s="10" t="s">
@@ -27258,15 +27357,15 @@
         <v>8</v>
       </c>
       <c r="AY152" t="e">
-        <f t="shared" si="266"/>
+        <f t="shared" ref="AY152:AY164" si="271">AQ152-AU152</f>
         <v>#VALUE!</v>
       </c>
       <c r="AZ152" t="e">
-        <f t="shared" si="267"/>
+        <f t="shared" ref="AZ152:AZ164" si="272">AR152-AV152</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA152" s="10" t="e">
-        <f t="shared" si="268"/>
+        <f t="shared" ref="BA152:BA164" si="273">AS152-AW152</f>
         <v>#VALUE!</v>
       </c>
       <c r="BB152" t="s">
@@ -27279,21 +27378,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="153" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
-        <v>117</v>
+        <v>594</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>117</v>
+        <v>616</v>
       </c>
       <c r="C153" t="s">
-        <v>117</v>
+        <v>477</v>
       </c>
       <c r="D153" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E153" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F153" s="64" t="s">
         <v>117</v>
@@ -27354,11 +27453,11 @@
         <v>117</v>
       </c>
       <c r="AK153" t="e">
-        <f t="shared" ref="AK153" si="269">AI153+AJ153</f>
+        <f t="shared" si="269"/>
         <v>#VALUE!</v>
       </c>
       <c r="AL153" t="e">
-        <f t="shared" ref="AL153" si="270" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ153*AR153*AS153) * (AA153 / 5) + 441</f>
+        <f t="shared" si="270"/>
         <v>#VALUE!</v>
       </c>
       <c r="AM153" s="10" t="s">
@@ -27398,15 +27497,15 @@
         <v>8</v>
       </c>
       <c r="AY153" t="e">
-        <f t="shared" ref="AY153" si="271">AQ153-AU153</f>
+        <f t="shared" si="271"/>
         <v>#VALUE!</v>
       </c>
       <c r="AZ153" t="e">
-        <f t="shared" ref="AZ153" si="272">AR153-AV153</f>
+        <f t="shared" si="272"/>
         <v>#VALUE!</v>
       </c>
       <c r="BA153" s="10" t="e">
-        <f t="shared" ref="BA153" si="273">AS153-AW153</f>
+        <f t="shared" si="273"/>
         <v>#VALUE!</v>
       </c>
       <c r="BB153" t="s">
@@ -27416,6 +27515,1686 @@
         <v>117</v>
       </c>
       <c r="BD153" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="154" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A154" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="B154" s="12" t="s">
+        <v>617</v>
+      </c>
+      <c r="C154" t="s">
+        <v>477</v>
+      </c>
+      <c r="D154" t="s">
+        <v>406</v>
+      </c>
+      <c r="E154" t="s">
+        <v>409</v>
+      </c>
+      <c r="F154" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G154" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H154" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I154" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J154" t="s">
+        <v>117</v>
+      </c>
+      <c r="L154" t="s">
+        <v>117</v>
+      </c>
+      <c r="T154" s="12"/>
+      <c r="U154" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V154" t="s">
+        <v>117</v>
+      </c>
+      <c r="W154" t="s">
+        <v>117</v>
+      </c>
+      <c r="X154" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y154" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI154" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ154" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK154" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL154" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM154" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP154" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT154" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW154" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX154" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY154" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ154" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA154" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB154" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC154" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD154" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="155" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A155" s="12" t="s">
+        <v>596</v>
+      </c>
+      <c r="B155" s="12" t="s">
+        <v>618</v>
+      </c>
+      <c r="C155" t="s">
+        <v>477</v>
+      </c>
+      <c r="D155" t="s">
+        <v>406</v>
+      </c>
+      <c r="E155" t="s">
+        <v>409</v>
+      </c>
+      <c r="F155" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G155" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H155" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I155" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J155" t="s">
+        <v>117</v>
+      </c>
+      <c r="L155" t="s">
+        <v>117</v>
+      </c>
+      <c r="T155" s="12"/>
+      <c r="U155" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V155" t="s">
+        <v>117</v>
+      </c>
+      <c r="W155" t="s">
+        <v>117</v>
+      </c>
+      <c r="X155" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y155" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI155" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ155" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK155" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL155" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM155" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP155" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT155" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW155" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX155" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY155" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ155" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA155" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB155" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC155" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD155" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="156" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A156" s="12" t="s">
+        <v>597</v>
+      </c>
+      <c r="B156" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="C156" t="s">
+        <v>477</v>
+      </c>
+      <c r="D156" t="s">
+        <v>406</v>
+      </c>
+      <c r="E156" t="s">
+        <v>409</v>
+      </c>
+      <c r="F156" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G156" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H156" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I156" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J156" t="s">
+        <v>117</v>
+      </c>
+      <c r="L156" t="s">
+        <v>117</v>
+      </c>
+      <c r="T156" s="12"/>
+      <c r="U156" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V156" t="s">
+        <v>117</v>
+      </c>
+      <c r="W156" t="s">
+        <v>117</v>
+      </c>
+      <c r="X156" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y156" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI156" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ156" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK156" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL156" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM156" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP156" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT156" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW156" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX156" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY156" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ156" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA156" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB156" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC156" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD156" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="157" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A157" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="B157" s="12" t="s">
+        <v>620</v>
+      </c>
+      <c r="C157" t="s">
+        <v>477</v>
+      </c>
+      <c r="D157" t="s">
+        <v>406</v>
+      </c>
+      <c r="E157" t="s">
+        <v>409</v>
+      </c>
+      <c r="F157" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G157" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H157" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I157" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J157" t="s">
+        <v>117</v>
+      </c>
+      <c r="L157" t="s">
+        <v>117</v>
+      </c>
+      <c r="T157" s="12"/>
+      <c r="U157" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V157" t="s">
+        <v>117</v>
+      </c>
+      <c r="W157" t="s">
+        <v>117</v>
+      </c>
+      <c r="X157" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y157" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI157" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ157" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK157" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL157" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM157" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP157" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT157" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW157" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX157" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY157" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ157" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA157" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB157" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC157" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD157" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="158" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A158" s="12" t="s">
+        <v>599</v>
+      </c>
+      <c r="B158" s="12" t="s">
+        <v>621</v>
+      </c>
+      <c r="C158" t="s">
+        <v>477</v>
+      </c>
+      <c r="D158" t="s">
+        <v>406</v>
+      </c>
+      <c r="E158" t="s">
+        <v>409</v>
+      </c>
+      <c r="F158" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G158" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H158" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I158" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J158" t="s">
+        <v>117</v>
+      </c>
+      <c r="L158" t="s">
+        <v>117</v>
+      </c>
+      <c r="T158" s="12"/>
+      <c r="U158" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V158" t="s">
+        <v>117</v>
+      </c>
+      <c r="W158" t="s">
+        <v>117</v>
+      </c>
+      <c r="X158" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y158" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI158" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ158" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK158" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL158" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM158" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP158" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT158" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX158" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY158" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ158" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA158" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB158" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC158" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD158" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="159" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A159" s="12" t="s">
+        <v>600</v>
+      </c>
+      <c r="B159" s="12" t="s">
+        <v>622</v>
+      </c>
+      <c r="C159" t="s">
+        <v>477</v>
+      </c>
+      <c r="D159" t="s">
+        <v>406</v>
+      </c>
+      <c r="E159" t="s">
+        <v>409</v>
+      </c>
+      <c r="F159" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G159" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H159" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I159" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J159" t="s">
+        <v>117</v>
+      </c>
+      <c r="L159" t="s">
+        <v>117</v>
+      </c>
+      <c r="T159" s="12"/>
+      <c r="U159" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V159" t="s">
+        <v>117</v>
+      </c>
+      <c r="W159" t="s">
+        <v>117</v>
+      </c>
+      <c r="X159" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y159" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI159" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ159" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK159" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL159" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM159" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP159" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT159" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX159" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY159" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ159" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA159" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB159" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC159" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD159" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="160" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A160" s="12" t="s">
+        <v>601</v>
+      </c>
+      <c r="B160" s="12" t="s">
+        <v>623</v>
+      </c>
+      <c r="C160" t="s">
+        <v>477</v>
+      </c>
+      <c r="D160" t="s">
+        <v>406</v>
+      </c>
+      <c r="E160" t="s">
+        <v>409</v>
+      </c>
+      <c r="F160" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G160" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H160" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I160" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J160" t="s">
+        <v>117</v>
+      </c>
+      <c r="L160" t="s">
+        <v>117</v>
+      </c>
+      <c r="T160" s="12"/>
+      <c r="U160" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V160" t="s">
+        <v>117</v>
+      </c>
+      <c r="W160" t="s">
+        <v>117</v>
+      </c>
+      <c r="X160" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y160" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI160" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ160" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK160" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL160" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM160" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP160" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT160" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX160" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY160" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ160" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA160" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB160" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC160" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD160" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="161" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A161" s="12" t="s">
+        <v>602</v>
+      </c>
+      <c r="B161" s="12" t="s">
+        <v>624</v>
+      </c>
+      <c r="C161" t="s">
+        <v>477</v>
+      </c>
+      <c r="D161" t="s">
+        <v>406</v>
+      </c>
+      <c r="E161" t="s">
+        <v>409</v>
+      </c>
+      <c r="F161" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G161" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H161" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I161" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J161" t="s">
+        <v>117</v>
+      </c>
+      <c r="L161" t="s">
+        <v>117</v>
+      </c>
+      <c r="T161" s="12"/>
+      <c r="U161" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V161" t="s">
+        <v>117</v>
+      </c>
+      <c r="W161" t="s">
+        <v>117</v>
+      </c>
+      <c r="X161" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y161" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI161" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ161" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK161" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL161" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM161" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP161" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT161" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX161" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY161" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ161" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA161" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB161" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC161" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD161" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="162" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A162" s="12" t="s">
+        <v>603</v>
+      </c>
+      <c r="B162" s="12" t="s">
+        <v>625</v>
+      </c>
+      <c r="C162" t="s">
+        <v>477</v>
+      </c>
+      <c r="D162" t="s">
+        <v>406</v>
+      </c>
+      <c r="E162" t="s">
+        <v>409</v>
+      </c>
+      <c r="F162" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G162" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H162" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I162" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J162" t="s">
+        <v>117</v>
+      </c>
+      <c r="L162" t="s">
+        <v>117</v>
+      </c>
+      <c r="T162" s="12"/>
+      <c r="U162" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V162" t="s">
+        <v>117</v>
+      </c>
+      <c r="W162" t="s">
+        <v>117</v>
+      </c>
+      <c r="X162" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y162" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI162" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ162" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK162" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL162" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM162" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP162" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT162" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX162" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY162" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ162" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA162" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB162" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC162" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD162" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="163" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A163" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="B163" s="12" t="s">
+        <v>626</v>
+      </c>
+      <c r="C163" t="s">
+        <v>477</v>
+      </c>
+      <c r="D163" t="s">
+        <v>406</v>
+      </c>
+      <c r="E163" t="s">
+        <v>409</v>
+      </c>
+      <c r="F163" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G163" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H163" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I163" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J163" t="s">
+        <v>117</v>
+      </c>
+      <c r="L163" t="s">
+        <v>117</v>
+      </c>
+      <c r="T163" s="12"/>
+      <c r="U163" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V163" t="s">
+        <v>117</v>
+      </c>
+      <c r="W163" t="s">
+        <v>117</v>
+      </c>
+      <c r="X163" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y163" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI163" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ163" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK163" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL163" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM163" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP163" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT163" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW163" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX163" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY163" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ163" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA163" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB163" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC163" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD163" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="164" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A164" s="12" t="s">
+        <v>605</v>
+      </c>
+      <c r="B164" s="12" t="s">
+        <v>627</v>
+      </c>
+      <c r="C164" t="s">
+        <v>477</v>
+      </c>
+      <c r="D164" t="s">
+        <v>406</v>
+      </c>
+      <c r="E164" t="s">
+        <v>409</v>
+      </c>
+      <c r="F164" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G164" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H164" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I164" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J164" t="s">
+        <v>117</v>
+      </c>
+      <c r="L164" t="s">
+        <v>117</v>
+      </c>
+      <c r="T164" s="12"/>
+      <c r="U164" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V164" t="s">
+        <v>117</v>
+      </c>
+      <c r="W164" t="s">
+        <v>117</v>
+      </c>
+      <c r="X164" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y164" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI164" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ164" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK164" t="e">
+        <f t="shared" si="269"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL164" t="e">
+        <f t="shared" si="270"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM164" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP164" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT164" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW164" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX164" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY164" t="e">
+        <f t="shared" si="271"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ164" t="e">
+        <f t="shared" si="272"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA164" s="10" t="e">
+        <f t="shared" si="273"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB164" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC164" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD164" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="165" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A165" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B165" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C165" t="s">
+        <v>117</v>
+      </c>
+      <c r="D165" t="s">
+        <v>117</v>
+      </c>
+      <c r="E165" t="s">
+        <v>117</v>
+      </c>
+      <c r="F165" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G165" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H165" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I165" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J165" t="s">
+        <v>117</v>
+      </c>
+      <c r="L165" t="s">
+        <v>117</v>
+      </c>
+      <c r="T165" s="12"/>
+      <c r="U165" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V165" t="s">
+        <v>117</v>
+      </c>
+      <c r="W165" t="s">
+        <v>117</v>
+      </c>
+      <c r="X165" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y165" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI165" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ165" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK165" t="e">
+        <f t="shared" ref="AK154:AK165" si="274">AI165+AJ165</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL165" t="e">
+        <f t="shared" ref="AL154:AL165" si="275" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ165*AR165*AS165) * (AA165 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM165" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP165" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT165" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW165" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX165" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY165" t="e">
+        <f t="shared" ref="AY154:AY165" si="276">AQ165-AU165</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ165" t="e">
+        <f t="shared" ref="AZ154:AZ165" si="277">AR165-AV165</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA165" s="10" t="e">
+        <f t="shared" ref="BA154:BA165" si="278">AS165-AW165</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB165" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC165" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD165" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare predict3dunet 1.8.2 chpt-240131-0 to -7
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D83568C-7F8E-4E59-AAEC-989FAE6D7785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0647D92A-41CF-4A01-92CE-9AD2C8F8CAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-21720" yWindow="2550" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4964" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4940" uniqueCount="628">
   <si>
     <t>patch z</t>
   </si>
@@ -2786,10 +2786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BF165"/>
+  <dimension ref="A1:BG165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView tabSelected="1" topLeftCell="AH115" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BD136" sqref="BD136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2806,8 +2806,8 @@
     <col min="11" max="11" width="30.7109375" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="9.42578125" customWidth="1" outlineLevel="1"/>
     <col min="13" max="13" width="33" customWidth="1"/>
-    <col min="14" max="20" width="9.140625" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="9.140625" style="20"/>
+    <col min="14" max="20" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="9.140625" style="20" collapsed="1"/>
     <col min="22" max="22" width="15.140625" customWidth="1" outlineLevel="1"/>
     <col min="23" max="23" width="9.140625" customWidth="1" outlineLevel="1"/>
     <col min="25" max="25" width="6.7109375" customWidth="1" outlineLevel="1"/>
@@ -2823,8 +2823,8 @@
     <col min="35" max="35" width="16.7109375" style="6" customWidth="1"/>
     <col min="36" max="37" width="14.85546875" customWidth="1"/>
     <col min="38" max="38" width="21" customWidth="1"/>
-    <col min="39" max="39" width="26.28515625" style="10" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="10.7109375" customWidth="1"/>
+    <col min="39" max="39" width="26.28515625" style="10" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="10.7109375" customWidth="1" collapsed="1"/>
     <col min="41" max="41" width="10.5703125" customWidth="1"/>
     <col min="42" max="42" width="10.85546875" style="20" customWidth="1"/>
     <col min="43" max="43" width="5.28515625" customWidth="1"/>
@@ -2837,12 +2837,12 @@
     <col min="50" max="50" width="6" style="20" customWidth="1"/>
     <col min="51" max="52" width="6" customWidth="1"/>
     <col min="53" max="53" width="6" style="10" customWidth="1"/>
-    <col min="54" max="54" width="74.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="76.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="5.140625" customWidth="1"/>
-    <col min="57" max="57" width="135.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="206" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="74.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="76.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="5.140625" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="135.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="206" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="59" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="60" max="60" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="12.7109375" customWidth="1"/>
@@ -25736,7 +25736,7 @@
       <c r="U141" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V141" t="s">
+      <c r="V141" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W141" t="s">
@@ -25757,8 +25757,8 @@
       <c r="AB141" t="s">
         <v>117</v>
       </c>
-      <c r="AC141" t="s">
-        <v>117</v>
+      <c r="AC141" s="3">
+        <v>3</v>
       </c>
       <c r="AE141" t="s">
         <v>117</v>
@@ -25876,7 +25876,7 @@
       <c r="U142" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V142" t="s">
+      <c r="V142" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W142" t="s">
@@ -25897,8 +25897,8 @@
       <c r="AB142" t="s">
         <v>117</v>
       </c>
-      <c r="AC142" t="s">
-        <v>117</v>
+      <c r="AC142" s="3">
+        <v>3</v>
       </c>
       <c r="AE142" t="s">
         <v>117</v>
@@ -26016,7 +26016,7 @@
       <c r="U143" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V143" t="s">
+      <c r="V143" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W143" t="s">
@@ -26037,8 +26037,8 @@
       <c r="AB143" t="s">
         <v>117</v>
       </c>
-      <c r="AC143" t="s">
-        <v>117</v>
+      <c r="AC143" s="3">
+        <v>3</v>
       </c>
       <c r="AE143" t="s">
         <v>117</v>
@@ -26156,7 +26156,7 @@
       <c r="U144" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V144" t="s">
+      <c r="V144" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W144" t="s">
@@ -26177,8 +26177,8 @@
       <c r="AB144" t="s">
         <v>117</v>
       </c>
-      <c r="AC144" t="s">
-        <v>117</v>
+      <c r="AC144" s="3">
+        <v>3</v>
       </c>
       <c r="AE144" t="s">
         <v>117</v>
@@ -26296,7 +26296,7 @@
       <c r="U145" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V145" t="s">
+      <c r="V145" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W145" t="s">
@@ -26317,8 +26317,8 @@
       <c r="AB145" t="s">
         <v>117</v>
       </c>
-      <c r="AC145" t="s">
-        <v>117</v>
+      <c r="AC145" s="3">
+        <v>3</v>
       </c>
       <c r="AE145" t="s">
         <v>117</v>
@@ -26436,7 +26436,7 @@
       <c r="U146" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V146" t="s">
+      <c r="V146" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W146" t="s">
@@ -26457,8 +26457,8 @@
       <c r="AB146" t="s">
         <v>117</v>
       </c>
-      <c r="AC146" t="s">
-        <v>117</v>
+      <c r="AC146" s="3">
+        <v>3</v>
       </c>
       <c r="AE146" t="s">
         <v>117</v>
@@ -26576,7 +26576,7 @@
       <c r="U147" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V147" t="s">
+      <c r="V147" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W147" t="s">
@@ -26597,8 +26597,8 @@
       <c r="AB147" t="s">
         <v>117</v>
       </c>
-      <c r="AC147" t="s">
-        <v>117</v>
+      <c r="AC147" s="3">
+        <v>3</v>
       </c>
       <c r="AE147" t="s">
         <v>117</v>
@@ -26716,7 +26716,7 @@
       <c r="U148" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V148" t="s">
+      <c r="V148" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W148" t="s">
@@ -26737,8 +26737,8 @@
       <c r="AB148" t="s">
         <v>117</v>
       </c>
-      <c r="AC148" t="s">
-        <v>117</v>
+      <c r="AC148" s="3">
+        <v>3</v>
       </c>
       <c r="AE148" t="s">
         <v>117</v>
@@ -26856,7 +26856,7 @@
       <c r="U149" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V149" t="s">
+      <c r="V149" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W149" t="s">
@@ -26877,8 +26877,8 @@
       <c r="AB149" t="s">
         <v>117</v>
       </c>
-      <c r="AC149" t="s">
-        <v>117</v>
+      <c r="AC149" s="3">
+        <v>3</v>
       </c>
       <c r="AE149" t="s">
         <v>117</v>
@@ -26996,7 +26996,7 @@
       <c r="U150" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V150" t="s">
+      <c r="V150" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W150" t="s">
@@ -27017,8 +27017,8 @@
       <c r="AB150" t="s">
         <v>117</v>
       </c>
-      <c r="AC150" t="s">
-        <v>117</v>
+      <c r="AC150" s="3">
+        <v>3</v>
       </c>
       <c r="AE150" t="s">
         <v>117</v>
@@ -27136,7 +27136,7 @@
       <c r="U151" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V151" t="s">
+      <c r="V151" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W151" t="s">
@@ -27157,8 +27157,8 @@
       <c r="AB151" t="s">
         <v>117</v>
       </c>
-      <c r="AC151" t="s">
-        <v>117</v>
+      <c r="AC151" s="3">
+        <v>3</v>
       </c>
       <c r="AE151" t="s">
         <v>117</v>
@@ -27276,7 +27276,7 @@
       <c r="U152" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V152" t="s">
+      <c r="V152" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W152" t="s">
@@ -27297,8 +27297,8 @@
       <c r="AB152" t="s">
         <v>117</v>
       </c>
-      <c r="AC152" t="s">
-        <v>117</v>
+      <c r="AC152" s="3">
+        <v>3</v>
       </c>
       <c r="AE152" t="s">
         <v>117</v>
@@ -27416,7 +27416,7 @@
       <c r="U153" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V153" t="s">
+      <c r="V153" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W153" t="s">
@@ -27437,8 +27437,8 @@
       <c r="AB153" t="s">
         <v>117</v>
       </c>
-      <c r="AC153" t="s">
-        <v>117</v>
+      <c r="AC153" s="3">
+        <v>3</v>
       </c>
       <c r="AE153" t="s">
         <v>117</v>
@@ -27556,7 +27556,7 @@
       <c r="U154" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V154" t="s">
+      <c r="V154" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W154" t="s">
@@ -27577,8 +27577,8 @@
       <c r="AB154" t="s">
         <v>117</v>
       </c>
-      <c r="AC154" t="s">
-        <v>117</v>
+      <c r="AC154" s="3">
+        <v>3</v>
       </c>
       <c r="AE154" t="s">
         <v>117</v>
@@ -27696,7 +27696,7 @@
       <c r="U155" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V155" t="s">
+      <c r="V155" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W155" t="s">
@@ -27717,8 +27717,8 @@
       <c r="AB155" t="s">
         <v>117</v>
       </c>
-      <c r="AC155" t="s">
-        <v>117</v>
+      <c r="AC155" s="3">
+        <v>3</v>
       </c>
       <c r="AE155" t="s">
         <v>117</v>
@@ -27836,7 +27836,7 @@
       <c r="U156" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V156" t="s">
+      <c r="V156" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W156" t="s">
@@ -27857,8 +27857,8 @@
       <c r="AB156" t="s">
         <v>117</v>
       </c>
-      <c r="AC156" t="s">
-        <v>117</v>
+      <c r="AC156" s="3">
+        <v>3</v>
       </c>
       <c r="AE156" t="s">
         <v>117</v>
@@ -27976,7 +27976,7 @@
       <c r="U157" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V157" t="s">
+      <c r="V157" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W157" t="s">
@@ -27997,8 +27997,8 @@
       <c r="AB157" t="s">
         <v>117</v>
       </c>
-      <c r="AC157" t="s">
-        <v>117</v>
+      <c r="AC157" s="3">
+        <v>3</v>
       </c>
       <c r="AE157" t="s">
         <v>117</v>
@@ -28116,7 +28116,7 @@
       <c r="U158" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V158" t="s">
+      <c r="V158" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W158" t="s">
@@ -28137,8 +28137,8 @@
       <c r="AB158" t="s">
         <v>117</v>
       </c>
-      <c r="AC158" t="s">
-        <v>117</v>
+      <c r="AC158" s="3">
+        <v>3</v>
       </c>
       <c r="AE158" t="s">
         <v>117</v>
@@ -28256,7 +28256,7 @@
       <c r="U159" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V159" t="s">
+      <c r="V159" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W159" t="s">
@@ -28277,8 +28277,8 @@
       <c r="AB159" t="s">
         <v>117</v>
       </c>
-      <c r="AC159" t="s">
-        <v>117</v>
+      <c r="AC159" s="3">
+        <v>3</v>
       </c>
       <c r="AE159" t="s">
         <v>117</v>
@@ -28396,7 +28396,7 @@
       <c r="U160" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V160" t="s">
+      <c r="V160" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W160" t="s">
@@ -28417,8 +28417,8 @@
       <c r="AB160" t="s">
         <v>117</v>
       </c>
-      <c r="AC160" t="s">
-        <v>117</v>
+      <c r="AC160" s="3">
+        <v>3</v>
       </c>
       <c r="AE160" t="s">
         <v>117</v>
@@ -28536,7 +28536,7 @@
       <c r="U161" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V161" t="s">
+      <c r="V161" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W161" t="s">
@@ -28557,8 +28557,8 @@
       <c r="AB161" t="s">
         <v>117</v>
       </c>
-      <c r="AC161" t="s">
-        <v>117</v>
+      <c r="AC161" s="3">
+        <v>3</v>
       </c>
       <c r="AE161" t="s">
         <v>117</v>
@@ -28676,7 +28676,7 @@
       <c r="U162" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V162" t="s">
+      <c r="V162" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W162" t="s">
@@ -28697,8 +28697,8 @@
       <c r="AB162" t="s">
         <v>117</v>
       </c>
-      <c r="AC162" t="s">
-        <v>117</v>
+      <c r="AC162" s="3">
+        <v>3</v>
       </c>
       <c r="AE162" t="s">
         <v>117</v>
@@ -28816,7 +28816,7 @@
       <c r="U163" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V163" t="s">
+      <c r="V163" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W163" t="s">
@@ -28837,8 +28837,8 @@
       <c r="AB163" t="s">
         <v>117</v>
       </c>
-      <c r="AC163" t="s">
-        <v>117</v>
+      <c r="AC163" s="3">
+        <v>3</v>
       </c>
       <c r="AE163" t="s">
         <v>117</v>
@@ -28956,7 +28956,7 @@
       <c r="U164" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="V164" t="s">
+      <c r="V164" s="3" t="s">
         <v>117</v>
       </c>
       <c r="W164" t="s">
@@ -28977,8 +28977,8 @@
       <c r="AB164" t="s">
         <v>117</v>
       </c>
-      <c r="AC164" t="s">
-        <v>117</v>
+      <c r="AC164" s="3">
+        <v>3</v>
       </c>
       <c r="AE164" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
prepare train3dunet 1.8.2 chpt-240131-8 to -10
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0647D92A-41CF-4A01-92CE-9AD2C8F8CAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA6C99E-8D78-44F5-A26F-9540DB7E4308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2550" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4940" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5004" uniqueCount="630">
   <si>
     <t>patch z</t>
   </si>
@@ -2008,6 +2008,12 @@
   </si>
   <si>
     <t>240125-7 last</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Adapt patch shape for eyes to be in the patch for sure (y shape critical)</t>
   </si>
 </sst>
 </file>
@@ -2360,7 +2366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2469,9 +2475,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2786,10 +2791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG165"/>
+  <dimension ref="A1:BG169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH115" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BD136" sqref="BD136"/>
+    <sheetView tabSelected="1" topLeftCell="E136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H167" sqref="H167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -25702,7 +25707,7 @@
       <c r="A141" s="12" t="s">
         <v>582</v>
       </c>
-      <c r="B141" s="70" t="s">
+      <c r="B141" s="12" t="s">
         <v>580</v>
       </c>
       <c r="C141" t="s">
@@ -25913,11 +25918,11 @@
         <v>117</v>
       </c>
       <c r="AK142" t="e">
-        <f t="shared" ref="AK142:AK152" si="264">AI142+AJ142</f>
+        <f t="shared" ref="AK142:AK151" si="264">AI142+AJ142</f>
         <v>#VALUE!</v>
       </c>
       <c r="AL142" t="e">
-        <f t="shared" ref="AL142:AL152" si="265" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ142*AR142*AS142) * (AA142 / 5) + 441</f>
+        <f t="shared" ref="AL142:AL151" si="265" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ142*AR142*AS142) * (AA142 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
       <c r="AM142" s="10" t="s">
@@ -25957,15 +25962,15 @@
         <v>8</v>
       </c>
       <c r="AY142" t="e">
-        <f t="shared" ref="AY142:AY152" si="266">AQ142-AU142</f>
+        <f t="shared" ref="AY142:AY151" si="266">AQ142-AU142</f>
         <v>#VALUE!</v>
       </c>
       <c r="AZ142" t="e">
-        <f t="shared" ref="AZ142:AZ152" si="267">AR142-AV142</f>
+        <f t="shared" ref="AZ142:AZ151" si="267">AR142-AV142</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA142" s="10" t="e">
-        <f t="shared" ref="BA142:BA152" si="268">AS142-AW142</f>
+        <f t="shared" ref="BA142:BA151" si="268">AS142-AW142</f>
         <v>#VALUE!</v>
       </c>
       <c r="BB142" t="s">
@@ -27102,7 +27107,7 @@
       <c r="A151" s="12" t="s">
         <v>592</v>
       </c>
-      <c r="B151" s="70" t="s">
+      <c r="B151" s="12" t="s">
         <v>614</v>
       </c>
       <c r="C151" t="s">
@@ -27317,7 +27322,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AL152" t="e">
-        <f t="shared" ref="AL152:AL164" si="270" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ152*AR152*AS152) * (AA152 / 5) + 441</f>
+        <f t="shared" ref="AL152:AL166" si="270" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ152*AR152*AS152) * (AA152 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
       <c r="AM152" s="10" t="s">
@@ -27357,15 +27362,15 @@
         <v>8</v>
       </c>
       <c r="AY152" t="e">
-        <f t="shared" ref="AY152:AY164" si="271">AQ152-AU152</f>
+        <f t="shared" ref="AY152:AY166" si="271">AQ152-AU152</f>
         <v>#VALUE!</v>
       </c>
       <c r="AZ152" t="e">
-        <f t="shared" ref="AZ152:AZ164" si="272">AR152-AV152</f>
+        <f t="shared" ref="AZ152:AZ166" si="272">AR152-AV152</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA152" s="10" t="e">
-        <f t="shared" ref="BA152:BA164" si="273">AS152-AW152</f>
+        <f t="shared" ref="BA152:BA166" si="273">AS152-AW152</f>
         <v>#VALUE!</v>
       </c>
       <c r="BB152" t="s">
@@ -28840,6 +28845,9 @@
       <c r="AC163" s="3">
         <v>3</v>
       </c>
+      <c r="AD163" t="s">
+        <v>628</v>
+      </c>
       <c r="AE163" t="s">
         <v>117</v>
       </c>
@@ -28918,167 +28926,167 @@
         <v>117</v>
       </c>
     </row>
-    <row r="164" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A164" s="12" t="s">
+    <row r="164" spans="1:56" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="17" t="s">
         <v>605</v>
       </c>
-      <c r="B164" s="12" t="s">
+      <c r="B164" s="17" t="s">
         <v>627</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C164" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="D164" t="s">
+      <c r="D164" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E164" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="F164" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="G164" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="H164" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I164" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="J164" t="s">
-        <v>117</v>
-      </c>
-      <c r="L164" t="s">
-        <v>117</v>
-      </c>
-      <c r="T164" s="12"/>
-      <c r="U164" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="V164" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="W164" t="s">
-        <v>117</v>
-      </c>
-      <c r="X164" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y164" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC164" s="3">
+      <c r="F164" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="G164" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="H164" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I164" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="L164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="T164" s="17"/>
+      <c r="U164" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="V164" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="X164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC164" s="1">
         <v>3</v>
       </c>
-      <c r="AE164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI164" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ164" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK164" t="e">
+      <c r="AE164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI164" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ164" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK164" s="4" t="e">
         <f t="shared" si="269"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL164" t="e">
+      <c r="AL164" s="4" t="e">
         <f t="shared" si="270"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AM164" s="10" t="s">
+      <c r="AM164" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="AN164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP164" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AT164" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW164" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX164" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY164" t="e">
+      <c r="AN164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP164" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT164" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX164" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY164" s="4" t="e">
         <f t="shared" si="271"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ164" t="e">
+      <c r="AZ164" s="4" t="e">
         <f t="shared" si="272"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BA164" s="10" t="e">
+      <c r="BA164" s="29" t="e">
         <f t="shared" si="273"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BB164" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC164" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD164" t="s">
+      <c r="BB164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC164" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD164" s="4" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="165" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
-        <v>117</v>
+        <v>590</v>
       </c>
       <c r="B165" s="12" t="s">
         <v>117</v>
       </c>
       <c r="C165" t="s">
-        <v>117</v>
+        <v>457</v>
       </c>
       <c r="D165" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="E165" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="F165" s="64" t="s">
-        <v>117</v>
+        <v>629</v>
       </c>
       <c r="G165" s="12" t="s">
-        <v>117</v>
+        <v>516</v>
       </c>
       <c r="H165" s="12" t="s">
         <v>117</v>
@@ -29097,106 +29105,526 @@
         <v>117</v>
       </c>
       <c r="V165" t="s">
-        <v>117</v>
-      </c>
-      <c r="W165" t="s">
-        <v>117</v>
+        <v>529</v>
+      </c>
+      <c r="W165">
+        <v>6</v>
       </c>
       <c r="X165" t="s">
         <v>117</v>
       </c>
-      <c r="Y165" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC165" t="s">
-        <v>117</v>
+      <c r="Y165">
+        <v>5</v>
+      </c>
+      <c r="Z165">
+        <v>1</v>
+      </c>
+      <c r="AA165">
+        <f t="shared" ref="AA165:AA167" si="274">Y165+Z165</f>
+        <v>6</v>
+      </c>
+      <c r="AB165">
+        <v>1</v>
+      </c>
+      <c r="AC165">
+        <v>3</v>
       </c>
       <c r="AE165" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AH165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI165" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ165" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK165" t="e">
-        <f t="shared" ref="AK154:AK165" si="274">AI165+AJ165</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AL165" t="e">
-        <f t="shared" ref="AL154:AL165" si="275" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ165*AR165*AS165) * (AA165 / 5) + 441</f>
-        <v>#VALUE!</v>
+        <v>96</v>
+      </c>
+      <c r="AJ165" s="12"/>
+      <c r="AL165">
+        <f t="shared" si="270"/>
+        <v>74552.537876951479</v>
       </c>
       <c r="AM165" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AN165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP165" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS165" t="s">
-        <v>117</v>
+      <c r="AN165">
+        <v>173</v>
+      </c>
+      <c r="AO165">
+        <v>743</v>
+      </c>
+      <c r="AP165" s="20">
+        <v>435</v>
+      </c>
+      <c r="AQ165">
+        <v>133</v>
+      </c>
+      <c r="AR165">
+        <v>720</v>
+      </c>
+      <c r="AS165">
+        <v>300</v>
       </c>
       <c r="AT165" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV165" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW165" t="s">
-        <v>117</v>
+        <v>45</v>
+      </c>
+      <c r="AU165">
+        <f t="shared" ref="AU165:AU166" si="275" xml:space="preserve"> _xlfn.FLOOR.MATH((AN165 - AQ165) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV165">
+        <f t="shared" ref="AV165:AV166" si="276" xml:space="preserve"> _xlfn.FLOOR.MATH((AO165 - AR165) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW165">
+        <f t="shared" ref="AW165:AW166" si="277" xml:space="preserve"> _xlfn.FLOOR.MATH((AP165 - AS165) / 2)</f>
+        <v>67</v>
       </c>
       <c r="AX165" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY165" t="e">
-        <f t="shared" ref="AY154:AY165" si="276">AQ165-AU165</f>
+        <v>45</v>
+      </c>
+      <c r="AY165">
+        <f t="shared" si="271"/>
+        <v>113</v>
+      </c>
+      <c r="AZ165">
+        <f t="shared" si="272"/>
+        <v>709</v>
+      </c>
+      <c r="BA165" s="10">
+        <f t="shared" si="273"/>
+        <v>233</v>
+      </c>
+      <c r="BB165" t="s">
+        <v>537</v>
+      </c>
+      <c r="BC165" t="s">
+        <v>528</v>
+      </c>
+      <c r="BD165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A166" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="B166" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C166" t="s">
+        <v>457</v>
+      </c>
+      <c r="D166" t="s">
+        <v>406</v>
+      </c>
+      <c r="E166" t="s">
+        <v>409</v>
+      </c>
+      <c r="F166" s="64" t="s">
+        <v>629</v>
+      </c>
+      <c r="G166" s="12" t="s">
+        <v>516</v>
+      </c>
+      <c r="H166" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I166" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J166" t="s">
+        <v>117</v>
+      </c>
+      <c r="L166" t="s">
+        <v>117</v>
+      </c>
+      <c r="T166" s="12"/>
+      <c r="U166" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V166" t="s">
+        <v>544</v>
+      </c>
+      <c r="W166">
+        <v>6</v>
+      </c>
+      <c r="X166" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y166">
+        <v>5</v>
+      </c>
+      <c r="Z166">
+        <v>1</v>
+      </c>
+      <c r="AA166">
+        <f t="shared" si="274"/>
+        <v>6</v>
+      </c>
+      <c r="AB166">
+        <v>1</v>
+      </c>
+      <c r="AC166">
+        <v>1</v>
+      </c>
+      <c r="AE166" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH166" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ166" s="12"/>
+      <c r="AL166">
+        <f t="shared" si="270"/>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM166" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN166">
+        <v>173</v>
+      </c>
+      <c r="AO166">
+        <v>743</v>
+      </c>
+      <c r="AP166" s="20">
+        <v>435</v>
+      </c>
+      <c r="AQ166">
+        <v>133</v>
+      </c>
+      <c r="AR166">
+        <v>720</v>
+      </c>
+      <c r="AS166">
+        <v>300</v>
+      </c>
+      <c r="AT166" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU166">
+        <f t="shared" si="275"/>
+        <v>20</v>
+      </c>
+      <c r="AV166">
+        <f t="shared" si="276"/>
+        <v>11</v>
+      </c>
+      <c r="AW166">
+        <f t="shared" si="277"/>
+        <v>67</v>
+      </c>
+      <c r="AX166" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY166">
+        <f t="shared" si="271"/>
+        <v>113</v>
+      </c>
+      <c r="AZ166">
+        <f t="shared" si="272"/>
+        <v>709</v>
+      </c>
+      <c r="BA166" s="10">
+        <f t="shared" si="273"/>
+        <v>233</v>
+      </c>
+      <c r="BB166" t="s">
+        <v>537</v>
+      </c>
+      <c r="BC166" t="s">
+        <v>528</v>
+      </c>
+      <c r="BD166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A167" s="12" t="s">
+        <v>592</v>
+      </c>
+      <c r="B167" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C167" t="s">
+        <v>457</v>
+      </c>
+      <c r="D167" t="s">
+        <v>406</v>
+      </c>
+      <c r="E167" t="s">
+        <v>409</v>
+      </c>
+      <c r="F167" s="64" t="s">
+        <v>629</v>
+      </c>
+      <c r="G167" s="12" t="s">
+        <v>578</v>
+      </c>
+      <c r="H167" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I167" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J167" t="s">
+        <v>117</v>
+      </c>
+      <c r="L167" t="s">
+        <v>117</v>
+      </c>
+      <c r="T167" s="12"/>
+      <c r="U167" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V167" s="71" t="s">
+        <v>579</v>
+      </c>
+      <c r="W167" s="71">
+        <v>6</v>
+      </c>
+      <c r="X167" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y167" s="71">
+        <v>3</v>
+      </c>
+      <c r="Z167" s="71">
+        <v>2</v>
+      </c>
+      <c r="AA167" s="71">
+        <f t="shared" si="274"/>
+        <v>5</v>
+      </c>
+      <c r="AB167" s="71">
+        <v>2</v>
+      </c>
+      <c r="AC167" s="71">
+        <v>1</v>
+      </c>
+      <c r="AD167" s="71"/>
+      <c r="AE167" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF167" s="71"/>
+      <c r="AG167" s="71"/>
+      <c r="AH167" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ167" s="12"/>
+      <c r="AL167">
+        <f t="shared" ref="AL167" si="278" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ167*AR167*AS167) * (AA167 / 5) + 441</f>
+        <v>62451.959152962088</v>
+      </c>
+      <c r="AM167" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN167">
+        <v>173</v>
+      </c>
+      <c r="AO167">
+        <v>743</v>
+      </c>
+      <c r="AP167" s="20">
+        <v>435</v>
+      </c>
+      <c r="AQ167">
+        <v>133</v>
+      </c>
+      <c r="AR167">
+        <v>720</v>
+      </c>
+      <c r="AS167">
+        <v>300</v>
+      </c>
+      <c r="AT167" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU167">
+        <f t="shared" ref="AU167" si="279" xml:space="preserve"> _xlfn.FLOOR.MATH((AN167 - AQ167) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV167">
+        <f t="shared" ref="AV167" si="280" xml:space="preserve"> _xlfn.FLOOR.MATH((AO167 - AR167) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW167">
+        <f t="shared" ref="AW167" si="281" xml:space="preserve"> _xlfn.FLOOR.MATH((AP167 - AS167) / 2)</f>
+        <v>67</v>
+      </c>
+      <c r="AX167" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY167">
+        <f t="shared" ref="AY167" si="282">AQ167-AU167</f>
+        <v>113</v>
+      </c>
+      <c r="AZ167">
+        <f t="shared" ref="AZ167" si="283">AR167-AV167</f>
+        <v>709</v>
+      </c>
+      <c r="BA167" s="10">
+        <f t="shared" ref="BA167" si="284">AS167-AW167</f>
+        <v>233</v>
+      </c>
+      <c r="BB167" t="s">
+        <v>537</v>
+      </c>
+      <c r="BC167" t="s">
+        <v>528</v>
+      </c>
+      <c r="BD167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A168" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B168" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C168" t="s">
+        <v>117</v>
+      </c>
+      <c r="D168" t="s">
+        <v>117</v>
+      </c>
+      <c r="E168" t="s">
+        <v>117</v>
+      </c>
+      <c r="F168" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="G168" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="H168" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I168" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J168" t="s">
+        <v>117</v>
+      </c>
+      <c r="L168" t="s">
+        <v>117</v>
+      </c>
+      <c r="T168" s="12"/>
+      <c r="U168" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="V168" s="70" t="s">
+        <v>117</v>
+      </c>
+      <c r="W168" t="s">
+        <v>117</v>
+      </c>
+      <c r="X168" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y168" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI168" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ168" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK168" t="e">
+        <f t="shared" ref="AK168" si="285">AI168+AJ168</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ165" t="e">
-        <f t="shared" ref="AZ154:AZ165" si="277">AR165-AV165</f>
+      <c r="AL168" t="e">
+        <f t="shared" ref="AL168" si="286" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ168*AR168*AS168) * (AA168 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA165" s="10" t="e">
-        <f t="shared" ref="BA154:BA165" si="278">AS165-AW165</f>
+      <c r="AM168" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP168" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT168" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX168" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY168" t="e">
+        <f t="shared" ref="AY168" si="287">AQ168-AU168</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB165" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC165" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD165" t="s">
-        <v>117</v>
-      </c>
+      <c r="AZ168" t="e">
+        <f t="shared" ref="AZ168" si="288">AR168-AV168</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA168" s="10" t="e">
+        <f t="shared" ref="BA168" si="289">AS168-AW168</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB168" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC168" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD168" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="169" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A169" s="12"/>
+      <c r="B169" s="12"/>
+      <c r="F169" s="64"/>
+      <c r="G169" s="12"/>
+      <c r="H169" s="12"/>
+      <c r="T169" s="12"/>
+      <c r="V169" s="70"/>
+      <c r="AJ169" s="12"/>
+      <c r="AT169" s="25"/>
+      <c r="AX169" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
generic commit message, Thu 20:35:17 01.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B338AFF3-7F93-461D-9B5A-125A1AE9A52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943D2291-A3B2-4038-94D3-B3320B01A822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2565" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-21720" yWindow="2550" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4498" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4498" uniqueCount="626">
   <si>
     <t>patch z</t>
   </si>
@@ -1875,15 +1875,9 @@
     <t>240201-3</t>
   </si>
   <si>
-    <t>240131-8 best, dataset10.b autofluo eye</t>
-  </si>
-  <si>
     <t>240201-4</t>
   </si>
   <si>
-    <t>240131-8 last, dataset10.b autofluo eye</t>
-  </si>
-  <si>
     <t>autofluo eye</t>
   </si>
   <si>
@@ -1912,6 +1906,18 @@
   </si>
   <si>
     <t>stride = same as during model training</t>
+  </si>
+  <si>
+    <t>240131-8 last, autofluo eye</t>
+  </si>
+  <si>
+    <t>240131-8 best, autofluo eye</t>
+  </si>
+  <si>
+    <t>different LR factor, now 10 steps - better than dataset10.b models with less steps?</t>
+  </si>
+  <si>
+    <t>different LR factor, now 10 steps - better than dataset10.b models with less steps? (expect last_checkpoint to be better because boundary model and volume input labels)</t>
   </si>
 </sst>
 </file>
@@ -2719,8 +2725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BG164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AO156" sqref="AO156"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G155" activeCellId="1" sqref="H155 G155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2769,9 +2775,9 @@
     <col min="50" max="50" width="6" style="74" customWidth="1"/>
     <col min="51" max="52" width="6" customWidth="1"/>
     <col min="53" max="53" width="6" style="10" customWidth="1"/>
-    <col min="54" max="54" width="74.85546875" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="76.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="5.140625" customWidth="1"/>
+    <col min="54" max="54" width="74.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="76.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="5.140625" customWidth="1" collapsed="1"/>
     <col min="57" max="57" width="135.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="58" max="58" width="206" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="59" max="59" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -26755,7 +26761,7 @@
         <v>586</v>
       </c>
       <c r="B149" s="76" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C149" s="37" t="s">
         <v>525</v>
@@ -26883,7 +26889,7 @@
         <v>524</v>
       </c>
       <c r="BD149" s="77" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="150" spans="1:56" x14ac:dyDescent="0.25">
@@ -26891,7 +26897,7 @@
         <v>587</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>540</v>
@@ -27029,7 +27035,7 @@
         <v>588</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>575</v>
@@ -27167,7 +27173,7 @@
         <v>596</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>540</v>
@@ -27302,7 +27308,7 @@
         <v>597</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>575</v>
@@ -27561,10 +27567,10 @@
         <v>177</v>
       </c>
       <c r="BB154" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="BC154" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="BD154" t="s">
         <v>117</v>
@@ -27575,7 +27581,7 @@
         <v>610</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>611</v>
+        <v>623</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>525</v>
@@ -27590,7 +27596,7 @@
         <v>409</v>
       </c>
       <c r="G155" s="66" t="s">
-        <v>117</v>
+        <v>624</v>
       </c>
       <c r="H155" s="12" t="s">
         <v>117</v>
@@ -27705,10 +27711,10 @@
         <v>233</v>
       </c>
       <c r="BB155" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="BC155" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="BD155" t="s">
         <v>117</v>
@@ -27716,10 +27722,10 @@
     </row>
     <row r="156" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A156" s="61" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>525</v>
@@ -27734,7 +27740,7 @@
         <v>409</v>
       </c>
       <c r="G156" s="66" t="s">
-        <v>117</v>
+        <v>625</v>
       </c>
       <c r="H156" s="12" t="s">
         <v>117</v>
@@ -27849,10 +27855,10 @@
         <v>233</v>
       </c>
       <c r="BB156" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="BC156" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="BD156" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
generic commit message, Thu 21:22:27 01.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943D2291-A3B2-4038-94D3-B3320B01A822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E407A420-012D-464B-9E46-67BD3AF6F47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="2550" windowWidth="21840" windowHeight="13740" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4498" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4678" uniqueCount="637">
   <si>
     <t>patch z</t>
   </si>
@@ -1878,9 +1878,6 @@
     <t>240201-4</t>
   </si>
   <si>
-    <t>autofluo eye</t>
-  </si>
-  <si>
     <t>fluo eye FAIL</t>
   </si>
   <si>
@@ -1918,6 +1915,42 @@
   </si>
   <si>
     <t>different LR factor, now 10 steps - better than dataset10.b models with less steps? (expect last_checkpoint to be better because boundary model and volume input labels)</t>
+  </si>
+  <si>
+    <t>Increase LR steps to 10 with a factor of .588. (*this is fine.: Adapt patch shape for eyes to be in the patch for sure (y shape critical) - faulty assumption. Everything fine, just RNG stuff of tensorboard stats that looks weird.)</t>
+  </si>
+  <si>
+    <t>240201-5</t>
+  </si>
+  <si>
+    <t>autofluo eye, 10 LR steps at factor .588, patience 10</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>LR scheduler experiment: Compare with 240131-8: Increase only patience</t>
+  </si>
+  <si>
+    <t>LR scheduler experiment: Compare with 240131-8: Increase only LR factor</t>
+  </si>
+  <si>
+    <t>LR scheduler experiment: Compare with 240131-8: Decrease only validation frequency</t>
+  </si>
+  <si>
+    <t>LR scheduler experiment: …</t>
+  </si>
+  <si>
+    <t>LR scheduler experiment: Compare with 240131-8 (best &amp; last checkpoint, best checkpoint starts to rival last checkpoint in this model): Increase only patience</t>
+  </si>
+  <si>
+    <t>patch = same as during this experiment's control model training (240131-8)</t>
+  </si>
+  <si>
+    <t>stride = same as during this experiment's control model training (240131-8)</t>
+  </si>
+  <si>
+    <t>autofluo eye, patience 20 (x2), val frequency 30 (x1/1.5) =&gt; 3x train time</t>
   </si>
 </sst>
 </file>
@@ -2285,7 +2318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2409,6 +2442,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2725,14 +2760,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
   <dimension ref="A1:BG164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G155" activeCellId="1" sqref="H155 G155"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B151" activeCellId="1" sqref="B158 B151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="65.140625" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="3" customWidth="1" outlineLevel="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" customWidth="1"/>
@@ -2775,9 +2810,9 @@
     <col min="50" max="50" width="6" style="74" customWidth="1"/>
     <col min="51" max="52" width="6" customWidth="1"/>
     <col min="53" max="53" width="6" style="10" customWidth="1"/>
-    <col min="54" max="54" width="74.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="76.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="5.140625" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="74.85546875" customWidth="1" outlineLevel="1"/>
+    <col min="55" max="55" width="76.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="5.140625" customWidth="1"/>
     <col min="57" max="57" width="135.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="58" max="58" width="206" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="59" max="59" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -26761,7 +26796,7 @@
         <v>586</v>
       </c>
       <c r="B149" s="76" t="s">
-        <v>612</v>
+        <v>627</v>
       </c>
       <c r="C149" s="37" t="s">
         <v>525</v>
@@ -26776,7 +26811,7 @@
         <v>409</v>
       </c>
       <c r="G149" s="57" t="s">
-        <v>595</v>
+        <v>625</v>
       </c>
       <c r="H149" s="76" t="s">
         <v>516</v>
@@ -26889,7 +26924,7 @@
         <v>524</v>
       </c>
       <c r="BD149" s="77" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="150" spans="1:56" x14ac:dyDescent="0.25">
@@ -26897,7 +26932,7 @@
         <v>587</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>540</v>
@@ -27035,7 +27070,7 @@
         <v>588</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>575</v>
@@ -27173,7 +27208,7 @@
         <v>596</v>
       </c>
       <c r="B152" s="12" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>540</v>
@@ -27308,7 +27343,7 @@
         <v>597</v>
       </c>
       <c r="B153" s="12" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>575</v>
@@ -27442,7 +27477,7 @@
       <c r="A154" s="61" t="s">
         <v>602</v>
       </c>
-      <c r="B154" s="61" t="s">
+      <c r="B154" s="12" t="s">
         <v>603</v>
       </c>
       <c r="C154" s="3" t="s">
@@ -27567,10 +27602,10 @@
         <v>177</v>
       </c>
       <c r="BB154" t="s">
+        <v>617</v>
+      </c>
+      <c r="BC154" t="s">
         <v>618</v>
-      </c>
-      <c r="BC154" t="s">
-        <v>619</v>
       </c>
       <c r="BD154" t="s">
         <v>117</v>
@@ -27581,7 +27616,7 @@
         <v>610</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>525</v>
@@ -27596,7 +27631,7 @@
         <v>409</v>
       </c>
       <c r="G155" s="66" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H155" s="12" t="s">
         <v>117</v>
@@ -27662,61 +27697,61 @@
       <c r="AM155" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AN155" s="37">
+      <c r="AN155" s="3">
         <v>173</v>
       </c>
-      <c r="AO155" s="37">
+      <c r="AO155" s="3">
         <v>743</v>
       </c>
-      <c r="AP155" s="39">
+      <c r="AP155" s="74">
         <v>435</v>
       </c>
-      <c r="AQ155" s="37">
+      <c r="AQ155" s="3">
         <v>133</v>
       </c>
-      <c r="AR155" s="37">
+      <c r="AR155" s="3">
         <v>720</v>
       </c>
-      <c r="AS155" s="37">
+      <c r="AS155" s="3">
         <v>300</v>
       </c>
-      <c r="AT155" s="42" t="s">
+      <c r="AT155" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="AU155" s="37">
+      <c r="AU155" s="3">
         <f t="shared" ref="AU155:AU156" si="293" xml:space="preserve"> _xlfn.FLOOR.MATH((AN155 - AQ155) / 2)</f>
         <v>20</v>
       </c>
-      <c r="AV155" s="37">
+      <c r="AV155" s="3">
         <f t="shared" ref="AV155:AV156" si="294" xml:space="preserve"> _xlfn.FLOOR.MATH((AO155 - AR155) / 2)</f>
         <v>11</v>
       </c>
-      <c r="AW155" s="37">
+      <c r="AW155" s="3">
         <f t="shared" ref="AW155:AW156" si="295" xml:space="preserve"> _xlfn.FLOOR.MATH((AP155 - AS155) / 2)</f>
         <v>67</v>
       </c>
-      <c r="AX155" s="42" t="s">
+      <c r="AX155" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="AY155" s="77">
-        <f t="shared" ref="AY155:AY156" si="296">AQ155-AU155</f>
+      <c r="AY155" s="81">
+        <f t="shared" ref="AY155:AY157" si="296">AQ155-AU155</f>
         <v>113</v>
       </c>
-      <c r="AZ155" s="77">
-        <f t="shared" ref="AZ155:AZ156" si="297">AR155-AV155</f>
+      <c r="AZ155" s="81">
+        <f t="shared" ref="AZ155:AZ157" si="297">AR155-AV155</f>
         <v>709</v>
       </c>
-      <c r="BA155" s="80">
-        <f t="shared" ref="BA155:BA156" si="298">AS155-AW155</f>
+      <c r="BA155" s="82">
+        <f t="shared" ref="BA155:BA157" si="298">AS155-AW155</f>
         <v>233</v>
       </c>
-      <c r="BB155" t="s">
+      <c r="BB155" s="81" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC155" s="81" t="s">
         <v>620</v>
       </c>
-      <c r="BC155" t="s">
-        <v>621</v>
-      </c>
-      <c r="BD155" t="s">
+      <c r="BD155" s="81" t="s">
         <v>117</v>
       </c>
     </row>
@@ -27725,7 +27760,7 @@
         <v>611</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>525</v>
@@ -27740,7 +27775,7 @@
         <v>409</v>
       </c>
       <c r="G156" s="66" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="H156" s="12" t="s">
         <v>117</v>
@@ -27796,270 +27831,910 @@
         <v>117</v>
       </c>
       <c r="AK156" t="e">
-        <f t="shared" ref="AK156" si="299">AI156+AJ156</f>
+        <f t="shared" ref="AK156:AK157" si="299">AI156+AJ156</f>
         <v>#VALUE!</v>
       </c>
       <c r="AL156">
-        <f t="shared" ref="AL156" si="300" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ156*AR156*AS156) * (AA156 / 5) + 441</f>
+        <f t="shared" ref="AL156:AL157" si="300" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ156*AR156*AS156) * (AA156 / 5) + 441</f>
         <v>74552.537876951479</v>
       </c>
       <c r="AM156" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AN156" s="37">
+      <c r="AN156" s="3">
         <v>173</v>
       </c>
-      <c r="AO156" s="37">
+      <c r="AO156" s="3">
         <v>743</v>
       </c>
-      <c r="AP156" s="39">
+      <c r="AP156" s="74">
         <v>435</v>
       </c>
-      <c r="AQ156" s="37">
+      <c r="AQ156" s="3">
         <v>133</v>
       </c>
-      <c r="AR156" s="37">
+      <c r="AR156" s="3">
         <v>720</v>
       </c>
-      <c r="AS156" s="37">
+      <c r="AS156" s="3">
         <v>300</v>
       </c>
-      <c r="AT156" s="42" t="s">
+      <c r="AT156" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="AU156" s="37">
+      <c r="AU156" s="3">
         <f t="shared" si="293"/>
         <v>20</v>
       </c>
-      <c r="AV156" s="37">
+      <c r="AV156" s="3">
         <f t="shared" si="294"/>
         <v>11</v>
       </c>
-      <c r="AW156" s="37">
+      <c r="AW156" s="3">
         <f t="shared" si="295"/>
         <v>67</v>
       </c>
-      <c r="AX156" s="42" t="s">
+      <c r="AX156" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="AY156" s="77">
+      <c r="AY156" s="81">
         <f t="shared" si="296"/>
         <v>113</v>
       </c>
-      <c r="AZ156" s="77">
+      <c r="AZ156" s="81">
         <f t="shared" si="297"/>
         <v>709</v>
       </c>
-      <c r="BA156" s="80">
+      <c r="BA156" s="82">
         <f t="shared" si="298"/>
         <v>233</v>
       </c>
-      <c r="BB156" t="s">
+      <c r="BB156" s="81" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC156" s="81" t="s">
         <v>620</v>
       </c>
-      <c r="BC156" t="s">
-        <v>621</v>
-      </c>
-      <c r="BD156" t="s">
+      <c r="BD156" s="81" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="157" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A157" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B157" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D157" t="s">
-        <v>117</v>
-      </c>
-      <c r="E157" t="s">
-        <v>117</v>
-      </c>
-      <c r="F157" t="s">
-        <v>117</v>
-      </c>
-      <c r="G157" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="H157" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="I157" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J157" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="K157" t="s">
-        <v>117</v>
-      </c>
-      <c r="M157" t="s">
-        <v>117</v>
-      </c>
-      <c r="U157" s="12"/>
-      <c r="V157" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="W157" t="s">
-        <v>117</v>
-      </c>
-      <c r="X157" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y157" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z157" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA157" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB157" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE157" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH157" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI157" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ157" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK157" t="e">
-        <f t="shared" ref="AK157" si="301">AI157+AJ157</f>
+    <row r="157" spans="1:56" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="62" t="s">
+        <v>626</v>
+      </c>
+      <c r="B157" s="17" t="s">
+        <v>636</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="F157" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="G157" s="67" t="s">
+        <v>633</v>
+      </c>
+      <c r="H157" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I157" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="J157" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="K157" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="M157" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U157" s="17"/>
+      <c r="V157" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="W157" s="4">
+        <v>6</v>
+      </c>
+      <c r="X157" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y157" s="4">
+        <v>5</v>
+      </c>
+      <c r="Z157" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA157" s="4">
+        <v>6</v>
+      </c>
+      <c r="AB157" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC157" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE157" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH157" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI157" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ157" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK157" s="4" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="AL157" t="e">
-        <f t="shared" ref="AL157" si="302" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ157*AR157*AS157) * (AA157 / 5) + 441</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AM157" s="10" t="s">
+      <c r="AL157" s="4">
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM157" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="AN157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP157" s="74" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AT157" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW157" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX157" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY157" t="e">
-        <f t="shared" ref="AY157" si="303">AQ157-AU157</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ157" t="e">
-        <f t="shared" ref="AZ157" si="304">AR157-AV157</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA157" s="10" t="e">
-        <f t="shared" ref="BA157" si="305">AS157-AW157</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB157" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC157" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD157" t="s">
+      <c r="AN157" s="1">
+        <v>173</v>
+      </c>
+      <c r="AO157" s="1">
+        <v>743</v>
+      </c>
+      <c r="AP157" s="19">
+        <v>435</v>
+      </c>
+      <c r="AQ157" s="1">
+        <v>133</v>
+      </c>
+      <c r="AR157" s="1">
+        <v>720</v>
+      </c>
+      <c r="AS157" s="1">
+        <v>300</v>
+      </c>
+      <c r="AT157" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU157" s="1">
+        <v>20</v>
+      </c>
+      <c r="AV157" s="1">
+        <v>11</v>
+      </c>
+      <c r="AW157" s="1">
+        <v>67</v>
+      </c>
+      <c r="AX157" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY157" s="4">
+        <v>113</v>
+      </c>
+      <c r="AZ157" s="4">
+        <v>709</v>
+      </c>
+      <c r="BA157" s="27">
+        <v>233</v>
+      </c>
+      <c r="BB157" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="BC157" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="BD157" s="4" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="158" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A158" s="61"/>
-      <c r="B158" s="12"/>
-      <c r="G158" s="66"/>
-      <c r="H158" s="12"/>
-      <c r="I158" s="12"/>
+      <c r="A158" s="61" t="s">
+        <v>628</v>
+      </c>
+      <c r="B158" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D158" t="s">
+        <v>457</v>
+      </c>
+      <c r="E158" t="s">
+        <v>406</v>
+      </c>
+      <c r="F158" t="s">
+        <v>409</v>
+      </c>
+      <c r="G158" s="66" t="s">
+        <v>629</v>
+      </c>
+      <c r="H158" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I158" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J158" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K158" t="s">
+        <v>117</v>
+      </c>
+      <c r="M158" t="s">
+        <v>117</v>
+      </c>
       <c r="U158" s="12"/>
-      <c r="AJ158" s="12"/>
-      <c r="AT158" s="49"/>
-      <c r="AX158" s="49"/>
+      <c r="V158" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="W158" t="s">
+        <v>117</v>
+      </c>
+      <c r="X158" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y158" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH158" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI158" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ158" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK158" t="e">
+        <f t="shared" ref="AK158" si="301">AI158+AJ158</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL158" t="e">
+        <f t="shared" ref="AL158" si="302" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ158*AR158*AS158) * (AA158 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM158" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP158" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT158" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW158" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX158" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY158" t="e">
+        <f t="shared" ref="AY158" si="303">AQ158-AU158</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ158" t="e">
+        <f t="shared" ref="AZ158" si="304">AR158-AV158</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA158" s="10" t="e">
+        <f t="shared" ref="BA158" si="305">AS158-AW158</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB158" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC158" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD158" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="159" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A159" s="61"/>
-      <c r="B159" s="12"/>
-      <c r="G159" s="66"/>
-      <c r="H159" s="12"/>
-      <c r="I159" s="12"/>
+      <c r="A159" s="61" t="s">
+        <v>628</v>
+      </c>
+      <c r="B159" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D159" t="s">
+        <v>457</v>
+      </c>
+      <c r="E159" t="s">
+        <v>406</v>
+      </c>
+      <c r="F159" t="s">
+        <v>409</v>
+      </c>
+      <c r="G159" s="66" t="s">
+        <v>630</v>
+      </c>
+      <c r="H159" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I159" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J159" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K159" t="s">
+        <v>117</v>
+      </c>
+      <c r="M159" t="s">
+        <v>117</v>
+      </c>
       <c r="U159" s="12"/>
-      <c r="AJ159" s="12"/>
-      <c r="AT159" s="49"/>
-      <c r="AX159" s="49"/>
+      <c r="V159" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="W159" t="s">
+        <v>117</v>
+      </c>
+      <c r="X159" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y159" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC159" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH159" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI159" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ159" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK159" t="e">
+        <f t="shared" ref="AK159" si="306">AI159+AJ159</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL159" t="e">
+        <f t="shared" ref="AL159" si="307" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ159*AR159*AS159) * (AA159 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM159" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN159" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO159" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP159" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ159" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR159" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS159" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT159" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU159" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV159" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW159" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX159" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY159" t="e">
+        <f t="shared" ref="AY159" si="308">AQ159-AU159</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ159" t="e">
+        <f t="shared" ref="AZ159" si="309">AR159-AV159</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA159" s="10" t="e">
+        <f t="shared" ref="BA159" si="310">AS159-AW159</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB159" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC159" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD159" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="160" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A160" s="61"/>
-      <c r="B160" s="12"/>
-      <c r="G160" s="66"/>
-      <c r="H160" s="12"/>
-      <c r="I160" s="12"/>
+      <c r="A160" s="61" t="s">
+        <v>628</v>
+      </c>
+      <c r="B160" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D160" t="s">
+        <v>457</v>
+      </c>
+      <c r="E160" t="s">
+        <v>406</v>
+      </c>
+      <c r="F160" t="s">
+        <v>409</v>
+      </c>
+      <c r="G160" s="66" t="s">
+        <v>631</v>
+      </c>
+      <c r="H160" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I160" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J160" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K160" t="s">
+        <v>117</v>
+      </c>
+      <c r="M160" t="s">
+        <v>117</v>
+      </c>
       <c r="U160" s="12"/>
-      <c r="AJ160" s="12"/>
-      <c r="AT160" s="49"/>
-      <c r="AX160" s="49"/>
+      <c r="V160" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="W160" t="s">
+        <v>117</v>
+      </c>
+      <c r="X160" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y160" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC160" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH160" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI160" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ160" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK160" t="e">
+        <f t="shared" ref="AK160" si="311">AI160+AJ160</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL160" t="e">
+        <f t="shared" ref="AL160" si="312" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ160*AR160*AS160) * (AA160 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM160" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN160" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO160" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP160" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ160" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR160" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS160" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT160" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU160" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV160" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW160" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX160" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY160" t="e">
+        <f t="shared" ref="AY160" si="313">AQ160-AU160</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ160" t="e">
+        <f t="shared" ref="AZ160" si="314">AR160-AV160</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA160" s="10" t="e">
+        <f t="shared" ref="BA160" si="315">AS160-AW160</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB160" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC160" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD160" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="161" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A161" s="61"/>
-      <c r="B161" s="12"/>
-      <c r="G161" s="66"/>
-      <c r="H161" s="12"/>
-      <c r="I161" s="12"/>
+    <row r="161" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A161" s="61" t="s">
+        <v>628</v>
+      </c>
+      <c r="B161" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D161" t="s">
+        <v>457</v>
+      </c>
+      <c r="E161" t="s">
+        <v>406</v>
+      </c>
+      <c r="F161" t="s">
+        <v>409</v>
+      </c>
+      <c r="G161" s="66" t="s">
+        <v>632</v>
+      </c>
+      <c r="H161" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I161" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J161" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K161" t="s">
+        <v>117</v>
+      </c>
+      <c r="M161" t="s">
+        <v>117</v>
+      </c>
       <c r="U161" s="12"/>
-      <c r="AJ161" s="12"/>
-      <c r="AT161" s="49"/>
-      <c r="AX161" s="49"/>
+      <c r="V161" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="W161" t="s">
+        <v>117</v>
+      </c>
+      <c r="X161" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y161" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC161" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH161" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI161" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ161" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK161" t="e">
+        <f t="shared" ref="AK161" si="316">AI161+AJ161</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL161" t="e">
+        <f t="shared" ref="AL161" si="317" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ161*AR161*AS161) * (AA161 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM161" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN161" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO161" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP161" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ161" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR161" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS161" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT161" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU161" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV161" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW161" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX161" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY161" t="e">
+        <f t="shared" ref="AY161" si="318">AQ161-AU161</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ161" t="e">
+        <f t="shared" ref="AZ161" si="319">AR161-AV161</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA161" s="10" t="e">
+        <f t="shared" ref="BA161" si="320">AS161-AW161</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB161" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC161" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD161" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="162" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A162" s="61"/>
-      <c r="B162" s="12"/>
-      <c r="G162" s="66"/>
-      <c r="H162" s="12"/>
-      <c r="I162" s="12"/>
+    <row r="162" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A162" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="B162" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D162" t="s">
+        <v>117</v>
+      </c>
+      <c r="E162" t="s">
+        <v>117</v>
+      </c>
+      <c r="F162" t="s">
+        <v>117</v>
+      </c>
+      <c r="G162" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="H162" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I162" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J162" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K162" t="s">
+        <v>117</v>
+      </c>
+      <c r="M162" t="s">
+        <v>117</v>
+      </c>
       <c r="U162" s="12"/>
-      <c r="AJ162" s="12"/>
-      <c r="AT162" s="49"/>
-      <c r="AX162" s="49"/>
+      <c r="V162" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="W162" t="s">
+        <v>117</v>
+      </c>
+      <c r="X162" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y162" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH162" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI162" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ162" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK162" t="e">
+        <f t="shared" ref="AK162" si="321">AI162+AJ162</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL162" t="e">
+        <f t="shared" ref="AL162" si="322" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ162*AR162*AS162) * (AA162 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM162" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP162" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT162" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW162" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX162" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY162" t="e">
+        <f t="shared" ref="AY162" si="323">AQ162-AU162</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ162" t="e">
+        <f t="shared" ref="AZ162" si="324">AR162-AV162</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA162" s="10" t="e">
+        <f t="shared" ref="BA162" si="325">AS162-AW162</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB162" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC162" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD162" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="163" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A163" s="61"/>
       <c r="B163" s="12"/>
       <c r="G163" s="66"/>
@@ -28070,7 +28745,7 @@
       <c r="AT163" s="49"/>
       <c r="AX163" s="49"/>
     </row>
-    <row r="164" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A164" s="61"/>
       <c r="B164" s="12"/>
       <c r="G164" s="66"/>

</xml_diff>

<commit_message>
generic commit message, Sat 21:15:55 03.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC5553E-E1F5-47A0-AFD6-27908495C84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EE7AD7-921D-4ED7-B95F-CECA67F6E9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4670" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4646" uniqueCount="667">
   <si>
     <t>patch z</t>
   </si>
@@ -2046,12 +2046,6 @@
     <t>240203-2</t>
   </si>
   <si>
-    <t>240203-?</t>
-  </si>
-  <si>
-    <t>1?</t>
-  </si>
-  <si>
     <t>21.96% underestimated</t>
   </si>
   <si>
@@ -2062,13 +2056,28 @@
   </si>
   <si>
     <t>29.08% underestimated, precisely 2* previous run (k^3*vram ~ patch(k*x * k*y * k*z))</t>
+  </si>
+  <si>
+    <t>240203-5</t>
+  </si>
+  <si>
+    <t>Train a model that segments blobs instead of boundaries like previously</t>
+  </si>
+  <si>
+    <t>expect blobs (volumes) where eyes are</t>
+  </si>
+  <si>
+    <t>patch = same as during the analog boundary model (240131-8)</t>
+  </si>
+  <si>
+    <t>stride = same as during the analog boundary model (240131-8)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2159,8 +2168,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2181,6 +2197,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD6EE8A"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -2466,13 +2488,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyFont="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2576,8 +2599,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="gelb grün" xfId="2" xr:uid="{C6C8E641-F74F-4C6C-A8F4-FD2B0DFFAC6F}"/>
     <cellStyle name="Neutral-Good" xfId="3" xr:uid="{7D20F6EC-0149-4C40-9844-566C0E598255}"/>
@@ -2899,13 +2924,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG171"/>
+  <dimension ref="A1:BG169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V139" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AL139" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL164" sqref="AL164"/>
+      <selection pane="bottomRight" activeCell="AX166" sqref="AX166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -28054,7 +28079,7 @@
         <f t="shared" si="33"/>
         <v>81052</v>
       </c>
-      <c r="AL157">
+      <c r="AL157" s="67">
         <f t="shared" si="26"/>
         <v>74552.537876951479</v>
       </c>
@@ -28529,10 +28554,16 @@
         <v>644</v>
       </c>
       <c r="I161" s="32" t="s">
-        <v>662</v>
-      </c>
-      <c r="J161" s="34" t="s">
-        <v>117</v>
+        <v>660</v>
+      </c>
+      <c r="J161" s="34">
+        <v>0</v>
+      </c>
+      <c r="K161" s="33">
+        <v>1</v>
+      </c>
+      <c r="L161" s="33" t="s">
+        <v>642</v>
       </c>
       <c r="U161" s="32"/>
       <c r="V161" s="35">
@@ -28634,8 +28665,8 @@
       <c r="BC161" s="33" t="s">
         <v>524</v>
       </c>
-      <c r="BD161" s="33" t="s">
-        <v>117</v>
+      <c r="BD161" s="33">
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
@@ -28664,10 +28695,16 @@
         <v>644</v>
       </c>
       <c r="I162" s="32" t="s">
-        <v>661</v>
-      </c>
-      <c r="J162" s="34" t="s">
-        <v>117</v>
+        <v>659</v>
+      </c>
+      <c r="J162" s="34">
+        <v>0</v>
+      </c>
+      <c r="K162" s="33">
+        <v>1</v>
+      </c>
+      <c r="L162" s="33" t="s">
+        <v>642</v>
       </c>
       <c r="U162" s="32"/>
       <c r="V162" s="35">
@@ -28769,8 +28806,8 @@
       <c r="BC162" s="33" t="s">
         <v>649</v>
       </c>
-      <c r="BD162" s="33" t="s">
-        <v>117</v>
+      <c r="BD162" s="33">
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
@@ -28799,14 +28836,20 @@
         <v>644</v>
       </c>
       <c r="I163" s="32" t="s">
-        <v>661</v>
-      </c>
-      <c r="J163" s="34" t="s">
-        <v>117</v>
+        <v>659</v>
+      </c>
+      <c r="J163" s="34">
+        <v>0</v>
+      </c>
+      <c r="K163" s="33">
+        <v>1</v>
+      </c>
+      <c r="L163" s="33" t="s">
+        <v>642</v>
       </c>
       <c r="U163" s="32"/>
-      <c r="V163" s="35" t="s">
-        <v>659</v>
+      <c r="V163" s="35">
+        <v>1</v>
       </c>
       <c r="W163">
         <v>3</v>
@@ -28904,8 +28947,8 @@
       <c r="BC163" s="33" t="s">
         <v>648</v>
       </c>
-      <c r="BD163" s="33" t="s">
-        <v>117</v>
+      <c r="BD163" s="33">
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
@@ -28934,14 +28977,20 @@
         <v>644</v>
       </c>
       <c r="I164" s="32" t="s">
-        <v>660</v>
-      </c>
-      <c r="J164" s="34" t="s">
-        <v>117</v>
+        <v>658</v>
+      </c>
+      <c r="J164" s="34">
+        <v>0</v>
+      </c>
+      <c r="K164" s="33">
+        <v>1</v>
+      </c>
+      <c r="L164" s="33" t="s">
+        <v>642</v>
       </c>
       <c r="U164" s="32"/>
-      <c r="V164" s="35" t="s">
-        <v>659</v>
+      <c r="V164" s="35">
+        <v>1</v>
       </c>
       <c r="W164">
         <v>3</v>
@@ -29010,15 +29059,15 @@
         <v>45</v>
       </c>
       <c r="AU164" s="33">
-        <f t="shared" ref="AU164:AU165" si="43" xml:space="preserve"> _xlfn.FLOOR.MATH((AN164 - AQ164) / 2)</f>
+        <f t="shared" ref="AU164:AU166" si="43" xml:space="preserve"> _xlfn.FLOOR.MATH((AN164 - AQ164) / 2)</f>
         <v>37</v>
       </c>
       <c r="AV164" s="33">
-        <f t="shared" ref="AV164:AV165" si="44" xml:space="preserve"> _xlfn.FLOOR.MATH((AO164 - AR164) / 2)</f>
+        <f t="shared" ref="AV164:AV166" si="44" xml:space="preserve"> _xlfn.FLOOR.MATH((AO164 - AR164) / 2)</f>
         <v>74</v>
       </c>
       <c r="AW164" s="33">
-        <f t="shared" ref="AW164:AW165" si="45" xml:space="preserve"> _xlfn.FLOOR.MATH((AP164 - AS164) / 2)</f>
+        <f t="shared" ref="AW164:AW166" si="45" xml:space="preserve"> _xlfn.FLOOR.MATH((AP164 - AS164) / 2)</f>
         <v>74</v>
       </c>
       <c r="AX164" s="51" t="s">
@@ -29042,8 +29091,8 @@
       <c r="BC164" s="33" t="s">
         <v>650</v>
       </c>
-      <c r="BD164" s="33" t="s">
-        <v>117</v>
+      <c r="BD164" s="33">
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
@@ -29072,14 +29121,20 @@
         <v>644</v>
       </c>
       <c r="I165" s="32" t="s">
-        <v>663</v>
-      </c>
-      <c r="J165" s="34" t="s">
-        <v>117</v>
+        <v>661</v>
+      </c>
+      <c r="J165" s="34">
+        <v>0</v>
+      </c>
+      <c r="K165" s="33">
+        <v>1</v>
+      </c>
+      <c r="L165" s="33" t="s">
+        <v>642</v>
       </c>
       <c r="U165" s="32"/>
-      <c r="V165" s="35" t="s">
-        <v>659</v>
+      <c r="V165" s="35">
+        <v>1</v>
       </c>
       <c r="W165">
         <v>3</v>
@@ -29094,7 +29149,7 @@
         <v>1</v>
       </c>
       <c r="AA165">
-        <f t="shared" ref="AA165" si="49">X165+Y165</f>
+        <f t="shared" ref="AA165:AA166" si="49">X165+Y165</f>
         <v>2</v>
       </c>
       <c r="AB165">
@@ -29115,7 +29170,7 @@
         <v>35373</v>
       </c>
       <c r="AK165">
-        <f t="shared" ref="AK165" si="50">AI165+AJ165</f>
+        <f t="shared" ref="AK165:AK166" si="50">AI165+AJ165</f>
         <v>81052</v>
       </c>
       <c r="AL165" s="66">
@@ -29180,454 +29235,458 @@
       <c r="BC165" s="33" t="s">
         <v>650</v>
       </c>
-      <c r="BD165" s="33" t="s">
-        <v>117</v>
+      <c r="BD165" s="33">
+        <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="32"/>
-      <c r="B166" s="32"/>
-      <c r="C166"/>
-      <c r="D166"/>
-      <c r="E166"/>
-      <c r="F166"/>
-      <c r="G166" s="43"/>
-      <c r="H166" s="32"/>
-      <c r="I166" s="32"/>
-      <c r="J166" s="34"/>
-      <c r="U166" s="32"/>
-      <c r="V166" s="35"/>
-      <c r="W166"/>
-      <c r="X166"/>
-      <c r="Y166"/>
-      <c r="Z166"/>
-      <c r="AA166"/>
-      <c r="AB166"/>
-      <c r="AC166"/>
-      <c r="AD166"/>
-      <c r="AE166"/>
-      <c r="AF166"/>
-      <c r="AG166"/>
-      <c r="AH166" s="8"/>
-      <c r="AI166"/>
-      <c r="AJ166"/>
-      <c r="AK166"/>
-      <c r="AL166"/>
-      <c r="AM166" s="8"/>
-      <c r="AN166"/>
-      <c r="AO166"/>
-      <c r="AP166" s="17"/>
-      <c r="AQ166"/>
-      <c r="AR166"/>
-      <c r="AS166"/>
-      <c r="AT166" s="47"/>
-      <c r="AU166"/>
-      <c r="AV166"/>
-      <c r="AW166"/>
-      <c r="AX166" s="47"/>
-      <c r="BA166" s="36"/>
+    <row r="166" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A166" s="32" t="s">
+        <v>662</v>
+      </c>
+      <c r="B166" s="10" t="s">
+        <v>640</v>
+      </c>
+      <c r="C166" t="s">
+        <v>525</v>
+      </c>
+      <c r="D166" t="s">
+        <v>457</v>
+      </c>
+      <c r="E166" t="s">
+        <v>406</v>
+      </c>
+      <c r="F166" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="G166" s="40" t="s">
+        <v>663</v>
+      </c>
+      <c r="H166" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="I166" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J166" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U166" s="10"/>
+      <c r="V166" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W166">
+        <v>6</v>
+      </c>
+      <c r="X166">
+        <v>5</v>
+      </c>
+      <c r="Y166">
+        <v>1</v>
+      </c>
+      <c r="Z166">
+        <v>1</v>
+      </c>
+      <c r="AA166">
+        <f t="shared" si="49"/>
+        <v>6</v>
+      </c>
+      <c r="AB166">
+        <v>6</v>
+      </c>
+      <c r="AC166">
+        <v>3</v>
+      </c>
+      <c r="AE166" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH166" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI166" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ166" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK166" t="e">
+        <f t="shared" si="50"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL166" s="67">
+        <f t="shared" ref="AL166" si="54" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ166*AR166*AS166) * (AA166 / 5) + 441</f>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM166" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN166">
+        <v>173</v>
+      </c>
+      <c r="AO166">
+        <v>743</v>
+      </c>
+      <c r="AP166" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ166">
+        <v>133</v>
+      </c>
+      <c r="AR166">
+        <v>720</v>
+      </c>
+      <c r="AS166">
+        <v>300</v>
+      </c>
+      <c r="AT166" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU166">
+        <f t="shared" si="43"/>
+        <v>20</v>
+      </c>
+      <c r="AV166">
+        <f t="shared" si="44"/>
+        <v>11</v>
+      </c>
+      <c r="AW166">
+        <f t="shared" si="45"/>
+        <v>67</v>
+      </c>
+      <c r="AX166" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY166">
+        <f t="shared" ref="AY166:BA167" si="55">AQ166-AU166</f>
+        <v>113</v>
+      </c>
+      <c r="AZ166">
+        <f t="shared" si="55"/>
+        <v>709</v>
+      </c>
+      <c r="BA166" s="8">
+        <f t="shared" si="55"/>
+        <v>233</v>
+      </c>
+      <c r="BB166" t="s">
+        <v>665</v>
+      </c>
+      <c r="BC166" t="s">
+        <v>666</v>
+      </c>
+      <c r="BD166" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="169" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A169" s="32" t="s">
-        <v>658</v>
-      </c>
-      <c r="B169" s="10" t="s">
-        <v>640</v>
-      </c>
-      <c r="C169" t="s">
-        <v>525</v>
-      </c>
-      <c r="D169" t="s">
-        <v>457</v>
-      </c>
-      <c r="E169" t="s">
-        <v>406</v>
-      </c>
-      <c r="F169" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="G169" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="H169" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I169" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J169" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="U169" s="10"/>
-      <c r="V169" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="W169" t="s">
-        <v>117</v>
-      </c>
-      <c r="X169" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y169" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH169" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK169" t="e">
-        <f>AI169+AJ169</f>
+    <row r="167" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A167" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B167" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C167" t="s">
+        <v>117</v>
+      </c>
+      <c r="D167" t="s">
+        <v>117</v>
+      </c>
+      <c r="E167" t="s">
+        <v>117</v>
+      </c>
+      <c r="F167" t="s">
+        <v>117</v>
+      </c>
+      <c r="G167" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H167" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I167" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J167" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U167" s="10"/>
+      <c r="V167" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W167" t="s">
+        <v>117</v>
+      </c>
+      <c r="X167" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y167" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH167" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK167" t="e">
+        <f>AI167+AJ167</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AL169" t="e">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ169*AR169*AS169) * (AA169 / 5) + 441</f>
+      <c r="AL167" t="e">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ167*AR167*AS167) * (AA167 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM169" s="8" t="s">
+      <c r="AM167" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AN169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP169" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AT169" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX169" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY169" t="e">
-        <f t="shared" ref="AY169:BA170" si="54">AQ169-AU169</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ169" t="e">
-        <f t="shared" si="54"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA169" s="8" t="e">
-        <f t="shared" si="54"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB169" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC169" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD169" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="170" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A170" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B170" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C170" t="s">
-        <v>117</v>
-      </c>
-      <c r="D170" t="s">
-        <v>117</v>
-      </c>
-      <c r="E170" t="s">
-        <v>117</v>
-      </c>
-      <c r="F170" t="s">
-        <v>117</v>
-      </c>
-      <c r="G170" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="H170" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I170" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J170" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="U170" s="10"/>
-      <c r="V170" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="W170" t="s">
-        <v>117</v>
-      </c>
-      <c r="X170" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y170" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH170" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK170" t="e">
-        <f>AI170+AJ170</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AL170" t="e">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ170*AR170*AS170) * (AA170 / 5) + 441</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AM170" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP170" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AT170" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX170" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY170" t="e">
-        <f t="shared" si="54"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ170" t="e">
-        <f t="shared" si="54"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA170" s="8" t="e">
-        <f t="shared" si="54"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB170" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC170" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD170" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="171" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A171" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B171" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C171" t="s">
-        <v>117</v>
-      </c>
-      <c r="D171" t="s">
-        <v>117</v>
-      </c>
-      <c r="E171" t="s">
-        <v>117</v>
-      </c>
-      <c r="F171" t="s">
-        <v>117</v>
-      </c>
-      <c r="G171" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="H171" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I171" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J171" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="U171" s="10"/>
-      <c r="V171" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="W171" t="s">
-        <v>117</v>
-      </c>
-      <c r="X171" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y171" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH171" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK171" t="e">
-        <f>AI171+AJ171</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AL171" t="e">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ171*AR171*AS171) * (AA171 / 5) + 441</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AM171" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP171" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AT171" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW171" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX171" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY171" t="e">
-        <f t="shared" ref="AY171:BA171" si="55">AQ171-AU171</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ171" t="e">
+      <c r="AN167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP167" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT167" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW167" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX167" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY167" t="e">
         <f t="shared" si="55"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BA171" s="8" t="e">
+      <c r="AZ167" t="e">
         <f t="shared" si="55"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BB171" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC171" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD171" t="s">
-        <v>117</v>
-      </c>
+      <c r="BA167" s="8" t="e">
+        <f t="shared" si="55"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB167" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC167" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD167" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="168" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A168" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B168" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C168" t="s">
+        <v>117</v>
+      </c>
+      <c r="D168" t="s">
+        <v>117</v>
+      </c>
+      <c r="E168" t="s">
+        <v>117</v>
+      </c>
+      <c r="F168" t="s">
+        <v>117</v>
+      </c>
+      <c r="G168" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H168" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I168" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J168" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U168" s="10"/>
+      <c r="V168" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W168" t="s">
+        <v>117</v>
+      </c>
+      <c r="X168" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y168" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH168" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK168" t="e">
+        <f>AI168+AJ168</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL168" t="e">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ168*AR168*AS168) * (AA168 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM168" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP168" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT168" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX168" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY168" t="e">
+        <f t="shared" ref="AY168:BA168" si="56">AQ168-AU168</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ168" t="e">
+        <f t="shared" si="56"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA168" s="8" t="e">
+        <f t="shared" si="56"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB168" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC168" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD168" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="169" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="32"/>
+      <c r="B169" s="32"/>
+      <c r="C169"/>
+      <c r="D169"/>
+      <c r="E169"/>
+      <c r="F169"/>
+      <c r="G169" s="43"/>
+      <c r="H169" s="32"/>
+      <c r="I169" s="32"/>
+      <c r="J169" s="34"/>
+      <c r="U169" s="32"/>
+      <c r="V169" s="35"/>
+      <c r="W169"/>
+      <c r="X169"/>
+      <c r="Y169"/>
+      <c r="Z169"/>
+      <c r="AA169"/>
+      <c r="AB169"/>
+      <c r="AC169"/>
+      <c r="AD169"/>
+      <c r="AE169"/>
+      <c r="AF169"/>
+      <c r="AG169"/>
+      <c r="AH169" s="8"/>
+      <c r="AI169"/>
+      <c r="AJ169"/>
+      <c r="AK169"/>
+      <c r="AL169"/>
+      <c r="AM169" s="8"/>
+      <c r="AN169"/>
+      <c r="AO169"/>
+      <c r="AP169" s="17"/>
+      <c r="AQ169"/>
+      <c r="AR169"/>
+      <c r="AS169"/>
+      <c r="AT169" s="47"/>
+      <c r="AU169"/>
+      <c r="AV169"/>
+      <c r="AW169"/>
+      <c r="AX169" s="47"/>
+      <c r="BA169" s="36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
generic commit message, Sun 12:18:54 04.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EE7AD7-921D-4ED7-B95F-CECA67F6E9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CDD146-9261-4F33-B131-2F06E960789F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4646" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4607" uniqueCount="667">
   <si>
     <t>patch z</t>
   </si>
@@ -2176,7 +2176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2203,6 +2203,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -2488,14 +2493,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyFont="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2600,11 +2606,16 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="gelb grün" xfId="2" xr:uid="{C6C8E641-F74F-4C6C-A8F4-FD2B0DFFAC6F}"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Neutral-Good" xfId="3" xr:uid="{7D20F6EC-0149-4C40-9844-566C0E598255}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2927,10 +2938,10 @@
   <dimension ref="A1:BG169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AL139" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AX166" sqref="AX166"/>
+      <selection pane="bottomRight" activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -29240,22 +29251,22 @@
       </c>
     </row>
     <row r="166" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A166" s="32" t="s">
+      <c r="A166" s="68" t="s">
         <v>662</v>
       </c>
-      <c r="B166" s="10" t="s">
+      <c r="B166" s="68" t="s">
         <v>640</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C166" s="69" t="s">
         <v>525</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="69" t="s">
         <v>457</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="69" t="s">
         <v>406</v>
       </c>
-      <c r="F166" s="2" t="s">
+      <c r="F166" s="69" t="s">
         <v>636</v>
       </c>
       <c r="G166" s="40" t="s">
@@ -29302,15 +29313,15 @@
       <c r="AH166" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AI166" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ166" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK166" t="e">
+      <c r="AI166">
+        <v>78075</v>
+      </c>
+      <c r="AJ166" s="10">
+        <v>2977</v>
+      </c>
+      <c r="AK166">
         <f t="shared" si="50"/>
-        <v>#VALUE!</v>
+        <v>81052</v>
       </c>
       <c r="AL166" s="67">
         <f t="shared" ref="AL166" si="54" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ166*AR166*AS166) * (AA166 / 5) + 441</f>
@@ -29512,138 +29523,14 @@
       </c>
     </row>
     <row r="168" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A168" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B168" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C168" t="s">
-        <v>117</v>
-      </c>
-      <c r="D168" t="s">
-        <v>117</v>
-      </c>
-      <c r="E168" t="s">
-        <v>117</v>
-      </c>
-      <c r="F168" t="s">
-        <v>117</v>
-      </c>
-      <c r="G168" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="H168" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I168" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J168" s="4" t="s">
-        <v>117</v>
-      </c>
+      <c r="A168" s="10"/>
+      <c r="B168" s="10"/>
+      <c r="G168" s="40"/>
+      <c r="H168" s="10"/>
+      <c r="I168" s="10"/>
       <c r="U168" s="10"/>
-      <c r="V168" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="W168" t="s">
-        <v>117</v>
-      </c>
-      <c r="X168" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y168" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH168" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK168" t="e">
-        <f>AI168+AJ168</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AL168" t="e">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ168*AR168*AS168) * (AA168 / 5) + 441</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AM168" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="AN168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP168" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AT168" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX168" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY168" t="e">
-        <f t="shared" ref="AY168:BA168" si="56">AQ168-AU168</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ168" t="e">
-        <f t="shared" si="56"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA168" s="8" t="e">
-        <f t="shared" si="56"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BB168" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC168" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD168" t="s">
-        <v>117</v>
-      </c>
+      <c r="AT168" s="47"/>
+      <c r="AX168" s="47"/>
     </row>
     <row r="169" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="32"/>

</xml_diff>

<commit_message>
prepare train3dunet chpt-240204-0 to -2; Sun 15:52:02 04.02.2024
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CDD146-9261-4F33-B131-2F06E960789F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20A18CB-D1AA-4F11-8F1A-32AE6B46CE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4607" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4669" uniqueCount="685">
   <si>
     <t>patch z</t>
   </si>
@@ -1960,9 +1960,6 @@
   </si>
   <si>
     <t>patch = arbitrary large number &lt;= min image size - 2</t>
-  </si>
-  <si>
-    <t>autofluo eye, nuclei model type</t>
   </si>
   <si>
     <t>hyperparameter experiment invalid due to wrong 3dunet architecture (boundary) chosen for volumetric blob-like eye segmentation</t>
@@ -2072,12 +2069,93 @@
   <si>
     <t>stride = same as during the analog boundary model (240131-8)</t>
   </si>
+  <si>
+    <t>240204-0</t>
+  </si>
+  <si>
+    <t>240204-1</t>
+  </si>
+  <si>
+    <t>autofluo eye, nuclei model type, val=id07, test=06</t>
+  </si>
+  <si>
+    <t>autofluo eye, nuclei model type, val=id03, test=05</t>
+  </si>
+  <si>
+    <t>autofluo eye, nuclei model type, val=id04, test=01</t>
+  </si>
+  <si>
+    <t>expect model of equal predictive power</t>
+  </si>
+  <si>
+    <t>patch = same as for model comparison chpt-240203-5</t>
+  </si>
+  <si>
+    <t>stride = same as for model comparison chpt-240203-5</t>
+  </si>
+  <si>
+    <t>240204-2</t>
+  </si>
+  <si>
+    <t>Successful test run! I think this is the one. Proof of concept.</t>
+  </si>
+  <si>
+    <t>totally adequate model performance (tb train stats)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Exp.: autofluo eye, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nuclei model type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, val=id04, test=01</t>
+    </r>
+  </si>
+  <si>
+    <t>dataset10.b.0</t>
+  </si>
+  <si>
+    <t>dataset10.b.1</t>
+  </si>
+  <si>
+    <t>dataset10.b.2</t>
+  </si>
+  <si>
+    <t>Train the same model (as) again, with 5 LR steps for faster results (model is already overfitting at that point).</t>
+  </si>
+  <si>
+    <t>Vary validation and test sample compared to chpt-240204-0</t>
+  </si>
+  <si>
+    <t>Vary validation and test sample compared to chpt-240204-0 and chpt-240204-1</t>
+  </si>
+  <si>
+    <t>expect model of good predictive power</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2171,6 +2249,15 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2935,19 +3022,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG169"/>
+  <dimension ref="A1:BG170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AI140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F165" sqref="F165"/>
+      <selection pane="bottomRight" activeCell="BC167" sqref="BC167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
     <col min="5" max="5" width="6.5546875" customWidth="1"/>
@@ -27493,7 +27580,7 @@
         <v>1</v>
       </c>
       <c r="L153" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="U153" s="10"/>
       <c r="V153" s="17" t="s">
@@ -27628,7 +27715,7 @@
         <v>1</v>
       </c>
       <c r="L154" s="10" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="U154" s="10"/>
       <c r="V154" s="17" t="s">
@@ -28046,7 +28133,7 @@
         <v>1</v>
       </c>
       <c r="N157" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="U157" s="10"/>
       <c r="V157" s="17">
@@ -28541,7 +28628,7 @@
     </row>
     <row r="161" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="32" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B161" s="32" t="s">
         <v>519</v>
@@ -28559,13 +28646,13 @@
         <v>636</v>
       </c>
       <c r="G161" s="43" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="H161" s="32" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I161" s="32" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J161" s="34">
         <v>0</v>
@@ -28574,7 +28661,7 @@
         <v>1</v>
       </c>
       <c r="L161" s="33" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="U161" s="32"/>
       <c r="V161" s="35">
@@ -28682,7 +28769,7 @@
     </row>
     <row r="162" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="32" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B162" s="32" t="s">
         <v>519</v>
@@ -28700,13 +28787,13 @@
         <v>636</v>
       </c>
       <c r="G162" s="43" t="s">
+        <v>642</v>
+      </c>
+      <c r="H162" s="32" t="s">
         <v>643</v>
       </c>
-      <c r="H162" s="32" t="s">
-        <v>644</v>
-      </c>
       <c r="I162" s="32" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J162" s="34">
         <v>0</v>
@@ -28715,7 +28802,7 @@
         <v>1</v>
       </c>
       <c r="L162" s="33" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="U162" s="32"/>
       <c r="V162" s="35">
@@ -28812,10 +28899,10 @@
         <v>150</v>
       </c>
       <c r="BB162" s="33" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="BC162" s="33" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="BD162" s="33">
         <v>0</v>
@@ -28823,7 +28910,7 @@
     </row>
     <row r="163" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="32" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B163" s="32" t="s">
         <v>519</v>
@@ -28841,13 +28928,13 @@
         <v>636</v>
       </c>
       <c r="G163" s="43" t="s">
+        <v>642</v>
+      </c>
+      <c r="H163" s="32" t="s">
         <v>643</v>
       </c>
-      <c r="H163" s="32" t="s">
-        <v>644</v>
-      </c>
       <c r="I163" s="32" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="J163" s="34">
         <v>0</v>
@@ -28856,7 +28943,7 @@
         <v>1</v>
       </c>
       <c r="L163" s="33" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="U163" s="32"/>
       <c r="V163" s="35">
@@ -28953,10 +29040,10 @@
         <v>167</v>
       </c>
       <c r="BB163" s="33" t="s">
+        <v>646</v>
+      </c>
+      <c r="BC163" s="33" t="s">
         <v>647</v>
-      </c>
-      <c r="BC163" s="33" t="s">
-        <v>648</v>
       </c>
       <c r="BD163" s="33">
         <v>0</v>
@@ -28964,7 +29051,7 @@
     </row>
     <row r="164" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="32" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B164" s="32" t="s">
         <v>519</v>
@@ -28982,13 +29069,13 @@
         <v>636</v>
       </c>
       <c r="G164" s="43" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H164" s="32" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I164" s="32" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="J164" s="34">
         <v>0</v>
@@ -28997,7 +29084,7 @@
         <v>1</v>
       </c>
       <c r="L164" s="33" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="U164" s="32"/>
       <c r="V164" s="35">
@@ -29097,10 +29184,10 @@
         <v>178</v>
       </c>
       <c r="BB164" s="33" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="BC164" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="BD164" s="33">
         <v>0</v>
@@ -29108,7 +29195,7 @@
     </row>
     <row r="165" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="32" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B165" s="32" t="s">
         <v>519</v>
@@ -29126,13 +29213,13 @@
         <v>636</v>
       </c>
       <c r="G165" s="43" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H165" s="32" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I165" s="32" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="J165" s="34">
         <v>0</v>
@@ -29141,7 +29228,7 @@
         <v>1</v>
       </c>
       <c r="L165" s="33" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="U165" s="32"/>
       <c r="V165" s="35">
@@ -29241,10 +29328,10 @@
         <v>276</v>
       </c>
       <c r="BB165" s="33" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="BC165" s="33" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="BD165" s="33">
         <v>0</v>
@@ -29252,10 +29339,10 @@
     </row>
     <row r="166" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A166" s="68" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B166" s="68" t="s">
-        <v>640</v>
+        <v>677</v>
       </c>
       <c r="C166" s="69" t="s">
         <v>525</v>
@@ -29270,20 +29357,26 @@
         <v>636</v>
       </c>
       <c r="G166" s="40" t="s">
+        <v>662</v>
+      </c>
+      <c r="H166" s="10" t="s">
         <v>663</v>
       </c>
-      <c r="H166" s="10" t="s">
-        <v>664</v>
-      </c>
-      <c r="I166" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J166" s="4" t="s">
-        <v>117</v>
+      <c r="I166" s="32" t="s">
+        <v>675</v>
+      </c>
+      <c r="J166" s="4">
+        <v>0</v>
+      </c>
+      <c r="M166">
+        <v>1</v>
+      </c>
+      <c r="N166" t="s">
+        <v>676</v>
       </c>
       <c r="U166" s="10"/>
-      <c r="V166" s="17" t="s">
-        <v>117</v>
+      <c r="V166" s="17">
+        <v>1</v>
       </c>
       <c r="W166">
         <v>6</v>
@@ -29379,39 +29472,39 @@
         <v>233</v>
       </c>
       <c r="BB166" t="s">
+        <v>664</v>
+      </c>
+      <c r="BC166" t="s">
         <v>665</v>
-      </c>
-      <c r="BC166" t="s">
-        <v>666</v>
       </c>
       <c r="BD166" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="167" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A167" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B167" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C167" t="s">
-        <v>117</v>
-      </c>
-      <c r="D167" t="s">
-        <v>117</v>
-      </c>
-      <c r="E167" t="s">
-        <v>117</v>
-      </c>
-      <c r="F167" t="s">
-        <v>117</v>
+      <c r="A167" s="68" t="s">
+        <v>666</v>
+      </c>
+      <c r="B167" s="68" t="s">
+        <v>670</v>
+      </c>
+      <c r="C167" s="69" t="s">
+        <v>678</v>
+      </c>
+      <c r="D167" s="69" t="s">
+        <v>457</v>
+      </c>
+      <c r="E167" s="69" t="s">
+        <v>406</v>
+      </c>
+      <c r="F167" s="69" t="s">
+        <v>636</v>
       </c>
       <c r="G167" s="40" t="s">
-        <v>117</v>
+        <v>681</v>
       </c>
       <c r="H167" s="10" t="s">
-        <v>117</v>
+        <v>684</v>
       </c>
       <c r="I167" s="10" t="s">
         <v>117</v>
@@ -29423,157 +29516,518 @@
       <c r="V167" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="W167" t="s">
-        <v>117</v>
-      </c>
-      <c r="X167" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y167" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC167" t="s">
-        <v>117</v>
+      <c r="W167">
+        <v>6</v>
+      </c>
+      <c r="X167">
+        <v>5</v>
+      </c>
+      <c r="Y167">
+        <v>1</v>
+      </c>
+      <c r="Z167">
+        <v>1</v>
+      </c>
+      <c r="AA167">
+        <f t="shared" ref="AA167:AA168" si="56">X167+Y167</f>
+        <v>6</v>
+      </c>
+      <c r="AB167">
+        <v>6</v>
+      </c>
+      <c r="AC167">
+        <v>3</v>
       </c>
       <c r="AE167" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AH167" s="8" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="AI167" t="s">
         <v>117</v>
       </c>
-      <c r="AJ167" t="s">
+      <c r="AJ167" s="10" t="s">
         <v>117</v>
       </c>
       <c r="AK167" t="e">
-        <f>AI167+AJ167</f>
+        <f t="shared" ref="AK167:AK168" si="57">AI167+AJ167</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AL167" t="e">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ167*AR167*AS167) * (AA167 / 5) + 441</f>
-        <v>#VALUE!</v>
+      <c r="AL167" s="67">
+        <f t="shared" ref="AL167:AL168" si="58" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ167*AR167*AS167) * (AA167 / 5) + 441</f>
+        <v>74552.537876951479</v>
       </c>
       <c r="AM167" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AN167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP167" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS167" t="s">
-        <v>117</v>
+      <c r="AN167">
+        <v>173</v>
+      </c>
+      <c r="AO167">
+        <v>743</v>
+      </c>
+      <c r="AP167" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ167">
+        <v>133</v>
+      </c>
+      <c r="AR167">
+        <v>720</v>
+      </c>
+      <c r="AS167">
+        <v>300</v>
       </c>
       <c r="AT167" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW167" t="s">
-        <v>117</v>
+        <v>45</v>
+      </c>
+      <c r="AU167">
+        <f t="shared" ref="AU167:AU168" si="59" xml:space="preserve"> _xlfn.FLOOR.MATH((AN167 - AQ167) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV167">
+        <f t="shared" ref="AV167:AV168" si="60" xml:space="preserve"> _xlfn.FLOOR.MATH((AO167 - AR167) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW167">
+        <f t="shared" ref="AW167:AW168" si="61" xml:space="preserve"> _xlfn.FLOOR.MATH((AP167 - AS167) / 2)</f>
+        <v>67</v>
       </c>
       <c r="AX167" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY167" t="e">
+        <v>45</v>
+      </c>
+      <c r="AY167">
         <f t="shared" si="55"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AZ167" t="e">
+        <v>113</v>
+      </c>
+      <c r="AZ167">
         <f t="shared" si="55"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="BA167" s="8" t="e">
+        <v>709</v>
+      </c>
+      <c r="BA167" s="8">
         <f t="shared" si="55"/>
-        <v>#VALUE!</v>
+        <v>233</v>
       </c>
       <c r="BB167" t="s">
-        <v>117</v>
+        <v>672</v>
       </c>
       <c r="BC167" t="s">
-        <v>117</v>
+        <v>673</v>
       </c>
       <c r="BD167" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="168" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A168" s="10"/>
-      <c r="B168" s="10"/>
-      <c r="G168" s="40"/>
-      <c r="H168" s="10"/>
-      <c r="I168" s="10"/>
+      <c r="A168" s="68" t="s">
+        <v>667</v>
+      </c>
+      <c r="B168" s="68" t="s">
+        <v>668</v>
+      </c>
+      <c r="C168" s="69" t="s">
+        <v>679</v>
+      </c>
+      <c r="D168" s="69" t="s">
+        <v>457</v>
+      </c>
+      <c r="E168" s="69" t="s">
+        <v>406</v>
+      </c>
+      <c r="F168" s="69" t="s">
+        <v>636</v>
+      </c>
+      <c r="G168" s="40" t="s">
+        <v>682</v>
+      </c>
+      <c r="H168" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="I168" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J168" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="U168" s="10"/>
-      <c r="AT168" s="47"/>
-      <c r="AX168" s="47"/>
+      <c r="V168" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W168">
+        <v>6</v>
+      </c>
+      <c r="X168">
+        <v>5</v>
+      </c>
+      <c r="Y168">
+        <v>1</v>
+      </c>
+      <c r="Z168">
+        <v>1</v>
+      </c>
+      <c r="AA168">
+        <f t="shared" si="56"/>
+        <v>6</v>
+      </c>
+      <c r="AB168">
+        <v>6</v>
+      </c>
+      <c r="AC168">
+        <v>3</v>
+      </c>
+      <c r="AE168" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH168" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI168" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ168" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK168" t="e">
+        <f t="shared" si="57"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL168" s="67">
+        <f t="shared" si="58"/>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM168" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN168">
+        <v>173</v>
+      </c>
+      <c r="AO168">
+        <v>743</v>
+      </c>
+      <c r="AP168" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ168">
+        <v>133</v>
+      </c>
+      <c r="AR168">
+        <v>720</v>
+      </c>
+      <c r="AS168">
+        <v>300</v>
+      </c>
+      <c r="AT168" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU168">
+        <f t="shared" si="59"/>
+        <v>20</v>
+      </c>
+      <c r="AV168">
+        <f t="shared" si="60"/>
+        <v>11</v>
+      </c>
+      <c r="AW168">
+        <f t="shared" si="61"/>
+        <v>67</v>
+      </c>
+      <c r="AX168" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY168">
+        <f t="shared" ref="AY168" si="62">AQ168-AU168</f>
+        <v>113</v>
+      </c>
+      <c r="AZ168">
+        <f t="shared" ref="AZ168" si="63">AR168-AV168</f>
+        <v>709</v>
+      </c>
+      <c r="BA168" s="8">
+        <f t="shared" ref="BA168" si="64">AS168-AW168</f>
+        <v>233</v>
+      </c>
+      <c r="BB168" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC168" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD168" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="169" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="32"/>
-      <c r="B169" s="32"/>
-      <c r="C169"/>
-      <c r="D169"/>
-      <c r="E169"/>
-      <c r="F169"/>
-      <c r="G169" s="43"/>
-      <c r="H169" s="32"/>
-      <c r="I169" s="32"/>
-      <c r="J169" s="34"/>
-      <c r="U169" s="32"/>
-      <c r="V169" s="35"/>
-      <c r="W169"/>
-      <c r="X169"/>
-      <c r="Y169"/>
-      <c r="Z169"/>
-      <c r="AA169"/>
-      <c r="AB169"/>
-      <c r="AC169"/>
-      <c r="AD169"/>
-      <c r="AE169"/>
-      <c r="AF169"/>
-      <c r="AG169"/>
-      <c r="AH169" s="8"/>
-      <c r="AI169"/>
-      <c r="AJ169"/>
-      <c r="AK169"/>
-      <c r="AL169"/>
-      <c r="AM169" s="8"/>
-      <c r="AN169"/>
-      <c r="AO169"/>
-      <c r="AP169" s="17"/>
-      <c r="AQ169"/>
-      <c r="AR169"/>
-      <c r="AS169"/>
-      <c r="AT169" s="47"/>
-      <c r="AU169"/>
-      <c r="AV169"/>
-      <c r="AW169"/>
-      <c r="AX169" s="47"/>
-      <c r="BA169" s="36"/>
+    <row r="169" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A169" s="68" t="s">
+        <v>674</v>
+      </c>
+      <c r="B169" s="68" t="s">
+        <v>669</v>
+      </c>
+      <c r="C169" s="69" t="s">
+        <v>680</v>
+      </c>
+      <c r="D169" s="69" t="s">
+        <v>457</v>
+      </c>
+      <c r="E169" s="69" t="s">
+        <v>406</v>
+      </c>
+      <c r="F169" s="69" t="s">
+        <v>636</v>
+      </c>
+      <c r="G169" s="40" t="s">
+        <v>683</v>
+      </c>
+      <c r="H169" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="I169" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J169" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U169" s="10"/>
+      <c r="V169" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W169">
+        <v>6</v>
+      </c>
+      <c r="X169">
+        <v>5</v>
+      </c>
+      <c r="Y169">
+        <v>1</v>
+      </c>
+      <c r="Z169">
+        <v>1</v>
+      </c>
+      <c r="AA169">
+        <f t="shared" ref="AA169" si="65">X169+Y169</f>
+        <v>6</v>
+      </c>
+      <c r="AB169">
+        <v>6</v>
+      </c>
+      <c r="AC169">
+        <v>3</v>
+      </c>
+      <c r="AE169" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH169" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI169" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ169" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK169" t="e">
+        <f t="shared" ref="AK169" si="66">AI169+AJ169</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL169" s="67">
+        <f t="shared" ref="AL169" si="67" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ169*AR169*AS169) * (AA169 / 5) + 441</f>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM169" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN169">
+        <v>173</v>
+      </c>
+      <c r="AO169">
+        <v>743</v>
+      </c>
+      <c r="AP169" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ169">
+        <v>133</v>
+      </c>
+      <c r="AR169">
+        <v>720</v>
+      </c>
+      <c r="AS169">
+        <v>300</v>
+      </c>
+      <c r="AT169" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU169">
+        <f t="shared" ref="AU169" si="68" xml:space="preserve"> _xlfn.FLOOR.MATH((AN169 - AQ169) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV169">
+        <f t="shared" ref="AV169" si="69" xml:space="preserve"> _xlfn.FLOOR.MATH((AO169 - AR169) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW169">
+        <f t="shared" ref="AW169" si="70" xml:space="preserve"> _xlfn.FLOOR.MATH((AP169 - AS169) / 2)</f>
+        <v>67</v>
+      </c>
+      <c r="AX169" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY169">
+        <f t="shared" ref="AY169" si="71">AQ169-AU169</f>
+        <v>113</v>
+      </c>
+      <c r="AZ169">
+        <f t="shared" ref="AZ169" si="72">AR169-AV169</f>
+        <v>709</v>
+      </c>
+      <c r="BA169" s="8">
+        <f t="shared" ref="BA169" si="73">AS169-AW169</f>
+        <v>233</v>
+      </c>
+      <c r="BB169" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC169" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD169" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="170" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A170" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B170" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C170" t="s">
+        <v>117</v>
+      </c>
+      <c r="D170" t="s">
+        <v>117</v>
+      </c>
+      <c r="E170" t="s">
+        <v>117</v>
+      </c>
+      <c r="F170" t="s">
+        <v>117</v>
+      </c>
+      <c r="G170" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H170" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I170" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J170" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U170" s="10"/>
+      <c r="V170" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W170" t="s">
+        <v>117</v>
+      </c>
+      <c r="X170" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y170" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH170" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK170" t="e">
+        <f t="shared" ref="AK170" si="74">AI170+AJ170</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL170" t="e">
+        <f t="shared" ref="AL170" si="75" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ170*AR170*AS170) * (AA170 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM170" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP170" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT170" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW170" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX170" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY170" t="e">
+        <f t="shared" ref="AY170" si="76">AQ170-AU170</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ170" t="e">
+        <f t="shared" ref="AZ170" si="77">AR170-AV170</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA170" s="8" t="e">
+        <f t="shared" ref="BA170" si="78">AS170-AW170</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB170" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC170" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD170" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
generic commit message, Mon 08:02:43 05.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20A18CB-D1AA-4F11-8F1A-32AE6B46CE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E816C9-0C38-4C56-924C-2677B7DBA151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4669" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4809" uniqueCount="702">
   <si>
     <t>patch z</t>
   </si>
@@ -2149,6 +2149,57 @@
   </si>
   <si>
     <t>expect model of good predictive power</t>
+  </si>
+  <si>
+    <t>240205-0</t>
+  </si>
+  <si>
+    <t>240205-1</t>
+  </si>
+  <si>
+    <t>240205-2</t>
+  </si>
+  <si>
+    <t>240205-3</t>
+  </si>
+  <si>
+    <t>240205-4</t>
+  </si>
+  <si>
+    <t>240205-5</t>
+  </si>
+  <si>
+    <t>dataset10.b.3</t>
+  </si>
+  <si>
+    <t>240204-2 best, autofluo eye, nuclei model type, val=id03, test=05</t>
+  </si>
+  <si>
+    <t>240204-2 last, autofluo eye, nuclei model type, val=id03, test=05</t>
+  </si>
+  <si>
+    <t>240204-0 best, autofluo eye, nuclei model type, val=id04, test=01</t>
+  </si>
+  <si>
+    <t>240204-1 best, autofluo eye, nuclei model type, val=id07, test=06</t>
+  </si>
+  <si>
+    <t>240204-0 last, autofluo eye, nuclei model type, val=id04, test=01</t>
+  </si>
+  <si>
+    <t>240204-1 last, autofluo eye, nuclei model type, val=id07, test=06</t>
+  </si>
+  <si>
+    <t>240205-6</t>
+  </si>
+  <si>
+    <t>240205-7</t>
+  </si>
+  <si>
+    <t>240204-3 last, autofluo eye, nuclei model type, val=id02, test=07</t>
+  </si>
+  <si>
+    <t>240204-3 best, autofluo eye, nuclei model type, val=id02, test=07</t>
   </si>
 </sst>
 </file>
@@ -3022,19 +3073,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG170"/>
+  <dimension ref="A1:BG178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AI140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B153" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BC167" sqref="BC167"/>
+      <selection pane="bottomRight" activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="2" max="2" width="102.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
     <col min="5" max="5" width="6.5546875" customWidth="1"/>
@@ -29509,12 +29560,12 @@
       <c r="I167" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J167" s="4" t="s">
-        <v>117</v>
+      <c r="J167" s="4">
+        <v>1</v>
       </c>
       <c r="U167" s="10"/>
-      <c r="V167" s="17" t="s">
-        <v>117</v>
+      <c r="V167" s="17">
+        <v>1</v>
       </c>
       <c r="W167">
         <v>6</v>
@@ -29544,15 +29595,15 @@
       <c r="AH167" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AI167" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ167" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK167" t="e">
+      <c r="AI167">
+        <v>78075</v>
+      </c>
+      <c r="AJ167" s="10">
+        <v>2977</v>
+      </c>
+      <c r="AK167">
         <f t="shared" ref="AK167:AK168" si="57">AI167+AJ167</f>
-        <v>#VALUE!</v>
+        <v>81052</v>
       </c>
       <c r="AL167" s="67">
         <f t="shared" ref="AL167:AL168" si="58" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ167*AR167*AS167) * (AA167 / 5) + 441</f>
@@ -29647,12 +29698,12 @@
       <c r="I168" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J168" s="4" t="s">
-        <v>117</v>
+      <c r="J168" s="4">
+        <v>1</v>
       </c>
       <c r="U168" s="10"/>
-      <c r="V168" s="17" t="s">
-        <v>117</v>
+      <c r="V168" s="17">
+        <v>1</v>
       </c>
       <c r="W168">
         <v>6</v>
@@ -29682,15 +29733,15 @@
       <c r="AH168" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AI168" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ168" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK168" t="e">
+      <c r="AI168">
+        <v>78075</v>
+      </c>
+      <c r="AJ168" s="10">
+        <v>2977</v>
+      </c>
+      <c r="AK168">
         <f t="shared" si="57"/>
-        <v>#VALUE!</v>
+        <v>81052</v>
       </c>
       <c r="AL168" s="67">
         <f t="shared" si="58"/>
@@ -29785,12 +29836,12 @@
       <c r="I169" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J169" s="4" t="s">
-        <v>117</v>
+      <c r="J169" s="4">
+        <v>1</v>
       </c>
       <c r="U169" s="10"/>
-      <c r="V169" s="17" t="s">
-        <v>117</v>
+      <c r="V169" s="17">
+        <v>1</v>
       </c>
       <c r="W169">
         <v>6</v>
@@ -29820,15 +29871,15 @@
       <c r="AH169" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AI169" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ169" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK169" t="e">
+      <c r="AI169">
+        <v>78075</v>
+      </c>
+      <c r="AJ169" s="10">
+        <v>2977</v>
+      </c>
+      <c r="AK169">
         <f t="shared" ref="AK169" si="66">AI169+AJ169</f>
-        <v>#VALUE!</v>
+        <v>81052</v>
       </c>
       <c r="AL169" s="67">
         <f t="shared" ref="AL169" si="67" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ169*AR169*AS169) * (AA169 / 5) + 441</f>
@@ -29897,22 +29948,22 @@
     </row>
     <row r="170" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A170" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B170" s="10" t="s">
-        <v>117</v>
+        <v>685</v>
+      </c>
+      <c r="B170" t="s">
+        <v>694</v>
       </c>
       <c r="C170" t="s">
-        <v>117</v>
+        <v>678</v>
       </c>
       <c r="D170" t="s">
-        <v>117</v>
+        <v>477</v>
       </c>
       <c r="E170" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="F170" t="s">
-        <v>117</v>
+        <v>636</v>
       </c>
       <c r="G170" s="40" t="s">
         <v>117</v>
@@ -29930,102 +29981,1166 @@
       <c r="V170" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="W170" t="s">
-        <v>117</v>
-      </c>
-      <c r="X170" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y170" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC170" t="s">
-        <v>117</v>
+      <c r="W170">
+        <v>1</v>
+      </c>
+      <c r="X170">
+        <v>5</v>
+      </c>
+      <c r="Y170">
+        <v>1</v>
+      </c>
+      <c r="Z170">
+        <v>1</v>
+      </c>
+      <c r="AA170">
+        <f t="shared" ref="AA170" si="74">X170+Y170</f>
+        <v>6</v>
+      </c>
+      <c r="AB170">
+        <v>6</v>
+      </c>
+      <c r="AC170">
+        <v>3</v>
       </c>
       <c r="AE170" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AH170" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK170" t="e">
-        <f t="shared" ref="AK170" si="74">AI170+AJ170</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AL170" t="e">
-        <f t="shared" ref="AL170" si="75" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ170*AR170*AS170) * (AA170 / 5) + 441</f>
-        <v>#VALUE!</v>
+        <v>96</v>
+      </c>
+      <c r="AJ170" s="10"/>
+      <c r="AK170">
+        <f t="shared" ref="AK170" si="75">AI170+AJ170</f>
+        <v>0</v>
+      </c>
+      <c r="AL170" s="67">
+        <f t="shared" ref="AL170" si="76" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ170*AR170*AS170) * (AA170 / 5) + 441</f>
+        <v>74552.537876951479</v>
       </c>
       <c r="AM170" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AN170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP170" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS170" t="s">
-        <v>117</v>
+      <c r="AN170">
+        <v>173</v>
+      </c>
+      <c r="AO170">
+        <v>743</v>
+      </c>
+      <c r="AP170" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ170">
+        <v>133</v>
+      </c>
+      <c r="AR170">
+        <v>720</v>
+      </c>
+      <c r="AS170">
+        <v>300</v>
       </c>
       <c r="AT170" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="AU170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV170" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW170" t="s">
-        <v>117</v>
+      <c r="AU170">
+        <f t="shared" ref="AU170" si="77" xml:space="preserve"> _xlfn.FLOOR.MATH((AN170 - AQ170) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV170">
+        <f t="shared" ref="AV170" si="78" xml:space="preserve"> _xlfn.FLOOR.MATH((AO170 - AR170) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW170">
+        <f t="shared" ref="AW170" si="79" xml:space="preserve"> _xlfn.FLOOR.MATH((AP170 - AS170) / 2)</f>
+        <v>67</v>
       </c>
       <c r="AX170" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="AY170" t="e">
-        <f t="shared" ref="AY170" si="76">AQ170-AU170</f>
+      <c r="AY170">
+        <f t="shared" ref="AY170" si="80">AQ170-AU170</f>
+        <v>113</v>
+      </c>
+      <c r="AZ170">
+        <f t="shared" ref="AZ170" si="81">AR170-AV170</f>
+        <v>709</v>
+      </c>
+      <c r="BA170" s="8">
+        <f t="shared" ref="BA170" si="82">AS170-AW170</f>
+        <v>233</v>
+      </c>
+      <c r="BB170" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC170" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD170" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="171" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A171" s="10" t="s">
+        <v>686</v>
+      </c>
+      <c r="B171" t="s">
+        <v>695</v>
+      </c>
+      <c r="C171" t="s">
+        <v>679</v>
+      </c>
+      <c r="D171" t="s">
+        <v>477</v>
+      </c>
+      <c r="E171" t="s">
+        <v>406</v>
+      </c>
+      <c r="F171" t="s">
+        <v>636</v>
+      </c>
+      <c r="G171" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H171" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I171" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J171" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U171" s="10"/>
+      <c r="V171" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W171">
+        <v>1</v>
+      </c>
+      <c r="X171">
+        <v>5</v>
+      </c>
+      <c r="Y171">
+        <v>1</v>
+      </c>
+      <c r="Z171">
+        <v>1</v>
+      </c>
+      <c r="AA171">
+        <f t="shared" ref="AA171:AA175" si="83">X171+Y171</f>
+        <v>6</v>
+      </c>
+      <c r="AB171">
+        <v>6</v>
+      </c>
+      <c r="AC171">
+        <v>3</v>
+      </c>
+      <c r="AE171" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH171" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ171" s="10"/>
+      <c r="AK171">
+        <f t="shared" ref="AK171:AK175" si="84">AI171+AJ171</f>
+        <v>0</v>
+      </c>
+      <c r="AL171" s="67">
+        <f t="shared" ref="AL171:AL175" si="85" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ171*AR171*AS171) * (AA171 / 5) + 441</f>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM171" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN171">
+        <v>173</v>
+      </c>
+      <c r="AO171">
+        <v>743</v>
+      </c>
+      <c r="AP171" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ171">
+        <v>133</v>
+      </c>
+      <c r="AR171">
+        <v>720</v>
+      </c>
+      <c r="AS171">
+        <v>300</v>
+      </c>
+      <c r="AT171" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU171">
+        <f t="shared" ref="AU171:AU175" si="86" xml:space="preserve"> _xlfn.FLOOR.MATH((AN171 - AQ171) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV171">
+        <f t="shared" ref="AV171:AV175" si="87" xml:space="preserve"> _xlfn.FLOOR.MATH((AO171 - AR171) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW171">
+        <f t="shared" ref="AW171:AW175" si="88" xml:space="preserve"> _xlfn.FLOOR.MATH((AP171 - AS171) / 2)</f>
+        <v>67</v>
+      </c>
+      <c r="AX171" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY171">
+        <f t="shared" ref="AY171:AY175" si="89">AQ171-AU171</f>
+        <v>113</v>
+      </c>
+      <c r="AZ171">
+        <f t="shared" ref="AZ171:AZ175" si="90">AR171-AV171</f>
+        <v>709</v>
+      </c>
+      <c r="BA171" s="8">
+        <f t="shared" ref="BA171:BA175" si="91">AS171-AW171</f>
+        <v>233</v>
+      </c>
+      <c r="BB171" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC171" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD171" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="172" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A172" s="10" t="s">
+        <v>687</v>
+      </c>
+      <c r="B172" t="s">
+        <v>692</v>
+      </c>
+      <c r="C172" t="s">
+        <v>680</v>
+      </c>
+      <c r="D172" t="s">
+        <v>477</v>
+      </c>
+      <c r="E172" t="s">
+        <v>406</v>
+      </c>
+      <c r="F172" t="s">
+        <v>636</v>
+      </c>
+      <c r="G172" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H172" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I172" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J172" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U172" s="10"/>
+      <c r="V172" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W172">
+        <v>1</v>
+      </c>
+      <c r="X172">
+        <v>5</v>
+      </c>
+      <c r="Y172">
+        <v>1</v>
+      </c>
+      <c r="Z172">
+        <v>1</v>
+      </c>
+      <c r="AA172">
+        <f t="shared" si="83"/>
+        <v>6</v>
+      </c>
+      <c r="AB172">
+        <v>6</v>
+      </c>
+      <c r="AC172">
+        <v>3</v>
+      </c>
+      <c r="AE172" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH172" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ172" s="10"/>
+      <c r="AK172">
+        <f t="shared" si="84"/>
+        <v>0</v>
+      </c>
+      <c r="AL172" s="67">
+        <f t="shared" si="85"/>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM172" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN172">
+        <v>173</v>
+      </c>
+      <c r="AO172">
+        <v>743</v>
+      </c>
+      <c r="AP172" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ172">
+        <v>133</v>
+      </c>
+      <c r="AR172">
+        <v>720</v>
+      </c>
+      <c r="AS172">
+        <v>300</v>
+      </c>
+      <c r="AT172" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU172">
+        <f t="shared" si="86"/>
+        <v>20</v>
+      </c>
+      <c r="AV172">
+        <f t="shared" si="87"/>
+        <v>11</v>
+      </c>
+      <c r="AW172">
+        <f t="shared" si="88"/>
+        <v>67</v>
+      </c>
+      <c r="AX172" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY172">
+        <f t="shared" si="89"/>
+        <v>113</v>
+      </c>
+      <c r="AZ172">
+        <f t="shared" si="90"/>
+        <v>709</v>
+      </c>
+      <c r="BA172" s="8">
+        <f t="shared" si="91"/>
+        <v>233</v>
+      </c>
+      <c r="BB172" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC172" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD172" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="173" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A173" s="10" t="s">
+        <v>688</v>
+      </c>
+      <c r="B173" t="s">
+        <v>701</v>
+      </c>
+      <c r="C173" t="s">
+        <v>691</v>
+      </c>
+      <c r="D173" t="s">
+        <v>477</v>
+      </c>
+      <c r="E173" t="s">
+        <v>406</v>
+      </c>
+      <c r="F173" t="s">
+        <v>636</v>
+      </c>
+      <c r="G173" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H173" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I173" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J173" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U173" s="10"/>
+      <c r="V173" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W173">
+        <v>1</v>
+      </c>
+      <c r="X173">
+        <v>5</v>
+      </c>
+      <c r="Y173">
+        <v>1</v>
+      </c>
+      <c r="Z173">
+        <v>1</v>
+      </c>
+      <c r="AA173">
+        <f t="shared" ref="AA173" si="92">X173+Y173</f>
+        <v>6</v>
+      </c>
+      <c r="AB173">
+        <v>6</v>
+      </c>
+      <c r="AC173">
+        <v>3</v>
+      </c>
+      <c r="AE173" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH173" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ173" s="10"/>
+      <c r="AK173">
+        <f t="shared" ref="AK173" si="93">AI173+AJ173</f>
+        <v>0</v>
+      </c>
+      <c r="AL173" s="67">
+        <f t="shared" ref="AL173" si="94" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ173*AR173*AS173) * (AA173 / 5) + 441</f>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM173" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN173">
+        <v>173</v>
+      </c>
+      <c r="AO173">
+        <v>743</v>
+      </c>
+      <c r="AP173" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ173">
+        <v>133</v>
+      </c>
+      <c r="AR173">
+        <v>720</v>
+      </c>
+      <c r="AS173">
+        <v>300</v>
+      </c>
+      <c r="AT173" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU173">
+        <f t="shared" ref="AU173" si="95" xml:space="preserve"> _xlfn.FLOOR.MATH((AN173 - AQ173) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV173">
+        <f t="shared" ref="AV173" si="96" xml:space="preserve"> _xlfn.FLOOR.MATH((AO173 - AR173) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW173">
+        <f t="shared" ref="AW173" si="97" xml:space="preserve"> _xlfn.FLOOR.MATH((AP173 - AS173) / 2)</f>
+        <v>67</v>
+      </c>
+      <c r="AX173" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY173">
+        <f t="shared" ref="AY173" si="98">AQ173-AU173</f>
+        <v>113</v>
+      </c>
+      <c r="AZ173">
+        <f t="shared" ref="AZ173" si="99">AR173-AV173</f>
+        <v>709</v>
+      </c>
+      <c r="BA173" s="8">
+        <f t="shared" ref="BA173" si="100">AS173-AW173</f>
+        <v>233</v>
+      </c>
+      <c r="BB173" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC173" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD173" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="174" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A174" s="10" t="s">
+        <v>689</v>
+      </c>
+      <c r="B174" t="s">
+        <v>696</v>
+      </c>
+      <c r="C174" t="s">
+        <v>678</v>
+      </c>
+      <c r="D174" t="s">
+        <v>477</v>
+      </c>
+      <c r="E174" t="s">
+        <v>406</v>
+      </c>
+      <c r="F174" t="s">
+        <v>636</v>
+      </c>
+      <c r="G174" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H174" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I174" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J174" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U174" s="10"/>
+      <c r="V174" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W174">
+        <v>1</v>
+      </c>
+      <c r="X174">
+        <v>5</v>
+      </c>
+      <c r="Y174">
+        <v>1</v>
+      </c>
+      <c r="Z174">
+        <v>1</v>
+      </c>
+      <c r="AA174">
+        <f>X174+Y174</f>
+        <v>6</v>
+      </c>
+      <c r="AB174">
+        <v>6</v>
+      </c>
+      <c r="AC174">
+        <v>3</v>
+      </c>
+      <c r="AE174" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH174" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ174" s="10"/>
+      <c r="AK174">
+        <f>AI174+AJ174</f>
+        <v>0</v>
+      </c>
+      <c r="AL174" s="67">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ174*AR174*AS174) * (AA174 / 5) + 441</f>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM174" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN174">
+        <v>173</v>
+      </c>
+      <c r="AO174">
+        <v>743</v>
+      </c>
+      <c r="AP174" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ174">
+        <v>133</v>
+      </c>
+      <c r="AR174">
+        <v>720</v>
+      </c>
+      <c r="AS174">
+        <v>300</v>
+      </c>
+      <c r="AT174" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU174">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN174 - AQ174) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV174">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO174 - AR174) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW174">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP174 - AS174) / 2)</f>
+        <v>67</v>
+      </c>
+      <c r="AX174" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY174">
+        <f>AQ174-AU174</f>
+        <v>113</v>
+      </c>
+      <c r="AZ174">
+        <f>AR174-AV174</f>
+        <v>709</v>
+      </c>
+      <c r="BA174" s="8">
+        <f>AS174-AW174</f>
+        <v>233</v>
+      </c>
+      <c r="BB174" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC174" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD174" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="175" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A175" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="B175" t="s">
+        <v>697</v>
+      </c>
+      <c r="C175" t="s">
+        <v>679</v>
+      </c>
+      <c r="D175" t="s">
+        <v>477</v>
+      </c>
+      <c r="E175" t="s">
+        <v>406</v>
+      </c>
+      <c r="F175" t="s">
+        <v>636</v>
+      </c>
+      <c r="G175" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H175" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I175" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J175" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U175" s="10"/>
+      <c r="V175" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W175">
+        <v>1</v>
+      </c>
+      <c r="X175">
+        <v>5</v>
+      </c>
+      <c r="Y175">
+        <v>1</v>
+      </c>
+      <c r="Z175">
+        <v>1</v>
+      </c>
+      <c r="AA175">
+        <f>X175+Y175</f>
+        <v>6</v>
+      </c>
+      <c r="AB175">
+        <v>6</v>
+      </c>
+      <c r="AC175">
+        <v>3</v>
+      </c>
+      <c r="AE175" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH175" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ175" s="10"/>
+      <c r="AK175">
+        <f>AI175+AJ175</f>
+        <v>0</v>
+      </c>
+      <c r="AL175" s="67">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ175*AR175*AS175) * (AA175 / 5) + 441</f>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM175" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN175">
+        <v>173</v>
+      </c>
+      <c r="AO175">
+        <v>743</v>
+      </c>
+      <c r="AP175" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ175">
+        <v>133</v>
+      </c>
+      <c r="AR175">
+        <v>720</v>
+      </c>
+      <c r="AS175">
+        <v>300</v>
+      </c>
+      <c r="AT175" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU175">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN175 - AQ175) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV175">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO175 - AR175) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW175">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP175 - AS175) / 2)</f>
+        <v>67</v>
+      </c>
+      <c r="AX175" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY175">
+        <f>AQ175-AU175</f>
+        <v>113</v>
+      </c>
+      <c r="AZ175">
+        <f>AR175-AV175</f>
+        <v>709</v>
+      </c>
+      <c r="BA175" s="8">
+        <f>AS175-AW175</f>
+        <v>233</v>
+      </c>
+      <c r="BB175" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC175" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD175" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="176" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A176" s="10" t="s">
+        <v>698</v>
+      </c>
+      <c r="B176" t="s">
+        <v>693</v>
+      </c>
+      <c r="C176" t="s">
+        <v>680</v>
+      </c>
+      <c r="D176" t="s">
+        <v>477</v>
+      </c>
+      <c r="E176" t="s">
+        <v>406</v>
+      </c>
+      <c r="F176" t="s">
+        <v>636</v>
+      </c>
+      <c r="G176" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H176" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I176" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J176" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U176" s="10"/>
+      <c r="V176" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W176">
+        <v>1</v>
+      </c>
+      <c r="X176">
+        <v>5</v>
+      </c>
+      <c r="Y176">
+        <v>1</v>
+      </c>
+      <c r="Z176">
+        <v>1</v>
+      </c>
+      <c r="AA176">
+        <f>X176+Y176</f>
+        <v>6</v>
+      </c>
+      <c r="AB176">
+        <v>6</v>
+      </c>
+      <c r="AC176">
+        <v>3</v>
+      </c>
+      <c r="AE176" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH176" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ176" s="10"/>
+      <c r="AK176">
+        <f>AI176+AJ176</f>
+        <v>0</v>
+      </c>
+      <c r="AL176" s="67">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ176*AR176*AS176) * (AA176 / 5) + 441</f>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM176" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN176">
+        <v>173</v>
+      </c>
+      <c r="AO176">
+        <v>743</v>
+      </c>
+      <c r="AP176" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ176">
+        <v>133</v>
+      </c>
+      <c r="AR176">
+        <v>720</v>
+      </c>
+      <c r="AS176">
+        <v>300</v>
+      </c>
+      <c r="AT176" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU176">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN176 - AQ176) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV176">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO176 - AR176) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW176">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP176 - AS176) / 2)</f>
+        <v>67</v>
+      </c>
+      <c r="AX176" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY176">
+        <f>AQ176-AU176</f>
+        <v>113</v>
+      </c>
+      <c r="AZ176">
+        <f>AR176-AV176</f>
+        <v>709</v>
+      </c>
+      <c r="BA176" s="8">
+        <f>AS176-AW176</f>
+        <v>233</v>
+      </c>
+      <c r="BB176" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC176" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD176" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="177" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A177" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="B177" t="s">
+        <v>700</v>
+      </c>
+      <c r="C177" t="s">
+        <v>691</v>
+      </c>
+      <c r="D177" t="s">
+        <v>477</v>
+      </c>
+      <c r="E177" t="s">
+        <v>406</v>
+      </c>
+      <c r="F177" t="s">
+        <v>636</v>
+      </c>
+      <c r="G177" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H177" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I177" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J177" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U177" s="10"/>
+      <c r="V177" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W177">
+        <v>1</v>
+      </c>
+      <c r="X177">
+        <v>5</v>
+      </c>
+      <c r="Y177">
+        <v>1</v>
+      </c>
+      <c r="Z177">
+        <v>1</v>
+      </c>
+      <c r="AA177">
+        <f>X177+Y177</f>
+        <v>6</v>
+      </c>
+      <c r="AB177">
+        <v>6</v>
+      </c>
+      <c r="AC177">
+        <v>3</v>
+      </c>
+      <c r="AE177" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH177" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ177" s="10"/>
+      <c r="AK177">
+        <f>AI177+AJ177</f>
+        <v>0</v>
+      </c>
+      <c r="AL177" s="67">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ177*AR177*AS177) * (AA177 / 5) + 441</f>
+        <v>74552.537876951479</v>
+      </c>
+      <c r="AM177" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN177">
+        <v>173</v>
+      </c>
+      <c r="AO177">
+        <v>743</v>
+      </c>
+      <c r="AP177" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ177">
+        <v>133</v>
+      </c>
+      <c r="AR177">
+        <v>720</v>
+      </c>
+      <c r="AS177">
+        <v>300</v>
+      </c>
+      <c r="AT177" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU177">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN177 - AQ177) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV177">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO177 - AR177) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW177">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP177 - AS177) / 2)</f>
+        <v>67</v>
+      </c>
+      <c r="AX177" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY177">
+        <f>AQ177-AU177</f>
+        <v>113</v>
+      </c>
+      <c r="AZ177">
+        <f>AR177-AV177</f>
+        <v>709</v>
+      </c>
+      <c r="BA177" s="8">
+        <f>AS177-AW177</f>
+        <v>233</v>
+      </c>
+      <c r="BB177" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC177" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD177" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="178" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A178" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B178" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C178" t="s">
+        <v>117</v>
+      </c>
+      <c r="D178" t="s">
+        <v>117</v>
+      </c>
+      <c r="E178" t="s">
+        <v>117</v>
+      </c>
+      <c r="F178" t="s">
+        <v>117</v>
+      </c>
+      <c r="G178" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H178" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I178" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J178" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U178" s="10"/>
+      <c r="V178" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W178" t="s">
+        <v>117</v>
+      </c>
+      <c r="X178" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y178" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH178" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK178" t="e">
+        <f t="shared" ref="AK177:AK178" si="101">AI178+AJ178</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ170" t="e">
-        <f t="shared" ref="AZ170" si="77">AR170-AV170</f>
+      <c r="AL178" t="e">
+        <f t="shared" ref="AL177:AL178" si="102" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ178*AR178*AS178) * (AA178 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA170" s="8" t="e">
-        <f t="shared" ref="BA170" si="78">AS170-AW170</f>
+      <c r="AM178" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP178" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT178" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW178" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX178" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY178" t="e">
+        <f t="shared" ref="AY177:AY178" si="103">AQ178-AU178</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB170" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC170" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD170" t="s">
+      <c r="AZ178" t="e">
+        <f t="shared" ref="AZ177:AZ178" si="104">AR178-AV178</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA178" s="8" t="e">
+        <f t="shared" ref="BA177:BA178" si="105">AS178-AW178</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB178" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC178" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD178" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generic commit message, Mon 08:24:25 05.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E816C9-0C38-4C56-924C-2677B7DBA151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D004188-A03C-434E-A7BB-DD0F7F75A369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4809" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4820" uniqueCount="705">
   <si>
     <t>patch z</t>
   </si>
@@ -2200,6 +2200,15 @@
   </si>
   <si>
     <t>240204-3 best, autofluo eye, nuclei model type, val=id02, test=07</t>
+  </si>
+  <si>
+    <t>240204-3</t>
+  </si>
+  <si>
+    <t>autofluo eye, nuclei model type, val=id02(?), test=07</t>
+  </si>
+  <si>
+    <t>Vary validation and test sample compared to chpt-240204-0, chpt-240204-1 and chpt-240204-2</t>
   </si>
 </sst>
 </file>
@@ -3073,13 +3082,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG178"/>
+  <dimension ref="A1:BG179"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B153" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J154" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B170" sqref="B170"/>
+      <selection pane="bottomRight" activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -29528,8 +29537,8 @@
       <c r="BC166" t="s">
         <v>665</v>
       </c>
-      <c r="BD166" t="s">
-        <v>117</v>
+      <c r="BD166">
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:56" x14ac:dyDescent="0.3">
@@ -29666,8 +29675,8 @@
       <c r="BC167" t="s">
         <v>673</v>
       </c>
-      <c r="BD167" t="s">
-        <v>117</v>
+      <c r="BD167">
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:56" x14ac:dyDescent="0.3">
@@ -29804,8 +29813,8 @@
       <c r="BC168" t="s">
         <v>673</v>
       </c>
-      <c r="BD168" t="s">
-        <v>117</v>
+      <c r="BD168">
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:56" x14ac:dyDescent="0.3">
@@ -29856,7 +29865,7 @@
         <v>1</v>
       </c>
       <c r="AA169">
-        <f t="shared" ref="AA169" si="65">X169+Y169</f>
+        <f t="shared" ref="AA169:AA170" si="65">X169+Y169</f>
         <v>6</v>
       </c>
       <c r="AB169">
@@ -29878,11 +29887,11 @@
         <v>2977</v>
       </c>
       <c r="AK169">
-        <f t="shared" ref="AK169" si="66">AI169+AJ169</f>
+        <f t="shared" ref="AK169:AK170" si="66">AI169+AJ169</f>
         <v>81052</v>
       </c>
       <c r="AL169" s="67">
-        <f t="shared" ref="AL169" si="67" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ169*AR169*AS169) * (AA169 / 5) + 441</f>
+        <f t="shared" ref="AL169:AL170" si="67" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ169*AR169*AS169) * (AA169 / 5) + 441</f>
         <v>74552.537876951479</v>
       </c>
       <c r="AM169" s="8" t="s">
@@ -29910,15 +29919,15 @@
         <v>45</v>
       </c>
       <c r="AU169">
-        <f t="shared" ref="AU169" si="68" xml:space="preserve"> _xlfn.FLOOR.MATH((AN169 - AQ169) / 2)</f>
+        <f t="shared" ref="AU169:AU170" si="68" xml:space="preserve"> _xlfn.FLOOR.MATH((AN169 - AQ169) / 2)</f>
         <v>20</v>
       </c>
       <c r="AV169">
-        <f t="shared" ref="AV169" si="69" xml:space="preserve"> _xlfn.FLOOR.MATH((AO169 - AR169) / 2)</f>
+        <f t="shared" ref="AV169:AV170" si="69" xml:space="preserve"> _xlfn.FLOOR.MATH((AO169 - AR169) / 2)</f>
         <v>11</v>
       </c>
       <c r="AW169">
-        <f t="shared" ref="AW169" si="70" xml:space="preserve"> _xlfn.FLOOR.MATH((AP169 - AS169) / 2)</f>
+        <f t="shared" ref="AW169:AW170" si="70" xml:space="preserve"> _xlfn.FLOOR.MATH((AP169 - AS169) / 2)</f>
         <v>67</v>
       </c>
       <c r="AX169" s="47" t="s">
@@ -29942,47 +29951,46 @@
       <c r="BC169" t="s">
         <v>673</v>
       </c>
-      <c r="BD169" t="s">
-        <v>117</v>
+      <c r="BD169">
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A170" s="10" t="s">
-        <v>685</v>
-      </c>
-      <c r="B170" t="s">
-        <v>694</v>
-      </c>
-      <c r="C170" t="s">
-        <v>678</v>
-      </c>
-      <c r="D170" t="s">
-        <v>477</v>
-      </c>
-      <c r="E170" t="s">
+      <c r="A170" s="68" t="s">
+        <v>702</v>
+      </c>
+      <c r="B170" s="68" t="s">
+        <v>703</v>
+      </c>
+      <c r="C170" s="69" t="s">
+        <v>691</v>
+      </c>
+      <c r="D170" s="69" t="s">
+        <v>457</v>
+      </c>
+      <c r="E170" s="69" t="s">
         <v>406</v>
       </c>
-      <c r="F170" t="s">
+      <c r="F170" s="69" t="s">
         <v>636</v>
       </c>
       <c r="G170" s="40" t="s">
-        <v>117</v>
+        <v>704</v>
       </c>
       <c r="H170" s="10" t="s">
-        <v>117</v>
+        <v>671</v>
       </c>
       <c r="I170" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J170" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="U170" s="10"/>
-      <c r="V170" s="17" t="s">
-        <v>117</v>
+      <c r="J170" s="4">
+        <v>1</v>
+      </c>
+      <c r="V170" s="17">
+        <v>1</v>
       </c>
       <c r="W170">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="X170">
         <v>5</v>
@@ -29994,7 +30002,7 @@
         <v>1</v>
       </c>
       <c r="AA170">
-        <f t="shared" ref="AA170" si="74">X170+Y170</f>
+        <f t="shared" si="65"/>
         <v>6</v>
       </c>
       <c r="AB170">
@@ -30009,17 +30017,19 @@
       <c r="AH170" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="AJ170" s="10"/>
+      <c r="AI170">
+        <v>78075</v>
+      </c>
+      <c r="AJ170" s="10">
+        <v>2977</v>
+      </c>
       <c r="AK170">
-        <f t="shared" ref="AK170" si="75">AI170+AJ170</f>
-        <v>0</v>
+        <f t="shared" si="66"/>
+        <v>81052</v>
       </c>
       <c r="AL170" s="67">
-        <f t="shared" ref="AL170" si="76" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ170*AR170*AS170) * (AA170 / 5) + 441</f>
+        <f t="shared" si="67"/>
         <v>74552.537876951479</v>
-      </c>
-      <c r="AM170" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="AN170">
         <v>173</v>
@@ -30040,34 +30050,22 @@
         <v>300</v>
       </c>
       <c r="AT170" s="47" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="AU170">
-        <f t="shared" ref="AU170" si="77" xml:space="preserve"> _xlfn.FLOOR.MATH((AN170 - AQ170) / 2)</f>
+        <f t="shared" si="68"/>
         <v>20</v>
       </c>
       <c r="AV170">
-        <f t="shared" ref="AV170" si="78" xml:space="preserve"> _xlfn.FLOOR.MATH((AO170 - AR170) / 2)</f>
+        <f t="shared" si="69"/>
         <v>11</v>
       </c>
       <c r="AW170">
-        <f t="shared" ref="AW170" si="79" xml:space="preserve"> _xlfn.FLOOR.MATH((AP170 - AS170) / 2)</f>
+        <f t="shared" si="70"/>
         <v>67</v>
       </c>
       <c r="AX170" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY170">
-        <f t="shared" ref="AY170" si="80">AQ170-AU170</f>
-        <v>113</v>
-      </c>
-      <c r="AZ170">
-        <f t="shared" ref="AZ170" si="81">AR170-AV170</f>
-        <v>709</v>
-      </c>
-      <c r="BA170" s="8">
-        <f t="shared" ref="BA170" si="82">AS170-AW170</f>
-        <v>233</v>
+        <v>45</v>
       </c>
       <c r="BB170" t="s">
         <v>672</v>
@@ -30075,19 +30073,19 @@
       <c r="BC170" t="s">
         <v>673</v>
       </c>
-      <c r="BD170" t="s">
-        <v>117</v>
+      <c r="BD170">
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A171" s="10" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B171" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C171" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D171" t="s">
         <v>477</v>
@@ -30127,7 +30125,7 @@
         <v>1</v>
       </c>
       <c r="AA171">
-        <f t="shared" ref="AA171:AA175" si="83">X171+Y171</f>
+        <f t="shared" ref="AA171" si="74">X171+Y171</f>
         <v>6</v>
       </c>
       <c r="AB171">
@@ -30144,11 +30142,11 @@
       </c>
       <c r="AJ171" s="10"/>
       <c r="AK171">
-        <f t="shared" ref="AK171:AK175" si="84">AI171+AJ171</f>
+        <f t="shared" ref="AK171" si="75">AI171+AJ171</f>
         <v>0</v>
       </c>
       <c r="AL171" s="67">
-        <f t="shared" ref="AL171:AL175" si="85" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ171*AR171*AS171) * (AA171 / 5) + 441</f>
+        <f t="shared" ref="AL171" si="76" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ171*AR171*AS171) * (AA171 / 5) + 441</f>
         <v>74552.537876951479</v>
       </c>
       <c r="AM171" s="8" t="s">
@@ -30176,30 +30174,30 @@
         <v>8</v>
       </c>
       <c r="AU171">
-        <f t="shared" ref="AU171:AU175" si="86" xml:space="preserve"> _xlfn.FLOOR.MATH((AN171 - AQ171) / 2)</f>
+        <f t="shared" ref="AU171" si="77" xml:space="preserve"> _xlfn.FLOOR.MATH((AN171 - AQ171) / 2)</f>
         <v>20</v>
       </c>
       <c r="AV171">
-        <f t="shared" ref="AV171:AV175" si="87" xml:space="preserve"> _xlfn.FLOOR.MATH((AO171 - AR171) / 2)</f>
+        <f t="shared" ref="AV171" si="78" xml:space="preserve"> _xlfn.FLOOR.MATH((AO171 - AR171) / 2)</f>
         <v>11</v>
       </c>
       <c r="AW171">
-        <f t="shared" ref="AW171:AW175" si="88" xml:space="preserve"> _xlfn.FLOOR.MATH((AP171 - AS171) / 2)</f>
+        <f t="shared" ref="AW171" si="79" xml:space="preserve"> _xlfn.FLOOR.MATH((AP171 - AS171) / 2)</f>
         <v>67</v>
       </c>
       <c r="AX171" s="47" t="s">
         <v>8</v>
       </c>
       <c r="AY171">
-        <f t="shared" ref="AY171:AY175" si="89">AQ171-AU171</f>
+        <f t="shared" ref="AY171" si="80">AQ171-AU171</f>
         <v>113</v>
       </c>
       <c r="AZ171">
-        <f t="shared" ref="AZ171:AZ175" si="90">AR171-AV171</f>
+        <f t="shared" ref="AZ171" si="81">AR171-AV171</f>
         <v>709</v>
       </c>
       <c r="BA171" s="8">
-        <f t="shared" ref="BA171:BA175" si="91">AS171-AW171</f>
+        <f t="shared" ref="BA171" si="82">AS171-AW171</f>
         <v>233</v>
       </c>
       <c r="BB171" t="s">
@@ -30214,13 +30212,13 @@
     </row>
     <row r="172" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A172" s="10" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B172" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="C172" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D172" t="s">
         <v>477</v>
@@ -30260,7 +30258,7 @@
         <v>1</v>
       </c>
       <c r="AA172">
-        <f t="shared" si="83"/>
+        <f t="shared" ref="AA172:AA176" si="83">X172+Y172</f>
         <v>6</v>
       </c>
       <c r="AB172">
@@ -30277,11 +30275,11 @@
       </c>
       <c r="AJ172" s="10"/>
       <c r="AK172">
-        <f t="shared" si="84"/>
+        <f t="shared" ref="AK172:AK176" si="84">AI172+AJ172</f>
         <v>0</v>
       </c>
       <c r="AL172" s="67">
-        <f t="shared" si="85"/>
+        <f t="shared" ref="AL172:AL176" si="85" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ172*AR172*AS172) * (AA172 / 5) + 441</f>
         <v>74552.537876951479</v>
       </c>
       <c r="AM172" s="8" t="s">
@@ -30309,30 +30307,30 @@
         <v>8</v>
       </c>
       <c r="AU172">
-        <f t="shared" si="86"/>
+        <f t="shared" ref="AU172:AU176" si="86" xml:space="preserve"> _xlfn.FLOOR.MATH((AN172 - AQ172) / 2)</f>
         <v>20</v>
       </c>
       <c r="AV172">
-        <f t="shared" si="87"/>
+        <f t="shared" ref="AV172:AV176" si="87" xml:space="preserve"> _xlfn.FLOOR.MATH((AO172 - AR172) / 2)</f>
         <v>11</v>
       </c>
       <c r="AW172">
-        <f t="shared" si="88"/>
+        <f t="shared" ref="AW172:AW176" si="88" xml:space="preserve"> _xlfn.FLOOR.MATH((AP172 - AS172) / 2)</f>
         <v>67</v>
       </c>
       <c r="AX172" s="47" t="s">
         <v>8</v>
       </c>
       <c r="AY172">
-        <f t="shared" si="89"/>
+        <f t="shared" ref="AY172:AY176" si="89">AQ172-AU172</f>
         <v>113</v>
       </c>
       <c r="AZ172">
-        <f t="shared" si="90"/>
+        <f t="shared" ref="AZ172:AZ176" si="90">AR172-AV172</f>
         <v>709</v>
       </c>
       <c r="BA172" s="8">
-        <f t="shared" si="91"/>
+        <f t="shared" ref="BA172:BA176" si="91">AS172-AW172</f>
         <v>233</v>
       </c>
       <c r="BB172" t="s">
@@ -30347,13 +30345,13 @@
     </row>
     <row r="173" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A173" s="10" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B173" t="s">
-        <v>701</v>
+        <v>692</v>
       </c>
       <c r="C173" t="s">
-        <v>691</v>
+        <v>680</v>
       </c>
       <c r="D173" t="s">
         <v>477</v>
@@ -30393,7 +30391,7 @@
         <v>1</v>
       </c>
       <c r="AA173">
-        <f t="shared" ref="AA173" si="92">X173+Y173</f>
+        <f t="shared" si="83"/>
         <v>6</v>
       </c>
       <c r="AB173">
@@ -30410,11 +30408,11 @@
       </c>
       <c r="AJ173" s="10"/>
       <c r="AK173">
-        <f t="shared" ref="AK173" si="93">AI173+AJ173</f>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="AL173" s="67">
-        <f t="shared" ref="AL173" si="94" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ173*AR173*AS173) * (AA173 / 5) + 441</f>
+        <f t="shared" si="85"/>
         <v>74552.537876951479</v>
       </c>
       <c r="AM173" s="8" t="s">
@@ -30442,30 +30440,30 @@
         <v>8</v>
       </c>
       <c r="AU173">
-        <f t="shared" ref="AU173" si="95" xml:space="preserve"> _xlfn.FLOOR.MATH((AN173 - AQ173) / 2)</f>
+        <f t="shared" si="86"/>
         <v>20</v>
       </c>
       <c r="AV173">
-        <f t="shared" ref="AV173" si="96" xml:space="preserve"> _xlfn.FLOOR.MATH((AO173 - AR173) / 2)</f>
+        <f t="shared" si="87"/>
         <v>11</v>
       </c>
       <c r="AW173">
-        <f t="shared" ref="AW173" si="97" xml:space="preserve"> _xlfn.FLOOR.MATH((AP173 - AS173) / 2)</f>
+        <f t="shared" si="88"/>
         <v>67</v>
       </c>
       <c r="AX173" s="47" t="s">
         <v>8</v>
       </c>
       <c r="AY173">
-        <f t="shared" ref="AY173" si="98">AQ173-AU173</f>
+        <f t="shared" si="89"/>
         <v>113</v>
       </c>
       <c r="AZ173">
-        <f t="shared" ref="AZ173" si="99">AR173-AV173</f>
+        <f t="shared" si="90"/>
         <v>709</v>
       </c>
       <c r="BA173" s="8">
-        <f t="shared" ref="BA173" si="100">AS173-AW173</f>
+        <f t="shared" si="91"/>
         <v>233</v>
       </c>
       <c r="BB173" t="s">
@@ -30480,13 +30478,13 @@
     </row>
     <row r="174" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A174" s="10" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B174" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
       <c r="C174" t="s">
-        <v>678</v>
+        <v>691</v>
       </c>
       <c r="D174" t="s">
         <v>477</v>
@@ -30526,7 +30524,7 @@
         <v>1</v>
       </c>
       <c r="AA174">
-        <f>X174+Y174</f>
+        <f t="shared" ref="AA174" si="92">X174+Y174</f>
         <v>6</v>
       </c>
       <c r="AB174">
@@ -30543,11 +30541,11 @@
       </c>
       <c r="AJ174" s="10"/>
       <c r="AK174">
-        <f>AI174+AJ174</f>
+        <f t="shared" ref="AK174" si="93">AI174+AJ174</f>
         <v>0</v>
       </c>
       <c r="AL174" s="67">
-        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ174*AR174*AS174) * (AA174 / 5) + 441</f>
+        <f t="shared" ref="AL174" si="94" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ174*AR174*AS174) * (AA174 / 5) + 441</f>
         <v>74552.537876951479</v>
       </c>
       <c r="AM174" s="8" t="s">
@@ -30575,30 +30573,30 @@
         <v>8</v>
       </c>
       <c r="AU174">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN174 - AQ174) / 2)</f>
+        <f t="shared" ref="AU174" si="95" xml:space="preserve"> _xlfn.FLOOR.MATH((AN174 - AQ174) / 2)</f>
         <v>20</v>
       </c>
       <c r="AV174">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO174 - AR174) / 2)</f>
+        <f t="shared" ref="AV174" si="96" xml:space="preserve"> _xlfn.FLOOR.MATH((AO174 - AR174) / 2)</f>
         <v>11</v>
       </c>
       <c r="AW174">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP174 - AS174) / 2)</f>
+        <f t="shared" ref="AW174" si="97" xml:space="preserve"> _xlfn.FLOOR.MATH((AP174 - AS174) / 2)</f>
         <v>67</v>
       </c>
       <c r="AX174" s="47" t="s">
         <v>8</v>
       </c>
       <c r="AY174">
-        <f>AQ174-AU174</f>
+        <f t="shared" ref="AY174" si="98">AQ174-AU174</f>
         <v>113</v>
       </c>
       <c r="AZ174">
-        <f>AR174-AV174</f>
+        <f t="shared" ref="AZ174" si="99">AR174-AV174</f>
         <v>709</v>
       </c>
       <c r="BA174" s="8">
-        <f>AS174-AW174</f>
+        <f t="shared" ref="BA174" si="100">AS174-AW174</f>
         <v>233</v>
       </c>
       <c r="BB174" t="s">
@@ -30613,13 +30611,13 @@
     </row>
     <row r="175" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A175" s="10" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B175" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C175" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D175" t="s">
         <v>477</v>
@@ -30746,13 +30744,13 @@
     </row>
     <row r="176" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A176" s="10" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="B176" t="s">
-        <v>693</v>
+        <v>697</v>
       </c>
       <c r="C176" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D176" t="s">
         <v>477</v>
@@ -30879,13 +30877,13 @@
     </row>
     <row r="177" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A177" s="10" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B177" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="C177" t="s">
-        <v>691</v>
+        <v>680</v>
       </c>
       <c r="D177" t="s">
         <v>477</v>
@@ -31012,22 +31010,22 @@
     </row>
     <row r="178" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A178" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B178" s="10" t="s">
-        <v>117</v>
+        <v>699</v>
+      </c>
+      <c r="B178" t="s">
+        <v>700</v>
       </c>
       <c r="C178" t="s">
-        <v>117</v>
+        <v>691</v>
       </c>
       <c r="D178" t="s">
-        <v>117</v>
+        <v>477</v>
       </c>
       <c r="E178" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="F178" t="s">
-        <v>117</v>
+        <v>636</v>
       </c>
       <c r="G178" s="40" t="s">
         <v>117</v>
@@ -31045,102 +31043,235 @@
       <c r="V178" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="W178" t="s">
-        <v>117</v>
-      </c>
-      <c r="X178" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y178" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC178" t="s">
-        <v>117</v>
+      <c r="W178">
+        <v>1</v>
+      </c>
+      <c r="X178">
+        <v>5</v>
+      </c>
+      <c r="Y178">
+        <v>1</v>
+      </c>
+      <c r="Z178">
+        <v>1</v>
+      </c>
+      <c r="AA178">
+        <f>X178+Y178</f>
+        <v>6</v>
+      </c>
+      <c r="AB178">
+        <v>6</v>
+      </c>
+      <c r="AC178">
+        <v>3</v>
       </c>
       <c r="AE178" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AH178" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK178" t="e">
-        <f t="shared" ref="AK177:AK178" si="101">AI178+AJ178</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AL178" t="e">
-        <f t="shared" ref="AL177:AL178" si="102" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ178*AR178*AS178) * (AA178 / 5) + 441</f>
-        <v>#VALUE!</v>
+        <v>96</v>
+      </c>
+      <c r="AJ178" s="10"/>
+      <c r="AK178">
+        <f>AI178+AJ178</f>
+        <v>0</v>
+      </c>
+      <c r="AL178" s="67">
+        <f xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ178*AR178*AS178) * (AA178 / 5) + 441</f>
+        <v>74552.537876951479</v>
       </c>
       <c r="AM178" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AN178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP178" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS178" t="s">
-        <v>117</v>
+      <c r="AN178">
+        <v>173</v>
+      </c>
+      <c r="AO178">
+        <v>743</v>
+      </c>
+      <c r="AP178" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ178">
+        <v>133</v>
+      </c>
+      <c r="AR178">
+        <v>720</v>
+      </c>
+      <c r="AS178">
+        <v>300</v>
       </c>
       <c r="AT178" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="AU178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV178" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW178" t="s">
-        <v>117</v>
+      <c r="AU178">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN178 - AQ178) / 2)</f>
+        <v>20</v>
+      </c>
+      <c r="AV178">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO178 - AR178) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW178">
+        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP178 - AS178) / 2)</f>
+        <v>67</v>
       </c>
       <c r="AX178" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="AY178" t="e">
-        <f t="shared" ref="AY177:AY178" si="103">AQ178-AU178</f>
+      <c r="AY178">
+        <f>AQ178-AU178</f>
+        <v>113</v>
+      </c>
+      <c r="AZ178">
+        <f>AR178-AV178</f>
+        <v>709</v>
+      </c>
+      <c r="BA178" s="8">
+        <f>AS178-AW178</f>
+        <v>233</v>
+      </c>
+      <c r="BB178" t="s">
+        <v>672</v>
+      </c>
+      <c r="BC178" t="s">
+        <v>673</v>
+      </c>
+      <c r="BD178" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="179" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A179" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B179" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C179" t="s">
+        <v>117</v>
+      </c>
+      <c r="D179" t="s">
+        <v>117</v>
+      </c>
+      <c r="E179" t="s">
+        <v>117</v>
+      </c>
+      <c r="F179" t="s">
+        <v>117</v>
+      </c>
+      <c r="G179" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H179" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I179" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J179" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U179" s="10"/>
+      <c r="V179" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W179" t="s">
+        <v>117</v>
+      </c>
+      <c r="X179" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y179" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH179" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK179" t="e">
+        <f t="shared" ref="AK178:AK179" si="101">AI179+AJ179</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ178" t="e">
-        <f t="shared" ref="AZ177:AZ178" si="104">AR178-AV178</f>
+      <c r="AL179" t="e">
+        <f t="shared" ref="AL178:AL179" si="102" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ179*AR179*AS179) * (AA179 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA178" s="8" t="e">
-        <f t="shared" ref="BA177:BA178" si="105">AS178-AW178</f>
+      <c r="AM179" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP179" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT179" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW179" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX179" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY179" t="e">
+        <f t="shared" ref="AY178:AY179" si="103">AQ179-AU179</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB178" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC178" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD178" t="s">
+      <c r="AZ179" t="e">
+        <f t="shared" ref="AZ178:AZ179" si="104">AR179-AV179</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA179" s="8" t="e">
+        <f t="shared" ref="BA178:BA179" si="105">AS179-AW179</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB179" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC179" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD179" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generic commit message, Mon 12:10:30 05.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popsicle_cell\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D004188-A03C-434E-A7BB-DD0F7F75A369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AB1CB1-1E1B-4930-9500-19AD58ABFFF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -25,10 +25,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3085,16 +3085,16 @@
   <dimension ref="A1:BG179"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J154" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B142" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A171" sqref="A171"/>
+      <selection pane="bottomRight" activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="102.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.77734375" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
     <col min="5" max="5" width="6.5546875" customWidth="1"/>
@@ -30258,7 +30258,7 @@
         <v>1</v>
       </c>
       <c r="AA172">
-        <f t="shared" ref="AA172:AA176" si="83">X172+Y172</f>
+        <f t="shared" ref="AA172:AA173" si="83">X172+Y172</f>
         <v>6</v>
       </c>
       <c r="AB172">
@@ -30275,11 +30275,11 @@
       </c>
       <c r="AJ172" s="10"/>
       <c r="AK172">
-        <f t="shared" ref="AK172:AK176" si="84">AI172+AJ172</f>
+        <f t="shared" ref="AK172:AK173" si="84">AI172+AJ172</f>
         <v>0</v>
       </c>
       <c r="AL172" s="67">
-        <f t="shared" ref="AL172:AL176" si="85" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ172*AR172*AS172) * (AA172 / 5) + 441</f>
+        <f t="shared" ref="AL172:AL173" si="85" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ172*AR172*AS172) * (AA172 / 5) + 441</f>
         <v>74552.537876951479</v>
       </c>
       <c r="AM172" s="8" t="s">
@@ -30307,30 +30307,30 @@
         <v>8</v>
       </c>
       <c r="AU172">
-        <f t="shared" ref="AU172:AU176" si="86" xml:space="preserve"> _xlfn.FLOOR.MATH((AN172 - AQ172) / 2)</f>
+        <f t="shared" ref="AU172:AU173" si="86" xml:space="preserve"> _xlfn.FLOOR.MATH((AN172 - AQ172) / 2)</f>
         <v>20</v>
       </c>
       <c r="AV172">
-        <f t="shared" ref="AV172:AV176" si="87" xml:space="preserve"> _xlfn.FLOOR.MATH((AO172 - AR172) / 2)</f>
+        <f t="shared" ref="AV172:AV173" si="87" xml:space="preserve"> _xlfn.FLOOR.MATH((AO172 - AR172) / 2)</f>
         <v>11</v>
       </c>
       <c r="AW172">
-        <f t="shared" ref="AW172:AW176" si="88" xml:space="preserve"> _xlfn.FLOOR.MATH((AP172 - AS172) / 2)</f>
+        <f t="shared" ref="AW172:AW173" si="88" xml:space="preserve"> _xlfn.FLOOR.MATH((AP172 - AS172) / 2)</f>
         <v>67</v>
       </c>
       <c r="AX172" s="47" t="s">
         <v>8</v>
       </c>
       <c r="AY172">
-        <f t="shared" ref="AY172:AY176" si="89">AQ172-AU172</f>
+        <f t="shared" ref="AY172:AY173" si="89">AQ172-AU172</f>
         <v>113</v>
       </c>
       <c r="AZ172">
-        <f t="shared" ref="AZ172:AZ176" si="90">AR172-AV172</f>
+        <f t="shared" ref="AZ172:AZ173" si="90">AR172-AV172</f>
         <v>709</v>
       </c>
       <c r="BA172" s="8">
-        <f t="shared" ref="BA172:BA176" si="91">AS172-AW172</f>
+        <f t="shared" ref="BA172:BA173" si="91">AS172-AW172</f>
         <v>233</v>
       </c>
       <c r="BB172" t="s">
@@ -30706,30 +30706,30 @@
         <v>8</v>
       </c>
       <c r="AU175">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN175 - AQ175) / 2)</f>
+        <f t="shared" ref="AU175:AW178" si="101" xml:space="preserve"> _xlfn.FLOOR.MATH((AN175 - AQ175) / 2)</f>
         <v>20</v>
       </c>
       <c r="AV175">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO175 - AR175) / 2)</f>
+        <f t="shared" si="101"/>
         <v>11</v>
       </c>
       <c r="AW175">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP175 - AS175) / 2)</f>
+        <f t="shared" si="101"/>
         <v>67</v>
       </c>
       <c r="AX175" s="47" t="s">
         <v>8</v>
       </c>
       <c r="AY175">
-        <f>AQ175-AU175</f>
+        <f t="shared" ref="AY175:BA178" si="102">AQ175-AU175</f>
         <v>113</v>
       </c>
       <c r="AZ175">
-        <f>AR175-AV175</f>
+        <f t="shared" si="102"/>
         <v>709</v>
       </c>
       <c r="BA175" s="8">
-        <f>AS175-AW175</f>
+        <f t="shared" si="102"/>
         <v>233</v>
       </c>
       <c r="BB175" t="s">
@@ -30839,30 +30839,30 @@
         <v>8</v>
       </c>
       <c r="AU176">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN176 - AQ176) / 2)</f>
+        <f t="shared" si="101"/>
         <v>20</v>
       </c>
       <c r="AV176">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO176 - AR176) / 2)</f>
+        <f t="shared" si="101"/>
         <v>11</v>
       </c>
       <c r="AW176">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP176 - AS176) / 2)</f>
+        <f t="shared" si="101"/>
         <v>67</v>
       </c>
       <c r="AX176" s="47" t="s">
         <v>8</v>
       </c>
       <c r="AY176">
-        <f>AQ176-AU176</f>
+        <f t="shared" si="102"/>
         <v>113</v>
       </c>
       <c r="AZ176">
-        <f>AR176-AV176</f>
+        <f t="shared" si="102"/>
         <v>709</v>
       </c>
       <c r="BA176" s="8">
-        <f>AS176-AW176</f>
+        <f t="shared" si="102"/>
         <v>233</v>
       </c>
       <c r="BB176" t="s">
@@ -30972,30 +30972,30 @@
         <v>8</v>
       </c>
       <c r="AU177">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN177 - AQ177) / 2)</f>
+        <f t="shared" si="101"/>
         <v>20</v>
       </c>
       <c r="AV177">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO177 - AR177) / 2)</f>
+        <f t="shared" si="101"/>
         <v>11</v>
       </c>
       <c r="AW177">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP177 - AS177) / 2)</f>
+        <f t="shared" si="101"/>
         <v>67</v>
       </c>
       <c r="AX177" s="47" t="s">
         <v>8</v>
       </c>
       <c r="AY177">
-        <f>AQ177-AU177</f>
+        <f t="shared" si="102"/>
         <v>113</v>
       </c>
       <c r="AZ177">
-        <f>AR177-AV177</f>
+        <f t="shared" si="102"/>
         <v>709</v>
       </c>
       <c r="BA177" s="8">
-        <f>AS177-AW177</f>
+        <f t="shared" si="102"/>
         <v>233</v>
       </c>
       <c r="BB177" t="s">
@@ -31105,30 +31105,30 @@
         <v>8</v>
       </c>
       <c r="AU178">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AN178 - AQ178) / 2)</f>
+        <f t="shared" si="101"/>
         <v>20</v>
       </c>
       <c r="AV178">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AO178 - AR178) / 2)</f>
+        <f t="shared" si="101"/>
         <v>11</v>
       </c>
       <c r="AW178">
-        <f xml:space="preserve"> _xlfn.FLOOR.MATH((AP178 - AS178) / 2)</f>
+        <f t="shared" si="101"/>
         <v>67</v>
       </c>
       <c r="AX178" s="47" t="s">
         <v>8</v>
       </c>
       <c r="AY178">
-        <f>AQ178-AU178</f>
+        <f t="shared" si="102"/>
         <v>113</v>
       </c>
       <c r="AZ178">
-        <f>AR178-AV178</f>
+        <f t="shared" si="102"/>
         <v>709</v>
       </c>
       <c r="BA178" s="8">
-        <f>AS178-AW178</f>
+        <f t="shared" si="102"/>
         <v>233</v>
       </c>
       <c r="BB178" t="s">
@@ -31210,11 +31210,11 @@
         <v>117</v>
       </c>
       <c r="AK179" t="e">
-        <f t="shared" ref="AK178:AK179" si="101">AI179+AJ179</f>
+        <f t="shared" ref="AK179" si="103">AI179+AJ179</f>
         <v>#VALUE!</v>
       </c>
       <c r="AL179" t="e">
-        <f t="shared" ref="AL178:AL179" si="102" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ179*AR179*AS179) * (AA179 / 5) + 441</f>
+        <f t="shared" ref="AL179" si="104" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ179*AR179*AS179) * (AA179 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
       <c r="AM179" s="8" t="s">
@@ -31254,15 +31254,15 @@
         <v>8</v>
       </c>
       <c r="AY179" t="e">
-        <f t="shared" ref="AY178:AY179" si="103">AQ179-AU179</f>
+        <f t="shared" ref="AY179" si="105">AQ179-AU179</f>
         <v>#VALUE!</v>
       </c>
       <c r="AZ179" t="e">
-        <f t="shared" ref="AZ178:AZ179" si="104">AR179-AV179</f>
+        <f t="shared" ref="AZ179" si="106">AR179-AV179</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA179" s="8" t="e">
-        <f t="shared" ref="BA178:BA179" si="105">AS179-AW179</f>
+        <f t="shared" ref="BA179" si="107">AS179-AW179</f>
         <v>#VALUE!</v>
       </c>
       <c r="BB179" t="s">

</xml_diff>

<commit_message>
prepare train3dunet chpt-240209-0 to -7; Fri 07:45:43 09.02.2024
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AB1CB1-1E1B-4930-9500-19AD58ABFFF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB69AF7A-C263-476B-A22F-BF420A472EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2151,24 +2140,6 @@
     <t>expect model of good predictive power</t>
   </si>
   <si>
-    <t>240205-0</t>
-  </si>
-  <si>
-    <t>240205-1</t>
-  </si>
-  <si>
-    <t>240205-2</t>
-  </si>
-  <si>
-    <t>240205-3</t>
-  </si>
-  <si>
-    <t>240205-4</t>
-  </si>
-  <si>
-    <t>240205-5</t>
-  </si>
-  <si>
     <t>dataset10.b.3</t>
   </si>
   <si>
@@ -2190,12 +2161,6 @@
     <t>240204-1 last, autofluo eye, nuclei model type, val=id07, test=06</t>
   </si>
   <si>
-    <t>240205-6</t>
-  </si>
-  <si>
-    <t>240205-7</t>
-  </si>
-  <si>
     <t>240204-3 last, autofluo eye, nuclei model type, val=id02, test=07</t>
   </si>
   <si>
@@ -2209,6 +2174,30 @@
   </si>
   <si>
     <t>Vary validation and test sample compared to chpt-240204-0, chpt-240204-1 and chpt-240204-2</t>
+  </si>
+  <si>
+    <t>240209-0</t>
+  </si>
+  <si>
+    <t>240209-1</t>
+  </si>
+  <si>
+    <t>240209-2</t>
+  </si>
+  <si>
+    <t>240209-3</t>
+  </si>
+  <si>
+    <t>240209-4</t>
+  </si>
+  <si>
+    <t>240209-5</t>
+  </si>
+  <si>
+    <t>240209-6</t>
+  </si>
+  <si>
+    <t>240209-7</t>
   </si>
 </sst>
 </file>
@@ -3088,69 +3077,69 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B142" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A156" sqref="A156"/>
+      <selection pane="bottomRight" activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="57.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" customWidth="1"/>
-    <col min="7" max="7" width="57" style="38" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="35.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="64.5546875" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.5546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1"/>
+    <col min="7" max="7" width="57" style="38" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="35.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="64.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
     <col min="14" max="14" width="33" customWidth="1"/>
-    <col min="15" max="21" width="9.109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="9.109375" style="17" collapsed="1"/>
-    <col min="23" max="23" width="9.109375" customWidth="1"/>
-    <col min="24" max="24" width="6.6640625" customWidth="1"/>
-    <col min="25" max="25" width="5.109375" customWidth="1"/>
+    <col min="15" max="21" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="9.140625" style="17" collapsed="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1"/>
+    <col min="24" max="24" width="6.7109375" customWidth="1"/>
+    <col min="25" max="25" width="5.140625" customWidth="1"/>
     <col min="26" max="26" width="6" customWidth="1"/>
-    <col min="27" max="27" width="11.109375" customWidth="1"/>
-    <col min="29" max="29" width="7.6640625" customWidth="1"/>
-    <col min="30" max="30" width="9.5546875" customWidth="1"/>
+    <col min="27" max="27" width="11.140625" customWidth="1"/>
+    <col min="29" max="29" width="7.7109375" customWidth="1"/>
+    <col min="30" max="30" width="9.5703125" customWidth="1"/>
     <col min="31" max="31" width="9" customWidth="1"/>
-    <col min="32" max="32" width="8.88671875" customWidth="1"/>
-    <col min="33" max="33" width="9.88671875" customWidth="1"/>
-    <col min="34" max="34" width="9.6640625" style="8" customWidth="1"/>
-    <col min="35" max="35" width="11.6640625" customWidth="1"/>
-    <col min="36" max="36" width="10.44140625" customWidth="1"/>
-    <col min="37" max="37" width="9.6640625" customWidth="1"/>
-    <col min="38" max="38" width="15.44140625" customWidth="1"/>
-    <col min="39" max="39" width="26.33203125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="6.5546875" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.6640625" customWidth="1"/>
-    <col min="42" max="42" width="6.6640625" style="17" customWidth="1"/>
-    <col min="43" max="43" width="5.33203125" customWidth="1"/>
-    <col min="44" max="44" width="6.109375" customWidth="1"/>
+    <col min="32" max="32" width="8.85546875" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" customWidth="1"/>
+    <col min="34" max="34" width="9.7109375" style="8" customWidth="1"/>
+    <col min="35" max="35" width="11.7109375" customWidth="1"/>
+    <col min="36" max="36" width="10.42578125" customWidth="1"/>
+    <col min="37" max="37" width="9.7109375" customWidth="1"/>
+    <col min="38" max="38" width="15.42578125" customWidth="1"/>
+    <col min="39" max="39" width="26.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="6.5703125" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.7109375" customWidth="1"/>
+    <col min="42" max="42" width="6.7109375" style="17" customWidth="1"/>
+    <col min="43" max="43" width="5.28515625" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" customWidth="1"/>
     <col min="45" max="45" width="5" customWidth="1"/>
     <col min="46" max="46" width="5" style="17" customWidth="1"/>
-    <col min="47" max="47" width="6.109375" customWidth="1"/>
-    <col min="48" max="48" width="6.5546875" customWidth="1"/>
+    <col min="47" max="47" width="6.140625" customWidth="1"/>
+    <col min="48" max="48" width="6.5703125" customWidth="1"/>
     <col min="49" max="49" width="5" customWidth="1"/>
     <col min="50" max="50" width="6" style="17" customWidth="1"/>
     <col min="51" max="52" width="6" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="53" max="53" width="6" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="32.109375" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="35.44140625" customWidth="1"/>
-    <col min="56" max="56" width="5.109375" customWidth="1"/>
-    <col min="57" max="57" width="135.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="32.140625" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="35.42578125" customWidth="1"/>
+    <col min="56" max="56" width="5.140625" customWidth="1"/>
+    <col min="57" max="57" width="135.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="58" max="58" width="206" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.6640625" customWidth="1"/>
-    <col min="63" max="63" width="12.109375" customWidth="1"/>
+    <col min="59" max="59" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.7109375" customWidth="1"/>
+    <col min="63" max="63" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -3326,7 +3315,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -3494,7 +3483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3663,7 +3652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:58" s="6" customFormat="1" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" s="6" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>51</v>
       </c>
@@ -3831,7 +3820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3996,7 +3985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4161,7 +4150,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4326,7 +4315,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4491,7 +4480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4662,7 +4651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -4827,7 +4816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:58" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -4992,7 +4981,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -5158,7 +5147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -5323,7 +5312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -5488,7 +5477,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -5654,7 +5643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -5821,7 +5810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -5987,7 +5976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -6153,7 +6142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -6319,7 +6308,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -6485,7 +6474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -6651,7 +6640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -6817,7 +6806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -6983,7 +6972,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -7149,7 +7138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -7316,7 +7305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
@@ -7483,7 +7472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -7653,7 +7642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -7822,7 +7811,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -7992,7 +7981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -8162,7 +8151,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -8332,7 +8321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -8501,7 +8490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -8670,7 +8659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -8839,7 +8828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -9008,7 +8997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>180</v>
       </c>
@@ -9177,7 +9166,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -9346,7 +9335,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -9515,7 +9504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>191</v>
       </c>
@@ -9684,7 +9673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>195</v>
       </c>
@@ -9853,7 +9842,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>196</v>
       </c>
@@ -10022,7 +10011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>198</v>
       </c>
@@ -10191,7 +10180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>201</v>
       </c>
@@ -10360,7 +10349,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>202</v>
       </c>
@@ -10530,7 +10519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>203</v>
       </c>
@@ -10701,7 +10690,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>235</v>
       </c>
@@ -10866,7 +10855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>236</v>
       </c>
@@ -11031,7 +11020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>237</v>
       </c>
@@ -11196,7 +11185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>238</v>
       </c>
@@ -11361,7 +11350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>239</v>
       </c>
@@ -11526,7 +11515,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>240</v>
       </c>
@@ -11691,7 +11680,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>241</v>
       </c>
@@ -11856,7 +11845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>242</v>
       </c>
@@ -12021,7 +12010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>243</v>
       </c>
@@ -12186,7 +12175,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>244</v>
       </c>
@@ -12351,7 +12340,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>245</v>
       </c>
@@ -12516,7 +12505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>246</v>
       </c>
@@ -12681,7 +12670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>247</v>
       </c>
@@ -12846,7 +12835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>248</v>
       </c>
@@ -13011,7 +13000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>249</v>
       </c>
@@ -13176,7 +13165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>250</v>
       </c>
@@ -13341,7 +13330,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>251</v>
       </c>
@@ -13506,7 +13495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>252</v>
       </c>
@@ -13672,7 +13661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:58" s="25" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:58" s="25" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
         <v>267</v>
       </c>
@@ -13842,7 +13831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>269</v>
       </c>
@@ -14019,7 +14008,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="66" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>274</v>
       </c>
@@ -14196,7 +14185,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="67" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>289</v>
       </c>
@@ -14373,7 +14362,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="68" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>292</v>
       </c>
@@ -14550,7 +14539,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>293</v>
       </c>
@@ -14727,7 +14716,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>298</v>
       </c>
@@ -14907,7 +14896,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>299</v>
       </c>
@@ -15084,7 +15073,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="72" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>302</v>
       </c>
@@ -15261,7 +15250,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="73" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>321</v>
       </c>
@@ -15441,7 +15430,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>323</v>
       </c>
@@ -15618,7 +15607,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="75" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>331</v>
       </c>
@@ -15792,7 +15781,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="76" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>334</v>
       </c>
@@ -15966,7 +15955,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="77" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>350</v>
       </c>
@@ -15975,7 +15964,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="78" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>350</v>
       </c>
@@ -15984,7 +15973,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>351</v>
       </c>
@@ -16158,7 +16147,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="80" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>361</v>
       </c>
@@ -16335,7 +16324,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
         <v>365</v>
       </c>
@@ -16512,7 +16501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
         <v>369</v>
       </c>
@@ -16689,7 +16678,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
         <v>373</v>
       </c>
@@ -16866,7 +16855,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="84" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>374</v>
       </c>
@@ -17043,7 +17032,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="85" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>375</v>
       </c>
@@ -17220,7 +17209,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>377</v>
       </c>
@@ -17397,7 +17386,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="87" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
         <v>378</v>
       </c>
@@ -17574,7 +17563,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>379</v>
       </c>
@@ -17751,7 +17740,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="89" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>380</v>
       </c>
@@ -17928,7 +17917,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="90" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>381</v>
       </c>
@@ -18105,7 +18094,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="91" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
         <v>382</v>
       </c>
@@ -18282,7 +18271,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="92" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>383</v>
       </c>
@@ -18459,7 +18448,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="93" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
         <v>384</v>
       </c>
@@ -18636,7 +18625,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>392</v>
       </c>
@@ -18813,7 +18802,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="95" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
         <v>402</v>
       </c>
@@ -18990,7 +18979,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="96" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
         <v>402</v>
       </c>
@@ -19167,7 +19156,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="97" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
         <v>403</v>
       </c>
@@ -19344,7 +19333,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="98" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
         <v>412</v>
       </c>
@@ -19521,7 +19510,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="99" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
         <v>413</v>
       </c>
@@ -19698,7 +19687,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="100" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
         <v>429</v>
       </c>
@@ -19878,7 +19867,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
         <v>432</v>
       </c>
@@ -20058,7 +20047,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
         <v>433</v>
       </c>
@@ -20238,7 +20227,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="103" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
         <v>434</v>
       </c>
@@ -20420,7 +20409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
         <v>435</v>
       </c>
@@ -20602,7 +20591,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="105" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
         <v>436</v>
       </c>
@@ -20784,7 +20773,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="106" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
         <v>431</v>
       </c>
@@ -20966,7 +20955,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="107" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
         <v>456</v>
       </c>
@@ -21145,7 +21134,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
         <v>460</v>
       </c>
@@ -21327,7 +21316,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
         <v>466</v>
       </c>
@@ -21506,7 +21495,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="110" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
         <v>470</v>
       </c>
@@ -21688,7 +21677,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="111" spans="1:58" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:58" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="32" t="s">
         <v>472</v>
       </c>
@@ -21870,7 +21859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:58" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:58" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="45" t="s">
         <v>476</v>
       </c>
@@ -22049,7 +22038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
         <v>484</v>
       </c>
@@ -22233,7 +22222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A114" s="10" t="s">
         <v>485</v>
       </c>
@@ -22359,7 +22348,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="s">
         <v>493</v>
       </c>
@@ -22485,7 +22474,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
         <v>494</v>
       </c>
@@ -22613,7 +22602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A117" s="10" t="s">
         <v>505</v>
       </c>
@@ -22741,7 +22730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A118" s="10" t="s">
         <v>504</v>
       </c>
@@ -22869,7 +22858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A119" s="10" t="s">
         <v>502</v>
       </c>
@@ -22997,7 +22986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
         <v>507</v>
       </c>
@@ -23147,7 +23136,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="s">
         <v>508</v>
       </c>
@@ -23297,7 +23286,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A122" s="10" t="s">
         <v>520</v>
       </c>
@@ -23428,7 +23417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A123" s="10" t="s">
         <v>521</v>
       </c>
@@ -23559,7 +23548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A124" s="10" t="s">
         <v>522</v>
       </c>
@@ -23690,7 +23679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A125" s="10" t="s">
         <v>523</v>
       </c>
@@ -23821,7 +23810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A126" s="10" t="s">
         <v>529</v>
       </c>
@@ -23966,7 +23955,7 @@
       </c>
       <c r="BF126" s="1"/>
     </row>
-    <row r="127" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A127" s="10" t="s">
         <v>530</v>
       </c>
@@ -24114,7 +24103,7 @@
       </c>
       <c r="BF127" s="1"/>
     </row>
-    <row r="128" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
         <v>531</v>
       </c>
@@ -24262,7 +24251,7 @@
       </c>
       <c r="BF128" s="1"/>
     </row>
-    <row r="129" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
         <v>532</v>
       </c>
@@ -24410,7 +24399,7 @@
       </c>
       <c r="BF129" s="1"/>
     </row>
-    <row r="130" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
         <v>534</v>
       </c>
@@ -24557,7 +24546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>541</v>
       </c>
@@ -24701,7 +24690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
         <v>542</v>
       </c>
@@ -24845,7 +24834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>543</v>
       </c>
@@ -24989,7 +24978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
         <v>544</v>
       </c>
@@ -25133,7 +25122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A135" s="10" t="s">
         <v>545</v>
       </c>
@@ -25277,7 +25266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="s">
         <v>546</v>
       </c>
@@ -25421,7 +25410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="s">
         <v>547</v>
       </c>
@@ -25565,7 +25554,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="138" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A138" s="10" t="s">
         <v>548</v>
       </c>
@@ -25709,7 +25698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A139" s="10" t="s">
         <v>549</v>
       </c>
@@ -25852,7 +25841,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="140" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
         <v>570</v>
       </c>
@@ -25999,7 +25988,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="141" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A141" s="10" t="s">
         <v>578</v>
       </c>
@@ -26133,7 +26122,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="142" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A142" s="10" t="s">
         <v>579</v>
       </c>
@@ -26267,7 +26256,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="143" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A143" s="10" t="s">
         <v>580</v>
       </c>
@@ -26401,7 +26390,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="144" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A144" s="10" t="s">
         <v>581</v>
       </c>
@@ -26535,7 +26524,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A145" s="10" t="s">
         <v>582</v>
       </c>
@@ -26669,7 +26658,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="146" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A146" s="10" t="s">
         <v>583</v>
       </c>
@@ -26803,7 +26792,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="147" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A147" s="10" t="s">
         <v>584</v>
       </c>
@@ -26937,7 +26926,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="148" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A148" s="10" t="s">
         <v>585</v>
       </c>
@@ -27071,7 +27060,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="149" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="32" t="s">
         <v>586</v>
       </c>
@@ -27200,7 +27189,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="150" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A150" s="10" t="s">
         <v>587</v>
       </c>
@@ -27338,7 +27327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A151" s="10" t="s">
         <v>588</v>
       </c>
@@ -27476,7 +27465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A152" s="10" t="s">
         <v>596</v>
       </c>
@@ -27605,7 +27594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A153" s="10" t="s">
         <v>597</v>
       </c>
@@ -27740,7 +27729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A154" s="10" t="s">
         <v>602</v>
       </c>
@@ -27881,7 +27870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A155" s="10" t="s">
         <v>610</v>
       </c>
@@ -28019,7 +28008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A156" s="10" t="s">
         <v>611</v>
       </c>
@@ -28157,7 +28146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A157" s="10" t="s">
         <v>626</v>
       </c>
@@ -28302,7 +28291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>632</v>
       </c>
@@ -28430,7 +28419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>633</v>
       </c>
@@ -28558,7 +28547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>634</v>
       </c>
@@ -28686,7 +28675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="32" t="s">
         <v>654</v>
       </c>
@@ -28827,7 +28816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="32" t="s">
         <v>655</v>
       </c>
@@ -28968,7 +28957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="32" t="s">
         <v>656</v>
       </c>
@@ -29109,7 +29098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="32" t="s">
         <v>652</v>
       </c>
@@ -29253,7 +29242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="32" t="s">
         <v>653</v>
       </c>
@@ -29397,7 +29386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A166" s="68" t="s">
         <v>661</v>
       </c>
@@ -29541,7 +29530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A167" s="68" t="s">
         <v>666</v>
       </c>
@@ -29679,7 +29668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A168" s="68" t="s">
         <v>667</v>
       </c>
@@ -29817,7 +29806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A169" s="68" t="s">
         <v>674</v>
       </c>
@@ -29955,15 +29944,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A170" s="68" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="B170" s="68" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="C170" s="69" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="D170" s="69" t="s">
         <v>457</v>
@@ -29975,7 +29964,7 @@
         <v>636</v>
       </c>
       <c r="G170" s="40" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="H170" s="10" t="s">
         <v>671</v>
@@ -30077,12 +30066,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A171" s="10" t="s">
-        <v>685</v>
+        <v>697</v>
       </c>
       <c r="B171" t="s">
-        <v>694</v>
+        <v>688</v>
       </c>
       <c r="C171" t="s">
         <v>678</v>
@@ -30210,12 +30199,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="172" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A172" s="10" t="s">
-        <v>686</v>
+        <v>698</v>
       </c>
       <c r="B172" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="C172" t="s">
         <v>679</v>
@@ -30343,12 +30332,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="173" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A173" s="10" t="s">
-        <v>687</v>
+        <v>699</v>
       </c>
       <c r="B173" t="s">
-        <v>692</v>
+        <v>686</v>
       </c>
       <c r="C173" t="s">
         <v>680</v>
@@ -30476,15 +30465,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="174" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
-        <v>688</v>
+        <v>700</v>
       </c>
       <c r="B174" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="C174" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="D174" t="s">
         <v>477</v>
@@ -30609,12 +30598,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="175" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A175" s="10" t="s">
-        <v>689</v>
+        <v>701</v>
       </c>
       <c r="B175" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="C175" t="s">
         <v>678</v>
@@ -30742,12 +30731,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="176" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A176" s="10" t="s">
-        <v>690</v>
+        <v>702</v>
       </c>
       <c r="B176" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="C176" t="s">
         <v>679</v>
@@ -30875,12 +30864,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="177" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A177" s="10" t="s">
-        <v>698</v>
+        <v>703</v>
       </c>
       <c r="B177" t="s">
-        <v>693</v>
+        <v>687</v>
       </c>
       <c r="C177" t="s">
         <v>680</v>
@@ -31008,15 +30997,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="178" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A178" s="10" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
       <c r="B178" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="C178" t="s">
-        <v>691</v>
+        <v>685</v>
       </c>
       <c r="D178" t="s">
         <v>477</v>
@@ -31141,7 +31130,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="179" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A179" s="10" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
generic commit message, Wed 17:04:18 14.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB69AF7A-C263-476B-A22F-BF420A472EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E6BADA-A157-4B24-AF72-F057DCF332EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4820" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4857" uniqueCount="706">
   <si>
     <t>patch z</t>
   </si>
@@ -2198,6 +2198,9 @@
   </si>
   <si>
     <t>240209-7</t>
+  </si>
+  <si>
+    <t>240213-0</t>
   </si>
 </sst>
 </file>
@@ -2347,7 +2350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -2628,6 +2631,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2637,7 +2675,7 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2746,6 +2784,23 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="17" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="4" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -3071,13 +3126,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG179"/>
+  <dimension ref="A1:BG180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B142" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B171" sqref="B171"/>
+      <selection pane="bottomRight" activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -29386,147 +29441,147 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A166" s="68" t="s">
+    <row r="166" spans="1:56" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="70" t="s">
         <v>661</v>
       </c>
-      <c r="B166" s="68" t="s">
+      <c r="B166" s="70" t="s">
         <v>677</v>
       </c>
-      <c r="C166" s="69" t="s">
+      <c r="C166" s="71" t="s">
         <v>525</v>
       </c>
-      <c r="D166" s="69" t="s">
+      <c r="D166" s="71" t="s">
         <v>457</v>
       </c>
-      <c r="E166" s="69" t="s">
+      <c r="E166" s="71" t="s">
         <v>406</v>
       </c>
-      <c r="F166" s="69" t="s">
+      <c r="F166" s="71" t="s">
         <v>636</v>
       </c>
-      <c r="G166" s="40" t="s">
+      <c r="G166" s="72" t="s">
         <v>662</v>
       </c>
-      <c r="H166" s="10" t="s">
+      <c r="H166" s="73" t="s">
         <v>663</v>
       </c>
-      <c r="I166" s="32" t="s">
+      <c r="I166" s="74" t="s">
         <v>675</v>
       </c>
-      <c r="J166" s="4">
-        <v>0</v>
-      </c>
-      <c r="M166">
-        <v>1</v>
-      </c>
-      <c r="N166" t="s">
+      <c r="J166" s="75">
+        <v>0</v>
+      </c>
+      <c r="M166" s="30">
+        <v>1</v>
+      </c>
+      <c r="N166" s="30" t="s">
         <v>676</v>
       </c>
-      <c r="U166" s="10"/>
-      <c r="V166" s="17">
-        <v>1</v>
-      </c>
-      <c r="W166">
+      <c r="U166" s="73"/>
+      <c r="V166" s="76">
+        <v>1</v>
+      </c>
+      <c r="W166" s="30">
         <v>6</v>
       </c>
-      <c r="X166">
+      <c r="X166" s="30">
         <v>5</v>
       </c>
-      <c r="Y166">
-        <v>1</v>
-      </c>
-      <c r="Z166">
-        <v>1</v>
-      </c>
-      <c r="AA166">
+      <c r="Y166" s="30">
+        <v>1</v>
+      </c>
+      <c r="Z166" s="30">
+        <v>1</v>
+      </c>
+      <c r="AA166" s="30">
         <f t="shared" si="49"/>
         <v>6</v>
       </c>
-      <c r="AB166">
+      <c r="AB166" s="30">
         <v>6</v>
       </c>
-      <c r="AC166">
+      <c r="AC166" s="30">
         <v>3</v>
       </c>
-      <c r="AE166" t="s">
+      <c r="AE166" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="AH166" s="8" t="s">
+      <c r="AH166" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="AI166">
+      <c r="AI166" s="30">
         <v>78075</v>
       </c>
-      <c r="AJ166" s="10">
+      <c r="AJ166" s="73">
         <v>2977</v>
       </c>
-      <c r="AK166">
+      <c r="AK166" s="30">
         <f t="shared" si="50"/>
         <v>81052</v>
       </c>
-      <c r="AL166" s="67">
+      <c r="AL166" s="78">
         <f t="shared" ref="AL166" si="54" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ166*AR166*AS166) * (AA166 / 5) + 441</f>
         <v>74552.537876951479</v>
       </c>
-      <c r="AM166" s="8" t="s">
+      <c r="AM166" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="AN166">
+      <c r="AN166" s="30">
         <v>173</v>
       </c>
-      <c r="AO166">
+      <c r="AO166" s="30">
         <v>743</v>
       </c>
-      <c r="AP166" s="17">
+      <c r="AP166" s="76">
         <v>435</v>
       </c>
-      <c r="AQ166">
+      <c r="AQ166" s="30">
         <v>133</v>
       </c>
-      <c r="AR166">
+      <c r="AR166" s="30">
         <v>720</v>
       </c>
-      <c r="AS166">
+      <c r="AS166" s="30">
         <v>300</v>
       </c>
-      <c r="AT166" s="47" t="s">
+      <c r="AT166" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="AU166">
+      <c r="AU166" s="30">
         <f t="shared" si="43"/>
         <v>20</v>
       </c>
-      <c r="AV166">
+      <c r="AV166" s="30">
         <f t="shared" si="44"/>
         <v>11</v>
       </c>
-      <c r="AW166">
+      <c r="AW166" s="30">
         <f t="shared" si="45"/>
         <v>67</v>
       </c>
-      <c r="AX166" s="47" t="s">
+      <c r="AX166" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="AY166">
+      <c r="AY166" s="30">
         <f t="shared" ref="AY166:BA167" si="55">AQ166-AU166</f>
         <v>113</v>
       </c>
-      <c r="AZ166">
+      <c r="AZ166" s="30">
         <f t="shared" si="55"/>
         <v>709</v>
       </c>
-      <c r="BA166" s="8">
+      <c r="BA166" s="77">
         <f t="shared" si="55"/>
         <v>233</v>
       </c>
-      <c r="BB166" t="s">
+      <c r="BB166" s="30" t="s">
         <v>664</v>
       </c>
-      <c r="BC166" t="s">
+      <c r="BC166" s="30" t="s">
         <v>665</v>
       </c>
-      <c r="BD166">
+      <c r="BD166" s="30">
         <v>0</v>
       </c>
     </row>
@@ -31130,137 +31185,271 @@
         <v>117</v>
       </c>
     </row>
-    <row r="179" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A179" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B179" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C179" t="s">
-        <v>117</v>
-      </c>
-      <c r="D179" t="s">
-        <v>117</v>
-      </c>
-      <c r="E179" t="s">
-        <v>117</v>
-      </c>
-      <c r="F179" t="s">
-        <v>117</v>
-      </c>
-      <c r="G179" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="H179" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I179" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J179" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="U179" s="10"/>
-      <c r="V179" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="W179" t="s">
-        <v>117</v>
-      </c>
-      <c r="X179" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y179" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH179" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK179" t="e">
+    <row r="179" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="15" t="s">
+        <v>705</v>
+      </c>
+      <c r="B179" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G179" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="H179" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I179" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="J179" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="U179" s="15"/>
+      <c r="V179" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="W179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="X179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH179" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK179" s="3" t="e">
         <f t="shared" ref="AK179" si="103">AI179+AJ179</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AL179" t="e">
+      <c r="AL179" s="3" t="e">
         <f t="shared" ref="AL179" si="104" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ179*AR179*AS179) * (AA179 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AM179" s="8" t="s">
+      <c r="AM179" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="AN179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP179" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AT179" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW179" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX179" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY179" t="e">
+      <c r="AN179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP179" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT179" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX179" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY179" s="3" t="e">
         <f t="shared" ref="AY179" si="105">AQ179-AU179</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ179" t="e">
+      <c r="AZ179" s="3" t="e">
         <f t="shared" ref="AZ179" si="106">AR179-AV179</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA179" s="8" t="e">
+      <c r="BA179" s="23" t="e">
         <f t="shared" ref="BA179" si="107">AS179-AW179</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB179" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC179" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD179" t="s">
+      <c r="BB179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC179" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD179" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="180" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A180" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B180" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C180" t="s">
+        <v>117</v>
+      </c>
+      <c r="D180" t="s">
+        <v>117</v>
+      </c>
+      <c r="E180" t="s">
+        <v>117</v>
+      </c>
+      <c r="F180" t="s">
+        <v>117</v>
+      </c>
+      <c r="G180" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H180" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I180" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J180" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U180" s="10"/>
+      <c r="V180" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W180" t="s">
+        <v>117</v>
+      </c>
+      <c r="X180" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y180" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH180" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK180" t="e">
+        <f t="shared" ref="AK180" si="108">AI180+AJ180</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL180" t="e">
+        <f t="shared" ref="AL180" si="109" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ180*AR180*AS180) * (AA180 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM180" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP180" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT180" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW180" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX180" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY180" t="e">
+        <f t="shared" ref="AY180" si="110">AQ180-AU180</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ180" t="e">
+        <f t="shared" ref="AZ180" si="111">AR180-AV180</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA180" s="8" t="e">
+        <f t="shared" ref="BA180" si="112">AS180-AW180</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB180" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC180" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD180" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare train3dunet 240220-0 to -5
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E6BADA-A157-4B24-AF72-F057DCF332EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AD9383-1E39-4592-9055-8120A35D0917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13170" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15990" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4857" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4949" uniqueCount="728">
   <si>
     <t>patch z</t>
   </si>
@@ -2201,6 +2212,72 @@
   </si>
   <si>
     <t>240213-0</t>
+  </si>
+  <si>
+    <t>240220-0</t>
+  </si>
+  <si>
+    <t>240220-1</t>
+  </si>
+  <si>
+    <t>240220-2</t>
+  </si>
+  <si>
+    <t>240220-3</t>
+  </si>
+  <si>
+    <t>240220-4</t>
+  </si>
+  <si>
+    <t>240220-5</t>
+  </si>
+  <si>
+    <t>autofluo kidney, boundary model type, id07 test, id05 val</t>
+  </si>
+  <si>
+    <t>autofluo kidney, nuclei model type, id07 test, id05 val</t>
+  </si>
+  <si>
+    <t>autofluo kidney, boundary model type, id02 test, id01 val</t>
+  </si>
+  <si>
+    <t>autofluo kidney, boundary model type, id04 test, id06 val</t>
+  </si>
+  <si>
+    <t>autofluo kidney, nuclei model type, id02 test, id01 val</t>
+  </si>
+  <si>
+    <t>autofluo kidney, nuclei model type, id04 test, id06 val</t>
+  </si>
+  <si>
+    <t>dataset11.a.0</t>
+  </si>
+  <si>
+    <t>dataset11.b.0</t>
+  </si>
+  <si>
+    <t>dataset11.a.1</t>
+  </si>
+  <si>
+    <t>dataset11.a.2</t>
+  </si>
+  <si>
+    <t>dataset11.b.1</t>
+  </si>
+  <si>
+    <t>dataset11.b.2</t>
+  </si>
+  <si>
+    <t>patch = arbitrary number as close to embryo size as possible (z smaller, y &amp; x bigger than embryo)</t>
+  </si>
+  <si>
+    <t>stride = arbitrary number as close to embryo size as possible (z smaller, y &amp; x bigger than embryo)</t>
+  </si>
+  <si>
+    <t>patch = same as for model comparison chpt-240220-0</t>
+  </si>
+  <si>
+    <t>stride = same as for model comparison chpt-240220-0</t>
   </si>
 </sst>
 </file>
@@ -2830,9 +2907,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2870,7 +2947,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2976,7 +3053,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3118,7 +3195,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3126,13 +3203,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG180"/>
+  <dimension ref="A1:BG186"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B142" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J154" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B179" sqref="B179"/>
+      <selection pane="bottomRight" activeCell="L166" sqref="L166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -26075,8 +26152,8 @@
         <v>1</v>
       </c>
       <c r="U141" s="10"/>
-      <c r="V141" s="17" t="s">
-        <v>117</v>
+      <c r="V141" s="17">
+        <v>0</v>
       </c>
       <c r="W141" t="s">
         <v>117</v>
@@ -26209,8 +26286,8 @@
         <v>1</v>
       </c>
       <c r="U142" s="10"/>
-      <c r="V142" s="17" t="s">
-        <v>117</v>
+      <c r="V142" s="17">
+        <v>0</v>
       </c>
       <c r="W142" t="s">
         <v>117</v>
@@ -26343,8 +26420,8 @@
         <v>1</v>
       </c>
       <c r="U143" s="10"/>
-      <c r="V143" s="17" t="s">
-        <v>117</v>
+      <c r="V143" s="17">
+        <v>0</v>
       </c>
       <c r="W143" t="s">
         <v>117</v>
@@ -26477,8 +26554,8 @@
         <v>1</v>
       </c>
       <c r="U144" s="10"/>
-      <c r="V144" s="17" t="s">
-        <v>117</v>
+      <c r="V144" s="17">
+        <v>0</v>
       </c>
       <c r="W144" t="s">
         <v>117</v>
@@ -26611,8 +26688,8 @@
         <v>1</v>
       </c>
       <c r="U145" s="10"/>
-      <c r="V145" s="17" t="s">
-        <v>117</v>
+      <c r="V145" s="17">
+        <v>0</v>
       </c>
       <c r="W145" t="s">
         <v>117</v>
@@ -26745,8 +26822,8 @@
         <v>1</v>
       </c>
       <c r="U146" s="10"/>
-      <c r="V146" s="17" t="s">
-        <v>117</v>
+      <c r="V146" s="17">
+        <v>0</v>
       </c>
       <c r="W146" t="s">
         <v>117</v>
@@ -26879,8 +26956,8 @@
         <v>1</v>
       </c>
       <c r="U147" s="10"/>
-      <c r="V147" s="17" t="s">
-        <v>117</v>
+      <c r="V147" s="17">
+        <v>0</v>
       </c>
       <c r="W147" t="s">
         <v>117</v>
@@ -27013,8 +27090,8 @@
         <v>1</v>
       </c>
       <c r="U148" s="10"/>
-      <c r="V148" s="17" t="s">
-        <v>117</v>
+      <c r="V148" s="17">
+        <v>0</v>
       </c>
       <c r="W148" t="s">
         <v>117</v>
@@ -27957,8 +28034,8 @@
         <v>1</v>
       </c>
       <c r="U155" s="10"/>
-      <c r="V155" s="17" t="s">
-        <v>117</v>
+      <c r="V155" s="17">
+        <v>0</v>
       </c>
       <c r="W155">
         <v>6</v>
@@ -28095,8 +28172,8 @@
         <v>1</v>
       </c>
       <c r="U156" s="10"/>
-      <c r="V156" s="17" t="s">
-        <v>117</v>
+      <c r="V156" s="17">
+        <v>0</v>
       </c>
       <c r="W156">
         <v>6</v>
@@ -30149,12 +30226,12 @@
       <c r="I171" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J171" s="4" t="s">
-        <v>117</v>
+      <c r="J171" s="4">
+        <v>1</v>
       </c>
       <c r="U171" s="10"/>
-      <c r="V171" s="17" t="s">
-        <v>117</v>
+      <c r="V171" s="17">
+        <v>0</v>
       </c>
       <c r="W171">
         <v>1</v>
@@ -30250,8 +30327,8 @@
       <c r="BC171" t="s">
         <v>673</v>
       </c>
-      <c r="BD171" t="s">
-        <v>117</v>
+      <c r="BD171">
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:56" x14ac:dyDescent="0.25">
@@ -30282,12 +30359,12 @@
       <c r="I172" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J172" s="4" t="s">
-        <v>117</v>
+      <c r="J172" s="4">
+        <v>1</v>
       </c>
       <c r="U172" s="10"/>
-      <c r="V172" s="17" t="s">
-        <v>117</v>
+      <c r="V172" s="17">
+        <v>0</v>
       </c>
       <c r="W172">
         <v>1</v>
@@ -30383,8 +30460,8 @@
       <c r="BC172" t="s">
         <v>673</v>
       </c>
-      <c r="BD172" t="s">
-        <v>117</v>
+      <c r="BD172">
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:56" x14ac:dyDescent="0.25">
@@ -30415,12 +30492,12 @@
       <c r="I173" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J173" s="4" t="s">
-        <v>117</v>
+      <c r="J173" s="4">
+        <v>1</v>
       </c>
       <c r="U173" s="10"/>
-      <c r="V173" s="17" t="s">
-        <v>117</v>
+      <c r="V173" s="17">
+        <v>0</v>
       </c>
       <c r="W173">
         <v>1</v>
@@ -30516,8 +30593,8 @@
       <c r="BC173" t="s">
         <v>673</v>
       </c>
-      <c r="BD173" t="s">
-        <v>117</v>
+      <c r="BD173">
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:56" x14ac:dyDescent="0.25">
@@ -30548,12 +30625,12 @@
       <c r="I174" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J174" s="4" t="s">
-        <v>117</v>
+      <c r="J174" s="4">
+        <v>1</v>
       </c>
       <c r="U174" s="10"/>
-      <c r="V174" s="17" t="s">
-        <v>117</v>
+      <c r="V174" s="17">
+        <v>0</v>
       </c>
       <c r="W174">
         <v>1</v>
@@ -30649,8 +30726,8 @@
       <c r="BC174" t="s">
         <v>673</v>
       </c>
-      <c r="BD174" t="s">
-        <v>117</v>
+      <c r="BD174">
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:56" x14ac:dyDescent="0.25">
@@ -30681,12 +30758,12 @@
       <c r="I175" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J175" s="4" t="s">
-        <v>117</v>
+      <c r="J175" s="4">
+        <v>1</v>
       </c>
       <c r="U175" s="10"/>
-      <c r="V175" s="17" t="s">
-        <v>117</v>
+      <c r="V175" s="17">
+        <v>0</v>
       </c>
       <c r="W175">
         <v>1</v>
@@ -30782,8 +30859,8 @@
       <c r="BC175" t="s">
         <v>673</v>
       </c>
-      <c r="BD175" t="s">
-        <v>117</v>
+      <c r="BD175">
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:56" x14ac:dyDescent="0.25">
@@ -30814,12 +30891,12 @@
       <c r="I176" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J176" s="4" t="s">
-        <v>117</v>
+      <c r="J176" s="4">
+        <v>1</v>
       </c>
       <c r="U176" s="10"/>
-      <c r="V176" s="17" t="s">
-        <v>117</v>
+      <c r="V176" s="17">
+        <v>0</v>
       </c>
       <c r="W176">
         <v>1</v>
@@ -30915,8 +30992,8 @@
       <c r="BC176" t="s">
         <v>673</v>
       </c>
-      <c r="BD176" t="s">
-        <v>117</v>
+      <c r="BD176">
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:56" x14ac:dyDescent="0.25">
@@ -30947,12 +31024,12 @@
       <c r="I177" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J177" s="4" t="s">
-        <v>117</v>
+      <c r="J177" s="4">
+        <v>1</v>
       </c>
       <c r="U177" s="10"/>
-      <c r="V177" s="17" t="s">
-        <v>117</v>
+      <c r="V177" s="17">
+        <v>0</v>
       </c>
       <c r="W177">
         <v>1</v>
@@ -31048,8 +31125,8 @@
       <c r="BC177" t="s">
         <v>673</v>
       </c>
-      <c r="BD177" t="s">
-        <v>117</v>
+      <c r="BD177">
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:56" x14ac:dyDescent="0.25">
@@ -31080,12 +31157,12 @@
       <c r="I178" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J178" s="4" t="s">
-        <v>117</v>
+      <c r="J178" s="4">
+        <v>1</v>
       </c>
       <c r="U178" s="10"/>
-      <c r="V178" s="17" t="s">
-        <v>117</v>
+      <c r="V178" s="17">
+        <v>0</v>
       </c>
       <c r="W178">
         <v>1</v>
@@ -31181,8 +31258,8 @@
       <c r="BC178" t="s">
         <v>673</v>
       </c>
-      <c r="BD178" t="s">
-        <v>117</v>
+      <c r="BD178">
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -31321,22 +31398,22 @@
     </row>
     <row r="180" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A180" s="10" t="s">
-        <v>117</v>
+        <v>706</v>
       </c>
       <c r="B180" s="10" t="s">
-        <v>117</v>
+        <v>712</v>
       </c>
       <c r="C180" t="s">
-        <v>117</v>
+        <v>718</v>
       </c>
       <c r="D180" t="s">
-        <v>117</v>
+        <v>457</v>
       </c>
       <c r="E180" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="F180" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="G180" s="40" t="s">
         <v>117</v>
@@ -31354,32 +31431,33 @@
       <c r="V180" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="W180" t="s">
-        <v>117</v>
-      </c>
-      <c r="X180" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y180" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z180" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA180" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB180" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC180" t="s">
-        <v>117</v>
+      <c r="W180">
+        <v>1</v>
+      </c>
+      <c r="X180">
+        <v>5</v>
+      </c>
+      <c r="Y180">
+        <v>1</v>
+      </c>
+      <c r="Z180">
+        <v>1</v>
+      </c>
+      <c r="AA180">
+        <f t="shared" ref="AA180:AA185" si="108">X180+Y180</f>
+        <v>6</v>
+      </c>
+      <c r="AB180">
+        <v>6</v>
+      </c>
+      <c r="AC180">
+        <v>3</v>
       </c>
       <c r="AE180" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AH180" s="8" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="AI180" t="s">
         <v>117</v>
@@ -31388,68 +31466,895 @@
         <v>117</v>
       </c>
       <c r="AK180" t="e">
-        <f t="shared" ref="AK180" si="108">AI180+AJ180</f>
+        <f t="shared" ref="AK180" si="109">AI180+AJ180</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AL180" t="e">
-        <f t="shared" ref="AL180" si="109" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ180*AR180*AS180) * (AA180 / 5) + 441</f>
-        <v>#VALUE!</v>
+      <c r="AL180">
+        <f t="shared" ref="AL180" si="110" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ180*AR180*AS180) * (AA180 / 5) + 441</f>
+        <v>74764.828731758302</v>
       </c>
       <c r="AM180" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AN180" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO180" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP180" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ180" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR180" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS180" t="s">
-        <v>117</v>
+      <c r="AN180">
+        <v>149</v>
+      </c>
+      <c r="AO180">
+        <v>743</v>
+      </c>
+      <c r="AP180" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ180">
+        <v>147</v>
+      </c>
+      <c r="AR180">
+        <v>700</v>
+      </c>
+      <c r="AS180">
+        <v>280</v>
       </c>
       <c r="AT180" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="AU180" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV180" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW180" t="s">
-        <v>117</v>
+      <c r="AU180">
+        <f t="shared" ref="AU180:AU185" si="111" xml:space="preserve"> _xlfn.FLOOR.MATH((AN180 - AQ180) / 2)</f>
+        <v>1</v>
+      </c>
+      <c r="AV180">
+        <f t="shared" ref="AV180:AV185" si="112" xml:space="preserve"> _xlfn.FLOOR.MATH((AO180 - AR180) / 2)</f>
+        <v>21</v>
+      </c>
+      <c r="AW180">
+        <f t="shared" ref="AW180:AW185" si="113" xml:space="preserve"> _xlfn.FLOOR.MATH((AP180 - AS180) / 2)</f>
+        <v>77</v>
       </c>
       <c r="AX180" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY180" t="e">
-        <f t="shared" ref="AY180" si="110">AQ180-AU180</f>
+        <v>45</v>
+      </c>
+      <c r="AY180">
+        <f t="shared" ref="AY180" si="114">AQ180-AU180</f>
+        <v>146</v>
+      </c>
+      <c r="AZ180">
+        <f t="shared" ref="AZ180" si="115">AR180-AV180</f>
+        <v>679</v>
+      </c>
+      <c r="BA180" s="8">
+        <f t="shared" ref="BA180" si="116">AS180-AW180</f>
+        <v>203</v>
+      </c>
+      <c r="BB180" t="s">
+        <v>724</v>
+      </c>
+      <c r="BC180" t="s">
+        <v>725</v>
+      </c>
+      <c r="BD180" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="181" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A181" s="10" t="s">
+        <v>707</v>
+      </c>
+      <c r="B181" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="C181" t="s">
+        <v>720</v>
+      </c>
+      <c r="D181" t="s">
+        <v>457</v>
+      </c>
+      <c r="E181" t="s">
+        <v>406</v>
+      </c>
+      <c r="F181" t="s">
+        <v>409</v>
+      </c>
+      <c r="G181" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H181" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I181" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J181" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U181" s="10"/>
+      <c r="V181" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W181">
+        <v>1</v>
+      </c>
+      <c r="X181">
+        <v>5</v>
+      </c>
+      <c r="Y181">
+        <v>1</v>
+      </c>
+      <c r="Z181">
+        <v>1</v>
+      </c>
+      <c r="AA181">
+        <f t="shared" si="108"/>
+        <v>6</v>
+      </c>
+      <c r="AB181">
+        <v>6</v>
+      </c>
+      <c r="AC181">
+        <v>3</v>
+      </c>
+      <c r="AE181" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH181" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI181" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ181" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK181" t="e">
+        <f t="shared" ref="AK181" si="117">AI181+AJ181</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ180" t="e">
-        <f t="shared" ref="AZ180" si="111">AR180-AV180</f>
+      <c r="AL181">
+        <f t="shared" ref="AL181" si="118" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ181*AR181*AS181) * (AA181 / 5) + 441</f>
+        <v>74764.828731758302</v>
+      </c>
+      <c r="AM181" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN181">
+        <v>149</v>
+      </c>
+      <c r="AO181">
+        <v>743</v>
+      </c>
+      <c r="AP181" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ181">
+        <v>147</v>
+      </c>
+      <c r="AR181">
+        <v>700</v>
+      </c>
+      <c r="AS181">
+        <v>280</v>
+      </c>
+      <c r="AT181" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU181">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="AV181">
+        <f t="shared" si="112"/>
+        <v>21</v>
+      </c>
+      <c r="AW181">
+        <f t="shared" si="113"/>
+        <v>77</v>
+      </c>
+      <c r="AX181" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY181">
+        <f t="shared" ref="AY181" si="119">AQ181-AU181</f>
+        <v>146</v>
+      </c>
+      <c r="AZ181">
+        <f t="shared" ref="AZ181" si="120">AR181-AV181</f>
+        <v>679</v>
+      </c>
+      <c r="BA181" s="8">
+        <f t="shared" ref="BA181" si="121">AS181-AW181</f>
+        <v>203</v>
+      </c>
+      <c r="BB181" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC181" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD181" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="182" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A182" s="10" t="s">
+        <v>708</v>
+      </c>
+      <c r="B182" s="10" t="s">
+        <v>715</v>
+      </c>
+      <c r="C182" t="s">
+        <v>721</v>
+      </c>
+      <c r="D182" t="s">
+        <v>457</v>
+      </c>
+      <c r="E182" t="s">
+        <v>406</v>
+      </c>
+      <c r="F182" t="s">
+        <v>409</v>
+      </c>
+      <c r="G182" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H182" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I182" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J182" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U182" s="10"/>
+      <c r="V182" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W182">
+        <v>1</v>
+      </c>
+      <c r="X182">
+        <v>5</v>
+      </c>
+      <c r="Y182">
+        <v>1</v>
+      </c>
+      <c r="Z182">
+        <v>1</v>
+      </c>
+      <c r="AA182">
+        <f t="shared" si="108"/>
+        <v>6</v>
+      </c>
+      <c r="AB182">
+        <v>6</v>
+      </c>
+      <c r="AC182">
+        <v>3</v>
+      </c>
+      <c r="AE182" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH182" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI182" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ182" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK182" t="e">
+        <f t="shared" ref="AK182:AK186" si="122">AI182+AJ182</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA180" s="8" t="e">
-        <f t="shared" ref="BA180" si="112">AS180-AW180</f>
+      <c r="AL182">
+        <f t="shared" ref="AL182:AL186" si="123" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ182*AR182*AS182) * (AA182 / 5) + 441</f>
+        <v>74764.828731758302</v>
+      </c>
+      <c r="AM182" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN182">
+        <v>149</v>
+      </c>
+      <c r="AO182">
+        <v>743</v>
+      </c>
+      <c r="AP182" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ182">
+        <v>147</v>
+      </c>
+      <c r="AR182">
+        <v>700</v>
+      </c>
+      <c r="AS182">
+        <v>280</v>
+      </c>
+      <c r="AT182" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU182">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="AV182">
+        <f t="shared" si="112"/>
+        <v>21</v>
+      </c>
+      <c r="AW182">
+        <f t="shared" si="113"/>
+        <v>77</v>
+      </c>
+      <c r="AX182" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY182">
+        <f t="shared" ref="AY182:AY186" si="124">AQ182-AU182</f>
+        <v>146</v>
+      </c>
+      <c r="AZ182">
+        <f t="shared" ref="AZ182:AZ186" si="125">AR182-AV182</f>
+        <v>679</v>
+      </c>
+      <c r="BA182" s="8">
+        <f t="shared" ref="BA182:BA186" si="126">AS182-AW182</f>
+        <v>203</v>
+      </c>
+      <c r="BB182" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC182" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD182" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="183" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A183" s="10" t="s">
+        <v>709</v>
+      </c>
+      <c r="B183" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="C183" t="s">
+        <v>719</v>
+      </c>
+      <c r="D183" t="s">
+        <v>457</v>
+      </c>
+      <c r="E183" t="s">
+        <v>406</v>
+      </c>
+      <c r="F183" t="s">
+        <v>636</v>
+      </c>
+      <c r="G183" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H183" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I183" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J183" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U183" s="10"/>
+      <c r="V183" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W183">
+        <v>1</v>
+      </c>
+      <c r="X183">
+        <v>5</v>
+      </c>
+      <c r="Y183">
+        <v>1</v>
+      </c>
+      <c r="Z183">
+        <v>1</v>
+      </c>
+      <c r="AA183">
+        <f t="shared" si="108"/>
+        <v>6</v>
+      </c>
+      <c r="AB183">
+        <v>6</v>
+      </c>
+      <c r="AC183">
+        <v>3</v>
+      </c>
+      <c r="AE183" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH183" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI183" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ183" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK183" t="e">
+        <f t="shared" si="122"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BB180" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC180" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD180" t="s">
+      <c r="AL183">
+        <f t="shared" si="123"/>
+        <v>74764.828731758302</v>
+      </c>
+      <c r="AM183" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN183">
+        <v>149</v>
+      </c>
+      <c r="AO183">
+        <v>743</v>
+      </c>
+      <c r="AP183" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ183">
+        <v>147</v>
+      </c>
+      <c r="AR183">
+        <v>700</v>
+      </c>
+      <c r="AS183">
+        <v>280</v>
+      </c>
+      <c r="AT183" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU183">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="AV183">
+        <f t="shared" si="112"/>
+        <v>21</v>
+      </c>
+      <c r="AW183">
+        <f t="shared" si="113"/>
+        <v>77</v>
+      </c>
+      <c r="AX183" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY183">
+        <f t="shared" si="124"/>
+        <v>146</v>
+      </c>
+      <c r="AZ183">
+        <f t="shared" si="125"/>
+        <v>679</v>
+      </c>
+      <c r="BA183" s="8">
+        <f t="shared" si="126"/>
+        <v>203</v>
+      </c>
+      <c r="BB183" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC183" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD183" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="184" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A184" s="10" t="s">
+        <v>710</v>
+      </c>
+      <c r="B184" s="10" t="s">
+        <v>716</v>
+      </c>
+      <c r="C184" t="s">
+        <v>722</v>
+      </c>
+      <c r="D184" t="s">
+        <v>457</v>
+      </c>
+      <c r="E184" t="s">
+        <v>406</v>
+      </c>
+      <c r="F184" t="s">
+        <v>636</v>
+      </c>
+      <c r="G184" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H184" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I184" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J184" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U184" s="10"/>
+      <c r="V184" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W184">
+        <v>1</v>
+      </c>
+      <c r="X184">
+        <v>5</v>
+      </c>
+      <c r="Y184">
+        <v>1</v>
+      </c>
+      <c r="Z184">
+        <v>1</v>
+      </c>
+      <c r="AA184">
+        <f t="shared" si="108"/>
+        <v>6</v>
+      </c>
+      <c r="AB184">
+        <v>6</v>
+      </c>
+      <c r="AC184">
+        <v>3</v>
+      </c>
+      <c r="AE184" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH184" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI184" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ184" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK184" t="e">
+        <f t="shared" si="122"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL184">
+        <f t="shared" si="123"/>
+        <v>74764.828731758302</v>
+      </c>
+      <c r="AM184" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN184">
+        <v>149</v>
+      </c>
+      <c r="AO184">
+        <v>743</v>
+      </c>
+      <c r="AP184" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ184">
+        <v>147</v>
+      </c>
+      <c r="AR184">
+        <v>700</v>
+      </c>
+      <c r="AS184">
+        <v>280</v>
+      </c>
+      <c r="AT184" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU184">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="AV184">
+        <f t="shared" si="112"/>
+        <v>21</v>
+      </c>
+      <c r="AW184">
+        <f t="shared" si="113"/>
+        <v>77</v>
+      </c>
+      <c r="AX184" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY184">
+        <f t="shared" si="124"/>
+        <v>146</v>
+      </c>
+      <c r="AZ184">
+        <f t="shared" si="125"/>
+        <v>679</v>
+      </c>
+      <c r="BA184" s="8">
+        <f t="shared" si="126"/>
+        <v>203</v>
+      </c>
+      <c r="BB184" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC184" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD184" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="185" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A185" s="10" t="s">
+        <v>711</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>717</v>
+      </c>
+      <c r="C185" t="s">
+        <v>723</v>
+      </c>
+      <c r="D185" t="s">
+        <v>457</v>
+      </c>
+      <c r="E185" t="s">
+        <v>406</v>
+      </c>
+      <c r="F185" t="s">
+        <v>636</v>
+      </c>
+      <c r="G185" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H185" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I185" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J185" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U185" s="10"/>
+      <c r="V185" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W185">
+        <v>1</v>
+      </c>
+      <c r="X185">
+        <v>5</v>
+      </c>
+      <c r="Y185">
+        <v>1</v>
+      </c>
+      <c r="Z185">
+        <v>1</v>
+      </c>
+      <c r="AA185">
+        <f t="shared" si="108"/>
+        <v>6</v>
+      </c>
+      <c r="AB185">
+        <v>6</v>
+      </c>
+      <c r="AC185">
+        <v>3</v>
+      </c>
+      <c r="AE185" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH185" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI185" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ185" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK185" t="e">
+        <f t="shared" si="122"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL185">
+        <f t="shared" si="123"/>
+        <v>74764.828731758302</v>
+      </c>
+      <c r="AM185" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN185">
+        <v>149</v>
+      </c>
+      <c r="AO185">
+        <v>743</v>
+      </c>
+      <c r="AP185" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ185">
+        <v>147</v>
+      </c>
+      <c r="AR185">
+        <v>700</v>
+      </c>
+      <c r="AS185">
+        <v>280</v>
+      </c>
+      <c r="AT185" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU185">
+        <f t="shared" si="111"/>
+        <v>1</v>
+      </c>
+      <c r="AV185">
+        <f t="shared" si="112"/>
+        <v>21</v>
+      </c>
+      <c r="AW185">
+        <f t="shared" si="113"/>
+        <v>77</v>
+      </c>
+      <c r="AX185" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY185">
+        <f t="shared" si="124"/>
+        <v>146</v>
+      </c>
+      <c r="AZ185">
+        <f t="shared" si="125"/>
+        <v>679</v>
+      </c>
+      <c r="BA185" s="8">
+        <f t="shared" si="126"/>
+        <v>203</v>
+      </c>
+      <c r="BB185" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC185" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD185" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="186" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A186" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B186" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C186" t="s">
+        <v>117</v>
+      </c>
+      <c r="D186" t="s">
+        <v>117</v>
+      </c>
+      <c r="E186" t="s">
+        <v>117</v>
+      </c>
+      <c r="F186" t="s">
+        <v>117</v>
+      </c>
+      <c r="G186" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H186" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I186" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J186" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U186" s="10"/>
+      <c r="V186" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W186" t="s">
+        <v>117</v>
+      </c>
+      <c r="X186" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y186" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH186" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK186" t="e">
+        <f t="shared" si="122"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL186" t="e">
+        <f t="shared" si="123"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM186" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP186" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT186" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW186" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX186" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY186" t="e">
+        <f t="shared" si="124"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ186" t="e">
+        <f t="shared" si="125"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA186" s="8" t="e">
+        <f t="shared" si="126"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB186" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC186" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD186" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare train3dunet 240221-0 to -5
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AD9383-1E39-4592-9055-8120A35D0917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1708ABCD-8B56-4B38-91DA-25CEF33454B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15990" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="41235" yWindow="0" windowWidth="25935" windowHeight="15750" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4949" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5069" uniqueCount="735">
   <si>
     <t>patch z</t>
   </si>
@@ -2278,6 +2278,27 @@
   </si>
   <si>
     <t>stride = same as for model comparison chpt-240220-0</t>
+  </si>
+  <si>
+    <t>240221-0</t>
+  </si>
+  <si>
+    <t>240221-1</t>
+  </si>
+  <si>
+    <t>240221-2</t>
+  </si>
+  <si>
+    <t>240221-3</t>
+  </si>
+  <si>
+    <t>240221-4</t>
+  </si>
+  <si>
+    <t>240221-5</t>
+  </si>
+  <si>
+    <t>out of memory (probably cpu)</t>
   </si>
 </sst>
 </file>
@@ -2752,7 +2773,7 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2878,6 +2899,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -3203,13 +3227,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG186"/>
+  <dimension ref="A1:BG192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J154" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AC170" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L166" sqref="L166"/>
+      <selection pane="bottomRight" activeCell="AC190" sqref="AC190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -30996,7 +31020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A177" s="10" t="s">
         <v>703</v>
       </c>
@@ -31129,7 +31153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A178" s="10" t="s">
         <v>704</v>
       </c>
@@ -31262,7 +31286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:56" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="15" t="s">
         <v>705</v>
       </c>
@@ -31396,7 +31420,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="180" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A180" s="10" t="s">
         <v>706</v>
       </c>
@@ -31424,12 +31448,18 @@
       <c r="I180" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J180" s="4" t="s">
-        <v>117</v>
+      <c r="J180" s="4">
+        <v>0</v>
+      </c>
+      <c r="K180">
+        <v>1</v>
+      </c>
+      <c r="L180" s="79" t="s">
+        <v>450</v>
       </c>
       <c r="U180" s="10"/>
-      <c r="V180" s="17" t="s">
-        <v>117</v>
+      <c r="V180" s="17">
+        <v>0</v>
       </c>
       <c r="W180">
         <v>1</v>
@@ -31448,7 +31478,7 @@
         <v>6</v>
       </c>
       <c r="AB180">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="AC180">
         <v>3</v>
@@ -31530,11 +31560,14 @@
       <c r="BC180" t="s">
         <v>725</v>
       </c>
-      <c r="BD180" t="s">
-        <v>117</v>
+      <c r="BD180">
+        <v>1</v>
+      </c>
+      <c r="BG180" t="s">
+        <v>734</v>
       </c>
     </row>
-    <row r="181" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A181" s="10" t="s">
         <v>707</v>
       </c>
@@ -31562,12 +31595,18 @@
       <c r="I181" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J181" s="4" t="s">
-        <v>117</v>
+      <c r="J181" s="4">
+        <v>0</v>
+      </c>
+      <c r="K181">
+        <v>1</v>
+      </c>
+      <c r="L181" s="79" t="s">
+        <v>450</v>
       </c>
       <c r="U181" s="10"/>
-      <c r="V181" s="17" t="s">
-        <v>117</v>
+      <c r="V181" s="17">
+        <v>0</v>
       </c>
       <c r="W181">
         <v>1</v>
@@ -31586,7 +31625,7 @@
         <v>6</v>
       </c>
       <c r="AB181">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="AC181">
         <v>3</v>
@@ -31668,11 +31707,14 @@
       <c r="BC181" t="s">
         <v>727</v>
       </c>
-      <c r="BD181" t="s">
-        <v>117</v>
+      <c r="BD181">
+        <v>1</v>
+      </c>
+      <c r="BG181" t="s">
+        <v>734</v>
       </c>
     </row>
-    <row r="182" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A182" s="10" t="s">
         <v>708</v>
       </c>
@@ -31700,12 +31742,18 @@
       <c r="I182" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J182" s="4" t="s">
-        <v>117</v>
+      <c r="J182" s="4">
+        <v>0</v>
+      </c>
+      <c r="K182">
+        <v>1</v>
+      </c>
+      <c r="L182" s="79" t="s">
+        <v>450</v>
       </c>
       <c r="U182" s="10"/>
-      <c r="V182" s="17" t="s">
-        <v>117</v>
+      <c r="V182" s="17">
+        <v>0</v>
       </c>
       <c r="W182">
         <v>1</v>
@@ -31724,7 +31772,7 @@
         <v>6</v>
       </c>
       <c r="AB182">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="AC182">
         <v>3</v>
@@ -31742,11 +31790,11 @@
         <v>117</v>
       </c>
       <c r="AK182" t="e">
-        <f t="shared" ref="AK182:AK186" si="122">AI182+AJ182</f>
+        <f t="shared" ref="AK182:AK187" si="122">AI182+AJ182</f>
         <v>#VALUE!</v>
       </c>
       <c r="AL182">
-        <f t="shared" ref="AL182:AL186" si="123" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ182*AR182*AS182) * (AA182 / 5) + 441</f>
+        <f t="shared" ref="AL182:AL187" si="123" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ182*AR182*AS182) * (AA182 / 5) + 441</f>
         <v>74764.828731758302</v>
       </c>
       <c r="AM182" s="8" t="s">
@@ -31789,15 +31837,15 @@
         <v>45</v>
       </c>
       <c r="AY182">
-        <f t="shared" ref="AY182:AY186" si="124">AQ182-AU182</f>
+        <f t="shared" ref="AY182:AY187" si="124">AQ182-AU182</f>
         <v>146</v>
       </c>
       <c r="AZ182">
-        <f t="shared" ref="AZ182:AZ186" si="125">AR182-AV182</f>
+        <f t="shared" ref="AZ182:AZ187" si="125">AR182-AV182</f>
         <v>679</v>
       </c>
       <c r="BA182" s="8">
-        <f t="shared" ref="BA182:BA186" si="126">AS182-AW182</f>
+        <f t="shared" ref="BA182:BA187" si="126">AS182-AW182</f>
         <v>203</v>
       </c>
       <c r="BB182" t="s">
@@ -31806,11 +31854,14 @@
       <c r="BC182" t="s">
         <v>727</v>
       </c>
-      <c r="BD182" t="s">
-        <v>117</v>
+      <c r="BD182">
+        <v>1</v>
+      </c>
+      <c r="BG182" t="s">
+        <v>734</v>
       </c>
     </row>
-    <row r="183" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A183" s="10" t="s">
         <v>709</v>
       </c>
@@ -31838,12 +31889,18 @@
       <c r="I183" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J183" s="4" t="s">
-        <v>117</v>
+      <c r="J183" s="4">
+        <v>0</v>
+      </c>
+      <c r="K183">
+        <v>1</v>
+      </c>
+      <c r="L183" s="79" t="s">
+        <v>450</v>
       </c>
       <c r="U183" s="10"/>
-      <c r="V183" s="17" t="s">
-        <v>117</v>
+      <c r="V183" s="17">
+        <v>0</v>
       </c>
       <c r="W183">
         <v>1</v>
@@ -31862,7 +31919,7 @@
         <v>6</v>
       </c>
       <c r="AB183">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="AC183">
         <v>3</v>
@@ -31944,11 +32001,14 @@
       <c r="BC183" t="s">
         <v>727</v>
       </c>
-      <c r="BD183" t="s">
-        <v>117</v>
+      <c r="BD183">
+        <v>1</v>
+      </c>
+      <c r="BG183" t="s">
+        <v>734</v>
       </c>
     </row>
-    <row r="184" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A184" s="10" t="s">
         <v>710</v>
       </c>
@@ -31976,12 +32036,18 @@
       <c r="I184" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J184" s="4" t="s">
-        <v>117</v>
+      <c r="J184" s="4">
+        <v>0</v>
+      </c>
+      <c r="K184">
+        <v>1</v>
+      </c>
+      <c r="L184" s="79" t="s">
+        <v>450</v>
       </c>
       <c r="U184" s="10"/>
-      <c r="V184" s="17" t="s">
-        <v>117</v>
+      <c r="V184" s="17">
+        <v>0</v>
       </c>
       <c r="W184">
         <v>1</v>
@@ -32000,7 +32066,7 @@
         <v>6</v>
       </c>
       <c r="AB184">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="AC184">
         <v>3</v>
@@ -32082,166 +32148,178 @@
       <c r="BC184" t="s">
         <v>727</v>
       </c>
-      <c r="BD184" t="s">
-        <v>117</v>
+      <c r="BD184">
+        <v>1</v>
+      </c>
+      <c r="BG184" t="s">
+        <v>734</v>
       </c>
     </row>
-    <row r="185" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A185" s="10" t="s">
+    <row r="185" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="15" t="s">
         <v>711</v>
       </c>
-      <c r="B185" s="10" t="s">
+      <c r="B185" s="15" t="s">
         <v>717</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="3" t="s">
         <v>723</v>
       </c>
-      <c r="D185" t="s">
+      <c r="D185" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="E185" t="s">
+      <c r="E185" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="F185" t="s">
+      <c r="F185" s="3" t="s">
         <v>636</v>
       </c>
-      <c r="G185" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="H185" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I185" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J185" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="U185" s="10"/>
-      <c r="V185" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="W185">
-        <v>1</v>
-      </c>
-      <c r="X185">
+      <c r="G185" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="H185" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I185" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="J185" s="5">
+        <v>0</v>
+      </c>
+      <c r="K185" s="3">
+        <v>1</v>
+      </c>
+      <c r="L185" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="U185" s="15"/>
+      <c r="V185" s="19">
+        <v>0</v>
+      </c>
+      <c r="W185" s="3">
+        <v>1</v>
+      </c>
+      <c r="X185" s="3">
         <v>5</v>
       </c>
-      <c r="Y185">
-        <v>1</v>
-      </c>
-      <c r="Z185">
-        <v>1</v>
-      </c>
-      <c r="AA185">
+      <c r="Y185" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z185" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA185" s="3">
         <f t="shared" si="108"/>
         <v>6</v>
       </c>
-      <c r="AB185">
-        <v>6</v>
-      </c>
-      <c r="AC185">
+      <c r="AB185" s="3">
+        <v>33</v>
+      </c>
+      <c r="AC185" s="3">
         <v>3</v>
       </c>
-      <c r="AE185" t="s">
+      <c r="AE185" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AH185" s="8" t="s">
+      <c r="AH185" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="AI185" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ185" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK185" t="e">
+      <c r="AI185" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ185" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK185" s="3" t="e">
         <f t="shared" si="122"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL185">
+      <c r="AL185" s="3">
         <f t="shared" si="123"/>
         <v>74764.828731758302</v>
       </c>
-      <c r="AM185" s="8" t="s">
+      <c r="AM185" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="AN185">
+      <c r="AN185" s="3">
         <v>149</v>
       </c>
-      <c r="AO185">
+      <c r="AO185" s="3">
         <v>743</v>
       </c>
-      <c r="AP185" s="17">
+      <c r="AP185" s="19">
         <v>435</v>
       </c>
-      <c r="AQ185">
+      <c r="AQ185" s="3">
         <v>147</v>
       </c>
-      <c r="AR185">
+      <c r="AR185" s="3">
         <v>700</v>
       </c>
-      <c r="AS185">
+      <c r="AS185" s="3">
         <v>280</v>
       </c>
-      <c r="AT185" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU185">
+      <c r="AT185" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU185" s="3">
         <f t="shared" si="111"/>
         <v>1</v>
       </c>
-      <c r="AV185">
+      <c r="AV185" s="3">
         <f t="shared" si="112"/>
         <v>21</v>
       </c>
-      <c r="AW185">
+      <c r="AW185" s="3">
         <f t="shared" si="113"/>
         <v>77</v>
       </c>
-      <c r="AX185" s="47" t="s">
+      <c r="AX185" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="AY185">
+      <c r="AY185" s="3">
         <f t="shared" si="124"/>
         <v>146</v>
       </c>
-      <c r="AZ185">
+      <c r="AZ185" s="3">
         <f t="shared" si="125"/>
         <v>679</v>
       </c>
-      <c r="BA185" s="8">
+      <c r="BA185" s="23">
         <f t="shared" si="126"/>
         <v>203</v>
       </c>
-      <c r="BB185" t="s">
+      <c r="BB185" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="BC185" t="s">
+      <c r="BC185" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="BD185" t="s">
-        <v>117</v>
+      <c r="BD185" s="3">
+        <v>1</v>
+      </c>
+      <c r="BG185" s="3" t="s">
+        <v>734</v>
       </c>
     </row>
-    <row r="186" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A186" s="10" t="s">
-        <v>117</v>
+        <v>728</v>
       </c>
       <c r="B186" s="10" t="s">
-        <v>117</v>
+        <v>712</v>
       </c>
       <c r="C186" t="s">
-        <v>117</v>
+        <v>718</v>
       </c>
       <c r="D186" t="s">
-        <v>117</v>
+        <v>457</v>
       </c>
       <c r="E186" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="F186" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="G186" s="40" t="s">
         <v>117</v>
@@ -32259,32 +32337,33 @@
       <c r="V186" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="W186" t="s">
-        <v>117</v>
-      </c>
-      <c r="X186" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y186" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z186" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA186" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB186" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC186" t="s">
-        <v>117</v>
+      <c r="W186">
+        <v>1</v>
+      </c>
+      <c r="X186">
+        <v>5</v>
+      </c>
+      <c r="Y186">
+        <v>1</v>
+      </c>
+      <c r="Z186">
+        <v>1</v>
+      </c>
+      <c r="AA186">
+        <f t="shared" ref="AA186:AA191" si="127">X186+Y186</f>
+        <v>6</v>
+      </c>
+      <c r="AB186">
+        <v>6</v>
+      </c>
+      <c r="AC186">
+        <v>3</v>
       </c>
       <c r="AE186" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AH186" s="8" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="AI186" t="s">
         <v>117</v>
@@ -32296,65 +32375,892 @@
         <f t="shared" si="122"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL186" t="e">
+      <c r="AL186">
         <f t="shared" si="123"/>
-        <v>#VALUE!</v>
+        <v>71823.084029435064</v>
       </c>
       <c r="AM186" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AN186" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO186" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP186" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ186" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR186" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS186" t="s">
-        <v>117</v>
+      <c r="AN186">
+        <v>149</v>
+      </c>
+      <c r="AO186">
+        <v>743</v>
+      </c>
+      <c r="AP186" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ186">
+        <v>120</v>
+      </c>
+      <c r="AR186">
+        <v>720</v>
+      </c>
+      <c r="AS186">
+        <v>320</v>
       </c>
       <c r="AT186" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="AU186" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV186" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW186" t="s">
-        <v>117</v>
+      <c r="AU186">
+        <f t="shared" ref="AU186:AU191" si="128" xml:space="preserve"> _xlfn.FLOOR.MATH((AN186 - AQ186) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AV186">
+        <f t="shared" ref="AV186:AV191" si="129" xml:space="preserve"> _xlfn.FLOOR.MATH((AO186 - AR186) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW186">
+        <f t="shared" ref="AW186:AW191" si="130" xml:space="preserve"> _xlfn.FLOOR.MATH((AP186 - AS186) / 2)</f>
+        <v>57</v>
       </c>
       <c r="AX186" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY186" t="e">
+        <v>45</v>
+      </c>
+      <c r="AY186">
         <f t="shared" si="124"/>
+        <v>106</v>
+      </c>
+      <c r="AZ186">
+        <f t="shared" si="125"/>
+        <v>709</v>
+      </c>
+      <c r="BA186" s="8">
+        <f t="shared" si="126"/>
+        <v>263</v>
+      </c>
+      <c r="BB186" t="s">
+        <v>724</v>
+      </c>
+      <c r="BC186" t="s">
+        <v>725</v>
+      </c>
+      <c r="BD186" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="187" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A187" s="10" t="s">
+        <v>729</v>
+      </c>
+      <c r="B187" s="10" t="s">
+        <v>714</v>
+      </c>
+      <c r="C187" t="s">
+        <v>720</v>
+      </c>
+      <c r="D187" t="s">
+        <v>457</v>
+      </c>
+      <c r="E187" t="s">
+        <v>406</v>
+      </c>
+      <c r="F187" t="s">
+        <v>409</v>
+      </c>
+      <c r="G187" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H187" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I187" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J187" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U187" s="10"/>
+      <c r="V187" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W187">
+        <v>1</v>
+      </c>
+      <c r="X187">
+        <v>5</v>
+      </c>
+      <c r="Y187">
+        <v>1</v>
+      </c>
+      <c r="Z187">
+        <v>1</v>
+      </c>
+      <c r="AA187">
+        <f t="shared" si="127"/>
+        <v>6</v>
+      </c>
+      <c r="AB187">
+        <v>6</v>
+      </c>
+      <c r="AC187">
+        <v>3</v>
+      </c>
+      <c r="AE187" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH187" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI187" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ187" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK187" t="e">
+        <f t="shared" si="122"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ186" t="e">
+      <c r="AL187">
+        <f t="shared" si="123"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM187" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN187">
+        <v>149</v>
+      </c>
+      <c r="AO187">
+        <v>743</v>
+      </c>
+      <c r="AP187" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ187">
+        <v>120</v>
+      </c>
+      <c r="AR187">
+        <v>720</v>
+      </c>
+      <c r="AS187">
+        <v>320</v>
+      </c>
+      <c r="AT187" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU187">
+        <f t="shared" si="128"/>
+        <v>14</v>
+      </c>
+      <c r="AV187">
+        <f t="shared" si="129"/>
+        <v>11</v>
+      </c>
+      <c r="AW187">
+        <f t="shared" si="130"/>
+        <v>57</v>
+      </c>
+      <c r="AX187" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY187">
+        <f t="shared" si="124"/>
+        <v>106</v>
+      </c>
+      <c r="AZ187">
         <f t="shared" si="125"/>
+        <v>709</v>
+      </c>
+      <c r="BA187" s="8">
+        <f t="shared" si="126"/>
+        <v>263</v>
+      </c>
+      <c r="BB187" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC187" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD187" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="188" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A188" s="10" t="s">
+        <v>730</v>
+      </c>
+      <c r="B188" s="10" t="s">
+        <v>715</v>
+      </c>
+      <c r="C188" t="s">
+        <v>721</v>
+      </c>
+      <c r="D188" t="s">
+        <v>457</v>
+      </c>
+      <c r="E188" t="s">
+        <v>406</v>
+      </c>
+      <c r="F188" t="s">
+        <v>409</v>
+      </c>
+      <c r="G188" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H188" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I188" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J188" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U188" s="10"/>
+      <c r="V188" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W188">
+        <v>1</v>
+      </c>
+      <c r="X188">
+        <v>5</v>
+      </c>
+      <c r="Y188">
+        <v>1</v>
+      </c>
+      <c r="Z188">
+        <v>1</v>
+      </c>
+      <c r="AA188">
+        <f t="shared" si="127"/>
+        <v>6</v>
+      </c>
+      <c r="AB188">
+        <v>6</v>
+      </c>
+      <c r="AC188">
+        <v>3</v>
+      </c>
+      <c r="AE188" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH188" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI188" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ188" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK188" t="e">
+        <f t="shared" ref="AK188:AK191" si="131">AI188+AJ188</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA186" s="8" t="e">
-        <f t="shared" si="126"/>
+      <c r="AL188">
+        <f t="shared" ref="AL188:AL191" si="132" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ188*AR188*AS188) * (AA188 / 5) + 441</f>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM188" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN188">
+        <v>149</v>
+      </c>
+      <c r="AO188">
+        <v>743</v>
+      </c>
+      <c r="AP188" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ188">
+        <v>120</v>
+      </c>
+      <c r="AR188">
+        <v>720</v>
+      </c>
+      <c r="AS188">
+        <v>320</v>
+      </c>
+      <c r="AT188" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU188">
+        <f t="shared" si="128"/>
+        <v>14</v>
+      </c>
+      <c r="AV188">
+        <f t="shared" si="129"/>
+        <v>11</v>
+      </c>
+      <c r="AW188">
+        <f t="shared" si="130"/>
+        <v>57</v>
+      </c>
+      <c r="AX188" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY188">
+        <f t="shared" ref="AY188:AY191" si="133">AQ188-AU188</f>
+        <v>106</v>
+      </c>
+      <c r="AZ188">
+        <f t="shared" ref="AZ188:AZ191" si="134">AR188-AV188</f>
+        <v>709</v>
+      </c>
+      <c r="BA188" s="8">
+        <f t="shared" ref="BA188:BA191" si="135">AS188-AW188</f>
+        <v>263</v>
+      </c>
+      <c r="BB188" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC188" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD188" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="189" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A189" s="10" t="s">
+        <v>731</v>
+      </c>
+      <c r="B189" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="C189" t="s">
+        <v>719</v>
+      </c>
+      <c r="D189" t="s">
+        <v>457</v>
+      </c>
+      <c r="E189" t="s">
+        <v>406</v>
+      </c>
+      <c r="F189" t="s">
+        <v>636</v>
+      </c>
+      <c r="G189" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H189" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I189" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J189" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U189" s="10"/>
+      <c r="V189" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W189">
+        <v>1</v>
+      </c>
+      <c r="X189">
+        <v>5</v>
+      </c>
+      <c r="Y189">
+        <v>1</v>
+      </c>
+      <c r="Z189">
+        <v>1</v>
+      </c>
+      <c r="AA189">
+        <f t="shared" si="127"/>
+        <v>6</v>
+      </c>
+      <c r="AB189">
+        <v>6</v>
+      </c>
+      <c r="AC189">
+        <v>3</v>
+      </c>
+      <c r="AE189" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH189" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI189" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ189" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK189" t="e">
+        <f t="shared" si="131"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BB186" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC186" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD186" t="s">
+      <c r="AL189">
+        <f t="shared" si="132"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM189" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN189">
+        <v>149</v>
+      </c>
+      <c r="AO189">
+        <v>743</v>
+      </c>
+      <c r="AP189" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ189">
+        <v>120</v>
+      </c>
+      <c r="AR189">
+        <v>720</v>
+      </c>
+      <c r="AS189">
+        <v>320</v>
+      </c>
+      <c r="AT189" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU189">
+        <f t="shared" si="128"/>
+        <v>14</v>
+      </c>
+      <c r="AV189">
+        <f t="shared" si="129"/>
+        <v>11</v>
+      </c>
+      <c r="AW189">
+        <f t="shared" si="130"/>
+        <v>57</v>
+      </c>
+      <c r="AX189" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY189">
+        <f t="shared" si="133"/>
+        <v>106</v>
+      </c>
+      <c r="AZ189">
+        <f t="shared" si="134"/>
+        <v>709</v>
+      </c>
+      <c r="BA189" s="8">
+        <f t="shared" si="135"/>
+        <v>263</v>
+      </c>
+      <c r="BB189" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC189" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD189" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="190" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A190" s="10" t="s">
+        <v>732</v>
+      </c>
+      <c r="B190" s="10" t="s">
+        <v>716</v>
+      </c>
+      <c r="C190" t="s">
+        <v>722</v>
+      </c>
+      <c r="D190" t="s">
+        <v>457</v>
+      </c>
+      <c r="E190" t="s">
+        <v>406</v>
+      </c>
+      <c r="F190" t="s">
+        <v>636</v>
+      </c>
+      <c r="G190" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H190" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I190" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J190" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U190" s="10"/>
+      <c r="V190" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W190">
+        <v>1</v>
+      </c>
+      <c r="X190">
+        <v>5</v>
+      </c>
+      <c r="Y190">
+        <v>1</v>
+      </c>
+      <c r="Z190">
+        <v>1</v>
+      </c>
+      <c r="AA190">
+        <f t="shared" si="127"/>
+        <v>6</v>
+      </c>
+      <c r="AB190">
+        <v>6</v>
+      </c>
+      <c r="AC190">
+        <v>3</v>
+      </c>
+      <c r="AE190" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH190" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI190" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ190" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK190" t="e">
+        <f t="shared" si="131"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL190">
+        <f t="shared" si="132"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM190" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN190">
+        <v>149</v>
+      </c>
+      <c r="AO190">
+        <v>743</v>
+      </c>
+      <c r="AP190" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ190">
+        <v>120</v>
+      </c>
+      <c r="AR190">
+        <v>720</v>
+      </c>
+      <c r="AS190">
+        <v>320</v>
+      </c>
+      <c r="AT190" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU190">
+        <f t="shared" si="128"/>
+        <v>14</v>
+      </c>
+      <c r="AV190">
+        <f t="shared" si="129"/>
+        <v>11</v>
+      </c>
+      <c r="AW190">
+        <f t="shared" si="130"/>
+        <v>57</v>
+      </c>
+      <c r="AX190" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY190">
+        <f t="shared" si="133"/>
+        <v>106</v>
+      </c>
+      <c r="AZ190">
+        <f t="shared" si="134"/>
+        <v>709</v>
+      </c>
+      <c r="BA190" s="8">
+        <f t="shared" si="135"/>
+        <v>263</v>
+      </c>
+      <c r="BB190" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC190" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD190" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="191" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A191" s="10" t="s">
+        <v>733</v>
+      </c>
+      <c r="B191" s="10" t="s">
+        <v>717</v>
+      </c>
+      <c r="C191" t="s">
+        <v>723</v>
+      </c>
+      <c r="D191" t="s">
+        <v>457</v>
+      </c>
+      <c r="E191" t="s">
+        <v>406</v>
+      </c>
+      <c r="F191" t="s">
+        <v>636</v>
+      </c>
+      <c r="G191" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H191" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I191" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J191" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U191" s="10"/>
+      <c r="V191" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W191">
+        <v>1</v>
+      </c>
+      <c r="X191">
+        <v>5</v>
+      </c>
+      <c r="Y191">
+        <v>1</v>
+      </c>
+      <c r="Z191">
+        <v>1</v>
+      </c>
+      <c r="AA191">
+        <f t="shared" si="127"/>
+        <v>6</v>
+      </c>
+      <c r="AB191">
+        <v>6</v>
+      </c>
+      <c r="AC191">
+        <v>3</v>
+      </c>
+      <c r="AE191" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH191" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI191" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ191" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK191" t="e">
+        <f t="shared" si="131"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL191">
+        <f t="shared" si="132"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM191" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN191">
+        <v>149</v>
+      </c>
+      <c r="AO191">
+        <v>743</v>
+      </c>
+      <c r="AP191" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ191">
+        <v>120</v>
+      </c>
+      <c r="AR191">
+        <v>720</v>
+      </c>
+      <c r="AS191">
+        <v>320</v>
+      </c>
+      <c r="AT191" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU191">
+        <f t="shared" si="128"/>
+        <v>14</v>
+      </c>
+      <c r="AV191">
+        <f t="shared" si="129"/>
+        <v>11</v>
+      </c>
+      <c r="AW191">
+        <f t="shared" si="130"/>
+        <v>57</v>
+      </c>
+      <c r="AX191" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY191">
+        <f t="shared" si="133"/>
+        <v>106</v>
+      </c>
+      <c r="AZ191">
+        <f t="shared" si="134"/>
+        <v>709</v>
+      </c>
+      <c r="BA191" s="8">
+        <f t="shared" si="135"/>
+        <v>263</v>
+      </c>
+      <c r="BB191" t="s">
+        <v>726</v>
+      </c>
+      <c r="BC191" t="s">
+        <v>727</v>
+      </c>
+      <c r="BD191" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="192" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A192" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B192" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C192" t="s">
+        <v>117</v>
+      </c>
+      <c r="D192" t="s">
+        <v>117</v>
+      </c>
+      <c r="E192" t="s">
+        <v>117</v>
+      </c>
+      <c r="F192" t="s">
+        <v>117</v>
+      </c>
+      <c r="G192" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H192" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I192" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J192" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U192" s="10"/>
+      <c r="V192" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W192" t="s">
+        <v>117</v>
+      </c>
+      <c r="X192" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y192" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH192" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK192" t="e">
+        <f t="shared" ref="AK187:AK192" si="136">AI192+AJ192</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL192" t="e">
+        <f t="shared" ref="AL187:AL192" si="137" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ192*AR192*AS192) * (AA192 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM192" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP192" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT192" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW192" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX192" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY192" t="e">
+        <f t="shared" ref="AY187:AY192" si="138">AQ192-AU192</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ192" t="e">
+        <f t="shared" ref="AZ187:AZ192" si="139">AR192-AV192</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA192" s="8" t="e">
+        <f t="shared" ref="BA187:BA192" si="140">AS192-AW192</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB192" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC192" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD192" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
generic commit message, Thu 18:29:24 22.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1708ABCD-8B56-4B38-91DA-25CEF33454B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ECE07F-76F1-43AA-9971-340ADC256AAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41235" yWindow="0" windowWidth="25935" windowHeight="15750" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="41232" yWindow="0" windowWidth="25932" windowHeight="15756" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5069" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5080" uniqueCount="736">
   <si>
     <t>patch z</t>
   </si>
@@ -2299,6 +2288,9 @@
   </si>
   <si>
     <t>out of memory (probably cpu)</t>
+  </si>
+  <si>
+    <t>0 (no  log file)</t>
   </si>
 </sst>
 </file>
@@ -2931,9 +2923,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2971,7 +2963,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3077,7 +3069,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3219,7 +3211,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3230,72 +3222,72 @@
   <dimension ref="A1:BG192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AC170" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J170" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC190" sqref="AC190"/>
+      <selection pane="bottomRight" activeCell="BC192" sqref="BC192"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="57.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="57.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
     <col min="7" max="7" width="57" style="38" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="35.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="64.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8.5703125" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="35.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="64.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8.5546875" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" customWidth="1"/>
     <col min="14" max="14" width="33" customWidth="1"/>
-    <col min="15" max="21" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="9.140625" style="17" collapsed="1"/>
-    <col min="23" max="23" width="9.140625" customWidth="1"/>
-    <col min="24" max="24" width="6.7109375" customWidth="1"/>
-    <col min="25" max="25" width="5.140625" customWidth="1"/>
+    <col min="15" max="21" width="9.109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="9.109375" style="17" collapsed="1"/>
+    <col min="23" max="23" width="9.109375" customWidth="1"/>
+    <col min="24" max="24" width="6.6640625" customWidth="1"/>
+    <col min="25" max="25" width="5.109375" customWidth="1"/>
     <col min="26" max="26" width="6" customWidth="1"/>
-    <col min="27" max="27" width="11.140625" customWidth="1"/>
-    <col min="29" max="29" width="7.7109375" customWidth="1"/>
-    <col min="30" max="30" width="9.5703125" customWidth="1"/>
+    <col min="27" max="27" width="11.109375" customWidth="1"/>
+    <col min="29" max="29" width="7.6640625" customWidth="1"/>
+    <col min="30" max="30" width="9.5546875" customWidth="1"/>
     <col min="31" max="31" width="9" customWidth="1"/>
-    <col min="32" max="32" width="8.85546875" customWidth="1"/>
-    <col min="33" max="33" width="9.85546875" customWidth="1"/>
-    <col min="34" max="34" width="9.7109375" style="8" customWidth="1"/>
-    <col min="35" max="35" width="11.7109375" customWidth="1"/>
-    <col min="36" max="36" width="10.42578125" customWidth="1"/>
-    <col min="37" max="37" width="9.7109375" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" customWidth="1"/>
-    <col min="39" max="39" width="26.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="6.5703125" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.7109375" customWidth="1"/>
-    <col min="42" max="42" width="6.7109375" style="17" customWidth="1"/>
-    <col min="43" max="43" width="5.28515625" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" customWidth="1"/>
+    <col min="32" max="32" width="8.88671875" customWidth="1"/>
+    <col min="33" max="33" width="9.88671875" customWidth="1"/>
+    <col min="34" max="34" width="9.6640625" style="8" customWidth="1"/>
+    <col min="35" max="35" width="11.6640625" customWidth="1"/>
+    <col min="36" max="36" width="10.44140625" customWidth="1"/>
+    <col min="37" max="37" width="9.6640625" customWidth="1"/>
+    <col min="38" max="38" width="15.44140625" customWidth="1"/>
+    <col min="39" max="39" width="26.33203125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="6.5546875" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.6640625" customWidth="1"/>
+    <col min="42" max="42" width="6.6640625" style="17" customWidth="1"/>
+    <col min="43" max="43" width="5.33203125" customWidth="1"/>
+    <col min="44" max="44" width="6.109375" customWidth="1"/>
     <col min="45" max="45" width="5" customWidth="1"/>
     <col min="46" max="46" width="5" style="17" customWidth="1"/>
-    <col min="47" max="47" width="6.140625" customWidth="1"/>
-    <col min="48" max="48" width="6.5703125" customWidth="1"/>
+    <col min="47" max="47" width="6.109375" customWidth="1"/>
+    <col min="48" max="48" width="6.5546875" customWidth="1"/>
     <col min="49" max="49" width="5" customWidth="1"/>
     <col min="50" max="50" width="6" style="17" customWidth="1"/>
     <col min="51" max="52" width="6" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="53" max="53" width="6" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="35.42578125" customWidth="1"/>
-    <col min="56" max="56" width="5.140625" customWidth="1"/>
-    <col min="57" max="57" width="135.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="32.109375" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="35.44140625" customWidth="1"/>
+    <col min="56" max="56" width="5.109375" customWidth="1"/>
+    <col min="57" max="57" width="135.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="58" max="58" width="206" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.7109375" customWidth="1"/>
-    <col min="63" max="63" width="12.140625" customWidth="1"/>
+    <col min="59" max="59" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.6640625" customWidth="1"/>
+    <col min="63" max="63" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -3471,7 +3463,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -3639,7 +3631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3808,7 +3800,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:58" s="6" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58" s="6" customFormat="1" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>51</v>
       </c>
@@ -3976,7 +3968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -4141,7 +4133,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4306,7 +4298,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4471,7 +4463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4636,7 +4628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4807,7 +4799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -4972,7 +4964,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:58" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -5137,7 +5129,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -5303,7 +5295,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -5468,7 +5460,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -5633,7 +5625,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -5799,7 +5791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -5966,7 +5958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -6132,7 +6124,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -6298,7 +6290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -6464,7 +6456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -6630,7 +6622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -6796,7 +6788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -6962,7 +6954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -7128,7 +7120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -7294,7 +7286,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -7461,7 +7453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
@@ -7628,7 +7620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -7798,7 +7790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -7967,7 +7959,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -8137,7 +8129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -8307,7 +8299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -8477,7 +8469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -8646,7 +8638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -8815,7 +8807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -8984,7 +8976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -9153,7 +9145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>180</v>
       </c>
@@ -9322,7 +9314,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -9491,7 +9483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -9660,7 +9652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>191</v>
       </c>
@@ -9829,7 +9821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>195</v>
       </c>
@@ -9998,7 +9990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>196</v>
       </c>
@@ -10167,7 +10159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>198</v>
       </c>
@@ -10336,7 +10328,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>201</v>
       </c>
@@ -10505,7 +10497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>202</v>
       </c>
@@ -10675,7 +10667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>203</v>
       </c>
@@ -10846,7 +10838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>235</v>
       </c>
@@ -11011,7 +11003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>236</v>
       </c>
@@ -11176,7 +11168,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>237</v>
       </c>
@@ -11341,7 +11333,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>238</v>
       </c>
@@ -11506,7 +11498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>239</v>
       </c>
@@ -11671,7 +11663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>240</v>
       </c>
@@ -11836,7 +11828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>241</v>
       </c>
@@ -12001,7 +11993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>242</v>
       </c>
@@ -12166,7 +12158,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>243</v>
       </c>
@@ -12331,7 +12323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>244</v>
       </c>
@@ -12496,7 +12488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>245</v>
       </c>
@@ -12661,7 +12653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>246</v>
       </c>
@@ -12826,7 +12818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>247</v>
       </c>
@@ -12991,7 +12983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>248</v>
       </c>
@@ -13156,7 +13148,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>249</v>
       </c>
@@ -13321,7 +13313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>250</v>
       </c>
@@ -13486,7 +13478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>251</v>
       </c>
@@ -13651,7 +13643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A63" s="15" t="s">
         <v>252</v>
       </c>
@@ -13817,7 +13809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:58" s="25" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:58" s="25" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A64" s="24" t="s">
         <v>267</v>
       </c>
@@ -13987,7 +13979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>269</v>
       </c>
@@ -14164,7 +14156,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="66" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>274</v>
       </c>
@@ -14341,7 +14333,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="67" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>289</v>
       </c>
@@ -14518,7 +14510,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="68" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>292</v>
       </c>
@@ -14695,7 +14687,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
         <v>293</v>
       </c>
@@ -14872,7 +14864,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
         <v>298</v>
       </c>
@@ -15052,7 +15044,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
         <v>299</v>
       </c>
@@ -15229,7 +15221,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="72" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A72" s="10" t="s">
         <v>302</v>
       </c>
@@ -15406,7 +15398,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="73" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A73" s="10" t="s">
         <v>321</v>
       </c>
@@ -15586,7 +15578,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
         <v>323</v>
       </c>
@@ -15763,7 +15755,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="75" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>331</v>
       </c>
@@ -15937,7 +15929,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="76" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
         <v>334</v>
       </c>
@@ -16111,7 +16103,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="77" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
         <v>350</v>
       </c>
@@ -16120,7 +16112,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="78" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="s">
         <v>350</v>
       </c>
@@ -16129,7 +16121,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A79" s="10" t="s">
         <v>351</v>
       </c>
@@ -16303,7 +16295,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="80" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A80" s="10" t="s">
         <v>361</v>
       </c>
@@ -16480,7 +16472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A81" s="10" t="s">
         <v>365</v>
       </c>
@@ -16657,7 +16649,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A82" s="10" t="s">
         <v>369</v>
       </c>
@@ -16834,7 +16826,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A83" s="10" t="s">
         <v>373</v>
       </c>
@@ -17011,7 +17003,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="84" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A84" s="10" t="s">
         <v>374</v>
       </c>
@@ -17188,7 +17180,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="85" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10" t="s">
         <v>375</v>
       </c>
@@ -17365,7 +17357,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A86" s="10" t="s">
         <v>377</v>
       </c>
@@ -17542,7 +17534,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="87" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A87" s="10" t="s">
         <v>378</v>
       </c>
@@ -17719,7 +17711,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A88" s="10" t="s">
         <v>379</v>
       </c>
@@ -17896,7 +17888,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="89" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A89" s="10" t="s">
         <v>380</v>
       </c>
@@ -18073,7 +18065,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="90" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
         <v>381</v>
       </c>
@@ -18250,7 +18242,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="91" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A91" s="10" t="s">
         <v>382</v>
       </c>
@@ -18427,7 +18419,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="92" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A92" s="10" t="s">
         <v>383</v>
       </c>
@@ -18604,7 +18596,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="93" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
         <v>384</v>
       </c>
@@ -18781,7 +18773,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A94" s="10" t="s">
         <v>392</v>
       </c>
@@ -18958,7 +18950,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="95" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A95" s="10" t="s">
         <v>402</v>
       </c>
@@ -19135,7 +19127,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="96" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A96" s="10" t="s">
         <v>402</v>
       </c>
@@ -19312,7 +19304,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="97" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A97" s="10" t="s">
         <v>403</v>
       </c>
@@ -19489,7 +19481,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="98" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A98" s="10" t="s">
         <v>412</v>
       </c>
@@ -19666,7 +19658,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="99" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A99" s="10" t="s">
         <v>413</v>
       </c>
@@ -19843,7 +19835,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="100" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A100" s="10" t="s">
         <v>429</v>
       </c>
@@ -20023,7 +20015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A101" s="10" t="s">
         <v>432</v>
       </c>
@@ -20203,7 +20195,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A102" s="10" t="s">
         <v>433</v>
       </c>
@@ -20383,7 +20375,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="103" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A103" s="10" t="s">
         <v>434</v>
       </c>
@@ -20565,7 +20557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A104" s="10" t="s">
         <v>435</v>
       </c>
@@ -20747,7 +20739,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="105" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A105" s="10" t="s">
         <v>436</v>
       </c>
@@ -20929,7 +20921,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="106" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A106" s="10" t="s">
         <v>431</v>
       </c>
@@ -21111,7 +21103,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="107" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A107" s="10" t="s">
         <v>456</v>
       </c>
@@ -21290,7 +21282,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A108" s="10" t="s">
         <v>460</v>
       </c>
@@ -21472,7 +21464,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A109" s="10" t="s">
         <v>466</v>
       </c>
@@ -21651,7 +21643,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="110" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A110" s="10" t="s">
         <v>470</v>
       </c>
@@ -21833,7 +21825,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="111" spans="1:58" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:58" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="32" t="s">
         <v>472</v>
       </c>
@@ -22015,7 +22007,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:58" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:58" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="45" t="s">
         <v>476</v>
       </c>
@@ -22194,7 +22186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A113" s="10" t="s">
         <v>484</v>
       </c>
@@ -22378,7 +22370,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A114" s="10" t="s">
         <v>485</v>
       </c>
@@ -22504,7 +22496,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A115" s="10" t="s">
         <v>493</v>
       </c>
@@ -22630,7 +22622,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A116" s="10" t="s">
         <v>494</v>
       </c>
@@ -22758,7 +22750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A117" s="10" t="s">
         <v>505</v>
       </c>
@@ -22886,7 +22878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A118" s="10" t="s">
         <v>504</v>
       </c>
@@ -23014,7 +23006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A119" s="10" t="s">
         <v>502</v>
       </c>
@@ -23142,7 +23134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A120" s="10" t="s">
         <v>507</v>
       </c>
@@ -23292,7 +23284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A121" s="10" t="s">
         <v>508</v>
       </c>
@@ -23442,7 +23434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A122" s="10" t="s">
         <v>520</v>
       </c>
@@ -23573,7 +23565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A123" s="10" t="s">
         <v>521</v>
       </c>
@@ -23704,7 +23696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A124" s="10" t="s">
         <v>522</v>
       </c>
@@ -23835,7 +23827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A125" s="10" t="s">
         <v>523</v>
       </c>
@@ -23966,7 +23958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A126" s="10" t="s">
         <v>529</v>
       </c>
@@ -24111,7 +24103,7 @@
       </c>
       <c r="BF126" s="1"/>
     </row>
-    <row r="127" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A127" s="10" t="s">
         <v>530</v>
       </c>
@@ -24259,7 +24251,7 @@
       </c>
       <c r="BF127" s="1"/>
     </row>
-    <row r="128" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A128" s="10" t="s">
         <v>531</v>
       </c>
@@ -24407,7 +24399,7 @@
       </c>
       <c r="BF128" s="1"/>
     </row>
-    <row r="129" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A129" s="10" t="s">
         <v>532</v>
       </c>
@@ -24555,7 +24547,7 @@
       </c>
       <c r="BF129" s="1"/>
     </row>
-    <row r="130" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="15" t="s">
         <v>534</v>
       </c>
@@ -24702,7 +24694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A131" s="10" t="s">
         <v>541</v>
       </c>
@@ -24846,7 +24838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A132" s="10" t="s">
         <v>542</v>
       </c>
@@ -24990,7 +24982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A133" s="10" t="s">
         <v>543</v>
       </c>
@@ -25134,7 +25126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A134" s="10" t="s">
         <v>544</v>
       </c>
@@ -25278,7 +25270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A135" s="10" t="s">
         <v>545</v>
       </c>
@@ -25422,7 +25414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A136" s="10" t="s">
         <v>546</v>
       </c>
@@ -25566,7 +25558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A137" s="10" t="s">
         <v>547</v>
       </c>
@@ -25710,7 +25702,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="138" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A138" s="10" t="s">
         <v>548</v>
       </c>
@@ -25854,7 +25846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A139" s="10" t="s">
         <v>549</v>
       </c>
@@ -25997,7 +25989,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="140" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="15" t="s">
         <v>570</v>
       </c>
@@ -26144,7 +26136,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="141" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A141" s="10" t="s">
         <v>578</v>
       </c>
@@ -26278,7 +26270,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="142" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A142" s="10" t="s">
         <v>579</v>
       </c>
@@ -26412,7 +26404,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="143" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A143" s="10" t="s">
         <v>580</v>
       </c>
@@ -26546,7 +26538,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="144" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A144" s="10" t="s">
         <v>581</v>
       </c>
@@ -26680,7 +26672,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A145" s="10" t="s">
         <v>582</v>
       </c>
@@ -26814,7 +26806,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="146" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A146" s="10" t="s">
         <v>583</v>
       </c>
@@ -26948,7 +26940,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="147" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A147" s="10" t="s">
         <v>584</v>
       </c>
@@ -27082,7 +27074,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="148" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A148" s="10" t="s">
         <v>585</v>
       </c>
@@ -27216,7 +27208,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="149" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="32" t="s">
         <v>586</v>
       </c>
@@ -27345,7 +27337,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="150" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A150" s="10" t="s">
         <v>587</v>
       </c>
@@ -27483,7 +27475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A151" s="10" t="s">
         <v>588</v>
       </c>
@@ -27621,7 +27613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A152" s="10" t="s">
         <v>596</v>
       </c>
@@ -27750,7 +27742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A153" s="10" t="s">
         <v>597</v>
       </c>
@@ -27885,7 +27877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A154" s="10" t="s">
         <v>602</v>
       </c>
@@ -28026,7 +28018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A155" s="10" t="s">
         <v>610</v>
       </c>
@@ -28164,7 +28156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A156" s="10" t="s">
         <v>611</v>
       </c>
@@ -28302,7 +28294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A157" s="10" t="s">
         <v>626</v>
       </c>
@@ -28447,7 +28439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>632</v>
       </c>
@@ -28575,7 +28567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>633</v>
       </c>
@@ -28703,7 +28695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>634</v>
       </c>
@@ -28831,7 +28823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="32" t="s">
         <v>654</v>
       </c>
@@ -28972,7 +28964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="32" t="s">
         <v>655</v>
       </c>
@@ -29113,7 +29105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="32" t="s">
         <v>656</v>
       </c>
@@ -29254,7 +29246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="32" t="s">
         <v>652</v>
       </c>
@@ -29398,7 +29390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="32" t="s">
         <v>653</v>
       </c>
@@ -29542,7 +29534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:56" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:56" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="70" t="s">
         <v>661</v>
       </c>
@@ -29686,7 +29678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A167" s="68" t="s">
         <v>666</v>
       </c>
@@ -29824,7 +29816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A168" s="68" t="s">
         <v>667</v>
       </c>
@@ -29962,7 +29954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A169" s="68" t="s">
         <v>674</v>
       </c>
@@ -30100,7 +30092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A170" s="68" t="s">
         <v>694</v>
       </c>
@@ -30222,7 +30214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A171" s="10" t="s">
         <v>697</v>
       </c>
@@ -30355,7 +30347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A172" s="10" t="s">
         <v>698</v>
       </c>
@@ -30488,7 +30480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A173" s="10" t="s">
         <v>699</v>
       </c>
@@ -30621,7 +30613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A174" s="10" t="s">
         <v>700</v>
       </c>
@@ -30754,7 +30746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A175" s="10" t="s">
         <v>701</v>
       </c>
@@ -30887,7 +30879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A176" s="10" t="s">
         <v>702</v>
       </c>
@@ -31020,7 +31012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A177" s="10" t="s">
         <v>703</v>
       </c>
@@ -31153,7 +31145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A178" s="10" t="s">
         <v>704</v>
       </c>
@@ -31286,7 +31278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="15" t="s">
         <v>705</v>
       </c>
@@ -31420,7 +31412,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="180" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A180" s="10" t="s">
         <v>706</v>
       </c>
@@ -31458,8 +31450,8 @@
         <v>450</v>
       </c>
       <c r="U180" s="10"/>
-      <c r="V180" s="17">
-        <v>0</v>
+      <c r="V180" s="17" t="s">
+        <v>735</v>
       </c>
       <c r="W180">
         <v>1</v>
@@ -31567,7 +31559,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="181" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A181" s="10" t="s">
         <v>707</v>
       </c>
@@ -31605,8 +31597,8 @@
         <v>450</v>
       </c>
       <c r="U181" s="10"/>
-      <c r="V181" s="17">
-        <v>0</v>
+      <c r="V181" s="17" t="s">
+        <v>735</v>
       </c>
       <c r="W181">
         <v>1</v>
@@ -31714,7 +31706,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="182" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A182" s="10" t="s">
         <v>708</v>
       </c>
@@ -31752,8 +31744,8 @@
         <v>450</v>
       </c>
       <c r="U182" s="10"/>
-      <c r="V182" s="17">
-        <v>0</v>
+      <c r="V182" s="17" t="s">
+        <v>735</v>
       </c>
       <c r="W182">
         <v>1</v>
@@ -31861,7 +31853,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="183" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A183" s="10" t="s">
         <v>709</v>
       </c>
@@ -31899,8 +31891,8 @@
         <v>450</v>
       </c>
       <c r="U183" s="10"/>
-      <c r="V183" s="17">
-        <v>0</v>
+      <c r="V183" s="17" t="s">
+        <v>735</v>
       </c>
       <c r="W183">
         <v>1</v>
@@ -32008,7 +32000,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="184" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A184" s="10" t="s">
         <v>710</v>
       </c>
@@ -32046,8 +32038,8 @@
         <v>450</v>
       </c>
       <c r="U184" s="10"/>
-      <c r="V184" s="17">
-        <v>0</v>
+      <c r="V184" s="17" t="s">
+        <v>735</v>
       </c>
       <c r="W184">
         <v>1</v>
@@ -32155,7 +32147,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="185" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="15" t="s">
         <v>711</v>
       </c>
@@ -32193,8 +32185,8 @@
         <v>450</v>
       </c>
       <c r="U185" s="15"/>
-      <c r="V185" s="19">
-        <v>0</v>
+      <c r="V185" s="19" t="s">
+        <v>735</v>
       </c>
       <c r="W185" s="3">
         <v>1</v>
@@ -32302,7 +32294,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="186" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A186" s="10" t="s">
         <v>728</v>
       </c>
@@ -32335,7 +32327,7 @@
       </c>
       <c r="U186" s="10"/>
       <c r="V186" s="17" t="s">
-        <v>117</v>
+        <v>735</v>
       </c>
       <c r="W186">
         <v>1</v>
@@ -32354,7 +32346,7 @@
         <v>6</v>
       </c>
       <c r="AB186">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC186">
         <v>3</v>
@@ -32440,7 +32432,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="187" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A187" s="10" t="s">
         <v>729</v>
       </c>
@@ -32473,7 +32465,7 @@
       </c>
       <c r="U187" s="10"/>
       <c r="V187" s="17" t="s">
-        <v>117</v>
+        <v>735</v>
       </c>
       <c r="W187">
         <v>1</v>
@@ -32491,8 +32483,8 @@
         <f t="shared" si="127"/>
         <v>6</v>
       </c>
-      <c r="AB187">
-        <v>6</v>
+      <c r="AB187" t="s">
+        <v>117</v>
       </c>
       <c r="AC187">
         <v>3</v>
@@ -32578,7 +32570,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="188" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A188" s="10" t="s">
         <v>730</v>
       </c>
@@ -32611,7 +32603,7 @@
       </c>
       <c r="U188" s="10"/>
       <c r="V188" s="17" t="s">
-        <v>117</v>
+        <v>735</v>
       </c>
       <c r="W188">
         <v>1</v>
@@ -32629,8 +32621,8 @@
         <f t="shared" si="127"/>
         <v>6</v>
       </c>
-      <c r="AB188">
-        <v>6</v>
+      <c r="AB188" t="s">
+        <v>117</v>
       </c>
       <c r="AC188">
         <v>3</v>
@@ -32716,7 +32708,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="189" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A189" s="10" t="s">
         <v>731</v>
       </c>
@@ -32749,7 +32741,7 @@
       </c>
       <c r="U189" s="10"/>
       <c r="V189" s="17" t="s">
-        <v>117</v>
+        <v>735</v>
       </c>
       <c r="W189">
         <v>1</v>
@@ -32767,8 +32759,8 @@
         <f t="shared" si="127"/>
         <v>6</v>
       </c>
-      <c r="AB189">
-        <v>6</v>
+      <c r="AB189" t="s">
+        <v>117</v>
       </c>
       <c r="AC189">
         <v>3</v>
@@ -32854,7 +32846,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="190" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A190" s="10" t="s">
         <v>732</v>
       </c>
@@ -32887,7 +32879,7 @@
       </c>
       <c r="U190" s="10"/>
       <c r="V190" s="17" t="s">
-        <v>117</v>
+        <v>735</v>
       </c>
       <c r="W190">
         <v>1</v>
@@ -32905,8 +32897,8 @@
         <f t="shared" si="127"/>
         <v>6</v>
       </c>
-      <c r="AB190">
-        <v>6</v>
+      <c r="AB190" t="s">
+        <v>117</v>
       </c>
       <c r="AC190">
         <v>3</v>
@@ -32992,7 +32984,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="191" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A191" s="10" t="s">
         <v>733</v>
       </c>
@@ -33025,7 +33017,7 @@
       </c>
       <c r="U191" s="10"/>
       <c r="V191" s="17" t="s">
-        <v>117</v>
+        <v>735</v>
       </c>
       <c r="W191">
         <v>1</v>
@@ -33043,8 +33035,8 @@
         <f t="shared" si="127"/>
         <v>6</v>
       </c>
-      <c r="AB191">
-        <v>6</v>
+      <c r="AB191" t="s">
+        <v>117</v>
       </c>
       <c r="AC191">
         <v>3</v>
@@ -33130,7 +33122,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="192" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A192" s="10" t="s">
         <v>117</v>
       </c>
@@ -33199,11 +33191,11 @@
         <v>117</v>
       </c>
       <c r="AK192" t="e">
-        <f t="shared" ref="AK187:AK192" si="136">AI192+AJ192</f>
+        <f t="shared" ref="AK192" si="136">AI192+AJ192</f>
         <v>#VALUE!</v>
       </c>
       <c r="AL192" t="e">
-        <f t="shared" ref="AL187:AL192" si="137" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ192*AR192*AS192) * (AA192 / 5) + 441</f>
+        <f t="shared" ref="AL192" si="137" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ192*AR192*AS192) * (AA192 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
       <c r="AM192" s="8" t="s">
@@ -33243,15 +33235,15 @@
         <v>8</v>
       </c>
       <c r="AY192" t="e">
-        <f t="shared" ref="AY187:AY192" si="138">AQ192-AU192</f>
+        <f t="shared" ref="AY192" si="138">AQ192-AU192</f>
         <v>#VALUE!</v>
       </c>
       <c r="AZ192" t="e">
-        <f t="shared" ref="AZ187:AZ192" si="139">AR192-AV192</f>
+        <f t="shared" ref="AZ192" si="139">AR192-AV192</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA192" s="8" t="e">
-        <f t="shared" ref="BA187:BA192" si="140">AS192-AW192</f>
+        <f t="shared" ref="BA192" si="140">AS192-AW192</f>
         <v>#VALUE!</v>
       </c>
       <c r="BB192" t="s">

</xml_diff>

<commit_message>
generic commit message, Mon 10:33:17 26.02.2024.
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27ECE07F-76F1-43AA-9971-340ADC256AAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB14EE8-CBEC-48AD-939D-5BF7FE073A13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41232" yWindow="0" windowWidth="25932" windowHeight="15756" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="41232" yWindow="0" windowWidth="4848" windowHeight="15756" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5080" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5398" uniqueCount="760">
   <si>
     <t>patch z</t>
   </si>
@@ -2291,6 +2291,78 @@
   </si>
   <si>
     <t>0 (no  log file)</t>
+  </si>
+  <si>
+    <t>240226-0</t>
+  </si>
+  <si>
+    <t>240226-1</t>
+  </si>
+  <si>
+    <t>240226-2</t>
+  </si>
+  <si>
+    <t>240226-3</t>
+  </si>
+  <si>
+    <t>240226-4</t>
+  </si>
+  <si>
+    <t>240226-5</t>
+  </si>
+  <si>
+    <t>240226-6</t>
+  </si>
+  <si>
+    <t>240226-7</t>
+  </si>
+  <si>
+    <t>240226-8</t>
+  </si>
+  <si>
+    <t>240226-9</t>
+  </si>
+  <si>
+    <t>240226-10</t>
+  </si>
+  <si>
+    <t>240226-11</t>
+  </si>
+  <si>
+    <t>240221-0 best, autofluo kidney, boundary model type, id07 test, id05 val</t>
+  </si>
+  <si>
+    <t>240221-0 last, autofluo kidney, boundary model type, id07 test, id05 val</t>
+  </si>
+  <si>
+    <t>240221-1 best, autofluo kidney, boundary model type, id02 test, id01 val</t>
+  </si>
+  <si>
+    <t>240221-2 best, autofluo kidney, boundary model type, id04 test, id06 val</t>
+  </si>
+  <si>
+    <t>240221-2 last, autofluo kidney, boundary model type, id04 test, id06 val</t>
+  </si>
+  <si>
+    <t>240221-3 best, autofluo kidney, nuclei model type, id07 test, id05 val</t>
+  </si>
+  <si>
+    <t>240221-1 last, autofluo kidney, boundary model type, id02 test, id01 val</t>
+  </si>
+  <si>
+    <t>240221-4 best, autofluo kidney, nuclei model type, id02 test, id01 val</t>
+  </si>
+  <si>
+    <t>240221-3 last, autofluo kidney, nuclei model type, id07 test, id05 val</t>
+  </si>
+  <si>
+    <t>240221-4 last, autofluo kidney, nuclei model type, id02 test, id01 val</t>
+  </si>
+  <si>
+    <t>240221-5 best, autofluo kidney, nuclei model type, id04 test, id06 val</t>
+  </si>
+  <si>
+    <t>240221-5 last, autofluo kidney, nuclei model type, id04 test, id06 val</t>
   </si>
 </sst>
 </file>
@@ -3219,19 +3291,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG192"/>
+  <dimension ref="A1:BG204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J170" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="W150" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BC192" sqref="BC192"/>
+      <selection pane="bottomRight" activeCell="AA194" sqref="AA194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="57.6640625" customWidth="1"/>
+    <col min="2" max="2" width="69.5546875" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
     <col min="5" max="5" width="6.5546875" customWidth="1"/>
@@ -32322,8 +32394,8 @@
       <c r="I186" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J186" s="4" t="s">
-        <v>117</v>
+      <c r="J186" s="4">
+        <v>1</v>
       </c>
       <c r="U186" s="10"/>
       <c r="V186" s="17" t="s">
@@ -32460,8 +32532,8 @@
       <c r="I187" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J187" s="4" t="s">
-        <v>117</v>
+      <c r="J187" s="4">
+        <v>1</v>
       </c>
       <c r="U187" s="10"/>
       <c r="V187" s="17" t="s">
@@ -32598,8 +32670,8 @@
       <c r="I188" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J188" s="4" t="s">
-        <v>117</v>
+      <c r="J188" s="4">
+        <v>1</v>
       </c>
       <c r="U188" s="10"/>
       <c r="V188" s="17" t="s">
@@ -32736,8 +32808,8 @@
       <c r="I189" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J189" s="4" t="s">
-        <v>117</v>
+      <c r="J189" s="4">
+        <v>1</v>
       </c>
       <c r="U189" s="10"/>
       <c r="V189" s="17" t="s">
@@ -32874,8 +32946,8 @@
       <c r="I190" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J190" s="4" t="s">
-        <v>117</v>
+      <c r="J190" s="4">
+        <v>1</v>
       </c>
       <c r="U190" s="10"/>
       <c r="V190" s="17" t="s">
@@ -33012,8 +33084,8 @@
       <c r="I191" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J191" s="4" t="s">
-        <v>117</v>
+      <c r="J191" s="4">
+        <v>1</v>
       </c>
       <c r="U191" s="10"/>
       <c r="V191" s="17" t="s">
@@ -33124,22 +33196,22 @@
     </row>
     <row r="192" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A192" s="10" t="s">
-        <v>117</v>
+        <v>736</v>
       </c>
       <c r="B192" s="10" t="s">
-        <v>117</v>
+        <v>748</v>
       </c>
       <c r="C192" t="s">
-        <v>117</v>
+        <v>718</v>
       </c>
       <c r="D192" t="s">
-        <v>117</v>
+        <v>477</v>
       </c>
       <c r="E192" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="F192" t="s">
-        <v>117</v>
+        <v>409</v>
       </c>
       <c r="G192" s="40" t="s">
         <v>117</v>
@@ -33175,8 +33247,8 @@
       <c r="AB192" t="s">
         <v>117</v>
       </c>
-      <c r="AC192" t="s">
-        <v>117</v>
+      <c r="AC192">
+        <v>3</v>
       </c>
       <c r="AE192" t="s">
         <v>117</v>
@@ -33201,58 +33273,1702 @@
       <c r="AM192" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AN192" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO192" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP192" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ192" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR192" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS192" t="s">
-        <v>117</v>
+      <c r="AN192">
+        <v>149</v>
+      </c>
+      <c r="AO192">
+        <v>743</v>
+      </c>
+      <c r="AP192" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ192">
+        <v>120</v>
+      </c>
+      <c r="AR192">
+        <v>720</v>
+      </c>
+      <c r="AS192">
+        <v>320</v>
       </c>
       <c r="AT192" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="AU192" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV192" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW192" t="s">
-        <v>117</v>
+      <c r="AU192">
+        <f t="shared" ref="AU192:AU203" si="138" xml:space="preserve"> _xlfn.FLOOR.MATH((AN192 - AQ192) / 2)</f>
+        <v>14</v>
+      </c>
+      <c r="AV192">
+        <f t="shared" ref="AV192:AV203" si="139" xml:space="preserve"> _xlfn.FLOOR.MATH((AO192 - AR192) / 2)</f>
+        <v>11</v>
+      </c>
+      <c r="AW192">
+        <f t="shared" ref="AW192:AW203" si="140" xml:space="preserve"> _xlfn.FLOOR.MATH((AP192 - AS192) / 2)</f>
+        <v>57</v>
       </c>
       <c r="AX192" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="AY192" t="e">
-        <f t="shared" ref="AY192" si="138">AQ192-AU192</f>
+      <c r="AY192">
+        <f t="shared" ref="AY192" si="141">AQ192-AU192</f>
+        <v>106</v>
+      </c>
+      <c r="AZ192">
+        <f t="shared" ref="AZ192" si="142">AR192-AV192</f>
+        <v>709</v>
+      </c>
+      <c r="BA192" s="8">
+        <f t="shared" ref="BA192" si="143">AS192-AW192</f>
+        <v>263</v>
+      </c>
+      <c r="BB192" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC192" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD192" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="193" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A193" s="10" t="s">
+        <v>737</v>
+      </c>
+      <c r="B193" s="10" t="s">
+        <v>749</v>
+      </c>
+      <c r="C193" t="s">
+        <v>718</v>
+      </c>
+      <c r="D193" t="s">
+        <v>477</v>
+      </c>
+      <c r="E193" t="s">
+        <v>406</v>
+      </c>
+      <c r="F193" t="s">
+        <v>409</v>
+      </c>
+      <c r="G193" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H193" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I193" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J193" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U193" s="10"/>
+      <c r="V193" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W193" t="s">
+        <v>117</v>
+      </c>
+      <c r="X193" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y193" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z193" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA193" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB193" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC193">
+        <v>3</v>
+      </c>
+      <c r="AE193" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH193" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI193" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ193" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK193" t="e">
+        <f t="shared" ref="AK193:AK198" si="144">AI193+AJ193</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ192" t="e">
-        <f t="shared" ref="AZ192" si="139">AR192-AV192</f>
+      <c r="AL193" t="e">
+        <f t="shared" ref="AL193:AL198" si="145" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ193*AR193*AS193) * (AA193 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA192" s="8" t="e">
-        <f t="shared" ref="BA192" si="140">AS192-AW192</f>
+      <c r="AM193" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN193">
+        <v>149</v>
+      </c>
+      <c r="AO193">
+        <v>743</v>
+      </c>
+      <c r="AP193" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ193">
+        <v>120</v>
+      </c>
+      <c r="AR193">
+        <v>720</v>
+      </c>
+      <c r="AS193">
+        <v>320</v>
+      </c>
+      <c r="AT193" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU193">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV193">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW193">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX193" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY193">
+        <f t="shared" ref="AY193:AY198" si="146">AQ193-AU193</f>
+        <v>106</v>
+      </c>
+      <c r="AZ193">
+        <f t="shared" ref="AZ193:AZ198" si="147">AR193-AV193</f>
+        <v>709</v>
+      </c>
+      <c r="BA193" s="8">
+        <f t="shared" ref="BA193:BA198" si="148">AS193-AW193</f>
+        <v>263</v>
+      </c>
+      <c r="BB193" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC193" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD193" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="194" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A194" s="10" t="s">
+        <v>738</v>
+      </c>
+      <c r="B194" s="10" t="s">
+        <v>750</v>
+      </c>
+      <c r="C194" t="s">
+        <v>720</v>
+      </c>
+      <c r="D194" t="s">
+        <v>477</v>
+      </c>
+      <c r="E194" t="s">
+        <v>406</v>
+      </c>
+      <c r="F194" t="s">
+        <v>409</v>
+      </c>
+      <c r="G194" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H194" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I194" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J194" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U194" s="10"/>
+      <c r="V194" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W194" t="s">
+        <v>117</v>
+      </c>
+      <c r="X194" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y194" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z194" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA194" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB194" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC194">
+        <v>3</v>
+      </c>
+      <c r="AE194" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH194" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI194" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ194" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK194" t="e">
+        <f t="shared" si="144"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BB192" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC192" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD192" t="s">
+      <c r="AL194" t="e">
+        <f t="shared" si="145"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM194" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN194">
+        <v>149</v>
+      </c>
+      <c r="AO194">
+        <v>743</v>
+      </c>
+      <c r="AP194" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ194">
+        <v>120</v>
+      </c>
+      <c r="AR194">
+        <v>720</v>
+      </c>
+      <c r="AS194">
+        <v>320</v>
+      </c>
+      <c r="AT194" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU194">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV194">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW194">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX194" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY194">
+        <f t="shared" si="146"/>
+        <v>106</v>
+      </c>
+      <c r="AZ194">
+        <f t="shared" si="147"/>
+        <v>709</v>
+      </c>
+      <c r="BA194" s="8">
+        <f t="shared" si="148"/>
+        <v>263</v>
+      </c>
+      <c r="BB194" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC194" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD194" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="195" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A195" s="10" t="s">
+        <v>739</v>
+      </c>
+      <c r="B195" s="10" t="s">
+        <v>754</v>
+      </c>
+      <c r="C195" t="s">
+        <v>720</v>
+      </c>
+      <c r="D195" t="s">
+        <v>477</v>
+      </c>
+      <c r="E195" t="s">
+        <v>406</v>
+      </c>
+      <c r="F195" t="s">
+        <v>409</v>
+      </c>
+      <c r="G195" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H195" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I195" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J195" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U195" s="10"/>
+      <c r="V195" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W195" t="s">
+        <v>117</v>
+      </c>
+      <c r="X195" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y195" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z195" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA195" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB195" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC195">
+        <v>3</v>
+      </c>
+      <c r="AE195" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH195" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI195" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ195" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK195" t="e">
+        <f t="shared" si="144"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL195" t="e">
+        <f t="shared" si="145"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM195" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN195">
+        <v>149</v>
+      </c>
+      <c r="AO195">
+        <v>743</v>
+      </c>
+      <c r="AP195" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ195">
+        <v>120</v>
+      </c>
+      <c r="AR195">
+        <v>720</v>
+      </c>
+      <c r="AS195">
+        <v>320</v>
+      </c>
+      <c r="AT195" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU195">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV195">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW195">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX195" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY195">
+        <f t="shared" si="146"/>
+        <v>106</v>
+      </c>
+      <c r="AZ195">
+        <f t="shared" si="147"/>
+        <v>709</v>
+      </c>
+      <c r="BA195" s="8">
+        <f t="shared" si="148"/>
+        <v>263</v>
+      </c>
+      <c r="BB195" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC195" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD195" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="196" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A196" s="10" t="s">
+        <v>740</v>
+      </c>
+      <c r="B196" s="10" t="s">
+        <v>751</v>
+      </c>
+      <c r="C196" t="s">
+        <v>721</v>
+      </c>
+      <c r="D196" t="s">
+        <v>477</v>
+      </c>
+      <c r="E196" t="s">
+        <v>406</v>
+      </c>
+      <c r="F196" t="s">
+        <v>409</v>
+      </c>
+      <c r="G196" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H196" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I196" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J196" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U196" s="10"/>
+      <c r="V196" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W196" t="s">
+        <v>117</v>
+      </c>
+      <c r="X196" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y196" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z196" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA196" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB196" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC196">
+        <v>3</v>
+      </c>
+      <c r="AE196" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH196" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI196" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ196" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK196" t="e">
+        <f t="shared" si="144"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL196" t="e">
+        <f t="shared" si="145"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM196" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN196">
+        <v>149</v>
+      </c>
+      <c r="AO196">
+        <v>743</v>
+      </c>
+      <c r="AP196" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ196">
+        <v>120</v>
+      </c>
+      <c r="AR196">
+        <v>720</v>
+      </c>
+      <c r="AS196">
+        <v>320</v>
+      </c>
+      <c r="AT196" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU196">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV196">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW196">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX196" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY196">
+        <f t="shared" si="146"/>
+        <v>106</v>
+      </c>
+      <c r="AZ196">
+        <f t="shared" si="147"/>
+        <v>709</v>
+      </c>
+      <c r="BA196" s="8">
+        <f t="shared" si="148"/>
+        <v>263</v>
+      </c>
+      <c r="BB196" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC196" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD196" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="197" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A197" s="10" t="s">
+        <v>741</v>
+      </c>
+      <c r="B197" s="10" t="s">
+        <v>752</v>
+      </c>
+      <c r="C197" t="s">
+        <v>721</v>
+      </c>
+      <c r="D197" t="s">
+        <v>477</v>
+      </c>
+      <c r="E197" t="s">
+        <v>406</v>
+      </c>
+      <c r="F197" t="s">
+        <v>409</v>
+      </c>
+      <c r="G197" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H197" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I197" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J197" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U197" s="10"/>
+      <c r="V197" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W197" t="s">
+        <v>117</v>
+      </c>
+      <c r="X197" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y197" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z197" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA197" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB197" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC197">
+        <v>3</v>
+      </c>
+      <c r="AE197" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH197" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI197" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ197" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK197" t="e">
+        <f t="shared" si="144"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL197" t="e">
+        <f t="shared" si="145"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM197" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN197">
+        <v>149</v>
+      </c>
+      <c r="AO197">
+        <v>743</v>
+      </c>
+      <c r="AP197" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ197">
+        <v>120</v>
+      </c>
+      <c r="AR197">
+        <v>720</v>
+      </c>
+      <c r="AS197">
+        <v>320</v>
+      </c>
+      <c r="AT197" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU197">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV197">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW197">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX197" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY197">
+        <f t="shared" si="146"/>
+        <v>106</v>
+      </c>
+      <c r="AZ197">
+        <f t="shared" si="147"/>
+        <v>709</v>
+      </c>
+      <c r="BA197" s="8">
+        <f t="shared" si="148"/>
+        <v>263</v>
+      </c>
+      <c r="BB197" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC197" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD197" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="198" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A198" s="10" t="s">
+        <v>742</v>
+      </c>
+      <c r="B198" s="10" t="s">
+        <v>753</v>
+      </c>
+      <c r="C198" t="s">
+        <v>719</v>
+      </c>
+      <c r="D198" t="s">
+        <v>477</v>
+      </c>
+      <c r="E198" t="s">
+        <v>406</v>
+      </c>
+      <c r="F198" t="s">
+        <v>636</v>
+      </c>
+      <c r="G198" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H198" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I198" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J198" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U198" s="10"/>
+      <c r="V198" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W198" t="s">
+        <v>117</v>
+      </c>
+      <c r="X198" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y198" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z198" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA198" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB198" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC198">
+        <v>3</v>
+      </c>
+      <c r="AE198" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH198" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI198" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ198" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK198" t="e">
+        <f t="shared" si="144"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL198" t="e">
+        <f t="shared" si="145"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM198" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN198">
+        <v>149</v>
+      </c>
+      <c r="AO198">
+        <v>743</v>
+      </c>
+      <c r="AP198" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ198">
+        <v>120</v>
+      </c>
+      <c r="AR198">
+        <v>720</v>
+      </c>
+      <c r="AS198">
+        <v>320</v>
+      </c>
+      <c r="AT198" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU198">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV198">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW198">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX198" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY198">
+        <f t="shared" si="146"/>
+        <v>106</v>
+      </c>
+      <c r="AZ198">
+        <f t="shared" si="147"/>
+        <v>709</v>
+      </c>
+      <c r="BA198" s="8">
+        <f t="shared" si="148"/>
+        <v>263</v>
+      </c>
+      <c r="BB198" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC198" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD198" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="199" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A199" s="10" t="s">
+        <v>743</v>
+      </c>
+      <c r="B199" s="10" t="s">
+        <v>756</v>
+      </c>
+      <c r="C199" t="s">
+        <v>719</v>
+      </c>
+      <c r="D199" t="s">
+        <v>477</v>
+      </c>
+      <c r="E199" t="s">
+        <v>406</v>
+      </c>
+      <c r="F199" t="s">
+        <v>636</v>
+      </c>
+      <c r="G199" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H199" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I199" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J199" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U199" s="10"/>
+      <c r="V199" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W199" t="s">
+        <v>117</v>
+      </c>
+      <c r="X199" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y199" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z199" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA199" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB199" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC199">
+        <v>3</v>
+      </c>
+      <c r="AE199" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH199" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI199" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ199" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK199" t="e">
+        <f t="shared" ref="AK199:AK204" si="149">AI199+AJ199</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL199" t="e">
+        <f t="shared" ref="AL199:AL204" si="150" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ199*AR199*AS199) * (AA199 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM199" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN199">
+        <v>149</v>
+      </c>
+      <c r="AO199">
+        <v>743</v>
+      </c>
+      <c r="AP199" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ199">
+        <v>120</v>
+      </c>
+      <c r="AR199">
+        <v>720</v>
+      </c>
+      <c r="AS199">
+        <v>320</v>
+      </c>
+      <c r="AT199" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU199">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV199">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW199">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX199" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY199">
+        <f t="shared" ref="AY199:AY204" si="151">AQ199-AU199</f>
+        <v>106</v>
+      </c>
+      <c r="AZ199">
+        <f t="shared" ref="AZ199:AZ204" si="152">AR199-AV199</f>
+        <v>709</v>
+      </c>
+      <c r="BA199" s="8">
+        <f t="shared" ref="BA199:BA204" si="153">AS199-AW199</f>
+        <v>263</v>
+      </c>
+      <c r="BB199" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC199" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD199" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="200" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A200" s="10" t="s">
+        <v>744</v>
+      </c>
+      <c r="B200" s="10" t="s">
+        <v>755</v>
+      </c>
+      <c r="C200" t="s">
+        <v>722</v>
+      </c>
+      <c r="D200" t="s">
+        <v>477</v>
+      </c>
+      <c r="E200" t="s">
+        <v>406</v>
+      </c>
+      <c r="F200" t="s">
+        <v>636</v>
+      </c>
+      <c r="G200" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H200" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I200" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J200" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U200" s="10"/>
+      <c r="V200" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W200" t="s">
+        <v>117</v>
+      </c>
+      <c r="X200" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y200" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z200" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA200" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB200" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC200">
+        <v>3</v>
+      </c>
+      <c r="AE200" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH200" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI200" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ200" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK200" t="e">
+        <f t="shared" si="149"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL200" t="e">
+        <f t="shared" si="150"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM200" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN200">
+        <v>149</v>
+      </c>
+      <c r="AO200">
+        <v>743</v>
+      </c>
+      <c r="AP200" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ200">
+        <v>120</v>
+      </c>
+      <c r="AR200">
+        <v>720</v>
+      </c>
+      <c r="AS200">
+        <v>320</v>
+      </c>
+      <c r="AT200" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU200">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV200">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW200">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX200" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY200">
+        <f t="shared" si="151"/>
+        <v>106</v>
+      </c>
+      <c r="AZ200">
+        <f t="shared" si="152"/>
+        <v>709</v>
+      </c>
+      <c r="BA200" s="8">
+        <f t="shared" si="153"/>
+        <v>263</v>
+      </c>
+      <c r="BB200" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC200" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD200" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="201" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A201" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="B201" s="10" t="s">
+        <v>757</v>
+      </c>
+      <c r="C201" t="s">
+        <v>722</v>
+      </c>
+      <c r="D201" t="s">
+        <v>477</v>
+      </c>
+      <c r="E201" t="s">
+        <v>406</v>
+      </c>
+      <c r="F201" t="s">
+        <v>636</v>
+      </c>
+      <c r="G201" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H201" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I201" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J201" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U201" s="10"/>
+      <c r="V201" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W201" t="s">
+        <v>117</v>
+      </c>
+      <c r="X201" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y201" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z201" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA201" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB201" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC201">
+        <v>3</v>
+      </c>
+      <c r="AE201" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH201" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI201" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ201" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK201" t="e">
+        <f t="shared" si="149"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL201" t="e">
+        <f t="shared" si="150"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM201" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN201">
+        <v>149</v>
+      </c>
+      <c r="AO201">
+        <v>743</v>
+      </c>
+      <c r="AP201" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ201">
+        <v>120</v>
+      </c>
+      <c r="AR201">
+        <v>720</v>
+      </c>
+      <c r="AS201">
+        <v>320</v>
+      </c>
+      <c r="AT201" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU201">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV201">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW201">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX201" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY201">
+        <f t="shared" si="151"/>
+        <v>106</v>
+      </c>
+      <c r="AZ201">
+        <f t="shared" si="152"/>
+        <v>709</v>
+      </c>
+      <c r="BA201" s="8">
+        <f t="shared" si="153"/>
+        <v>263</v>
+      </c>
+      <c r="BB201" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC201" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD201" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="202" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A202" s="10" t="s">
+        <v>746</v>
+      </c>
+      <c r="B202" s="10" t="s">
+        <v>758</v>
+      </c>
+      <c r="C202" t="s">
+        <v>723</v>
+      </c>
+      <c r="D202" t="s">
+        <v>477</v>
+      </c>
+      <c r="E202" t="s">
+        <v>406</v>
+      </c>
+      <c r="F202" t="s">
+        <v>636</v>
+      </c>
+      <c r="G202" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H202" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I202" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J202" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U202" s="10"/>
+      <c r="V202" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W202" t="s">
+        <v>117</v>
+      </c>
+      <c r="X202" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y202" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z202" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA202" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB202" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC202">
+        <v>3</v>
+      </c>
+      <c r="AE202" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH202" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI202" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ202" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK202" t="e">
+        <f t="shared" si="149"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL202" t="e">
+        <f t="shared" si="150"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM202" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN202">
+        <v>149</v>
+      </c>
+      <c r="AO202">
+        <v>743</v>
+      </c>
+      <c r="AP202" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ202">
+        <v>120</v>
+      </c>
+      <c r="AR202">
+        <v>720</v>
+      </c>
+      <c r="AS202">
+        <v>320</v>
+      </c>
+      <c r="AT202" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU202">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV202">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW202">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX202" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY202">
+        <f t="shared" si="151"/>
+        <v>106</v>
+      </c>
+      <c r="AZ202">
+        <f t="shared" si="152"/>
+        <v>709</v>
+      </c>
+      <c r="BA202" s="8">
+        <f t="shared" si="153"/>
+        <v>263</v>
+      </c>
+      <c r="BB202" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC202" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD202" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="203" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A203" s="10" t="s">
+        <v>747</v>
+      </c>
+      <c r="B203" s="10" t="s">
+        <v>759</v>
+      </c>
+      <c r="C203" t="s">
+        <v>723</v>
+      </c>
+      <c r="D203" t="s">
+        <v>477</v>
+      </c>
+      <c r="E203" t="s">
+        <v>406</v>
+      </c>
+      <c r="F203" t="s">
+        <v>636</v>
+      </c>
+      <c r="G203" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H203" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I203" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J203" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U203" s="10"/>
+      <c r="V203" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W203" t="s">
+        <v>117</v>
+      </c>
+      <c r="X203" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y203" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z203" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA203" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB203" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC203">
+        <v>3</v>
+      </c>
+      <c r="AE203" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH203" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI203" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ203" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK203" t="e">
+        <f t="shared" si="149"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL203" t="e">
+        <f t="shared" si="150"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM203" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN203">
+        <v>149</v>
+      </c>
+      <c r="AO203">
+        <v>743</v>
+      </c>
+      <c r="AP203" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ203">
+        <v>120</v>
+      </c>
+      <c r="AR203">
+        <v>720</v>
+      </c>
+      <c r="AS203">
+        <v>320</v>
+      </c>
+      <c r="AT203" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU203">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV203">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW203">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX203" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY203">
+        <f t="shared" si="151"/>
+        <v>106</v>
+      </c>
+      <c r="AZ203">
+        <f t="shared" si="152"/>
+        <v>709</v>
+      </c>
+      <c r="BA203" s="8">
+        <f t="shared" si="153"/>
+        <v>263</v>
+      </c>
+      <c r="BB203" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC203" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD203" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="204" spans="1:56" x14ac:dyDescent="0.3">
+      <c r="A204" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B204" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C204" t="s">
+        <v>117</v>
+      </c>
+      <c r="D204" t="s">
+        <v>117</v>
+      </c>
+      <c r="E204" t="s">
+        <v>117</v>
+      </c>
+      <c r="F204" t="s">
+        <v>117</v>
+      </c>
+      <c r="G204" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H204" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I204" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J204" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U204" s="10"/>
+      <c r="V204" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W204" t="s">
+        <v>117</v>
+      </c>
+      <c r="X204" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y204" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH204" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK204" t="e">
+        <f t="shared" si="149"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL204" t="e">
+        <f t="shared" si="150"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM204" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP204" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT204" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW204" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX204" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY204" t="e">
+        <f t="shared" si="151"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ204" t="e">
+        <f t="shared" si="152"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA204" s="8" t="e">
+        <f t="shared" si="153"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB204" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC204" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD204" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare train3dunet 1.8.2 chpt-240304-0 to -2
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\cloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB14EE8-CBEC-48AD-939D-5BF7FE073A13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB0CA85-5D1E-499F-995B-B87D645112C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41232" yWindow="0" windowWidth="4848" windowHeight="15756" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5398" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5430" uniqueCount="777">
   <si>
     <t>patch z</t>
   </si>
@@ -2363,6 +2374,57 @@
   </si>
   <si>
     <t>240221-5 last, autofluo kidney, nuclei model type, id04 test, id06 val</t>
+  </si>
+  <si>
+    <t>240304-0</t>
+  </si>
+  <si>
+    <t>240304-1</t>
+  </si>
+  <si>
+    <t>240304-2</t>
+  </si>
+  <si>
+    <t>model 11.b.0, autofluo kidney, nuclei model type, id07 test, id05 val</t>
+  </si>
+  <si>
+    <t>model 11.b.1, autofluo kidney, nuclei model type, id02 test, id01 val</t>
+  </si>
+  <si>
+    <t>model 11.b.0, autofluo kidney, nuclei model type, id04 test, id06 val</t>
+  </si>
+  <si>
+    <t>model 11.c.0, autofluo kidney, nuclei model type, id07 test, id05 val</t>
+  </si>
+  <si>
+    <t>model 11.c.1, autofluo kidney, nuclei model type, id02 test, id01 val</t>
+  </si>
+  <si>
+    <t>model 11.c.2, autofluo kidney, nuclei model type, id04 test, id06 val</t>
+  </si>
+  <si>
+    <t>dataset11.c.0</t>
+  </si>
+  <si>
+    <t>dataset11.c.1</t>
+  </si>
+  <si>
+    <t>dataset11.c.2</t>
+  </si>
+  <si>
+    <t>TBD (no log file(?))</t>
+  </si>
+  <si>
+    <t>patch = same as similar previous (chpt-240221-0 - arbitrary number as close to embryo size as possible (z smaller, y &amp; x bigger than embryo))</t>
+  </si>
+  <si>
+    <t>stride = same as similar previous (chpt-240221-0 - arbitrary number as close to embryo size as possible (z smaller, y &amp; x bigger than embryo))</t>
+  </si>
+  <si>
+    <t>patch = same as for model comparison chpt-240304-0</t>
+  </si>
+  <si>
+    <t>stride = same as for model comparison chpt-240304-0</t>
   </si>
 </sst>
 </file>
@@ -2837,7 +2899,7 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2963,9 +3025,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
@@ -2995,9 +3054,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3035,7 +3094,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3141,7 +3200,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3283,7 +3342,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3291,75 +3350,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG204"/>
+  <dimension ref="A1:BG207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="W150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N181" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA194" sqref="AA194"/>
+      <selection pane="bottomRight" activeCell="AT207" sqref="AT207"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="69.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" customWidth="1"/>
     <col min="7" max="7" width="57" style="38" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="35.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="64.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.5546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="30.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="64.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" customWidth="1"/>
     <col min="14" max="14" width="33" customWidth="1"/>
-    <col min="15" max="21" width="9.109375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="9.109375" style="17" collapsed="1"/>
-    <col min="23" max="23" width="9.109375" customWidth="1"/>
-    <col min="24" max="24" width="6.6640625" customWidth="1"/>
-    <col min="25" max="25" width="5.109375" customWidth="1"/>
+    <col min="15" max="21" width="9.140625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="9.140625" style="17" collapsed="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1"/>
+    <col min="24" max="24" width="6.7109375" customWidth="1"/>
+    <col min="25" max="25" width="5.140625" customWidth="1"/>
     <col min="26" max="26" width="6" customWidth="1"/>
-    <col min="27" max="27" width="11.109375" customWidth="1"/>
-    <col min="29" max="29" width="7.6640625" customWidth="1"/>
-    <col min="30" max="30" width="9.5546875" customWidth="1"/>
+    <col min="27" max="27" width="11.140625" customWidth="1"/>
+    <col min="29" max="29" width="7.7109375" customWidth="1"/>
+    <col min="30" max="30" width="9.5703125" customWidth="1"/>
     <col min="31" max="31" width="9" customWidth="1"/>
-    <col min="32" max="32" width="8.88671875" customWidth="1"/>
-    <col min="33" max="33" width="9.88671875" customWidth="1"/>
-    <col min="34" max="34" width="9.6640625" style="8" customWidth="1"/>
-    <col min="35" max="35" width="11.6640625" customWidth="1"/>
-    <col min="36" max="36" width="10.44140625" customWidth="1"/>
-    <col min="37" max="37" width="9.6640625" customWidth="1"/>
-    <col min="38" max="38" width="15.44140625" customWidth="1"/>
-    <col min="39" max="39" width="26.33203125" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="6.5546875" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="6.6640625" customWidth="1"/>
-    <col min="42" max="42" width="6.6640625" style="17" customWidth="1"/>
-    <col min="43" max="43" width="5.33203125" customWidth="1"/>
-    <col min="44" max="44" width="6.109375" customWidth="1"/>
+    <col min="32" max="32" width="8.85546875" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" customWidth="1"/>
+    <col min="34" max="34" width="9.7109375" style="8" customWidth="1"/>
+    <col min="35" max="35" width="11.7109375" customWidth="1"/>
+    <col min="36" max="36" width="10.42578125" customWidth="1"/>
+    <col min="37" max="37" width="9.7109375" customWidth="1"/>
+    <col min="38" max="38" width="15.42578125" customWidth="1"/>
+    <col min="39" max="39" width="26.28515625" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="6.5703125" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="6.7109375" customWidth="1"/>
+    <col min="42" max="42" width="6.7109375" style="17" customWidth="1"/>
+    <col min="43" max="43" width="5.28515625" customWidth="1"/>
+    <col min="44" max="44" width="6.140625" customWidth="1"/>
     <col min="45" max="45" width="5" customWidth="1"/>
     <col min="46" max="46" width="5" style="17" customWidth="1"/>
-    <col min="47" max="47" width="6.109375" customWidth="1"/>
-    <col min="48" max="48" width="6.5546875" customWidth="1"/>
+    <col min="47" max="47" width="6.140625" customWidth="1"/>
+    <col min="48" max="48" width="6.5703125" customWidth="1"/>
     <col min="49" max="49" width="5" customWidth="1"/>
     <col min="50" max="50" width="6" style="17" customWidth="1"/>
     <col min="51" max="52" width="6" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="53" max="53" width="6" style="8" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="32.109375" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="35.44140625" customWidth="1"/>
-    <col min="56" max="56" width="5.109375" customWidth="1"/>
-    <col min="57" max="57" width="135.33203125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="54" max="54" width="32.140625" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="35.42578125" customWidth="1"/>
+    <col min="56" max="56" width="5.140625" customWidth="1"/>
+    <col min="57" max="57" width="135.28515625" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="58" max="58" width="206" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="12.6640625" customWidth="1"/>
-    <col min="63" max="63" width="12.109375" customWidth="1"/>
+    <col min="59" max="59" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.7109375" customWidth="1"/>
+    <col min="63" max="63" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -3535,7 +3594,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -3703,7 +3762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -3872,7 +3931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:58" s="6" customFormat="1" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" s="6" customFormat="1" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>51</v>
       </c>
@@ -4040,7 +4099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -4205,7 +4264,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4370,7 +4429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4535,7 +4594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4700,7 +4759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -4871,7 +4930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -5036,7 +5095,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:58" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -5201,7 +5260,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -5367,7 +5426,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -5532,7 +5591,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -5697,7 +5756,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -5863,7 +5922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -6030,7 +6089,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -6196,7 +6255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -6362,7 +6421,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -6528,7 +6587,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -6694,7 +6753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -6860,7 +6919,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -7026,7 +7085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -7192,7 +7251,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -7358,7 +7417,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -7525,7 +7584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>99</v>
       </c>
@@ -7692,7 +7751,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -7862,7 +7921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -8031,7 +8090,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -8201,7 +8260,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>141</v>
       </c>
@@ -8371,7 +8430,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -8541,7 +8600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -8710,7 +8769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>165</v>
       </c>
@@ -8879,7 +8938,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>166</v>
       </c>
@@ -9048,7 +9107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>175</v>
       </c>
@@ -9217,7 +9276,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>180</v>
       </c>
@@ -9386,7 +9445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -9555,7 +9614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>188</v>
       </c>
@@ -9724,7 +9783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>191</v>
       </c>
@@ -9893,7 +9952,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>195</v>
       </c>
@@ -10062,7 +10121,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>196</v>
       </c>
@@ -10231,7 +10290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>198</v>
       </c>
@@ -10400,7 +10459,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>201</v>
       </c>
@@ -10569,7 +10628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>202</v>
       </c>
@@ -10739,7 +10798,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>203</v>
       </c>
@@ -10910,7 +10969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>235</v>
       </c>
@@ -11075,7 +11134,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>236</v>
       </c>
@@ -11240,7 +11299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>237</v>
       </c>
@@ -11405,7 +11464,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>238</v>
       </c>
@@ -11570,7 +11629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>239</v>
       </c>
@@ -11735,7 +11794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>240</v>
       </c>
@@ -11900,7 +11959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>241</v>
       </c>
@@ -12065,7 +12124,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>242</v>
       </c>
@@ -12230,7 +12289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>243</v>
       </c>
@@ -12395,7 +12454,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>244</v>
       </c>
@@ -12560,7 +12619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>245</v>
       </c>
@@ -12725,7 +12784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>246</v>
       </c>
@@ -12890,7 +12949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>247</v>
       </c>
@@ -13055,7 +13114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>248</v>
       </c>
@@ -13220,7 +13279,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>249</v>
       </c>
@@ -13385,7 +13444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>250</v>
       </c>
@@ -13550,7 +13609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="62" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>251</v>
       </c>
@@ -13715,7 +13774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>252</v>
       </c>
@@ -13881,7 +13940,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:58" s="25" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:58" s="25" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
         <v>267</v>
       </c>
@@ -14051,7 +14110,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>269</v>
       </c>
@@ -14228,7 +14287,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="66" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>274</v>
       </c>
@@ -14405,7 +14464,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="67" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>289</v>
       </c>
@@ -14582,7 +14641,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="68" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>292</v>
       </c>
@@ -14759,7 +14818,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="69" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>293</v>
       </c>
@@ -14936,7 +14995,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="70" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>298</v>
       </c>
@@ -15116,7 +15175,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>299</v>
       </c>
@@ -15293,7 +15352,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="72" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>302</v>
       </c>
@@ -15470,7 +15529,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="73" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>321</v>
       </c>
@@ -15650,7 +15709,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="74" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>323</v>
       </c>
@@ -15827,7 +15886,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="75" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>331</v>
       </c>
@@ -16001,7 +16060,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="76" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>334</v>
       </c>
@@ -16175,7 +16234,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="77" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>350</v>
       </c>
@@ -16184,7 +16243,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="78" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>350</v>
       </c>
@@ -16193,7 +16252,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="79" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>351</v>
       </c>
@@ -16367,7 +16426,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="80" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>361</v>
       </c>
@@ -16544,7 +16603,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="81" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
         <v>365</v>
       </c>
@@ -16721,7 +16780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
         <v>369</v>
       </c>
@@ -16898,7 +16957,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
         <v>373</v>
       </c>
@@ -17075,7 +17134,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="84" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>374</v>
       </c>
@@ -17252,7 +17311,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="85" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>375</v>
       </c>
@@ -17429,7 +17488,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="86" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>377</v>
       </c>
@@ -17606,7 +17665,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="87" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
         <v>378</v>
       </c>
@@ -17783,7 +17842,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>379</v>
       </c>
@@ -17960,7 +18019,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="89" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>380</v>
       </c>
@@ -18137,7 +18196,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="90" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>381</v>
       </c>
@@ -18314,7 +18373,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="91" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
         <v>382</v>
       </c>
@@ -18491,7 +18550,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="92" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>383</v>
       </c>
@@ -18668,7 +18727,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="93" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:58" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
         <v>384</v>
       </c>
@@ -18845,7 +18904,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>392</v>
       </c>
@@ -19022,7 +19081,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="95" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
         <v>402</v>
       </c>
@@ -19199,7 +19258,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="96" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
         <v>402</v>
       </c>
@@ -19376,7 +19435,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="97" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
         <v>403</v>
       </c>
@@ -19553,7 +19612,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="98" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
         <v>412</v>
       </c>
@@ -19730,7 +19789,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="99" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
         <v>413</v>
       </c>
@@ -19907,7 +19966,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="100" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
         <v>429</v>
       </c>
@@ -20087,7 +20146,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
         <v>432</v>
       </c>
@@ -20267,7 +20326,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="102" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
         <v>433</v>
       </c>
@@ -20447,7 +20506,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="103" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
         <v>434</v>
       </c>
@@ -20629,7 +20688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="s">
         <v>435</v>
       </c>
@@ -20811,7 +20870,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="105" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
         <v>436</v>
       </c>
@@ -20993,7 +21052,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="106" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
         <v>431</v>
       </c>
@@ -21175,7 +21234,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="107" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
         <v>456</v>
       </c>
@@ -21354,7 +21413,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
         <v>460</v>
       </c>
@@ -21536,7 +21595,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="109" spans="1:58" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:58" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
         <v>466</v>
       </c>
@@ -21715,7 +21774,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="110" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="s">
         <v>470</v>
       </c>
@@ -21897,7 +21956,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="111" spans="1:58" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:58" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="32" t="s">
         <v>472</v>
       </c>
@@ -22079,7 +22138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:58" s="52" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:58" s="52" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="45" t="s">
         <v>476</v>
       </c>
@@ -22258,7 +22317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
         <v>484</v>
       </c>
@@ -22442,7 +22501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A114" s="10" t="s">
         <v>485</v>
       </c>
@@ -22568,7 +22627,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="115" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="s">
         <v>493</v>
       </c>
@@ -22694,7 +22753,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="116" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
         <v>494</v>
       </c>
@@ -22822,7 +22881,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A117" s="10" t="s">
         <v>505</v>
       </c>
@@ -22950,7 +23009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A118" s="10" t="s">
         <v>504</v>
       </c>
@@ -23078,7 +23137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A119" s="10" t="s">
         <v>502</v>
       </c>
@@ -23206,7 +23265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
         <v>507</v>
       </c>
@@ -23356,7 +23415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="121" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="s">
         <v>508</v>
       </c>
@@ -23506,7 +23565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A122" s="10" t="s">
         <v>520</v>
       </c>
@@ -23637,7 +23696,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A123" s="10" t="s">
         <v>521</v>
       </c>
@@ -23768,7 +23827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A124" s="10" t="s">
         <v>522</v>
       </c>
@@ -23899,7 +23958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="125" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A125" s="10" t="s">
         <v>523</v>
       </c>
@@ -24030,7 +24089,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="126" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A126" s="10" t="s">
         <v>529</v>
       </c>
@@ -24175,7 +24234,7 @@
       </c>
       <c r="BF126" s="1"/>
     </row>
-    <row r="127" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A127" s="10" t="s">
         <v>530</v>
       </c>
@@ -24323,7 +24382,7 @@
       </c>
       <c r="BF127" s="1"/>
     </row>
-    <row r="128" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
         <v>531</v>
       </c>
@@ -24471,7 +24530,7 @@
       </c>
       <c r="BF128" s="1"/>
     </row>
-    <row r="129" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
         <v>532</v>
       </c>
@@ -24619,7 +24678,7 @@
       </c>
       <c r="BF129" s="1"/>
     </row>
-    <row r="130" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
         <v>534</v>
       </c>
@@ -24766,7 +24825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>541</v>
       </c>
@@ -24910,7 +24969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
         <v>542</v>
       </c>
@@ -25054,7 +25113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>543</v>
       </c>
@@ -25198,7 +25257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
         <v>544</v>
       </c>
@@ -25342,7 +25401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A135" s="10" t="s">
         <v>545</v>
       </c>
@@ -25486,7 +25545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="s">
         <v>546</v>
       </c>
@@ -25630,7 +25689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="s">
         <v>547</v>
       </c>
@@ -25774,7 +25833,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="138" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A138" s="10" t="s">
         <v>548</v>
       </c>
@@ -25918,7 +25977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A139" s="10" t="s">
         <v>549</v>
       </c>
@@ -26061,7 +26120,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="140" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
         <v>570</v>
       </c>
@@ -26208,7 +26267,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="141" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A141" s="10" t="s">
         <v>578</v>
       </c>
@@ -26342,7 +26401,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="142" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A142" s="10" t="s">
         <v>579</v>
       </c>
@@ -26476,7 +26535,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="143" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A143" s="10" t="s">
         <v>580</v>
       </c>
@@ -26610,7 +26669,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="144" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A144" s="10" t="s">
         <v>581</v>
       </c>
@@ -26744,7 +26803,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A145" s="10" t="s">
         <v>582</v>
       </c>
@@ -26878,7 +26937,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="146" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A146" s="10" t="s">
         <v>583</v>
       </c>
@@ -27012,7 +27071,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="147" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A147" s="10" t="s">
         <v>584</v>
       </c>
@@ -27146,7 +27205,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="148" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A148" s="10" t="s">
         <v>585</v>
       </c>
@@ -27280,7 +27339,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="149" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="32" t="s">
         <v>586</v>
       </c>
@@ -27409,7 +27468,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="150" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A150" s="10" t="s">
         <v>587</v>
       </c>
@@ -27547,7 +27606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A151" s="10" t="s">
         <v>588</v>
       </c>
@@ -27685,7 +27744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A152" s="10" t="s">
         <v>596</v>
       </c>
@@ -27814,7 +27873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A153" s="10" t="s">
         <v>597</v>
       </c>
@@ -27949,7 +28008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A154" s="10" t="s">
         <v>602</v>
       </c>
@@ -28090,7 +28149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A155" s="10" t="s">
         <v>610</v>
       </c>
@@ -28228,7 +28287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A156" s="10" t="s">
         <v>611</v>
       </c>
@@ -28366,7 +28425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A157" s="10" t="s">
         <v>626</v>
       </c>
@@ -28511,7 +28570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>632</v>
       </c>
@@ -28639,7 +28698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>633</v>
       </c>
@@ -28767,7 +28826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>634</v>
       </c>
@@ -28895,7 +28954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="32" t="s">
         <v>654</v>
       </c>
@@ -29036,7 +29095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="32" t="s">
         <v>655</v>
       </c>
@@ -29177,7 +29236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="32" t="s">
         <v>656</v>
       </c>
@@ -29318,7 +29377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="32" t="s">
         <v>652</v>
       </c>
@@ -29462,7 +29521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:56" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="32" t="s">
         <v>653</v>
       </c>
@@ -29606,7 +29665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:56" s="30" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:56" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="70" t="s">
         <v>661</v>
       </c>
@@ -29750,7 +29809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A167" s="68" t="s">
         <v>666</v>
       </c>
@@ -29888,7 +29947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A168" s="68" t="s">
         <v>667</v>
       </c>
@@ -30026,7 +30085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A169" s="68" t="s">
         <v>674</v>
       </c>
@@ -30164,7 +30223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A170" s="68" t="s">
         <v>694</v>
       </c>
@@ -30286,7 +30345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A171" s="10" t="s">
         <v>697</v>
       </c>
@@ -30419,7 +30478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A172" s="10" t="s">
         <v>698</v>
       </c>
@@ -30552,7 +30611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A173" s="10" t="s">
         <v>699</v>
       </c>
@@ -30685,7 +30744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
         <v>700</v>
       </c>
@@ -30818,7 +30877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A175" s="10" t="s">
         <v>701</v>
       </c>
@@ -30951,7 +31010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A176" s="10" t="s">
         <v>702</v>
       </c>
@@ -31084,7 +31143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A177" s="10" t="s">
         <v>703</v>
       </c>
@@ -31217,7 +31276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A178" s="10" t="s">
         <v>704</v>
       </c>
@@ -31350,7 +31409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="15" t="s">
         <v>705</v>
       </c>
@@ -31484,7 +31543,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="180" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A180" s="10" t="s">
         <v>706</v>
       </c>
@@ -31518,7 +31577,7 @@
       <c r="K180">
         <v>1</v>
       </c>
-      <c r="L180" s="79" t="s">
+      <c r="L180" s="10" t="s">
         <v>450</v>
       </c>
       <c r="U180" s="10"/>
@@ -31631,7 +31690,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="181" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A181" s="10" t="s">
         <v>707</v>
       </c>
@@ -31665,7 +31724,7 @@
       <c r="K181">
         <v>1</v>
       </c>
-      <c r="L181" s="79" t="s">
+      <c r="L181" s="10" t="s">
         <v>450</v>
       </c>
       <c r="U181" s="10"/>
@@ -31778,7 +31837,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="182" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A182" s="10" t="s">
         <v>708</v>
       </c>
@@ -31812,7 +31871,7 @@
       <c r="K182">
         <v>1</v>
       </c>
-      <c r="L182" s="79" t="s">
+      <c r="L182" s="10" t="s">
         <v>450</v>
       </c>
       <c r="U182" s="10"/>
@@ -31925,7 +31984,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="183" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A183" s="10" t="s">
         <v>709</v>
       </c>
@@ -31959,7 +32018,7 @@
       <c r="K183">
         <v>1</v>
       </c>
-      <c r="L183" s="79" t="s">
+      <c r="L183" s="10" t="s">
         <v>450</v>
       </c>
       <c r="U183" s="10"/>
@@ -32072,7 +32131,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="184" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A184" s="10" t="s">
         <v>710</v>
       </c>
@@ -32106,7 +32165,7 @@
       <c r="K184">
         <v>1</v>
       </c>
-      <c r="L184" s="79" t="s">
+      <c r="L184" s="10" t="s">
         <v>450</v>
       </c>
       <c r="U184" s="10"/>
@@ -32219,7 +32278,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="185" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:59" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="15" t="s">
         <v>711</v>
       </c>
@@ -32366,7 +32425,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="186" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A186" s="10" t="s">
         <v>728</v>
       </c>
@@ -32465,7 +32524,7 @@
         <v>320</v>
       </c>
       <c r="AT186" s="47" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="AU186">
         <f t="shared" ref="AU186:AU191" si="128" xml:space="preserve"> _xlfn.FLOOR.MATH((AN186 - AQ186) / 2)</f>
@@ -32500,11 +32559,11 @@
       <c r="BC186" t="s">
         <v>725</v>
       </c>
-      <c r="BD186" t="s">
-        <v>117</v>
+      <c r="BD186">
+        <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A187" s="10" t="s">
         <v>729</v>
       </c>
@@ -32603,7 +32662,7 @@
         <v>320</v>
       </c>
       <c r="AT187" s="47" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="AU187">
         <f t="shared" si="128"/>
@@ -32638,11 +32697,11 @@
       <c r="BC187" t="s">
         <v>727</v>
       </c>
-      <c r="BD187" t="s">
-        <v>117</v>
+      <c r="BD187">
+        <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A188" s="10" t="s">
         <v>730</v>
       </c>
@@ -32741,7 +32800,7 @@
         <v>320</v>
       </c>
       <c r="AT188" s="47" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="AU188">
         <f t="shared" si="128"/>
@@ -32776,16 +32835,16 @@
       <c r="BC188" t="s">
         <v>727</v>
       </c>
-      <c r="BD188" t="s">
-        <v>117</v>
+      <c r="BD188">
+        <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A189" s="10" t="s">
         <v>731</v>
       </c>
       <c r="B189" s="10" t="s">
-        <v>713</v>
+        <v>763</v>
       </c>
       <c r="C189" t="s">
         <v>719</v>
@@ -32879,7 +32938,7 @@
         <v>320</v>
       </c>
       <c r="AT189" s="47" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="AU189">
         <f t="shared" si="128"/>
@@ -32914,16 +32973,16 @@
       <c r="BC189" t="s">
         <v>727</v>
       </c>
-      <c r="BD189" t="s">
-        <v>117</v>
+      <c r="BD189">
+        <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A190" s="10" t="s">
         <v>732</v>
       </c>
       <c r="B190" s="10" t="s">
-        <v>716</v>
+        <v>764</v>
       </c>
       <c r="C190" t="s">
         <v>722</v>
@@ -33017,7 +33076,7 @@
         <v>320</v>
       </c>
       <c r="AT190" s="47" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="AU190">
         <f t="shared" si="128"/>
@@ -33052,16 +33111,16 @@
       <c r="BC190" t="s">
         <v>727</v>
       </c>
-      <c r="BD190" t="s">
-        <v>117</v>
+      <c r="BD190">
+        <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A191" s="10" t="s">
         <v>733</v>
       </c>
       <c r="B191" s="10" t="s">
-        <v>717</v>
+        <v>765</v>
       </c>
       <c r="C191" t="s">
         <v>723</v>
@@ -33155,7 +33214,7 @@
         <v>320</v>
       </c>
       <c r="AT191" s="47" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="AU191">
         <f t="shared" si="128"/>
@@ -33190,11 +33249,11 @@
       <c r="BC191" t="s">
         <v>727</v>
       </c>
-      <c r="BD191" t="s">
-        <v>117</v>
+      <c r="BD191">
+        <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A192" s="10" t="s">
         <v>736</v>
       </c>
@@ -33222,8 +33281,8 @@
       <c r="I192" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J192" s="4" t="s">
-        <v>117</v>
+      <c r="J192" s="4">
+        <v>1</v>
       </c>
       <c r="U192" s="10"/>
       <c r="V192" s="17" t="s">
@@ -33295,15 +33354,15 @@
         <v>8</v>
       </c>
       <c r="AU192">
-        <f t="shared" ref="AU192:AU203" si="138" xml:space="preserve"> _xlfn.FLOOR.MATH((AN192 - AQ192) / 2)</f>
+        <f t="shared" ref="AU192:AU206" si="138" xml:space="preserve"> _xlfn.FLOOR.MATH((AN192 - AQ192) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV192">
-        <f t="shared" ref="AV192:AV203" si="139" xml:space="preserve"> _xlfn.FLOOR.MATH((AO192 - AR192) / 2)</f>
+        <f t="shared" ref="AV192:AV206" si="139" xml:space="preserve"> _xlfn.FLOOR.MATH((AO192 - AR192) / 2)</f>
         <v>11</v>
       </c>
       <c r="AW192">
-        <f t="shared" ref="AW192:AW203" si="140" xml:space="preserve"> _xlfn.FLOOR.MATH((AP192 - AS192) / 2)</f>
+        <f t="shared" ref="AW192:AW206" si="140" xml:space="preserve"> _xlfn.FLOOR.MATH((AP192 - AS192) / 2)</f>
         <v>57</v>
       </c>
       <c r="AX192" s="47" t="s">
@@ -33327,11 +33386,11 @@
       <c r="BC192" t="s">
         <v>620</v>
       </c>
-      <c r="BD192" t="s">
-        <v>117</v>
+      <c r="BD192">
+        <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A193" s="10" t="s">
         <v>737</v>
       </c>
@@ -33359,8 +33418,8 @@
       <c r="I193" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J193" s="4" t="s">
-        <v>117</v>
+      <c r="J193" s="4">
+        <v>1</v>
       </c>
       <c r="U193" s="10"/>
       <c r="V193" s="17" t="s">
@@ -33464,11 +33523,11 @@
       <c r="BC193" t="s">
         <v>620</v>
       </c>
-      <c r="BD193" t="s">
-        <v>117</v>
+      <c r="BD193">
+        <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A194" s="10" t="s">
         <v>738</v>
       </c>
@@ -33496,8 +33555,8 @@
       <c r="I194" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J194" s="4" t="s">
-        <v>117</v>
+      <c r="J194" s="4">
+        <v>1</v>
       </c>
       <c r="U194" s="10"/>
       <c r="V194" s="17" t="s">
@@ -33601,11 +33660,11 @@
       <c r="BC194" t="s">
         <v>620</v>
       </c>
-      <c r="BD194" t="s">
-        <v>117</v>
+      <c r="BD194">
+        <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A195" s="10" t="s">
         <v>739</v>
       </c>
@@ -33633,8 +33692,8 @@
       <c r="I195" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J195" s="4" t="s">
-        <v>117</v>
+      <c r="J195" s="4">
+        <v>1</v>
       </c>
       <c r="U195" s="10"/>
       <c r="V195" s="17" t="s">
@@ -33738,11 +33797,11 @@
       <c r="BC195" t="s">
         <v>620</v>
       </c>
-      <c r="BD195" t="s">
-        <v>117</v>
+      <c r="BD195">
+        <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A196" s="10" t="s">
         <v>740</v>
       </c>
@@ -33770,8 +33829,8 @@
       <c r="I196" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J196" s="4" t="s">
-        <v>117</v>
+      <c r="J196" s="4">
+        <v>1</v>
       </c>
       <c r="U196" s="10"/>
       <c r="V196" s="17" t="s">
@@ -33875,11 +33934,11 @@
       <c r="BC196" t="s">
         <v>620</v>
       </c>
-      <c r="BD196" t="s">
-        <v>117</v>
+      <c r="BD196">
+        <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A197" s="10" t="s">
         <v>741</v>
       </c>
@@ -33907,8 +33966,8 @@
       <c r="I197" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J197" s="4" t="s">
-        <v>117</v>
+      <c r="J197" s="4">
+        <v>1</v>
       </c>
       <c r="U197" s="10"/>
       <c r="V197" s="17" t="s">
@@ -34012,11 +34071,11 @@
       <c r="BC197" t="s">
         <v>620</v>
       </c>
-      <c r="BD197" t="s">
-        <v>117</v>
+      <c r="BD197">
+        <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A198" s="10" t="s">
         <v>742</v>
       </c>
@@ -34044,8 +34103,8 @@
       <c r="I198" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J198" s="4" t="s">
-        <v>117</v>
+      <c r="J198" s="4">
+        <v>1</v>
       </c>
       <c r="U198" s="10"/>
       <c r="V198" s="17" t="s">
@@ -34149,11 +34208,11 @@
       <c r="BC198" t="s">
         <v>620</v>
       </c>
-      <c r="BD198" t="s">
-        <v>117</v>
+      <c r="BD198">
+        <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A199" s="10" t="s">
         <v>743</v>
       </c>
@@ -34181,8 +34240,8 @@
       <c r="I199" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J199" s="4" t="s">
-        <v>117</v>
+      <c r="J199" s="4">
+        <v>1</v>
       </c>
       <c r="U199" s="10"/>
       <c r="V199" s="17" t="s">
@@ -34222,11 +34281,11 @@
         <v>117</v>
       </c>
       <c r="AK199" t="e">
-        <f t="shared" ref="AK199:AK204" si="149">AI199+AJ199</f>
+        <f t="shared" ref="AK199:AK206" si="149">AI199+AJ199</f>
         <v>#VALUE!</v>
       </c>
       <c r="AL199" t="e">
-        <f t="shared" ref="AL199:AL204" si="150" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ199*AR199*AS199) * (AA199 / 5) + 441</f>
+        <f t="shared" ref="AL199:AL206" si="150" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ199*AR199*AS199) * (AA199 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
       <c r="AM199" s="8" t="s">
@@ -34269,15 +34328,15 @@
         <v>8</v>
       </c>
       <c r="AY199">
-        <f t="shared" ref="AY199:AY204" si="151">AQ199-AU199</f>
+        <f t="shared" ref="AY199:AY206" si="151">AQ199-AU199</f>
         <v>106</v>
       </c>
       <c r="AZ199">
-        <f t="shared" ref="AZ199:AZ204" si="152">AR199-AV199</f>
+        <f t="shared" ref="AZ199:AZ206" si="152">AR199-AV199</f>
         <v>709</v>
       </c>
       <c r="BA199" s="8">
-        <f t="shared" ref="BA199:BA204" si="153">AS199-AW199</f>
+        <f t="shared" ref="BA199:BA206" si="153">AS199-AW199</f>
         <v>263</v>
       </c>
       <c r="BB199" t="s">
@@ -34286,11 +34345,11 @@
       <c r="BC199" t="s">
         <v>620</v>
       </c>
-      <c r="BD199" t="s">
-        <v>117</v>
+      <c r="BD199">
+        <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A200" s="10" t="s">
         <v>744</v>
       </c>
@@ -34318,8 +34377,8 @@
       <c r="I200" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J200" s="4" t="s">
-        <v>117</v>
+      <c r="J200" s="4">
+        <v>1</v>
       </c>
       <c r="U200" s="10"/>
       <c r="V200" s="17" t="s">
@@ -34423,11 +34482,11 @@
       <c r="BC200" t="s">
         <v>620</v>
       </c>
-      <c r="BD200" t="s">
-        <v>117</v>
+      <c r="BD200">
+        <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A201" s="10" t="s">
         <v>745</v>
       </c>
@@ -34455,8 +34514,8 @@
       <c r="I201" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J201" s="4" t="s">
-        <v>117</v>
+      <c r="J201" s="4">
+        <v>1</v>
       </c>
       <c r="U201" s="10"/>
       <c r="V201" s="17" t="s">
@@ -34560,11 +34619,11 @@
       <c r="BC201" t="s">
         <v>620</v>
       </c>
-      <c r="BD201" t="s">
-        <v>117</v>
+      <c r="BD201">
+        <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A202" s="10" t="s">
         <v>746</v>
       </c>
@@ -34592,8 +34651,8 @@
       <c r="I202" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J202" s="4" t="s">
-        <v>117</v>
+      <c r="J202" s="4">
+        <v>1</v>
       </c>
       <c r="U202" s="10"/>
       <c r="V202" s="17" t="s">
@@ -34697,11 +34756,11 @@
       <c r="BC202" t="s">
         <v>620</v>
       </c>
-      <c r="BD202" t="s">
-        <v>117</v>
+      <c r="BD202">
+        <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A203" s="10" t="s">
         <v>747</v>
       </c>
@@ -34729,8 +34788,8 @@
       <c r="I203" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J203" s="4" t="s">
-        <v>117</v>
+      <c r="J203" s="4">
+        <v>1</v>
       </c>
       <c r="U203" s="10"/>
       <c r="V203" s="17" t="s">
@@ -34834,28 +34893,28 @@
       <c r="BC203" t="s">
         <v>620</v>
       </c>
-      <c r="BD203" t="s">
-        <v>117</v>
+      <c r="BD203">
+        <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A204" s="10" t="s">
-        <v>117</v>
+        <v>760</v>
       </c>
       <c r="B204" s="10" t="s">
-        <v>117</v>
+        <v>766</v>
       </c>
       <c r="C204" t="s">
-        <v>117</v>
+        <v>769</v>
       </c>
       <c r="D204" t="s">
-        <v>117</v>
+        <v>457</v>
       </c>
       <c r="E204" t="s">
-        <v>117</v>
+        <v>406</v>
       </c>
       <c r="F204" t="s">
-        <v>117</v>
+        <v>636</v>
       </c>
       <c r="G204" s="40" t="s">
         <v>117</v>
@@ -34866,39 +34925,40 @@
       <c r="I204" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="J204" s="4" t="s">
-        <v>117</v>
+      <c r="J204" s="4">
+        <v>1</v>
       </c>
       <c r="U204" s="10"/>
       <c r="V204" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="W204" t="s">
-        <v>117</v>
-      </c>
-      <c r="X204" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y204" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z204" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA204" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB204" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC204" t="s">
-        <v>117</v>
+        <v>772</v>
+      </c>
+      <c r="W204">
+        <v>1</v>
+      </c>
+      <c r="X204">
+        <v>5</v>
+      </c>
+      <c r="Y204">
+        <v>1</v>
+      </c>
+      <c r="Z204">
+        <v>1</v>
+      </c>
+      <c r="AA204">
+        <f t="shared" ref="AA204:AA206" si="154">X204+Y204</f>
+        <v>6</v>
+      </c>
+      <c r="AB204">
+        <v>7</v>
+      </c>
+      <c r="AC204">
+        <v>3</v>
       </c>
       <c r="AE204" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
       <c r="AH204" s="8" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="AI204" t="s">
         <v>117</v>
@@ -34910,65 +34970,478 @@
         <f t="shared" si="149"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL204" t="e">
+      <c r="AL204">
         <f t="shared" si="150"/>
-        <v>#VALUE!</v>
+        <v>71823.084029435064</v>
       </c>
       <c r="AM204" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AN204" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO204" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP204" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ204" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR204" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS204" t="s">
-        <v>117</v>
+      <c r="AN204">
+        <v>149</v>
+      </c>
+      <c r="AO204">
+        <v>743</v>
+      </c>
+      <c r="AP204" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ204">
+        <v>120</v>
+      </c>
+      <c r="AR204">
+        <v>720</v>
+      </c>
+      <c r="AS204">
+        <v>320</v>
       </c>
       <c r="AT204" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU204" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV204" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW204" t="s">
-        <v>117</v>
+        <v>45</v>
+      </c>
+      <c r="AU204">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV204">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW204">
+        <f t="shared" si="140"/>
+        <v>57</v>
       </c>
       <c r="AX204" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY204" t="e">
+        <v>45</v>
+      </c>
+      <c r="AY204">
         <f t="shared" si="151"/>
+        <v>106</v>
+      </c>
+      <c r="AZ204">
+        <f t="shared" si="152"/>
+        <v>709</v>
+      </c>
+      <c r="BA204" s="8">
+        <f t="shared" si="153"/>
+        <v>263</v>
+      </c>
+      <c r="BB204" t="s">
+        <v>773</v>
+      </c>
+      <c r="BC204" t="s">
+        <v>774</v>
+      </c>
+      <c r="BD204" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="205" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A205" s="10" t="s">
+        <v>761</v>
+      </c>
+      <c r="B205" s="10" t="s">
+        <v>767</v>
+      </c>
+      <c r="C205" t="s">
+        <v>770</v>
+      </c>
+      <c r="D205" t="s">
+        <v>457</v>
+      </c>
+      <c r="E205" t="s">
+        <v>406</v>
+      </c>
+      <c r="F205" t="s">
+        <v>636</v>
+      </c>
+      <c r="G205" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H205" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I205" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J205" s="4">
+        <v>1</v>
+      </c>
+      <c r="U205" s="10"/>
+      <c r="V205" s="17" t="s">
+        <v>772</v>
+      </c>
+      <c r="W205">
+        <v>1</v>
+      </c>
+      <c r="X205">
+        <v>5</v>
+      </c>
+      <c r="Y205">
+        <v>1</v>
+      </c>
+      <c r="Z205">
+        <v>1</v>
+      </c>
+      <c r="AA205">
+        <f t="shared" si="154"/>
+        <v>6</v>
+      </c>
+      <c r="AB205" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC205">
+        <v>3</v>
+      </c>
+      <c r="AE205" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH205" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI205" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ205" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK205" t="e">
+        <f t="shared" si="149"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ204" t="e">
+      <c r="AL205">
+        <f t="shared" si="150"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM205" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN205">
+        <v>149</v>
+      </c>
+      <c r="AO205">
+        <v>743</v>
+      </c>
+      <c r="AP205" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ205">
+        <v>120</v>
+      </c>
+      <c r="AR205">
+        <v>720</v>
+      </c>
+      <c r="AS205">
+        <v>320</v>
+      </c>
+      <c r="AT205" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU205">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV205">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW205">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX205" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY205">
+        <f t="shared" si="151"/>
+        <v>106</v>
+      </c>
+      <c r="AZ205">
         <f t="shared" si="152"/>
+        <v>709</v>
+      </c>
+      <c r="BA205" s="8">
+        <f t="shared" si="153"/>
+        <v>263</v>
+      </c>
+      <c r="BB205" t="s">
+        <v>775</v>
+      </c>
+      <c r="BC205" t="s">
+        <v>776</v>
+      </c>
+      <c r="BD205" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="206" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A206" s="10" t="s">
+        <v>762</v>
+      </c>
+      <c r="B206" s="10" t="s">
+        <v>768</v>
+      </c>
+      <c r="C206" t="s">
+        <v>771</v>
+      </c>
+      <c r="D206" t="s">
+        <v>457</v>
+      </c>
+      <c r="E206" t="s">
+        <v>406</v>
+      </c>
+      <c r="F206" t="s">
+        <v>636</v>
+      </c>
+      <c r="G206" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H206" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I206" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J206" s="4">
+        <v>1</v>
+      </c>
+      <c r="U206" s="10"/>
+      <c r="V206" s="17" t="s">
+        <v>772</v>
+      </c>
+      <c r="W206">
+        <v>1</v>
+      </c>
+      <c r="X206">
+        <v>5</v>
+      </c>
+      <c r="Y206">
+        <v>1</v>
+      </c>
+      <c r="Z206">
+        <v>1</v>
+      </c>
+      <c r="AA206">
+        <f t="shared" si="154"/>
+        <v>6</v>
+      </c>
+      <c r="AB206" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC206">
+        <v>3</v>
+      </c>
+      <c r="AE206" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH206" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI206" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ206" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK206" t="e">
+        <f t="shared" si="149"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BA204" s="8" t="e">
+      <c r="AL206">
+        <f t="shared" si="150"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM206" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN206">
+        <v>149</v>
+      </c>
+      <c r="AO206">
+        <v>743</v>
+      </c>
+      <c r="AP206" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ206">
+        <v>120</v>
+      </c>
+      <c r="AR206">
+        <v>720</v>
+      </c>
+      <c r="AS206">
+        <v>320</v>
+      </c>
+      <c r="AT206" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU206">
+        <f t="shared" si="138"/>
+        <v>14</v>
+      </c>
+      <c r="AV206">
+        <f t="shared" si="139"/>
+        <v>11</v>
+      </c>
+      <c r="AW206">
+        <f t="shared" si="140"/>
+        <v>57</v>
+      </c>
+      <c r="AX206" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY206">
+        <f t="shared" si="151"/>
+        <v>106</v>
+      </c>
+      <c r="AZ206">
+        <f t="shared" si="152"/>
+        <v>709</v>
+      </c>
+      <c r="BA206" s="8">
         <f t="shared" si="153"/>
+        <v>263</v>
+      </c>
+      <c r="BB206" t="s">
+        <v>775</v>
+      </c>
+      <c r="BC206" t="s">
+        <v>776</v>
+      </c>
+      <c r="BD206" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="207" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A207" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B207" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C207" t="s">
+        <v>117</v>
+      </c>
+      <c r="D207" t="s">
+        <v>117</v>
+      </c>
+      <c r="E207" t="s">
+        <v>117</v>
+      </c>
+      <c r="F207" t="s">
+        <v>117</v>
+      </c>
+      <c r="G207" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H207" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I207" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J207" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U207" s="10"/>
+      <c r="V207" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W207" t="s">
+        <v>117</v>
+      </c>
+      <c r="X207" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y207" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH207" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK207" t="e">
+        <f t="shared" ref="AK205:AK207" si="155">AI207+AJ207</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB204" t="s">
-        <v>117</v>
-      </c>
-      <c r="BC204" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD204" t="s">
+      <c r="AL207" t="e">
+        <f t="shared" ref="AL205:AL207" si="156" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ207*AR207*AS207) * (AA207 / 5) + 441</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM207" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP207" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AQ207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AT207" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AV207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AW207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX207" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY207" t="e">
+        <f t="shared" ref="AY205:AY207" si="157">AQ207-AU207</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AZ207" t="e">
+        <f t="shared" ref="AZ205:AZ207" si="158">AR207-AV207</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BA207" s="8" t="e">
+        <f t="shared" ref="BA205:BA207" si="159">AS207-AW207</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BB207" t="s">
+        <v>117</v>
+      </c>
+      <c r="BC207" t="s">
+        <v>117</v>
+      </c>
+      <c r="BD207" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepare predict3unet 1.8.2 chpt-240304-3 to -8
</commit_message>
<xml_diff>
--- a/3dunet session annotations.xlsx
+++ b/3dunet session annotations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2250BEFF-C4EE-4EFD-B5A0-5BAE3A0F04EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE31147-92D0-4E12-B75A-BC7BA3C005DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" tabRatio="130" xr2:uid="{5A38CEB4-EA53-422C-BFAF-71A244E8F13D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5551" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5707" uniqueCount="799">
   <si>
     <t>patch z</t>
   </si>
@@ -2470,6 +2470,27 @@
   </si>
   <si>
     <t>same model as before (11.b) but with (mostly) filled labels now</t>
+  </si>
+  <si>
+    <t>240304-0 best, model 11.c.0</t>
+  </si>
+  <si>
+    <t>240304-0 last, model 11.c.0</t>
+  </si>
+  <si>
+    <t>240304-1 best, model 11.c.1</t>
+  </si>
+  <si>
+    <t>240304-1 last, model 11.c.1</t>
+  </si>
+  <si>
+    <t>240304-2 best, model 11.c.2</t>
+  </si>
+  <si>
+    <t>240304-2 last, model 11.c.2</t>
+  </si>
+  <si>
+    <t>find best model of the 3 train/val/test divisions to tune patience hyperparameters</t>
   </si>
 </sst>
 </file>
@@ -3395,13 +3416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A205867-9158-4A30-AB8D-184C978ABB6F}">
-  <dimension ref="A1:BG213"/>
+  <dimension ref="A1:BG222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B175" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AE195" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G206" sqref="G206"/>
+      <selection pane="bottomRight" activeCell="BD208" sqref="BD208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3412,10 +3433,10 @@
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" customWidth="1"/>
     <col min="6" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="72.28515625" style="38" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="35.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="64.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="14.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="75.5703125" style="38" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="35.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="64.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="14.5703125" style="4" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="8.5703125" customWidth="1"/>
     <col min="12" max="12" width="30.7109375" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" customWidth="1"/>
@@ -34326,11 +34347,11 @@
         <v>117</v>
       </c>
       <c r="AK199" t="e">
-        <f t="shared" ref="AK199:AK206" si="149">AI199+AJ199</f>
+        <f t="shared" ref="AK199:AK207" si="149">AI199+AJ199</f>
         <v>#VALUE!</v>
       </c>
       <c r="AL199" t="e">
-        <f t="shared" ref="AL199:AL206" si="150" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ199*AR199*AS199) * (AA199 / 5) + 441</f>
+        <f t="shared" ref="AL199:AL207" si="150" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ199*AR199*AS199) * (AA199 / 5) + 441</f>
         <v>#VALUE!</v>
       </c>
       <c r="AM199" s="8" t="s">
@@ -34373,15 +34394,15 @@
         <v>8</v>
       </c>
       <c r="AY199">
-        <f t="shared" ref="AY199:AY206" si="151">AQ199-AU199</f>
+        <f t="shared" ref="AY199:AY207" si="151">AQ199-AU199</f>
         <v>106</v>
       </c>
       <c r="AZ199">
-        <f t="shared" ref="AZ199:AZ206" si="152">AR199-AV199</f>
+        <f t="shared" ref="AZ199:AZ207" si="152">AR199-AV199</f>
         <v>709</v>
       </c>
       <c r="BA199" s="8">
-        <f t="shared" ref="BA199:BA206" si="153">AS199-AW199</f>
+        <f t="shared" ref="BA199:BA207" si="153">AS199-AW199</f>
         <v>263</v>
       </c>
       <c r="BB199" t="s">
@@ -35361,13 +35382,13 @@
         <v>774</v>
       </c>
       <c r="B207" s="10" t="s">
-        <v>780</v>
+        <v>792</v>
       </c>
       <c r="C207" t="s">
         <v>766</v>
       </c>
       <c r="D207" t="s">
-        <v>457</v>
+        <v>477</v>
       </c>
       <c r="E207" t="s">
         <v>406</v>
@@ -35376,7 +35397,7 @@
         <v>636</v>
       </c>
       <c r="G207" s="40" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="H207" s="10" t="s">
         <v>117</v>
@@ -35391,33 +35412,32 @@
       <c r="V207" s="17" t="s">
         <v>769</v>
       </c>
-      <c r="W207">
-        <v>1</v>
-      </c>
-      <c r="X207">
-        <v>5</v>
-      </c>
-      <c r="Y207">
-        <v>1</v>
-      </c>
-      <c r="Z207">
-        <v>1</v>
-      </c>
-      <c r="AA207">
-        <f t="shared" ref="AA207:AA212" si="155">X207+Y207</f>
-        <v>6</v>
-      </c>
-      <c r="AB207">
-        <v>7</v>
+      <c r="W207" t="s">
+        <v>117</v>
+      </c>
+      <c r="X207" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y207" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA207" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB207" t="s">
+        <v>117</v>
       </c>
       <c r="AC207">
         <v>3</v>
       </c>
       <c r="AE207" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="AH207" s="8" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AI207" t="s">
         <v>117</v>
@@ -35426,12 +35446,12 @@
         <v>117</v>
       </c>
       <c r="AK207" t="e">
-        <f t="shared" ref="AK207:AK212" si="156">AI207+AJ207</f>
+        <f t="shared" si="149"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL207">
-        <f t="shared" ref="AL207:AL212" si="157" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ207*AR207*AS207) * (AA207 / 5) + 441</f>
-        <v>71823.084029435064</v>
+      <c r="AL207" t="e">
+        <f t="shared" si="150"/>
+        <v>#VALUE!</v>
       </c>
       <c r="AM207" s="8" t="s">
         <v>105</v>
@@ -35455,43 +35475,43 @@
         <v>320</v>
       </c>
       <c r="AT207" s="47" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AU207">
-        <f t="shared" ref="AU207:AU212" si="158" xml:space="preserve"> _xlfn.FLOOR.MATH((AN207 - AQ207) / 2)</f>
+        <f t="shared" ref="AU207:AU212" si="155" xml:space="preserve"> _xlfn.FLOOR.MATH((AN207 - AQ207) / 2)</f>
         <v>14</v>
       </c>
       <c r="AV207">
-        <f t="shared" ref="AV207:AV212" si="159" xml:space="preserve"> _xlfn.FLOOR.MATH((AO207 - AR207) / 2)</f>
+        <f t="shared" ref="AV207:AV212" si="156" xml:space="preserve"> _xlfn.FLOOR.MATH((AO207 - AR207) / 2)</f>
         <v>11</v>
       </c>
       <c r="AW207">
-        <f t="shared" ref="AW207:AW212" si="160" xml:space="preserve"> _xlfn.FLOOR.MATH((AP207 - AS207) / 2)</f>
+        <f t="shared" ref="AW207:AW212" si="157" xml:space="preserve"> _xlfn.FLOOR.MATH((AP207 - AS207) / 2)</f>
         <v>57</v>
       </c>
       <c r="AX207" s="47" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AY207">
-        <f t="shared" ref="AY207:AY212" si="161">AQ207-AU207</f>
+        <f t="shared" si="151"/>
         <v>106</v>
       </c>
       <c r="AZ207">
-        <f t="shared" ref="AZ207:AZ212" si="162">AR207-AV207</f>
+        <f t="shared" si="152"/>
         <v>709</v>
       </c>
       <c r="BA207" s="8">
-        <f t="shared" ref="BA207:BA212" si="163">AS207-AW207</f>
+        <f t="shared" si="153"/>
         <v>263</v>
       </c>
       <c r="BB207" t="s">
-        <v>770</v>
+        <v>619</v>
       </c>
       <c r="BC207" t="s">
-        <v>771</v>
-      </c>
-      <c r="BD207" t="s">
-        <v>117</v>
+        <v>620</v>
+      </c>
+      <c r="BD207">
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:56" x14ac:dyDescent="0.25">
@@ -35499,13 +35519,13 @@
         <v>775</v>
       </c>
       <c r="B208" s="10" t="s">
-        <v>784</v>
+        <v>793</v>
       </c>
       <c r="C208" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D208" t="s">
-        <v>457</v>
+        <v>477</v>
       </c>
       <c r="E208" t="s">
         <v>406</v>
@@ -35514,7 +35534,7 @@
         <v>636</v>
       </c>
       <c r="G208" s="40" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="H208" s="10" t="s">
         <v>117</v>
@@ -35529,21 +35549,20 @@
       <c r="V208" s="17" t="s">
         <v>769</v>
       </c>
-      <c r="W208">
-        <v>1</v>
-      </c>
-      <c r="X208">
-        <v>5</v>
-      </c>
-      <c r="Y208">
-        <v>1</v>
-      </c>
-      <c r="Z208">
-        <v>1</v>
-      </c>
-      <c r="AA208">
-        <f t="shared" si="155"/>
-        <v>6</v>
+      <c r="W208" t="s">
+        <v>117</v>
+      </c>
+      <c r="X208" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y208" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z208" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA208" t="s">
+        <v>117</v>
       </c>
       <c r="AB208" t="s">
         <v>117</v>
@@ -35552,10 +35571,10 @@
         <v>3</v>
       </c>
       <c r="AE208" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="AH208" s="8" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AI208" t="s">
         <v>117</v>
@@ -35564,12 +35583,12 @@
         <v>117</v>
       </c>
       <c r="AK208" t="e">
-        <f t="shared" si="156"/>
+        <f t="shared" ref="AK208:AK212" si="158">AI208+AJ208</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AL208">
-        <f t="shared" si="157"/>
-        <v>71823.084029435064</v>
+      <c r="AL208" t="e">
+        <f t="shared" ref="AL208:AL212" si="159" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ208*AR208*AS208) * (AA208 / 5) + 441</f>
+        <v>#VALUE!</v>
       </c>
       <c r="AM208" s="8" t="s">
         <v>105</v>
@@ -35593,43 +35612,43 @@
         <v>320</v>
       </c>
       <c r="AT208" s="47" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AU208">
-        <f t="shared" si="158"/>
+        <f t="shared" si="155"/>
         <v>14</v>
       </c>
       <c r="AV208">
-        <f t="shared" si="159"/>
+        <f t="shared" si="156"/>
         <v>11</v>
       </c>
       <c r="AW208">
-        <f t="shared" si="160"/>
+        <f t="shared" si="157"/>
         <v>57</v>
       </c>
       <c r="AX208" s="47" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AY208">
-        <f t="shared" si="161"/>
+        <f t="shared" ref="AY208:AY212" si="160">AQ208-AU208</f>
         <v>106</v>
       </c>
       <c r="AZ208">
-        <f t="shared" si="162"/>
+        <f t="shared" ref="AZ208:AZ212" si="161">AR208-AV208</f>
         <v>709</v>
       </c>
       <c r="BA208" s="8">
-        <f t="shared" si="163"/>
+        <f t="shared" ref="BA208:BA212" si="162">AS208-AW208</f>
         <v>263</v>
       </c>
       <c r="BB208" t="s">
-        <v>772</v>
+        <v>619</v>
       </c>
       <c r="BC208" t="s">
-        <v>773</v>
-      </c>
-      <c r="BD208" t="s">
-        <v>117</v>
+        <v>620</v>
+      </c>
+      <c r="BD208">
+        <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:56" x14ac:dyDescent="0.25">
@@ -35637,13 +35656,13 @@
         <v>776</v>
       </c>
       <c r="B209" s="10" t="s">
-        <v>785</v>
+        <v>794</v>
       </c>
       <c r="C209" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D209" t="s">
-        <v>457</v>
+        <v>477</v>
       </c>
       <c r="E209" t="s">
         <v>406</v>
@@ -35652,7 +35671,7 @@
         <v>636</v>
       </c>
       <c r="G209" s="40" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="H209" s="10" t="s">
         <v>117</v>
@@ -35667,21 +35686,20 @@
       <c r="V209" s="17" t="s">
         <v>769</v>
       </c>
-      <c r="W209">
-        <v>1</v>
-      </c>
-      <c r="X209">
-        <v>5</v>
-      </c>
-      <c r="Y209">
-        <v>1</v>
-      </c>
-      <c r="Z209">
-        <v>1</v>
-      </c>
-      <c r="AA209">
-        <f t="shared" si="155"/>
-        <v>6</v>
+      <c r="W209" t="s">
+        <v>117</v>
+      </c>
+      <c r="X209" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y209" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z209" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA209" t="s">
+        <v>117</v>
       </c>
       <c r="AB209" t="s">
         <v>117</v>
@@ -35690,10 +35708,10 @@
         <v>3</v>
       </c>
       <c r="AE209" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="AH209" s="8" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AI209" t="s">
         <v>117</v>
@@ -35702,12 +35720,12 @@
         <v>117</v>
       </c>
       <c r="AK209" t="e">
-        <f t="shared" si="156"/>
+        <f t="shared" si="158"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL209">
-        <f t="shared" si="157"/>
-        <v>71823.084029435064</v>
+      <c r="AL209" t="e">
+        <f t="shared" si="159"/>
+        <v>#VALUE!</v>
       </c>
       <c r="AM209" s="8" t="s">
         <v>105</v>
@@ -35731,43 +35749,43 @@
         <v>320</v>
       </c>
       <c r="AT209" s="47" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AU209">
-        <f t="shared" si="158"/>
+        <f t="shared" si="155"/>
         <v>14</v>
       </c>
       <c r="AV209">
-        <f t="shared" si="159"/>
+        <f t="shared" si="156"/>
         <v>11</v>
       </c>
       <c r="AW209">
+        <f t="shared" si="157"/>
+        <v>57</v>
+      </c>
+      <c r="AX209" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY209">
         <f t="shared" si="160"/>
-        <v>57</v>
-      </c>
-      <c r="AX209" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY209">
+        <v>106</v>
+      </c>
+      <c r="AZ209">
         <f t="shared" si="161"/>
-        <v>106</v>
-      </c>
-      <c r="AZ209">
+        <v>709</v>
+      </c>
+      <c r="BA209" s="8">
         <f t="shared" si="162"/>
-        <v>709</v>
-      </c>
-      <c r="BA209" s="8">
-        <f t="shared" si="163"/>
         <v>263</v>
       </c>
       <c r="BB209" t="s">
-        <v>772</v>
+        <v>619</v>
       </c>
       <c r="BC209" t="s">
-        <v>773</v>
-      </c>
-      <c r="BD209" t="s">
-        <v>117</v>
+        <v>620</v>
+      </c>
+      <c r="BD209">
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:56" x14ac:dyDescent="0.25">
@@ -35775,13 +35793,13 @@
         <v>777</v>
       </c>
       <c r="B210" s="10" t="s">
-        <v>786</v>
+        <v>795</v>
       </c>
       <c r="C210" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="D210" t="s">
-        <v>457</v>
+        <v>477</v>
       </c>
       <c r="E210" t="s">
         <v>406</v>
@@ -35790,7 +35808,7 @@
         <v>636</v>
       </c>
       <c r="G210" s="40" t="s">
-        <v>790</v>
+        <v>798</v>
       </c>
       <c r="H210" s="10" t="s">
         <v>117</v>
@@ -35805,33 +35823,32 @@
       <c r="V210" s="17" t="s">
         <v>769</v>
       </c>
-      <c r="W210">
-        <v>1</v>
-      </c>
-      <c r="X210">
-        <v>5</v>
-      </c>
-      <c r="Y210">
-        <v>1</v>
-      </c>
-      <c r="Z210">
-        <v>1</v>
-      </c>
-      <c r="AA210">
-        <f t="shared" si="155"/>
-        <v>6</v>
-      </c>
-      <c r="AB210">
-        <v>7</v>
+      <c r="W210" t="s">
+        <v>117</v>
+      </c>
+      <c r="X210" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y210" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z210" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA210" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB210" t="s">
+        <v>117</v>
       </c>
       <c r="AC210">
         <v>3</v>
       </c>
       <c r="AE210" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="AH210" s="8" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AI210" t="s">
         <v>117</v>
@@ -35840,12 +35857,12 @@
         <v>117</v>
       </c>
       <c r="AK210" t="e">
-        <f t="shared" si="156"/>
+        <f t="shared" si="158"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL210">
-        <f t="shared" si="157"/>
-        <v>71823.084029435064</v>
+      <c r="AL210" t="e">
+        <f t="shared" si="159"/>
+        <v>#VALUE!</v>
       </c>
       <c r="AM210" s="8" t="s">
         <v>105</v>
@@ -35869,43 +35886,43 @@
         <v>320</v>
       </c>
       <c r="AT210" s="47" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AU210">
-        <f t="shared" si="158"/>
+        <f t="shared" si="155"/>
         <v>14</v>
       </c>
       <c r="AV210">
-        <f t="shared" si="159"/>
+        <f t="shared" si="156"/>
         <v>11</v>
       </c>
       <c r="AW210">
+        <f t="shared" si="157"/>
+        <v>57</v>
+      </c>
+      <c r="AX210" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY210">
         <f t="shared" si="160"/>
-        <v>57</v>
-      </c>
-      <c r="AX210" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY210">
+        <v>106</v>
+      </c>
+      <c r="AZ210">
         <f t="shared" si="161"/>
-        <v>106</v>
-      </c>
-      <c r="AZ210">
+        <v>709</v>
+      </c>
+      <c r="BA210" s="8">
         <f t="shared" si="162"/>
-        <v>709</v>
-      </c>
-      <c r="BA210" s="8">
-        <f t="shared" si="163"/>
         <v>263</v>
       </c>
       <c r="BB210" t="s">
-        <v>770</v>
+        <v>619</v>
       </c>
       <c r="BC210" t="s">
-        <v>771</v>
-      </c>
-      <c r="BD210" t="s">
-        <v>117</v>
+        <v>620</v>
+      </c>
+      <c r="BD210">
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:56" x14ac:dyDescent="0.25">
@@ -35913,13 +35930,13 @@
         <v>778</v>
       </c>
       <c r="B211" s="10" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="C211" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D211" t="s">
-        <v>457</v>
+        <v>477</v>
       </c>
       <c r="E211" t="s">
         <v>406</v>
@@ -35928,7 +35945,7 @@
         <v>636</v>
       </c>
       <c r="G211" s="40" t="s">
-        <v>790</v>
+        <v>798</v>
       </c>
       <c r="H211" s="10" t="s">
         <v>117</v>
@@ -35943,21 +35960,20 @@
       <c r="V211" s="17" t="s">
         <v>769</v>
       </c>
-      <c r="W211">
-        <v>1</v>
-      </c>
-      <c r="X211">
-        <v>5</v>
-      </c>
-      <c r="Y211">
-        <v>1</v>
-      </c>
-      <c r="Z211">
-        <v>1</v>
-      </c>
-      <c r="AA211">
-        <f t="shared" si="155"/>
-        <v>6</v>
+      <c r="W211" t="s">
+        <v>117</v>
+      </c>
+      <c r="X211" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y211" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z211" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA211" t="s">
+        <v>117</v>
       </c>
       <c r="AB211" t="s">
         <v>117</v>
@@ -35966,10 +35982,10 @@
         <v>3</v>
       </c>
       <c r="AE211" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="AH211" s="8" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AI211" t="s">
         <v>117</v>
@@ -35978,12 +35994,12 @@
         <v>117</v>
       </c>
       <c r="AK211" t="e">
-        <f t="shared" si="156"/>
+        <f t="shared" si="158"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL211">
-        <f t="shared" si="157"/>
-        <v>71823.084029435064</v>
+      <c r="AL211" t="e">
+        <f t="shared" si="159"/>
+        <v>#VALUE!</v>
       </c>
       <c r="AM211" s="8" t="s">
         <v>105</v>
@@ -36007,43 +36023,43 @@
         <v>320</v>
       </c>
       <c r="AT211" s="47" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AU211">
-        <f t="shared" si="158"/>
+        <f t="shared" si="155"/>
         <v>14</v>
       </c>
       <c r="AV211">
-        <f t="shared" si="159"/>
+        <f t="shared" si="156"/>
         <v>11</v>
       </c>
       <c r="AW211">
+        <f t="shared" si="157"/>
+        <v>57</v>
+      </c>
+      <c r="AX211" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY211">
         <f t="shared" si="160"/>
-        <v>57</v>
-      </c>
-      <c r="AX211" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY211">
+        <v>106</v>
+      </c>
+      <c r="AZ211">
         <f t="shared" si="161"/>
-        <v>106</v>
-      </c>
-      <c r="AZ211">
+        <v>709</v>
+      </c>
+      <c r="BA211" s="8">
         <f t="shared" si="162"/>
-        <v>709</v>
-      </c>
-      <c r="BA211" s="8">
-        <f t="shared" si="163"/>
         <v>263</v>
       </c>
       <c r="BB211" t="s">
-        <v>772</v>
+        <v>619</v>
       </c>
       <c r="BC211" t="s">
-        <v>773</v>
-      </c>
-      <c r="BD211" t="s">
-        <v>117</v>
+        <v>620</v>
+      </c>
+      <c r="BD211">
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:56" x14ac:dyDescent="0.25">
@@ -36051,13 +36067,13 @@
         <v>779</v>
       </c>
       <c r="B212" s="10" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="C212" t="s">
         <v>768</v>
       </c>
       <c r="D212" t="s">
-        <v>457</v>
+        <v>477</v>
       </c>
       <c r="E212" t="s">
         <v>406</v>
@@ -36066,7 +36082,7 @@
         <v>636</v>
       </c>
       <c r="G212" s="40" t="s">
-        <v>790</v>
+        <v>798</v>
       </c>
       <c r="H212" s="10" t="s">
         <v>117</v>
@@ -36081,21 +36097,20 @@
       <c r="V212" s="17" t="s">
         <v>769</v>
       </c>
-      <c r="W212">
-        <v>1</v>
-      </c>
-      <c r="X212">
-        <v>5</v>
-      </c>
-      <c r="Y212">
-        <v>1</v>
-      </c>
-      <c r="Z212">
-        <v>1</v>
-      </c>
-      <c r="AA212">
-        <f t="shared" si="155"/>
-        <v>6</v>
+      <c r="W212" t="s">
+        <v>117</v>
+      </c>
+      <c r="X212" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y212" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z212" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA212" t="s">
+        <v>117</v>
       </c>
       <c r="AB212" t="s">
         <v>117</v>
@@ -36104,10 +36119,10 @@
         <v>3</v>
       </c>
       <c r="AE212" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="AH212" s="8" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AI212" t="s">
         <v>117</v>
@@ -36116,12 +36131,12 @@
         <v>117</v>
       </c>
       <c r="AK212" t="e">
-        <f t="shared" si="156"/>
+        <f t="shared" si="158"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL212">
-        <f t="shared" si="157"/>
-        <v>71823.084029435064</v>
+      <c r="AL212" t="e">
+        <f t="shared" si="159"/>
+        <v>#VALUE!</v>
       </c>
       <c r="AM212" s="8" t="s">
         <v>105</v>
@@ -36145,176 +36160,1004 @@
         <v>320</v>
       </c>
       <c r="AT212" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AU212">
+        <f t="shared" si="155"/>
+        <v>14</v>
+      </c>
+      <c r="AV212">
+        <f t="shared" si="156"/>
+        <v>11</v>
+      </c>
+      <c r="AW212">
+        <f t="shared" si="157"/>
+        <v>57</v>
+      </c>
+      <c r="AX212" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY212">
+        <f t="shared" si="160"/>
+        <v>106</v>
+      </c>
+      <c r="AZ212">
+        <f t="shared" si="161"/>
+        <v>709</v>
+      </c>
+      <c r="BA212" s="8">
+        <f t="shared" si="162"/>
+        <v>263</v>
+      </c>
+      <c r="BB212" t="s">
+        <v>619</v>
+      </c>
+      <c r="BC212" t="s">
+        <v>620</v>
+      </c>
+      <c r="BD212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A216" s="10" t="s">
+        <v>774</v>
+      </c>
+      <c r="B216" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="C216" t="s">
+        <v>766</v>
+      </c>
+      <c r="D216" t="s">
+        <v>457</v>
+      </c>
+      <c r="E216" t="s">
+        <v>406</v>
+      </c>
+      <c r="F216" t="s">
+        <v>636</v>
+      </c>
+      <c r="G216" s="40" t="s">
+        <v>789</v>
+      </c>
+      <c r="H216" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I216" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J216" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U216" s="10"/>
+      <c r="V216" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="W216">
+        <v>1</v>
+      </c>
+      <c r="X216">
+        <v>5</v>
+      </c>
+      <c r="Y216">
+        <v>1</v>
+      </c>
+      <c r="Z216">
+        <v>1</v>
+      </c>
+      <c r="AA216">
+        <f t="shared" ref="AA216:AA221" si="163">X216+Y216</f>
+        <v>6</v>
+      </c>
+      <c r="AB216">
+        <v>7</v>
+      </c>
+      <c r="AC216">
+        <v>3</v>
+      </c>
+      <c r="AE216" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH216" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI216" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ216" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK216" t="e">
+        <f t="shared" ref="AK216:AK221" si="164">AI216+AJ216</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL216">
+        <f t="shared" ref="AL216:AL221" si="165" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ216*AR216*AS216) * (AA216 / 5) + 441</f>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM216" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN216">
+        <v>149</v>
+      </c>
+      <c r="AO216">
+        <v>743</v>
+      </c>
+      <c r="AP216" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ216">
+        <v>120</v>
+      </c>
+      <c r="AR216">
+        <v>720</v>
+      </c>
+      <c r="AS216">
+        <v>320</v>
+      </c>
+      <c r="AT216" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="AU212">
-        <f t="shared" si="158"/>
+      <c r="AU216">
+        <f t="shared" ref="AU216:AU221" si="166" xml:space="preserve"> _xlfn.FLOOR.MATH((AN216 - AQ216) / 2)</f>
         <v>14</v>
       </c>
-      <c r="AV212">
-        <f t="shared" si="159"/>
+      <c r="AV216">
+        <f t="shared" ref="AV216:AV221" si="167" xml:space="preserve"> _xlfn.FLOOR.MATH((AO216 - AR216) / 2)</f>
         <v>11</v>
       </c>
-      <c r="AW212">
-        <f t="shared" si="160"/>
+      <c r="AW216">
+        <f t="shared" ref="AW216:AW221" si="168" xml:space="preserve"> _xlfn.FLOOR.MATH((AP216 - AS216) / 2)</f>
         <v>57</v>
       </c>
-      <c r="AX212" s="47" t="s">
+      <c r="AX216" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="AY212">
-        <f t="shared" si="161"/>
+      <c r="AY216">
+        <f t="shared" ref="AY216:AY221" si="169">AQ216-AU216</f>
         <v>106</v>
       </c>
-      <c r="AZ212">
-        <f t="shared" si="162"/>
+      <c r="AZ216">
+        <f t="shared" ref="AZ216:AZ221" si="170">AR216-AV216</f>
         <v>709</v>
       </c>
-      <c r="BA212" s="8">
+      <c r="BA216" s="8">
+        <f t="shared" ref="BA216:BA221" si="171">AS216-AW216</f>
+        <v>263</v>
+      </c>
+      <c r="BB216" t="s">
+        <v>770</v>
+      </c>
+      <c r="BC216" t="s">
+        <v>771</v>
+      </c>
+      <c r="BD216" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="217" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A217" s="10" t="s">
+        <v>775</v>
+      </c>
+      <c r="B217" s="10" t="s">
+        <v>784</v>
+      </c>
+      <c r="C217" t="s">
+        <v>767</v>
+      </c>
+      <c r="D217" t="s">
+        <v>457</v>
+      </c>
+      <c r="E217" t="s">
+        <v>406</v>
+      </c>
+      <c r="F217" t="s">
+        <v>636</v>
+      </c>
+      <c r="G217" s="40" t="s">
+        <v>789</v>
+      </c>
+      <c r="H217" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I217" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J217" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U217" s="10"/>
+      <c r="V217" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="W217">
+        <v>1</v>
+      </c>
+      <c r="X217">
+        <v>5</v>
+      </c>
+      <c r="Y217">
+        <v>1</v>
+      </c>
+      <c r="Z217">
+        <v>1</v>
+      </c>
+      <c r="AA217">
         <f t="shared" si="163"/>
+        <v>6</v>
+      </c>
+      <c r="AB217" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC217">
+        <v>3</v>
+      </c>
+      <c r="AE217" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH217" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI217" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ217" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK217" t="e">
+        <f t="shared" si="164"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL217">
+        <f t="shared" si="165"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM217" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN217">
+        <v>149</v>
+      </c>
+      <c r="AO217">
+        <v>743</v>
+      </c>
+      <c r="AP217" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ217">
+        <v>120</v>
+      </c>
+      <c r="AR217">
+        <v>720</v>
+      </c>
+      <c r="AS217">
+        <v>320</v>
+      </c>
+      <c r="AT217" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU217">
+        <f t="shared" si="166"/>
+        <v>14</v>
+      </c>
+      <c r="AV217">
+        <f t="shared" si="167"/>
+        <v>11</v>
+      </c>
+      <c r="AW217">
+        <f t="shared" si="168"/>
+        <v>57</v>
+      </c>
+      <c r="AX217" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY217">
+        <f t="shared" si="169"/>
+        <v>106</v>
+      </c>
+      <c r="AZ217">
+        <f t="shared" si="170"/>
+        <v>709</v>
+      </c>
+      <c r="BA217" s="8">
+        <f t="shared" si="171"/>
         <v>263</v>
       </c>
-      <c r="BB212" t="s">
+      <c r="BB217" t="s">
         <v>772</v>
       </c>
-      <c r="BC212" t="s">
+      <c r="BC217" t="s">
         <v>773</v>
       </c>
-      <c r="BD212" t="s">
+      <c r="BD217" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="213" spans="1:56" x14ac:dyDescent="0.25">
-      <c r="A213" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B213" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C213" t="s">
-        <v>117</v>
-      </c>
-      <c r="D213" t="s">
-        <v>117</v>
-      </c>
-      <c r="E213" t="s">
-        <v>117</v>
-      </c>
-      <c r="F213" t="s">
-        <v>117</v>
-      </c>
-      <c r="G213" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="H213" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="I213" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J213" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="U213" s="10"/>
-      <c r="V213" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="W213" t="s">
-        <v>117</v>
-      </c>
-      <c r="X213" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y213" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AE213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH213" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AJ213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK213" t="e">
-        <f t="shared" ref="AK213" si="164">AI213+AJ213</f>
+    <row r="218" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A218" s="10" t="s">
+        <v>776</v>
+      </c>
+      <c r="B218" s="10" t="s">
+        <v>785</v>
+      </c>
+      <c r="C218" t="s">
+        <v>768</v>
+      </c>
+      <c r="D218" t="s">
+        <v>457</v>
+      </c>
+      <c r="E218" t="s">
+        <v>406</v>
+      </c>
+      <c r="F218" t="s">
+        <v>636</v>
+      </c>
+      <c r="G218" s="40" t="s">
+        <v>789</v>
+      </c>
+      <c r="H218" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I218" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J218" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U218" s="10"/>
+      <c r="V218" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="W218">
+        <v>1</v>
+      </c>
+      <c r="X218">
+        <v>5</v>
+      </c>
+      <c r="Y218">
+        <v>1</v>
+      </c>
+      <c r="Z218">
+        <v>1</v>
+      </c>
+      <c r="AA218">
+        <f t="shared" si="163"/>
+        <v>6</v>
+      </c>
+      <c r="AB218" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC218">
+        <v>3</v>
+      </c>
+      <c r="AE218" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH218" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI218" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ218" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK218" t="e">
+        <f t="shared" si="164"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AL213" t="e">
-        <f t="shared" ref="AL213" si="165" xml:space="preserve"> 1508.06553301511 + 0.00210606006752809 * (AQ213*AR213*AS213) * (AA213 / 5) + 441</f>
+      <c r="AL218">
+        <f t="shared" si="165"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM218" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN218">
+        <v>149</v>
+      </c>
+      <c r="AO218">
+        <v>743</v>
+      </c>
+      <c r="AP218" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ218">
+        <v>120</v>
+      </c>
+      <c r="AR218">
+        <v>720</v>
+      </c>
+      <c r="AS218">
+        <v>320</v>
+      </c>
+      <c r="AT218" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU218">
+        <f t="shared" si="166"/>
+        <v>14</v>
+      </c>
+      <c r="AV218">
+        <f t="shared" si="167"/>
+        <v>11</v>
+      </c>
+      <c r="AW218">
+        <f t="shared" si="168"/>
+        <v>57</v>
+      </c>
+      <c r="AX218" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY218">
+        <f t="shared" si="169"/>
+        <v>106</v>
+      </c>
+      <c r="AZ218">
+        <f t="shared" si="170"/>
+        <v>709</v>
+      </c>
+      <c r="BA218" s="8">
+        <f t="shared" si="171"/>
+        <v>263</v>
+      </c>
+      <c r="BB218" t="s">
+        <v>772</v>
+      </c>
+      <c r="BC218" t="s">
+        <v>773</v>
+      </c>
+      <c r="BD218" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="219" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A219" s="10" t="s">
+        <v>777</v>
+      </c>
+      <c r="B219" s="10" t="s">
+        <v>786</v>
+      </c>
+      <c r="C219" t="s">
+        <v>766</v>
+      </c>
+      <c r="D219" t="s">
+        <v>457</v>
+      </c>
+      <c r="E219" t="s">
+        <v>406</v>
+      </c>
+      <c r="F219" t="s">
+        <v>636</v>
+      </c>
+      <c r="G219" s="40" t="s">
+        <v>790</v>
+      </c>
+      <c r="H219" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I219" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J219" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U219" s="10"/>
+      <c r="V219" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="W219">
+        <v>1</v>
+      </c>
+      <c r="X219">
+        <v>5</v>
+      </c>
+      <c r="Y219">
+        <v>1</v>
+      </c>
+      <c r="Z219">
+        <v>1</v>
+      </c>
+      <c r="AA219">
+        <f t="shared" si="163"/>
+        <v>6</v>
+      </c>
+      <c r="AB219">
+        <v>7</v>
+      </c>
+      <c r="AC219">
+        <v>3</v>
+      </c>
+      <c r="AE219" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH219" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI219" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ219" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK219" t="e">
+        <f t="shared" si="164"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AM213" s="8" t="s">
+      <c r="AL219">
+        <f t="shared" si="165"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM219" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AN213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AO213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP213" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="AQ213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AR213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AS213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AT213" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AV213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AW213" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX213" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="AY213" t="e">
-        <f t="shared" ref="AY213" si="166">AQ213-AU213</f>
+      <c r="AN219">
+        <v>149</v>
+      </c>
+      <c r="AO219">
+        <v>743</v>
+      </c>
+      <c r="AP219" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ219">
+        <v>120</v>
+      </c>
+      <c r="AR219">
+        <v>720</v>
+      </c>
+      <c r="AS219">
+        <v>320</v>
+      </c>
+      <c r="AT219" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU219">
+        <f t="shared" si="166"/>
+        <v>14</v>
+      </c>
+      <c r="AV219">
+        <f t="shared" si="167"/>
+        <v>11</v>
+      </c>
+      <c r="AW219">
+        <f t="shared" si="168"/>
+        <v>57</v>
+      </c>
+      <c r="AX219" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY219">
+        <f t="shared" si="169"/>
+        <v>106</v>
+      </c>
+      <c r="AZ219">
+        <f t="shared" si="170"/>
+        <v>709</v>
+      </c>
+      <c r="BA219" s="8">
+        <f t="shared" si="171"/>
+        <v>263</v>
+      </c>
+      <c r="BB219" t="s">
+        <v>770</v>
+      </c>
+      <c r="BC219" t="s">
+        <v>771</v>
+      </c>
+      <c r="BD219" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="220" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A220" s="10" t="s">
+        <v>778</v>
+      </c>
+      <c r="B220" s="10" t="s">
+        <v>787</v>
+      </c>
+      <c r="C220" t="s">
+        <v>767</v>
+      </c>
+      <c r="D220" t="s">
+        <v>457</v>
+      </c>
+      <c r="E220" t="s">
+        <v>406</v>
+      </c>
+      <c r="F220" t="s">
+        <v>636</v>
+      </c>
+      <c r="G220" s="40" t="s">
+        <v>790</v>
+      </c>
+      <c r="H220" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I220" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J220" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U220" s="10"/>
+      <c r="V220" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="W220">
+        <v>1</v>
+      </c>
+      <c r="X220">
+        <v>5</v>
+      </c>
+      <c r="Y220">
+        <v>1</v>
+      </c>
+      <c r="Z220">
+        <v>1</v>
+      </c>
+      <c r="AA220">
+        <f t="shared" si="163"/>
+        <v>6</v>
+      </c>
+      <c r="AB220" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC220">
+        <v>3</v>
+      </c>
+      <c r="AE220" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH220" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI220" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ220" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK220" t="e">
+        <f t="shared" si="164"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ213" t="e">
-        <f t="shared" ref="AZ213" si="167">AR213-AV213</f>
+      <c r="AL220">
+        <f t="shared" si="165"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM220" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN220">
+        <v>149</v>
+      </c>
+      <c r="AO220">
+        <v>743</v>
+      </c>
+      <c r="AP220" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ220">
+        <v>120</v>
+      </c>
+      <c r="AR220">
+        <v>720</v>
+      </c>
+      <c r="AS220">
+        <v>320</v>
+      </c>
+      <c r="AT220" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU220">
+        <f t="shared" si="166"/>
+        <v>14</v>
+      </c>
+      <c r="AV220">
+        <f t="shared" si="167"/>
+        <v>11</v>
+      </c>
+      <c r="AW220">
+        <f t="shared" si="168"/>
+        <v>57</v>
+      </c>
+      <c r="AX220" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY220">
+        <f t="shared" si="169"/>
+        <v>106</v>
+      </c>
+      <c r="AZ220">
+        <f t="shared" si="170"/>
+        <v>709</v>
+      </c>
+      <c r="BA220" s="8">
+        <f t="shared" si="171"/>
+        <v>263</v>
+      </c>
+      <c r="BB220" t="s">
+        <v>772</v>
+      </c>
+      <c r="BC220" t="s">
+        <v>773</v>
+      </c>
+      <c r="BD220" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="221" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A221" s="10" t="s">
+        <v>779</v>
+      </c>
+      <c r="B221" s="10" t="s">
+        <v>788</v>
+      </c>
+      <c r="C221" t="s">
+        <v>768</v>
+      </c>
+      <c r="D221" t="s">
+        <v>457</v>
+      </c>
+      <c r="E221" t="s">
+        <v>406</v>
+      </c>
+      <c r="F221" t="s">
+        <v>636</v>
+      </c>
+      <c r="G221" s="40" t="s">
+        <v>790</v>
+      </c>
+      <c r="H221" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I221" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J221" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U221" s="10"/>
+      <c r="V221" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="W221">
+        <v>1</v>
+      </c>
+      <c r="X221">
+        <v>5</v>
+      </c>
+      <c r="Y221">
+        <v>1</v>
+      </c>
+      <c r="Z221">
+        <v>1</v>
+      </c>
+      <c r="AA221">
+        <f t="shared" si="163"/>
+        <v>6</v>
+      </c>
+      <c r="AB221" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC221">
+        <v>3</v>
+      </c>
+      <c r="AE221" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH221" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AI221" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ221" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK221" t="e">
+        <f t="shared" si="164"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BA213" s="8" t="e">
-        <f t="shared" ref="BA213" si="168">AS213-AW213</f>
+      <c r="AL221">
+        <f t="shared" si="165"/>
+        <v>71823.084029435064</v>
+      </c>
+      <c r="AM221" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN221">
+        <v>149</v>
+      </c>
+      <c r="AO221">
+        <v>743</v>
+      </c>
+      <c r="AP221" s="17">
+        <v>435</v>
+      </c>
+      <c r="AQ221">
+        <v>120</v>
+      </c>
+      <c r="AR221">
+        <v>720</v>
+      </c>
+      <c r="AS221">
+        <v>320</v>
+      </c>
+      <c r="AT221" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU221">
+        <f t="shared" si="166"/>
+        <v>14</v>
+      </c>
+      <c r="AV221">
+        <f t="shared" si="167"/>
+        <v>11</v>
+      </c>
+      <c r="AW221">
+        <f t="shared" si="168"/>
+        <v>57</v>
+      </c>
+      <c r="AX221" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="AY221">
+        <f t="shared" si="169"/>
+        <v>106</v>
+      </c>
+      <c r="AZ221">
+        <f t="shared" si="170"/>
+        <v>709</v>
+      </c>
+      <c r="BA221" s="8">
+        <f t="shared" si="171"/>
+        <v>263</v>
+      </c>
+      <c r="BB221" t="s">
+        <v>772</v>
+      </c>
+      <c r="BC221" t="s">
+        <v>773</v>
+      </c>
+      <c r="BD221" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="222" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A222" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B222" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C222" t="s">
+        <v>117</v>
+      </c>
+      <c r="D222" t="s">
+        <v>117</v>
+      </c>
+      <c r="E222" t="s">
+        <v>117</v>
+      </c>
+      <c r="F222" t="s">
+        <v>117</v>
+      </c>
+      <c r="G222" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="H222" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I222" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J222" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="U222" s="10"/>
+      <c r="V222" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="W222" t="s">
+        <v>117</v>
+      </c>
+      <c r="X222" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y222" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z222" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA222" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB222" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC222" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE222" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH222" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI222" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ222" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK222" t="e">
+        <f t="shared" ref="AK222" si="172">AI222+AJ222</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB213" t="s">
-        <v>117</v>
-      </c>
-      <c r="B